<commit_message>
First drafting of db structure
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleca\Desktop\Main\University\Lab_AP\Progetto\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99E45E0-0BB9-4D2F-A49A-EA60F2D5AF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA13D475-259F-4786-B7AF-ED95DB411FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLE Gantt Chart &amp; Burndown" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="210">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -654,6 +654,18 @@
   </si>
   <si>
     <t>DB (Baldi/Dieni)</t>
+  </si>
+  <si>
+    <t>Implementation of II Sprit features</t>
+  </si>
+  <si>
+    <t>First drafting of db structure</t>
+  </si>
+  <si>
+    <t>everyone</t>
+  </si>
+  <si>
+    <t>Alessandro Catalano</t>
   </si>
 </sst>
 </file>
@@ -2349,11 +2361,53 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2384,48 +2438,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5330,184 +5342,184 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.75</c:v>
+                  <c:v>16.716666666666665</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.5</c:v>
+                  <c:v>16.43333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.25</c:v>
+                  <c:v>16.149999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>15.866666666666662</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.75</c:v>
+                  <c:v>15.583333333333329</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.5</c:v>
+                  <c:v>15.299999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.25</c:v>
+                  <c:v>15.016666666666662</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13</c:v>
+                  <c:v>14.733333333333329</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.75</c:v>
+                  <c:v>14.449999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12.5</c:v>
+                  <c:v>14.166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.25</c:v>
+                  <c:v>13.883333333333329</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>13.599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.75</c:v>
+                  <c:v>13.316666666666663</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.5</c:v>
+                  <c:v>13.03333333333333</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.25</c:v>
+                  <c:v>12.749999999999996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11</c:v>
+                  <c:v>12.466666666666663</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.75</c:v>
+                  <c:v>12.18333333333333</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.5</c:v>
+                  <c:v>11.899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.25</c:v>
+                  <c:v>11.616666666666664</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10</c:v>
+                  <c:v>11.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.75</c:v>
+                  <c:v>11.049999999999997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.5</c:v>
+                  <c:v>10.766666666666664</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.25</c:v>
+                  <c:v>10.483333333333331</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9</c:v>
+                  <c:v>10.199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.75</c:v>
+                  <c:v>9.9166666666666643</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8.5</c:v>
+                  <c:v>9.6333333333333311</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8.25</c:v>
+                  <c:v>9.3499999999999979</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8</c:v>
+                  <c:v>9.0666666666666647</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.75</c:v>
+                  <c:v>8.7833333333333314</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.5</c:v>
+                  <c:v>8.4999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.25</c:v>
+                  <c:v>8.216666666666665</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7</c:v>
+                  <c:v>7.9333333333333318</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.75</c:v>
+                  <c:v>7.6499999999999986</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.5</c:v>
+                  <c:v>7.3666666666666654</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.25</c:v>
+                  <c:v>7.0833333333333321</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6</c:v>
+                  <c:v>6.7999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.75</c:v>
+                  <c:v>6.5166666666666657</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.5</c:v>
+                  <c:v>6.2333333333333325</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.25</c:v>
+                  <c:v>5.9499999999999993</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5</c:v>
+                  <c:v>5.6666666666666661</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.75</c:v>
+                  <c:v>5.3833333333333329</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.5</c:v>
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>4.8166666666666664</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.5333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>4.25</c:v>
                 </c:pt>
-                <c:pt idx="44">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3.75</c:v>
-                </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.5</c:v>
+                  <c:v>3.9666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.25</c:v>
+                  <c:v>3.6833333333333336</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3</c:v>
+                  <c:v>3.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.75</c:v>
+                  <c:v>3.1166666666666671</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.5</c:v>
+                  <c:v>2.8333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.25</c:v>
+                  <c:v>2.5500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2</c:v>
+                  <c:v>2.2666666666666675</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.75</c:v>
+                  <c:v>1.9833333333333343</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.5</c:v>
+                  <c:v>1.7000000000000011</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.25</c:v>
+                  <c:v>1.4166666666666679</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1</c:v>
+                  <c:v>1.1333333333333346</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.75</c:v>
+                  <c:v>0.85000000000000131</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.5</c:v>
+                  <c:v>0.56666666666666798</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.25</c:v>
+                  <c:v>0.28333333333333466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5741,184 +5753,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6823,19 +6835,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="159" t="str">
+      <c r="BK2" s="177" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="160"/>
-      <c r="BM2" s="160"/>
-      <c r="BN2" s="160"/>
-      <c r="BO2" s="160"/>
-      <c r="BP2" s="160"/>
-      <c r="BQ2" s="160"/>
-      <c r="BR2" s="160"/>
-      <c r="BS2" s="160"/>
-      <c r="BT2" s="160"/>
+      <c r="BL2" s="178"/>
+      <c r="BM2" s="178"/>
+      <c r="BN2" s="178"/>
+      <c r="BO2" s="178"/>
+      <c r="BP2" s="178"/>
+      <c r="BQ2" s="178"/>
+      <c r="BR2" s="178"/>
+      <c r="BS2" s="178"/>
+      <c r="BT2" s="178"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -6863,7 +6875,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="161" t="s">
+      <c r="K4" s="179" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -6940,7 +6952,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="162"/>
+      <c r="K5" s="180"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7015,7 +7027,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="162"/>
+      <c r="K6" s="180"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7090,7 +7102,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="162"/>
+      <c r="K7" s="180"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7165,7 +7177,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="163"/>
+      <c r="K8" s="181"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7231,124 +7243,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="164" t="s">
+      <c r="B9" s="182" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="166" t="s">
+      <c r="C9" s="184" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="168" t="s">
+      <c r="D9" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="170" t="s">
+      <c r="E9" s="188" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="171"/>
-      <c r="G9" s="172"/>
-      <c r="H9" s="173" t="s">
+      <c r="F9" s="189"/>
+      <c r="G9" s="190"/>
+      <c r="H9" s="191" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="178" t="s">
+      <c r="I9" s="159" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="180" t="s">
+      <c r="J9" s="161" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="182" t="s">
+      <c r="K9" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="183" t="s">
+      <c r="L9" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="185" t="s">
+      <c r="M9" s="166" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="157"/>
-      <c r="O9" s="157"/>
-      <c r="P9" s="157"/>
-      <c r="Q9" s="186"/>
-      <c r="R9" s="187" t="s">
+      <c r="N9" s="167"/>
+      <c r="O9" s="167"/>
+      <c r="P9" s="167"/>
+      <c r="Q9" s="168"/>
+      <c r="R9" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="157"/>
-      <c r="T9" s="157"/>
-      <c r="U9" s="157"/>
-      <c r="V9" s="186"/>
-      <c r="W9" s="187" t="s">
+      <c r="S9" s="167"/>
+      <c r="T9" s="167"/>
+      <c r="U9" s="167"/>
+      <c r="V9" s="168"/>
+      <c r="W9" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="157"/>
-      <c r="Y9" s="157"/>
-      <c r="Z9" s="157"/>
-      <c r="AA9" s="158"/>
-      <c r="AB9" s="188" t="s">
+      <c r="X9" s="167"/>
+      <c r="Y9" s="167"/>
+      <c r="Z9" s="167"/>
+      <c r="AA9" s="170"/>
+      <c r="AB9" s="171" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="157"/>
-      <c r="AD9" s="157"/>
-      <c r="AE9" s="157"/>
-      <c r="AF9" s="186"/>
-      <c r="AG9" s="189" t="s">
+      <c r="AC9" s="167"/>
+      <c r="AD9" s="167"/>
+      <c r="AE9" s="167"/>
+      <c r="AF9" s="168"/>
+      <c r="AG9" s="172" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="157"/>
-      <c r="AI9" s="157"/>
-      <c r="AJ9" s="157"/>
-      <c r="AK9" s="186"/>
-      <c r="AL9" s="189" t="s">
+      <c r="AH9" s="167"/>
+      <c r="AI9" s="167"/>
+      <c r="AJ9" s="167"/>
+      <c r="AK9" s="168"/>
+      <c r="AL9" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="157"/>
-      <c r="AN9" s="157"/>
-      <c r="AO9" s="157"/>
-      <c r="AP9" s="158"/>
-      <c r="AQ9" s="190" t="s">
+      <c r="AM9" s="167"/>
+      <c r="AN9" s="167"/>
+      <c r="AO9" s="167"/>
+      <c r="AP9" s="170"/>
+      <c r="AQ9" s="173" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="157"/>
-      <c r="AS9" s="157"/>
-      <c r="AT9" s="157"/>
-      <c r="AU9" s="186"/>
-      <c r="AV9" s="191" t="s">
+      <c r="AR9" s="167"/>
+      <c r="AS9" s="167"/>
+      <c r="AT9" s="167"/>
+      <c r="AU9" s="168"/>
+      <c r="AV9" s="174" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="157"/>
-      <c r="AX9" s="157"/>
-      <c r="AY9" s="157"/>
-      <c r="AZ9" s="186"/>
-      <c r="BA9" s="191" t="s">
+      <c r="AW9" s="167"/>
+      <c r="AX9" s="167"/>
+      <c r="AY9" s="167"/>
+      <c r="AZ9" s="168"/>
+      <c r="BA9" s="174" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="157"/>
-      <c r="BC9" s="157"/>
-      <c r="BD9" s="157"/>
-      <c r="BE9" s="158"/>
-      <c r="BF9" s="192" t="s">
+      <c r="BB9" s="167"/>
+      <c r="BC9" s="167"/>
+      <c r="BD9" s="167"/>
+      <c r="BE9" s="170"/>
+      <c r="BF9" s="175" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="157"/>
-      <c r="BH9" s="157"/>
-      <c r="BI9" s="157"/>
-      <c r="BJ9" s="186"/>
-      <c r="BK9" s="156" t="s">
+      <c r="BG9" s="167"/>
+      <c r="BH9" s="167"/>
+      <c r="BI9" s="167"/>
+      <c r="BJ9" s="168"/>
+      <c r="BK9" s="176" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="157"/>
-      <c r="BM9" s="157"/>
-      <c r="BN9" s="157"/>
-      <c r="BO9" s="186"/>
-      <c r="BP9" s="156" t="s">
+      <c r="BL9" s="167"/>
+      <c r="BM9" s="167"/>
+      <c r="BN9" s="167"/>
+      <c r="BO9" s="168"/>
+      <c r="BP9" s="176" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="157"/>
-      <c r="BR9" s="157"/>
-      <c r="BS9" s="157"/>
-      <c r="BT9" s="158"/>
+      <c r="BQ9" s="167"/>
+      <c r="BR9" s="167"/>
+      <c r="BS9" s="167"/>
+      <c r="BT9" s="170"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="165"/>
-      <c r="C10" s="167"/>
-      <c r="D10" s="169"/>
+      <c r="B10" s="183"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="187"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7358,11 +7370,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="174"/>
-      <c r="I10" s="179"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="184"/>
+      <c r="H10" s="192"/>
+      <c r="I10" s="160"/>
+      <c r="J10" s="162"/>
+      <c r="K10" s="162"/>
+      <c r="L10" s="165"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -10971,80 +10983,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="175" t="str">
+      <c r="B45" s="156" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="176"/>
-      <c r="D45" s="176"/>
-      <c r="E45" s="176"/>
-      <c r="F45" s="176"/>
-      <c r="G45" s="176"/>
-      <c r="H45" s="176"/>
-      <c r="I45" s="176"/>
-      <c r="J45" s="176"/>
-      <c r="K45" s="176"/>
-      <c r="L45" s="176"/>
-      <c r="M45" s="176"/>
-      <c r="N45" s="176"/>
-      <c r="O45" s="176"/>
-      <c r="P45" s="176"/>
-      <c r="Q45" s="176"/>
-      <c r="R45" s="176"/>
-      <c r="S45" s="176"/>
-      <c r="T45" s="176"/>
-      <c r="U45" s="176"/>
-      <c r="V45" s="176"/>
-      <c r="W45" s="176"/>
-      <c r="X45" s="176"/>
-      <c r="Y45" s="176"/>
-      <c r="Z45" s="176"/>
-      <c r="AA45" s="176"/>
-      <c r="AB45" s="176"/>
-      <c r="AC45" s="176"/>
-      <c r="AD45" s="176"/>
-      <c r="AE45" s="176"/>
-      <c r="AF45" s="176"/>
-      <c r="AG45" s="176"/>
-      <c r="AH45" s="176"/>
-      <c r="AI45" s="176"/>
-      <c r="AJ45" s="176"/>
-      <c r="AK45" s="176"/>
-      <c r="AL45" s="176"/>
-      <c r="AM45" s="176"/>
-      <c r="AN45" s="176"/>
-      <c r="AO45" s="176"/>
-      <c r="AP45" s="176"/>
-      <c r="AQ45" s="176"/>
-      <c r="AR45" s="176"/>
-      <c r="AS45" s="176"/>
-      <c r="AT45" s="176"/>
-      <c r="AU45" s="176"/>
-      <c r="AV45" s="176"/>
-      <c r="AW45" s="176"/>
-      <c r="AX45" s="176"/>
-      <c r="AY45" s="176"/>
-      <c r="AZ45" s="176"/>
-      <c r="BA45" s="176"/>
-      <c r="BB45" s="176"/>
-      <c r="BC45" s="176"/>
-      <c r="BD45" s="176"/>
-      <c r="BE45" s="176"/>
-      <c r="BF45" s="176"/>
-      <c r="BG45" s="176"/>
-      <c r="BH45" s="176"/>
-      <c r="BI45" s="176"/>
-      <c r="BJ45" s="176"/>
-      <c r="BK45" s="176"/>
-      <c r="BL45" s="176"/>
-      <c r="BM45" s="176"/>
-      <c r="BN45" s="176"/>
-      <c r="BO45" s="176"/>
-      <c r="BP45" s="176"/>
-      <c r="BQ45" s="176"/>
-      <c r="BR45" s="176"/>
-      <c r="BS45" s="176"/>
-      <c r="BT45" s="177"/>
+      <c r="C45" s="157"/>
+      <c r="D45" s="157"/>
+      <c r="E45" s="157"/>
+      <c r="F45" s="157"/>
+      <c r="G45" s="157"/>
+      <c r="H45" s="157"/>
+      <c r="I45" s="157"/>
+      <c r="J45" s="157"/>
+      <c r="K45" s="157"/>
+      <c r="L45" s="157"/>
+      <c r="M45" s="157"/>
+      <c r="N45" s="157"/>
+      <c r="O45" s="157"/>
+      <c r="P45" s="157"/>
+      <c r="Q45" s="157"/>
+      <c r="R45" s="157"/>
+      <c r="S45" s="157"/>
+      <c r="T45" s="157"/>
+      <c r="U45" s="157"/>
+      <c r="V45" s="157"/>
+      <c r="W45" s="157"/>
+      <c r="X45" s="157"/>
+      <c r="Y45" s="157"/>
+      <c r="Z45" s="157"/>
+      <c r="AA45" s="157"/>
+      <c r="AB45" s="157"/>
+      <c r="AC45" s="157"/>
+      <c r="AD45" s="157"/>
+      <c r="AE45" s="157"/>
+      <c r="AF45" s="157"/>
+      <c r="AG45" s="157"/>
+      <c r="AH45" s="157"/>
+      <c r="AI45" s="157"/>
+      <c r="AJ45" s="157"/>
+      <c r="AK45" s="157"/>
+      <c r="AL45" s="157"/>
+      <c r="AM45" s="157"/>
+      <c r="AN45" s="157"/>
+      <c r="AO45" s="157"/>
+      <c r="AP45" s="157"/>
+      <c r="AQ45" s="157"/>
+      <c r="AR45" s="157"/>
+      <c r="AS45" s="157"/>
+      <c r="AT45" s="157"/>
+      <c r="AU45" s="157"/>
+      <c r="AV45" s="157"/>
+      <c r="AW45" s="157"/>
+      <c r="AX45" s="157"/>
+      <c r="AY45" s="157"/>
+      <c r="AZ45" s="157"/>
+      <c r="BA45" s="157"/>
+      <c r="BB45" s="157"/>
+      <c r="BC45" s="157"/>
+      <c r="BD45" s="157"/>
+      <c r="BE45" s="157"/>
+      <c r="BF45" s="157"/>
+      <c r="BG45" s="157"/>
+      <c r="BH45" s="157"/>
+      <c r="BI45" s="157"/>
+      <c r="BJ45" s="157"/>
+      <c r="BK45" s="157"/>
+      <c r="BL45" s="157"/>
+      <c r="BM45" s="157"/>
+      <c r="BN45" s="157"/>
+      <c r="BO45" s="157"/>
+      <c r="BP45" s="157"/>
+      <c r="BQ45" s="157"/>
+      <c r="BR45" s="157"/>
+      <c r="BS45" s="157"/>
+      <c r="BT45" s="158"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12007,6 +12019,14 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12023,14 +12043,6 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12045,8 +12057,8 @@
   </sheetPr>
   <dimension ref="B1:BV999"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12134,7 +12146,7 @@
       <c r="BP1" s="2"/>
       <c r="BQ1" s="109"/>
     </row>
-    <row r="2" spans="2:72" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:72" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -12159,7 +12171,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="161" t="s">
+      <c r="K3" s="179" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12236,12 +12248,11 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="162"/>
+      <c r="K4" s="180"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="M4" s="14"/>
-      <c r="N4" s="16"/>
       <c r="O4" s="14"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
@@ -12255,21 +12266,21 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="15"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="15"/>
-      <c r="AI4" s="15"/>
-      <c r="AJ4" s="15"/>
-      <c r="AK4" s="15"/>
-      <c r="AL4" s="15"/>
-      <c r="AM4" s="15"/>
-      <c r="AN4" s="15"/>
-      <c r="AO4" s="15"/>
-      <c r="AP4" s="15"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="16"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="16"/>
+      <c r="AN4" s="16"/>
+      <c r="AO4" s="16"/>
+      <c r="AP4" s="16"/>
       <c r="AQ4" s="15"/>
       <c r="AR4" s="15"/>
       <c r="AS4" s="15"/>
@@ -12311,7 +12322,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="162"/>
+      <c r="K5" s="180"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12386,7 +12397,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="162"/>
+      <c r="K6" s="180"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12461,7 +12472,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="163"/>
+      <c r="K7" s="181"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12527,124 +12538,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="164" t="s">
+      <c r="B8" s="182" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="166" t="s">
+      <c r="C8" s="184" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="168" t="s">
+      <c r="D8" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="170" t="s">
+      <c r="E8" s="188" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="171"/>
-      <c r="G8" s="172"/>
-      <c r="H8" s="173" t="s">
+      <c r="F8" s="189"/>
+      <c r="G8" s="190"/>
+      <c r="H8" s="191" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="178" t="s">
+      <c r="I8" s="159" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="180" t="s">
+      <c r="J8" s="161" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="182" t="s">
+      <c r="K8" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="183" t="s">
+      <c r="L8" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="185" t="s">
+      <c r="M8" s="166" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="157"/>
-      <c r="O8" s="157"/>
-      <c r="P8" s="157"/>
-      <c r="Q8" s="186"/>
-      <c r="R8" s="187" t="s">
+      <c r="N8" s="167"/>
+      <c r="O8" s="167"/>
+      <c r="P8" s="167"/>
+      <c r="Q8" s="168"/>
+      <c r="R8" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="157"/>
-      <c r="T8" s="157"/>
-      <c r="U8" s="157"/>
-      <c r="V8" s="186"/>
-      <c r="W8" s="187" t="s">
+      <c r="S8" s="167"/>
+      <c r="T8" s="167"/>
+      <c r="U8" s="167"/>
+      <c r="V8" s="168"/>
+      <c r="W8" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="157"/>
-      <c r="Y8" s="157"/>
-      <c r="Z8" s="157"/>
-      <c r="AA8" s="158"/>
-      <c r="AB8" s="188" t="s">
+      <c r="X8" s="167"/>
+      <c r="Y8" s="167"/>
+      <c r="Z8" s="167"/>
+      <c r="AA8" s="170"/>
+      <c r="AB8" s="171" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="157"/>
-      <c r="AD8" s="157"/>
-      <c r="AE8" s="157"/>
-      <c r="AF8" s="186"/>
-      <c r="AG8" s="189" t="s">
+      <c r="AC8" s="167"/>
+      <c r="AD8" s="167"/>
+      <c r="AE8" s="167"/>
+      <c r="AF8" s="168"/>
+      <c r="AG8" s="172" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="157"/>
-      <c r="AI8" s="157"/>
-      <c r="AJ8" s="157"/>
-      <c r="AK8" s="186"/>
-      <c r="AL8" s="189" t="s">
+      <c r="AH8" s="167"/>
+      <c r="AI8" s="167"/>
+      <c r="AJ8" s="167"/>
+      <c r="AK8" s="168"/>
+      <c r="AL8" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="157"/>
-      <c r="AN8" s="157"/>
-      <c r="AO8" s="157"/>
-      <c r="AP8" s="158"/>
-      <c r="AQ8" s="190" t="s">
+      <c r="AM8" s="167"/>
+      <c r="AN8" s="167"/>
+      <c r="AO8" s="167"/>
+      <c r="AP8" s="170"/>
+      <c r="AQ8" s="173" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="157"/>
-      <c r="AS8" s="157"/>
-      <c r="AT8" s="157"/>
-      <c r="AU8" s="186"/>
-      <c r="AV8" s="191" t="s">
+      <c r="AR8" s="167"/>
+      <c r="AS8" s="167"/>
+      <c r="AT8" s="167"/>
+      <c r="AU8" s="168"/>
+      <c r="AV8" s="174" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="157"/>
-      <c r="AX8" s="157"/>
-      <c r="AY8" s="157"/>
-      <c r="AZ8" s="186"/>
-      <c r="BA8" s="191" t="s">
+      <c r="AW8" s="167"/>
+      <c r="AX8" s="167"/>
+      <c r="AY8" s="167"/>
+      <c r="AZ8" s="168"/>
+      <c r="BA8" s="174" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="157"/>
-      <c r="BC8" s="157"/>
-      <c r="BD8" s="157"/>
-      <c r="BE8" s="158"/>
-      <c r="BF8" s="192" t="s">
+      <c r="BB8" s="167"/>
+      <c r="BC8" s="167"/>
+      <c r="BD8" s="167"/>
+      <c r="BE8" s="170"/>
+      <c r="BF8" s="175" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="157"/>
-      <c r="BH8" s="157"/>
-      <c r="BI8" s="157"/>
-      <c r="BJ8" s="186"/>
-      <c r="BK8" s="156" t="s">
+      <c r="BG8" s="167"/>
+      <c r="BH8" s="167"/>
+      <c r="BI8" s="167"/>
+      <c r="BJ8" s="168"/>
+      <c r="BK8" s="176" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="157"/>
-      <c r="BM8" s="157"/>
-      <c r="BN8" s="157"/>
-      <c r="BO8" s="186"/>
-      <c r="BP8" s="156" t="s">
+      <c r="BL8" s="167"/>
+      <c r="BM8" s="167"/>
+      <c r="BN8" s="167"/>
+      <c r="BO8" s="168"/>
+      <c r="BP8" s="176" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="157"/>
-      <c r="BR8" s="157"/>
-      <c r="BS8" s="157"/>
-      <c r="BT8" s="158"/>
+      <c r="BQ8" s="167"/>
+      <c r="BR8" s="167"/>
+      <c r="BS8" s="167"/>
+      <c r="BT8" s="170"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="165"/>
-      <c r="C9" s="167"/>
-      <c r="D9" s="169"/>
+      <c r="B9" s="183"/>
+      <c r="C9" s="185"/>
+      <c r="D9" s="187"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12654,11 +12665,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="174"/>
-      <c r="I9" s="179"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="184"/>
+      <c r="H9" s="192"/>
+      <c r="I9" s="160"/>
+      <c r="J9" s="162"/>
+      <c r="K9" s="162"/>
+      <c r="L9" s="165"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -12860,7 +12871,9 @@
         <f>SUM(G11:G16)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="45"/>
+      <c r="H10" s="45">
+        <v>1</v>
+      </c>
       <c r="I10" s="46"/>
       <c r="J10" s="47"/>
       <c r="K10" s="48"/>
@@ -12936,7 +12949,9 @@
       <c r="C11" s="54" t="s">
         <v>198</v>
       </c>
-      <c r="D11" s="55"/>
+      <c r="D11" s="55" t="s">
+        <v>208</v>
+      </c>
       <c r="E11" s="56">
         <v>4</v>
       </c>
@@ -12947,7 +12962,9 @@
         <f t="shared" ref="G11:G16" si="1">E11-F11</f>
         <v>0</v>
       </c>
-      <c r="H11" s="59"/>
+      <c r="H11" s="59">
+        <v>1</v>
+      </c>
       <c r="I11" s="60">
         <v>45355</v>
       </c>
@@ -13030,7 +13047,9 @@
       <c r="C12" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="55"/>
+      <c r="D12" s="55" t="s">
+        <v>208</v>
+      </c>
       <c r="E12" s="56">
         <v>3</v>
       </c>
@@ -13041,7 +13060,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12" s="59"/>
+      <c r="H12" s="59">
+        <v>1</v>
+      </c>
       <c r="I12" s="60">
         <v>45357</v>
       </c>
@@ -13124,7 +13145,9 @@
       <c r="C13" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="55"/>
+      <c r="D13" s="55" t="s">
+        <v>208</v>
+      </c>
       <c r="E13" s="56">
         <v>5</v>
       </c>
@@ -13135,7 +13158,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H13" s="59"/>
+      <c r="H13" s="59">
+        <v>1</v>
+      </c>
       <c r="I13" s="60">
         <v>45364</v>
       </c>
@@ -13218,7 +13243,9 @@
       <c r="C14" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="D14" s="55"/>
+      <c r="D14" s="55" t="s">
+        <v>208</v>
+      </c>
       <c r="E14" s="56">
         <v>1</v>
       </c>
@@ -13229,7 +13256,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="59"/>
+      <c r="H14" s="59">
+        <v>1</v>
+      </c>
       <c r="I14" s="60">
         <v>45365</v>
       </c>
@@ -13312,7 +13341,9 @@
       <c r="C15" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="D15" s="55"/>
+      <c r="D15" s="55" t="s">
+        <v>208</v>
+      </c>
       <c r="E15" s="56">
         <v>1</v>
       </c>
@@ -13323,7 +13354,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15" s="59"/>
+      <c r="H15" s="59">
+        <v>1</v>
+      </c>
       <c r="I15" s="60">
         <v>45371</v>
       </c>
@@ -13406,7 +13439,9 @@
       <c r="C16" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="D16" s="55"/>
+      <c r="D16" s="55" t="s">
+        <v>208</v>
+      </c>
       <c r="E16" s="56">
         <v>1</v>
       </c>
@@ -13417,7 +13452,9 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="H16" s="59"/>
+      <c r="H16" s="59">
+        <v>1</v>
+      </c>
       <c r="I16" s="60">
         <v>45373</v>
       </c>
@@ -13497,27 +13534,31 @@
       <c r="B17" s="53">
         <v>2</v>
       </c>
-      <c r="C17" s="73"/>
+      <c r="C17" s="73" t="s">
+        <v>206</v>
+      </c>
       <c r="D17" s="74"/>
       <c r="E17" s="42">
         <f t="shared" ref="E17:G17" si="3">SUM(E18:E21)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17" s="43">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="44">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H17" s="75"/>
+      <c r="H17" s="75">
+        <v>2</v>
+      </c>
       <c r="I17" s="76"/>
       <c r="J17" s="77"/>
       <c r="K17" s="77"/>
-      <c r="L17" s="49" t="e">
+      <c r="L17" s="49">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M17" s="50"/>
       <c r="N17" s="51"/>
@@ -13584,24 +13625,38 @@
       <c r="B18" s="53">
         <v>2.1</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="57"/>
+      <c r="C18" s="54" t="s">
+        <v>207</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" s="56">
+        <v>2</v>
+      </c>
+      <c r="F18" s="57">
+        <v>2</v>
+      </c>
       <c r="G18" s="58">
         <f t="shared" ref="G18:G21" si="4">E18-F18</f>
         <v>0</v>
       </c>
-      <c r="H18" s="59"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="61"/>
+      <c r="H18" s="59">
+        <v>2</v>
+      </c>
+      <c r="I18" s="60">
+        <v>45376</v>
+      </c>
+      <c r="J18" s="61">
+        <v>45376</v>
+      </c>
       <c r="K18" s="62">
         <f t="shared" ref="K18:K21" si="5">J18-I18+1</f>
         <v>1</v>
       </c>
-      <c r="L18" s="63" t="e">
+      <c r="L18" s="63">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M18" s="64"/>
       <c r="N18" s="65"/>
@@ -14956,11 +15011,11 @@
       </c>
       <c r="E35" s="101">
         <f>SUM(E11:E16,E18:E21,E23:E28,E30:E33)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F35" s="101">
         <f>SUM(F11:F16,F18:F21,F23:F28,F30:F33)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G35" s="101">
         <f>SUM(G11:G16,G18:G21,G23:G28,G30:G33)</f>
@@ -14971,7 +15026,7 @@
       </c>
       <c r="I35" s="101">
         <f>E35/H35</f>
-        <v>0.25</v>
+        <v>0.28333333333333333</v>
       </c>
       <c r="L35" s="102" t="s">
         <v>77</v>
@@ -15169,243 +15224,243 @@
       </c>
       <c r="M36" s="105">
         <f>E35</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N36" s="106">
         <f>M36-I35</f>
-        <v>14.75</v>
+        <v>16.716666666666665</v>
       </c>
       <c r="O36" s="106">
         <f>N36-I35</f>
-        <v>14.5</v>
+        <v>16.43333333333333</v>
       </c>
       <c r="P36" s="106">
         <f>O36-I35</f>
-        <v>14.25</v>
+        <v>16.149999999999995</v>
       </c>
       <c r="Q36" s="106">
         <f>P36-I35</f>
-        <v>14</v>
+        <v>15.866666666666662</v>
       </c>
       <c r="R36" s="106">
         <f>Q36-I35</f>
-        <v>13.75</v>
+        <v>15.583333333333329</v>
       </c>
       <c r="S36" s="106">
         <f>R36-I35</f>
-        <v>13.5</v>
+        <v>15.299999999999995</v>
       </c>
       <c r="T36" s="106">
         <f>S36-I35</f>
-        <v>13.25</v>
+        <v>15.016666666666662</v>
       </c>
       <c r="U36" s="106">
         <f>T36-I35</f>
-        <v>13</v>
+        <v>14.733333333333329</v>
       </c>
       <c r="V36" s="106">
         <f>U36-I35</f>
-        <v>12.75</v>
+        <v>14.449999999999996</v>
       </c>
       <c r="W36" s="106">
         <f>V36-I35</f>
-        <v>12.5</v>
+        <v>14.166666666666663</v>
       </c>
       <c r="X36" s="106">
         <f>W36-I35</f>
-        <v>12.25</v>
+        <v>13.883333333333329</v>
       </c>
       <c r="Y36" s="106">
         <f>X36-I35</f>
-        <v>12</v>
+        <v>13.599999999999996</v>
       </c>
       <c r="Z36" s="106">
         <f>Y36-I35</f>
-        <v>11.75</v>
+        <v>13.316666666666663</v>
       </c>
       <c r="AA36" s="106">
         <f>Z36-I35</f>
-        <v>11.5</v>
+        <v>13.03333333333333</v>
       </c>
       <c r="AB36" s="106">
         <f>AA36-I35</f>
-        <v>11.25</v>
+        <v>12.749999999999996</v>
       </c>
       <c r="AC36" s="106">
         <f>AB36-I35</f>
-        <v>11</v>
+        <v>12.466666666666663</v>
       </c>
       <c r="AD36" s="106">
         <f>AC36-I35</f>
-        <v>10.75</v>
+        <v>12.18333333333333</v>
       </c>
       <c r="AE36" s="106">
         <f>AD36-I35</f>
-        <v>10.5</v>
+        <v>11.899999999999997</v>
       </c>
       <c r="AF36" s="106">
         <f>AE36-I35</f>
-        <v>10.25</v>
+        <v>11.616666666666664</v>
       </c>
       <c r="AG36" s="106">
         <f>AF36-I35</f>
-        <v>10</v>
+        <v>11.33333333333333</v>
       </c>
       <c r="AH36" s="106">
         <f>AG36-I35</f>
-        <v>9.75</v>
+        <v>11.049999999999997</v>
       </c>
       <c r="AI36" s="106">
         <f>AH36-I35</f>
-        <v>9.5</v>
+        <v>10.766666666666664</v>
       </c>
       <c r="AJ36" s="106">
         <f>AI36-I35</f>
-        <v>9.25</v>
+        <v>10.483333333333331</v>
       </c>
       <c r="AK36" s="106">
         <f>AJ36-I35</f>
-        <v>9</v>
+        <v>10.199999999999998</v>
       </c>
       <c r="AL36" s="106">
         <f>AK36-I35</f>
-        <v>8.75</v>
+        <v>9.9166666666666643</v>
       </c>
       <c r="AM36" s="106">
         <f>AL36-I35</f>
-        <v>8.5</v>
+        <v>9.6333333333333311</v>
       </c>
       <c r="AN36" s="106">
         <f>AM36-I35</f>
-        <v>8.25</v>
+        <v>9.3499999999999979</v>
       </c>
       <c r="AO36" s="106">
         <f>AN36-I35</f>
-        <v>8</v>
+        <v>9.0666666666666647</v>
       </c>
       <c r="AP36" s="106">
         <f>AO36-I35</f>
-        <v>7.75</v>
+        <v>8.7833333333333314</v>
       </c>
       <c r="AQ36" s="106">
         <f>AP36-I35</f>
-        <v>7.5</v>
+        <v>8.4999999999999982</v>
       </c>
       <c r="AR36" s="106">
         <f>AQ36-I35</f>
-        <v>7.25</v>
+        <v>8.216666666666665</v>
       </c>
       <c r="AS36" s="106">
         <f>AR36-I35</f>
-        <v>7</v>
+        <v>7.9333333333333318</v>
       </c>
       <c r="AT36" s="106">
         <f>AS36-I35</f>
-        <v>6.75</v>
+        <v>7.6499999999999986</v>
       </c>
       <c r="AU36" s="106">
         <f>AT36-I35</f>
-        <v>6.5</v>
+        <v>7.3666666666666654</v>
       </c>
       <c r="AV36" s="106">
         <f>AU36-I35</f>
-        <v>6.25</v>
+        <v>7.0833333333333321</v>
       </c>
       <c r="AW36" s="106">
         <f>AV36-I35</f>
-        <v>6</v>
+        <v>6.7999999999999989</v>
       </c>
       <c r="AX36" s="106">
         <f>AW36-I35</f>
-        <v>5.75</v>
+        <v>6.5166666666666657</v>
       </c>
       <c r="AY36" s="106">
         <f>AX36-I35</f>
-        <v>5.5</v>
+        <v>6.2333333333333325</v>
       </c>
       <c r="AZ36" s="106">
         <f>AY36-I35</f>
-        <v>5.25</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="BA36" s="106">
         <f>AZ36-I35</f>
-        <v>5</v>
+        <v>5.6666666666666661</v>
       </c>
       <c r="BB36" s="106">
         <f>BA36-I35</f>
-        <v>4.75</v>
+        <v>5.3833333333333329</v>
       </c>
       <c r="BC36" s="106">
         <f>BB36-I35</f>
-        <v>4.5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="BD36" s="106">
         <f>BC36-I35</f>
-        <v>4.25</v>
+        <v>4.8166666666666664</v>
       </c>
       <c r="BE36" s="106">
         <f>BD36-I35</f>
-        <v>4</v>
+        <v>4.5333333333333332</v>
       </c>
       <c r="BF36" s="106">
         <f>BE36-I35</f>
-        <v>3.75</v>
+        <v>4.25</v>
       </c>
       <c r="BG36" s="106">
         <f>BF36-I35</f>
-        <v>3.5</v>
+        <v>3.9666666666666668</v>
       </c>
       <c r="BH36" s="106">
         <f>BG36-I35</f>
-        <v>3.25</v>
+        <v>3.6833333333333336</v>
       </c>
       <c r="BI36" s="106">
         <f>BH36-I35</f>
-        <v>3</v>
+        <v>3.4000000000000004</v>
       </c>
       <c r="BJ36" s="106">
         <f>BI36-I35</f>
-        <v>2.75</v>
+        <v>3.1166666666666671</v>
       </c>
       <c r="BK36" s="106">
         <f>BJ36-I35</f>
-        <v>2.5</v>
+        <v>2.8333333333333339</v>
       </c>
       <c r="BL36" s="106">
         <f>BK36-I35</f>
-        <v>2.25</v>
+        <v>2.5500000000000007</v>
       </c>
       <c r="BM36" s="106">
         <f>BL36-I35</f>
-        <v>2</v>
+        <v>2.2666666666666675</v>
       </c>
       <c r="BN36" s="106">
         <f>BM36-I35</f>
-        <v>1.75</v>
+        <v>1.9833333333333343</v>
       </c>
       <c r="BO36" s="106">
         <f>BN36-I35</f>
-        <v>1.5</v>
+        <v>1.7000000000000011</v>
       </c>
       <c r="BP36" s="106">
         <f>BO36-I35</f>
-        <v>1.25</v>
+        <v>1.4166666666666679</v>
       </c>
       <c r="BQ36" s="106">
         <f>BP36-I35</f>
-        <v>1</v>
+        <v>1.1333333333333346</v>
       </c>
       <c r="BR36" s="106">
         <f>BQ36-I35</f>
-        <v>0.75</v>
+        <v>0.85000000000000131</v>
       </c>
       <c r="BS36" s="106">
         <f>BR36-I35</f>
-        <v>0.5</v>
+        <v>0.56666666666666798</v>
       </c>
       <c r="BT36" s="106">
         <f>BS36-I35</f>
-        <v>0.25</v>
+        <v>0.28333333333333466</v>
       </c>
       <c r="BV36" s="101"/>
     </row>
@@ -15415,247 +15470,247 @@
       </c>
       <c r="M37" s="105">
         <f>E35</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N37" s="105">
         <f t="shared" ref="N37:BT37" si="12">M39</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="R37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="S37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="T37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="U37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="V37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="W37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="X37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Y37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Z37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AA37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AB37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AC37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AD37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AE37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AF37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AG37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AH37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AI37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AJ37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AK37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AL37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AM37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AN37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AO37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AP37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AQ37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AR37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AS37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AT37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AU37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AV37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AW37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AX37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AY37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AZ37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BA37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BB37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BC37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BD37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BE37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BF37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BG37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BH37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BI37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BJ37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BK37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BL37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BM37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BN37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BO37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BP37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BQ37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BR37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BS37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BT37" s="105">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BV37" s="101">
         <f t="shared" ref="BV37:BV39" si="13">SUM(M37:BT37)</f>
-        <v>900</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="38" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -15736,247 +15791,247 @@
       </c>
       <c r="M39" s="105">
         <f t="shared" ref="M39:BT39" si="14">M37-M38</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="R39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="S39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="T39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="U39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="V39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="W39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="X39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Y39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Z39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AA39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AB39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AC39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AD39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AE39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AF39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AG39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AH39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AI39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AJ39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AK39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AL39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AM39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AN39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AO39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AP39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AQ39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AR39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AS39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AT39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AU39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AV39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AW39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AX39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AY39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AZ39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BA39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BB39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BC39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BD39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BE39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BF39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BG39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BH39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BI39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BJ39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BK39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BL39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BM39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BN39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BO39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BP39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BQ39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BR39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BS39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BT39" s="105">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="BV39" s="101">
         <f t="shared" si="13"/>
-        <v>900</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="40" spans="2:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -15986,55 +16041,55 @@
       <c r="E43" s="193" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="176"/>
-      <c r="G43" s="176"/>
-      <c r="H43" s="176"/>
-      <c r="I43" s="176"/>
-      <c r="J43" s="176"/>
-      <c r="K43" s="176"/>
-      <c r="L43" s="176"/>
-      <c r="M43" s="176"/>
-      <c r="N43" s="176"/>
-      <c r="O43" s="176"/>
-      <c r="P43" s="176"/>
-      <c r="Q43" s="176"/>
-      <c r="R43" s="176"/>
-      <c r="S43" s="176"/>
-      <c r="T43" s="176"/>
-      <c r="U43" s="176"/>
-      <c r="V43" s="176"/>
-      <c r="W43" s="176"/>
-      <c r="X43" s="176"/>
-      <c r="Y43" s="176"/>
-      <c r="Z43" s="176"/>
-      <c r="AA43" s="176"/>
-      <c r="AB43" s="176"/>
-      <c r="AC43" s="176"/>
-      <c r="AD43" s="176"/>
-      <c r="AE43" s="176"/>
-      <c r="AF43" s="176"/>
-      <c r="AG43" s="176"/>
-      <c r="AH43" s="176"/>
-      <c r="AI43" s="176"/>
-      <c r="AJ43" s="176"/>
-      <c r="AK43" s="176"/>
-      <c r="AL43" s="176"/>
-      <c r="AM43" s="176"/>
-      <c r="AN43" s="176"/>
-      <c r="AO43" s="176"/>
-      <c r="AP43" s="176"/>
-      <c r="AQ43" s="176"/>
-      <c r="AR43" s="176"/>
-      <c r="AS43" s="176"/>
-      <c r="AT43" s="176"/>
-      <c r="AU43" s="176"/>
-      <c r="AV43" s="176"/>
-      <c r="AW43" s="176"/>
-      <c r="AX43" s="176"/>
-      <c r="AY43" s="176"/>
-      <c r="AZ43" s="176"/>
-      <c r="BA43" s="176"/>
-      <c r="BB43" s="177"/>
+      <c r="F43" s="157"/>
+      <c r="G43" s="157"/>
+      <c r="H43" s="157"/>
+      <c r="I43" s="157"/>
+      <c r="J43" s="157"/>
+      <c r="K43" s="157"/>
+      <c r="L43" s="157"/>
+      <c r="M43" s="157"/>
+      <c r="N43" s="157"/>
+      <c r="O43" s="157"/>
+      <c r="P43" s="157"/>
+      <c r="Q43" s="157"/>
+      <c r="R43" s="157"/>
+      <c r="S43" s="157"/>
+      <c r="T43" s="157"/>
+      <c r="U43" s="157"/>
+      <c r="V43" s="157"/>
+      <c r="W43" s="157"/>
+      <c r="X43" s="157"/>
+      <c r="Y43" s="157"/>
+      <c r="Z43" s="157"/>
+      <c r="AA43" s="157"/>
+      <c r="AB43" s="157"/>
+      <c r="AC43" s="157"/>
+      <c r="AD43" s="157"/>
+      <c r="AE43" s="157"/>
+      <c r="AF43" s="157"/>
+      <c r="AG43" s="157"/>
+      <c r="AH43" s="157"/>
+      <c r="AI43" s="157"/>
+      <c r="AJ43" s="157"/>
+      <c r="AK43" s="157"/>
+      <c r="AL43" s="157"/>
+      <c r="AM43" s="157"/>
+      <c r="AN43" s="157"/>
+      <c r="AO43" s="157"/>
+      <c r="AP43" s="157"/>
+      <c r="AQ43" s="157"/>
+      <c r="AR43" s="157"/>
+      <c r="AS43" s="157"/>
+      <c r="AT43" s="157"/>
+      <c r="AU43" s="157"/>
+      <c r="AV43" s="157"/>
+      <c r="AW43" s="157"/>
+      <c r="AX43" s="157"/>
+      <c r="AY43" s="157"/>
+      <c r="AZ43" s="157"/>
+      <c r="BA43" s="157"/>
+      <c r="BB43" s="158"/>
     </row>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16997,6 +17052,13 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
     <mergeCell ref="E43:BB43"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
@@ -17013,13 +17075,6 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17034,7 +17089,7 @@
   </sheetPr>
   <dimension ref="B1:K999"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Database within docker container
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e15298e05a6af3ae/Università/Magistrale/LabAdvProg/Proj/AnimalDEX/AnimalDex/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleca\Desktop\Main\University\Lab_AP\Progetto\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_57CD38E8F67BBE9C6E672C671D70A5B181D681E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F9AD944-EE64-4663-9B7D-F5A2ED2A6C38}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630AD4A4-20AE-45EC-B611-02DF1B718EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="215">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -678,13 +678,16 @@
   </si>
   <si>
     <t>First drafting of certification service</t>
+  </si>
+  <si>
+    <t>Database within the docker container</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -831,6 +834,13 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="28">
@@ -1986,7 +1996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2373,11 +2383,53 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2408,51 +2460,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -5354,184 +5365,184 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.583333333333332</c:v>
+                  <c:v>28.516666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.166666666666664</c:v>
+                  <c:v>28.033333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.749999999999996</c:v>
+                  <c:v>27.549999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.333333333333329</c:v>
+                  <c:v>27.066666666666663</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.916666666666661</c:v>
+                  <c:v>26.583333333333329</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.499999999999993</c:v>
+                  <c:v>26.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.083333333333325</c:v>
+                  <c:v>25.61666666666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.666666666666657</c:v>
+                  <c:v>25.133333333333326</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.249999999999989</c:v>
+                  <c:v>24.649999999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.833333333333321</c:v>
+                  <c:v>24.166666666666657</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.416666666666654</c:v>
+                  <c:v>23.683333333333323</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.999999999999986</c:v>
+                  <c:v>23.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.583333333333318</c:v>
+                  <c:v>22.716666666666654</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19.16666666666665</c:v>
+                  <c:v>22.23333333333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.749999999999982</c:v>
+                  <c:v>21.749999999999986</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18.333333333333314</c:v>
+                  <c:v>21.266666666666652</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.916666666666647</c:v>
+                  <c:v>20.783333333333317</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.499999999999979</c:v>
+                  <c:v>20.299999999999983</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.083333333333311</c:v>
+                  <c:v>19.816666666666649</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16.666666666666643</c:v>
+                  <c:v>19.333333333333314</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>16.249999999999975</c:v>
+                  <c:v>18.84999999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>15.833333333333309</c:v>
+                  <c:v>18.366666666666646</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15.416666666666643</c:v>
+                  <c:v>17.883333333333312</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>14.999999999999977</c:v>
+                  <c:v>17.399999999999977</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14.583333333333311</c:v>
+                  <c:v>16.916666666666643</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>14.166666666666645</c:v>
+                  <c:v>16.433333333333309</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13.749999999999979</c:v>
+                  <c:v>15.949999999999976</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13.333333333333313</c:v>
+                  <c:v>15.466666666666644</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>12.916666666666647</c:v>
+                  <c:v>14.983333333333311</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>12.49999999999998</c:v>
+                  <c:v>14.499999999999979</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12.083333333333314</c:v>
+                  <c:v>14.016666666666646</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11.666666666666648</c:v>
+                  <c:v>13.533333333333314</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>11.249999999999982</c:v>
+                  <c:v>13.049999999999981</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>10.833333333333316</c:v>
+                  <c:v>12.566666666666649</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>10.41666666666665</c:v>
+                  <c:v>12.083333333333316</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.999999999999984</c:v>
+                  <c:v>11.599999999999984</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9.5833333333333179</c:v>
+                  <c:v>11.116666666666651</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.1666666666666519</c:v>
+                  <c:v>10.633333333333319</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.7499999999999858</c:v>
+                  <c:v>10.149999999999986</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8.3333333333333197</c:v>
+                  <c:v>9.6666666666666536</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>7.9166666666666528</c:v>
+                  <c:v>9.1833333333333211</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7.4999999999999858</c:v>
+                  <c:v>8.6999999999999886</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7.0833333333333188</c:v>
+                  <c:v>8.2166666666666561</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6.6666666666666519</c:v>
+                  <c:v>7.7333333333333227</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6.2499999999999849</c:v>
+                  <c:v>7.2499999999999893</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.8333333333333179</c:v>
+                  <c:v>6.7666666666666559</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5.416666666666651</c:v>
+                  <c:v>6.2833333333333226</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.999999999999984</c:v>
+                  <c:v>5.7999999999999892</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.5833333333333171</c:v>
+                  <c:v>5.3166666666666558</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4.1666666666666501</c:v>
+                  <c:v>4.8333333333333224</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.7499999999999836</c:v>
+                  <c:v>4.349999999999989</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.3333333333333171</c:v>
+                  <c:v>3.8666666666666556</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.9166666666666505</c:v>
+                  <c:v>3.3833333333333222</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.499999999999984</c:v>
+                  <c:v>2.8999999999999888</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.0833333333333175</c:v>
+                  <c:v>2.4166666666666554</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.6666666666666508</c:v>
+                  <c:v>1.933333333333322</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.249999999999984</c:v>
+                  <c:v>1.4499999999999886</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.83333333333331727</c:v>
+                  <c:v>0.96666666666665524</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.41666666666665059</c:v>
+                  <c:v>0.4833333333333219</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5765,184 +5776,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>25</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6366,10 +6377,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella2" displayName="Tabella2" ref="B2:G42" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="B2:G42" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
@@ -6851,19 +6858,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="159" t="str">
+      <c r="BK2" s="177" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="160"/>
-      <c r="BM2" s="160"/>
-      <c r="BN2" s="160"/>
-      <c r="BO2" s="160"/>
-      <c r="BP2" s="160"/>
-      <c r="BQ2" s="160"/>
-      <c r="BR2" s="160"/>
-      <c r="BS2" s="160"/>
-      <c r="BT2" s="160"/>
+      <c r="BL2" s="178"/>
+      <c r="BM2" s="178"/>
+      <c r="BN2" s="178"/>
+      <c r="BO2" s="178"/>
+      <c r="BP2" s="178"/>
+      <c r="BQ2" s="178"/>
+      <c r="BR2" s="178"/>
+      <c r="BS2" s="178"/>
+      <c r="BT2" s="178"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -6891,7 +6898,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="161" t="s">
+      <c r="K4" s="179" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -6968,7 +6975,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="162"/>
+      <c r="K5" s="180"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7043,7 +7050,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="162"/>
+      <c r="K6" s="180"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7118,7 +7125,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="162"/>
+      <c r="K7" s="180"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7193,7 +7200,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="163"/>
+      <c r="K8" s="181"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7259,124 +7266,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="164" t="s">
+      <c r="B9" s="182" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="166" t="s">
+      <c r="C9" s="184" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="168" t="s">
+      <c r="D9" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="170" t="s">
+      <c r="E9" s="188" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="171"/>
-      <c r="G9" s="172"/>
-      <c r="H9" s="173" t="s">
+      <c r="F9" s="189"/>
+      <c r="G9" s="190"/>
+      <c r="H9" s="191" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="178" t="s">
+      <c r="I9" s="159" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="180" t="s">
+      <c r="J9" s="161" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="182" t="s">
+      <c r="K9" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="183" t="s">
+      <c r="L9" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="185" t="s">
+      <c r="M9" s="166" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="157"/>
-      <c r="O9" s="157"/>
-      <c r="P9" s="157"/>
-      <c r="Q9" s="186"/>
-      <c r="R9" s="187" t="s">
+      <c r="N9" s="167"/>
+      <c r="O9" s="167"/>
+      <c r="P9" s="167"/>
+      <c r="Q9" s="168"/>
+      <c r="R9" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="157"/>
-      <c r="T9" s="157"/>
-      <c r="U9" s="157"/>
-      <c r="V9" s="186"/>
-      <c r="W9" s="187" t="s">
+      <c r="S9" s="167"/>
+      <c r="T9" s="167"/>
+      <c r="U9" s="167"/>
+      <c r="V9" s="168"/>
+      <c r="W9" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="157"/>
-      <c r="Y9" s="157"/>
-      <c r="Z9" s="157"/>
-      <c r="AA9" s="158"/>
-      <c r="AB9" s="188" t="s">
+      <c r="X9" s="167"/>
+      <c r="Y9" s="167"/>
+      <c r="Z9" s="167"/>
+      <c r="AA9" s="170"/>
+      <c r="AB9" s="171" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="157"/>
-      <c r="AD9" s="157"/>
-      <c r="AE9" s="157"/>
-      <c r="AF9" s="186"/>
-      <c r="AG9" s="189" t="s">
+      <c r="AC9" s="167"/>
+      <c r="AD9" s="167"/>
+      <c r="AE9" s="167"/>
+      <c r="AF9" s="168"/>
+      <c r="AG9" s="172" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="157"/>
-      <c r="AI9" s="157"/>
-      <c r="AJ9" s="157"/>
-      <c r="AK9" s="186"/>
-      <c r="AL9" s="189" t="s">
+      <c r="AH9" s="167"/>
+      <c r="AI9" s="167"/>
+      <c r="AJ9" s="167"/>
+      <c r="AK9" s="168"/>
+      <c r="AL9" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="157"/>
-      <c r="AN9" s="157"/>
-      <c r="AO9" s="157"/>
-      <c r="AP9" s="158"/>
-      <c r="AQ9" s="190" t="s">
+      <c r="AM9" s="167"/>
+      <c r="AN9" s="167"/>
+      <c r="AO9" s="167"/>
+      <c r="AP9" s="170"/>
+      <c r="AQ9" s="173" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="157"/>
-      <c r="AS9" s="157"/>
-      <c r="AT9" s="157"/>
-      <c r="AU9" s="186"/>
-      <c r="AV9" s="191" t="s">
+      <c r="AR9" s="167"/>
+      <c r="AS9" s="167"/>
+      <c r="AT9" s="167"/>
+      <c r="AU9" s="168"/>
+      <c r="AV9" s="174" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="157"/>
-      <c r="AX9" s="157"/>
-      <c r="AY9" s="157"/>
-      <c r="AZ9" s="186"/>
-      <c r="BA9" s="191" t="s">
+      <c r="AW9" s="167"/>
+      <c r="AX9" s="167"/>
+      <c r="AY9" s="167"/>
+      <c r="AZ9" s="168"/>
+      <c r="BA9" s="174" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="157"/>
-      <c r="BC9" s="157"/>
-      <c r="BD9" s="157"/>
-      <c r="BE9" s="158"/>
-      <c r="BF9" s="192" t="s">
+      <c r="BB9" s="167"/>
+      <c r="BC9" s="167"/>
+      <c r="BD9" s="167"/>
+      <c r="BE9" s="170"/>
+      <c r="BF9" s="175" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="157"/>
-      <c r="BH9" s="157"/>
-      <c r="BI9" s="157"/>
-      <c r="BJ9" s="186"/>
-      <c r="BK9" s="156" t="s">
+      <c r="BG9" s="167"/>
+      <c r="BH9" s="167"/>
+      <c r="BI9" s="167"/>
+      <c r="BJ9" s="168"/>
+      <c r="BK9" s="176" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="157"/>
-      <c r="BM9" s="157"/>
-      <c r="BN9" s="157"/>
-      <c r="BO9" s="186"/>
-      <c r="BP9" s="156" t="s">
+      <c r="BL9" s="167"/>
+      <c r="BM9" s="167"/>
+      <c r="BN9" s="167"/>
+      <c r="BO9" s="168"/>
+      <c r="BP9" s="176" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="157"/>
-      <c r="BR9" s="157"/>
-      <c r="BS9" s="157"/>
-      <c r="BT9" s="158"/>
+      <c r="BQ9" s="167"/>
+      <c r="BR9" s="167"/>
+      <c r="BS9" s="167"/>
+      <c r="BT9" s="170"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="165"/>
-      <c r="C10" s="167"/>
-      <c r="D10" s="169"/>
+      <c r="B10" s="183"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="187"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7386,11 +7393,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="174"/>
-      <c r="I10" s="179"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="184"/>
+      <c r="H10" s="192"/>
+      <c r="I10" s="160"/>
+      <c r="J10" s="162"/>
+      <c r="K10" s="162"/>
+      <c r="L10" s="165"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -10999,80 +11006,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="175" t="str">
+      <c r="B45" s="156" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="176"/>
-      <c r="D45" s="176"/>
-      <c r="E45" s="176"/>
-      <c r="F45" s="176"/>
-      <c r="G45" s="176"/>
-      <c r="H45" s="176"/>
-      <c r="I45" s="176"/>
-      <c r="J45" s="176"/>
-      <c r="K45" s="176"/>
-      <c r="L45" s="176"/>
-      <c r="M45" s="176"/>
-      <c r="N45" s="176"/>
-      <c r="O45" s="176"/>
-      <c r="P45" s="176"/>
-      <c r="Q45" s="176"/>
-      <c r="R45" s="176"/>
-      <c r="S45" s="176"/>
-      <c r="T45" s="176"/>
-      <c r="U45" s="176"/>
-      <c r="V45" s="176"/>
-      <c r="W45" s="176"/>
-      <c r="X45" s="176"/>
-      <c r="Y45" s="176"/>
-      <c r="Z45" s="176"/>
-      <c r="AA45" s="176"/>
-      <c r="AB45" s="176"/>
-      <c r="AC45" s="176"/>
-      <c r="AD45" s="176"/>
-      <c r="AE45" s="176"/>
-      <c r="AF45" s="176"/>
-      <c r="AG45" s="176"/>
-      <c r="AH45" s="176"/>
-      <c r="AI45" s="176"/>
-      <c r="AJ45" s="176"/>
-      <c r="AK45" s="176"/>
-      <c r="AL45" s="176"/>
-      <c r="AM45" s="176"/>
-      <c r="AN45" s="176"/>
-      <c r="AO45" s="176"/>
-      <c r="AP45" s="176"/>
-      <c r="AQ45" s="176"/>
-      <c r="AR45" s="176"/>
-      <c r="AS45" s="176"/>
-      <c r="AT45" s="176"/>
-      <c r="AU45" s="176"/>
-      <c r="AV45" s="176"/>
-      <c r="AW45" s="176"/>
-      <c r="AX45" s="176"/>
-      <c r="AY45" s="176"/>
-      <c r="AZ45" s="176"/>
-      <c r="BA45" s="176"/>
-      <c r="BB45" s="176"/>
-      <c r="BC45" s="176"/>
-      <c r="BD45" s="176"/>
-      <c r="BE45" s="176"/>
-      <c r="BF45" s="176"/>
-      <c r="BG45" s="176"/>
-      <c r="BH45" s="176"/>
-      <c r="BI45" s="176"/>
-      <c r="BJ45" s="176"/>
-      <c r="BK45" s="176"/>
-      <c r="BL45" s="176"/>
-      <c r="BM45" s="176"/>
-      <c r="BN45" s="176"/>
-      <c r="BO45" s="176"/>
-      <c r="BP45" s="176"/>
-      <c r="BQ45" s="176"/>
-      <c r="BR45" s="176"/>
-      <c r="BS45" s="176"/>
-      <c r="BT45" s="177"/>
+      <c r="C45" s="157"/>
+      <c r="D45" s="157"/>
+      <c r="E45" s="157"/>
+      <c r="F45" s="157"/>
+      <c r="G45" s="157"/>
+      <c r="H45" s="157"/>
+      <c r="I45" s="157"/>
+      <c r="J45" s="157"/>
+      <c r="K45" s="157"/>
+      <c r="L45" s="157"/>
+      <c r="M45" s="157"/>
+      <c r="N45" s="157"/>
+      <c r="O45" s="157"/>
+      <c r="P45" s="157"/>
+      <c r="Q45" s="157"/>
+      <c r="R45" s="157"/>
+      <c r="S45" s="157"/>
+      <c r="T45" s="157"/>
+      <c r="U45" s="157"/>
+      <c r="V45" s="157"/>
+      <c r="W45" s="157"/>
+      <c r="X45" s="157"/>
+      <c r="Y45" s="157"/>
+      <c r="Z45" s="157"/>
+      <c r="AA45" s="157"/>
+      <c r="AB45" s="157"/>
+      <c r="AC45" s="157"/>
+      <c r="AD45" s="157"/>
+      <c r="AE45" s="157"/>
+      <c r="AF45" s="157"/>
+      <c r="AG45" s="157"/>
+      <c r="AH45" s="157"/>
+      <c r="AI45" s="157"/>
+      <c r="AJ45" s="157"/>
+      <c r="AK45" s="157"/>
+      <c r="AL45" s="157"/>
+      <c r="AM45" s="157"/>
+      <c r="AN45" s="157"/>
+      <c r="AO45" s="157"/>
+      <c r="AP45" s="157"/>
+      <c r="AQ45" s="157"/>
+      <c r="AR45" s="157"/>
+      <c r="AS45" s="157"/>
+      <c r="AT45" s="157"/>
+      <c r="AU45" s="157"/>
+      <c r="AV45" s="157"/>
+      <c r="AW45" s="157"/>
+      <c r="AX45" s="157"/>
+      <c r="AY45" s="157"/>
+      <c r="AZ45" s="157"/>
+      <c r="BA45" s="157"/>
+      <c r="BB45" s="157"/>
+      <c r="BC45" s="157"/>
+      <c r="BD45" s="157"/>
+      <c r="BE45" s="157"/>
+      <c r="BF45" s="157"/>
+      <c r="BG45" s="157"/>
+      <c r="BH45" s="157"/>
+      <c r="BI45" s="157"/>
+      <c r="BJ45" s="157"/>
+      <c r="BK45" s="157"/>
+      <c r="BL45" s="157"/>
+      <c r="BM45" s="157"/>
+      <c r="BN45" s="157"/>
+      <c r="BO45" s="157"/>
+      <c r="BP45" s="157"/>
+      <c r="BQ45" s="157"/>
+      <c r="BR45" s="157"/>
+      <c r="BS45" s="157"/>
+      <c r="BT45" s="158"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12035,6 +12042,14 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12051,14 +12066,6 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12073,8 +12080,8 @@
   </sheetPr>
   <dimension ref="B1:BV999"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD21" sqref="AD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12187,7 +12194,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="161" t="s">
+      <c r="K3" s="179" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12264,7 +12271,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="162"/>
+      <c r="K4" s="180"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12338,7 +12345,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="162"/>
+      <c r="K5" s="180"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12413,7 +12420,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="162"/>
+      <c r="K6" s="180"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12488,7 +12495,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="163"/>
+      <c r="K7" s="181"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12554,124 +12561,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="164" t="s">
+      <c r="B8" s="182" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="166" t="s">
+      <c r="C8" s="184" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="168" t="s">
+      <c r="D8" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="170" t="s">
+      <c r="E8" s="188" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="171"/>
-      <c r="G8" s="172"/>
-      <c r="H8" s="173" t="s">
+      <c r="F8" s="189"/>
+      <c r="G8" s="190"/>
+      <c r="H8" s="191" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="178" t="s">
+      <c r="I8" s="159" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="180" t="s">
+      <c r="J8" s="161" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="182" t="s">
+      <c r="K8" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="183" t="s">
+      <c r="L8" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="185" t="s">
+      <c r="M8" s="166" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="157"/>
-      <c r="O8" s="157"/>
-      <c r="P8" s="157"/>
-      <c r="Q8" s="186"/>
-      <c r="R8" s="187" t="s">
+      <c r="N8" s="167"/>
+      <c r="O8" s="167"/>
+      <c r="P8" s="167"/>
+      <c r="Q8" s="168"/>
+      <c r="R8" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="157"/>
-      <c r="T8" s="157"/>
-      <c r="U8" s="157"/>
-      <c r="V8" s="186"/>
-      <c r="W8" s="187" t="s">
+      <c r="S8" s="167"/>
+      <c r="T8" s="167"/>
+      <c r="U8" s="167"/>
+      <c r="V8" s="168"/>
+      <c r="W8" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="157"/>
-      <c r="Y8" s="157"/>
-      <c r="Z8" s="157"/>
-      <c r="AA8" s="158"/>
-      <c r="AB8" s="188" t="s">
+      <c r="X8" s="167"/>
+      <c r="Y8" s="167"/>
+      <c r="Z8" s="167"/>
+      <c r="AA8" s="170"/>
+      <c r="AB8" s="171" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="157"/>
-      <c r="AD8" s="157"/>
-      <c r="AE8" s="157"/>
-      <c r="AF8" s="186"/>
-      <c r="AG8" s="189" t="s">
+      <c r="AC8" s="167"/>
+      <c r="AD8" s="167"/>
+      <c r="AE8" s="167"/>
+      <c r="AF8" s="168"/>
+      <c r="AG8" s="172" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="157"/>
-      <c r="AI8" s="157"/>
-      <c r="AJ8" s="157"/>
-      <c r="AK8" s="186"/>
-      <c r="AL8" s="189" t="s">
+      <c r="AH8" s="167"/>
+      <c r="AI8" s="167"/>
+      <c r="AJ8" s="167"/>
+      <c r="AK8" s="168"/>
+      <c r="AL8" s="172" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="157"/>
-      <c r="AN8" s="157"/>
-      <c r="AO8" s="157"/>
-      <c r="AP8" s="158"/>
-      <c r="AQ8" s="190" t="s">
+      <c r="AM8" s="167"/>
+      <c r="AN8" s="167"/>
+      <c r="AO8" s="167"/>
+      <c r="AP8" s="170"/>
+      <c r="AQ8" s="173" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="157"/>
-      <c r="AS8" s="157"/>
-      <c r="AT8" s="157"/>
-      <c r="AU8" s="186"/>
-      <c r="AV8" s="191" t="s">
+      <c r="AR8" s="167"/>
+      <c r="AS8" s="167"/>
+      <c r="AT8" s="167"/>
+      <c r="AU8" s="168"/>
+      <c r="AV8" s="174" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="157"/>
-      <c r="AX8" s="157"/>
-      <c r="AY8" s="157"/>
-      <c r="AZ8" s="186"/>
-      <c r="BA8" s="191" t="s">
+      <c r="AW8" s="167"/>
+      <c r="AX8" s="167"/>
+      <c r="AY8" s="167"/>
+      <c r="AZ8" s="168"/>
+      <c r="BA8" s="174" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="157"/>
-      <c r="BC8" s="157"/>
-      <c r="BD8" s="157"/>
-      <c r="BE8" s="158"/>
-      <c r="BF8" s="192" t="s">
+      <c r="BB8" s="167"/>
+      <c r="BC8" s="167"/>
+      <c r="BD8" s="167"/>
+      <c r="BE8" s="170"/>
+      <c r="BF8" s="175" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="157"/>
-      <c r="BH8" s="157"/>
-      <c r="BI8" s="157"/>
-      <c r="BJ8" s="186"/>
-      <c r="BK8" s="156" t="s">
+      <c r="BG8" s="167"/>
+      <c r="BH8" s="167"/>
+      <c r="BI8" s="167"/>
+      <c r="BJ8" s="168"/>
+      <c r="BK8" s="176" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="157"/>
-      <c r="BM8" s="157"/>
-      <c r="BN8" s="157"/>
-      <c r="BO8" s="186"/>
-      <c r="BP8" s="156" t="s">
+      <c r="BL8" s="167"/>
+      <c r="BM8" s="167"/>
+      <c r="BN8" s="167"/>
+      <c r="BO8" s="168"/>
+      <c r="BP8" s="176" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="157"/>
-      <c r="BR8" s="157"/>
-      <c r="BS8" s="157"/>
-      <c r="BT8" s="158"/>
+      <c r="BQ8" s="167"/>
+      <c r="BR8" s="167"/>
+      <c r="BS8" s="167"/>
+      <c r="BT8" s="170"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="165"/>
-      <c r="C9" s="167"/>
-      <c r="D9" s="169"/>
+      <c r="B9" s="183"/>
+      <c r="C9" s="185"/>
+      <c r="D9" s="187"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12681,11 +12688,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="174"/>
-      <c r="I9" s="179"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="184"/>
+      <c r="H9" s="192"/>
+      <c r="I9" s="160"/>
+      <c r="J9" s="162"/>
+      <c r="K9" s="162"/>
+      <c r="L9" s="165"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -13556,11 +13563,11 @@
       <c r="D17" s="74"/>
       <c r="E17" s="42">
         <f t="shared" ref="E17:G17" si="3">SUM(E18:E21)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F17" s="43">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G17" s="44">
         <f t="shared" si="3"/>
@@ -13935,24 +13942,38 @@
       <c r="B21" s="53">
         <v>2.4</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="57"/>
+      <c r="C21" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>209</v>
+      </c>
+      <c r="E21" s="56">
+        <v>4</v>
+      </c>
+      <c r="F21" s="57">
+        <v>4</v>
+      </c>
       <c r="G21" s="58">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H21" s="59"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="61"/>
+      <c r="H21" s="59">
+        <v>2</v>
+      </c>
+      <c r="I21" s="60">
+        <v>45378</v>
+      </c>
+      <c r="J21" s="61">
+        <v>45378</v>
+      </c>
       <c r="K21" s="62">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="L21" s="63" t="e">
+      <c r="L21" s="63">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M21" s="64"/>
       <c r="N21" s="65"/>
@@ -13971,7 +13992,7 @@
       <c r="AA21" s="68"/>
       <c r="AB21" s="64"/>
       <c r="AC21" s="65"/>
-      <c r="AD21" s="65"/>
+      <c r="AD21" s="194"/>
       <c r="AE21" s="65"/>
       <c r="AF21" s="65"/>
       <c r="AG21" s="69"/>
@@ -15055,11 +15076,11 @@
       </c>
       <c r="E35" s="101">
         <f>SUM(E11:E16,E18:E21,E23:E28,E30:E33)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F35" s="101">
         <f>SUM(F11:F16,F18:F21,F23:F28,F30:F33)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G35" s="101">
         <f>SUM(G11:G16,G18:G21,G23:G28,G30:G33)</f>
@@ -15070,7 +15091,7 @@
       </c>
       <c r="I35" s="101">
         <f>E35/H35</f>
-        <v>0.41666666666666669</v>
+        <v>0.48333333333333334</v>
       </c>
       <c r="L35" s="102" t="s">
         <v>77</v>
@@ -15268,243 +15289,243 @@
       </c>
       <c r="M36" s="105">
         <f>E35</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N36" s="106">
         <f>M36-I35</f>
-        <v>24.583333333333332</v>
+        <v>28.516666666666666</v>
       </c>
       <c r="O36" s="106">
         <f>N36-I35</f>
-        <v>24.166666666666664</v>
+        <v>28.033333333333331</v>
       </c>
       <c r="P36" s="106">
         <f>O36-I35</f>
-        <v>23.749999999999996</v>
+        <v>27.549999999999997</v>
       </c>
       <c r="Q36" s="106">
         <f>P36-I35</f>
-        <v>23.333333333333329</v>
+        <v>27.066666666666663</v>
       </c>
       <c r="R36" s="106">
         <f>Q36-I35</f>
-        <v>22.916666666666661</v>
+        <v>26.583333333333329</v>
       </c>
       <c r="S36" s="106">
         <f>R36-I35</f>
-        <v>22.499999999999993</v>
+        <v>26.099999999999994</v>
       </c>
       <c r="T36" s="106">
         <f>S36-I35</f>
-        <v>22.083333333333325</v>
+        <v>25.61666666666666</v>
       </c>
       <c r="U36" s="106">
         <f>T36-I35</f>
-        <v>21.666666666666657</v>
+        <v>25.133333333333326</v>
       </c>
       <c r="V36" s="106">
         <f>U36-I35</f>
-        <v>21.249999999999989</v>
+        <v>24.649999999999991</v>
       </c>
       <c r="W36" s="106">
         <f>V36-I35</f>
-        <v>20.833333333333321</v>
+        <v>24.166666666666657</v>
       </c>
       <c r="X36" s="106">
         <f>W36-I35</f>
-        <v>20.416666666666654</v>
+        <v>23.683333333333323</v>
       </c>
       <c r="Y36" s="106">
         <f>X36-I35</f>
-        <v>19.999999999999986</v>
+        <v>23.199999999999989</v>
       </c>
       <c r="Z36" s="106">
         <f>Y36-I35</f>
-        <v>19.583333333333318</v>
+        <v>22.716666666666654</v>
       </c>
       <c r="AA36" s="106">
         <f>Z36-I35</f>
-        <v>19.16666666666665</v>
+        <v>22.23333333333332</v>
       </c>
       <c r="AB36" s="106">
         <f>AA36-I35</f>
-        <v>18.749999999999982</v>
+        <v>21.749999999999986</v>
       </c>
       <c r="AC36" s="106">
         <f>AB36-I35</f>
-        <v>18.333333333333314</v>
+        <v>21.266666666666652</v>
       </c>
       <c r="AD36" s="106">
         <f>AC36-I35</f>
-        <v>17.916666666666647</v>
+        <v>20.783333333333317</v>
       </c>
       <c r="AE36" s="106">
         <f>AD36-I35</f>
-        <v>17.499999999999979</v>
+        <v>20.299999999999983</v>
       </c>
       <c r="AF36" s="106">
         <f>AE36-I35</f>
-        <v>17.083333333333311</v>
+        <v>19.816666666666649</v>
       </c>
       <c r="AG36" s="106">
         <f>AF36-I35</f>
-        <v>16.666666666666643</v>
+        <v>19.333333333333314</v>
       </c>
       <c r="AH36" s="106">
         <f>AG36-I35</f>
-        <v>16.249999999999975</v>
+        <v>18.84999999999998</v>
       </c>
       <c r="AI36" s="106">
         <f>AH36-I35</f>
-        <v>15.833333333333309</v>
+        <v>18.366666666666646</v>
       </c>
       <c r="AJ36" s="106">
         <f>AI36-I35</f>
-        <v>15.416666666666643</v>
+        <v>17.883333333333312</v>
       </c>
       <c r="AK36" s="106">
         <f>AJ36-I35</f>
-        <v>14.999999999999977</v>
+        <v>17.399999999999977</v>
       </c>
       <c r="AL36" s="106">
         <f>AK36-I35</f>
-        <v>14.583333333333311</v>
+        <v>16.916666666666643</v>
       </c>
       <c r="AM36" s="106">
         <f>AL36-I35</f>
-        <v>14.166666666666645</v>
+        <v>16.433333333333309</v>
       </c>
       <c r="AN36" s="106">
         <f>AM36-I35</f>
-        <v>13.749999999999979</v>
+        <v>15.949999999999976</v>
       </c>
       <c r="AO36" s="106">
         <f>AN36-I35</f>
-        <v>13.333333333333313</v>
+        <v>15.466666666666644</v>
       </c>
       <c r="AP36" s="106">
         <f>AO36-I35</f>
-        <v>12.916666666666647</v>
+        <v>14.983333333333311</v>
       </c>
       <c r="AQ36" s="106">
         <f>AP36-I35</f>
-        <v>12.49999999999998</v>
+        <v>14.499999999999979</v>
       </c>
       <c r="AR36" s="106">
         <f>AQ36-I35</f>
-        <v>12.083333333333314</v>
+        <v>14.016666666666646</v>
       </c>
       <c r="AS36" s="106">
         <f>AR36-I35</f>
-        <v>11.666666666666648</v>
+        <v>13.533333333333314</v>
       </c>
       <c r="AT36" s="106">
         <f>AS36-I35</f>
-        <v>11.249999999999982</v>
+        <v>13.049999999999981</v>
       </c>
       <c r="AU36" s="106">
         <f>AT36-I35</f>
-        <v>10.833333333333316</v>
+        <v>12.566666666666649</v>
       </c>
       <c r="AV36" s="106">
         <f>AU36-I35</f>
-        <v>10.41666666666665</v>
+        <v>12.083333333333316</v>
       </c>
       <c r="AW36" s="106">
         <f>AV36-I35</f>
-        <v>9.999999999999984</v>
+        <v>11.599999999999984</v>
       </c>
       <c r="AX36" s="106">
         <f>AW36-I35</f>
-        <v>9.5833333333333179</v>
+        <v>11.116666666666651</v>
       </c>
       <c r="AY36" s="106">
         <f>AX36-I35</f>
-        <v>9.1666666666666519</v>
+        <v>10.633333333333319</v>
       </c>
       <c r="AZ36" s="106">
         <f>AY36-I35</f>
-        <v>8.7499999999999858</v>
+        <v>10.149999999999986</v>
       </c>
       <c r="BA36" s="106">
         <f>AZ36-I35</f>
-        <v>8.3333333333333197</v>
+        <v>9.6666666666666536</v>
       </c>
       <c r="BB36" s="106">
         <f>BA36-I35</f>
-        <v>7.9166666666666528</v>
+        <v>9.1833333333333211</v>
       </c>
       <c r="BC36" s="106">
         <f>BB36-I35</f>
-        <v>7.4999999999999858</v>
+        <v>8.6999999999999886</v>
       </c>
       <c r="BD36" s="106">
         <f>BC36-I35</f>
-        <v>7.0833333333333188</v>
+        <v>8.2166666666666561</v>
       </c>
       <c r="BE36" s="106">
         <f>BD36-I35</f>
-        <v>6.6666666666666519</v>
+        <v>7.7333333333333227</v>
       </c>
       <c r="BF36" s="106">
         <f>BE36-I35</f>
-        <v>6.2499999999999849</v>
+        <v>7.2499999999999893</v>
       </c>
       <c r="BG36" s="106">
         <f>BF36-I35</f>
-        <v>5.8333333333333179</v>
+        <v>6.7666666666666559</v>
       </c>
       <c r="BH36" s="106">
         <f>BG36-I35</f>
-        <v>5.416666666666651</v>
+        <v>6.2833333333333226</v>
       </c>
       <c r="BI36" s="106">
         <f>BH36-I35</f>
-        <v>4.999999999999984</v>
+        <v>5.7999999999999892</v>
       </c>
       <c r="BJ36" s="106">
         <f>BI36-I35</f>
-        <v>4.5833333333333171</v>
+        <v>5.3166666666666558</v>
       </c>
       <c r="BK36" s="106">
         <f>BJ36-I35</f>
-        <v>4.1666666666666501</v>
+        <v>4.8333333333333224</v>
       </c>
       <c r="BL36" s="106">
         <f>BK36-I35</f>
-        <v>3.7499999999999836</v>
+        <v>4.349999999999989</v>
       </c>
       <c r="BM36" s="106">
         <f>BL36-I35</f>
-        <v>3.3333333333333171</v>
+        <v>3.8666666666666556</v>
       </c>
       <c r="BN36" s="106">
         <f>BM36-I35</f>
-        <v>2.9166666666666505</v>
+        <v>3.3833333333333222</v>
       </c>
       <c r="BO36" s="106">
         <f>BN36-I35</f>
-        <v>2.499999999999984</v>
+        <v>2.8999999999999888</v>
       </c>
       <c r="BP36" s="106">
         <f>BO36-I35</f>
-        <v>2.0833333333333175</v>
+        <v>2.4166666666666554</v>
       </c>
       <c r="BQ36" s="106">
         <f>BP36-I35</f>
-        <v>1.6666666666666508</v>
+        <v>1.933333333333322</v>
       </c>
       <c r="BR36" s="106">
         <f>BQ36-I35</f>
-        <v>1.249999999999984</v>
+        <v>1.4499999999999886</v>
       </c>
       <c r="BS36" s="106">
         <f>BR36-I35</f>
-        <v>0.83333333333331727</v>
+        <v>0.96666666666665524</v>
       </c>
       <c r="BT36" s="106">
         <f>BS36-I35</f>
-        <v>0.41666666666665059</v>
+        <v>0.4833333333333219</v>
       </c>
       <c r="BV36" s="101"/>
     </row>
@@ -15514,247 +15535,247 @@
       </c>
       <c r="M37" s="105">
         <f>E35</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N37" s="105">
         <f t="shared" ref="N37:BT37" si="12">M39</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="O37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="P37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="R37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="S37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="T37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="U37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="V37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="W37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="X37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Y37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Z37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AA37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AB37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AC37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AD37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AE37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AF37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AG37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AH37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AI37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AJ37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AK37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AL37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AM37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AN37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AO37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AP37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AQ37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AR37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AS37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AT37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AU37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AV37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AW37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AX37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AY37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AZ37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BA37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BB37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BC37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BD37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BE37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BF37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BG37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BH37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BI37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BJ37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BK37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BL37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BM37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BN37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BO37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BP37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BQ37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BR37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BS37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BT37" s="105">
         <f t="shared" si="12"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BV37" s="101">
         <f t="shared" ref="BV37:BV39" si="13">SUM(M37:BT37)</f>
-        <v>1500</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="38" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -15835,247 +15856,247 @@
       </c>
       <c r="M39" s="105">
         <f t="shared" ref="M39:BT39" si="14">M37-M38</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="O39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="P39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="R39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="S39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="T39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="U39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="V39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="W39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="X39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Y39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Z39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AA39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AB39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AC39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AD39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AE39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AF39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AG39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AH39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AI39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AJ39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AK39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AL39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AM39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AN39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AO39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AP39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AQ39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AR39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AS39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AT39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AU39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AV39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AW39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AX39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AY39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AZ39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BA39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BB39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BC39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BD39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BE39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BF39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BG39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BH39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BI39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BJ39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BK39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BL39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BM39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BN39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BO39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BP39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BQ39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BR39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BS39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BT39" s="105">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="BV39" s="101">
         <f t="shared" si="13"/>
-        <v>1500</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="40" spans="2:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16085,55 +16106,55 @@
       <c r="E43" s="193" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="176"/>
-      <c r="G43" s="176"/>
-      <c r="H43" s="176"/>
-      <c r="I43" s="176"/>
-      <c r="J43" s="176"/>
-      <c r="K43" s="176"/>
-      <c r="L43" s="176"/>
-      <c r="M43" s="176"/>
-      <c r="N43" s="176"/>
-      <c r="O43" s="176"/>
-      <c r="P43" s="176"/>
-      <c r="Q43" s="176"/>
-      <c r="R43" s="176"/>
-      <c r="S43" s="176"/>
-      <c r="T43" s="176"/>
-      <c r="U43" s="176"/>
-      <c r="V43" s="176"/>
-      <c r="W43" s="176"/>
-      <c r="X43" s="176"/>
-      <c r="Y43" s="176"/>
-      <c r="Z43" s="176"/>
-      <c r="AA43" s="176"/>
-      <c r="AB43" s="176"/>
-      <c r="AC43" s="176"/>
-      <c r="AD43" s="176"/>
-      <c r="AE43" s="176"/>
-      <c r="AF43" s="176"/>
-      <c r="AG43" s="176"/>
-      <c r="AH43" s="176"/>
-      <c r="AI43" s="176"/>
-      <c r="AJ43" s="176"/>
-      <c r="AK43" s="176"/>
-      <c r="AL43" s="176"/>
-      <c r="AM43" s="176"/>
-      <c r="AN43" s="176"/>
-      <c r="AO43" s="176"/>
-      <c r="AP43" s="176"/>
-      <c r="AQ43" s="176"/>
-      <c r="AR43" s="176"/>
-      <c r="AS43" s="176"/>
-      <c r="AT43" s="176"/>
-      <c r="AU43" s="176"/>
-      <c r="AV43" s="176"/>
-      <c r="AW43" s="176"/>
-      <c r="AX43" s="176"/>
-      <c r="AY43" s="176"/>
-      <c r="AZ43" s="176"/>
-      <c r="BA43" s="176"/>
-      <c r="BB43" s="177"/>
+      <c r="F43" s="157"/>
+      <c r="G43" s="157"/>
+      <c r="H43" s="157"/>
+      <c r="I43" s="157"/>
+      <c r="J43" s="157"/>
+      <c r="K43" s="157"/>
+      <c r="L43" s="157"/>
+      <c r="M43" s="157"/>
+      <c r="N43" s="157"/>
+      <c r="O43" s="157"/>
+      <c r="P43" s="157"/>
+      <c r="Q43" s="157"/>
+      <c r="R43" s="157"/>
+      <c r="S43" s="157"/>
+      <c r="T43" s="157"/>
+      <c r="U43" s="157"/>
+      <c r="V43" s="157"/>
+      <c r="W43" s="157"/>
+      <c r="X43" s="157"/>
+      <c r="Y43" s="157"/>
+      <c r="Z43" s="157"/>
+      <c r="AA43" s="157"/>
+      <c r="AB43" s="157"/>
+      <c r="AC43" s="157"/>
+      <c r="AD43" s="157"/>
+      <c r="AE43" s="157"/>
+      <c r="AF43" s="157"/>
+      <c r="AG43" s="157"/>
+      <c r="AH43" s="157"/>
+      <c r="AI43" s="157"/>
+      <c r="AJ43" s="157"/>
+      <c r="AK43" s="157"/>
+      <c r="AL43" s="157"/>
+      <c r="AM43" s="157"/>
+      <c r="AN43" s="157"/>
+      <c r="AO43" s="157"/>
+      <c r="AP43" s="157"/>
+      <c r="AQ43" s="157"/>
+      <c r="AR43" s="157"/>
+      <c r="AS43" s="157"/>
+      <c r="AT43" s="157"/>
+      <c r="AU43" s="157"/>
+      <c r="AV43" s="157"/>
+      <c r="AW43" s="157"/>
+      <c r="AX43" s="157"/>
+      <c r="AY43" s="157"/>
+      <c r="AZ43" s="157"/>
+      <c r="BA43" s="157"/>
+      <c r="BB43" s="158"/>
     </row>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17096,6 +17117,13 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
     <mergeCell ref="E43:BB43"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
@@ -17112,13 +17140,6 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
communication between recognition and certification services
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e15298e05a6af3ae/Università/Magistrale/LabAdvProg/Proj/AnimalDEX/AnimalDex/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{F2D7B200-65B9-4AA7-B320-C5B64C684A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0AFFDA9-1B77-4025-9EC2-BF59ED0732BC}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{F2D7B200-65B9-4AA7-B320-C5B64C684A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E024993-44F7-41C2-89B3-73B4C6B3FF5E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="219">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -687,6 +687,12 @@
   </si>
   <si>
     <t>Certification service within the docker container</t>
+  </si>
+  <si>
+    <t>2,6</t>
+  </si>
+  <si>
+    <t>Certification service communication with recognition service</t>
   </si>
 </sst>
 </file>
@@ -2400,53 +2406,18 @@
     <xf numFmtId="14" fontId="27" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2477,16 +2448,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -4878,7 +4884,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$39</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4935,7 +4941,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$36:$BT$36</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$37:$BT$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5124,7 +5130,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$39:$BT$39</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$40:$BT$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5171,7 +5177,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$37</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5194,7 +5200,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$36:$BT$36</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$37:$BT$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5383,7 +5389,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$37:$BT$37</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$38:$BT$38</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5582,7 +5588,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$38</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5605,7 +5611,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$36:$BT$36</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$37:$BT$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5794,7 +5800,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$38:$BT$38</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$39:$BT$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6336,7 +6342,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="27632025" cy="7553325"/>
@@ -6398,6 +6404,10 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6881,19 +6891,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="179" t="str">
+      <c r="BK2" s="164" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="180"/>
-      <c r="BM2" s="180"/>
-      <c r="BN2" s="180"/>
-      <c r="BO2" s="180"/>
-      <c r="BP2" s="180"/>
-      <c r="BQ2" s="180"/>
-      <c r="BR2" s="180"/>
-      <c r="BS2" s="180"/>
-      <c r="BT2" s="180"/>
+      <c r="BL2" s="165"/>
+      <c r="BM2" s="165"/>
+      <c r="BN2" s="165"/>
+      <c r="BO2" s="165"/>
+      <c r="BP2" s="165"/>
+      <c r="BQ2" s="165"/>
+      <c r="BR2" s="165"/>
+      <c r="BS2" s="165"/>
+      <c r="BT2" s="165"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -6921,7 +6931,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="181" t="s">
+      <c r="K4" s="166" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -6998,7 +7008,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="182"/>
+      <c r="K5" s="167"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7073,7 +7083,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="182"/>
+      <c r="K6" s="167"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7148,7 +7158,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="182"/>
+      <c r="K7" s="167"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7223,7 +7233,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="183"/>
+      <c r="K8" s="168"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7289,124 +7299,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="184" t="s">
+      <c r="B9" s="169" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="186" t="s">
+      <c r="C9" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="188" t="s">
+      <c r="D9" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="190" t="s">
+      <c r="E9" s="175" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="191"/>
-      <c r="G9" s="192"/>
-      <c r="H9" s="193" t="s">
+      <c r="F9" s="176"/>
+      <c r="G9" s="177"/>
+      <c r="H9" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="161" t="s">
+      <c r="I9" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="163" t="s">
+      <c r="J9" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="165" t="s">
+      <c r="K9" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="166" t="s">
+      <c r="L9" s="188" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="168" t="s">
+      <c r="M9" s="190" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="169"/>
-      <c r="O9" s="169"/>
-      <c r="P9" s="169"/>
-      <c r="Q9" s="170"/>
-      <c r="R9" s="171" t="s">
+      <c r="N9" s="162"/>
+      <c r="O9" s="162"/>
+      <c r="P9" s="162"/>
+      <c r="Q9" s="191"/>
+      <c r="R9" s="192" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="169"/>
-      <c r="T9" s="169"/>
-      <c r="U9" s="169"/>
-      <c r="V9" s="170"/>
-      <c r="W9" s="171" t="s">
+      <c r="S9" s="162"/>
+      <c r="T9" s="162"/>
+      <c r="U9" s="162"/>
+      <c r="V9" s="191"/>
+      <c r="W9" s="192" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="169"/>
-      <c r="Y9" s="169"/>
-      <c r="Z9" s="169"/>
-      <c r="AA9" s="172"/>
-      <c r="AB9" s="173" t="s">
+      <c r="X9" s="162"/>
+      <c r="Y9" s="162"/>
+      <c r="Z9" s="162"/>
+      <c r="AA9" s="163"/>
+      <c r="AB9" s="193" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="169"/>
-      <c r="AD9" s="169"/>
-      <c r="AE9" s="169"/>
-      <c r="AF9" s="170"/>
-      <c r="AG9" s="174" t="s">
+      <c r="AC9" s="162"/>
+      <c r="AD9" s="162"/>
+      <c r="AE9" s="162"/>
+      <c r="AF9" s="191"/>
+      <c r="AG9" s="194" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="169"/>
-      <c r="AI9" s="169"/>
-      <c r="AJ9" s="169"/>
-      <c r="AK9" s="170"/>
-      <c r="AL9" s="174" t="s">
+      <c r="AH9" s="162"/>
+      <c r="AI9" s="162"/>
+      <c r="AJ9" s="162"/>
+      <c r="AK9" s="191"/>
+      <c r="AL9" s="194" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="169"/>
-      <c r="AN9" s="169"/>
-      <c r="AO9" s="169"/>
-      <c r="AP9" s="172"/>
-      <c r="AQ9" s="175" t="s">
+      <c r="AM9" s="162"/>
+      <c r="AN9" s="162"/>
+      <c r="AO9" s="162"/>
+      <c r="AP9" s="163"/>
+      <c r="AQ9" s="195" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="169"/>
-      <c r="AS9" s="169"/>
-      <c r="AT9" s="169"/>
-      <c r="AU9" s="170"/>
-      <c r="AV9" s="176" t="s">
+      <c r="AR9" s="162"/>
+      <c r="AS9" s="162"/>
+      <c r="AT9" s="162"/>
+      <c r="AU9" s="191"/>
+      <c r="AV9" s="196" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="169"/>
-      <c r="AX9" s="169"/>
-      <c r="AY9" s="169"/>
-      <c r="AZ9" s="170"/>
-      <c r="BA9" s="176" t="s">
+      <c r="AW9" s="162"/>
+      <c r="AX9" s="162"/>
+      <c r="AY9" s="162"/>
+      <c r="AZ9" s="191"/>
+      <c r="BA9" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="169"/>
-      <c r="BC9" s="169"/>
-      <c r="BD9" s="169"/>
-      <c r="BE9" s="172"/>
-      <c r="BF9" s="177" t="s">
+      <c r="BB9" s="162"/>
+      <c r="BC9" s="162"/>
+      <c r="BD9" s="162"/>
+      <c r="BE9" s="163"/>
+      <c r="BF9" s="197" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="169"/>
-      <c r="BH9" s="169"/>
-      <c r="BI9" s="169"/>
-      <c r="BJ9" s="170"/>
-      <c r="BK9" s="178" t="s">
+      <c r="BG9" s="162"/>
+      <c r="BH9" s="162"/>
+      <c r="BI9" s="162"/>
+      <c r="BJ9" s="191"/>
+      <c r="BK9" s="161" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="169"/>
-      <c r="BM9" s="169"/>
-      <c r="BN9" s="169"/>
-      <c r="BO9" s="170"/>
-      <c r="BP9" s="178" t="s">
+      <c r="BL9" s="162"/>
+      <c r="BM9" s="162"/>
+      <c r="BN9" s="162"/>
+      <c r="BO9" s="191"/>
+      <c r="BP9" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="169"/>
-      <c r="BR9" s="169"/>
-      <c r="BS9" s="169"/>
-      <c r="BT9" s="172"/>
+      <c r="BQ9" s="162"/>
+      <c r="BR9" s="162"/>
+      <c r="BS9" s="162"/>
+      <c r="BT9" s="163"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="185"/>
-      <c r="C10" s="187"/>
-      <c r="D10" s="189"/>
+      <c r="B10" s="170"/>
+      <c r="C10" s="172"/>
+      <c r="D10" s="174"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7416,11 +7426,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="194"/>
-      <c r="I10" s="162"/>
-      <c r="J10" s="164"/>
-      <c r="K10" s="164"/>
-      <c r="L10" s="167"/>
+      <c r="H10" s="179"/>
+      <c r="I10" s="184"/>
+      <c r="J10" s="186"/>
+      <c r="K10" s="186"/>
+      <c r="L10" s="189"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11029,80 +11039,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="158" t="str">
+      <c r="B45" s="180" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="159"/>
-      <c r="D45" s="159"/>
-      <c r="E45" s="159"/>
-      <c r="F45" s="159"/>
-      <c r="G45" s="159"/>
-      <c r="H45" s="159"/>
-      <c r="I45" s="159"/>
-      <c r="J45" s="159"/>
-      <c r="K45" s="159"/>
-      <c r="L45" s="159"/>
-      <c r="M45" s="159"/>
-      <c r="N45" s="159"/>
-      <c r="O45" s="159"/>
-      <c r="P45" s="159"/>
-      <c r="Q45" s="159"/>
-      <c r="R45" s="159"/>
-      <c r="S45" s="159"/>
-      <c r="T45" s="159"/>
-      <c r="U45" s="159"/>
-      <c r="V45" s="159"/>
-      <c r="W45" s="159"/>
-      <c r="X45" s="159"/>
-      <c r="Y45" s="159"/>
-      <c r="Z45" s="159"/>
-      <c r="AA45" s="159"/>
-      <c r="AB45" s="159"/>
-      <c r="AC45" s="159"/>
-      <c r="AD45" s="159"/>
-      <c r="AE45" s="159"/>
-      <c r="AF45" s="159"/>
-      <c r="AG45" s="159"/>
-      <c r="AH45" s="159"/>
-      <c r="AI45" s="159"/>
-      <c r="AJ45" s="159"/>
-      <c r="AK45" s="159"/>
-      <c r="AL45" s="159"/>
-      <c r="AM45" s="159"/>
-      <c r="AN45" s="159"/>
-      <c r="AO45" s="159"/>
-      <c r="AP45" s="159"/>
-      <c r="AQ45" s="159"/>
-      <c r="AR45" s="159"/>
-      <c r="AS45" s="159"/>
-      <c r="AT45" s="159"/>
-      <c r="AU45" s="159"/>
-      <c r="AV45" s="159"/>
-      <c r="AW45" s="159"/>
-      <c r="AX45" s="159"/>
-      <c r="AY45" s="159"/>
-      <c r="AZ45" s="159"/>
-      <c r="BA45" s="159"/>
-      <c r="BB45" s="159"/>
-      <c r="BC45" s="159"/>
-      <c r="BD45" s="159"/>
-      <c r="BE45" s="159"/>
-      <c r="BF45" s="159"/>
-      <c r="BG45" s="159"/>
-      <c r="BH45" s="159"/>
-      <c r="BI45" s="159"/>
-      <c r="BJ45" s="159"/>
-      <c r="BK45" s="159"/>
-      <c r="BL45" s="159"/>
-      <c r="BM45" s="159"/>
-      <c r="BN45" s="159"/>
-      <c r="BO45" s="159"/>
-      <c r="BP45" s="159"/>
-      <c r="BQ45" s="159"/>
-      <c r="BR45" s="159"/>
-      <c r="BS45" s="159"/>
-      <c r="BT45" s="160"/>
+      <c r="C45" s="181"/>
+      <c r="D45" s="181"/>
+      <c r="E45" s="181"/>
+      <c r="F45" s="181"/>
+      <c r="G45" s="181"/>
+      <c r="H45" s="181"/>
+      <c r="I45" s="181"/>
+      <c r="J45" s="181"/>
+      <c r="K45" s="181"/>
+      <c r="L45" s="181"/>
+      <c r="M45" s="181"/>
+      <c r="N45" s="181"/>
+      <c r="O45" s="181"/>
+      <c r="P45" s="181"/>
+      <c r="Q45" s="181"/>
+      <c r="R45" s="181"/>
+      <c r="S45" s="181"/>
+      <c r="T45" s="181"/>
+      <c r="U45" s="181"/>
+      <c r="V45" s="181"/>
+      <c r="W45" s="181"/>
+      <c r="X45" s="181"/>
+      <c r="Y45" s="181"/>
+      <c r="Z45" s="181"/>
+      <c r="AA45" s="181"/>
+      <c r="AB45" s="181"/>
+      <c r="AC45" s="181"/>
+      <c r="AD45" s="181"/>
+      <c r="AE45" s="181"/>
+      <c r="AF45" s="181"/>
+      <c r="AG45" s="181"/>
+      <c r="AH45" s="181"/>
+      <c r="AI45" s="181"/>
+      <c r="AJ45" s="181"/>
+      <c r="AK45" s="181"/>
+      <c r="AL45" s="181"/>
+      <c r="AM45" s="181"/>
+      <c r="AN45" s="181"/>
+      <c r="AO45" s="181"/>
+      <c r="AP45" s="181"/>
+      <c r="AQ45" s="181"/>
+      <c r="AR45" s="181"/>
+      <c r="AS45" s="181"/>
+      <c r="AT45" s="181"/>
+      <c r="AU45" s="181"/>
+      <c r="AV45" s="181"/>
+      <c r="AW45" s="181"/>
+      <c r="AX45" s="181"/>
+      <c r="AY45" s="181"/>
+      <c r="AZ45" s="181"/>
+      <c r="BA45" s="181"/>
+      <c r="BB45" s="181"/>
+      <c r="BC45" s="181"/>
+      <c r="BD45" s="181"/>
+      <c r="BE45" s="181"/>
+      <c r="BF45" s="181"/>
+      <c r="BG45" s="181"/>
+      <c r="BH45" s="181"/>
+      <c r="BI45" s="181"/>
+      <c r="BJ45" s="181"/>
+      <c r="BK45" s="181"/>
+      <c r="BL45" s="181"/>
+      <c r="BM45" s="181"/>
+      <c r="BN45" s="181"/>
+      <c r="BO45" s="181"/>
+      <c r="BP45" s="181"/>
+      <c r="BQ45" s="181"/>
+      <c r="BR45" s="181"/>
+      <c r="BS45" s="181"/>
+      <c r="BT45" s="182"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12065,14 +12075,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12089,6 +12091,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12101,10 +12111,10 @@
     <tabColor rgb="FF7B3C16"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:BV1000"/>
+  <dimension ref="B1:BV1001"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF22" sqref="AF22"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12217,7 +12227,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="181" t="s">
+      <c r="K3" s="166" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12294,7 +12304,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="182"/>
+      <c r="K4" s="167"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12368,7 +12378,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="182"/>
+      <c r="K5" s="167"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12443,7 +12453,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="182"/>
+      <c r="K6" s="167"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12518,7 +12528,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="183"/>
+      <c r="K7" s="168"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12584,124 +12594,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="184" t="s">
+      <c r="B8" s="169" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="186" t="s">
+      <c r="C8" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="188" t="s">
+      <c r="D8" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="190" t="s">
+      <c r="E8" s="175" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="191"/>
-      <c r="G8" s="192"/>
-      <c r="H8" s="193" t="s">
+      <c r="F8" s="176"/>
+      <c r="G8" s="177"/>
+      <c r="H8" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="161" t="s">
+      <c r="I8" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="163" t="s">
+      <c r="J8" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="165" t="s">
+      <c r="K8" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="166" t="s">
+      <c r="L8" s="188" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="168" t="s">
+      <c r="M8" s="190" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="169"/>
-      <c r="O8" s="169"/>
-      <c r="P8" s="169"/>
-      <c r="Q8" s="170"/>
-      <c r="R8" s="171" t="s">
+      <c r="N8" s="162"/>
+      <c r="O8" s="162"/>
+      <c r="P8" s="162"/>
+      <c r="Q8" s="191"/>
+      <c r="R8" s="192" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="169"/>
-      <c r="T8" s="169"/>
-      <c r="U8" s="169"/>
-      <c r="V8" s="170"/>
-      <c r="W8" s="171" t="s">
+      <c r="S8" s="162"/>
+      <c r="T8" s="162"/>
+      <c r="U8" s="162"/>
+      <c r="V8" s="191"/>
+      <c r="W8" s="192" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="169"/>
-      <c r="Y8" s="169"/>
-      <c r="Z8" s="169"/>
-      <c r="AA8" s="172"/>
-      <c r="AB8" s="173" t="s">
+      <c r="X8" s="162"/>
+      <c r="Y8" s="162"/>
+      <c r="Z8" s="162"/>
+      <c r="AA8" s="163"/>
+      <c r="AB8" s="193" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="169"/>
-      <c r="AD8" s="169"/>
-      <c r="AE8" s="169"/>
-      <c r="AF8" s="170"/>
-      <c r="AG8" s="174" t="s">
+      <c r="AC8" s="162"/>
+      <c r="AD8" s="162"/>
+      <c r="AE8" s="162"/>
+      <c r="AF8" s="191"/>
+      <c r="AG8" s="194" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="169"/>
-      <c r="AI8" s="169"/>
-      <c r="AJ8" s="169"/>
-      <c r="AK8" s="170"/>
-      <c r="AL8" s="174" t="s">
+      <c r="AH8" s="162"/>
+      <c r="AI8" s="162"/>
+      <c r="AJ8" s="162"/>
+      <c r="AK8" s="191"/>
+      <c r="AL8" s="194" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="169"/>
-      <c r="AN8" s="169"/>
-      <c r="AO8" s="169"/>
-      <c r="AP8" s="172"/>
-      <c r="AQ8" s="175" t="s">
+      <c r="AM8" s="162"/>
+      <c r="AN8" s="162"/>
+      <c r="AO8" s="162"/>
+      <c r="AP8" s="163"/>
+      <c r="AQ8" s="195" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="169"/>
-      <c r="AS8" s="169"/>
-      <c r="AT8" s="169"/>
-      <c r="AU8" s="170"/>
-      <c r="AV8" s="176" t="s">
+      <c r="AR8" s="162"/>
+      <c r="AS8" s="162"/>
+      <c r="AT8" s="162"/>
+      <c r="AU8" s="191"/>
+      <c r="AV8" s="196" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="169"/>
-      <c r="AX8" s="169"/>
-      <c r="AY8" s="169"/>
-      <c r="AZ8" s="170"/>
-      <c r="BA8" s="176" t="s">
+      <c r="AW8" s="162"/>
+      <c r="AX8" s="162"/>
+      <c r="AY8" s="162"/>
+      <c r="AZ8" s="191"/>
+      <c r="BA8" s="196" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="169"/>
-      <c r="BC8" s="169"/>
-      <c r="BD8" s="169"/>
-      <c r="BE8" s="172"/>
-      <c r="BF8" s="177" t="s">
+      <c r="BB8" s="162"/>
+      <c r="BC8" s="162"/>
+      <c r="BD8" s="162"/>
+      <c r="BE8" s="163"/>
+      <c r="BF8" s="197" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="169"/>
-      <c r="BH8" s="169"/>
-      <c r="BI8" s="169"/>
-      <c r="BJ8" s="170"/>
-      <c r="BK8" s="178" t="s">
+      <c r="BG8" s="162"/>
+      <c r="BH8" s="162"/>
+      <c r="BI8" s="162"/>
+      <c r="BJ8" s="191"/>
+      <c r="BK8" s="161" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="169"/>
-      <c r="BM8" s="169"/>
-      <c r="BN8" s="169"/>
-      <c r="BO8" s="170"/>
-      <c r="BP8" s="178" t="s">
+      <c r="BL8" s="162"/>
+      <c r="BM8" s="162"/>
+      <c r="BN8" s="162"/>
+      <c r="BO8" s="191"/>
+      <c r="BP8" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="169"/>
-      <c r="BR8" s="169"/>
-      <c r="BS8" s="169"/>
-      <c r="BT8" s="172"/>
+      <c r="BQ8" s="162"/>
+      <c r="BR8" s="162"/>
+      <c r="BS8" s="162"/>
+      <c r="BT8" s="163"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="185"/>
-      <c r="C9" s="187"/>
-      <c r="D9" s="189"/>
+      <c r="B9" s="170"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="174"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12711,11 +12721,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="194"/>
-      <c r="I9" s="162"/>
-      <c r="J9" s="164"/>
-      <c r="K9" s="164"/>
-      <c r="L9" s="167"/>
+      <c r="H9" s="179"/>
+      <c r="I9" s="184"/>
+      <c r="J9" s="186"/>
+      <c r="K9" s="186"/>
+      <c r="L9" s="189"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -12924,7 +12934,7 @@
       <c r="J10" s="47"/>
       <c r="K10" s="48"/>
       <c r="L10" s="49">
-        <f t="shared" ref="L10:L34" si="0">F10/E10</f>
+        <f t="shared" ref="L10:L35" si="0">F10/E10</f>
         <v>1</v>
       </c>
       <c r="M10" s="50"/>
@@ -13684,7 +13694,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="58">
-        <f t="shared" ref="G18:G22" si="3">E18-F18</f>
+        <f t="shared" ref="G18:G23" si="3">E18-F18</f>
         <v>0</v>
       </c>
       <c r="H18" s="59">
@@ -13697,7 +13707,7 @@
         <v>45376</v>
       </c>
       <c r="K18" s="62">
-        <f t="shared" ref="K18:K22" si="4">J18-I18+1</f>
+        <f t="shared" ref="K18:K23" si="4">J18-I18+1</f>
         <v>1</v>
       </c>
       <c r="L18" s="63">
@@ -14066,7 +14076,7 @@
       <c r="C22" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="D22" s="196" t="s">
+      <c r="D22" s="158" t="s">
         <v>212</v>
       </c>
       <c r="E22" s="56">
@@ -14082,7 +14092,7 @@
       <c r="H22" s="59">
         <v>2</v>
       </c>
-      <c r="I22" s="197">
+      <c r="I22" s="159">
         <v>45380</v>
       </c>
       <c r="J22" s="61">
@@ -14114,7 +14124,7 @@
       <c r="AB22" s="64"/>
       <c r="AC22" s="65"/>
       <c r="AE22" s="65"/>
-      <c r="AF22" s="198"/>
+      <c r="AF22" s="160"/>
       <c r="AG22" s="69"/>
       <c r="AH22" s="69"/>
       <c r="AI22" s="69"/>
@@ -14156,194 +14166,206 @@
       <c r="BS22" s="65"/>
       <c r="BT22" s="68"/>
     </row>
-    <row r="23" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="53">
-        <v>3</v>
-      </c>
-      <c r="C23" s="73"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="42">
-        <f t="shared" ref="E23:G23" si="5">SUM(E24:E29)</f>
+    <row r="23" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="53" t="s">
+        <v>217</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="D23" s="158" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" s="56">
+        <v>2</v>
+      </c>
+      <c r="F23" s="57">
+        <v>2</v>
+      </c>
+      <c r="G23" s="58">
         <v>0</v>
       </c>
-      <c r="F23" s="43">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="44">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="75"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="49" t="e">
+      <c r="H23" s="59">
+        <v>2</v>
+      </c>
+      <c r="I23" s="159">
+        <v>45384</v>
+      </c>
+      <c r="J23" s="61">
+        <v>45384</v>
+      </c>
+      <c r="K23" s="62">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="L23" s="63">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M23" s="50"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="51"/>
-      <c r="S23" s="51"/>
-      <c r="T23" s="51"/>
-      <c r="U23" s="51"/>
-      <c r="V23" s="51"/>
-      <c r="W23" s="51"/>
-      <c r="X23" s="51"/>
-      <c r="Y23" s="51"/>
-      <c r="Z23" s="51"/>
-      <c r="AA23" s="52"/>
-      <c r="AB23" s="50"/>
-      <c r="AC23" s="51"/>
-      <c r="AD23" s="51"/>
-      <c r="AE23" s="51"/>
-      <c r="AF23" s="51"/>
-      <c r="AG23" s="51"/>
-      <c r="AH23" s="51"/>
-      <c r="AI23" s="51"/>
-      <c r="AJ23" s="51"/>
-      <c r="AK23" s="51"/>
-      <c r="AL23" s="51"/>
-      <c r="AM23" s="51"/>
-      <c r="AN23" s="51"/>
-      <c r="AO23" s="51"/>
-      <c r="AP23" s="52"/>
-      <c r="AQ23" s="50"/>
-      <c r="AR23" s="51"/>
-      <c r="AS23" s="51"/>
-      <c r="AT23" s="51"/>
-      <c r="AU23" s="51"/>
-      <c r="AV23" s="51"/>
-      <c r="AW23" s="51"/>
-      <c r="AX23" s="51"/>
-      <c r="AY23" s="51"/>
-      <c r="AZ23" s="51"/>
-      <c r="BA23" s="51"/>
-      <c r="BB23" s="51"/>
-      <c r="BC23" s="51"/>
-      <c r="BD23" s="51"/>
-      <c r="BE23" s="52"/>
-      <c r="BF23" s="50"/>
-      <c r="BG23" s="51"/>
-      <c r="BH23" s="51"/>
-      <c r="BI23" s="51"/>
-      <c r="BJ23" s="51"/>
-      <c r="BK23" s="51"/>
-      <c r="BL23" s="51"/>
-      <c r="BM23" s="51"/>
-      <c r="BN23" s="51"/>
-      <c r="BO23" s="51"/>
-      <c r="BP23" s="51"/>
-      <c r="BQ23" s="51"/>
-      <c r="BR23" s="51"/>
-      <c r="BS23" s="51"/>
-      <c r="BT23" s="52"/>
+        <v>1</v>
+      </c>
+      <c r="M23" s="64"/>
+      <c r="N23" s="65"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="65"/>
+      <c r="Q23" s="65"/>
+      <c r="R23" s="67"/>
+      <c r="S23" s="67"/>
+      <c r="T23" s="67"/>
+      <c r="U23" s="67"/>
+      <c r="V23" s="67"/>
+      <c r="W23" s="65"/>
+      <c r="X23" s="65"/>
+      <c r="Y23" s="65"/>
+      <c r="Z23" s="65"/>
+      <c r="AA23" s="68"/>
+      <c r="AB23" s="64"/>
+      <c r="AC23" s="65"/>
+      <c r="AE23" s="65"/>
+      <c r="AF23" s="160"/>
+      <c r="AG23" s="69"/>
+      <c r="AH23" s="160"/>
+      <c r="AI23" s="69"/>
+      <c r="AJ23" s="69"/>
+      <c r="AK23" s="69"/>
+      <c r="AL23" s="65"/>
+      <c r="AM23" s="65"/>
+      <c r="AN23" s="65"/>
+      <c r="AO23" s="65"/>
+      <c r="AP23" s="68"/>
+      <c r="AQ23" s="64"/>
+      <c r="AR23" s="65"/>
+      <c r="AS23" s="65"/>
+      <c r="AT23" s="65"/>
+      <c r="AU23" s="65"/>
+      <c r="AV23" s="70"/>
+      <c r="AW23" s="70"/>
+      <c r="AX23" s="70"/>
+      <c r="AY23" s="70"/>
+      <c r="AZ23" s="70"/>
+      <c r="BA23" s="65"/>
+      <c r="BB23" s="65"/>
+      <c r="BC23" s="65"/>
+      <c r="BD23" s="65"/>
+      <c r="BE23" s="68"/>
+      <c r="BF23" s="64"/>
+      <c r="BG23" s="65"/>
+      <c r="BH23" s="65"/>
+      <c r="BI23" s="65"/>
+      <c r="BJ23" s="65"/>
+      <c r="BK23" s="71"/>
+      <c r="BL23" s="71"/>
+      <c r="BM23" s="71"/>
+      <c r="BN23" s="71"/>
+      <c r="BO23" s="71"/>
+      <c r="BP23" s="65"/>
+      <c r="BQ23" s="65"/>
+      <c r="BR23" s="65"/>
+      <c r="BS23" s="65"/>
+      <c r="BT23" s="68"/>
     </row>
     <row r="24" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="53">
-        <v>3.1</v>
-      </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="58">
-        <f t="shared" ref="G24:G29" si="6">E24-F24</f>
+        <v>3</v>
+      </c>
+      <c r="C24" s="73"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="42">
+        <f t="shared" ref="E24:G24" si="5">SUM(E25:E30)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="59"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="62">
-        <f t="shared" ref="K24:K29" si="7">J24-I24+1</f>
-        <v>1</v>
-      </c>
-      <c r="L24" s="63" t="e">
+      <c r="F24" s="43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="44">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="75"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="77"/>
+      <c r="L24" s="49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M24" s="64"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="65"/>
-      <c r="P24" s="65"/>
-      <c r="Q24" s="65"/>
-      <c r="R24" s="67"/>
-      <c r="S24" s="67"/>
-      <c r="T24" s="67"/>
-      <c r="U24" s="67"/>
-      <c r="V24" s="67"/>
-      <c r="W24" s="65"/>
-      <c r="X24" s="65"/>
-      <c r="Y24" s="65"/>
-      <c r="Z24" s="65"/>
-      <c r="AA24" s="68"/>
-      <c r="AB24" s="64"/>
-      <c r="AC24" s="65"/>
-      <c r="AD24" s="65"/>
-      <c r="AE24" s="65"/>
-      <c r="AF24" s="65"/>
-      <c r="AG24" s="69"/>
-      <c r="AH24" s="69"/>
-      <c r="AI24" s="69"/>
-      <c r="AJ24" s="69"/>
-      <c r="AK24" s="69"/>
-      <c r="AL24" s="65"/>
-      <c r="AM24" s="65"/>
-      <c r="AN24" s="65"/>
-      <c r="AO24" s="65"/>
-      <c r="AP24" s="68"/>
-      <c r="AQ24" s="112"/>
-      <c r="AR24" s="65"/>
-      <c r="AS24" s="65"/>
-      <c r="AT24" s="65"/>
-      <c r="AU24" s="65"/>
-      <c r="AV24" s="70"/>
-      <c r="AW24" s="70"/>
-      <c r="AX24" s="70"/>
-      <c r="AY24" s="70"/>
-      <c r="AZ24" s="70"/>
-      <c r="BA24" s="65"/>
-      <c r="BB24" s="65"/>
-      <c r="BC24" s="65"/>
-      <c r="BD24" s="65"/>
-      <c r="BE24" s="68"/>
-      <c r="BF24" s="64"/>
-      <c r="BG24" s="65"/>
-      <c r="BH24" s="65"/>
-      <c r="BI24" s="65"/>
-      <c r="BJ24" s="65"/>
-      <c r="BK24" s="71"/>
-      <c r="BL24" s="71"/>
-      <c r="BM24" s="71"/>
-      <c r="BN24" s="71"/>
-      <c r="BO24" s="71"/>
-      <c r="BP24" s="65"/>
-      <c r="BQ24" s="65"/>
-      <c r="BR24" s="65"/>
-      <c r="BS24" s="65"/>
-      <c r="BT24" s="68"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="51"/>
+      <c r="T24" s="51"/>
+      <c r="U24" s="51"/>
+      <c r="V24" s="51"/>
+      <c r="W24" s="51"/>
+      <c r="X24" s="51"/>
+      <c r="Y24" s="51"/>
+      <c r="Z24" s="51"/>
+      <c r="AA24" s="52"/>
+      <c r="AB24" s="50"/>
+      <c r="AC24" s="51"/>
+      <c r="AD24" s="51"/>
+      <c r="AE24" s="51"/>
+      <c r="AF24" s="51"/>
+      <c r="AG24" s="51"/>
+      <c r="AH24" s="51"/>
+      <c r="AI24" s="51"/>
+      <c r="AJ24" s="51"/>
+      <c r="AK24" s="51"/>
+      <c r="AL24" s="51"/>
+      <c r="AM24" s="51"/>
+      <c r="AN24" s="51"/>
+      <c r="AO24" s="51"/>
+      <c r="AP24" s="52"/>
+      <c r="AQ24" s="50"/>
+      <c r="AR24" s="51"/>
+      <c r="AS24" s="51"/>
+      <c r="AT24" s="51"/>
+      <c r="AU24" s="51"/>
+      <c r="AV24" s="51"/>
+      <c r="AW24" s="51"/>
+      <c r="AX24" s="51"/>
+      <c r="AY24" s="51"/>
+      <c r="AZ24" s="51"/>
+      <c r="BA24" s="51"/>
+      <c r="BB24" s="51"/>
+      <c r="BC24" s="51"/>
+      <c r="BD24" s="51"/>
+      <c r="BE24" s="52"/>
+      <c r="BF24" s="50"/>
+      <c r="BG24" s="51"/>
+      <c r="BH24" s="51"/>
+      <c r="BI24" s="51"/>
+      <c r="BJ24" s="51"/>
+      <c r="BK24" s="51"/>
+      <c r="BL24" s="51"/>
+      <c r="BM24" s="51"/>
+      <c r="BN24" s="51"/>
+      <c r="BO24" s="51"/>
+      <c r="BP24" s="51"/>
+      <c r="BQ24" s="51"/>
+      <c r="BR24" s="51"/>
+      <c r="BS24" s="51"/>
+      <c r="BT24" s="52"/>
     </row>
     <row r="25" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="53">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="55"/>
       <c r="E25" s="56"/>
       <c r="F25" s="57"/>
       <c r="G25" s="58">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="G25:G30" si="6">E25-F25</f>
         <v>0</v>
       </c>
       <c r="H25" s="59"/>
-      <c r="I25" s="157"/>
+      <c r="I25" s="60"/>
       <c r="J25" s="61"/>
       <c r="K25" s="62">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="K25:K30" si="7">J25-I25+1</f>
         <v>1</v>
       </c>
       <c r="L25" s="63" t="e">
@@ -14380,7 +14402,7 @@
       <c r="AN25" s="65"/>
       <c r="AO25" s="65"/>
       <c r="AP25" s="68"/>
-      <c r="AQ25" s="64"/>
+      <c r="AQ25" s="112"/>
       <c r="AR25" s="65"/>
       <c r="AS25" s="65"/>
       <c r="AT25" s="65"/>
@@ -14412,8 +14434,8 @@
       <c r="BT25" s="68"/>
     </row>
     <row r="26" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="53" t="s">
-        <v>60</v>
+      <c r="B26" s="53">
+        <v>3.2</v>
       </c>
       <c r="C26" s="54"/>
       <c r="D26" s="55"/>
@@ -14424,7 +14446,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="59"/>
-      <c r="I26" s="60"/>
+      <c r="I26" s="157"/>
       <c r="J26" s="61"/>
       <c r="K26" s="62">
         <f t="shared" si="7"/>
@@ -14497,7 +14519,7 @@
     </row>
     <row r="27" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="53" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27" s="54"/>
       <c r="D27" s="55"/>
@@ -14580,8 +14602,8 @@
       <c r="BT27" s="68"/>
     </row>
     <row r="28" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="53">
-        <v>3.3</v>
+      <c r="B28" s="53" t="s">
+        <v>62</v>
       </c>
       <c r="C28" s="54"/>
       <c r="D28" s="55"/>
@@ -14664,8 +14686,8 @@
       <c r="BT28" s="68"/>
     </row>
     <row r="29" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="53" t="s">
-        <v>65</v>
+      <c r="B29" s="53">
+        <v>3.3</v>
       </c>
       <c r="C29" s="54"/>
       <c r="D29" s="55"/>
@@ -14748,193 +14770,193 @@
       <c r="BT29" s="68"/>
     </row>
     <row r="30" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="53">
-        <v>4</v>
-      </c>
-      <c r="C30" s="73"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="42">
-        <f t="shared" ref="E30:G30" si="8">SUM(E31:E34)</f>
+      <c r="B30" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="54"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="58">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F30" s="43">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="44">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="75"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="77"/>
-      <c r="K30" s="77"/>
-      <c r="L30" s="49" t="e">
+      <c r="H30" s="59"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="62">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L30" s="63" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M30" s="50"/>
-      <c r="N30" s="51"/>
-      <c r="O30" s="51"/>
-      <c r="P30" s="51"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="51"/>
-      <c r="S30" s="51"/>
-      <c r="T30" s="51"/>
-      <c r="U30" s="51"/>
-      <c r="V30" s="51"/>
-      <c r="W30" s="51"/>
-      <c r="X30" s="51"/>
-      <c r="Y30" s="51"/>
-      <c r="Z30" s="51"/>
-      <c r="AA30" s="52"/>
-      <c r="AB30" s="50"/>
-      <c r="AC30" s="51"/>
-      <c r="AD30" s="51"/>
-      <c r="AE30" s="51"/>
-      <c r="AF30" s="51"/>
-      <c r="AG30" s="51"/>
-      <c r="AH30" s="51"/>
-      <c r="AI30" s="51"/>
-      <c r="AJ30" s="51"/>
-      <c r="AK30" s="51"/>
-      <c r="AL30" s="51"/>
-      <c r="AM30" s="51"/>
-      <c r="AN30" s="51"/>
-      <c r="AO30" s="51"/>
-      <c r="AP30" s="52"/>
-      <c r="AQ30" s="50"/>
-      <c r="AR30" s="51"/>
-      <c r="AS30" s="51"/>
-      <c r="AT30" s="51"/>
-      <c r="AU30" s="51"/>
-      <c r="AV30" s="51"/>
-      <c r="AW30" s="51"/>
-      <c r="AX30" s="51"/>
-      <c r="AY30" s="51"/>
-      <c r="AZ30" s="51"/>
-      <c r="BA30" s="51"/>
-      <c r="BB30" s="51"/>
-      <c r="BC30" s="51"/>
-      <c r="BD30" s="51"/>
-      <c r="BE30" s="52"/>
-      <c r="BF30" s="50"/>
-      <c r="BG30" s="51"/>
-      <c r="BH30" s="51"/>
-      <c r="BI30" s="51"/>
-      <c r="BJ30" s="51"/>
-      <c r="BK30" s="51"/>
-      <c r="BL30" s="51"/>
-      <c r="BM30" s="51"/>
-      <c r="BN30" s="51"/>
-      <c r="BO30" s="51"/>
-      <c r="BP30" s="51"/>
-      <c r="BQ30" s="51"/>
-      <c r="BR30" s="51"/>
-      <c r="BS30" s="51"/>
-      <c r="BT30" s="52"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="65"/>
+      <c r="O30" s="65"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="65"/>
+      <c r="R30" s="67"/>
+      <c r="S30" s="67"/>
+      <c r="T30" s="67"/>
+      <c r="U30" s="67"/>
+      <c r="V30" s="67"/>
+      <c r="W30" s="65"/>
+      <c r="X30" s="65"/>
+      <c r="Y30" s="65"/>
+      <c r="Z30" s="65"/>
+      <c r="AA30" s="68"/>
+      <c r="AB30" s="64"/>
+      <c r="AC30" s="65"/>
+      <c r="AD30" s="65"/>
+      <c r="AE30" s="65"/>
+      <c r="AF30" s="65"/>
+      <c r="AG30" s="69"/>
+      <c r="AH30" s="69"/>
+      <c r="AI30" s="69"/>
+      <c r="AJ30" s="69"/>
+      <c r="AK30" s="69"/>
+      <c r="AL30" s="65"/>
+      <c r="AM30" s="65"/>
+      <c r="AN30" s="65"/>
+      <c r="AO30" s="65"/>
+      <c r="AP30" s="68"/>
+      <c r="AQ30" s="64"/>
+      <c r="AR30" s="65"/>
+      <c r="AS30" s="65"/>
+      <c r="AT30" s="65"/>
+      <c r="AU30" s="65"/>
+      <c r="AV30" s="70"/>
+      <c r="AW30" s="70"/>
+      <c r="AX30" s="70"/>
+      <c r="AY30" s="70"/>
+      <c r="AZ30" s="70"/>
+      <c r="BA30" s="65"/>
+      <c r="BB30" s="65"/>
+      <c r="BC30" s="65"/>
+      <c r="BD30" s="65"/>
+      <c r="BE30" s="68"/>
+      <c r="BF30" s="64"/>
+      <c r="BG30" s="65"/>
+      <c r="BH30" s="65"/>
+      <c r="BI30" s="65"/>
+      <c r="BJ30" s="65"/>
+      <c r="BK30" s="71"/>
+      <c r="BL30" s="71"/>
+      <c r="BM30" s="71"/>
+      <c r="BN30" s="71"/>
+      <c r="BO30" s="71"/>
+      <c r="BP30" s="65"/>
+      <c r="BQ30" s="65"/>
+      <c r="BR30" s="65"/>
+      <c r="BS30" s="65"/>
+      <c r="BT30" s="68"/>
     </row>
     <row r="31" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="53">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="58">
-        <f t="shared" ref="G31:G34" si="9">E31-F31</f>
+        <v>4</v>
+      </c>
+      <c r="C31" s="73"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="42">
+        <f t="shared" ref="E31:G31" si="8">SUM(E32:E35)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="59"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="62">
-        <f t="shared" ref="K31:K34" si="10">J31-I31+1</f>
-        <v>1</v>
-      </c>
-      <c r="L31" s="63" t="e">
+      <c r="F31" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="44">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="75"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M31" s="64"/>
-      <c r="N31" s="65"/>
-      <c r="O31" s="65"/>
-      <c r="P31" s="65"/>
-      <c r="Q31" s="65"/>
-      <c r="R31" s="67"/>
-      <c r="S31" s="67"/>
-      <c r="T31" s="67"/>
-      <c r="U31" s="67"/>
-      <c r="V31" s="67"/>
-      <c r="W31" s="65"/>
-      <c r="X31" s="65"/>
-      <c r="Y31" s="65"/>
-      <c r="Z31" s="65"/>
-      <c r="AA31" s="68"/>
-      <c r="AB31" s="64"/>
-      <c r="AC31" s="65"/>
-      <c r="AD31" s="65"/>
-      <c r="AE31" s="65"/>
-      <c r="AF31" s="65"/>
-      <c r="AG31" s="69"/>
-      <c r="AH31" s="69"/>
-      <c r="AI31" s="69"/>
-      <c r="AJ31" s="69"/>
-      <c r="AK31" s="69"/>
-      <c r="AL31" s="65"/>
-      <c r="AM31" s="65"/>
-      <c r="AN31" s="65"/>
-      <c r="AO31" s="65"/>
-      <c r="AP31" s="68"/>
-      <c r="AQ31" s="64"/>
-      <c r="AR31" s="65"/>
-      <c r="AS31" s="65"/>
-      <c r="AT31" s="65"/>
-      <c r="AU31" s="65"/>
-      <c r="AV31" s="70"/>
-      <c r="AW31" s="70"/>
-      <c r="AX31" s="70"/>
-      <c r="AY31" s="70"/>
-      <c r="AZ31" s="70"/>
-      <c r="BA31" s="65"/>
-      <c r="BB31" s="65"/>
-      <c r="BC31" s="65"/>
-      <c r="BD31" s="65"/>
-      <c r="BE31" s="68"/>
-      <c r="BF31" s="113"/>
-      <c r="BG31" s="65"/>
-      <c r="BH31" s="65"/>
-      <c r="BI31" s="65"/>
-      <c r="BJ31" s="65"/>
-      <c r="BK31" s="71"/>
-      <c r="BL31" s="71"/>
-      <c r="BM31" s="71"/>
-      <c r="BN31" s="71"/>
-      <c r="BO31" s="71"/>
-      <c r="BP31" s="65"/>
-      <c r="BQ31" s="65"/>
-      <c r="BR31" s="65"/>
-      <c r="BS31" s="65"/>
-      <c r="BT31" s="68"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="51"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="51"/>
+      <c r="R31" s="51"/>
+      <c r="S31" s="51"/>
+      <c r="T31" s="51"/>
+      <c r="U31" s="51"/>
+      <c r="V31" s="51"/>
+      <c r="W31" s="51"/>
+      <c r="X31" s="51"/>
+      <c r="Y31" s="51"/>
+      <c r="Z31" s="51"/>
+      <c r="AA31" s="52"/>
+      <c r="AB31" s="50"/>
+      <c r="AC31" s="51"/>
+      <c r="AD31" s="51"/>
+      <c r="AE31" s="51"/>
+      <c r="AF31" s="51"/>
+      <c r="AG31" s="51"/>
+      <c r="AH31" s="51"/>
+      <c r="AI31" s="51"/>
+      <c r="AJ31" s="51"/>
+      <c r="AK31" s="51"/>
+      <c r="AL31" s="51"/>
+      <c r="AM31" s="51"/>
+      <c r="AN31" s="51"/>
+      <c r="AO31" s="51"/>
+      <c r="AP31" s="52"/>
+      <c r="AQ31" s="50"/>
+      <c r="AR31" s="51"/>
+      <c r="AS31" s="51"/>
+      <c r="AT31" s="51"/>
+      <c r="AU31" s="51"/>
+      <c r="AV31" s="51"/>
+      <c r="AW31" s="51"/>
+      <c r="AX31" s="51"/>
+      <c r="AY31" s="51"/>
+      <c r="AZ31" s="51"/>
+      <c r="BA31" s="51"/>
+      <c r="BB31" s="51"/>
+      <c r="BC31" s="51"/>
+      <c r="BD31" s="51"/>
+      <c r="BE31" s="52"/>
+      <c r="BF31" s="50"/>
+      <c r="BG31" s="51"/>
+      <c r="BH31" s="51"/>
+      <c r="BI31" s="51"/>
+      <c r="BJ31" s="51"/>
+      <c r="BK31" s="51"/>
+      <c r="BL31" s="51"/>
+      <c r="BM31" s="51"/>
+      <c r="BN31" s="51"/>
+      <c r="BO31" s="51"/>
+      <c r="BP31" s="51"/>
+      <c r="BQ31" s="51"/>
+      <c r="BR31" s="51"/>
+      <c r="BS31" s="51"/>
+      <c r="BT31" s="52"/>
     </row>
     <row r="32" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="53">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C32" s="54"/>
       <c r="D32" s="55"/>
       <c r="E32" s="56"/>
       <c r="F32" s="57"/>
       <c r="G32" s="58">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="G32:G35" si="9">E32-F32</f>
         <v>0</v>
       </c>
       <c r="H32" s="59"/>
       <c r="I32" s="60"/>
       <c r="J32" s="61"/>
       <c r="K32" s="62">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="K32:K35" si="10">J32-I32+1</f>
         <v>1</v>
       </c>
       <c r="L32" s="63" t="e">
@@ -14986,7 +15008,7 @@
       <c r="BC32" s="65"/>
       <c r="BD32" s="65"/>
       <c r="BE32" s="68"/>
-      <c r="BF32" s="64"/>
+      <c r="BF32" s="113"/>
       <c r="BG32" s="65"/>
       <c r="BH32" s="65"/>
       <c r="BI32" s="65"/>
@@ -15004,10 +15026,10 @@
     </row>
     <row r="33" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="53">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="C33" s="54"/>
-      <c r="D33" s="80"/>
+      <c r="D33" s="55"/>
       <c r="E33" s="56"/>
       <c r="F33" s="57"/>
       <c r="G33" s="58">
@@ -15086,1205 +15108,1288 @@
       <c r="BS33" s="65"/>
       <c r="BT33" s="68"/>
     </row>
-    <row r="34" spans="2:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="82"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="84"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="86">
+    <row r="34" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="53">
+        <v>4.3</v>
+      </c>
+      <c r="C34" s="54"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="58">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H34" s="87"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="89"/>
-      <c r="K34" s="90">
+      <c r="H34" s="59"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="62">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="L34" s="91" t="e">
+      <c r="L34" s="63" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M34" s="92"/>
-      <c r="N34" s="93"/>
-      <c r="O34" s="93"/>
-      <c r="P34" s="93"/>
-      <c r="Q34" s="93"/>
-      <c r="R34" s="94"/>
-      <c r="S34" s="94"/>
-      <c r="T34" s="94"/>
-      <c r="U34" s="94"/>
-      <c r="V34" s="94"/>
-      <c r="W34" s="93"/>
-      <c r="X34" s="93"/>
-      <c r="Y34" s="93"/>
-      <c r="Z34" s="93"/>
-      <c r="AA34" s="95"/>
-      <c r="AB34" s="92"/>
-      <c r="AC34" s="93"/>
-      <c r="AD34" s="93"/>
-      <c r="AE34" s="93"/>
-      <c r="AF34" s="93"/>
-      <c r="AG34" s="96"/>
-      <c r="AH34" s="96"/>
-      <c r="AI34" s="96"/>
-      <c r="AJ34" s="96"/>
-      <c r="AK34" s="96"/>
-      <c r="AL34" s="93"/>
-      <c r="AM34" s="93"/>
-      <c r="AN34" s="93"/>
-      <c r="AO34" s="93"/>
-      <c r="AP34" s="95"/>
-      <c r="AQ34" s="92"/>
-      <c r="AR34" s="93"/>
-      <c r="AS34" s="93"/>
-      <c r="AT34" s="93"/>
-      <c r="AU34" s="93"/>
-      <c r="AV34" s="97"/>
-      <c r="AW34" s="97"/>
-      <c r="AX34" s="97"/>
-      <c r="AY34" s="97"/>
-      <c r="AZ34" s="97"/>
-      <c r="BA34" s="93"/>
-      <c r="BB34" s="93"/>
-      <c r="BC34" s="93"/>
-      <c r="BD34" s="93"/>
-      <c r="BE34" s="95"/>
-      <c r="BF34" s="92"/>
-      <c r="BG34" s="93"/>
-      <c r="BH34" s="93"/>
-      <c r="BI34" s="93"/>
-      <c r="BJ34" s="93"/>
-      <c r="BK34" s="98"/>
-      <c r="BL34" s="98"/>
-      <c r="BM34" s="98"/>
-      <c r="BN34" s="98"/>
-      <c r="BO34" s="98"/>
-      <c r="BP34" s="93"/>
-      <c r="BQ34" s="93"/>
-      <c r="BR34" s="93"/>
-      <c r="BS34" s="93"/>
-      <c r="BT34" s="95"/>
+      <c r="M34" s="64"/>
+      <c r="N34" s="65"/>
+      <c r="O34" s="65"/>
+      <c r="P34" s="65"/>
+      <c r="Q34" s="65"/>
+      <c r="R34" s="67"/>
+      <c r="S34" s="67"/>
+      <c r="T34" s="67"/>
+      <c r="U34" s="67"/>
+      <c r="V34" s="67"/>
+      <c r="W34" s="65"/>
+      <c r="X34" s="65"/>
+      <c r="Y34" s="65"/>
+      <c r="Z34" s="65"/>
+      <c r="AA34" s="68"/>
+      <c r="AB34" s="64"/>
+      <c r="AC34" s="65"/>
+      <c r="AD34" s="65"/>
+      <c r="AE34" s="65"/>
+      <c r="AF34" s="65"/>
+      <c r="AG34" s="69"/>
+      <c r="AH34" s="69"/>
+      <c r="AI34" s="69"/>
+      <c r="AJ34" s="69"/>
+      <c r="AK34" s="69"/>
+      <c r="AL34" s="65"/>
+      <c r="AM34" s="65"/>
+      <c r="AN34" s="65"/>
+      <c r="AO34" s="65"/>
+      <c r="AP34" s="68"/>
+      <c r="AQ34" s="64"/>
+      <c r="AR34" s="65"/>
+      <c r="AS34" s="65"/>
+      <c r="AT34" s="65"/>
+      <c r="AU34" s="65"/>
+      <c r="AV34" s="70"/>
+      <c r="AW34" s="70"/>
+      <c r="AX34" s="70"/>
+      <c r="AY34" s="70"/>
+      <c r="AZ34" s="70"/>
+      <c r="BA34" s="65"/>
+      <c r="BB34" s="65"/>
+      <c r="BC34" s="65"/>
+      <c r="BD34" s="65"/>
+      <c r="BE34" s="68"/>
+      <c r="BF34" s="64"/>
+      <c r="BG34" s="65"/>
+      <c r="BH34" s="65"/>
+      <c r="BI34" s="65"/>
+      <c r="BJ34" s="65"/>
+      <c r="BK34" s="71"/>
+      <c r="BL34" s="71"/>
+      <c r="BM34" s="71"/>
+      <c r="BN34" s="71"/>
+      <c r="BO34" s="71"/>
+      <c r="BP34" s="65"/>
+      <c r="BQ34" s="65"/>
+      <c r="BR34" s="65"/>
+      <c r="BS34" s="65"/>
+      <c r="BT34" s="68"/>
     </row>
-    <row r="35" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E35" s="99" t="s">
-        <v>29</v>
-      </c>
-      <c r="F35" s="99" t="s">
-        <v>30</v>
-      </c>
-      <c r="G35" s="99" t="s">
-        <v>31</v>
-      </c>
-      <c r="H35" s="99" t="s">
-        <v>73</v>
-      </c>
-      <c r="I35" s="99" t="s">
-        <v>74</v>
-      </c>
+    <row r="35" spans="2:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="82"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="86">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="87"/>
+      <c r="I35" s="88"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="90">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="L35" s="91" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" s="92"/>
+      <c r="N35" s="93"/>
+      <c r="O35" s="93"/>
+      <c r="P35" s="93"/>
+      <c r="Q35" s="93"/>
+      <c r="R35" s="94"/>
+      <c r="S35" s="94"/>
+      <c r="T35" s="94"/>
+      <c r="U35" s="94"/>
+      <c r="V35" s="94"/>
+      <c r="W35" s="93"/>
+      <c r="X35" s="93"/>
+      <c r="Y35" s="93"/>
+      <c r="Z35" s="93"/>
+      <c r="AA35" s="95"/>
+      <c r="AB35" s="92"/>
+      <c r="AC35" s="93"/>
+      <c r="AD35" s="93"/>
+      <c r="AE35" s="93"/>
+      <c r="AF35" s="93"/>
+      <c r="AG35" s="96"/>
+      <c r="AH35" s="96"/>
+      <c r="AI35" s="96"/>
+      <c r="AJ35" s="96"/>
+      <c r="AK35" s="96"/>
+      <c r="AL35" s="93"/>
+      <c r="AM35" s="93"/>
+      <c r="AN35" s="93"/>
+      <c r="AO35" s="93"/>
+      <c r="AP35" s="95"/>
+      <c r="AQ35" s="92"/>
+      <c r="AR35" s="93"/>
+      <c r="AS35" s="93"/>
+      <c r="AT35" s="93"/>
+      <c r="AU35" s="93"/>
+      <c r="AV35" s="97"/>
+      <c r="AW35" s="97"/>
+      <c r="AX35" s="97"/>
+      <c r="AY35" s="97"/>
+      <c r="AZ35" s="97"/>
+      <c r="BA35" s="93"/>
+      <c r="BB35" s="93"/>
+      <c r="BC35" s="93"/>
+      <c r="BD35" s="93"/>
+      <c r="BE35" s="95"/>
+      <c r="BF35" s="92"/>
+      <c r="BG35" s="93"/>
+      <c r="BH35" s="93"/>
+      <c r="BI35" s="93"/>
+      <c r="BJ35" s="93"/>
+      <c r="BK35" s="98"/>
+      <c r="BL35" s="98"/>
+      <c r="BM35" s="98"/>
+      <c r="BN35" s="98"/>
+      <c r="BO35" s="98"/>
+      <c r="BP35" s="93"/>
+      <c r="BQ35" s="93"/>
+      <c r="BR35" s="93"/>
+      <c r="BS35" s="93"/>
+      <c r="BT35" s="95"/>
     </row>
     <row r="36" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="100" t="s">
-        <v>76</v>
-      </c>
-      <c r="E36" s="101">
-        <f>SUM(E11:E16,E18:E21,E24:E29,E31:E34)</f>
-        <v>28</v>
-      </c>
-      <c r="F36" s="101">
-        <f>SUM(F11:F16,F18:F21,F24:F29,F31:F34)</f>
-        <v>28</v>
-      </c>
-      <c r="G36" s="101">
-        <f>SUM(G11:G16,G18:G21,G24:G29,G31:G34)</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="101">
-        <v>60</v>
-      </c>
-      <c r="I36" s="101">
-        <f>E36/H36</f>
-        <v>0.46666666666666667</v>
-      </c>
-      <c r="L36" s="102" t="s">
-        <v>77</v>
-      </c>
-      <c r="M36" s="103">
-        <v>1</v>
-      </c>
-      <c r="N36" s="103">
-        <v>2</v>
-      </c>
-      <c r="O36" s="103">
-        <v>3</v>
-      </c>
-      <c r="P36" s="103">
-        <v>4</v>
-      </c>
-      <c r="Q36" s="103">
-        <v>5</v>
-      </c>
-      <c r="R36" s="103">
-        <v>6</v>
-      </c>
-      <c r="S36" s="103">
-        <v>7</v>
-      </c>
-      <c r="T36" s="103">
-        <v>8</v>
-      </c>
-      <c r="U36" s="103">
-        <v>9</v>
-      </c>
-      <c r="V36" s="103">
-        <v>10</v>
-      </c>
-      <c r="W36" s="103">
-        <v>11</v>
-      </c>
-      <c r="X36" s="103">
-        <v>12</v>
-      </c>
-      <c r="Y36" s="103">
-        <v>13</v>
-      </c>
-      <c r="Z36" s="103">
-        <v>14</v>
-      </c>
-      <c r="AA36" s="103">
-        <v>15</v>
-      </c>
-      <c r="AB36" s="103">
-        <v>16</v>
-      </c>
-      <c r="AC36" s="103">
-        <v>17</v>
-      </c>
-      <c r="AD36" s="103">
-        <v>18</v>
-      </c>
-      <c r="AE36" s="103">
-        <v>19</v>
-      </c>
-      <c r="AF36" s="103">
-        <v>20</v>
-      </c>
-      <c r="AG36" s="103">
-        <v>21</v>
-      </c>
-      <c r="AH36" s="103">
-        <v>22</v>
-      </c>
-      <c r="AI36" s="103">
-        <v>23</v>
-      </c>
-      <c r="AJ36" s="103">
-        <v>24</v>
-      </c>
-      <c r="AK36" s="103">
-        <v>25</v>
-      </c>
-      <c r="AL36" s="103">
-        <v>26</v>
-      </c>
-      <c r="AM36" s="103">
-        <v>27</v>
-      </c>
-      <c r="AN36" s="103">
-        <v>28</v>
-      </c>
-      <c r="AO36" s="103">
+      <c r="E36" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="AP36" s="103">
+      <c r="F36" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="AQ36" s="103">
+      <c r="G36" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="AR36" s="103">
-        <v>32</v>
-      </c>
-      <c r="AS36" s="103">
-        <v>33</v>
-      </c>
-      <c r="AT36" s="103">
-        <v>34</v>
-      </c>
-      <c r="AU36" s="103">
-        <v>35</v>
-      </c>
-      <c r="AV36" s="103">
-        <v>36</v>
-      </c>
-      <c r="AW36" s="103">
-        <v>37</v>
-      </c>
-      <c r="AX36" s="103">
-        <v>38</v>
-      </c>
-      <c r="AY36" s="103">
-        <v>39</v>
-      </c>
-      <c r="AZ36" s="103">
-        <v>40</v>
-      </c>
-      <c r="BA36" s="103">
-        <v>41</v>
-      </c>
-      <c r="BB36" s="103">
-        <v>42</v>
-      </c>
-      <c r="BC36" s="103">
-        <v>43</v>
-      </c>
-      <c r="BD36" s="103">
-        <v>44</v>
-      </c>
-      <c r="BE36" s="103">
-        <v>45</v>
-      </c>
-      <c r="BF36" s="103">
-        <v>46</v>
-      </c>
-      <c r="BG36" s="103">
-        <v>47</v>
-      </c>
-      <c r="BH36" s="103">
-        <v>48</v>
-      </c>
-      <c r="BI36" s="103">
-        <v>49</v>
-      </c>
-      <c r="BJ36" s="103">
-        <v>50</v>
-      </c>
-      <c r="BK36" s="103">
-        <v>51</v>
-      </c>
-      <c r="BL36" s="103">
-        <v>52</v>
-      </c>
-      <c r="BM36" s="103">
-        <v>53</v>
-      </c>
-      <c r="BN36" s="103">
-        <v>54</v>
-      </c>
-      <c r="BO36" s="103">
-        <v>55</v>
-      </c>
-      <c r="BP36" s="103">
-        <v>56</v>
-      </c>
-      <c r="BQ36" s="103">
-        <v>57</v>
-      </c>
-      <c r="BR36" s="103">
-        <v>58</v>
-      </c>
-      <c r="BS36" s="103">
-        <v>59</v>
-      </c>
-      <c r="BT36" s="103">
-        <v>60</v>
-      </c>
-      <c r="BV36" s="100" t="s">
-        <v>76</v>
+      <c r="H36" s="99" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" s="99" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="104" t="s">
-        <v>78</v>
+      <c r="C37" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" s="101">
+        <f>SUM(E11:E16,E18:E21,E25:E30,E32:E35)</f>
+        <v>28</v>
+      </c>
+      <c r="F37" s="101">
+        <f>SUM(F11:F16,F18:F21,F25:F30,F32:F35)</f>
+        <v>28</v>
+      </c>
+      <c r="G37" s="101">
+        <f>SUM(G11:G16,G18:G21,G25:G30,G32:G35)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="101">
+        <v>60</v>
+      </c>
+      <c r="I37" s="101">
+        <f>E37/H37</f>
+        <v>0.46666666666666667</v>
       </c>
       <c r="L37" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="M37" s="105">
-        <f>E36</f>
+        <v>77</v>
+      </c>
+      <c r="M37" s="103">
+        <v>1</v>
+      </c>
+      <c r="N37" s="103">
+        <v>2</v>
+      </c>
+      <c r="O37" s="103">
+        <v>3</v>
+      </c>
+      <c r="P37" s="103">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="103">
+        <v>5</v>
+      </c>
+      <c r="R37" s="103">
+        <v>6</v>
+      </c>
+      <c r="S37" s="103">
+        <v>7</v>
+      </c>
+      <c r="T37" s="103">
+        <v>8</v>
+      </c>
+      <c r="U37" s="103">
+        <v>9</v>
+      </c>
+      <c r="V37" s="103">
+        <v>10</v>
+      </c>
+      <c r="W37" s="103">
+        <v>11</v>
+      </c>
+      <c r="X37" s="103">
+        <v>12</v>
+      </c>
+      <c r="Y37" s="103">
+        <v>13</v>
+      </c>
+      <c r="Z37" s="103">
+        <v>14</v>
+      </c>
+      <c r="AA37" s="103">
+        <v>15</v>
+      </c>
+      <c r="AB37" s="103">
+        <v>16</v>
+      </c>
+      <c r="AC37" s="103">
+        <v>17</v>
+      </c>
+      <c r="AD37" s="103">
+        <v>18</v>
+      </c>
+      <c r="AE37" s="103">
+        <v>19</v>
+      </c>
+      <c r="AF37" s="103">
+        <v>20</v>
+      </c>
+      <c r="AG37" s="103">
+        <v>21</v>
+      </c>
+      <c r="AH37" s="103">
+        <v>22</v>
+      </c>
+      <c r="AI37" s="103">
+        <v>23</v>
+      </c>
+      <c r="AJ37" s="103">
+        <v>24</v>
+      </c>
+      <c r="AK37" s="103">
+        <v>25</v>
+      </c>
+      <c r="AL37" s="103">
+        <v>26</v>
+      </c>
+      <c r="AM37" s="103">
+        <v>27</v>
+      </c>
+      <c r="AN37" s="103">
         <v>28</v>
       </c>
-      <c r="N37" s="106">
-        <f>M37-I36</f>
-        <v>27.533333333333335</v>
-      </c>
-      <c r="O37" s="106">
-        <f>N37-I36</f>
-        <v>27.06666666666667</v>
-      </c>
-      <c r="P37" s="106">
-        <f>O37-I36</f>
-        <v>26.600000000000005</v>
-      </c>
-      <c r="Q37" s="106">
-        <f>P37-I36</f>
-        <v>26.13333333333334</v>
-      </c>
-      <c r="R37" s="106">
-        <f>Q37-I36</f>
-        <v>25.666666666666675</v>
-      </c>
-      <c r="S37" s="106">
-        <f>R37-I36</f>
-        <v>25.20000000000001</v>
-      </c>
-      <c r="T37" s="106">
-        <f>S37-I36</f>
-        <v>24.733333333333345</v>
-      </c>
-      <c r="U37" s="106">
-        <f>T37-I36</f>
-        <v>24.26666666666668</v>
-      </c>
-      <c r="V37" s="106">
-        <f>U37-I36</f>
-        <v>23.800000000000015</v>
-      </c>
-      <c r="W37" s="106">
-        <f>V37-I36</f>
-        <v>23.33333333333335</v>
-      </c>
-      <c r="X37" s="106">
-        <f>W37-I36</f>
-        <v>22.866666666666685</v>
-      </c>
-      <c r="Y37" s="106">
-        <f>X37-I36</f>
-        <v>22.40000000000002</v>
-      </c>
-      <c r="Z37" s="106">
-        <f>Y37-I36</f>
-        <v>21.933333333333355</v>
-      </c>
-      <c r="AA37" s="106">
-        <f>Z37-I36</f>
-        <v>21.46666666666669</v>
-      </c>
-      <c r="AB37" s="106">
-        <f>AA37-I36</f>
-        <v>21.000000000000025</v>
-      </c>
-      <c r="AC37" s="106">
-        <f>AB37-I36</f>
-        <v>20.53333333333336</v>
-      </c>
-      <c r="AD37" s="106">
-        <f>AC37-I36</f>
-        <v>20.066666666666695</v>
-      </c>
-      <c r="AE37" s="106">
-        <f>AD37-I36</f>
-        <v>19.60000000000003</v>
-      </c>
-      <c r="AF37" s="106">
-        <f>AE37-I36</f>
-        <v>19.133333333333365</v>
-      </c>
-      <c r="AG37" s="106">
-        <f>AF37-I36</f>
-        <v>18.6666666666667</v>
-      </c>
-      <c r="AH37" s="106">
-        <f>AG37-I36</f>
-        <v>18.200000000000035</v>
-      </c>
-      <c r="AI37" s="106">
-        <f>AH37-I36</f>
-        <v>17.73333333333337</v>
-      </c>
-      <c r="AJ37" s="106">
-        <f>AI37-I36</f>
-        <v>17.266666666666705</v>
-      </c>
-      <c r="AK37" s="106">
-        <f>AJ37-I36</f>
-        <v>16.80000000000004</v>
-      </c>
-      <c r="AL37" s="106">
-        <f>AK37-I36</f>
-        <v>16.333333333333375</v>
-      </c>
-      <c r="AM37" s="106">
-        <f>AL37-I36</f>
-        <v>15.866666666666708</v>
-      </c>
-      <c r="AN37" s="106">
-        <f>AM37-I36</f>
-        <v>15.400000000000041</v>
-      </c>
-      <c r="AO37" s="106">
-        <f>AN37-I36</f>
-        <v>14.933333333333374</v>
-      </c>
-      <c r="AP37" s="106">
-        <f>AO37-I36</f>
-        <v>14.466666666666708</v>
-      </c>
-      <c r="AQ37" s="106">
-        <f>AP37-I36</f>
-        <v>14.000000000000041</v>
-      </c>
-      <c r="AR37" s="106">
-        <f>AQ37-I36</f>
-        <v>13.533333333333374</v>
-      </c>
-      <c r="AS37" s="106">
-        <f>AR37-I36</f>
-        <v>13.066666666666707</v>
-      </c>
-      <c r="AT37" s="106">
-        <f>AS37-I36</f>
-        <v>12.600000000000041</v>
-      </c>
-      <c r="AU37" s="106">
-        <f>AT37-I36</f>
-        <v>12.133333333333374</v>
-      </c>
-      <c r="AV37" s="106">
-        <f>AU37-I36</f>
-        <v>11.666666666666707</v>
-      </c>
-      <c r="AW37" s="106">
-        <f>AV37-I36</f>
-        <v>11.20000000000004</v>
-      </c>
-      <c r="AX37" s="106">
-        <f>AW37-I36</f>
-        <v>10.733333333333373</v>
-      </c>
-      <c r="AY37" s="106">
-        <f>AX37-I36</f>
-        <v>10.266666666666707</v>
-      </c>
-      <c r="AZ37" s="106">
-        <f>AY37-I36</f>
-        <v>9.8000000000000398</v>
-      </c>
-      <c r="BA37" s="106">
-        <f>AZ37-I36</f>
-        <v>9.333333333333373</v>
-      </c>
-      <c r="BB37" s="106">
-        <f>BA37-I36</f>
-        <v>8.8666666666667062</v>
-      </c>
-      <c r="BC37" s="106">
-        <f>BB37-I36</f>
-        <v>8.4000000000000394</v>
-      </c>
-      <c r="BD37" s="106">
-        <f>BC37-I36</f>
-        <v>7.9333333333333727</v>
-      </c>
-      <c r="BE37" s="106">
-        <f>BD37-I36</f>
-        <v>7.4666666666667059</v>
-      </c>
-      <c r="BF37" s="106">
-        <f>BE37-I36</f>
-        <v>7.0000000000000391</v>
-      </c>
-      <c r="BG37" s="106">
-        <f>BF37-I36</f>
-        <v>6.5333333333333723</v>
-      </c>
-      <c r="BH37" s="106">
-        <f>BG37-I36</f>
-        <v>6.0666666666667055</v>
-      </c>
-      <c r="BI37" s="106">
-        <f>BH37-I36</f>
-        <v>5.6000000000000387</v>
-      </c>
-      <c r="BJ37" s="106">
-        <f>BI37-I36</f>
-        <v>5.1333333333333719</v>
-      </c>
-      <c r="BK37" s="106">
-        <f>BJ37-I36</f>
-        <v>4.6666666666667052</v>
-      </c>
-      <c r="BL37" s="106">
-        <f>BK37-I36</f>
-        <v>4.2000000000000384</v>
-      </c>
-      <c r="BM37" s="106">
-        <f>BL37-I36</f>
-        <v>3.7333333333333716</v>
-      </c>
-      <c r="BN37" s="106">
-        <f>BM37-I36</f>
-        <v>3.2666666666667048</v>
-      </c>
-      <c r="BO37" s="106">
-        <f>BN37-I36</f>
-        <v>2.800000000000038</v>
-      </c>
-      <c r="BP37" s="106">
-        <f>BO37-I36</f>
-        <v>2.3333333333333712</v>
-      </c>
-      <c r="BQ37" s="106">
-        <f>BP37-I36</f>
-        <v>1.8666666666667044</v>
-      </c>
-      <c r="BR37" s="106">
-        <f>BQ37-I36</f>
-        <v>1.4000000000000377</v>
-      </c>
-      <c r="BS37" s="106">
-        <f>BR37-I36</f>
-        <v>0.93333333333337098</v>
-      </c>
-      <c r="BT37" s="106">
-        <f>BS37-I36</f>
-        <v>0.46666666666670431</v>
-      </c>
-      <c r="BV37" s="101"/>
+      <c r="AO37" s="103">
+        <v>29</v>
+      </c>
+      <c r="AP37" s="103">
+        <v>30</v>
+      </c>
+      <c r="AQ37" s="103">
+        <v>31</v>
+      </c>
+      <c r="AR37" s="103">
+        <v>32</v>
+      </c>
+      <c r="AS37" s="103">
+        <v>33</v>
+      </c>
+      <c r="AT37" s="103">
+        <v>34</v>
+      </c>
+      <c r="AU37" s="103">
+        <v>35</v>
+      </c>
+      <c r="AV37" s="103">
+        <v>36</v>
+      </c>
+      <c r="AW37" s="103">
+        <v>37</v>
+      </c>
+      <c r="AX37" s="103">
+        <v>38</v>
+      </c>
+      <c r="AY37" s="103">
+        <v>39</v>
+      </c>
+      <c r="AZ37" s="103">
+        <v>40</v>
+      </c>
+      <c r="BA37" s="103">
+        <v>41</v>
+      </c>
+      <c r="BB37" s="103">
+        <v>42</v>
+      </c>
+      <c r="BC37" s="103">
+        <v>43</v>
+      </c>
+      <c r="BD37" s="103">
+        <v>44</v>
+      </c>
+      <c r="BE37" s="103">
+        <v>45</v>
+      </c>
+      <c r="BF37" s="103">
+        <v>46</v>
+      </c>
+      <c r="BG37" s="103">
+        <v>47</v>
+      </c>
+      <c r="BH37" s="103">
+        <v>48</v>
+      </c>
+      <c r="BI37" s="103">
+        <v>49</v>
+      </c>
+      <c r="BJ37" s="103">
+        <v>50</v>
+      </c>
+      <c r="BK37" s="103">
+        <v>51</v>
+      </c>
+      <c r="BL37" s="103">
+        <v>52</v>
+      </c>
+      <c r="BM37" s="103">
+        <v>53</v>
+      </c>
+      <c r="BN37" s="103">
+        <v>54</v>
+      </c>
+      <c r="BO37" s="103">
+        <v>55</v>
+      </c>
+      <c r="BP37" s="103">
+        <v>56</v>
+      </c>
+      <c r="BQ37" s="103">
+        <v>57</v>
+      </c>
+      <c r="BR37" s="103">
+        <v>58</v>
+      </c>
+      <c r="BS37" s="103">
+        <v>59</v>
+      </c>
+      <c r="BT37" s="103">
+        <v>60</v>
+      </c>
+      <c r="BV37" s="100" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="38" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H38" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="L38" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="M38" s="105">
+        <f>E37</f>
+        <v>28</v>
+      </c>
+      <c r="N38" s="106">
+        <f>M38-I37</f>
+        <v>27.533333333333335</v>
+      </c>
+      <c r="O38" s="106">
+        <f>N38-I37</f>
+        <v>27.06666666666667</v>
+      </c>
+      <c r="P38" s="106">
+        <f>O38-I37</f>
+        <v>26.600000000000005</v>
+      </c>
+      <c r="Q38" s="106">
+        <f>P38-I37</f>
+        <v>26.13333333333334</v>
+      </c>
+      <c r="R38" s="106">
+        <f>Q38-I37</f>
+        <v>25.666666666666675</v>
+      </c>
+      <c r="S38" s="106">
+        <f>R38-I37</f>
+        <v>25.20000000000001</v>
+      </c>
+      <c r="T38" s="106">
+        <f>S38-I37</f>
+        <v>24.733333333333345</v>
+      </c>
+      <c r="U38" s="106">
+        <f>T38-I37</f>
+        <v>24.26666666666668</v>
+      </c>
+      <c r="V38" s="106">
+        <f>U38-I37</f>
+        <v>23.800000000000015</v>
+      </c>
+      <c r="W38" s="106">
+        <f>V38-I37</f>
+        <v>23.33333333333335</v>
+      </c>
+      <c r="X38" s="106">
+        <f>W38-I37</f>
+        <v>22.866666666666685</v>
+      </c>
+      <c r="Y38" s="106">
+        <f>X38-I37</f>
+        <v>22.40000000000002</v>
+      </c>
+      <c r="Z38" s="106">
+        <f>Y38-I37</f>
+        <v>21.933333333333355</v>
+      </c>
+      <c r="AA38" s="106">
+        <f>Z38-I37</f>
+        <v>21.46666666666669</v>
+      </c>
+      <c r="AB38" s="106">
+        <f>AA38-I37</f>
+        <v>21.000000000000025</v>
+      </c>
+      <c r="AC38" s="106">
+        <f>AB38-I37</f>
+        <v>20.53333333333336</v>
+      </c>
+      <c r="AD38" s="106">
+        <f>AC38-I37</f>
+        <v>20.066666666666695</v>
+      </c>
+      <c r="AE38" s="106">
+        <f>AD38-I37</f>
+        <v>19.60000000000003</v>
+      </c>
+      <c r="AF38" s="106">
+        <f>AE38-I37</f>
+        <v>19.133333333333365</v>
+      </c>
+      <c r="AG38" s="106">
+        <f>AF38-I37</f>
+        <v>18.6666666666667</v>
+      </c>
+      <c r="AH38" s="106">
+        <f>AG38-I37</f>
+        <v>18.200000000000035</v>
+      </c>
+      <c r="AI38" s="106">
+        <f>AH38-I37</f>
+        <v>17.73333333333337</v>
+      </c>
+      <c r="AJ38" s="106">
+        <f>AI38-I37</f>
+        <v>17.266666666666705</v>
+      </c>
+      <c r="AK38" s="106">
+        <f>AJ38-I37</f>
+        <v>16.80000000000004</v>
+      </c>
+      <c r="AL38" s="106">
+        <f>AK38-I37</f>
+        <v>16.333333333333375</v>
+      </c>
+      <c r="AM38" s="106">
+        <f>AL38-I37</f>
+        <v>15.866666666666708</v>
+      </c>
+      <c r="AN38" s="106">
+        <f>AM38-I37</f>
+        <v>15.400000000000041</v>
+      </c>
+      <c r="AO38" s="106">
+        <f>AN38-I37</f>
+        <v>14.933333333333374</v>
+      </c>
+      <c r="AP38" s="106">
+        <f>AO38-I37</f>
+        <v>14.466666666666708</v>
+      </c>
+      <c r="AQ38" s="106">
+        <f>AP38-I37</f>
+        <v>14.000000000000041</v>
+      </c>
+      <c r="AR38" s="106">
+        <f>AQ38-I37</f>
+        <v>13.533333333333374</v>
+      </c>
+      <c r="AS38" s="106">
+        <f>AR38-I37</f>
+        <v>13.066666666666707</v>
+      </c>
+      <c r="AT38" s="106">
+        <f>AS38-I37</f>
+        <v>12.600000000000041</v>
+      </c>
+      <c r="AU38" s="106">
+        <f>AT38-I37</f>
+        <v>12.133333333333374</v>
+      </c>
+      <c r="AV38" s="106">
+        <f>AU38-I37</f>
+        <v>11.666666666666707</v>
+      </c>
+      <c r="AW38" s="106">
+        <f>AV38-I37</f>
+        <v>11.20000000000004</v>
+      </c>
+      <c r="AX38" s="106">
+        <f>AW38-I37</f>
+        <v>10.733333333333373</v>
+      </c>
+      <c r="AY38" s="106">
+        <f>AX38-I37</f>
+        <v>10.266666666666707</v>
+      </c>
+      <c r="AZ38" s="106">
+        <f>AY38-I37</f>
+        <v>9.8000000000000398</v>
+      </c>
+      <c r="BA38" s="106">
+        <f>AZ38-I37</f>
+        <v>9.333333333333373</v>
+      </c>
+      <c r="BB38" s="106">
+        <f>BA38-I37</f>
+        <v>8.8666666666667062</v>
+      </c>
+      <c r="BC38" s="106">
+        <f>BB38-I37</f>
+        <v>8.4000000000000394</v>
+      </c>
+      <c r="BD38" s="106">
+        <f>BC38-I37</f>
+        <v>7.9333333333333727</v>
+      </c>
+      <c r="BE38" s="106">
+        <f>BD38-I37</f>
+        <v>7.4666666666667059</v>
+      </c>
+      <c r="BF38" s="106">
+        <f>BE38-I37</f>
+        <v>7.0000000000000391</v>
+      </c>
+      <c r="BG38" s="106">
+        <f>BF38-I37</f>
+        <v>6.5333333333333723</v>
+      </c>
+      <c r="BH38" s="106">
+        <f>BG38-I37</f>
+        <v>6.0666666666667055</v>
+      </c>
+      <c r="BI38" s="106">
+        <f>BH38-I37</f>
+        <v>5.6000000000000387</v>
+      </c>
+      <c r="BJ38" s="106">
+        <f>BI38-I37</f>
+        <v>5.1333333333333719</v>
+      </c>
+      <c r="BK38" s="106">
+        <f>BJ38-I37</f>
+        <v>4.6666666666667052</v>
+      </c>
+      <c r="BL38" s="106">
+        <f>BK38-I37</f>
+        <v>4.2000000000000384</v>
+      </c>
+      <c r="BM38" s="106">
+        <f>BL38-I37</f>
+        <v>3.7333333333333716</v>
+      </c>
+      <c r="BN38" s="106">
+        <f>BM38-I37</f>
+        <v>3.2666666666667048</v>
+      </c>
+      <c r="BO38" s="106">
+        <f>BN38-I37</f>
+        <v>2.800000000000038</v>
+      </c>
+      <c r="BP38" s="106">
+        <f>BO38-I37</f>
+        <v>2.3333333333333712</v>
+      </c>
+      <c r="BQ38" s="106">
+        <f>BP38-I37</f>
+        <v>1.8666666666667044</v>
+      </c>
+      <c r="BR38" s="106">
+        <f>BQ38-I37</f>
+        <v>1.4000000000000377</v>
+      </c>
+      <c r="BS38" s="106">
+        <f>BR38-I37</f>
+        <v>0.93333333333337098</v>
+      </c>
+      <c r="BT38" s="106">
+        <f>BS38-I37</f>
+        <v>0.46666666666670431</v>
+      </c>
+      <c r="BV38" s="101"/>
+    </row>
+    <row r="39" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L39" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="M38" s="105">
-        <f>E36</f>
+      <c r="M39" s="105">
+        <f>E37</f>
         <v>28</v>
       </c>
-      <c r="N38" s="105">
-        <f t="shared" ref="N38:BT38" si="11">M40</f>
+      <c r="N39" s="105">
+        <f t="shared" ref="N39:BT39" si="11">M41</f>
         <v>28</v>
       </c>
-      <c r="O38" s="105">
+      <c r="O39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="P38" s="105">
+      <c r="P39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="Q38" s="105">
+      <c r="Q39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="R38" s="105">
+      <c r="R39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="S38" s="105">
+      <c r="S39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="T38" s="105">
+      <c r="T39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="U38" s="105">
+      <c r="U39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="V38" s="105">
+      <c r="V39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="W38" s="105">
+      <c r="W39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="X38" s="105">
+      <c r="X39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="Y38" s="105">
+      <c r="Y39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="Z38" s="105">
+      <c r="Z39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AA38" s="105">
+      <c r="AA39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AB38" s="105">
+      <c r="AB39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AC38" s="105">
+      <c r="AC39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AD38" s="105">
+      <c r="AD39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AE38" s="105">
+      <c r="AE39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AF38" s="105">
+      <c r="AF39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AG38" s="105">
+      <c r="AG39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AH38" s="105">
+      <c r="AH39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AI38" s="105">
+      <c r="AI39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AJ38" s="105">
+      <c r="AJ39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AK38" s="105">
+      <c r="AK39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AL38" s="105">
+      <c r="AL39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AM38" s="105">
+      <c r="AM39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AN38" s="105">
+      <c r="AN39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AO38" s="105">
+      <c r="AO39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AP38" s="105">
+      <c r="AP39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AQ38" s="105">
+      <c r="AQ39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AR38" s="105">
+      <c r="AR39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AS38" s="105">
+      <c r="AS39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AT38" s="105">
+      <c r="AT39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AU38" s="105">
+      <c r="AU39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AV38" s="105">
+      <c r="AV39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AW38" s="105">
+      <c r="AW39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AX38" s="105">
+      <c r="AX39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AY38" s="105">
+      <c r="AY39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AZ38" s="105">
+      <c r="AZ39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BA38" s="105">
+      <c r="BA39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BB38" s="105">
+      <c r="BB39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BC38" s="105">
+      <c r="BC39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BD38" s="105">
+      <c r="BD39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BE38" s="105">
+      <c r="BE39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BF38" s="105">
+      <c r="BF39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BG38" s="105">
+      <c r="BG39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BH38" s="105">
+      <c r="BH39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BI38" s="105">
+      <c r="BI39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BJ38" s="105">
+      <c r="BJ39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BK38" s="105">
+      <c r="BK39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BL38" s="105">
+      <c r="BL39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BM38" s="105">
+      <c r="BM39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BN38" s="105">
+      <c r="BN39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BO38" s="105">
+      <c r="BO39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BP38" s="105">
+      <c r="BP39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BQ38" s="105">
+      <c r="BQ39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BR38" s="105">
+      <c r="BR39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BS38" s="105">
+      <c r="BS39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BT38" s="105">
+      <c r="BT39" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BV38" s="101">
-        <f t="shared" ref="BV38:BV40" si="12">SUM(M38:BT38)</f>
+      <c r="BV39" s="101">
+        <f t="shared" ref="BV39:BV41" si="12">SUM(M39:BT39)</f>
         <v>1680</v>
       </c>
     </row>
-    <row r="39" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K39" s="107" t="s">
+    <row r="40" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K40" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="L39" s="102" t="s">
+      <c r="L40" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="M39" s="57"/>
-      <c r="N39" s="57"/>
-      <c r="O39" s="57"/>
-      <c r="P39" s="57"/>
-      <c r="Q39" s="57"/>
-      <c r="R39" s="57"/>
-      <c r="S39" s="57"/>
-      <c r="T39" s="57"/>
-      <c r="U39" s="57"/>
-      <c r="V39" s="57"/>
-      <c r="W39" s="57"/>
-      <c r="X39" s="57"/>
-      <c r="Y39" s="57"/>
-      <c r="Z39" s="57"/>
-      <c r="AA39" s="57"/>
-      <c r="AB39" s="57"/>
-      <c r="AC39" s="57"/>
-      <c r="AD39" s="57"/>
-      <c r="AE39" s="57"/>
-      <c r="AF39" s="57"/>
-      <c r="AG39" s="57"/>
-      <c r="AH39" s="57"/>
-      <c r="AI39" s="57"/>
-      <c r="AJ39" s="57"/>
-      <c r="AK39" s="57"/>
-      <c r="AL39" s="57"/>
-      <c r="AM39" s="57"/>
-      <c r="AN39" s="57"/>
-      <c r="AO39" s="57"/>
-      <c r="AP39" s="57"/>
-      <c r="AQ39" s="57"/>
-      <c r="AR39" s="57"/>
-      <c r="AS39" s="57"/>
-      <c r="AT39" s="57"/>
-      <c r="AU39" s="57"/>
-      <c r="AV39" s="57"/>
-      <c r="AW39" s="57"/>
-      <c r="AX39" s="57"/>
-      <c r="AY39" s="57"/>
-      <c r="AZ39" s="57"/>
-      <c r="BA39" s="57"/>
-      <c r="BB39" s="57"/>
-      <c r="BC39" s="57"/>
-      <c r="BD39" s="57"/>
-      <c r="BE39" s="57"/>
-      <c r="BF39" s="57"/>
-      <c r="BG39" s="57"/>
-      <c r="BH39" s="57"/>
-      <c r="BI39" s="57"/>
-      <c r="BJ39" s="57"/>
-      <c r="BK39" s="57"/>
-      <c r="BL39" s="57"/>
-      <c r="BM39" s="57"/>
-      <c r="BN39" s="57"/>
-      <c r="BO39" s="57"/>
-      <c r="BP39" s="57"/>
-      <c r="BQ39" s="57"/>
-      <c r="BR39" s="57"/>
-      <c r="BS39" s="57"/>
-      <c r="BT39" s="57"/>
-      <c r="BV39" s="101">
+      <c r="M40" s="57"/>
+      <c r="N40" s="57"/>
+      <c r="O40" s="57"/>
+      <c r="P40" s="57"/>
+      <c r="Q40" s="57"/>
+      <c r="R40" s="57"/>
+      <c r="S40" s="57"/>
+      <c r="T40" s="57"/>
+      <c r="U40" s="57"/>
+      <c r="V40" s="57"/>
+      <c r="W40" s="57"/>
+      <c r="X40" s="57"/>
+      <c r="Y40" s="57"/>
+      <c r="Z40" s="57"/>
+      <c r="AA40" s="57"/>
+      <c r="AB40" s="57"/>
+      <c r="AC40" s="57"/>
+      <c r="AD40" s="57"/>
+      <c r="AE40" s="57"/>
+      <c r="AF40" s="57"/>
+      <c r="AG40" s="57"/>
+      <c r="AH40" s="57"/>
+      <c r="AI40" s="57"/>
+      <c r="AJ40" s="57"/>
+      <c r="AK40" s="57"/>
+      <c r="AL40" s="57"/>
+      <c r="AM40" s="57"/>
+      <c r="AN40" s="57"/>
+      <c r="AO40" s="57"/>
+      <c r="AP40" s="57"/>
+      <c r="AQ40" s="57"/>
+      <c r="AR40" s="57"/>
+      <c r="AS40" s="57"/>
+      <c r="AT40" s="57"/>
+      <c r="AU40" s="57"/>
+      <c r="AV40" s="57"/>
+      <c r="AW40" s="57"/>
+      <c r="AX40" s="57"/>
+      <c r="AY40" s="57"/>
+      <c r="AZ40" s="57"/>
+      <c r="BA40" s="57"/>
+      <c r="BB40" s="57"/>
+      <c r="BC40" s="57"/>
+      <c r="BD40" s="57"/>
+      <c r="BE40" s="57"/>
+      <c r="BF40" s="57"/>
+      <c r="BG40" s="57"/>
+      <c r="BH40" s="57"/>
+      <c r="BI40" s="57"/>
+      <c r="BJ40" s="57"/>
+      <c r="BK40" s="57"/>
+      <c r="BL40" s="57"/>
+      <c r="BM40" s="57"/>
+      <c r="BN40" s="57"/>
+      <c r="BO40" s="57"/>
+      <c r="BP40" s="57"/>
+      <c r="BQ40" s="57"/>
+      <c r="BR40" s="57"/>
+      <c r="BS40" s="57"/>
+      <c r="BT40" s="57"/>
+      <c r="BV40" s="101">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L40" s="102" t="s">
+    <row r="41" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L41" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M40" s="105">
-        <f t="shared" ref="M40:BT40" si="13">M38-M39</f>
+      <c r="M41" s="105">
+        <f t="shared" ref="M41:BT41" si="13">M39-M40</f>
         <v>28</v>
       </c>
-      <c r="N40" s="105">
+      <c r="N41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="O40" s="105">
+      <c r="O41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="P40" s="105">
+      <c r="P41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="Q40" s="105">
+      <c r="Q41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="R40" s="105">
+      <c r="R41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="S40" s="105">
+      <c r="S41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="T40" s="105">
+      <c r="T41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="U40" s="105">
+      <c r="U41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="V40" s="105">
+      <c r="V41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="W40" s="105">
+      <c r="W41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="X40" s="105">
+      <c r="X41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="Y40" s="105">
+      <c r="Y41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="Z40" s="105">
+      <c r="Z41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AA40" s="105">
+      <c r="AA41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AB40" s="105">
+      <c r="AB41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AC40" s="105">
+      <c r="AC41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AD40" s="105">
+      <c r="AD41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AE40" s="105">
+      <c r="AE41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AF40" s="105">
+      <c r="AF41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AG40" s="105">
+      <c r="AG41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AH40" s="105">
+      <c r="AH41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AI40" s="105">
+      <c r="AI41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AJ40" s="105">
+      <c r="AJ41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AK40" s="105">
+      <c r="AK41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AL40" s="105">
+      <c r="AL41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AM40" s="105">
+      <c r="AM41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AN40" s="105">
+      <c r="AN41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AO40" s="105">
+      <c r="AO41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AP40" s="105">
+      <c r="AP41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AQ40" s="105">
+      <c r="AQ41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AR40" s="105">
+      <c r="AR41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AS40" s="105">
+      <c r="AS41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AT40" s="105">
+      <c r="AT41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AU40" s="105">
+      <c r="AU41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AV40" s="105">
+      <c r="AV41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AW40" s="105">
+      <c r="AW41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AX40" s="105">
+      <c r="AX41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AY40" s="105">
+      <c r="AY41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AZ40" s="105">
+      <c r="AZ41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BA40" s="105">
+      <c r="BA41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BB40" s="105">
+      <c r="BB41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BC40" s="105">
+      <c r="BC41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BD40" s="105">
+      <c r="BD41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BE40" s="105">
+      <c r="BE41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BF40" s="105">
+      <c r="BF41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BG40" s="105">
+      <c r="BG41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BH40" s="105">
+      <c r="BH41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BI40" s="105">
+      <c r="BI41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BJ40" s="105">
+      <c r="BJ41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BK40" s="105">
+      <c r="BK41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BL40" s="105">
+      <c r="BL41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BM40" s="105">
+      <c r="BM41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BN40" s="105">
+      <c r="BN41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BO40" s="105">
+      <c r="BO41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BP40" s="105">
+      <c r="BP41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BQ40" s="105">
+      <c r="BQ41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BR40" s="105">
+      <c r="BR41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BS40" s="105">
+      <c r="BS41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BT40" s="105">
+      <c r="BT41" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BV40" s="101">
+      <c r="BV41" s="101">
         <f t="shared" si="12"/>
         <v>1680</v>
       </c>
     </row>
-    <row r="41" spans="2:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E44" s="195" t="s">
+    <row r="42" spans="2:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E45" s="198" t="s">
         <v>83</v>
       </c>
-      <c r="F44" s="159"/>
-      <c r="G44" s="159"/>
-      <c r="H44" s="159"/>
-      <c r="I44" s="159"/>
-      <c r="J44" s="159"/>
-      <c r="K44" s="159"/>
-      <c r="L44" s="159"/>
-      <c r="M44" s="159"/>
-      <c r="N44" s="159"/>
-      <c r="O44" s="159"/>
-      <c r="P44" s="159"/>
-      <c r="Q44" s="159"/>
-      <c r="R44" s="159"/>
-      <c r="S44" s="159"/>
-      <c r="T44" s="159"/>
-      <c r="U44" s="159"/>
-      <c r="V44" s="159"/>
-      <c r="W44" s="159"/>
-      <c r="X44" s="159"/>
-      <c r="Y44" s="159"/>
-      <c r="Z44" s="159"/>
-      <c r="AA44" s="159"/>
-      <c r="AB44" s="159"/>
-      <c r="AC44" s="159"/>
-      <c r="AD44" s="159"/>
-      <c r="AE44" s="159"/>
-      <c r="AF44" s="159"/>
-      <c r="AG44" s="159"/>
-      <c r="AH44" s="159"/>
-      <c r="AI44" s="159"/>
-      <c r="AJ44" s="159"/>
-      <c r="AK44" s="159"/>
-      <c r="AL44" s="159"/>
-      <c r="AM44" s="159"/>
-      <c r="AN44" s="159"/>
-      <c r="AO44" s="159"/>
-      <c r="AP44" s="159"/>
-      <c r="AQ44" s="159"/>
-      <c r="AR44" s="159"/>
-      <c r="AS44" s="159"/>
-      <c r="AT44" s="159"/>
-      <c r="AU44" s="159"/>
-      <c r="AV44" s="159"/>
-      <c r="AW44" s="159"/>
-      <c r="AX44" s="159"/>
-      <c r="AY44" s="159"/>
-      <c r="AZ44" s="159"/>
-      <c r="BA44" s="159"/>
-      <c r="BB44" s="160"/>
+      <c r="F45" s="181"/>
+      <c r="G45" s="181"/>
+      <c r="H45" s="181"/>
+      <c r="I45" s="181"/>
+      <c r="J45" s="181"/>
+      <c r="K45" s="181"/>
+      <c r="L45" s="181"/>
+      <c r="M45" s="181"/>
+      <c r="N45" s="181"/>
+      <c r="O45" s="181"/>
+      <c r="P45" s="181"/>
+      <c r="Q45" s="181"/>
+      <c r="R45" s="181"/>
+      <c r="S45" s="181"/>
+      <c r="T45" s="181"/>
+      <c r="U45" s="181"/>
+      <c r="V45" s="181"/>
+      <c r="W45" s="181"/>
+      <c r="X45" s="181"/>
+      <c r="Y45" s="181"/>
+      <c r="Z45" s="181"/>
+      <c r="AA45" s="181"/>
+      <c r="AB45" s="181"/>
+      <c r="AC45" s="181"/>
+      <c r="AD45" s="181"/>
+      <c r="AE45" s="181"/>
+      <c r="AF45" s="181"/>
+      <c r="AG45" s="181"/>
+      <c r="AH45" s="181"/>
+      <c r="AI45" s="181"/>
+      <c r="AJ45" s="181"/>
+      <c r="AK45" s="181"/>
+      <c r="AL45" s="181"/>
+      <c r="AM45" s="181"/>
+      <c r="AN45" s="181"/>
+      <c r="AO45" s="181"/>
+      <c r="AP45" s="181"/>
+      <c r="AQ45" s="181"/>
+      <c r="AR45" s="181"/>
+      <c r="AS45" s="181"/>
+      <c r="AT45" s="181"/>
+      <c r="AU45" s="181"/>
+      <c r="AV45" s="181"/>
+      <c r="AW45" s="181"/>
+      <c r="AX45" s="181"/>
+      <c r="AY45" s="181"/>
+      <c r="AZ45" s="181"/>
+      <c r="BA45" s="181"/>
+      <c r="BB45" s="182"/>
     </row>
-    <row r="45" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="3:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C49" s="108"/>
-      <c r="D49" s="108"/>
+    <row r="49" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="3:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C50" s="108"/>
+      <c r="D50" s="108"/>
     </row>
-    <row r="50" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17235,16 +17340,10 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="E44:BB44"/>
+    <mergeCell ref="E45:BB45"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
     <mergeCell ref="BP8:BT8"/>
@@ -17260,6 +17359,13 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
first version of central server for certification service
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e15298e05a6af3ae/Università/Magistrale/LabAdvProg/Proj/AnimalDEX/AnimalDex/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{EA4D58A3-898E-4E98-BD04-C05701569307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53597F68-8830-4B01-9614-D3680630387A}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{EA4D58A3-898E-4E98-BD04-C05701569307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{615EB0D6-207B-4261-B789-CD654BC2D032}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLE Gantt Chart &amp; Burndown" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="224">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -702,6 +702,12 @@
   </si>
   <si>
     <t>Communication between certification and recognition service</t>
+  </si>
+  <si>
+    <t>2,8</t>
+  </si>
+  <si>
+    <t>First version of central server</t>
   </si>
 </sst>
 </file>
@@ -2030,7 +2036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2428,53 +2434,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2505,10 +2470,54 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -4900,7 +4909,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$41</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4957,7 +4966,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$38:$BT$38</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$39:$BT$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5146,7 +5155,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$41:$BT$41</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$42:$BT$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5193,7 +5202,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$39</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5216,7 +5225,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$38:$BT$38</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$39:$BT$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5405,7 +5414,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$39:$BT$39</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$40:$BT$40</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5604,7 +5613,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$40</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5627,7 +5636,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$38:$BT$38</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$39:$BT$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5816,7 +5825,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$40:$BT$40</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$41:$BT$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6358,7 +6367,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="27632025" cy="7553325"/>
@@ -6420,6 +6429,10 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6903,19 +6916,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="182" t="str">
+      <c r="BK2" s="165" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="183"/>
-      <c r="BM2" s="183"/>
-      <c r="BN2" s="183"/>
-      <c r="BO2" s="183"/>
-      <c r="BP2" s="183"/>
-      <c r="BQ2" s="183"/>
-      <c r="BR2" s="183"/>
-      <c r="BS2" s="183"/>
-      <c r="BT2" s="183"/>
+      <c r="BL2" s="166"/>
+      <c r="BM2" s="166"/>
+      <c r="BN2" s="166"/>
+      <c r="BO2" s="166"/>
+      <c r="BP2" s="166"/>
+      <c r="BQ2" s="166"/>
+      <c r="BR2" s="166"/>
+      <c r="BS2" s="166"/>
+      <c r="BT2" s="166"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -6943,7 +6956,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="184" t="s">
+      <c r="K4" s="167" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7020,7 +7033,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="185"/>
+      <c r="K5" s="168"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7095,7 +7108,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="185"/>
+      <c r="K6" s="168"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7170,7 +7183,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="185"/>
+      <c r="K7" s="168"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7245,7 +7258,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="186"/>
+      <c r="K8" s="169"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7311,124 +7324,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="187" t="s">
+      <c r="B9" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="189" t="s">
+      <c r="C9" s="172" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="191" t="s">
+      <c r="D9" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="193" t="s">
+      <c r="E9" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="194"/>
-      <c r="G9" s="195"/>
-      <c r="H9" s="196" t="s">
+      <c r="F9" s="177"/>
+      <c r="G9" s="178"/>
+      <c r="H9" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="164" t="s">
+      <c r="I9" s="184" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="166" t="s">
+      <c r="J9" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="168" t="s">
+      <c r="K9" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="169" t="s">
+      <c r="L9" s="189" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="171" t="s">
+      <c r="M9" s="191" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="172"/>
-      <c r="O9" s="172"/>
-      <c r="P9" s="172"/>
-      <c r="Q9" s="173"/>
-      <c r="R9" s="174" t="s">
+      <c r="N9" s="163"/>
+      <c r="O9" s="163"/>
+      <c r="P9" s="163"/>
+      <c r="Q9" s="192"/>
+      <c r="R9" s="193" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="172"/>
-      <c r="T9" s="172"/>
-      <c r="U9" s="172"/>
-      <c r="V9" s="173"/>
-      <c r="W9" s="174" t="s">
+      <c r="S9" s="163"/>
+      <c r="T9" s="163"/>
+      <c r="U9" s="163"/>
+      <c r="V9" s="192"/>
+      <c r="W9" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="172"/>
-      <c r="Y9" s="172"/>
-      <c r="Z9" s="172"/>
-      <c r="AA9" s="175"/>
-      <c r="AB9" s="176" t="s">
+      <c r="X9" s="163"/>
+      <c r="Y9" s="163"/>
+      <c r="Z9" s="163"/>
+      <c r="AA9" s="164"/>
+      <c r="AB9" s="194" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="172"/>
-      <c r="AD9" s="172"/>
-      <c r="AE9" s="172"/>
-      <c r="AF9" s="173"/>
-      <c r="AG9" s="177" t="s">
+      <c r="AC9" s="163"/>
+      <c r="AD9" s="163"/>
+      <c r="AE9" s="163"/>
+      <c r="AF9" s="192"/>
+      <c r="AG9" s="195" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="172"/>
-      <c r="AI9" s="172"/>
-      <c r="AJ9" s="172"/>
-      <c r="AK9" s="173"/>
-      <c r="AL9" s="177" t="s">
+      <c r="AH9" s="163"/>
+      <c r="AI9" s="163"/>
+      <c r="AJ9" s="163"/>
+      <c r="AK9" s="192"/>
+      <c r="AL9" s="195" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="172"/>
-      <c r="AN9" s="172"/>
-      <c r="AO9" s="172"/>
-      <c r="AP9" s="175"/>
-      <c r="AQ9" s="178" t="s">
+      <c r="AM9" s="163"/>
+      <c r="AN9" s="163"/>
+      <c r="AO9" s="163"/>
+      <c r="AP9" s="164"/>
+      <c r="AQ9" s="196" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="172"/>
-      <c r="AS9" s="172"/>
-      <c r="AT9" s="172"/>
-      <c r="AU9" s="173"/>
-      <c r="AV9" s="179" t="s">
+      <c r="AR9" s="163"/>
+      <c r="AS9" s="163"/>
+      <c r="AT9" s="163"/>
+      <c r="AU9" s="192"/>
+      <c r="AV9" s="197" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="172"/>
-      <c r="AX9" s="172"/>
-      <c r="AY9" s="172"/>
-      <c r="AZ9" s="173"/>
-      <c r="BA9" s="179" t="s">
+      <c r="AW9" s="163"/>
+      <c r="AX9" s="163"/>
+      <c r="AY9" s="163"/>
+      <c r="AZ9" s="192"/>
+      <c r="BA9" s="197" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="172"/>
-      <c r="BC9" s="172"/>
-      <c r="BD9" s="172"/>
-      <c r="BE9" s="175"/>
-      <c r="BF9" s="180" t="s">
+      <c r="BB9" s="163"/>
+      <c r="BC9" s="163"/>
+      <c r="BD9" s="163"/>
+      <c r="BE9" s="164"/>
+      <c r="BF9" s="198" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="172"/>
-      <c r="BH9" s="172"/>
-      <c r="BI9" s="172"/>
-      <c r="BJ9" s="173"/>
-      <c r="BK9" s="181" t="s">
+      <c r="BG9" s="163"/>
+      <c r="BH9" s="163"/>
+      <c r="BI9" s="163"/>
+      <c r="BJ9" s="192"/>
+      <c r="BK9" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="172"/>
-      <c r="BM9" s="172"/>
-      <c r="BN9" s="172"/>
-      <c r="BO9" s="173"/>
-      <c r="BP9" s="181" t="s">
+      <c r="BL9" s="163"/>
+      <c r="BM9" s="163"/>
+      <c r="BN9" s="163"/>
+      <c r="BO9" s="192"/>
+      <c r="BP9" s="162" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="172"/>
-      <c r="BR9" s="172"/>
-      <c r="BS9" s="172"/>
-      <c r="BT9" s="175"/>
+      <c r="BQ9" s="163"/>
+      <c r="BR9" s="163"/>
+      <c r="BS9" s="163"/>
+      <c r="BT9" s="164"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="188"/>
-      <c r="C10" s="190"/>
-      <c r="D10" s="192"/>
+      <c r="B10" s="171"/>
+      <c r="C10" s="173"/>
+      <c r="D10" s="175"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7438,11 +7451,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="197"/>
-      <c r="I10" s="165"/>
-      <c r="J10" s="167"/>
-      <c r="K10" s="167"/>
-      <c r="L10" s="170"/>
+      <c r="H10" s="180"/>
+      <c r="I10" s="185"/>
+      <c r="J10" s="187"/>
+      <c r="K10" s="187"/>
+      <c r="L10" s="190"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11051,80 +11064,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="161" t="str">
+      <c r="B45" s="181" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="162"/>
-      <c r="D45" s="162"/>
-      <c r="E45" s="162"/>
-      <c r="F45" s="162"/>
-      <c r="G45" s="162"/>
-      <c r="H45" s="162"/>
-      <c r="I45" s="162"/>
-      <c r="J45" s="162"/>
-      <c r="K45" s="162"/>
-      <c r="L45" s="162"/>
-      <c r="M45" s="162"/>
-      <c r="N45" s="162"/>
-      <c r="O45" s="162"/>
-      <c r="P45" s="162"/>
-      <c r="Q45" s="162"/>
-      <c r="R45" s="162"/>
-      <c r="S45" s="162"/>
-      <c r="T45" s="162"/>
-      <c r="U45" s="162"/>
-      <c r="V45" s="162"/>
-      <c r="W45" s="162"/>
-      <c r="X45" s="162"/>
-      <c r="Y45" s="162"/>
-      <c r="Z45" s="162"/>
-      <c r="AA45" s="162"/>
-      <c r="AB45" s="162"/>
-      <c r="AC45" s="162"/>
-      <c r="AD45" s="162"/>
-      <c r="AE45" s="162"/>
-      <c r="AF45" s="162"/>
-      <c r="AG45" s="162"/>
-      <c r="AH45" s="162"/>
-      <c r="AI45" s="162"/>
-      <c r="AJ45" s="162"/>
-      <c r="AK45" s="162"/>
-      <c r="AL45" s="162"/>
-      <c r="AM45" s="162"/>
-      <c r="AN45" s="162"/>
-      <c r="AO45" s="162"/>
-      <c r="AP45" s="162"/>
-      <c r="AQ45" s="162"/>
-      <c r="AR45" s="162"/>
-      <c r="AS45" s="162"/>
-      <c r="AT45" s="162"/>
-      <c r="AU45" s="162"/>
-      <c r="AV45" s="162"/>
-      <c r="AW45" s="162"/>
-      <c r="AX45" s="162"/>
-      <c r="AY45" s="162"/>
-      <c r="AZ45" s="162"/>
-      <c r="BA45" s="162"/>
-      <c r="BB45" s="162"/>
-      <c r="BC45" s="162"/>
-      <c r="BD45" s="162"/>
-      <c r="BE45" s="162"/>
-      <c r="BF45" s="162"/>
-      <c r="BG45" s="162"/>
-      <c r="BH45" s="162"/>
-      <c r="BI45" s="162"/>
-      <c r="BJ45" s="162"/>
-      <c r="BK45" s="162"/>
-      <c r="BL45" s="162"/>
-      <c r="BM45" s="162"/>
-      <c r="BN45" s="162"/>
-      <c r="BO45" s="162"/>
-      <c r="BP45" s="162"/>
-      <c r="BQ45" s="162"/>
-      <c r="BR45" s="162"/>
-      <c r="BS45" s="162"/>
-      <c r="BT45" s="163"/>
+      <c r="C45" s="182"/>
+      <c r="D45" s="182"/>
+      <c r="E45" s="182"/>
+      <c r="F45" s="182"/>
+      <c r="G45" s="182"/>
+      <c r="H45" s="182"/>
+      <c r="I45" s="182"/>
+      <c r="J45" s="182"/>
+      <c r="K45" s="182"/>
+      <c r="L45" s="182"/>
+      <c r="M45" s="182"/>
+      <c r="N45" s="182"/>
+      <c r="O45" s="182"/>
+      <c r="P45" s="182"/>
+      <c r="Q45" s="182"/>
+      <c r="R45" s="182"/>
+      <c r="S45" s="182"/>
+      <c r="T45" s="182"/>
+      <c r="U45" s="182"/>
+      <c r="V45" s="182"/>
+      <c r="W45" s="182"/>
+      <c r="X45" s="182"/>
+      <c r="Y45" s="182"/>
+      <c r="Z45" s="182"/>
+      <c r="AA45" s="182"/>
+      <c r="AB45" s="182"/>
+      <c r="AC45" s="182"/>
+      <c r="AD45" s="182"/>
+      <c r="AE45" s="182"/>
+      <c r="AF45" s="182"/>
+      <c r="AG45" s="182"/>
+      <c r="AH45" s="182"/>
+      <c r="AI45" s="182"/>
+      <c r="AJ45" s="182"/>
+      <c r="AK45" s="182"/>
+      <c r="AL45" s="182"/>
+      <c r="AM45" s="182"/>
+      <c r="AN45" s="182"/>
+      <c r="AO45" s="182"/>
+      <c r="AP45" s="182"/>
+      <c r="AQ45" s="182"/>
+      <c r="AR45" s="182"/>
+      <c r="AS45" s="182"/>
+      <c r="AT45" s="182"/>
+      <c r="AU45" s="182"/>
+      <c r="AV45" s="182"/>
+      <c r="AW45" s="182"/>
+      <c r="AX45" s="182"/>
+      <c r="AY45" s="182"/>
+      <c r="AZ45" s="182"/>
+      <c r="BA45" s="182"/>
+      <c r="BB45" s="182"/>
+      <c r="BC45" s="182"/>
+      <c r="BD45" s="182"/>
+      <c r="BE45" s="182"/>
+      <c r="BF45" s="182"/>
+      <c r="BG45" s="182"/>
+      <c r="BH45" s="182"/>
+      <c r="BI45" s="182"/>
+      <c r="BJ45" s="182"/>
+      <c r="BK45" s="182"/>
+      <c r="BL45" s="182"/>
+      <c r="BM45" s="182"/>
+      <c r="BN45" s="182"/>
+      <c r="BO45" s="182"/>
+      <c r="BP45" s="182"/>
+      <c r="BQ45" s="182"/>
+      <c r="BR45" s="182"/>
+      <c r="BS45" s="182"/>
+      <c r="BT45" s="183"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12087,14 +12100,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12111,6 +12116,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12123,10 +12136,10 @@
     <tabColor rgb="FF7B3C16"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:BV1002"/>
+  <dimension ref="B1:BV1003"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH24" sqref="AH24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12239,7 +12252,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="184" t="s">
+      <c r="K3" s="167" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12316,7 +12329,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="185"/>
+      <c r="K4" s="168"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12390,7 +12403,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="185"/>
+      <c r="K5" s="168"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12465,7 +12478,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="185"/>
+      <c r="K6" s="168"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12540,7 +12553,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="186"/>
+      <c r="K7" s="169"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12606,124 +12619,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="187" t="s">
+      <c r="B8" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="189" t="s">
+      <c r="C8" s="172" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="191" t="s">
+      <c r="D8" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="193" t="s">
+      <c r="E8" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="194"/>
-      <c r="G8" s="195"/>
-      <c r="H8" s="196" t="s">
+      <c r="F8" s="177"/>
+      <c r="G8" s="178"/>
+      <c r="H8" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="164" t="s">
+      <c r="I8" s="184" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="166" t="s">
+      <c r="J8" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="168" t="s">
+      <c r="K8" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="169" t="s">
+      <c r="L8" s="189" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="171" t="s">
+      <c r="M8" s="191" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="172"/>
-      <c r="O8" s="172"/>
-      <c r="P8" s="172"/>
-      <c r="Q8" s="173"/>
-      <c r="R8" s="174" t="s">
+      <c r="N8" s="163"/>
+      <c r="O8" s="163"/>
+      <c r="P8" s="163"/>
+      <c r="Q8" s="192"/>
+      <c r="R8" s="193" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="172"/>
-      <c r="T8" s="172"/>
-      <c r="U8" s="172"/>
-      <c r="V8" s="173"/>
-      <c r="W8" s="174" t="s">
+      <c r="S8" s="163"/>
+      <c r="T8" s="163"/>
+      <c r="U8" s="163"/>
+      <c r="V8" s="192"/>
+      <c r="W8" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="172"/>
-      <c r="Y8" s="172"/>
-      <c r="Z8" s="172"/>
-      <c r="AA8" s="175"/>
-      <c r="AB8" s="176" t="s">
+      <c r="X8" s="163"/>
+      <c r="Y8" s="163"/>
+      <c r="Z8" s="163"/>
+      <c r="AA8" s="164"/>
+      <c r="AB8" s="194" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="172"/>
-      <c r="AD8" s="172"/>
-      <c r="AE8" s="172"/>
-      <c r="AF8" s="173"/>
-      <c r="AG8" s="177" t="s">
+      <c r="AC8" s="163"/>
+      <c r="AD8" s="163"/>
+      <c r="AE8" s="163"/>
+      <c r="AF8" s="192"/>
+      <c r="AG8" s="195" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="172"/>
-      <c r="AI8" s="172"/>
-      <c r="AJ8" s="172"/>
-      <c r="AK8" s="173"/>
-      <c r="AL8" s="177" t="s">
+      <c r="AH8" s="163"/>
+      <c r="AI8" s="163"/>
+      <c r="AJ8" s="163"/>
+      <c r="AK8" s="192"/>
+      <c r="AL8" s="195" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="172"/>
-      <c r="AN8" s="172"/>
-      <c r="AO8" s="172"/>
-      <c r="AP8" s="175"/>
-      <c r="AQ8" s="178" t="s">
+      <c r="AM8" s="163"/>
+      <c r="AN8" s="163"/>
+      <c r="AO8" s="163"/>
+      <c r="AP8" s="164"/>
+      <c r="AQ8" s="196" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="172"/>
-      <c r="AS8" s="172"/>
-      <c r="AT8" s="172"/>
-      <c r="AU8" s="173"/>
-      <c r="AV8" s="179" t="s">
+      <c r="AR8" s="163"/>
+      <c r="AS8" s="163"/>
+      <c r="AT8" s="163"/>
+      <c r="AU8" s="192"/>
+      <c r="AV8" s="197" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="172"/>
-      <c r="AX8" s="172"/>
-      <c r="AY8" s="172"/>
-      <c r="AZ8" s="173"/>
-      <c r="BA8" s="179" t="s">
+      <c r="AW8" s="163"/>
+      <c r="AX8" s="163"/>
+      <c r="AY8" s="163"/>
+      <c r="AZ8" s="192"/>
+      <c r="BA8" s="197" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="172"/>
-      <c r="BC8" s="172"/>
-      <c r="BD8" s="172"/>
-      <c r="BE8" s="175"/>
-      <c r="BF8" s="180" t="s">
+      <c r="BB8" s="163"/>
+      <c r="BC8" s="163"/>
+      <c r="BD8" s="163"/>
+      <c r="BE8" s="164"/>
+      <c r="BF8" s="198" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="172"/>
-      <c r="BH8" s="172"/>
-      <c r="BI8" s="172"/>
-      <c r="BJ8" s="173"/>
-      <c r="BK8" s="181" t="s">
+      <c r="BG8" s="163"/>
+      <c r="BH8" s="163"/>
+      <c r="BI8" s="163"/>
+      <c r="BJ8" s="192"/>
+      <c r="BK8" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="172"/>
-      <c r="BM8" s="172"/>
-      <c r="BN8" s="172"/>
-      <c r="BO8" s="173"/>
-      <c r="BP8" s="181" t="s">
+      <c r="BL8" s="163"/>
+      <c r="BM8" s="163"/>
+      <c r="BN8" s="163"/>
+      <c r="BO8" s="192"/>
+      <c r="BP8" s="162" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="172"/>
-      <c r="BR8" s="172"/>
-      <c r="BS8" s="172"/>
-      <c r="BT8" s="175"/>
+      <c r="BQ8" s="163"/>
+      <c r="BR8" s="163"/>
+      <c r="BS8" s="163"/>
+      <c r="BT8" s="164"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="188"/>
-      <c r="C9" s="190"/>
-      <c r="D9" s="192"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="173"/>
+      <c r="D9" s="175"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12733,11 +12746,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="197"/>
-      <c r="I9" s="165"/>
-      <c r="J9" s="167"/>
-      <c r="K9" s="167"/>
-      <c r="L9" s="170"/>
+      <c r="H9" s="180"/>
+      <c r="I9" s="185"/>
+      <c r="J9" s="187"/>
+      <c r="K9" s="187"/>
+      <c r="L9" s="190"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -12946,7 +12959,7 @@
       <c r="J10" s="47"/>
       <c r="K10" s="48"/>
       <c r="L10" s="49">
-        <f t="shared" ref="L10:L36" si="0">F10/E10</f>
+        <f t="shared" ref="L10:L37" si="0">F10/E10</f>
         <v>1</v>
       </c>
       <c r="M10" s="50"/>
@@ -13706,7 +13719,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="58">
-        <f t="shared" ref="G18:G24" si="3">E18-F18</f>
+        <f t="shared" ref="G18:G25" si="3">E18-F18</f>
         <v>0</v>
       </c>
       <c r="H18" s="59">
@@ -14326,7 +14339,7 @@
       <c r="AE24" s="65"/>
       <c r="AF24" s="160"/>
       <c r="AG24" s="69"/>
-      <c r="AH24" s="199"/>
+      <c r="AH24" s="161"/>
       <c r="AI24" s="69"/>
       <c r="AJ24" s="69"/>
       <c r="AK24" s="69"/>
@@ -14366,194 +14379,206 @@
       <c r="BS24" s="65"/>
       <c r="BT24" s="68"/>
     </row>
-    <row r="25" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="53">
+    <row r="25" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="53" t="s">
+        <v>222</v>
+      </c>
+      <c r="C25" s="200" t="s">
+        <v>223</v>
+      </c>
+      <c r="D25" s="158" t="s">
+        <v>212</v>
+      </c>
+      <c r="E25" s="56">
+        <v>8</v>
+      </c>
+      <c r="F25" s="57">
+        <v>10</v>
+      </c>
+      <c r="G25" s="58">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="H25" s="59">
+        <v>2</v>
+      </c>
+      <c r="I25" s="159">
+        <v>45385</v>
+      </c>
+      <c r="J25" s="61">
+        <v>45387</v>
+      </c>
+      <c r="K25" s="62">
         <v>3</v>
       </c>
-      <c r="C25" s="73"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="42">
-        <f t="shared" ref="E25:G25" si="5">SUM(E26:E31)</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="43">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="44">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="75"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="49" t="e">
+      <c r="L25" s="63">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" s="50"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="51"/>
-      <c r="S25" s="51"/>
-      <c r="T25" s="51"/>
-      <c r="U25" s="51"/>
-      <c r="V25" s="51"/>
-      <c r="W25" s="51"/>
-      <c r="X25" s="51"/>
-      <c r="Y25" s="51"/>
-      <c r="Z25" s="51"/>
-      <c r="AA25" s="52"/>
-      <c r="AB25" s="50"/>
-      <c r="AC25" s="51"/>
-      <c r="AD25" s="51"/>
-      <c r="AE25" s="51"/>
-      <c r="AF25" s="51"/>
-      <c r="AG25" s="51"/>
-      <c r="AH25" s="51"/>
-      <c r="AI25" s="51"/>
-      <c r="AJ25" s="51"/>
-      <c r="AK25" s="51"/>
-      <c r="AL25" s="51"/>
-      <c r="AM25" s="51"/>
-      <c r="AN25" s="51"/>
-      <c r="AO25" s="51"/>
-      <c r="AP25" s="52"/>
-      <c r="AQ25" s="50"/>
-      <c r="AR25" s="51"/>
-      <c r="AS25" s="51"/>
-      <c r="AT25" s="51"/>
-      <c r="AU25" s="51"/>
-      <c r="AV25" s="51"/>
-      <c r="AW25" s="51"/>
-      <c r="AX25" s="51"/>
-      <c r="AY25" s="51"/>
-      <c r="AZ25" s="51"/>
-      <c r="BA25" s="51"/>
-      <c r="BB25" s="51"/>
-      <c r="BC25" s="51"/>
-      <c r="BD25" s="51"/>
-      <c r="BE25" s="52"/>
-      <c r="BF25" s="50"/>
-      <c r="BG25" s="51"/>
-      <c r="BH25" s="51"/>
-      <c r="BI25" s="51"/>
-      <c r="BJ25" s="51"/>
-      <c r="BK25" s="51"/>
-      <c r="BL25" s="51"/>
-      <c r="BM25" s="51"/>
-      <c r="BN25" s="51"/>
-      <c r="BO25" s="51"/>
-      <c r="BP25" s="51"/>
-      <c r="BQ25" s="51"/>
-      <c r="BR25" s="51"/>
-      <c r="BS25" s="51"/>
-      <c r="BT25" s="52"/>
+        <v>1.25</v>
+      </c>
+      <c r="M25" s="64"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="65"/>
+      <c r="R25" s="67"/>
+      <c r="S25" s="67"/>
+      <c r="T25" s="67"/>
+      <c r="U25" s="67"/>
+      <c r="V25" s="67"/>
+      <c r="W25" s="65"/>
+      <c r="X25" s="65"/>
+      <c r="Y25" s="65"/>
+      <c r="Z25" s="65"/>
+      <c r="AA25" s="68"/>
+      <c r="AB25" s="64"/>
+      <c r="AC25" s="65"/>
+      <c r="AE25" s="65"/>
+      <c r="AF25" s="160"/>
+      <c r="AG25" s="69"/>
+      <c r="AH25" s="161"/>
+      <c r="AI25" s="161"/>
+      <c r="AJ25" s="161"/>
+      <c r="AK25" s="160"/>
+      <c r="AL25" s="65"/>
+      <c r="AM25" s="65"/>
+      <c r="AN25" s="65"/>
+      <c r="AO25" s="65"/>
+      <c r="AP25" s="68"/>
+      <c r="AQ25" s="64"/>
+      <c r="AR25" s="65"/>
+      <c r="AS25" s="65"/>
+      <c r="AT25" s="65"/>
+      <c r="AU25" s="65"/>
+      <c r="AV25" s="70"/>
+      <c r="AW25" s="70"/>
+      <c r="AX25" s="70"/>
+      <c r="AY25" s="70"/>
+      <c r="AZ25" s="70"/>
+      <c r="BA25" s="65"/>
+      <c r="BB25" s="65"/>
+      <c r="BC25" s="65"/>
+      <c r="BD25" s="65"/>
+      <c r="BE25" s="68"/>
+      <c r="BF25" s="64"/>
+      <c r="BG25" s="65"/>
+      <c r="BH25" s="65"/>
+      <c r="BI25" s="65"/>
+      <c r="BJ25" s="65"/>
+      <c r="BK25" s="71"/>
+      <c r="BL25" s="71"/>
+      <c r="BM25" s="71"/>
+      <c r="BN25" s="71"/>
+      <c r="BO25" s="71"/>
+      <c r="BP25" s="65"/>
+      <c r="BQ25" s="65"/>
+      <c r="BR25" s="65"/>
+      <c r="BS25" s="65"/>
+      <c r="BT25" s="68"/>
     </row>
     <row r="26" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="53">
-        <v>3.1</v>
-      </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="58">
-        <f t="shared" ref="G26:G31" si="6">E26-F26</f>
+        <v>3</v>
+      </c>
+      <c r="C26" s="73"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="42">
+        <f t="shared" ref="E26:G26" si="5">SUM(E27:E32)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="59"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="62">
-        <f t="shared" ref="K26:K31" si="7">J26-I26+1</f>
-        <v>1</v>
-      </c>
-      <c r="L26" s="63" t="e">
+      <c r="F26" s="43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="44">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="75"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M26" s="64"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="65"/>
-      <c r="P26" s="65"/>
-      <c r="Q26" s="65"/>
-      <c r="R26" s="67"/>
-      <c r="S26" s="67"/>
-      <c r="T26" s="67"/>
-      <c r="U26" s="67"/>
-      <c r="V26" s="67"/>
-      <c r="W26" s="65"/>
-      <c r="X26" s="65"/>
-      <c r="Y26" s="65"/>
-      <c r="Z26" s="65"/>
-      <c r="AA26" s="68"/>
-      <c r="AB26" s="64"/>
-      <c r="AC26" s="65"/>
-      <c r="AD26" s="65"/>
-      <c r="AE26" s="65"/>
-      <c r="AF26" s="65"/>
-      <c r="AG26" s="69"/>
-      <c r="AH26" s="69"/>
-      <c r="AI26" s="69"/>
-      <c r="AJ26" s="69"/>
-      <c r="AK26" s="69"/>
-      <c r="AL26" s="65"/>
-      <c r="AM26" s="65"/>
-      <c r="AN26" s="65"/>
-      <c r="AO26" s="65"/>
-      <c r="AP26" s="68"/>
-      <c r="AQ26" s="112"/>
-      <c r="AR26" s="65"/>
-      <c r="AS26" s="65"/>
-      <c r="AT26" s="65"/>
-      <c r="AU26" s="65"/>
-      <c r="AV26" s="70"/>
-      <c r="AW26" s="70"/>
-      <c r="AX26" s="70"/>
-      <c r="AY26" s="70"/>
-      <c r="AZ26" s="70"/>
-      <c r="BA26" s="65"/>
-      <c r="BB26" s="65"/>
-      <c r="BC26" s="65"/>
-      <c r="BD26" s="65"/>
-      <c r="BE26" s="68"/>
-      <c r="BF26" s="64"/>
-      <c r="BG26" s="65"/>
-      <c r="BH26" s="65"/>
-      <c r="BI26" s="65"/>
-      <c r="BJ26" s="65"/>
-      <c r="BK26" s="71"/>
-      <c r="BL26" s="71"/>
-      <c r="BM26" s="71"/>
-      <c r="BN26" s="71"/>
-      <c r="BO26" s="71"/>
-      <c r="BP26" s="65"/>
-      <c r="BQ26" s="65"/>
-      <c r="BR26" s="65"/>
-      <c r="BS26" s="65"/>
-      <c r="BT26" s="68"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="51"/>
+      <c r="X26" s="51"/>
+      <c r="Y26" s="51"/>
+      <c r="Z26" s="51"/>
+      <c r="AA26" s="52"/>
+      <c r="AB26" s="50"/>
+      <c r="AC26" s="51"/>
+      <c r="AD26" s="51"/>
+      <c r="AE26" s="51"/>
+      <c r="AF26" s="51"/>
+      <c r="AG26" s="51"/>
+      <c r="AH26" s="51"/>
+      <c r="AI26" s="51"/>
+      <c r="AJ26" s="51"/>
+      <c r="AK26" s="51"/>
+      <c r="AL26" s="51"/>
+      <c r="AM26" s="51"/>
+      <c r="AN26" s="51"/>
+      <c r="AO26" s="51"/>
+      <c r="AP26" s="52"/>
+      <c r="AQ26" s="50"/>
+      <c r="AR26" s="51"/>
+      <c r="AS26" s="51"/>
+      <c r="AT26" s="51"/>
+      <c r="AU26" s="51"/>
+      <c r="AV26" s="51"/>
+      <c r="AW26" s="51"/>
+      <c r="AX26" s="51"/>
+      <c r="AY26" s="51"/>
+      <c r="AZ26" s="51"/>
+      <c r="BA26" s="51"/>
+      <c r="BB26" s="51"/>
+      <c r="BC26" s="51"/>
+      <c r="BD26" s="51"/>
+      <c r="BE26" s="52"/>
+      <c r="BF26" s="50"/>
+      <c r="BG26" s="51"/>
+      <c r="BH26" s="51"/>
+      <c r="BI26" s="51"/>
+      <c r="BJ26" s="51"/>
+      <c r="BK26" s="51"/>
+      <c r="BL26" s="51"/>
+      <c r="BM26" s="51"/>
+      <c r="BN26" s="51"/>
+      <c r="BO26" s="51"/>
+      <c r="BP26" s="51"/>
+      <c r="BQ26" s="51"/>
+      <c r="BR26" s="51"/>
+      <c r="BS26" s="51"/>
+      <c r="BT26" s="52"/>
     </row>
     <row r="27" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="53">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="C27" s="54"/>
       <c r="D27" s="55"/>
       <c r="E27" s="56"/>
       <c r="F27" s="57"/>
       <c r="G27" s="58">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="G27:G32" si="6">E27-F27</f>
         <v>0</v>
       </c>
       <c r="H27" s="59"/>
-      <c r="I27" s="157"/>
+      <c r="I27" s="60"/>
       <c r="J27" s="61"/>
       <c r="K27" s="62">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="K27:K32" si="7">J27-I27+1</f>
         <v>1</v>
       </c>
       <c r="L27" s="63" t="e">
@@ -14590,7 +14615,7 @@
       <c r="AN27" s="65"/>
       <c r="AO27" s="65"/>
       <c r="AP27" s="68"/>
-      <c r="AQ27" s="64"/>
+      <c r="AQ27" s="112"/>
       <c r="AR27" s="65"/>
       <c r="AS27" s="65"/>
       <c r="AT27" s="65"/>
@@ -14622,8 +14647,8 @@
       <c r="BT27" s="68"/>
     </row>
     <row r="28" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="53" t="s">
-        <v>60</v>
+      <c r="B28" s="53">
+        <v>3.2</v>
       </c>
       <c r="C28" s="54"/>
       <c r="D28" s="55"/>
@@ -14634,7 +14659,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="59"/>
-      <c r="I28" s="60"/>
+      <c r="I28" s="157"/>
       <c r="J28" s="61"/>
       <c r="K28" s="62">
         <f t="shared" si="7"/>
@@ -14707,7 +14732,7 @@
     </row>
     <row r="29" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="53" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C29" s="54"/>
       <c r="D29" s="55"/>
@@ -14790,8 +14815,8 @@
       <c r="BT29" s="68"/>
     </row>
     <row r="30" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="53">
-        <v>3.3</v>
+      <c r="B30" s="53" t="s">
+        <v>62</v>
       </c>
       <c r="C30" s="54"/>
       <c r="D30" s="55"/>
@@ -14874,8 +14899,8 @@
       <c r="BT30" s="68"/>
     </row>
     <row r="31" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="53" t="s">
-        <v>65</v>
+      <c r="B31" s="53">
+        <v>3.3</v>
       </c>
       <c r="C31" s="54"/>
       <c r="D31" s="55"/>
@@ -14958,193 +14983,193 @@
       <c r="BT31" s="68"/>
     </row>
     <row r="32" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="53">
-        <v>4</v>
-      </c>
-      <c r="C32" s="73"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="42">
-        <f t="shared" ref="E32:G32" si="8">SUM(E33:E36)</f>
+      <c r="B32" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="58">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F32" s="43">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="44">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="75"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="77"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="49" t="e">
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="62">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L32" s="63" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M32" s="50"/>
-      <c r="N32" s="51"/>
-      <c r="O32" s="51"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="51"/>
-      <c r="S32" s="51"/>
-      <c r="T32" s="51"/>
-      <c r="U32" s="51"/>
-      <c r="V32" s="51"/>
-      <c r="W32" s="51"/>
-      <c r="X32" s="51"/>
-      <c r="Y32" s="51"/>
-      <c r="Z32" s="51"/>
-      <c r="AA32" s="52"/>
-      <c r="AB32" s="50"/>
-      <c r="AC32" s="51"/>
-      <c r="AD32" s="51"/>
-      <c r="AE32" s="51"/>
-      <c r="AF32" s="51"/>
-      <c r="AG32" s="51"/>
-      <c r="AH32" s="51"/>
-      <c r="AI32" s="51"/>
-      <c r="AJ32" s="51"/>
-      <c r="AK32" s="51"/>
-      <c r="AL32" s="51"/>
-      <c r="AM32" s="51"/>
-      <c r="AN32" s="51"/>
-      <c r="AO32" s="51"/>
-      <c r="AP32" s="52"/>
-      <c r="AQ32" s="50"/>
-      <c r="AR32" s="51"/>
-      <c r="AS32" s="51"/>
-      <c r="AT32" s="51"/>
-      <c r="AU32" s="51"/>
-      <c r="AV32" s="51"/>
-      <c r="AW32" s="51"/>
-      <c r="AX32" s="51"/>
-      <c r="AY32" s="51"/>
-      <c r="AZ32" s="51"/>
-      <c r="BA32" s="51"/>
-      <c r="BB32" s="51"/>
-      <c r="BC32" s="51"/>
-      <c r="BD32" s="51"/>
-      <c r="BE32" s="52"/>
-      <c r="BF32" s="50"/>
-      <c r="BG32" s="51"/>
-      <c r="BH32" s="51"/>
-      <c r="BI32" s="51"/>
-      <c r="BJ32" s="51"/>
-      <c r="BK32" s="51"/>
-      <c r="BL32" s="51"/>
-      <c r="BM32" s="51"/>
-      <c r="BN32" s="51"/>
-      <c r="BO32" s="51"/>
-      <c r="BP32" s="51"/>
-      <c r="BQ32" s="51"/>
-      <c r="BR32" s="51"/>
-      <c r="BS32" s="51"/>
-      <c r="BT32" s="52"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="65"/>
+      <c r="O32" s="65"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="65"/>
+      <c r="R32" s="67"/>
+      <c r="S32" s="67"/>
+      <c r="T32" s="67"/>
+      <c r="U32" s="67"/>
+      <c r="V32" s="67"/>
+      <c r="W32" s="65"/>
+      <c r="X32" s="65"/>
+      <c r="Y32" s="65"/>
+      <c r="Z32" s="65"/>
+      <c r="AA32" s="68"/>
+      <c r="AB32" s="64"/>
+      <c r="AC32" s="65"/>
+      <c r="AD32" s="65"/>
+      <c r="AE32" s="65"/>
+      <c r="AF32" s="65"/>
+      <c r="AG32" s="69"/>
+      <c r="AH32" s="69"/>
+      <c r="AI32" s="69"/>
+      <c r="AJ32" s="69"/>
+      <c r="AK32" s="69"/>
+      <c r="AL32" s="65"/>
+      <c r="AM32" s="65"/>
+      <c r="AN32" s="65"/>
+      <c r="AO32" s="65"/>
+      <c r="AP32" s="68"/>
+      <c r="AQ32" s="64"/>
+      <c r="AR32" s="65"/>
+      <c r="AS32" s="65"/>
+      <c r="AT32" s="65"/>
+      <c r="AU32" s="65"/>
+      <c r="AV32" s="70"/>
+      <c r="AW32" s="70"/>
+      <c r="AX32" s="70"/>
+      <c r="AY32" s="70"/>
+      <c r="AZ32" s="70"/>
+      <c r="BA32" s="65"/>
+      <c r="BB32" s="65"/>
+      <c r="BC32" s="65"/>
+      <c r="BD32" s="65"/>
+      <c r="BE32" s="68"/>
+      <c r="BF32" s="64"/>
+      <c r="BG32" s="65"/>
+      <c r="BH32" s="65"/>
+      <c r="BI32" s="65"/>
+      <c r="BJ32" s="65"/>
+      <c r="BK32" s="71"/>
+      <c r="BL32" s="71"/>
+      <c r="BM32" s="71"/>
+      <c r="BN32" s="71"/>
+      <c r="BO32" s="71"/>
+      <c r="BP32" s="65"/>
+      <c r="BQ32" s="65"/>
+      <c r="BR32" s="65"/>
+      <c r="BS32" s="65"/>
+      <c r="BT32" s="68"/>
     </row>
     <row r="33" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="53">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="58">
-        <f t="shared" ref="G33:G36" si="9">E33-F33</f>
+        <v>4</v>
+      </c>
+      <c r="C33" s="73"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="42">
+        <f t="shared" ref="E33:G33" si="8">SUM(E34:E37)</f>
         <v>0</v>
       </c>
-      <c r="H33" s="59"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="62">
-        <f t="shared" ref="K33:K36" si="10">J33-I33+1</f>
-        <v>1</v>
-      </c>
-      <c r="L33" s="63" t="e">
+      <c r="F33" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="44">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="75"/>
+      <c r="I33" s="76"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="77"/>
+      <c r="L33" s="49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M33" s="64"/>
-      <c r="N33" s="65"/>
-      <c r="O33" s="65"/>
-      <c r="P33" s="65"/>
-      <c r="Q33" s="65"/>
-      <c r="R33" s="67"/>
-      <c r="S33" s="67"/>
-      <c r="T33" s="67"/>
-      <c r="U33" s="67"/>
-      <c r="V33" s="67"/>
-      <c r="W33" s="65"/>
-      <c r="X33" s="65"/>
-      <c r="Y33" s="65"/>
-      <c r="Z33" s="65"/>
-      <c r="AA33" s="68"/>
-      <c r="AB33" s="64"/>
-      <c r="AC33" s="65"/>
-      <c r="AD33" s="65"/>
-      <c r="AE33" s="65"/>
-      <c r="AF33" s="65"/>
-      <c r="AG33" s="69"/>
-      <c r="AH33" s="69"/>
-      <c r="AI33" s="69"/>
-      <c r="AJ33" s="69"/>
-      <c r="AK33" s="69"/>
-      <c r="AL33" s="65"/>
-      <c r="AM33" s="65"/>
-      <c r="AN33" s="65"/>
-      <c r="AO33" s="65"/>
-      <c r="AP33" s="68"/>
-      <c r="AQ33" s="64"/>
-      <c r="AR33" s="65"/>
-      <c r="AS33" s="65"/>
-      <c r="AT33" s="65"/>
-      <c r="AU33" s="65"/>
-      <c r="AV33" s="70"/>
-      <c r="AW33" s="70"/>
-      <c r="AX33" s="70"/>
-      <c r="AY33" s="70"/>
-      <c r="AZ33" s="70"/>
-      <c r="BA33" s="65"/>
-      <c r="BB33" s="65"/>
-      <c r="BC33" s="65"/>
-      <c r="BD33" s="65"/>
-      <c r="BE33" s="68"/>
-      <c r="BF33" s="113"/>
-      <c r="BG33" s="65"/>
-      <c r="BH33" s="65"/>
-      <c r="BI33" s="65"/>
-      <c r="BJ33" s="65"/>
-      <c r="BK33" s="71"/>
-      <c r="BL33" s="71"/>
-      <c r="BM33" s="71"/>
-      <c r="BN33" s="71"/>
-      <c r="BO33" s="71"/>
-      <c r="BP33" s="65"/>
-      <c r="BQ33" s="65"/>
-      <c r="BR33" s="65"/>
-      <c r="BS33" s="65"/>
-      <c r="BT33" s="68"/>
+      <c r="M33" s="50"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="51"/>
+      <c r="R33" s="51"/>
+      <c r="S33" s="51"/>
+      <c r="T33" s="51"/>
+      <c r="U33" s="51"/>
+      <c r="V33" s="51"/>
+      <c r="W33" s="51"/>
+      <c r="X33" s="51"/>
+      <c r="Y33" s="51"/>
+      <c r="Z33" s="51"/>
+      <c r="AA33" s="52"/>
+      <c r="AB33" s="50"/>
+      <c r="AC33" s="51"/>
+      <c r="AD33" s="51"/>
+      <c r="AE33" s="51"/>
+      <c r="AF33" s="51"/>
+      <c r="AG33" s="51"/>
+      <c r="AH33" s="51"/>
+      <c r="AI33" s="51"/>
+      <c r="AJ33" s="51"/>
+      <c r="AK33" s="51"/>
+      <c r="AL33" s="51"/>
+      <c r="AM33" s="51"/>
+      <c r="AN33" s="51"/>
+      <c r="AO33" s="51"/>
+      <c r="AP33" s="52"/>
+      <c r="AQ33" s="50"/>
+      <c r="AR33" s="51"/>
+      <c r="AS33" s="51"/>
+      <c r="AT33" s="51"/>
+      <c r="AU33" s="51"/>
+      <c r="AV33" s="51"/>
+      <c r="AW33" s="51"/>
+      <c r="AX33" s="51"/>
+      <c r="AY33" s="51"/>
+      <c r="AZ33" s="51"/>
+      <c r="BA33" s="51"/>
+      <c r="BB33" s="51"/>
+      <c r="BC33" s="51"/>
+      <c r="BD33" s="51"/>
+      <c r="BE33" s="52"/>
+      <c r="BF33" s="50"/>
+      <c r="BG33" s="51"/>
+      <c r="BH33" s="51"/>
+      <c r="BI33" s="51"/>
+      <c r="BJ33" s="51"/>
+      <c r="BK33" s="51"/>
+      <c r="BL33" s="51"/>
+      <c r="BM33" s="51"/>
+      <c r="BN33" s="51"/>
+      <c r="BO33" s="51"/>
+      <c r="BP33" s="51"/>
+      <c r="BQ33" s="51"/>
+      <c r="BR33" s="51"/>
+      <c r="BS33" s="51"/>
+      <c r="BT33" s="52"/>
     </row>
     <row r="34" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="53">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C34" s="54"/>
       <c r="D34" s="55"/>
       <c r="E34" s="56"/>
       <c r="F34" s="57"/>
       <c r="G34" s="58">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="G34:G37" si="9">E34-F34</f>
         <v>0</v>
       </c>
       <c r="H34" s="59"/>
       <c r="I34" s="60"/>
       <c r="J34" s="61"/>
       <c r="K34" s="62">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="K34:K37" si="10">J34-I34+1</f>
         <v>1</v>
       </c>
       <c r="L34" s="63" t="e">
@@ -15196,7 +15221,7 @@
       <c r="BC34" s="65"/>
       <c r="BD34" s="65"/>
       <c r="BE34" s="68"/>
-      <c r="BF34" s="64"/>
+      <c r="BF34" s="113"/>
       <c r="BG34" s="65"/>
       <c r="BH34" s="65"/>
       <c r="BI34" s="65"/>
@@ -15214,10 +15239,10 @@
     </row>
     <row r="35" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="53">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="C35" s="54"/>
-      <c r="D35" s="80"/>
+      <c r="D35" s="55"/>
       <c r="E35" s="56"/>
       <c r="F35" s="57"/>
       <c r="G35" s="58">
@@ -15296,1205 +15321,1288 @@
       <c r="BS35" s="65"/>
       <c r="BT35" s="68"/>
     </row>
-    <row r="36" spans="2:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="82"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="85"/>
-      <c r="G36" s="86">
+    <row r="36" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="53">
+        <v>4.3</v>
+      </c>
+      <c r="C36" s="54"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="58">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H36" s="87"/>
-      <c r="I36" s="88"/>
-      <c r="J36" s="89"/>
-      <c r="K36" s="90">
+      <c r="H36" s="59"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="62">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="L36" s="91" t="e">
+      <c r="L36" s="63" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M36" s="92"/>
-      <c r="N36" s="93"/>
-      <c r="O36" s="93"/>
-      <c r="P36" s="93"/>
-      <c r="Q36" s="93"/>
-      <c r="R36" s="94"/>
-      <c r="S36" s="94"/>
-      <c r="T36" s="94"/>
-      <c r="U36" s="94"/>
-      <c r="V36" s="94"/>
-      <c r="W36" s="93"/>
-      <c r="X36" s="93"/>
-      <c r="Y36" s="93"/>
-      <c r="Z36" s="93"/>
-      <c r="AA36" s="95"/>
-      <c r="AB36" s="92"/>
-      <c r="AC36" s="93"/>
-      <c r="AD36" s="93"/>
-      <c r="AE36" s="93"/>
-      <c r="AF36" s="93"/>
-      <c r="AG36" s="96"/>
-      <c r="AH36" s="96"/>
-      <c r="AI36" s="96"/>
-      <c r="AJ36" s="96"/>
-      <c r="AK36" s="96"/>
-      <c r="AL36" s="93"/>
-      <c r="AM36" s="93"/>
-      <c r="AN36" s="93"/>
-      <c r="AO36" s="93"/>
-      <c r="AP36" s="95"/>
-      <c r="AQ36" s="92"/>
-      <c r="AR36" s="93"/>
-      <c r="AS36" s="93"/>
-      <c r="AT36" s="93"/>
-      <c r="AU36" s="93"/>
-      <c r="AV36" s="97"/>
-      <c r="AW36" s="97"/>
-      <c r="AX36" s="97"/>
-      <c r="AY36" s="97"/>
-      <c r="AZ36" s="97"/>
-      <c r="BA36" s="93"/>
-      <c r="BB36" s="93"/>
-      <c r="BC36" s="93"/>
-      <c r="BD36" s="93"/>
-      <c r="BE36" s="95"/>
-      <c r="BF36" s="92"/>
-      <c r="BG36" s="93"/>
-      <c r="BH36" s="93"/>
-      <c r="BI36" s="93"/>
-      <c r="BJ36" s="93"/>
-      <c r="BK36" s="98"/>
-      <c r="BL36" s="98"/>
-      <c r="BM36" s="98"/>
-      <c r="BN36" s="98"/>
-      <c r="BO36" s="98"/>
-      <c r="BP36" s="93"/>
-      <c r="BQ36" s="93"/>
-      <c r="BR36" s="93"/>
-      <c r="BS36" s="93"/>
-      <c r="BT36" s="95"/>
+      <c r="M36" s="64"/>
+      <c r="N36" s="65"/>
+      <c r="O36" s="65"/>
+      <c r="P36" s="65"/>
+      <c r="Q36" s="65"/>
+      <c r="R36" s="67"/>
+      <c r="S36" s="67"/>
+      <c r="T36" s="67"/>
+      <c r="U36" s="67"/>
+      <c r="V36" s="67"/>
+      <c r="W36" s="65"/>
+      <c r="X36" s="65"/>
+      <c r="Y36" s="65"/>
+      <c r="Z36" s="65"/>
+      <c r="AA36" s="68"/>
+      <c r="AB36" s="64"/>
+      <c r="AC36" s="65"/>
+      <c r="AD36" s="65"/>
+      <c r="AE36" s="65"/>
+      <c r="AF36" s="65"/>
+      <c r="AG36" s="69"/>
+      <c r="AH36" s="69"/>
+      <c r="AI36" s="69"/>
+      <c r="AJ36" s="69"/>
+      <c r="AK36" s="69"/>
+      <c r="AL36" s="65"/>
+      <c r="AM36" s="65"/>
+      <c r="AN36" s="65"/>
+      <c r="AO36" s="65"/>
+      <c r="AP36" s="68"/>
+      <c r="AQ36" s="64"/>
+      <c r="AR36" s="65"/>
+      <c r="AS36" s="65"/>
+      <c r="AT36" s="65"/>
+      <c r="AU36" s="65"/>
+      <c r="AV36" s="70"/>
+      <c r="AW36" s="70"/>
+      <c r="AX36" s="70"/>
+      <c r="AY36" s="70"/>
+      <c r="AZ36" s="70"/>
+      <c r="BA36" s="65"/>
+      <c r="BB36" s="65"/>
+      <c r="BC36" s="65"/>
+      <c r="BD36" s="65"/>
+      <c r="BE36" s="68"/>
+      <c r="BF36" s="64"/>
+      <c r="BG36" s="65"/>
+      <c r="BH36" s="65"/>
+      <c r="BI36" s="65"/>
+      <c r="BJ36" s="65"/>
+      <c r="BK36" s="71"/>
+      <c r="BL36" s="71"/>
+      <c r="BM36" s="71"/>
+      <c r="BN36" s="71"/>
+      <c r="BO36" s="71"/>
+      <c r="BP36" s="65"/>
+      <c r="BQ36" s="65"/>
+      <c r="BR36" s="65"/>
+      <c r="BS36" s="65"/>
+      <c r="BT36" s="68"/>
     </row>
-    <row r="37" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E37" s="99" t="s">
-        <v>29</v>
-      </c>
-      <c r="F37" s="99" t="s">
-        <v>30</v>
-      </c>
-      <c r="G37" s="99" t="s">
-        <v>31</v>
-      </c>
-      <c r="H37" s="99" t="s">
-        <v>73</v>
-      </c>
-      <c r="I37" s="99" t="s">
-        <v>74</v>
-      </c>
+    <row r="37" spans="2:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="82"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="86">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="87"/>
+      <c r="I37" s="88"/>
+      <c r="J37" s="89"/>
+      <c r="K37" s="90">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="L37" s="91" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M37" s="92"/>
+      <c r="N37" s="93"/>
+      <c r="O37" s="93"/>
+      <c r="P37" s="93"/>
+      <c r="Q37" s="93"/>
+      <c r="R37" s="94"/>
+      <c r="S37" s="94"/>
+      <c r="T37" s="94"/>
+      <c r="U37" s="94"/>
+      <c r="V37" s="94"/>
+      <c r="W37" s="93"/>
+      <c r="X37" s="93"/>
+      <c r="Y37" s="93"/>
+      <c r="Z37" s="93"/>
+      <c r="AA37" s="95"/>
+      <c r="AB37" s="92"/>
+      <c r="AC37" s="93"/>
+      <c r="AD37" s="93"/>
+      <c r="AE37" s="93"/>
+      <c r="AF37" s="93"/>
+      <c r="AG37" s="96"/>
+      <c r="AH37" s="96"/>
+      <c r="AI37" s="96"/>
+      <c r="AJ37" s="96"/>
+      <c r="AK37" s="96"/>
+      <c r="AL37" s="93"/>
+      <c r="AM37" s="93"/>
+      <c r="AN37" s="93"/>
+      <c r="AO37" s="93"/>
+      <c r="AP37" s="95"/>
+      <c r="AQ37" s="92"/>
+      <c r="AR37" s="93"/>
+      <c r="AS37" s="93"/>
+      <c r="AT37" s="93"/>
+      <c r="AU37" s="93"/>
+      <c r="AV37" s="97"/>
+      <c r="AW37" s="97"/>
+      <c r="AX37" s="97"/>
+      <c r="AY37" s="97"/>
+      <c r="AZ37" s="97"/>
+      <c r="BA37" s="93"/>
+      <c r="BB37" s="93"/>
+      <c r="BC37" s="93"/>
+      <c r="BD37" s="93"/>
+      <c r="BE37" s="95"/>
+      <c r="BF37" s="92"/>
+      <c r="BG37" s="93"/>
+      <c r="BH37" s="93"/>
+      <c r="BI37" s="93"/>
+      <c r="BJ37" s="93"/>
+      <c r="BK37" s="98"/>
+      <c r="BL37" s="98"/>
+      <c r="BM37" s="98"/>
+      <c r="BN37" s="98"/>
+      <c r="BO37" s="98"/>
+      <c r="BP37" s="93"/>
+      <c r="BQ37" s="93"/>
+      <c r="BR37" s="93"/>
+      <c r="BS37" s="93"/>
+      <c r="BT37" s="95"/>
     </row>
     <row r="38" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="100" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" s="101">
-        <f>SUM(E11:E16,E18:E21,E26:E31,E33:E36)</f>
-        <v>28</v>
-      </c>
-      <c r="F38" s="101">
-        <f>SUM(F11:F16,F18:F21,F26:F31,F33:F36)</f>
-        <v>28</v>
-      </c>
-      <c r="G38" s="101">
-        <f>SUM(G11:G16,G18:G21,G26:G31,G33:G36)</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="101">
-        <v>60</v>
-      </c>
-      <c r="I38" s="101">
-        <f>E38/H38</f>
-        <v>0.46666666666666667</v>
-      </c>
-      <c r="L38" s="102" t="s">
-        <v>77</v>
-      </c>
-      <c r="M38" s="103">
-        <v>1</v>
-      </c>
-      <c r="N38" s="103">
-        <v>2</v>
-      </c>
-      <c r="O38" s="103">
-        <v>3</v>
-      </c>
-      <c r="P38" s="103">
-        <v>4</v>
-      </c>
-      <c r="Q38" s="103">
-        <v>5</v>
-      </c>
-      <c r="R38" s="103">
-        <v>6</v>
-      </c>
-      <c r="S38" s="103">
-        <v>7</v>
-      </c>
-      <c r="T38" s="103">
-        <v>8</v>
-      </c>
-      <c r="U38" s="103">
-        <v>9</v>
-      </c>
-      <c r="V38" s="103">
-        <v>10</v>
-      </c>
-      <c r="W38" s="103">
-        <v>11</v>
-      </c>
-      <c r="X38" s="103">
-        <v>12</v>
-      </c>
-      <c r="Y38" s="103">
-        <v>13</v>
-      </c>
-      <c r="Z38" s="103">
-        <v>14</v>
-      </c>
-      <c r="AA38" s="103">
-        <v>15</v>
-      </c>
-      <c r="AB38" s="103">
-        <v>16</v>
-      </c>
-      <c r="AC38" s="103">
-        <v>17</v>
-      </c>
-      <c r="AD38" s="103">
-        <v>18</v>
-      </c>
-      <c r="AE38" s="103">
-        <v>19</v>
-      </c>
-      <c r="AF38" s="103">
-        <v>20</v>
-      </c>
-      <c r="AG38" s="103">
-        <v>21</v>
-      </c>
-      <c r="AH38" s="103">
-        <v>22</v>
-      </c>
-      <c r="AI38" s="103">
-        <v>23</v>
-      </c>
-      <c r="AJ38" s="103">
-        <v>24</v>
-      </c>
-      <c r="AK38" s="103">
-        <v>25</v>
-      </c>
-      <c r="AL38" s="103">
-        <v>26</v>
-      </c>
-      <c r="AM38" s="103">
-        <v>27</v>
-      </c>
-      <c r="AN38" s="103">
-        <v>28</v>
-      </c>
-      <c r="AO38" s="103">
+      <c r="E38" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="AP38" s="103">
+      <c r="F38" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="AQ38" s="103">
+      <c r="G38" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="AR38" s="103">
-        <v>32</v>
-      </c>
-      <c r="AS38" s="103">
-        <v>33</v>
-      </c>
-      <c r="AT38" s="103">
-        <v>34</v>
-      </c>
-      <c r="AU38" s="103">
-        <v>35</v>
-      </c>
-      <c r="AV38" s="103">
-        <v>36</v>
-      </c>
-      <c r="AW38" s="103">
-        <v>37</v>
-      </c>
-      <c r="AX38" s="103">
-        <v>38</v>
-      </c>
-      <c r="AY38" s="103">
-        <v>39</v>
-      </c>
-      <c r="AZ38" s="103">
-        <v>40</v>
-      </c>
-      <c r="BA38" s="103">
-        <v>41</v>
-      </c>
-      <c r="BB38" s="103">
-        <v>42</v>
-      </c>
-      <c r="BC38" s="103">
-        <v>43</v>
-      </c>
-      <c r="BD38" s="103">
-        <v>44</v>
-      </c>
-      <c r="BE38" s="103">
-        <v>45</v>
-      </c>
-      <c r="BF38" s="103">
-        <v>46</v>
-      </c>
-      <c r="BG38" s="103">
-        <v>47</v>
-      </c>
-      <c r="BH38" s="103">
-        <v>48</v>
-      </c>
-      <c r="BI38" s="103">
-        <v>49</v>
-      </c>
-      <c r="BJ38" s="103">
-        <v>50</v>
-      </c>
-      <c r="BK38" s="103">
-        <v>51</v>
-      </c>
-      <c r="BL38" s="103">
-        <v>52</v>
-      </c>
-      <c r="BM38" s="103">
-        <v>53</v>
-      </c>
-      <c r="BN38" s="103">
-        <v>54</v>
-      </c>
-      <c r="BO38" s="103">
-        <v>55</v>
-      </c>
-      <c r="BP38" s="103">
-        <v>56</v>
-      </c>
-      <c r="BQ38" s="103">
-        <v>57</v>
-      </c>
-      <c r="BR38" s="103">
-        <v>58</v>
-      </c>
-      <c r="BS38" s="103">
-        <v>59</v>
-      </c>
-      <c r="BT38" s="103">
-        <v>60</v>
-      </c>
-      <c r="BV38" s="100" t="s">
-        <v>76</v>
+      <c r="H38" s="99" t="s">
+        <v>73</v>
+      </c>
+      <c r="I38" s="99" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H39" s="104" t="s">
-        <v>78</v>
+      <c r="C39" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="101">
+        <f>SUM(E11:E16,E18:E21,E27:E32,E34:E37)</f>
+        <v>28</v>
+      </c>
+      <c r="F39" s="101">
+        <f>SUM(F11:F16,F18:F21,F27:F32,F34:F37)</f>
+        <v>28</v>
+      </c>
+      <c r="G39" s="101">
+        <f>SUM(G11:G16,G18:G21,G27:G32,G34:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="101">
+        <v>60</v>
+      </c>
+      <c r="I39" s="101">
+        <f>E39/H39</f>
+        <v>0.46666666666666667</v>
       </c>
       <c r="L39" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="M39" s="105">
-        <f>E38</f>
+        <v>77</v>
+      </c>
+      <c r="M39" s="103">
+        <v>1</v>
+      </c>
+      <c r="N39" s="103">
+        <v>2</v>
+      </c>
+      <c r="O39" s="103">
+        <v>3</v>
+      </c>
+      <c r="P39" s="103">
+        <v>4</v>
+      </c>
+      <c r="Q39" s="103">
+        <v>5</v>
+      </c>
+      <c r="R39" s="103">
+        <v>6</v>
+      </c>
+      <c r="S39" s="103">
+        <v>7</v>
+      </c>
+      <c r="T39" s="103">
+        <v>8</v>
+      </c>
+      <c r="U39" s="103">
+        <v>9</v>
+      </c>
+      <c r="V39" s="103">
+        <v>10</v>
+      </c>
+      <c r="W39" s="103">
+        <v>11</v>
+      </c>
+      <c r="X39" s="103">
+        <v>12</v>
+      </c>
+      <c r="Y39" s="103">
+        <v>13</v>
+      </c>
+      <c r="Z39" s="103">
+        <v>14</v>
+      </c>
+      <c r="AA39" s="103">
+        <v>15</v>
+      </c>
+      <c r="AB39" s="103">
+        <v>16</v>
+      </c>
+      <c r="AC39" s="103">
+        <v>17</v>
+      </c>
+      <c r="AD39" s="103">
+        <v>18</v>
+      </c>
+      <c r="AE39" s="103">
+        <v>19</v>
+      </c>
+      <c r="AF39" s="103">
+        <v>20</v>
+      </c>
+      <c r="AG39" s="103">
+        <v>21</v>
+      </c>
+      <c r="AH39" s="103">
+        <v>22</v>
+      </c>
+      <c r="AI39" s="103">
+        <v>23</v>
+      </c>
+      <c r="AJ39" s="103">
+        <v>24</v>
+      </c>
+      <c r="AK39" s="103">
+        <v>25</v>
+      </c>
+      <c r="AL39" s="103">
+        <v>26</v>
+      </c>
+      <c r="AM39" s="103">
+        <v>27</v>
+      </c>
+      <c r="AN39" s="103">
         <v>28</v>
       </c>
-      <c r="N39" s="106">
-        <f>M39-I38</f>
-        <v>27.533333333333335</v>
-      </c>
-      <c r="O39" s="106">
-        <f>N39-I38</f>
-        <v>27.06666666666667</v>
-      </c>
-      <c r="P39" s="106">
-        <f>O39-I38</f>
-        <v>26.600000000000005</v>
-      </c>
-      <c r="Q39" s="106">
-        <f>P39-I38</f>
-        <v>26.13333333333334</v>
-      </c>
-      <c r="R39" s="106">
-        <f>Q39-I38</f>
-        <v>25.666666666666675</v>
-      </c>
-      <c r="S39" s="106">
-        <f>R39-I38</f>
-        <v>25.20000000000001</v>
-      </c>
-      <c r="T39" s="106">
-        <f>S39-I38</f>
-        <v>24.733333333333345</v>
-      </c>
-      <c r="U39" s="106">
-        <f>T39-I38</f>
-        <v>24.26666666666668</v>
-      </c>
-      <c r="V39" s="106">
-        <f>U39-I38</f>
-        <v>23.800000000000015</v>
-      </c>
-      <c r="W39" s="106">
-        <f>V39-I38</f>
-        <v>23.33333333333335</v>
-      </c>
-      <c r="X39" s="106">
-        <f>W39-I38</f>
-        <v>22.866666666666685</v>
-      </c>
-      <c r="Y39" s="106">
-        <f>X39-I38</f>
-        <v>22.40000000000002</v>
-      </c>
-      <c r="Z39" s="106">
-        <f>Y39-I38</f>
-        <v>21.933333333333355</v>
-      </c>
-      <c r="AA39" s="106">
-        <f>Z39-I38</f>
-        <v>21.46666666666669</v>
-      </c>
-      <c r="AB39" s="106">
-        <f>AA39-I38</f>
-        <v>21.000000000000025</v>
-      </c>
-      <c r="AC39" s="106">
-        <f>AB39-I38</f>
-        <v>20.53333333333336</v>
-      </c>
-      <c r="AD39" s="106">
-        <f>AC39-I38</f>
-        <v>20.066666666666695</v>
-      </c>
-      <c r="AE39" s="106">
-        <f>AD39-I38</f>
-        <v>19.60000000000003</v>
-      </c>
-      <c r="AF39" s="106">
-        <f>AE39-I38</f>
-        <v>19.133333333333365</v>
-      </c>
-      <c r="AG39" s="106">
-        <f>AF39-I38</f>
-        <v>18.6666666666667</v>
-      </c>
-      <c r="AH39" s="106">
-        <f>AG39-I38</f>
-        <v>18.200000000000035</v>
-      </c>
-      <c r="AI39" s="106">
-        <f>AH39-I38</f>
-        <v>17.73333333333337</v>
-      </c>
-      <c r="AJ39" s="106">
-        <f>AI39-I38</f>
-        <v>17.266666666666705</v>
-      </c>
-      <c r="AK39" s="106">
-        <f>AJ39-I38</f>
-        <v>16.80000000000004</v>
-      </c>
-      <c r="AL39" s="106">
-        <f>AK39-I38</f>
-        <v>16.333333333333375</v>
-      </c>
-      <c r="AM39" s="106">
-        <f>AL39-I38</f>
-        <v>15.866666666666708</v>
-      </c>
-      <c r="AN39" s="106">
-        <f>AM39-I38</f>
-        <v>15.400000000000041</v>
-      </c>
-      <c r="AO39" s="106">
-        <f>AN39-I38</f>
-        <v>14.933333333333374</v>
-      </c>
-      <c r="AP39" s="106">
-        <f>AO39-I38</f>
-        <v>14.466666666666708</v>
-      </c>
-      <c r="AQ39" s="106">
-        <f>AP39-I38</f>
-        <v>14.000000000000041</v>
-      </c>
-      <c r="AR39" s="106">
-        <f>AQ39-I38</f>
-        <v>13.533333333333374</v>
-      </c>
-      <c r="AS39" s="106">
-        <f>AR39-I38</f>
-        <v>13.066666666666707</v>
-      </c>
-      <c r="AT39" s="106">
-        <f>AS39-I38</f>
-        <v>12.600000000000041</v>
-      </c>
-      <c r="AU39" s="106">
-        <f>AT39-I38</f>
-        <v>12.133333333333374</v>
-      </c>
-      <c r="AV39" s="106">
-        <f>AU39-I38</f>
-        <v>11.666666666666707</v>
-      </c>
-      <c r="AW39" s="106">
-        <f>AV39-I38</f>
-        <v>11.20000000000004</v>
-      </c>
-      <c r="AX39" s="106">
-        <f>AW39-I38</f>
-        <v>10.733333333333373</v>
-      </c>
-      <c r="AY39" s="106">
-        <f>AX39-I38</f>
-        <v>10.266666666666707</v>
-      </c>
-      <c r="AZ39" s="106">
-        <f>AY39-I38</f>
-        <v>9.8000000000000398</v>
-      </c>
-      <c r="BA39" s="106">
-        <f>AZ39-I38</f>
-        <v>9.333333333333373</v>
-      </c>
-      <c r="BB39" s="106">
-        <f>BA39-I38</f>
-        <v>8.8666666666667062</v>
-      </c>
-      <c r="BC39" s="106">
-        <f>BB39-I38</f>
-        <v>8.4000000000000394</v>
-      </c>
-      <c r="BD39" s="106">
-        <f>BC39-I38</f>
-        <v>7.9333333333333727</v>
-      </c>
-      <c r="BE39" s="106">
-        <f>BD39-I38</f>
-        <v>7.4666666666667059</v>
-      </c>
-      <c r="BF39" s="106">
-        <f>BE39-I38</f>
-        <v>7.0000000000000391</v>
-      </c>
-      <c r="BG39" s="106">
-        <f>BF39-I38</f>
-        <v>6.5333333333333723</v>
-      </c>
-      <c r="BH39" s="106">
-        <f>BG39-I38</f>
-        <v>6.0666666666667055</v>
-      </c>
-      <c r="BI39" s="106">
-        <f>BH39-I38</f>
-        <v>5.6000000000000387</v>
-      </c>
-      <c r="BJ39" s="106">
-        <f>BI39-I38</f>
-        <v>5.1333333333333719</v>
-      </c>
-      <c r="BK39" s="106">
-        <f>BJ39-I38</f>
-        <v>4.6666666666667052</v>
-      </c>
-      <c r="BL39" s="106">
-        <f>BK39-I38</f>
-        <v>4.2000000000000384</v>
-      </c>
-      <c r="BM39" s="106">
-        <f>BL39-I38</f>
-        <v>3.7333333333333716</v>
-      </c>
-      <c r="BN39" s="106">
-        <f>BM39-I38</f>
-        <v>3.2666666666667048</v>
-      </c>
-      <c r="BO39" s="106">
-        <f>BN39-I38</f>
-        <v>2.800000000000038</v>
-      </c>
-      <c r="BP39" s="106">
-        <f>BO39-I38</f>
-        <v>2.3333333333333712</v>
-      </c>
-      <c r="BQ39" s="106">
-        <f>BP39-I38</f>
-        <v>1.8666666666667044</v>
-      </c>
-      <c r="BR39" s="106">
-        <f>BQ39-I38</f>
-        <v>1.4000000000000377</v>
-      </c>
-      <c r="BS39" s="106">
-        <f>BR39-I38</f>
-        <v>0.93333333333337098</v>
-      </c>
-      <c r="BT39" s="106">
-        <f>BS39-I38</f>
-        <v>0.46666666666670431</v>
-      </c>
-      <c r="BV39" s="101"/>
+      <c r="AO39" s="103">
+        <v>29</v>
+      </c>
+      <c r="AP39" s="103">
+        <v>30</v>
+      </c>
+      <c r="AQ39" s="103">
+        <v>31</v>
+      </c>
+      <c r="AR39" s="103">
+        <v>32</v>
+      </c>
+      <c r="AS39" s="103">
+        <v>33</v>
+      </c>
+      <c r="AT39" s="103">
+        <v>34</v>
+      </c>
+      <c r="AU39" s="103">
+        <v>35</v>
+      </c>
+      <c r="AV39" s="103">
+        <v>36</v>
+      </c>
+      <c r="AW39" s="103">
+        <v>37</v>
+      </c>
+      <c r="AX39" s="103">
+        <v>38</v>
+      </c>
+      <c r="AY39" s="103">
+        <v>39</v>
+      </c>
+      <c r="AZ39" s="103">
+        <v>40</v>
+      </c>
+      <c r="BA39" s="103">
+        <v>41</v>
+      </c>
+      <c r="BB39" s="103">
+        <v>42</v>
+      </c>
+      <c r="BC39" s="103">
+        <v>43</v>
+      </c>
+      <c r="BD39" s="103">
+        <v>44</v>
+      </c>
+      <c r="BE39" s="103">
+        <v>45</v>
+      </c>
+      <c r="BF39" s="103">
+        <v>46</v>
+      </c>
+      <c r="BG39" s="103">
+        <v>47</v>
+      </c>
+      <c r="BH39" s="103">
+        <v>48</v>
+      </c>
+      <c r="BI39" s="103">
+        <v>49</v>
+      </c>
+      <c r="BJ39" s="103">
+        <v>50</v>
+      </c>
+      <c r="BK39" s="103">
+        <v>51</v>
+      </c>
+      <c r="BL39" s="103">
+        <v>52</v>
+      </c>
+      <c r="BM39" s="103">
+        <v>53</v>
+      </c>
+      <c r="BN39" s="103">
+        <v>54</v>
+      </c>
+      <c r="BO39" s="103">
+        <v>55</v>
+      </c>
+      <c r="BP39" s="103">
+        <v>56</v>
+      </c>
+      <c r="BQ39" s="103">
+        <v>57</v>
+      </c>
+      <c r="BR39" s="103">
+        <v>58</v>
+      </c>
+      <c r="BS39" s="103">
+        <v>59</v>
+      </c>
+      <c r="BT39" s="103">
+        <v>60</v>
+      </c>
+      <c r="BV39" s="100" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="40" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H40" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="L40" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="M40" s="105">
+        <f>E39</f>
+        <v>28</v>
+      </c>
+      <c r="N40" s="106">
+        <f>M40-I39</f>
+        <v>27.533333333333335</v>
+      </c>
+      <c r="O40" s="106">
+        <f>N40-I39</f>
+        <v>27.06666666666667</v>
+      </c>
+      <c r="P40" s="106">
+        <f>O40-I39</f>
+        <v>26.600000000000005</v>
+      </c>
+      <c r="Q40" s="106">
+        <f>P40-I39</f>
+        <v>26.13333333333334</v>
+      </c>
+      <c r="R40" s="106">
+        <f>Q40-I39</f>
+        <v>25.666666666666675</v>
+      </c>
+      <c r="S40" s="106">
+        <f>R40-I39</f>
+        <v>25.20000000000001</v>
+      </c>
+      <c r="T40" s="106">
+        <f>S40-I39</f>
+        <v>24.733333333333345</v>
+      </c>
+      <c r="U40" s="106">
+        <f>T40-I39</f>
+        <v>24.26666666666668</v>
+      </c>
+      <c r="V40" s="106">
+        <f>U40-I39</f>
+        <v>23.800000000000015</v>
+      </c>
+      <c r="W40" s="106">
+        <f>V40-I39</f>
+        <v>23.33333333333335</v>
+      </c>
+      <c r="X40" s="106">
+        <f>W40-I39</f>
+        <v>22.866666666666685</v>
+      </c>
+      <c r="Y40" s="106">
+        <f>X40-I39</f>
+        <v>22.40000000000002</v>
+      </c>
+      <c r="Z40" s="106">
+        <f>Y40-I39</f>
+        <v>21.933333333333355</v>
+      </c>
+      <c r="AA40" s="106">
+        <f>Z40-I39</f>
+        <v>21.46666666666669</v>
+      </c>
+      <c r="AB40" s="106">
+        <f>AA40-I39</f>
+        <v>21.000000000000025</v>
+      </c>
+      <c r="AC40" s="106">
+        <f>AB40-I39</f>
+        <v>20.53333333333336</v>
+      </c>
+      <c r="AD40" s="106">
+        <f>AC40-I39</f>
+        <v>20.066666666666695</v>
+      </c>
+      <c r="AE40" s="106">
+        <f>AD40-I39</f>
+        <v>19.60000000000003</v>
+      </c>
+      <c r="AF40" s="106">
+        <f>AE40-I39</f>
+        <v>19.133333333333365</v>
+      </c>
+      <c r="AG40" s="106">
+        <f>AF40-I39</f>
+        <v>18.6666666666667</v>
+      </c>
+      <c r="AH40" s="106">
+        <f>AG40-I39</f>
+        <v>18.200000000000035</v>
+      </c>
+      <c r="AI40" s="106">
+        <f>AH40-I39</f>
+        <v>17.73333333333337</v>
+      </c>
+      <c r="AJ40" s="106">
+        <f>AI40-I39</f>
+        <v>17.266666666666705</v>
+      </c>
+      <c r="AK40" s="106">
+        <f>AJ40-I39</f>
+        <v>16.80000000000004</v>
+      </c>
+      <c r="AL40" s="106">
+        <f>AK40-I39</f>
+        <v>16.333333333333375</v>
+      </c>
+      <c r="AM40" s="106">
+        <f>AL40-I39</f>
+        <v>15.866666666666708</v>
+      </c>
+      <c r="AN40" s="106">
+        <f>AM40-I39</f>
+        <v>15.400000000000041</v>
+      </c>
+      <c r="AO40" s="106">
+        <f>AN40-I39</f>
+        <v>14.933333333333374</v>
+      </c>
+      <c r="AP40" s="106">
+        <f>AO40-I39</f>
+        <v>14.466666666666708</v>
+      </c>
+      <c r="AQ40" s="106">
+        <f>AP40-I39</f>
+        <v>14.000000000000041</v>
+      </c>
+      <c r="AR40" s="106">
+        <f>AQ40-I39</f>
+        <v>13.533333333333374</v>
+      </c>
+      <c r="AS40" s="106">
+        <f>AR40-I39</f>
+        <v>13.066666666666707</v>
+      </c>
+      <c r="AT40" s="106">
+        <f>AS40-I39</f>
+        <v>12.600000000000041</v>
+      </c>
+      <c r="AU40" s="106">
+        <f>AT40-I39</f>
+        <v>12.133333333333374</v>
+      </c>
+      <c r="AV40" s="106">
+        <f>AU40-I39</f>
+        <v>11.666666666666707</v>
+      </c>
+      <c r="AW40" s="106">
+        <f>AV40-I39</f>
+        <v>11.20000000000004</v>
+      </c>
+      <c r="AX40" s="106">
+        <f>AW40-I39</f>
+        <v>10.733333333333373</v>
+      </c>
+      <c r="AY40" s="106">
+        <f>AX40-I39</f>
+        <v>10.266666666666707</v>
+      </c>
+      <c r="AZ40" s="106">
+        <f>AY40-I39</f>
+        <v>9.8000000000000398</v>
+      </c>
+      <c r="BA40" s="106">
+        <f>AZ40-I39</f>
+        <v>9.333333333333373</v>
+      </c>
+      <c r="BB40" s="106">
+        <f>BA40-I39</f>
+        <v>8.8666666666667062</v>
+      </c>
+      <c r="BC40" s="106">
+        <f>BB40-I39</f>
+        <v>8.4000000000000394</v>
+      </c>
+      <c r="BD40" s="106">
+        <f>BC40-I39</f>
+        <v>7.9333333333333727</v>
+      </c>
+      <c r="BE40" s="106">
+        <f>BD40-I39</f>
+        <v>7.4666666666667059</v>
+      </c>
+      <c r="BF40" s="106">
+        <f>BE40-I39</f>
+        <v>7.0000000000000391</v>
+      </c>
+      <c r="BG40" s="106">
+        <f>BF40-I39</f>
+        <v>6.5333333333333723</v>
+      </c>
+      <c r="BH40" s="106">
+        <f>BG40-I39</f>
+        <v>6.0666666666667055</v>
+      </c>
+      <c r="BI40" s="106">
+        <f>BH40-I39</f>
+        <v>5.6000000000000387</v>
+      </c>
+      <c r="BJ40" s="106">
+        <f>BI40-I39</f>
+        <v>5.1333333333333719</v>
+      </c>
+      <c r="BK40" s="106">
+        <f>BJ40-I39</f>
+        <v>4.6666666666667052</v>
+      </c>
+      <c r="BL40" s="106">
+        <f>BK40-I39</f>
+        <v>4.2000000000000384</v>
+      </c>
+      <c r="BM40" s="106">
+        <f>BL40-I39</f>
+        <v>3.7333333333333716</v>
+      </c>
+      <c r="BN40" s="106">
+        <f>BM40-I39</f>
+        <v>3.2666666666667048</v>
+      </c>
+      <c r="BO40" s="106">
+        <f>BN40-I39</f>
+        <v>2.800000000000038</v>
+      </c>
+      <c r="BP40" s="106">
+        <f>BO40-I39</f>
+        <v>2.3333333333333712</v>
+      </c>
+      <c r="BQ40" s="106">
+        <f>BP40-I39</f>
+        <v>1.8666666666667044</v>
+      </c>
+      <c r="BR40" s="106">
+        <f>BQ40-I39</f>
+        <v>1.4000000000000377</v>
+      </c>
+      <c r="BS40" s="106">
+        <f>BR40-I39</f>
+        <v>0.93333333333337098</v>
+      </c>
+      <c r="BT40" s="106">
+        <f>BS40-I39</f>
+        <v>0.46666666666670431</v>
+      </c>
+      <c r="BV40" s="101"/>
+    </row>
+    <row r="41" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L41" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="M40" s="105">
-        <f>E38</f>
+      <c r="M41" s="105">
+        <f>E39</f>
         <v>28</v>
       </c>
-      <c r="N40" s="105">
-        <f t="shared" ref="N40:BT40" si="11">M42</f>
+      <c r="N41" s="105">
+        <f t="shared" ref="N41:BT41" si="11">M43</f>
         <v>28</v>
       </c>
-      <c r="O40" s="105">
+      <c r="O41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="P40" s="105">
+      <c r="P41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="Q40" s="105">
+      <c r="Q41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="R40" s="105">
+      <c r="R41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="S40" s="105">
+      <c r="S41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="T40" s="105">
+      <c r="T41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="U40" s="105">
+      <c r="U41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="V40" s="105">
+      <c r="V41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="W40" s="105">
+      <c r="W41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="X40" s="105">
+      <c r="X41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="Y40" s="105">
+      <c r="Y41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="Z40" s="105">
+      <c r="Z41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AA40" s="105">
+      <c r="AA41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AB40" s="105">
+      <c r="AB41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AC40" s="105">
+      <c r="AC41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AD40" s="105">
+      <c r="AD41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AE40" s="105">
+      <c r="AE41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AF40" s="105">
+      <c r="AF41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AG40" s="105">
+      <c r="AG41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AH40" s="105">
+      <c r="AH41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AI40" s="105">
+      <c r="AI41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AJ40" s="105">
+      <c r="AJ41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AK40" s="105">
+      <c r="AK41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AL40" s="105">
+      <c r="AL41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AM40" s="105">
+      <c r="AM41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AN40" s="105">
+      <c r="AN41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AO40" s="105">
+      <c r="AO41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AP40" s="105">
+      <c r="AP41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AQ40" s="105">
+      <c r="AQ41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AR40" s="105">
+      <c r="AR41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AS40" s="105">
+      <c r="AS41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AT40" s="105">
+      <c r="AT41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AU40" s="105">
+      <c r="AU41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AV40" s="105">
+      <c r="AV41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AW40" s="105">
+      <c r="AW41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AX40" s="105">
+      <c r="AX41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AY40" s="105">
+      <c r="AY41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="AZ40" s="105">
+      <c r="AZ41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BA40" s="105">
+      <c r="BA41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BB40" s="105">
+      <c r="BB41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BC40" s="105">
+      <c r="BC41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BD40" s="105">
+      <c r="BD41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BE40" s="105">
+      <c r="BE41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BF40" s="105">
+      <c r="BF41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BG40" s="105">
+      <c r="BG41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BH40" s="105">
+      <c r="BH41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BI40" s="105">
+      <c r="BI41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BJ40" s="105">
+      <c r="BJ41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BK40" s="105">
+      <c r="BK41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BL40" s="105">
+      <c r="BL41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BM40" s="105">
+      <c r="BM41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BN40" s="105">
+      <c r="BN41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BO40" s="105">
+      <c r="BO41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BP40" s="105">
+      <c r="BP41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BQ40" s="105">
+      <c r="BQ41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BR40" s="105">
+      <c r="BR41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BS40" s="105">
+      <c r="BS41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BT40" s="105">
+      <c r="BT41" s="105">
         <f t="shared" si="11"/>
         <v>28</v>
       </c>
-      <c r="BV40" s="101">
-        <f t="shared" ref="BV40:BV42" si="12">SUM(M40:BT40)</f>
+      <c r="BV41" s="101">
+        <f t="shared" ref="BV41:BV43" si="12">SUM(M41:BT41)</f>
         <v>1680</v>
       </c>
     </row>
-    <row r="41" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K41" s="107" t="s">
+    <row r="42" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K42" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="L41" s="102" t="s">
+      <c r="L42" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="M41" s="57"/>
-      <c r="N41" s="57"/>
-      <c r="O41" s="57"/>
-      <c r="P41" s="57"/>
-      <c r="Q41" s="57"/>
-      <c r="R41" s="57"/>
-      <c r="S41" s="57"/>
-      <c r="T41" s="57"/>
-      <c r="U41" s="57"/>
-      <c r="V41" s="57"/>
-      <c r="W41" s="57"/>
-      <c r="X41" s="57"/>
-      <c r="Y41" s="57"/>
-      <c r="Z41" s="57"/>
-      <c r="AA41" s="57"/>
-      <c r="AB41" s="57"/>
-      <c r="AC41" s="57"/>
-      <c r="AD41" s="57"/>
-      <c r="AE41" s="57"/>
-      <c r="AF41" s="57"/>
-      <c r="AG41" s="57"/>
-      <c r="AH41" s="57"/>
-      <c r="AI41" s="57"/>
-      <c r="AJ41" s="57"/>
-      <c r="AK41" s="57"/>
-      <c r="AL41" s="57"/>
-      <c r="AM41" s="57"/>
-      <c r="AN41" s="57"/>
-      <c r="AO41" s="57"/>
-      <c r="AP41" s="57"/>
-      <c r="AQ41" s="57"/>
-      <c r="AR41" s="57"/>
-      <c r="AS41" s="57"/>
-      <c r="AT41" s="57"/>
-      <c r="AU41" s="57"/>
-      <c r="AV41" s="57"/>
-      <c r="AW41" s="57"/>
-      <c r="AX41" s="57"/>
-      <c r="AY41" s="57"/>
-      <c r="AZ41" s="57"/>
-      <c r="BA41" s="57"/>
-      <c r="BB41" s="57"/>
-      <c r="BC41" s="57"/>
-      <c r="BD41" s="57"/>
-      <c r="BE41" s="57"/>
-      <c r="BF41" s="57"/>
-      <c r="BG41" s="57"/>
-      <c r="BH41" s="57"/>
-      <c r="BI41" s="57"/>
-      <c r="BJ41" s="57"/>
-      <c r="BK41" s="57"/>
-      <c r="BL41" s="57"/>
-      <c r="BM41" s="57"/>
-      <c r="BN41" s="57"/>
-      <c r="BO41" s="57"/>
-      <c r="BP41" s="57"/>
-      <c r="BQ41" s="57"/>
-      <c r="BR41" s="57"/>
-      <c r="BS41" s="57"/>
-      <c r="BT41" s="57"/>
-      <c r="BV41" s="101">
+      <c r="M42" s="57"/>
+      <c r="N42" s="57"/>
+      <c r="O42" s="57"/>
+      <c r="P42" s="57"/>
+      <c r="Q42" s="57"/>
+      <c r="R42" s="57"/>
+      <c r="S42" s="57"/>
+      <c r="T42" s="57"/>
+      <c r="U42" s="57"/>
+      <c r="V42" s="57"/>
+      <c r="W42" s="57"/>
+      <c r="X42" s="57"/>
+      <c r="Y42" s="57"/>
+      <c r="Z42" s="57"/>
+      <c r="AA42" s="57"/>
+      <c r="AB42" s="57"/>
+      <c r="AC42" s="57"/>
+      <c r="AD42" s="57"/>
+      <c r="AE42" s="57"/>
+      <c r="AF42" s="57"/>
+      <c r="AG42" s="57"/>
+      <c r="AH42" s="57"/>
+      <c r="AI42" s="57"/>
+      <c r="AJ42" s="57"/>
+      <c r="AK42" s="57"/>
+      <c r="AL42" s="57"/>
+      <c r="AM42" s="57"/>
+      <c r="AN42" s="57"/>
+      <c r="AO42" s="57"/>
+      <c r="AP42" s="57"/>
+      <c r="AQ42" s="57"/>
+      <c r="AR42" s="57"/>
+      <c r="AS42" s="57"/>
+      <c r="AT42" s="57"/>
+      <c r="AU42" s="57"/>
+      <c r="AV42" s="57"/>
+      <c r="AW42" s="57"/>
+      <c r="AX42" s="57"/>
+      <c r="AY42" s="57"/>
+      <c r="AZ42" s="57"/>
+      <c r="BA42" s="57"/>
+      <c r="BB42" s="57"/>
+      <c r="BC42" s="57"/>
+      <c r="BD42" s="57"/>
+      <c r="BE42" s="57"/>
+      <c r="BF42" s="57"/>
+      <c r="BG42" s="57"/>
+      <c r="BH42" s="57"/>
+      <c r="BI42" s="57"/>
+      <c r="BJ42" s="57"/>
+      <c r="BK42" s="57"/>
+      <c r="BL42" s="57"/>
+      <c r="BM42" s="57"/>
+      <c r="BN42" s="57"/>
+      <c r="BO42" s="57"/>
+      <c r="BP42" s="57"/>
+      <c r="BQ42" s="57"/>
+      <c r="BR42" s="57"/>
+      <c r="BS42" s="57"/>
+      <c r="BT42" s="57"/>
+      <c r="BV42" s="101">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L42" s="102" t="s">
+    <row r="43" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L43" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M42" s="105">
-        <f t="shared" ref="M42:BT42" si="13">M40-M41</f>
+      <c r="M43" s="105">
+        <f t="shared" ref="M43:BT43" si="13">M41-M42</f>
         <v>28</v>
       </c>
-      <c r="N42" s="105">
+      <c r="N43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="O42" s="105">
+      <c r="O43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="P42" s="105">
+      <c r="P43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="Q42" s="105">
+      <c r="Q43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="R42" s="105">
+      <c r="R43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="S42" s="105">
+      <c r="S43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="T42" s="105">
+      <c r="T43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="U42" s="105">
+      <c r="U43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="V42" s="105">
+      <c r="V43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="W42" s="105">
+      <c r="W43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="X42" s="105">
+      <c r="X43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="Y42" s="105">
+      <c r="Y43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="Z42" s="105">
+      <c r="Z43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AA42" s="105">
+      <c r="AA43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AB42" s="105">
+      <c r="AB43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AC42" s="105">
+      <c r="AC43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AD42" s="105">
+      <c r="AD43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AE42" s="105">
+      <c r="AE43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AF42" s="105">
+      <c r="AF43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AG42" s="105">
+      <c r="AG43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AH42" s="105">
+      <c r="AH43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AI42" s="105">
+      <c r="AI43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AJ42" s="105">
+      <c r="AJ43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AK42" s="105">
+      <c r="AK43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AL42" s="105">
+      <c r="AL43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AM42" s="105">
+      <c r="AM43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AN42" s="105">
+      <c r="AN43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AO42" s="105">
+      <c r="AO43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AP42" s="105">
+      <c r="AP43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AQ42" s="105">
+      <c r="AQ43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AR42" s="105">
+      <c r="AR43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AS42" s="105">
+      <c r="AS43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AT42" s="105">
+      <c r="AT43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AU42" s="105">
+      <c r="AU43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AV42" s="105">
+      <c r="AV43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AW42" s="105">
+      <c r="AW43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AX42" s="105">
+      <c r="AX43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AY42" s="105">
+      <c r="AY43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="AZ42" s="105">
+      <c r="AZ43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BA42" s="105">
+      <c r="BA43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BB42" s="105">
+      <c r="BB43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BC42" s="105">
+      <c r="BC43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BD42" s="105">
+      <c r="BD43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BE42" s="105">
+      <c r="BE43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BF42" s="105">
+      <c r="BF43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BG42" s="105">
+      <c r="BG43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BH42" s="105">
+      <c r="BH43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BI42" s="105">
+      <c r="BI43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BJ42" s="105">
+      <c r="BJ43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BK42" s="105">
+      <c r="BK43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BL42" s="105">
+      <c r="BL43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BM42" s="105">
+      <c r="BM43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BN42" s="105">
+      <c r="BN43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BO42" s="105">
+      <c r="BO43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BP42" s="105">
+      <c r="BP43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BQ42" s="105">
+      <c r="BQ43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BR42" s="105">
+      <c r="BR43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BS42" s="105">
+      <c r="BS43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BT42" s="105">
+      <c r="BT43" s="105">
         <f t="shared" si="13"/>
         <v>28</v>
       </c>
-      <c r="BV42" s="101">
+      <c r="BV43" s="101">
         <f t="shared" si="12"/>
         <v>1680</v>
       </c>
     </row>
-    <row r="43" spans="2:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E46" s="198" t="s">
+    <row r="44" spans="2:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="199" t="s">
         <v>83</v>
       </c>
-      <c r="F46" s="162"/>
-      <c r="G46" s="162"/>
-      <c r="H46" s="162"/>
-      <c r="I46" s="162"/>
-      <c r="J46" s="162"/>
-      <c r="K46" s="162"/>
-      <c r="L46" s="162"/>
-      <c r="M46" s="162"/>
-      <c r="N46" s="162"/>
-      <c r="O46" s="162"/>
-      <c r="P46" s="162"/>
-      <c r="Q46" s="162"/>
-      <c r="R46" s="162"/>
-      <c r="S46" s="162"/>
-      <c r="T46" s="162"/>
-      <c r="U46" s="162"/>
-      <c r="V46" s="162"/>
-      <c r="W46" s="162"/>
-      <c r="X46" s="162"/>
-      <c r="Y46" s="162"/>
-      <c r="Z46" s="162"/>
-      <c r="AA46" s="162"/>
-      <c r="AB46" s="162"/>
-      <c r="AC46" s="162"/>
-      <c r="AD46" s="162"/>
-      <c r="AE46" s="162"/>
-      <c r="AF46" s="162"/>
-      <c r="AG46" s="162"/>
-      <c r="AH46" s="162"/>
-      <c r="AI46" s="162"/>
-      <c r="AJ46" s="162"/>
-      <c r="AK46" s="162"/>
-      <c r="AL46" s="162"/>
-      <c r="AM46" s="162"/>
-      <c r="AN46" s="162"/>
-      <c r="AO46" s="162"/>
-      <c r="AP46" s="162"/>
-      <c r="AQ46" s="162"/>
-      <c r="AR46" s="162"/>
-      <c r="AS46" s="162"/>
-      <c r="AT46" s="162"/>
-      <c r="AU46" s="162"/>
-      <c r="AV46" s="162"/>
-      <c r="AW46" s="162"/>
-      <c r="AX46" s="162"/>
-      <c r="AY46" s="162"/>
-      <c r="AZ46" s="162"/>
-      <c r="BA46" s="162"/>
-      <c r="BB46" s="163"/>
+      <c r="F47" s="182"/>
+      <c r="G47" s="182"/>
+      <c r="H47" s="182"/>
+      <c r="I47" s="182"/>
+      <c r="J47" s="182"/>
+      <c r="K47" s="182"/>
+      <c r="L47" s="182"/>
+      <c r="M47" s="182"/>
+      <c r="N47" s="182"/>
+      <c r="O47" s="182"/>
+      <c r="P47" s="182"/>
+      <c r="Q47" s="182"/>
+      <c r="R47" s="182"/>
+      <c r="S47" s="182"/>
+      <c r="T47" s="182"/>
+      <c r="U47" s="182"/>
+      <c r="V47" s="182"/>
+      <c r="W47" s="182"/>
+      <c r="X47" s="182"/>
+      <c r="Y47" s="182"/>
+      <c r="Z47" s="182"/>
+      <c r="AA47" s="182"/>
+      <c r="AB47" s="182"/>
+      <c r="AC47" s="182"/>
+      <c r="AD47" s="182"/>
+      <c r="AE47" s="182"/>
+      <c r="AF47" s="182"/>
+      <c r="AG47" s="182"/>
+      <c r="AH47" s="182"/>
+      <c r="AI47" s="182"/>
+      <c r="AJ47" s="182"/>
+      <c r="AK47" s="182"/>
+      <c r="AL47" s="182"/>
+      <c r="AM47" s="182"/>
+      <c r="AN47" s="182"/>
+      <c r="AO47" s="182"/>
+      <c r="AP47" s="182"/>
+      <c r="AQ47" s="182"/>
+      <c r="AR47" s="182"/>
+      <c r="AS47" s="182"/>
+      <c r="AT47" s="182"/>
+      <c r="AU47" s="182"/>
+      <c r="AV47" s="182"/>
+      <c r="AW47" s="182"/>
+      <c r="AX47" s="182"/>
+      <c r="AY47" s="182"/>
+      <c r="AZ47" s="182"/>
+      <c r="BA47" s="182"/>
+      <c r="BB47" s="183"/>
     </row>
-    <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="3:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C51" s="108"/>
-      <c r="D51" s="108"/>
+    <row r="51" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="3:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C52" s="108"/>
+      <c r="D52" s="108"/>
     </row>
-    <row r="52" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17445,16 +17553,10 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="E46:BB46"/>
+    <mergeCell ref="E47:BB47"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
     <mergeCell ref="BP8:BT8"/>
@@ -17470,6 +17572,13 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17484,7 +17593,7 @@
   </sheetPr>
   <dimension ref="B1:K999"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -19217,7 +19326,7 @@
   </sheetPr>
   <dimension ref="B1:G1003"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
minor fix on scrum doc
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\Progetto\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61520DE-0333-48EA-9519-AF0573EC7C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57DF773-0A37-4D83-87A8-74F44418E541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2441,53 +2441,11 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2518,6 +2476,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6915,19 +6915,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="183" t="str">
+      <c r="BK2" s="165" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="184"/>
-      <c r="BM2" s="184"/>
-      <c r="BN2" s="184"/>
-      <c r="BO2" s="184"/>
-      <c r="BP2" s="184"/>
-      <c r="BQ2" s="184"/>
-      <c r="BR2" s="184"/>
-      <c r="BS2" s="184"/>
-      <c r="BT2" s="184"/>
+      <c r="BL2" s="166"/>
+      <c r="BM2" s="166"/>
+      <c r="BN2" s="166"/>
+      <c r="BO2" s="166"/>
+      <c r="BP2" s="166"/>
+      <c r="BQ2" s="166"/>
+      <c r="BR2" s="166"/>
+      <c r="BS2" s="166"/>
+      <c r="BT2" s="166"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -6955,7 +6955,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="185" t="s">
+      <c r="K4" s="167" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7032,7 +7032,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="186"/>
+      <c r="K5" s="168"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7107,7 +7107,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="186"/>
+      <c r="K6" s="168"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7182,7 +7182,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="186"/>
+      <c r="K7" s="168"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7257,7 +7257,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="187"/>
+      <c r="K8" s="169"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7323,124 +7323,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="188" t="s">
+      <c r="B9" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="190" t="s">
+      <c r="C9" s="172" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="192" t="s">
+      <c r="D9" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="194" t="s">
+      <c r="E9" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="195"/>
-      <c r="G9" s="196"/>
-      <c r="H9" s="197" t="s">
+      <c r="F9" s="177"/>
+      <c r="G9" s="178"/>
+      <c r="H9" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="165" t="s">
+      <c r="I9" s="184" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="167" t="s">
+      <c r="J9" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="169" t="s">
+      <c r="K9" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="170" t="s">
+      <c r="L9" s="189" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="172" t="s">
+      <c r="M9" s="191" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="173"/>
-      <c r="O9" s="173"/>
-      <c r="P9" s="173"/>
-      <c r="Q9" s="174"/>
-      <c r="R9" s="175" t="s">
+      <c r="N9" s="163"/>
+      <c r="O9" s="163"/>
+      <c r="P9" s="163"/>
+      <c r="Q9" s="192"/>
+      <c r="R9" s="193" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="173"/>
-      <c r="T9" s="173"/>
-      <c r="U9" s="173"/>
-      <c r="V9" s="174"/>
-      <c r="W9" s="175" t="s">
+      <c r="S9" s="163"/>
+      <c r="T9" s="163"/>
+      <c r="U9" s="163"/>
+      <c r="V9" s="192"/>
+      <c r="W9" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="173"/>
-      <c r="Y9" s="173"/>
-      <c r="Z9" s="173"/>
-      <c r="AA9" s="176"/>
-      <c r="AB9" s="177" t="s">
+      <c r="X9" s="163"/>
+      <c r="Y9" s="163"/>
+      <c r="Z9" s="163"/>
+      <c r="AA9" s="164"/>
+      <c r="AB9" s="194" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="173"/>
-      <c r="AD9" s="173"/>
-      <c r="AE9" s="173"/>
-      <c r="AF9" s="174"/>
-      <c r="AG9" s="178" t="s">
+      <c r="AC9" s="163"/>
+      <c r="AD9" s="163"/>
+      <c r="AE9" s="163"/>
+      <c r="AF9" s="192"/>
+      <c r="AG9" s="195" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="173"/>
-      <c r="AI9" s="173"/>
-      <c r="AJ9" s="173"/>
-      <c r="AK9" s="174"/>
-      <c r="AL9" s="178" t="s">
+      <c r="AH9" s="163"/>
+      <c r="AI9" s="163"/>
+      <c r="AJ9" s="163"/>
+      <c r="AK9" s="192"/>
+      <c r="AL9" s="195" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="173"/>
-      <c r="AN9" s="173"/>
-      <c r="AO9" s="173"/>
-      <c r="AP9" s="176"/>
-      <c r="AQ9" s="179" t="s">
+      <c r="AM9" s="163"/>
+      <c r="AN9" s="163"/>
+      <c r="AO9" s="163"/>
+      <c r="AP9" s="164"/>
+      <c r="AQ9" s="196" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="173"/>
-      <c r="AS9" s="173"/>
-      <c r="AT9" s="173"/>
-      <c r="AU9" s="174"/>
-      <c r="AV9" s="180" t="s">
+      <c r="AR9" s="163"/>
+      <c r="AS9" s="163"/>
+      <c r="AT9" s="163"/>
+      <c r="AU9" s="192"/>
+      <c r="AV9" s="197" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="173"/>
-      <c r="AX9" s="173"/>
-      <c r="AY9" s="173"/>
-      <c r="AZ9" s="174"/>
-      <c r="BA9" s="180" t="s">
+      <c r="AW9" s="163"/>
+      <c r="AX9" s="163"/>
+      <c r="AY9" s="163"/>
+      <c r="AZ9" s="192"/>
+      <c r="BA9" s="197" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="173"/>
-      <c r="BC9" s="173"/>
-      <c r="BD9" s="173"/>
-      <c r="BE9" s="176"/>
-      <c r="BF9" s="181" t="s">
+      <c r="BB9" s="163"/>
+      <c r="BC9" s="163"/>
+      <c r="BD9" s="163"/>
+      <c r="BE9" s="164"/>
+      <c r="BF9" s="198" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="173"/>
-      <c r="BH9" s="173"/>
-      <c r="BI9" s="173"/>
-      <c r="BJ9" s="174"/>
-      <c r="BK9" s="182" t="s">
+      <c r="BG9" s="163"/>
+      <c r="BH9" s="163"/>
+      <c r="BI9" s="163"/>
+      <c r="BJ9" s="192"/>
+      <c r="BK9" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="173"/>
-      <c r="BM9" s="173"/>
-      <c r="BN9" s="173"/>
-      <c r="BO9" s="174"/>
-      <c r="BP9" s="182" t="s">
+      <c r="BL9" s="163"/>
+      <c r="BM9" s="163"/>
+      <c r="BN9" s="163"/>
+      <c r="BO9" s="192"/>
+      <c r="BP9" s="162" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="173"/>
-      <c r="BR9" s="173"/>
-      <c r="BS9" s="173"/>
-      <c r="BT9" s="176"/>
+      <c r="BQ9" s="163"/>
+      <c r="BR9" s="163"/>
+      <c r="BS9" s="163"/>
+      <c r="BT9" s="164"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="189"/>
-      <c r="C10" s="191"/>
-      <c r="D10" s="193"/>
+      <c r="B10" s="171"/>
+      <c r="C10" s="173"/>
+      <c r="D10" s="175"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7450,11 +7450,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="198"/>
-      <c r="I10" s="166"/>
-      <c r="J10" s="168"/>
-      <c r="K10" s="168"/>
-      <c r="L10" s="171"/>
+      <c r="H10" s="180"/>
+      <c r="I10" s="185"/>
+      <c r="J10" s="187"/>
+      <c r="K10" s="187"/>
+      <c r="L10" s="190"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11063,80 +11063,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="162" t="str">
+      <c r="B45" s="181" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="163"/>
-      <c r="D45" s="163"/>
-      <c r="E45" s="163"/>
-      <c r="F45" s="163"/>
-      <c r="G45" s="163"/>
-      <c r="H45" s="163"/>
-      <c r="I45" s="163"/>
-      <c r="J45" s="163"/>
-      <c r="K45" s="163"/>
-      <c r="L45" s="163"/>
-      <c r="M45" s="163"/>
-      <c r="N45" s="163"/>
-      <c r="O45" s="163"/>
-      <c r="P45" s="163"/>
-      <c r="Q45" s="163"/>
-      <c r="R45" s="163"/>
-      <c r="S45" s="163"/>
-      <c r="T45" s="163"/>
-      <c r="U45" s="163"/>
-      <c r="V45" s="163"/>
-      <c r="W45" s="163"/>
-      <c r="X45" s="163"/>
-      <c r="Y45" s="163"/>
-      <c r="Z45" s="163"/>
-      <c r="AA45" s="163"/>
-      <c r="AB45" s="163"/>
-      <c r="AC45" s="163"/>
-      <c r="AD45" s="163"/>
-      <c r="AE45" s="163"/>
-      <c r="AF45" s="163"/>
-      <c r="AG45" s="163"/>
-      <c r="AH45" s="163"/>
-      <c r="AI45" s="163"/>
-      <c r="AJ45" s="163"/>
-      <c r="AK45" s="163"/>
-      <c r="AL45" s="163"/>
-      <c r="AM45" s="163"/>
-      <c r="AN45" s="163"/>
-      <c r="AO45" s="163"/>
-      <c r="AP45" s="163"/>
-      <c r="AQ45" s="163"/>
-      <c r="AR45" s="163"/>
-      <c r="AS45" s="163"/>
-      <c r="AT45" s="163"/>
-      <c r="AU45" s="163"/>
-      <c r="AV45" s="163"/>
-      <c r="AW45" s="163"/>
-      <c r="AX45" s="163"/>
-      <c r="AY45" s="163"/>
-      <c r="AZ45" s="163"/>
-      <c r="BA45" s="163"/>
-      <c r="BB45" s="163"/>
-      <c r="BC45" s="163"/>
-      <c r="BD45" s="163"/>
-      <c r="BE45" s="163"/>
-      <c r="BF45" s="163"/>
-      <c r="BG45" s="163"/>
-      <c r="BH45" s="163"/>
-      <c r="BI45" s="163"/>
-      <c r="BJ45" s="163"/>
-      <c r="BK45" s="163"/>
-      <c r="BL45" s="163"/>
-      <c r="BM45" s="163"/>
-      <c r="BN45" s="163"/>
-      <c r="BO45" s="163"/>
-      <c r="BP45" s="163"/>
-      <c r="BQ45" s="163"/>
-      <c r="BR45" s="163"/>
-      <c r="BS45" s="163"/>
-      <c r="BT45" s="164"/>
+      <c r="C45" s="182"/>
+      <c r="D45" s="182"/>
+      <c r="E45" s="182"/>
+      <c r="F45" s="182"/>
+      <c r="G45" s="182"/>
+      <c r="H45" s="182"/>
+      <c r="I45" s="182"/>
+      <c r="J45" s="182"/>
+      <c r="K45" s="182"/>
+      <c r="L45" s="182"/>
+      <c r="M45" s="182"/>
+      <c r="N45" s="182"/>
+      <c r="O45" s="182"/>
+      <c r="P45" s="182"/>
+      <c r="Q45" s="182"/>
+      <c r="R45" s="182"/>
+      <c r="S45" s="182"/>
+      <c r="T45" s="182"/>
+      <c r="U45" s="182"/>
+      <c r="V45" s="182"/>
+      <c r="W45" s="182"/>
+      <c r="X45" s="182"/>
+      <c r="Y45" s="182"/>
+      <c r="Z45" s="182"/>
+      <c r="AA45" s="182"/>
+      <c r="AB45" s="182"/>
+      <c r="AC45" s="182"/>
+      <c r="AD45" s="182"/>
+      <c r="AE45" s="182"/>
+      <c r="AF45" s="182"/>
+      <c r="AG45" s="182"/>
+      <c r="AH45" s="182"/>
+      <c r="AI45" s="182"/>
+      <c r="AJ45" s="182"/>
+      <c r="AK45" s="182"/>
+      <c r="AL45" s="182"/>
+      <c r="AM45" s="182"/>
+      <c r="AN45" s="182"/>
+      <c r="AO45" s="182"/>
+      <c r="AP45" s="182"/>
+      <c r="AQ45" s="182"/>
+      <c r="AR45" s="182"/>
+      <c r="AS45" s="182"/>
+      <c r="AT45" s="182"/>
+      <c r="AU45" s="182"/>
+      <c r="AV45" s="182"/>
+      <c r="AW45" s="182"/>
+      <c r="AX45" s="182"/>
+      <c r="AY45" s="182"/>
+      <c r="AZ45" s="182"/>
+      <c r="BA45" s="182"/>
+      <c r="BB45" s="182"/>
+      <c r="BC45" s="182"/>
+      <c r="BD45" s="182"/>
+      <c r="BE45" s="182"/>
+      <c r="BF45" s="182"/>
+      <c r="BG45" s="182"/>
+      <c r="BH45" s="182"/>
+      <c r="BI45" s="182"/>
+      <c r="BJ45" s="182"/>
+      <c r="BK45" s="182"/>
+      <c r="BL45" s="182"/>
+      <c r="BM45" s="182"/>
+      <c r="BN45" s="182"/>
+      <c r="BO45" s="182"/>
+      <c r="BP45" s="182"/>
+      <c r="BQ45" s="182"/>
+      <c r="BR45" s="182"/>
+      <c r="BS45" s="182"/>
+      <c r="BT45" s="183"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12099,14 +12099,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12123,6 +12115,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12138,7 +12138,7 @@
   <dimension ref="B1:BV1004"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE27" sqref="AE27"/>
+      <selection activeCell="AS26" sqref="AS26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12251,7 +12251,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="185" t="s">
+      <c r="K3" s="167" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12328,7 +12328,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="186"/>
+      <c r="K4" s="168"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12402,7 +12402,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="186"/>
+      <c r="K5" s="168"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12477,7 +12477,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="186"/>
+      <c r="K6" s="168"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12552,7 +12552,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="187"/>
+      <c r="K7" s="169"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12618,124 +12618,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="188" t="s">
+      <c r="B8" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="190" t="s">
+      <c r="C8" s="172" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="192" t="s">
+      <c r="D8" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="194" t="s">
+      <c r="E8" s="176" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="195"/>
-      <c r="G8" s="196"/>
-      <c r="H8" s="197" t="s">
+      <c r="F8" s="177"/>
+      <c r="G8" s="178"/>
+      <c r="H8" s="179" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="165" t="s">
+      <c r="I8" s="184" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="167" t="s">
+      <c r="J8" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="169" t="s">
+      <c r="K8" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="170" t="s">
+      <c r="L8" s="189" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="172" t="s">
+      <c r="M8" s="191" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="173"/>
-      <c r="O8" s="173"/>
-      <c r="P8" s="173"/>
-      <c r="Q8" s="174"/>
-      <c r="R8" s="175" t="s">
+      <c r="N8" s="163"/>
+      <c r="O8" s="163"/>
+      <c r="P8" s="163"/>
+      <c r="Q8" s="192"/>
+      <c r="R8" s="193" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="173"/>
-      <c r="T8" s="173"/>
-      <c r="U8" s="173"/>
-      <c r="V8" s="174"/>
-      <c r="W8" s="175" t="s">
+      <c r="S8" s="163"/>
+      <c r="T8" s="163"/>
+      <c r="U8" s="163"/>
+      <c r="V8" s="192"/>
+      <c r="W8" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="173"/>
-      <c r="Y8" s="173"/>
-      <c r="Z8" s="173"/>
-      <c r="AA8" s="176"/>
-      <c r="AB8" s="177" t="s">
+      <c r="X8" s="163"/>
+      <c r="Y8" s="163"/>
+      <c r="Z8" s="163"/>
+      <c r="AA8" s="164"/>
+      <c r="AB8" s="194" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="173"/>
-      <c r="AD8" s="173"/>
-      <c r="AE8" s="173"/>
-      <c r="AF8" s="174"/>
-      <c r="AG8" s="178" t="s">
+      <c r="AC8" s="163"/>
+      <c r="AD8" s="163"/>
+      <c r="AE8" s="163"/>
+      <c r="AF8" s="192"/>
+      <c r="AG8" s="195" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="173"/>
-      <c r="AI8" s="173"/>
-      <c r="AJ8" s="173"/>
-      <c r="AK8" s="174"/>
-      <c r="AL8" s="178" t="s">
+      <c r="AH8" s="163"/>
+      <c r="AI8" s="163"/>
+      <c r="AJ8" s="163"/>
+      <c r="AK8" s="192"/>
+      <c r="AL8" s="195" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="173"/>
-      <c r="AN8" s="173"/>
-      <c r="AO8" s="173"/>
-      <c r="AP8" s="176"/>
-      <c r="AQ8" s="179" t="s">
+      <c r="AM8" s="163"/>
+      <c r="AN8" s="163"/>
+      <c r="AO8" s="163"/>
+      <c r="AP8" s="164"/>
+      <c r="AQ8" s="196" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="173"/>
-      <c r="AS8" s="173"/>
-      <c r="AT8" s="173"/>
-      <c r="AU8" s="174"/>
-      <c r="AV8" s="180" t="s">
+      <c r="AR8" s="163"/>
+      <c r="AS8" s="163"/>
+      <c r="AT8" s="163"/>
+      <c r="AU8" s="192"/>
+      <c r="AV8" s="197" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="173"/>
-      <c r="AX8" s="173"/>
-      <c r="AY8" s="173"/>
-      <c r="AZ8" s="174"/>
-      <c r="BA8" s="180" t="s">
+      <c r="AW8" s="163"/>
+      <c r="AX8" s="163"/>
+      <c r="AY8" s="163"/>
+      <c r="AZ8" s="192"/>
+      <c r="BA8" s="197" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="173"/>
-      <c r="BC8" s="173"/>
-      <c r="BD8" s="173"/>
-      <c r="BE8" s="176"/>
-      <c r="BF8" s="181" t="s">
+      <c r="BB8" s="163"/>
+      <c r="BC8" s="163"/>
+      <c r="BD8" s="163"/>
+      <c r="BE8" s="164"/>
+      <c r="BF8" s="198" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="173"/>
-      <c r="BH8" s="173"/>
-      <c r="BI8" s="173"/>
-      <c r="BJ8" s="174"/>
-      <c r="BK8" s="182" t="s">
+      <c r="BG8" s="163"/>
+      <c r="BH8" s="163"/>
+      <c r="BI8" s="163"/>
+      <c r="BJ8" s="192"/>
+      <c r="BK8" s="162" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="173"/>
-      <c r="BM8" s="173"/>
-      <c r="BN8" s="173"/>
-      <c r="BO8" s="174"/>
-      <c r="BP8" s="182" t="s">
+      <c r="BL8" s="163"/>
+      <c r="BM8" s="163"/>
+      <c r="BN8" s="163"/>
+      <c r="BO8" s="192"/>
+      <c r="BP8" s="162" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="173"/>
-      <c r="BR8" s="173"/>
-      <c r="BS8" s="173"/>
-      <c r="BT8" s="176"/>
+      <c r="BQ8" s="163"/>
+      <c r="BR8" s="163"/>
+      <c r="BS8" s="163"/>
+      <c r="BT8" s="164"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="189"/>
-      <c r="C9" s="191"/>
-      <c r="D9" s="193"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="173"/>
+      <c r="D9" s="175"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12745,11 +12745,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="198"/>
-      <c r="I9" s="166"/>
-      <c r="J9" s="168"/>
-      <c r="K9" s="168"/>
-      <c r="L9" s="171"/>
+      <c r="H9" s="180"/>
+      <c r="I9" s="185"/>
+      <c r="J9" s="187"/>
+      <c r="K9" s="187"/>
+      <c r="L9" s="190"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -14526,12 +14526,12 @@
       <c r="AF26" s="65"/>
       <c r="AG26" s="69"/>
       <c r="AH26" s="69"/>
-      <c r="AI26" s="161"/>
+      <c r="AI26" s="69"/>
       <c r="AJ26" s="69"/>
       <c r="AK26" s="69"/>
       <c r="AL26" s="65"/>
       <c r="AM26" s="65"/>
-      <c r="AN26" s="65"/>
+      <c r="AN26" s="161"/>
       <c r="AO26" s="65"/>
       <c r="AP26" s="68"/>
       <c r="AQ26" s="64"/>
@@ -16635,55 +16635,55 @@
       <c r="E48" s="199" t="s">
         <v>83</v>
       </c>
-      <c r="F48" s="163"/>
-      <c r="G48" s="163"/>
-      <c r="H48" s="163"/>
-      <c r="I48" s="163"/>
-      <c r="J48" s="163"/>
-      <c r="K48" s="163"/>
-      <c r="L48" s="163"/>
-      <c r="M48" s="163"/>
-      <c r="N48" s="163"/>
-      <c r="O48" s="163"/>
-      <c r="P48" s="163"/>
-      <c r="Q48" s="163"/>
-      <c r="R48" s="163"/>
-      <c r="S48" s="163"/>
-      <c r="T48" s="163"/>
-      <c r="U48" s="163"/>
-      <c r="V48" s="163"/>
-      <c r="W48" s="163"/>
-      <c r="X48" s="163"/>
-      <c r="Y48" s="163"/>
-      <c r="Z48" s="163"/>
-      <c r="AA48" s="163"/>
-      <c r="AB48" s="163"/>
-      <c r="AC48" s="163"/>
-      <c r="AD48" s="163"/>
-      <c r="AE48" s="163"/>
-      <c r="AF48" s="163"/>
-      <c r="AG48" s="163"/>
-      <c r="AH48" s="163"/>
-      <c r="AI48" s="163"/>
-      <c r="AJ48" s="163"/>
-      <c r="AK48" s="163"/>
-      <c r="AL48" s="163"/>
-      <c r="AM48" s="163"/>
-      <c r="AN48" s="163"/>
-      <c r="AO48" s="163"/>
-      <c r="AP48" s="163"/>
-      <c r="AQ48" s="163"/>
-      <c r="AR48" s="163"/>
-      <c r="AS48" s="163"/>
-      <c r="AT48" s="163"/>
-      <c r="AU48" s="163"/>
-      <c r="AV48" s="163"/>
-      <c r="AW48" s="163"/>
-      <c r="AX48" s="163"/>
-      <c r="AY48" s="163"/>
-      <c r="AZ48" s="163"/>
-      <c r="BA48" s="163"/>
-      <c r="BB48" s="164"/>
+      <c r="F48" s="182"/>
+      <c r="G48" s="182"/>
+      <c r="H48" s="182"/>
+      <c r="I48" s="182"/>
+      <c r="J48" s="182"/>
+      <c r="K48" s="182"/>
+      <c r="L48" s="182"/>
+      <c r="M48" s="182"/>
+      <c r="N48" s="182"/>
+      <c r="O48" s="182"/>
+      <c r="P48" s="182"/>
+      <c r="Q48" s="182"/>
+      <c r="R48" s="182"/>
+      <c r="S48" s="182"/>
+      <c r="T48" s="182"/>
+      <c r="U48" s="182"/>
+      <c r="V48" s="182"/>
+      <c r="W48" s="182"/>
+      <c r="X48" s="182"/>
+      <c r="Y48" s="182"/>
+      <c r="Z48" s="182"/>
+      <c r="AA48" s="182"/>
+      <c r="AB48" s="182"/>
+      <c r="AC48" s="182"/>
+      <c r="AD48" s="182"/>
+      <c r="AE48" s="182"/>
+      <c r="AF48" s="182"/>
+      <c r="AG48" s="182"/>
+      <c r="AH48" s="182"/>
+      <c r="AI48" s="182"/>
+      <c r="AJ48" s="182"/>
+      <c r="AK48" s="182"/>
+      <c r="AL48" s="182"/>
+      <c r="AM48" s="182"/>
+      <c r="AN48" s="182"/>
+      <c r="AO48" s="182"/>
+      <c r="AP48" s="182"/>
+      <c r="AQ48" s="182"/>
+      <c r="AR48" s="182"/>
+      <c r="AS48" s="182"/>
+      <c r="AT48" s="182"/>
+      <c r="AU48" s="182"/>
+      <c r="AV48" s="182"/>
+      <c r="AW48" s="182"/>
+      <c r="AX48" s="182"/>
+      <c r="AY48" s="182"/>
+      <c r="AZ48" s="182"/>
+      <c r="BA48" s="182"/>
+      <c r="BB48" s="183"/>
     </row>
     <row r="49" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17646,13 +17646,6 @@
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
     <mergeCell ref="E48:BB48"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
@@ -17669,6 +17662,13 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Start of the logic for Signup/Login
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\Progetto\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6A82DF-D311-4267-BD2E-4F0D1EF125CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE3416F-7F09-4F1E-8F3F-EDAB46A61554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="237">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -741,6 +741,12 @@
   </si>
   <si>
     <t>Serving frontend with docker</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Signup/Login Logic</t>
   </si>
 </sst>
 </file>
@@ -2471,53 +2477,11 @@
     <xf numFmtId="16" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2548,6 +2512,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5452,184 +5458,184 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.5</c:v>
+                  <c:v>34.416666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>33.833333333333329</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.5</c:v>
+                  <c:v>33.249999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>32.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.5</c:v>
+                  <c:v>32.083333333333321</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>31.499999999999989</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.5</c:v>
+                  <c:v>30.916666666666657</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26</c:v>
+                  <c:v>30.333333333333325</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.5</c:v>
+                  <c:v>29.749999999999993</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>29.166666666666661</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24.5</c:v>
+                  <c:v>28.583333333333329</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24</c:v>
+                  <c:v>27.999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23.5</c:v>
+                  <c:v>27.416666666666664</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23</c:v>
+                  <c:v>26.833333333333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.5</c:v>
+                  <c:v>26.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22</c:v>
+                  <c:v>25.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21.5</c:v>
+                  <c:v>25.083333333333336</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>21</c:v>
+                  <c:v>24.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.5</c:v>
+                  <c:v>23.916666666666671</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>23.333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19.5</c:v>
+                  <c:v>22.750000000000007</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>19</c:v>
+                  <c:v>22.166666666666675</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>18.5</c:v>
+                  <c:v>21.583333333333343</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>18</c:v>
+                  <c:v>21.000000000000011</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>17.5</c:v>
+                  <c:v>20.416666666666679</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>17</c:v>
+                  <c:v>19.833333333333346</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>16.5</c:v>
+                  <c:v>19.250000000000014</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>16</c:v>
+                  <c:v>18.666666666666682</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15.5</c:v>
+                  <c:v>18.08333333333335</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15</c:v>
+                  <c:v>17.500000000000018</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>14.5</c:v>
+                  <c:v>16.916666666666686</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>14</c:v>
+                  <c:v>16.333333333333353</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>13.5</c:v>
+                  <c:v>15.75000000000002</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>13</c:v>
+                  <c:v>15.166666666666686</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>12.5</c:v>
+                  <c:v>14.583333333333352</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>12</c:v>
+                  <c:v>14.000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11.5</c:v>
+                  <c:v>13.416666666666684</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>11</c:v>
+                  <c:v>12.83333333333335</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>10.5</c:v>
+                  <c:v>12.250000000000016</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>10</c:v>
+                  <c:v>11.666666666666682</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>9.5</c:v>
+                  <c:v>11.083333333333348</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>9</c:v>
+                  <c:v>10.500000000000014</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>8.5</c:v>
+                  <c:v>9.9166666666666803</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>8</c:v>
+                  <c:v>9.3333333333333464</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>7.5</c:v>
+                  <c:v>8.7500000000000124</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7</c:v>
+                  <c:v>8.1666666666666785</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6.5</c:v>
+                  <c:v>7.5833333333333455</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6</c:v>
+                  <c:v>7.0000000000000124</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5.5</c:v>
+                  <c:v>6.4166666666666794</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5</c:v>
+                  <c:v>5.8333333333333464</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.5</c:v>
+                  <c:v>5.2500000000000133</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4</c:v>
+                  <c:v>4.6666666666666803</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>3.5</c:v>
+                  <c:v>4.0833333333333472</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>3</c:v>
+                  <c:v>3.5000000000000138</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.5</c:v>
+                  <c:v>2.9166666666666803</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2</c:v>
+                  <c:v>2.3333333333333468</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.5</c:v>
+                  <c:v>1.7500000000000133</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1</c:v>
+                  <c:v>1.1666666666666798</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.5</c:v>
+                  <c:v>0.58333333333334647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5863,184 +5869,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6945,19 +6951,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="184" t="str">
+      <c r="BK2" s="166" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="185"/>
-      <c r="BM2" s="185"/>
-      <c r="BN2" s="185"/>
-      <c r="BO2" s="185"/>
-      <c r="BP2" s="185"/>
-      <c r="BQ2" s="185"/>
-      <c r="BR2" s="185"/>
-      <c r="BS2" s="185"/>
-      <c r="BT2" s="185"/>
+      <c r="BL2" s="167"/>
+      <c r="BM2" s="167"/>
+      <c r="BN2" s="167"/>
+      <c r="BO2" s="167"/>
+      <c r="BP2" s="167"/>
+      <c r="BQ2" s="167"/>
+      <c r="BR2" s="167"/>
+      <c r="BS2" s="167"/>
+      <c r="BT2" s="167"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -6985,7 +6991,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="186" t="s">
+      <c r="K4" s="168" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7062,7 +7068,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="187"/>
+      <c r="K5" s="169"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7137,7 +7143,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="187"/>
+      <c r="K6" s="169"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7212,7 +7218,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="187"/>
+      <c r="K7" s="169"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7287,7 +7293,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="188"/>
+      <c r="K8" s="170"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7353,124 +7359,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="189" t="s">
+      <c r="B9" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="191" t="s">
+      <c r="C9" s="173" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="193" t="s">
+      <c r="D9" s="175" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="195" t="s">
+      <c r="E9" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="196"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="198" t="s">
+      <c r="F9" s="178"/>
+      <c r="G9" s="179"/>
+      <c r="H9" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="166" t="s">
+      <c r="I9" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="168" t="s">
+      <c r="J9" s="187" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="170" t="s">
+      <c r="K9" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="171" t="s">
+      <c r="L9" s="190" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="173" t="s">
+      <c r="M9" s="192" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="174"/>
-      <c r="O9" s="174"/>
-      <c r="P9" s="174"/>
-      <c r="Q9" s="175"/>
-      <c r="R9" s="176" t="s">
+      <c r="N9" s="164"/>
+      <c r="O9" s="164"/>
+      <c r="P9" s="164"/>
+      <c r="Q9" s="193"/>
+      <c r="R9" s="194" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="174"/>
-      <c r="T9" s="174"/>
-      <c r="U9" s="174"/>
-      <c r="V9" s="175"/>
-      <c r="W9" s="176" t="s">
+      <c r="S9" s="164"/>
+      <c r="T9" s="164"/>
+      <c r="U9" s="164"/>
+      <c r="V9" s="193"/>
+      <c r="W9" s="194" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="174"/>
-      <c r="Y9" s="174"/>
-      <c r="Z9" s="174"/>
-      <c r="AA9" s="177"/>
-      <c r="AB9" s="178" t="s">
+      <c r="X9" s="164"/>
+      <c r="Y9" s="164"/>
+      <c r="Z9" s="164"/>
+      <c r="AA9" s="165"/>
+      <c r="AB9" s="195" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="174"/>
-      <c r="AD9" s="174"/>
-      <c r="AE9" s="174"/>
-      <c r="AF9" s="175"/>
-      <c r="AG9" s="179" t="s">
+      <c r="AC9" s="164"/>
+      <c r="AD9" s="164"/>
+      <c r="AE9" s="164"/>
+      <c r="AF9" s="193"/>
+      <c r="AG9" s="196" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="174"/>
-      <c r="AI9" s="174"/>
-      <c r="AJ9" s="174"/>
-      <c r="AK9" s="175"/>
-      <c r="AL9" s="179" t="s">
+      <c r="AH9" s="164"/>
+      <c r="AI9" s="164"/>
+      <c r="AJ9" s="164"/>
+      <c r="AK9" s="193"/>
+      <c r="AL9" s="196" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="174"/>
-      <c r="AN9" s="174"/>
-      <c r="AO9" s="174"/>
-      <c r="AP9" s="177"/>
-      <c r="AQ9" s="180" t="s">
+      <c r="AM9" s="164"/>
+      <c r="AN9" s="164"/>
+      <c r="AO9" s="164"/>
+      <c r="AP9" s="165"/>
+      <c r="AQ9" s="197" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="174"/>
-      <c r="AS9" s="174"/>
-      <c r="AT9" s="174"/>
-      <c r="AU9" s="175"/>
-      <c r="AV9" s="181" t="s">
+      <c r="AR9" s="164"/>
+      <c r="AS9" s="164"/>
+      <c r="AT9" s="164"/>
+      <c r="AU9" s="193"/>
+      <c r="AV9" s="198" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="174"/>
-      <c r="AX9" s="174"/>
-      <c r="AY9" s="174"/>
-      <c r="AZ9" s="175"/>
-      <c r="BA9" s="181" t="s">
+      <c r="AW9" s="164"/>
+      <c r="AX9" s="164"/>
+      <c r="AY9" s="164"/>
+      <c r="AZ9" s="193"/>
+      <c r="BA9" s="198" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="174"/>
-      <c r="BC9" s="174"/>
-      <c r="BD9" s="174"/>
-      <c r="BE9" s="177"/>
-      <c r="BF9" s="182" t="s">
+      <c r="BB9" s="164"/>
+      <c r="BC9" s="164"/>
+      <c r="BD9" s="164"/>
+      <c r="BE9" s="165"/>
+      <c r="BF9" s="199" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="174"/>
-      <c r="BH9" s="174"/>
-      <c r="BI9" s="174"/>
-      <c r="BJ9" s="175"/>
-      <c r="BK9" s="183" t="s">
+      <c r="BG9" s="164"/>
+      <c r="BH9" s="164"/>
+      <c r="BI9" s="164"/>
+      <c r="BJ9" s="193"/>
+      <c r="BK9" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="174"/>
-      <c r="BM9" s="174"/>
-      <c r="BN9" s="174"/>
-      <c r="BO9" s="175"/>
-      <c r="BP9" s="183" t="s">
+      <c r="BL9" s="164"/>
+      <c r="BM9" s="164"/>
+      <c r="BN9" s="164"/>
+      <c r="BO9" s="193"/>
+      <c r="BP9" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="174"/>
-      <c r="BR9" s="174"/>
-      <c r="BS9" s="174"/>
-      <c r="BT9" s="177"/>
+      <c r="BQ9" s="164"/>
+      <c r="BR9" s="164"/>
+      <c r="BS9" s="164"/>
+      <c r="BT9" s="165"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="190"/>
-      <c r="C10" s="192"/>
-      <c r="D10" s="194"/>
+      <c r="B10" s="172"/>
+      <c r="C10" s="174"/>
+      <c r="D10" s="176"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7480,11 +7486,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="199"/>
-      <c r="I10" s="167"/>
-      <c r="J10" s="169"/>
-      <c r="K10" s="169"/>
-      <c r="L10" s="172"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="186"/>
+      <c r="J10" s="188"/>
+      <c r="K10" s="188"/>
+      <c r="L10" s="191"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11093,80 +11099,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="163" t="str">
+      <c r="B45" s="182" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="164"/>
-      <c r="D45" s="164"/>
-      <c r="E45" s="164"/>
-      <c r="F45" s="164"/>
-      <c r="G45" s="164"/>
-      <c r="H45" s="164"/>
-      <c r="I45" s="164"/>
-      <c r="J45" s="164"/>
-      <c r="K45" s="164"/>
-      <c r="L45" s="164"/>
-      <c r="M45" s="164"/>
-      <c r="N45" s="164"/>
-      <c r="O45" s="164"/>
-      <c r="P45" s="164"/>
-      <c r="Q45" s="164"/>
-      <c r="R45" s="164"/>
-      <c r="S45" s="164"/>
-      <c r="T45" s="164"/>
-      <c r="U45" s="164"/>
-      <c r="V45" s="164"/>
-      <c r="W45" s="164"/>
-      <c r="X45" s="164"/>
-      <c r="Y45" s="164"/>
-      <c r="Z45" s="164"/>
-      <c r="AA45" s="164"/>
-      <c r="AB45" s="164"/>
-      <c r="AC45" s="164"/>
-      <c r="AD45" s="164"/>
-      <c r="AE45" s="164"/>
-      <c r="AF45" s="164"/>
-      <c r="AG45" s="164"/>
-      <c r="AH45" s="164"/>
-      <c r="AI45" s="164"/>
-      <c r="AJ45" s="164"/>
-      <c r="AK45" s="164"/>
-      <c r="AL45" s="164"/>
-      <c r="AM45" s="164"/>
-      <c r="AN45" s="164"/>
-      <c r="AO45" s="164"/>
-      <c r="AP45" s="164"/>
-      <c r="AQ45" s="164"/>
-      <c r="AR45" s="164"/>
-      <c r="AS45" s="164"/>
-      <c r="AT45" s="164"/>
-      <c r="AU45" s="164"/>
-      <c r="AV45" s="164"/>
-      <c r="AW45" s="164"/>
-      <c r="AX45" s="164"/>
-      <c r="AY45" s="164"/>
-      <c r="AZ45" s="164"/>
-      <c r="BA45" s="164"/>
-      <c r="BB45" s="164"/>
-      <c r="BC45" s="164"/>
-      <c r="BD45" s="164"/>
-      <c r="BE45" s="164"/>
-      <c r="BF45" s="164"/>
-      <c r="BG45" s="164"/>
-      <c r="BH45" s="164"/>
-      <c r="BI45" s="164"/>
-      <c r="BJ45" s="164"/>
-      <c r="BK45" s="164"/>
-      <c r="BL45" s="164"/>
-      <c r="BM45" s="164"/>
-      <c r="BN45" s="164"/>
-      <c r="BO45" s="164"/>
-      <c r="BP45" s="164"/>
-      <c r="BQ45" s="164"/>
-      <c r="BR45" s="164"/>
-      <c r="BS45" s="164"/>
-      <c r="BT45" s="165"/>
+      <c r="C45" s="183"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="183"/>
+      <c r="F45" s="183"/>
+      <c r="G45" s="183"/>
+      <c r="H45" s="183"/>
+      <c r="I45" s="183"/>
+      <c r="J45" s="183"/>
+      <c r="K45" s="183"/>
+      <c r="L45" s="183"/>
+      <c r="M45" s="183"/>
+      <c r="N45" s="183"/>
+      <c r="O45" s="183"/>
+      <c r="P45" s="183"/>
+      <c r="Q45" s="183"/>
+      <c r="R45" s="183"/>
+      <c r="S45" s="183"/>
+      <c r="T45" s="183"/>
+      <c r="U45" s="183"/>
+      <c r="V45" s="183"/>
+      <c r="W45" s="183"/>
+      <c r="X45" s="183"/>
+      <c r="Y45" s="183"/>
+      <c r="Z45" s="183"/>
+      <c r="AA45" s="183"/>
+      <c r="AB45" s="183"/>
+      <c r="AC45" s="183"/>
+      <c r="AD45" s="183"/>
+      <c r="AE45" s="183"/>
+      <c r="AF45" s="183"/>
+      <c r="AG45" s="183"/>
+      <c r="AH45" s="183"/>
+      <c r="AI45" s="183"/>
+      <c r="AJ45" s="183"/>
+      <c r="AK45" s="183"/>
+      <c r="AL45" s="183"/>
+      <c r="AM45" s="183"/>
+      <c r="AN45" s="183"/>
+      <c r="AO45" s="183"/>
+      <c r="AP45" s="183"/>
+      <c r="AQ45" s="183"/>
+      <c r="AR45" s="183"/>
+      <c r="AS45" s="183"/>
+      <c r="AT45" s="183"/>
+      <c r="AU45" s="183"/>
+      <c r="AV45" s="183"/>
+      <c r="AW45" s="183"/>
+      <c r="AX45" s="183"/>
+      <c r="AY45" s="183"/>
+      <c r="AZ45" s="183"/>
+      <c r="BA45" s="183"/>
+      <c r="BB45" s="183"/>
+      <c r="BC45" s="183"/>
+      <c r="BD45" s="183"/>
+      <c r="BE45" s="183"/>
+      <c r="BF45" s="183"/>
+      <c r="BG45" s="183"/>
+      <c r="BH45" s="183"/>
+      <c r="BI45" s="183"/>
+      <c r="BJ45" s="183"/>
+      <c r="BK45" s="183"/>
+      <c r="BL45" s="183"/>
+      <c r="BM45" s="183"/>
+      <c r="BN45" s="183"/>
+      <c r="BO45" s="183"/>
+      <c r="BP45" s="183"/>
+      <c r="BQ45" s="183"/>
+      <c r="BR45" s="183"/>
+      <c r="BS45" s="183"/>
+      <c r="BT45" s="184"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12129,14 +12135,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12153,6 +12151,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12167,8 +12173,8 @@
   </sheetPr>
   <dimension ref="B1:BV1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM31" sqref="AM31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12281,7 +12287,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="186" t="s">
+      <c r="K3" s="168" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12358,7 +12364,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="187"/>
+      <c r="K4" s="169"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12432,7 +12438,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="187"/>
+      <c r="K5" s="169"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12506,7 +12512,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="187"/>
+      <c r="K6" s="169"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12581,7 +12587,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="188"/>
+      <c r="K7" s="170"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12647,124 +12653,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="189" t="s">
+      <c r="B8" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="191" t="s">
+      <c r="C8" s="173" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="193" t="s">
+      <c r="D8" s="175" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="195" t="s">
+      <c r="E8" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="196"/>
-      <c r="G8" s="197"/>
-      <c r="H8" s="198" t="s">
+      <c r="F8" s="178"/>
+      <c r="G8" s="179"/>
+      <c r="H8" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="166" t="s">
+      <c r="I8" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="168" t="s">
+      <c r="J8" s="187" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="170" t="s">
+      <c r="K8" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="171" t="s">
+      <c r="L8" s="190" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="173" t="s">
+      <c r="M8" s="192" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="174"/>
-      <c r="O8" s="174"/>
-      <c r="P8" s="174"/>
-      <c r="Q8" s="175"/>
-      <c r="R8" s="176" t="s">
+      <c r="N8" s="164"/>
+      <c r="O8" s="164"/>
+      <c r="P8" s="164"/>
+      <c r="Q8" s="193"/>
+      <c r="R8" s="194" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="174"/>
-      <c r="T8" s="174"/>
-      <c r="U8" s="174"/>
-      <c r="V8" s="175"/>
-      <c r="W8" s="176" t="s">
+      <c r="S8" s="164"/>
+      <c r="T8" s="164"/>
+      <c r="U8" s="164"/>
+      <c r="V8" s="193"/>
+      <c r="W8" s="194" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="174"/>
-      <c r="Y8" s="174"/>
-      <c r="Z8" s="174"/>
-      <c r="AA8" s="177"/>
-      <c r="AB8" s="178" t="s">
+      <c r="X8" s="164"/>
+      <c r="Y8" s="164"/>
+      <c r="Z8" s="164"/>
+      <c r="AA8" s="165"/>
+      <c r="AB8" s="195" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="174"/>
-      <c r="AD8" s="174"/>
-      <c r="AE8" s="174"/>
-      <c r="AF8" s="175"/>
-      <c r="AG8" s="179" t="s">
+      <c r="AC8" s="164"/>
+      <c r="AD8" s="164"/>
+      <c r="AE8" s="164"/>
+      <c r="AF8" s="193"/>
+      <c r="AG8" s="196" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="174"/>
-      <c r="AI8" s="174"/>
-      <c r="AJ8" s="174"/>
-      <c r="AK8" s="175"/>
-      <c r="AL8" s="179" t="s">
+      <c r="AH8" s="164"/>
+      <c r="AI8" s="164"/>
+      <c r="AJ8" s="164"/>
+      <c r="AK8" s="193"/>
+      <c r="AL8" s="196" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="174"/>
-      <c r="AN8" s="174"/>
-      <c r="AO8" s="174"/>
-      <c r="AP8" s="177"/>
-      <c r="AQ8" s="180" t="s">
+      <c r="AM8" s="164"/>
+      <c r="AN8" s="164"/>
+      <c r="AO8" s="164"/>
+      <c r="AP8" s="165"/>
+      <c r="AQ8" s="197" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="174"/>
-      <c r="AS8" s="174"/>
-      <c r="AT8" s="174"/>
-      <c r="AU8" s="175"/>
-      <c r="AV8" s="181" t="s">
+      <c r="AR8" s="164"/>
+      <c r="AS8" s="164"/>
+      <c r="AT8" s="164"/>
+      <c r="AU8" s="193"/>
+      <c r="AV8" s="198" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="174"/>
-      <c r="AX8" s="174"/>
-      <c r="AY8" s="174"/>
-      <c r="AZ8" s="175"/>
-      <c r="BA8" s="181" t="s">
+      <c r="AW8" s="164"/>
+      <c r="AX8" s="164"/>
+      <c r="AY8" s="164"/>
+      <c r="AZ8" s="193"/>
+      <c r="BA8" s="198" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="174"/>
-      <c r="BC8" s="174"/>
-      <c r="BD8" s="174"/>
-      <c r="BE8" s="177"/>
-      <c r="BF8" s="182" t="s">
+      <c r="BB8" s="164"/>
+      <c r="BC8" s="164"/>
+      <c r="BD8" s="164"/>
+      <c r="BE8" s="165"/>
+      <c r="BF8" s="199" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="174"/>
-      <c r="BH8" s="174"/>
-      <c r="BI8" s="174"/>
-      <c r="BJ8" s="175"/>
-      <c r="BK8" s="183" t="s">
+      <c r="BG8" s="164"/>
+      <c r="BH8" s="164"/>
+      <c r="BI8" s="164"/>
+      <c r="BJ8" s="193"/>
+      <c r="BK8" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="174"/>
-      <c r="BM8" s="174"/>
-      <c r="BN8" s="174"/>
-      <c r="BO8" s="175"/>
-      <c r="BP8" s="183" t="s">
+      <c r="BL8" s="164"/>
+      <c r="BM8" s="164"/>
+      <c r="BN8" s="164"/>
+      <c r="BO8" s="193"/>
+      <c r="BP8" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="174"/>
-      <c r="BR8" s="174"/>
-      <c r="BS8" s="174"/>
-      <c r="BT8" s="177"/>
+      <c r="BQ8" s="164"/>
+      <c r="BR8" s="164"/>
+      <c r="BS8" s="164"/>
+      <c r="BT8" s="165"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="190"/>
-      <c r="C9" s="192"/>
-      <c r="D9" s="194"/>
+      <c r="B9" s="172"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="176"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12774,11 +12780,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="199"/>
-      <c r="I9" s="167"/>
-      <c r="J9" s="169"/>
-      <c r="K9" s="169"/>
-      <c r="L9" s="172"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="186"/>
+      <c r="J9" s="188"/>
+      <c r="K9" s="188"/>
+      <c r="L9" s="191"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -14702,15 +14708,15 @@
       <c r="D28" s="74"/>
       <c r="E28" s="42">
         <f t="shared" ref="E28:G28" si="5">SUM(E29:E34)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F28" s="43">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G28" s="44">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H28" s="75">
         <v>3</v>
@@ -14720,7 +14726,7 @@
       <c r="K28" s="77"/>
       <c r="L28" s="49">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="M28" s="50"/>
       <c r="N28" s="51"/>
@@ -14884,24 +14890,36 @@
       <c r="B30" s="53">
         <v>3.2</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
+      <c r="C30" s="54" t="s">
+        <v>236</v>
+      </c>
+      <c r="D30" s="55" t="s">
+        <v>235</v>
+      </c>
+      <c r="E30" s="56">
+        <v>5</v>
+      </c>
+      <c r="F30" s="57">
+        <v>2</v>
+      </c>
       <c r="G30" s="58">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="59"/>
-      <c r="I30" s="157"/>
+        <v>3</v>
+      </c>
+      <c r="H30" s="59">
+        <v>3</v>
+      </c>
+      <c r="I30" s="157">
+        <v>45399</v>
+      </c>
       <c r="J30" s="61"/>
       <c r="K30" s="62">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="L30" s="63" t="e">
+        <v>-45398</v>
+      </c>
+      <c r="L30" s="63">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.4</v>
       </c>
       <c r="M30" s="64"/>
       <c r="N30" s="65"/>
@@ -14935,7 +14953,7 @@
       <c r="AP30" s="68"/>
       <c r="AQ30" s="64"/>
       <c r="AR30" s="65"/>
-      <c r="AS30" s="65"/>
+      <c r="AS30" s="112"/>
       <c r="AT30" s="65"/>
       <c r="AU30" s="65"/>
       <c r="AV30" s="70"/>
@@ -15749,22 +15767,22 @@
       </c>
       <c r="E41" s="101">
         <f>SUM(E11:E16,E18:E21,E29:E34,E36:E39)</f>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F41" s="101">
         <f>SUM(F11:F16,F18:F21,F29:F34,F36:F39)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G41" s="101">
         <f>SUM(G11:G16,G18:G21,G29:G34,G36:G39)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H41" s="101">
         <v>60</v>
       </c>
       <c r="I41" s="101">
         <f>E41/H41</f>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="L41" s="102" t="s">
         <v>77</v>
@@ -15962,243 +15980,243 @@
       </c>
       <c r="M42" s="105">
         <f>E41</f>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N42" s="106">
         <f>M42-I41</f>
-        <v>29.5</v>
+        <v>34.416666666666664</v>
       </c>
       <c r="O42" s="106">
         <f>N42-I41</f>
-        <v>29</v>
+        <v>33.833333333333329</v>
       </c>
       <c r="P42" s="106">
         <f>O42-I41</f>
-        <v>28.5</v>
+        <v>33.249999999999993</v>
       </c>
       <c r="Q42" s="106">
         <f>P42-I41</f>
-        <v>28</v>
+        <v>32.666666666666657</v>
       </c>
       <c r="R42" s="106">
         <f>Q42-I41</f>
-        <v>27.5</v>
+        <v>32.083333333333321</v>
       </c>
       <c r="S42" s="106">
         <f>R42-I41</f>
-        <v>27</v>
+        <v>31.499999999999989</v>
       </c>
       <c r="T42" s="106">
         <f>S42-I41</f>
-        <v>26.5</v>
+        <v>30.916666666666657</v>
       </c>
       <c r="U42" s="106">
         <f>T42-I41</f>
-        <v>26</v>
+        <v>30.333333333333325</v>
       </c>
       <c r="V42" s="106">
         <f>U42-I41</f>
-        <v>25.5</v>
+        <v>29.749999999999993</v>
       </c>
       <c r="W42" s="106">
         <f>V42-I41</f>
-        <v>25</v>
+        <v>29.166666666666661</v>
       </c>
       <c r="X42" s="106">
         <f>W42-I41</f>
-        <v>24.5</v>
+        <v>28.583333333333329</v>
       </c>
       <c r="Y42" s="106">
         <f>X42-I41</f>
-        <v>24</v>
+        <v>27.999999999999996</v>
       </c>
       <c r="Z42" s="106">
         <f>Y42-I41</f>
-        <v>23.5</v>
+        <v>27.416666666666664</v>
       </c>
       <c r="AA42" s="106">
         <f>Z42-I41</f>
-        <v>23</v>
+        <v>26.833333333333332</v>
       </c>
       <c r="AB42" s="106">
         <f>AA42-I41</f>
-        <v>22.5</v>
+        <v>26.25</v>
       </c>
       <c r="AC42" s="106">
         <f>AB42-I41</f>
-        <v>22</v>
+        <v>25.666666666666668</v>
       </c>
       <c r="AD42" s="106">
         <f>AC42-I41</f>
-        <v>21.5</v>
+        <v>25.083333333333336</v>
       </c>
       <c r="AE42" s="106">
         <f>AD42-I41</f>
-        <v>21</v>
+        <v>24.500000000000004</v>
       </c>
       <c r="AF42" s="106">
         <f>AE42-I41</f>
-        <v>20.5</v>
+        <v>23.916666666666671</v>
       </c>
       <c r="AG42" s="106">
         <f>AF42-I41</f>
-        <v>20</v>
+        <v>23.333333333333339</v>
       </c>
       <c r="AH42" s="106">
         <f>AG42-I41</f>
-        <v>19.5</v>
+        <v>22.750000000000007</v>
       </c>
       <c r="AI42" s="106">
         <f>AH42-I41</f>
-        <v>19</v>
+        <v>22.166666666666675</v>
       </c>
       <c r="AJ42" s="106">
         <f>AI42-I41</f>
-        <v>18.5</v>
+        <v>21.583333333333343</v>
       </c>
       <c r="AK42" s="106">
         <f>AJ42-I41</f>
-        <v>18</v>
+        <v>21.000000000000011</v>
       </c>
       <c r="AL42" s="106">
         <f>AK42-I41</f>
-        <v>17.5</v>
+        <v>20.416666666666679</v>
       </c>
       <c r="AM42" s="106">
         <f>AL42-I41</f>
-        <v>17</v>
+        <v>19.833333333333346</v>
       </c>
       <c r="AN42" s="106">
         <f>AM42-I41</f>
-        <v>16.5</v>
+        <v>19.250000000000014</v>
       </c>
       <c r="AO42" s="106">
         <f>AN42-I41</f>
-        <v>16</v>
+        <v>18.666666666666682</v>
       </c>
       <c r="AP42" s="106">
         <f>AO42-I41</f>
-        <v>15.5</v>
+        <v>18.08333333333335</v>
       </c>
       <c r="AQ42" s="106">
         <f>AP42-I41</f>
-        <v>15</v>
+        <v>17.500000000000018</v>
       </c>
       <c r="AR42" s="106">
         <f>AQ42-I41</f>
-        <v>14.5</v>
+        <v>16.916666666666686</v>
       </c>
       <c r="AS42" s="106">
         <f>AR42-I41</f>
-        <v>14</v>
+        <v>16.333333333333353</v>
       </c>
       <c r="AT42" s="106">
         <f>AS42-I41</f>
-        <v>13.5</v>
+        <v>15.75000000000002</v>
       </c>
       <c r="AU42" s="106">
         <f>AT42-I41</f>
-        <v>13</v>
+        <v>15.166666666666686</v>
       </c>
       <c r="AV42" s="106">
         <f>AU42-I41</f>
-        <v>12.5</v>
+        <v>14.583333333333352</v>
       </c>
       <c r="AW42" s="106">
         <f>AV42-I41</f>
-        <v>12</v>
+        <v>14.000000000000018</v>
       </c>
       <c r="AX42" s="106">
         <f>AW42-I41</f>
-        <v>11.5</v>
+        <v>13.416666666666684</v>
       </c>
       <c r="AY42" s="106">
         <f>AX42-I41</f>
-        <v>11</v>
+        <v>12.83333333333335</v>
       </c>
       <c r="AZ42" s="106">
         <f>AY42-I41</f>
-        <v>10.5</v>
+        <v>12.250000000000016</v>
       </c>
       <c r="BA42" s="106">
         <f>AZ42-I41</f>
-        <v>10</v>
+        <v>11.666666666666682</v>
       </c>
       <c r="BB42" s="106">
         <f>BA42-I41</f>
-        <v>9.5</v>
+        <v>11.083333333333348</v>
       </c>
       <c r="BC42" s="106">
         <f>BB42-I41</f>
-        <v>9</v>
+        <v>10.500000000000014</v>
       </c>
       <c r="BD42" s="106">
         <f>BC42-I41</f>
-        <v>8.5</v>
+        <v>9.9166666666666803</v>
       </c>
       <c r="BE42" s="106">
         <f>BD42-I41</f>
-        <v>8</v>
+        <v>9.3333333333333464</v>
       </c>
       <c r="BF42" s="106">
         <f>BE42-I41</f>
-        <v>7.5</v>
+        <v>8.7500000000000124</v>
       </c>
       <c r="BG42" s="106">
         <f>BF42-I41</f>
-        <v>7</v>
+        <v>8.1666666666666785</v>
       </c>
       <c r="BH42" s="106">
         <f>BG42-I41</f>
-        <v>6.5</v>
+        <v>7.5833333333333455</v>
       </c>
       <c r="BI42" s="106">
         <f>BH42-I41</f>
-        <v>6</v>
+        <v>7.0000000000000124</v>
       </c>
       <c r="BJ42" s="106">
         <f>BI42-I41</f>
-        <v>5.5</v>
+        <v>6.4166666666666794</v>
       </c>
       <c r="BK42" s="106">
         <f>BJ42-I41</f>
-        <v>5</v>
+        <v>5.8333333333333464</v>
       </c>
       <c r="BL42" s="106">
         <f>BK42-I41</f>
-        <v>4.5</v>
+        <v>5.2500000000000133</v>
       </c>
       <c r="BM42" s="106">
         <f>BL42-I41</f>
-        <v>4</v>
+        <v>4.6666666666666803</v>
       </c>
       <c r="BN42" s="106">
         <f>BM42-I41</f>
-        <v>3.5</v>
+        <v>4.0833333333333472</v>
       </c>
       <c r="BO42" s="106">
         <f>BN42-I41</f>
-        <v>3</v>
+        <v>3.5000000000000138</v>
       </c>
       <c r="BP42" s="106">
         <f>BO42-I41</f>
-        <v>2.5</v>
+        <v>2.9166666666666803</v>
       </c>
       <c r="BQ42" s="106">
         <f>BP42-I41</f>
-        <v>2</v>
+        <v>2.3333333333333468</v>
       </c>
       <c r="BR42" s="106">
         <f>BQ42-I41</f>
-        <v>1.5</v>
+        <v>1.7500000000000133</v>
       </c>
       <c r="BS42" s="106">
         <f>BR42-I41</f>
-        <v>1</v>
+        <v>1.1666666666666798</v>
       </c>
       <c r="BT42" s="106">
         <f>BS42-I41</f>
-        <v>0.5</v>
+        <v>0.58333333333334647</v>
       </c>
       <c r="BV42" s="101"/>
     </row>
@@ -16208,247 +16226,247 @@
       </c>
       <c r="M43" s="105">
         <f>E41</f>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N43" s="105">
         <f t="shared" ref="N43:BT43" si="11">M45</f>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="T43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="V43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="X43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Y43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Z43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AA43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AB43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AC43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AD43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AE43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AF43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AG43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AH43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AI43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AJ43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AK43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AL43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AM43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AN43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AO43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AP43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AQ43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AR43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AS43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AT43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AU43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AV43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AW43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AX43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AY43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AZ43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BA43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BB43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BC43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BD43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BE43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BF43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BG43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BH43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BI43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BJ43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BK43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BL43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BM43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BN43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BO43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BP43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BQ43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BR43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BS43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BT43" s="105">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BV43" s="101">
         <f t="shared" ref="BV43:BV45" si="12">SUM(M43:BT43)</f>
-        <v>1800</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16529,247 +16547,247 @@
       </c>
       <c r="M45" s="105">
         <f t="shared" ref="M45:BT45" si="13">M43-M44</f>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="T45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="V45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="X45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Y45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Z45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AA45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AB45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AC45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AD45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AE45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AF45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AG45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AH45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AI45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AJ45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AK45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AL45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AM45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AN45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AO45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AP45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AQ45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AR45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AS45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AT45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AU45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AV45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AW45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AX45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AY45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AZ45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BA45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BB45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BC45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BD45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BE45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BF45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BG45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BH45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BI45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BJ45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BK45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BL45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BM45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BN45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BO45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BP45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BQ45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BR45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BS45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BT45" s="105">
         <f t="shared" si="13"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="BV45" s="101">
         <f t="shared" si="12"/>
-        <v>1800</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="46" spans="2:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16779,55 +16797,55 @@
       <c r="E49" s="200" t="s">
         <v>83</v>
       </c>
-      <c r="F49" s="164"/>
-      <c r="G49" s="164"/>
-      <c r="H49" s="164"/>
-      <c r="I49" s="164"/>
-      <c r="J49" s="164"/>
-      <c r="K49" s="164"/>
-      <c r="L49" s="164"/>
-      <c r="M49" s="164"/>
-      <c r="N49" s="164"/>
-      <c r="O49" s="164"/>
-      <c r="P49" s="164"/>
-      <c r="Q49" s="164"/>
-      <c r="R49" s="164"/>
-      <c r="S49" s="164"/>
-      <c r="T49" s="164"/>
-      <c r="U49" s="164"/>
-      <c r="V49" s="164"/>
-      <c r="W49" s="164"/>
-      <c r="X49" s="164"/>
-      <c r="Y49" s="164"/>
-      <c r="Z49" s="164"/>
-      <c r="AA49" s="164"/>
-      <c r="AB49" s="164"/>
-      <c r="AC49" s="164"/>
-      <c r="AD49" s="164"/>
-      <c r="AE49" s="164"/>
-      <c r="AF49" s="164"/>
-      <c r="AG49" s="164"/>
-      <c r="AH49" s="164"/>
-      <c r="AI49" s="164"/>
-      <c r="AJ49" s="164"/>
-      <c r="AK49" s="164"/>
-      <c r="AL49" s="164"/>
-      <c r="AM49" s="164"/>
-      <c r="AN49" s="164"/>
-      <c r="AO49" s="164"/>
-      <c r="AP49" s="164"/>
-      <c r="AQ49" s="164"/>
-      <c r="AR49" s="164"/>
-      <c r="AS49" s="164"/>
-      <c r="AT49" s="164"/>
-      <c r="AU49" s="164"/>
-      <c r="AV49" s="164"/>
-      <c r="AW49" s="164"/>
-      <c r="AX49" s="164"/>
-      <c r="AY49" s="164"/>
-      <c r="AZ49" s="164"/>
-      <c r="BA49" s="164"/>
-      <c r="BB49" s="165"/>
+      <c r="F49" s="183"/>
+      <c r="G49" s="183"/>
+      <c r="H49" s="183"/>
+      <c r="I49" s="183"/>
+      <c r="J49" s="183"/>
+      <c r="K49" s="183"/>
+      <c r="L49" s="183"/>
+      <c r="M49" s="183"/>
+      <c r="N49" s="183"/>
+      <c r="O49" s="183"/>
+      <c r="P49" s="183"/>
+      <c r="Q49" s="183"/>
+      <c r="R49" s="183"/>
+      <c r="S49" s="183"/>
+      <c r="T49" s="183"/>
+      <c r="U49" s="183"/>
+      <c r="V49" s="183"/>
+      <c r="W49" s="183"/>
+      <c r="X49" s="183"/>
+      <c r="Y49" s="183"/>
+      <c r="Z49" s="183"/>
+      <c r="AA49" s="183"/>
+      <c r="AB49" s="183"/>
+      <c r="AC49" s="183"/>
+      <c r="AD49" s="183"/>
+      <c r="AE49" s="183"/>
+      <c r="AF49" s="183"/>
+      <c r="AG49" s="183"/>
+      <c r="AH49" s="183"/>
+      <c r="AI49" s="183"/>
+      <c r="AJ49" s="183"/>
+      <c r="AK49" s="183"/>
+      <c r="AL49" s="183"/>
+      <c r="AM49" s="183"/>
+      <c r="AN49" s="183"/>
+      <c r="AO49" s="183"/>
+      <c r="AP49" s="183"/>
+      <c r="AQ49" s="183"/>
+      <c r="AR49" s="183"/>
+      <c r="AS49" s="183"/>
+      <c r="AT49" s="183"/>
+      <c r="AU49" s="183"/>
+      <c r="AV49" s="183"/>
+      <c r="AW49" s="183"/>
+      <c r="AX49" s="183"/>
+      <c r="AY49" s="183"/>
+      <c r="AZ49" s="183"/>
+      <c r="BA49" s="183"/>
+      <c r="BB49" s="184"/>
     </row>
     <row r="50" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17790,13 +17808,6 @@
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
     <mergeCell ref="E49:BB49"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
@@ -17813,6 +17824,13 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
signup/login logic ended and continuing with Personal page logic
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\Progetto\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B235F6-9353-4BC4-9EA2-DF2979CC4854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F32D3BD-EFF5-4C4C-AB53-A7A71F74BDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="240">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -710,9 +710,6 @@
     <t xml:space="preserve"> Local db (sql file + docker)</t>
   </si>
   <si>
-    <t>Signup/login</t>
-  </si>
-  <si>
     <t>2.10</t>
   </si>
   <si>
@@ -746,13 +743,19 @@
     <t>Everyone</t>
   </si>
   <si>
-    <t>Signup/Login Logic</t>
-  </si>
-  <si>
     <t>User Personal Animaldex</t>
   </si>
   <si>
     <t>Valerio Baldi Saverio Dieni</t>
+  </si>
+  <si>
+    <t>PersonalPage Logic</t>
+  </si>
+  <si>
+    <t>Signup/Login Logic Part 2</t>
+  </si>
+  <si>
+    <t>Signup/login Logic Part 1</t>
   </si>
 </sst>
 </file>
@@ -2476,53 +2479,11 @@
     <xf numFmtId="14" fontId="24" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2553,6 +2514,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5457,184 +5460,184 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.31666666666667</c:v>
+                  <c:v>35.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.63333333333334</c:v>
+                  <c:v>34.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.95000000000001</c:v>
+                  <c:v>34.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.26666666666668</c:v>
+                  <c:v>33.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.58333333333335</c:v>
+                  <c:v>32.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.90000000000002</c:v>
+                  <c:v>32.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.21666666666669</c:v>
+                  <c:v>31.79999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.53333333333336</c:v>
+                  <c:v>31.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.85000000000003</c:v>
+                  <c:v>30.599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34.1666666666667</c:v>
+                  <c:v>29.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33.48333333333337</c:v>
+                  <c:v>29.399999999999984</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>32.80000000000004</c:v>
+                  <c:v>28.799999999999983</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.11666666666671</c:v>
+                  <c:v>28.199999999999982</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31.433333333333376</c:v>
+                  <c:v>27.59999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30.750000000000043</c:v>
+                  <c:v>26.999999999999979</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30.066666666666709</c:v>
+                  <c:v>26.399999999999977</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.383333333333375</c:v>
+                  <c:v>25.799999999999976</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>28.700000000000042</c:v>
+                  <c:v>25.199999999999974</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>28.016666666666708</c:v>
+                  <c:v>24.599999999999973</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>27.333333333333375</c:v>
+                  <c:v>23.999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26.650000000000041</c:v>
+                  <c:v>23.39999999999997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>25.966666666666708</c:v>
+                  <c:v>22.799999999999969</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>25.283333333333374</c:v>
+                  <c:v>22.199999999999967</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.600000000000041</c:v>
+                  <c:v>21.599999999999966</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.916666666666707</c:v>
+                  <c:v>20.999999999999964</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>23.233333333333373</c:v>
+                  <c:v>20.399999999999963</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>22.55000000000004</c:v>
+                  <c:v>19.799999999999962</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>21.866666666666706</c:v>
+                  <c:v>19.19999999999996</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>21.183333333333373</c:v>
+                  <c:v>18.599999999999959</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>20.500000000000039</c:v>
+                  <c:v>17.999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>19.816666666666706</c:v>
+                  <c:v>17.399999999999956</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>19.133333333333372</c:v>
+                  <c:v>16.799999999999955</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>18.450000000000038</c:v>
+                  <c:v>16.199999999999953</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>17.766666666666705</c:v>
+                  <c:v>15.599999999999953</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>17.083333333333371</c:v>
+                  <c:v>14.999999999999954</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>16.400000000000038</c:v>
+                  <c:v>14.399999999999954</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>15.716666666666704</c:v>
+                  <c:v>13.799999999999955</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>15.033333333333371</c:v>
+                  <c:v>13.199999999999955</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>14.350000000000037</c:v>
+                  <c:v>12.599999999999955</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>13.666666666666703</c:v>
+                  <c:v>11.999999999999956</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>12.98333333333337</c:v>
+                  <c:v>11.399999999999956</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>12.300000000000036</c:v>
+                  <c:v>10.799999999999956</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>11.616666666666703</c:v>
+                  <c:v>10.199999999999957</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>10.933333333333369</c:v>
+                  <c:v>9.599999999999957</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>10.250000000000036</c:v>
+                  <c:v>8.9999999999999574</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>9.566666666666702</c:v>
+                  <c:v>8.3999999999999577</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>8.8833333333333684</c:v>
+                  <c:v>7.7999999999999581</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>8.2000000000000348</c:v>
+                  <c:v>7.1999999999999584</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>7.5166666666667012</c:v>
+                  <c:v>6.5999999999999588</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6.8333333333333677</c:v>
+                  <c:v>5.9999999999999591</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6.1500000000000341</c:v>
+                  <c:v>5.3999999999999595</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>5.4666666666667005</c:v>
+                  <c:v>4.7999999999999599</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.783333333333367</c:v>
+                  <c:v>4.1999999999999602</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.1000000000000334</c:v>
+                  <c:v>3.5999999999999601</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3.4166666666666998</c:v>
+                  <c:v>2.99999999999996</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.7333333333333663</c:v>
+                  <c:v>2.3999999999999599</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.0500000000000327</c:v>
+                  <c:v>1.7999999999999599</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.3666666666666993</c:v>
+                  <c:v>1.1999999999999598</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.68333333333336599</c:v>
+                  <c:v>0.59999999999995979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5868,184 +5871,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6950,19 +6953,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="184" t="str">
+      <c r="BK2" s="166" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="185"/>
-      <c r="BM2" s="185"/>
-      <c r="BN2" s="185"/>
-      <c r="BO2" s="185"/>
-      <c r="BP2" s="185"/>
-      <c r="BQ2" s="185"/>
-      <c r="BR2" s="185"/>
-      <c r="BS2" s="185"/>
-      <c r="BT2" s="185"/>
+      <c r="BL2" s="167"/>
+      <c r="BM2" s="167"/>
+      <c r="BN2" s="167"/>
+      <c r="BO2" s="167"/>
+      <c r="BP2" s="167"/>
+      <c r="BQ2" s="167"/>
+      <c r="BR2" s="167"/>
+      <c r="BS2" s="167"/>
+      <c r="BT2" s="167"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -6990,7 +6993,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="186" t="s">
+      <c r="K4" s="168" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7067,7 +7070,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="187"/>
+      <c r="K5" s="169"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7142,7 +7145,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="187"/>
+      <c r="K6" s="169"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7217,7 +7220,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="187"/>
+      <c r="K7" s="169"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7292,7 +7295,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="188"/>
+      <c r="K8" s="170"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7358,124 +7361,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="189" t="s">
+      <c r="B9" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="191" t="s">
+      <c r="C9" s="173" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="193" t="s">
+      <c r="D9" s="175" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="195" t="s">
+      <c r="E9" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="196"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="198" t="s">
+      <c r="F9" s="178"/>
+      <c r="G9" s="179"/>
+      <c r="H9" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="166" t="s">
+      <c r="I9" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="168" t="s">
+      <c r="J9" s="187" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="170" t="s">
+      <c r="K9" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="171" t="s">
+      <c r="L9" s="190" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="173" t="s">
+      <c r="M9" s="192" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="174"/>
-      <c r="O9" s="174"/>
-      <c r="P9" s="174"/>
-      <c r="Q9" s="175"/>
-      <c r="R9" s="176" t="s">
+      <c r="N9" s="164"/>
+      <c r="O9" s="164"/>
+      <c r="P9" s="164"/>
+      <c r="Q9" s="193"/>
+      <c r="R9" s="194" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="174"/>
-      <c r="T9" s="174"/>
-      <c r="U9" s="174"/>
-      <c r="V9" s="175"/>
-      <c r="W9" s="176" t="s">
+      <c r="S9" s="164"/>
+      <c r="T9" s="164"/>
+      <c r="U9" s="164"/>
+      <c r="V9" s="193"/>
+      <c r="W9" s="194" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="174"/>
-      <c r="Y9" s="174"/>
-      <c r="Z9" s="174"/>
-      <c r="AA9" s="177"/>
-      <c r="AB9" s="178" t="s">
+      <c r="X9" s="164"/>
+      <c r="Y9" s="164"/>
+      <c r="Z9" s="164"/>
+      <c r="AA9" s="165"/>
+      <c r="AB9" s="195" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="174"/>
-      <c r="AD9" s="174"/>
-      <c r="AE9" s="174"/>
-      <c r="AF9" s="175"/>
-      <c r="AG9" s="179" t="s">
+      <c r="AC9" s="164"/>
+      <c r="AD9" s="164"/>
+      <c r="AE9" s="164"/>
+      <c r="AF9" s="193"/>
+      <c r="AG9" s="196" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="174"/>
-      <c r="AI9" s="174"/>
-      <c r="AJ9" s="174"/>
-      <c r="AK9" s="175"/>
-      <c r="AL9" s="179" t="s">
+      <c r="AH9" s="164"/>
+      <c r="AI9" s="164"/>
+      <c r="AJ9" s="164"/>
+      <c r="AK9" s="193"/>
+      <c r="AL9" s="196" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="174"/>
-      <c r="AN9" s="174"/>
-      <c r="AO9" s="174"/>
-      <c r="AP9" s="177"/>
-      <c r="AQ9" s="180" t="s">
+      <c r="AM9" s="164"/>
+      <c r="AN9" s="164"/>
+      <c r="AO9" s="164"/>
+      <c r="AP9" s="165"/>
+      <c r="AQ9" s="197" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="174"/>
-      <c r="AS9" s="174"/>
-      <c r="AT9" s="174"/>
-      <c r="AU9" s="175"/>
-      <c r="AV9" s="181" t="s">
+      <c r="AR9" s="164"/>
+      <c r="AS9" s="164"/>
+      <c r="AT9" s="164"/>
+      <c r="AU9" s="193"/>
+      <c r="AV9" s="198" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="174"/>
-      <c r="AX9" s="174"/>
-      <c r="AY9" s="174"/>
-      <c r="AZ9" s="175"/>
-      <c r="BA9" s="181" t="s">
+      <c r="AW9" s="164"/>
+      <c r="AX9" s="164"/>
+      <c r="AY9" s="164"/>
+      <c r="AZ9" s="193"/>
+      <c r="BA9" s="198" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="174"/>
-      <c r="BC9" s="174"/>
-      <c r="BD9" s="174"/>
-      <c r="BE9" s="177"/>
-      <c r="BF9" s="182" t="s">
+      <c r="BB9" s="164"/>
+      <c r="BC9" s="164"/>
+      <c r="BD9" s="164"/>
+      <c r="BE9" s="165"/>
+      <c r="BF9" s="199" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="174"/>
-      <c r="BH9" s="174"/>
-      <c r="BI9" s="174"/>
-      <c r="BJ9" s="175"/>
-      <c r="BK9" s="183" t="s">
+      <c r="BG9" s="164"/>
+      <c r="BH9" s="164"/>
+      <c r="BI9" s="164"/>
+      <c r="BJ9" s="193"/>
+      <c r="BK9" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="174"/>
-      <c r="BM9" s="174"/>
-      <c r="BN9" s="174"/>
-      <c r="BO9" s="175"/>
-      <c r="BP9" s="183" t="s">
+      <c r="BL9" s="164"/>
+      <c r="BM9" s="164"/>
+      <c r="BN9" s="164"/>
+      <c r="BO9" s="193"/>
+      <c r="BP9" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="174"/>
-      <c r="BR9" s="174"/>
-      <c r="BS9" s="174"/>
-      <c r="BT9" s="177"/>
+      <c r="BQ9" s="164"/>
+      <c r="BR9" s="164"/>
+      <c r="BS9" s="164"/>
+      <c r="BT9" s="165"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="190"/>
-      <c r="C10" s="192"/>
-      <c r="D10" s="194"/>
+      <c r="B10" s="172"/>
+      <c r="C10" s="174"/>
+      <c r="D10" s="176"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7485,11 +7488,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="199"/>
-      <c r="I10" s="167"/>
-      <c r="J10" s="169"/>
-      <c r="K10" s="169"/>
-      <c r="L10" s="172"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="186"/>
+      <c r="J10" s="188"/>
+      <c r="K10" s="188"/>
+      <c r="L10" s="191"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11098,80 +11101,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="163" t="str">
+      <c r="B45" s="182" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="164"/>
-      <c r="D45" s="164"/>
-      <c r="E45" s="164"/>
-      <c r="F45" s="164"/>
-      <c r="G45" s="164"/>
-      <c r="H45" s="164"/>
-      <c r="I45" s="164"/>
-      <c r="J45" s="164"/>
-      <c r="K45" s="164"/>
-      <c r="L45" s="164"/>
-      <c r="M45" s="164"/>
-      <c r="N45" s="164"/>
-      <c r="O45" s="164"/>
-      <c r="P45" s="164"/>
-      <c r="Q45" s="164"/>
-      <c r="R45" s="164"/>
-      <c r="S45" s="164"/>
-      <c r="T45" s="164"/>
-      <c r="U45" s="164"/>
-      <c r="V45" s="164"/>
-      <c r="W45" s="164"/>
-      <c r="X45" s="164"/>
-      <c r="Y45" s="164"/>
-      <c r="Z45" s="164"/>
-      <c r="AA45" s="164"/>
-      <c r="AB45" s="164"/>
-      <c r="AC45" s="164"/>
-      <c r="AD45" s="164"/>
-      <c r="AE45" s="164"/>
-      <c r="AF45" s="164"/>
-      <c r="AG45" s="164"/>
-      <c r="AH45" s="164"/>
-      <c r="AI45" s="164"/>
-      <c r="AJ45" s="164"/>
-      <c r="AK45" s="164"/>
-      <c r="AL45" s="164"/>
-      <c r="AM45" s="164"/>
-      <c r="AN45" s="164"/>
-      <c r="AO45" s="164"/>
-      <c r="AP45" s="164"/>
-      <c r="AQ45" s="164"/>
-      <c r="AR45" s="164"/>
-      <c r="AS45" s="164"/>
-      <c r="AT45" s="164"/>
-      <c r="AU45" s="164"/>
-      <c r="AV45" s="164"/>
-      <c r="AW45" s="164"/>
-      <c r="AX45" s="164"/>
-      <c r="AY45" s="164"/>
-      <c r="AZ45" s="164"/>
-      <c r="BA45" s="164"/>
-      <c r="BB45" s="164"/>
-      <c r="BC45" s="164"/>
-      <c r="BD45" s="164"/>
-      <c r="BE45" s="164"/>
-      <c r="BF45" s="164"/>
-      <c r="BG45" s="164"/>
-      <c r="BH45" s="164"/>
-      <c r="BI45" s="164"/>
-      <c r="BJ45" s="164"/>
-      <c r="BK45" s="164"/>
-      <c r="BL45" s="164"/>
-      <c r="BM45" s="164"/>
-      <c r="BN45" s="164"/>
-      <c r="BO45" s="164"/>
-      <c r="BP45" s="164"/>
-      <c r="BQ45" s="164"/>
-      <c r="BR45" s="164"/>
-      <c r="BS45" s="164"/>
-      <c r="BT45" s="165"/>
+      <c r="C45" s="183"/>
+      <c r="D45" s="183"/>
+      <c r="E45" s="183"/>
+      <c r="F45" s="183"/>
+      <c r="G45" s="183"/>
+      <c r="H45" s="183"/>
+      <c r="I45" s="183"/>
+      <c r="J45" s="183"/>
+      <c r="K45" s="183"/>
+      <c r="L45" s="183"/>
+      <c r="M45" s="183"/>
+      <c r="N45" s="183"/>
+      <c r="O45" s="183"/>
+      <c r="P45" s="183"/>
+      <c r="Q45" s="183"/>
+      <c r="R45" s="183"/>
+      <c r="S45" s="183"/>
+      <c r="T45" s="183"/>
+      <c r="U45" s="183"/>
+      <c r="V45" s="183"/>
+      <c r="W45" s="183"/>
+      <c r="X45" s="183"/>
+      <c r="Y45" s="183"/>
+      <c r="Z45" s="183"/>
+      <c r="AA45" s="183"/>
+      <c r="AB45" s="183"/>
+      <c r="AC45" s="183"/>
+      <c r="AD45" s="183"/>
+      <c r="AE45" s="183"/>
+      <c r="AF45" s="183"/>
+      <c r="AG45" s="183"/>
+      <c r="AH45" s="183"/>
+      <c r="AI45" s="183"/>
+      <c r="AJ45" s="183"/>
+      <c r="AK45" s="183"/>
+      <c r="AL45" s="183"/>
+      <c r="AM45" s="183"/>
+      <c r="AN45" s="183"/>
+      <c r="AO45" s="183"/>
+      <c r="AP45" s="183"/>
+      <c r="AQ45" s="183"/>
+      <c r="AR45" s="183"/>
+      <c r="AS45" s="183"/>
+      <c r="AT45" s="183"/>
+      <c r="AU45" s="183"/>
+      <c r="AV45" s="183"/>
+      <c r="AW45" s="183"/>
+      <c r="AX45" s="183"/>
+      <c r="AY45" s="183"/>
+      <c r="AZ45" s="183"/>
+      <c r="BA45" s="183"/>
+      <c r="BB45" s="183"/>
+      <c r="BC45" s="183"/>
+      <c r="BD45" s="183"/>
+      <c r="BE45" s="183"/>
+      <c r="BF45" s="183"/>
+      <c r="BG45" s="183"/>
+      <c r="BH45" s="183"/>
+      <c r="BI45" s="183"/>
+      <c r="BJ45" s="183"/>
+      <c r="BK45" s="183"/>
+      <c r="BL45" s="183"/>
+      <c r="BM45" s="183"/>
+      <c r="BN45" s="183"/>
+      <c r="BO45" s="183"/>
+      <c r="BP45" s="183"/>
+      <c r="BQ45" s="183"/>
+      <c r="BR45" s="183"/>
+      <c r="BS45" s="183"/>
+      <c r="BT45" s="184"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12134,14 +12137,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12158,6 +12153,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12172,8 +12175,8 @@
   </sheetPr>
   <dimension ref="B1:BV1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AU35" sqref="AU35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12286,7 +12289,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="186" t="s">
+      <c r="K3" s="168" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12363,7 +12366,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="187"/>
+      <c r="K4" s="169"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12437,7 +12440,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="187"/>
+      <c r="K5" s="169"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12511,7 +12514,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="187"/>
+      <c r="K6" s="169"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12586,7 +12589,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="188"/>
+      <c r="K7" s="170"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12652,124 +12655,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="189" t="s">
+      <c r="B8" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="191" t="s">
+      <c r="C8" s="173" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="193" t="s">
+      <c r="D8" s="175" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="195" t="s">
+      <c r="E8" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="196"/>
-      <c r="G8" s="197"/>
-      <c r="H8" s="198" t="s">
+      <c r="F8" s="178"/>
+      <c r="G8" s="179"/>
+      <c r="H8" s="180" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="166" t="s">
+      <c r="I8" s="185" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="168" t="s">
+      <c r="J8" s="187" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="170" t="s">
+      <c r="K8" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="171" t="s">
+      <c r="L8" s="190" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="173" t="s">
+      <c r="M8" s="192" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="174"/>
-      <c r="O8" s="174"/>
-      <c r="P8" s="174"/>
-      <c r="Q8" s="175"/>
-      <c r="R8" s="176" t="s">
+      <c r="N8" s="164"/>
+      <c r="O8" s="164"/>
+      <c r="P8" s="164"/>
+      <c r="Q8" s="193"/>
+      <c r="R8" s="194" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="174"/>
-      <c r="T8" s="174"/>
-      <c r="U8" s="174"/>
-      <c r="V8" s="175"/>
-      <c r="W8" s="176" t="s">
+      <c r="S8" s="164"/>
+      <c r="T8" s="164"/>
+      <c r="U8" s="164"/>
+      <c r="V8" s="193"/>
+      <c r="W8" s="194" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="174"/>
-      <c r="Y8" s="174"/>
-      <c r="Z8" s="174"/>
-      <c r="AA8" s="177"/>
-      <c r="AB8" s="178" t="s">
+      <c r="X8" s="164"/>
+      <c r="Y8" s="164"/>
+      <c r="Z8" s="164"/>
+      <c r="AA8" s="165"/>
+      <c r="AB8" s="195" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="174"/>
-      <c r="AD8" s="174"/>
-      <c r="AE8" s="174"/>
-      <c r="AF8" s="175"/>
-      <c r="AG8" s="179" t="s">
+      <c r="AC8" s="164"/>
+      <c r="AD8" s="164"/>
+      <c r="AE8" s="164"/>
+      <c r="AF8" s="193"/>
+      <c r="AG8" s="196" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="174"/>
-      <c r="AI8" s="174"/>
-      <c r="AJ8" s="174"/>
-      <c r="AK8" s="175"/>
-      <c r="AL8" s="179" t="s">
+      <c r="AH8" s="164"/>
+      <c r="AI8" s="164"/>
+      <c r="AJ8" s="164"/>
+      <c r="AK8" s="193"/>
+      <c r="AL8" s="196" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="174"/>
-      <c r="AN8" s="174"/>
-      <c r="AO8" s="174"/>
-      <c r="AP8" s="177"/>
-      <c r="AQ8" s="180" t="s">
+      <c r="AM8" s="164"/>
+      <c r="AN8" s="164"/>
+      <c r="AO8" s="164"/>
+      <c r="AP8" s="165"/>
+      <c r="AQ8" s="197" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="174"/>
-      <c r="AS8" s="174"/>
-      <c r="AT8" s="174"/>
-      <c r="AU8" s="175"/>
-      <c r="AV8" s="181" t="s">
+      <c r="AR8" s="164"/>
+      <c r="AS8" s="164"/>
+      <c r="AT8" s="164"/>
+      <c r="AU8" s="193"/>
+      <c r="AV8" s="198" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="174"/>
-      <c r="AX8" s="174"/>
-      <c r="AY8" s="174"/>
-      <c r="AZ8" s="175"/>
-      <c r="BA8" s="181" t="s">
+      <c r="AW8" s="164"/>
+      <c r="AX8" s="164"/>
+      <c r="AY8" s="164"/>
+      <c r="AZ8" s="193"/>
+      <c r="BA8" s="198" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="174"/>
-      <c r="BC8" s="174"/>
-      <c r="BD8" s="174"/>
-      <c r="BE8" s="177"/>
-      <c r="BF8" s="182" t="s">
+      <c r="BB8" s="164"/>
+      <c r="BC8" s="164"/>
+      <c r="BD8" s="164"/>
+      <c r="BE8" s="165"/>
+      <c r="BF8" s="199" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="174"/>
-      <c r="BH8" s="174"/>
-      <c r="BI8" s="174"/>
-      <c r="BJ8" s="175"/>
-      <c r="BK8" s="183" t="s">
+      <c r="BG8" s="164"/>
+      <c r="BH8" s="164"/>
+      <c r="BI8" s="164"/>
+      <c r="BJ8" s="193"/>
+      <c r="BK8" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="174"/>
-      <c r="BM8" s="174"/>
-      <c r="BN8" s="174"/>
-      <c r="BO8" s="175"/>
-      <c r="BP8" s="183" t="s">
+      <c r="BL8" s="164"/>
+      <c r="BM8" s="164"/>
+      <c r="BN8" s="164"/>
+      <c r="BO8" s="193"/>
+      <c r="BP8" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="174"/>
-      <c r="BR8" s="174"/>
-      <c r="BS8" s="174"/>
-      <c r="BT8" s="177"/>
+      <c r="BQ8" s="164"/>
+      <c r="BR8" s="164"/>
+      <c r="BS8" s="164"/>
+      <c r="BT8" s="165"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="190"/>
-      <c r="C9" s="192"/>
-      <c r="D9" s="194"/>
+      <c r="B9" s="172"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="176"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12779,11 +12782,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="199"/>
-      <c r="I9" s="167"/>
-      <c r="J9" s="169"/>
-      <c r="K9" s="169"/>
-      <c r="L9" s="172"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="186"/>
+      <c r="J9" s="188"/>
+      <c r="K9" s="188"/>
+      <c r="L9" s="191"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -13649,7 +13652,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D17" s="74"/>
       <c r="E17" s="42">
@@ -14230,20 +14233,20 @@
         <v>216</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="D23" s="157" t="s">
         <v>217</v>
       </c>
       <c r="E23" s="56">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F23" s="57">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G23" s="58">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="H23" s="59">
         <v>2</v>
@@ -14260,7 +14263,7 @@
       </c>
       <c r="L23" s="63">
         <f t="shared" si="0"/>
-        <v>0.7142857142857143</v>
+        <v>1.5</v>
       </c>
       <c r="M23" s="64"/>
       <c r="N23" s="65"/>
@@ -14619,13 +14622,13 @@
     </row>
     <row r="27" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="53" t="s">
+        <v>224</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>226</v>
+      </c>
+      <c r="D27" s="157" t="s">
         <v>225</v>
-      </c>
-      <c r="C27" s="54" t="s">
-        <v>227</v>
-      </c>
-      <c r="D27" s="157" t="s">
-        <v>226</v>
       </c>
       <c r="E27" s="56">
         <v>3</v>
@@ -14720,20 +14723,20 @@
         <v>3</v>
       </c>
       <c r="C28" s="73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D28" s="74"/>
       <c r="E28" s="42">
         <f t="shared" ref="E28:G28" si="6">SUM(E29:E34)</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F28" s="43">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G28" s="44">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H28" s="75">
         <v>3</v>
@@ -14743,7 +14746,7 @@
       <c r="K28" s="77"/>
       <c r="L28" s="49">
         <f t="shared" si="0"/>
-        <v>0.84615384615384615</v>
+        <v>1</v>
       </c>
       <c r="M28" s="50"/>
       <c r="N28" s="51"/>
@@ -14811,7 +14814,7 @@
         <v>3.1</v>
       </c>
       <c r="C29" s="54" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D29" s="55" t="s">
         <v>208</v>
@@ -14908,20 +14911,20 @@
         <v>3.2</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D30" s="55" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E30" s="56">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F30" s="57">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G30" s="58">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H30" s="59">
         <v>3</v>
@@ -14929,14 +14932,16 @@
       <c r="I30" s="162">
         <v>45399</v>
       </c>
-      <c r="J30" s="61"/>
+      <c r="J30" s="61">
+        <v>45405</v>
+      </c>
       <c r="K30" s="62">
         <f t="shared" si="8"/>
-        <v>-45398</v>
+        <v>7</v>
       </c>
       <c r="L30" s="63">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="M30" s="64"/>
       <c r="N30" s="65"/>
@@ -14974,7 +14979,7 @@
       <c r="AT30" s="112"/>
       <c r="AU30" s="65"/>
       <c r="AV30" s="112"/>
-      <c r="AW30" s="70"/>
+      <c r="AW30" s="112"/>
       <c r="AX30" s="70"/>
       <c r="AY30" s="70"/>
       <c r="AZ30" s="70"/>
@@ -15102,10 +15107,10 @@
         <v>62</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D32" s="55" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E32" s="56">
         <v>2</v>
@@ -15199,20 +15204,28 @@
       <c r="B33" s="53">
         <v>3.3</v>
       </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="55"/>
+      <c r="C33" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>208</v>
+      </c>
       <c r="E33" s="56"/>
       <c r="F33" s="57"/>
       <c r="G33" s="58">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H33" s="59"/>
-      <c r="I33" s="60"/>
+      <c r="H33" s="59">
+        <v>3</v>
+      </c>
+      <c r="I33" s="60">
+        <v>45405</v>
+      </c>
       <c r="J33" s="61"/>
       <c r="K33" s="62">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-45404</v>
       </c>
       <c r="L33" s="63" t="e">
         <f t="shared" si="0"/>
@@ -15253,8 +15266,8 @@
       <c r="AS33" s="65"/>
       <c r="AT33" s="65"/>
       <c r="AU33" s="65"/>
-      <c r="AV33" s="70"/>
-      <c r="AW33" s="70"/>
+      <c r="AV33" s="112"/>
+      <c r="AW33" s="112"/>
       <c r="AX33" s="70"/>
       <c r="AY33" s="70"/>
       <c r="AZ33" s="70"/>
@@ -15812,22 +15825,22 @@
       </c>
       <c r="E41" s="101">
         <f>SUM(E11:E16,E18:E21,E29:E34,E36:E39)</f>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F41" s="101">
         <f>SUM(F11:F16,F18:F21,F29:F34,F36:F39)</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G41" s="101">
         <f>SUM(G11:G16,G18:G21,G29:G34,G36:G39)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H41" s="101">
         <v>60</v>
       </c>
       <c r="I41" s="101">
         <f>E41/H41</f>
-        <v>0.68333333333333335</v>
+        <v>0.6</v>
       </c>
       <c r="L41" s="102" t="s">
         <v>77</v>
@@ -16025,243 +16038,243 @@
       </c>
       <c r="M42" s="105">
         <f>E41</f>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N42" s="106">
         <f>M42-I41</f>
-        <v>40.31666666666667</v>
+        <v>35.4</v>
       </c>
       <c r="O42" s="106">
         <f>N42-I41</f>
-        <v>39.63333333333334</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="P42" s="106">
         <f>O42-I41</f>
-        <v>38.95000000000001</v>
+        <v>34.199999999999996</v>
       </c>
       <c r="Q42" s="106">
         <f>P42-I41</f>
-        <v>38.26666666666668</v>
+        <v>33.599999999999994</v>
       </c>
       <c r="R42" s="106">
         <f>Q42-I41</f>
-        <v>37.58333333333335</v>
+        <v>32.999999999999993</v>
       </c>
       <c r="S42" s="106">
         <f>R42-I41</f>
-        <v>36.90000000000002</v>
+        <v>32.399999999999991</v>
       </c>
       <c r="T42" s="106">
         <f>S42-I41</f>
-        <v>36.21666666666669</v>
+        <v>31.79999999999999</v>
       </c>
       <c r="U42" s="106">
         <f>T42-I41</f>
-        <v>35.53333333333336</v>
+        <v>31.199999999999989</v>
       </c>
       <c r="V42" s="106">
         <f>U42-I41</f>
-        <v>34.85000000000003</v>
+        <v>30.599999999999987</v>
       </c>
       <c r="W42" s="106">
         <f>V42-I41</f>
-        <v>34.1666666666667</v>
+        <v>29.999999999999986</v>
       </c>
       <c r="X42" s="106">
         <f>W42-I41</f>
-        <v>33.48333333333337</v>
+        <v>29.399999999999984</v>
       </c>
       <c r="Y42" s="106">
         <f>X42-I41</f>
-        <v>32.80000000000004</v>
+        <v>28.799999999999983</v>
       </c>
       <c r="Z42" s="106">
         <f>Y42-I41</f>
-        <v>32.11666666666671</v>
+        <v>28.199999999999982</v>
       </c>
       <c r="AA42" s="106">
         <f>Z42-I41</f>
-        <v>31.433333333333376</v>
+        <v>27.59999999999998</v>
       </c>
       <c r="AB42" s="106">
         <f>AA42-I41</f>
-        <v>30.750000000000043</v>
+        <v>26.999999999999979</v>
       </c>
       <c r="AC42" s="106">
         <f>AB42-I41</f>
-        <v>30.066666666666709</v>
+        <v>26.399999999999977</v>
       </c>
       <c r="AD42" s="106">
         <f>AC42-I41</f>
-        <v>29.383333333333375</v>
+        <v>25.799999999999976</v>
       </c>
       <c r="AE42" s="106">
         <f>AD42-I41</f>
-        <v>28.700000000000042</v>
+        <v>25.199999999999974</v>
       </c>
       <c r="AF42" s="106">
         <f>AE42-I41</f>
-        <v>28.016666666666708</v>
+        <v>24.599999999999973</v>
       </c>
       <c r="AG42" s="106">
         <f>AF42-I41</f>
-        <v>27.333333333333375</v>
+        <v>23.999999999999972</v>
       </c>
       <c r="AH42" s="106">
         <f>AG42-I41</f>
-        <v>26.650000000000041</v>
+        <v>23.39999999999997</v>
       </c>
       <c r="AI42" s="106">
         <f>AH42-I41</f>
-        <v>25.966666666666708</v>
+        <v>22.799999999999969</v>
       </c>
       <c r="AJ42" s="106">
         <f>AI42-I41</f>
-        <v>25.283333333333374</v>
+        <v>22.199999999999967</v>
       </c>
       <c r="AK42" s="106">
         <f>AJ42-I41</f>
-        <v>24.600000000000041</v>
+        <v>21.599999999999966</v>
       </c>
       <c r="AL42" s="106">
         <f>AK42-I41</f>
-        <v>23.916666666666707</v>
+        <v>20.999999999999964</v>
       </c>
       <c r="AM42" s="106">
         <f>AL42-I41</f>
-        <v>23.233333333333373</v>
+        <v>20.399999999999963</v>
       </c>
       <c r="AN42" s="106">
         <f>AM42-I41</f>
-        <v>22.55000000000004</v>
+        <v>19.799999999999962</v>
       </c>
       <c r="AO42" s="106">
         <f>AN42-I41</f>
-        <v>21.866666666666706</v>
+        <v>19.19999999999996</v>
       </c>
       <c r="AP42" s="106">
         <f>AO42-I41</f>
-        <v>21.183333333333373</v>
+        <v>18.599999999999959</v>
       </c>
       <c r="AQ42" s="106">
         <f>AP42-I41</f>
-        <v>20.500000000000039</v>
+        <v>17.999999999999957</v>
       </c>
       <c r="AR42" s="106">
         <f>AQ42-I41</f>
-        <v>19.816666666666706</v>
+        <v>17.399999999999956</v>
       </c>
       <c r="AS42" s="106">
         <f>AR42-I41</f>
-        <v>19.133333333333372</v>
+        <v>16.799999999999955</v>
       </c>
       <c r="AT42" s="106">
         <f>AS42-I41</f>
-        <v>18.450000000000038</v>
+        <v>16.199999999999953</v>
       </c>
       <c r="AU42" s="106">
         <f>AT42-I41</f>
-        <v>17.766666666666705</v>
+        <v>15.599999999999953</v>
       </c>
       <c r="AV42" s="106">
         <f>AU42-I41</f>
-        <v>17.083333333333371</v>
+        <v>14.999999999999954</v>
       </c>
       <c r="AW42" s="106">
         <f>AV42-I41</f>
-        <v>16.400000000000038</v>
+        <v>14.399999999999954</v>
       </c>
       <c r="AX42" s="106">
         <f>AW42-I41</f>
-        <v>15.716666666666704</v>
+        <v>13.799999999999955</v>
       </c>
       <c r="AY42" s="106">
         <f>AX42-I41</f>
-        <v>15.033333333333371</v>
+        <v>13.199999999999955</v>
       </c>
       <c r="AZ42" s="106">
         <f>AY42-I41</f>
-        <v>14.350000000000037</v>
+        <v>12.599999999999955</v>
       </c>
       <c r="BA42" s="106">
         <f>AZ42-I41</f>
-        <v>13.666666666666703</v>
+        <v>11.999999999999956</v>
       </c>
       <c r="BB42" s="106">
         <f>BA42-I41</f>
-        <v>12.98333333333337</v>
+        <v>11.399999999999956</v>
       </c>
       <c r="BC42" s="106">
         <f>BB42-I41</f>
-        <v>12.300000000000036</v>
+        <v>10.799999999999956</v>
       </c>
       <c r="BD42" s="106">
         <f>BC42-I41</f>
-        <v>11.616666666666703</v>
+        <v>10.199999999999957</v>
       </c>
       <c r="BE42" s="106">
         <f>BD42-I41</f>
-        <v>10.933333333333369</v>
+        <v>9.599999999999957</v>
       </c>
       <c r="BF42" s="106">
         <f>BE42-I41</f>
-        <v>10.250000000000036</v>
+        <v>8.9999999999999574</v>
       </c>
       <c r="BG42" s="106">
         <f>BF42-I41</f>
-        <v>9.566666666666702</v>
+        <v>8.3999999999999577</v>
       </c>
       <c r="BH42" s="106">
         <f>BG42-I41</f>
-        <v>8.8833333333333684</v>
+        <v>7.7999999999999581</v>
       </c>
       <c r="BI42" s="106">
         <f>BH42-I41</f>
-        <v>8.2000000000000348</v>
+        <v>7.1999999999999584</v>
       </c>
       <c r="BJ42" s="106">
         <f>BI42-I41</f>
-        <v>7.5166666666667012</v>
+        <v>6.5999999999999588</v>
       </c>
       <c r="BK42" s="106">
         <f>BJ42-I41</f>
-        <v>6.8333333333333677</v>
+        <v>5.9999999999999591</v>
       </c>
       <c r="BL42" s="106">
         <f>BK42-I41</f>
-        <v>6.1500000000000341</v>
+        <v>5.3999999999999595</v>
       </c>
       <c r="BM42" s="106">
         <f>BL42-I41</f>
-        <v>5.4666666666667005</v>
+        <v>4.7999999999999599</v>
       </c>
       <c r="BN42" s="106">
         <f>BM42-I41</f>
-        <v>4.783333333333367</v>
+        <v>4.1999999999999602</v>
       </c>
       <c r="BO42" s="106">
         <f>BN42-I41</f>
-        <v>4.1000000000000334</v>
+        <v>3.5999999999999601</v>
       </c>
       <c r="BP42" s="106">
         <f>BO42-I41</f>
-        <v>3.4166666666666998</v>
+        <v>2.99999999999996</v>
       </c>
       <c r="BQ42" s="106">
         <f>BP42-I41</f>
-        <v>2.7333333333333663</v>
+        <v>2.3999999999999599</v>
       </c>
       <c r="BR42" s="106">
         <f>BQ42-I41</f>
-        <v>2.0500000000000327</v>
+        <v>1.7999999999999599</v>
       </c>
       <c r="BS42" s="106">
         <f>BR42-I41</f>
-        <v>1.3666666666666993</v>
+        <v>1.1999999999999598</v>
       </c>
       <c r="BT42" s="106">
         <f>BS42-I41</f>
-        <v>0.68333333333336599</v>
+        <v>0.59999999999995979</v>
       </c>
       <c r="BV42" s="101"/>
     </row>
@@ -16271,247 +16284,247 @@
       </c>
       <c r="M43" s="105">
         <f>E41</f>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N43" s="105">
         <f t="shared" ref="N43:BT43" si="12">M45</f>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="O43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Q43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="R43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="S43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="T43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="U43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="V43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="W43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="X43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Y43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Z43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AA43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AB43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AC43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AD43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AE43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AF43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AG43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AH43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AI43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AJ43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AK43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AL43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AM43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AN43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AO43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AP43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AQ43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AR43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AS43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AT43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AU43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AV43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AW43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AX43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AY43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AZ43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BA43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BB43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BC43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BD43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BE43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BF43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BG43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BH43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BI43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BJ43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BK43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BL43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BM43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BN43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BO43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BP43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BQ43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BR43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BS43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BT43" s="105">
         <f t="shared" si="12"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BV43" s="101">
         <f t="shared" ref="BV43:BV45" si="13">SUM(M43:BT43)</f>
-        <v>2460</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16592,247 +16605,247 @@
       </c>
       <c r="M45" s="105">
         <f t="shared" ref="M45:BT45" si="14">M43-M44</f>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="O45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="P45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Q45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="R45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="S45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="T45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="U45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="V45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="W45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="X45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Y45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Z45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AA45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AB45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AC45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AD45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AE45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AF45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AG45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AH45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AI45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AJ45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AK45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AL45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AM45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AN45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AO45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AP45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AQ45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AR45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AS45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AT45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AU45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AV45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AW45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AX45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AY45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AZ45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BA45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BB45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BC45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BD45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BE45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BF45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BG45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BH45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BI45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BJ45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BK45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BL45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BM45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BN45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BO45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BP45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BQ45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BR45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BS45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BT45" s="105">
         <f t="shared" si="14"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BV45" s="101">
         <f t="shared" si="13"/>
-        <v>2460</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="46" spans="2:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16842,55 +16855,55 @@
       <c r="E49" s="200" t="s">
         <v>83</v>
       </c>
-      <c r="F49" s="164"/>
-      <c r="G49" s="164"/>
-      <c r="H49" s="164"/>
-      <c r="I49" s="164"/>
-      <c r="J49" s="164"/>
-      <c r="K49" s="164"/>
-      <c r="L49" s="164"/>
-      <c r="M49" s="164"/>
-      <c r="N49" s="164"/>
-      <c r="O49" s="164"/>
-      <c r="P49" s="164"/>
-      <c r="Q49" s="164"/>
-      <c r="R49" s="164"/>
-      <c r="S49" s="164"/>
-      <c r="T49" s="164"/>
-      <c r="U49" s="164"/>
-      <c r="V49" s="164"/>
-      <c r="W49" s="164"/>
-      <c r="X49" s="164"/>
-      <c r="Y49" s="164"/>
-      <c r="Z49" s="164"/>
-      <c r="AA49" s="164"/>
-      <c r="AB49" s="164"/>
-      <c r="AC49" s="164"/>
-      <c r="AD49" s="164"/>
-      <c r="AE49" s="164"/>
-      <c r="AF49" s="164"/>
-      <c r="AG49" s="164"/>
-      <c r="AH49" s="164"/>
-      <c r="AI49" s="164"/>
-      <c r="AJ49" s="164"/>
-      <c r="AK49" s="164"/>
-      <c r="AL49" s="164"/>
-      <c r="AM49" s="164"/>
-      <c r="AN49" s="164"/>
-      <c r="AO49" s="164"/>
-      <c r="AP49" s="164"/>
-      <c r="AQ49" s="164"/>
-      <c r="AR49" s="164"/>
-      <c r="AS49" s="164"/>
-      <c r="AT49" s="164"/>
-      <c r="AU49" s="164"/>
-      <c r="AV49" s="164"/>
-      <c r="AW49" s="164"/>
-      <c r="AX49" s="164"/>
-      <c r="AY49" s="164"/>
-      <c r="AZ49" s="164"/>
-      <c r="BA49" s="164"/>
-      <c r="BB49" s="165"/>
+      <c r="F49" s="183"/>
+      <c r="G49" s="183"/>
+      <c r="H49" s="183"/>
+      <c r="I49" s="183"/>
+      <c r="J49" s="183"/>
+      <c r="K49" s="183"/>
+      <c r="L49" s="183"/>
+      <c r="M49" s="183"/>
+      <c r="N49" s="183"/>
+      <c r="O49" s="183"/>
+      <c r="P49" s="183"/>
+      <c r="Q49" s="183"/>
+      <c r="R49" s="183"/>
+      <c r="S49" s="183"/>
+      <c r="T49" s="183"/>
+      <c r="U49" s="183"/>
+      <c r="V49" s="183"/>
+      <c r="W49" s="183"/>
+      <c r="X49" s="183"/>
+      <c r="Y49" s="183"/>
+      <c r="Z49" s="183"/>
+      <c r="AA49" s="183"/>
+      <c r="AB49" s="183"/>
+      <c r="AC49" s="183"/>
+      <c r="AD49" s="183"/>
+      <c r="AE49" s="183"/>
+      <c r="AF49" s="183"/>
+      <c r="AG49" s="183"/>
+      <c r="AH49" s="183"/>
+      <c r="AI49" s="183"/>
+      <c r="AJ49" s="183"/>
+      <c r="AK49" s="183"/>
+      <c r="AL49" s="183"/>
+      <c r="AM49" s="183"/>
+      <c r="AN49" s="183"/>
+      <c r="AO49" s="183"/>
+      <c r="AP49" s="183"/>
+      <c r="AQ49" s="183"/>
+      <c r="AR49" s="183"/>
+      <c r="AS49" s="183"/>
+      <c r="AT49" s="183"/>
+      <c r="AU49" s="183"/>
+      <c r="AV49" s="183"/>
+      <c r="AW49" s="183"/>
+      <c r="AX49" s="183"/>
+      <c r="AY49" s="183"/>
+      <c r="AZ49" s="183"/>
+      <c r="BA49" s="183"/>
+      <c r="BB49" s="184"/>
     </row>
     <row r="50" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17853,13 +17866,6 @@
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
     <mergeCell ref="E49:BB49"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
@@ -17876,6 +17882,13 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17948,7 +17961,7 @@
     </row>
     <row r="3" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="115" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C3" s="115" t="s">
         <v>96</v>
@@ -17961,7 +17974,7 @@
       </c>
       <c r="F3" s="117"/>
       <c r="G3" s="118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I3" s="119" t="s">
         <v>89</v>
@@ -17985,7 +17998,7 @@
       </c>
       <c r="F4" s="117"/>
       <c r="G4" s="118" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I4" s="121" t="s">
         <v>90</v>
@@ -17996,7 +18009,7 @@
     </row>
     <row r="5" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="115" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C5" s="115" t="s">
         <v>106</v>
@@ -18009,7 +18022,7 @@
       </c>
       <c r="F5" s="117"/>
       <c r="G5" s="118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I5" s="122" t="s">
         <v>91</v>
@@ -18020,7 +18033,7 @@
     </row>
     <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="115" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6" s="115" t="s">
         <v>154</v>
@@ -18033,7 +18046,7 @@
       </c>
       <c r="F6" s="117"/>
       <c r="G6" s="118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K6" s="120">
         <v>8</v>
@@ -18041,7 +18054,7 @@
     </row>
     <row r="7" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="115" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C7" s="115" t="s">
         <v>158</v>
@@ -18054,7 +18067,7 @@
       </c>
       <c r="F7" s="117"/>
       <c r="G7" s="118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K7" s="120">
         <v>16</v>
@@ -18075,7 +18088,7 @@
       </c>
       <c r="F8" s="117"/>
       <c r="G8" s="118" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K8" s="120">
         <v>24</v>
@@ -18096,7 +18109,7 @@
       </c>
       <c r="F9" s="117"/>
       <c r="G9" s="118" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K9" s="120">
         <v>40</v>
@@ -18117,7 +18130,7 @@
       </c>
       <c r="F10" s="117"/>
       <c r="G10" s="118" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K10" s="124">
         <v>80</v>
@@ -18138,12 +18151,12 @@
       </c>
       <c r="F11" s="150"/>
       <c r="G11" s="153" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="115" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C12" s="148" t="s">
         <v>113</v>
@@ -18156,7 +18169,7 @@
       </c>
       <c r="F12" s="117"/>
       <c r="G12" s="123" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -18174,7 +18187,7 @@
       </c>
       <c r="F13" s="117"/>
       <c r="G13" s="118" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18192,7 +18205,7 @@
       </c>
       <c r="F14" s="117"/>
       <c r="G14" s="118" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18210,12 +18223,12 @@
       </c>
       <c r="F15" s="117"/>
       <c r="G15" s="118" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="115" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C16" s="115" t="s">
         <v>176</v>
@@ -18228,7 +18241,7 @@
       </c>
       <c r="F16" s="117"/>
       <c r="G16" s="118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18246,12 +18259,12 @@
       </c>
       <c r="F17" s="117"/>
       <c r="G17" s="118" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="115" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C18" s="115" t="s">
         <v>125</v>
@@ -18264,12 +18277,12 @@
       </c>
       <c r="F18" s="117"/>
       <c r="G18" s="118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="115" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C19" s="115" t="s">
         <v>135</v>
@@ -18282,7 +18295,7 @@
       </c>
       <c r="F19" s="117"/>
       <c r="G19" s="118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
signup/login logic ended also on operator side + operator table reshape
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\Progetto\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F32D3BD-EFF5-4C4C-AB53-A7A71F74BDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5522C1E9-48E9-4E59-BFFD-826E5EECC68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="243">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -756,13 +756,22 @@
   </si>
   <si>
     <t>Signup/login Logic Part 1</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>Signup/Login Logic Part 3 + operator table reshape</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -921,6 +930,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Corbel"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2077,7 +2093,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2479,11 +2495,53 @@
     <xf numFmtId="14" fontId="24" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2514,50 +2572,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4950,7 +4971,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$44</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5007,7 +5028,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$41:$BT$41</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$42:$BT$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5196,7 +5217,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$44:$BT$44</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$45:$BT$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5243,7 +5264,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$42</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5266,7 +5287,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$41:$BT$41</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$42:$BT$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5455,189 +5476,189 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$42:$BT$42</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$43:$BT$43</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0" formatCode="General">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>35.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>34.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34.199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>33.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>32.399999999999991</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>31.79999999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>31.199999999999989</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>30.599999999999987</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>29.999999999999986</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>29.399999999999984</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>28.799999999999983</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>28.199999999999982</c:v>
+                  <c:v>35.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.59999999999998</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.999999999999979</c:v>
+                  <c:v>33.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>26.399999999999977</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>25.799999999999976</c:v>
+                  <c:v>32.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25.199999999999974</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24.599999999999973</c:v>
+                  <c:v>30.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23.999999999999972</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>23.39999999999997</c:v>
+                  <c:v>29.25</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.799999999999969</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22.199999999999967</c:v>
+                  <c:v>27.75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>21.599999999999966</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20.999999999999964</c:v>
+                  <c:v>26.25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>20.399999999999963</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>19.799999999999962</c:v>
+                  <c:v>24.75</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>19.19999999999996</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>18.599999999999959</c:v>
+                  <c:v>23.25</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>17.999999999999957</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>17.399999999999956</c:v>
+                  <c:v>21.75</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>16.799999999999955</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>16.199999999999953</c:v>
+                  <c:v>20.25</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>15.599999999999953</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>14.999999999999954</c:v>
+                  <c:v>18.75</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>14.399999999999954</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>13.799999999999955</c:v>
+                  <c:v>17.25</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>13.199999999999955</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>12.599999999999955</c:v>
+                  <c:v>15.75</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>11.999999999999956</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>11.399999999999956</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>10.799999999999956</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>10.199999999999957</c:v>
+                  <c:v>12.75</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>9.599999999999957</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>8.9999999999999574</c:v>
+                  <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>8.3999999999999577</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>7.7999999999999581</c:v>
+                  <c:v>9.75</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>7.1999999999999584</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6.5999999999999588</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5.9999999999999591</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>5.3999999999999595</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.7999999999999599</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.1999999999999602</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>3.5999999999999601</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.99999999999996</c:v>
+                  <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.3999999999999599</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.7999999999999599</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.1999999999999598</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.59999999999995979</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5654,7 +5675,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$43</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5677,7 +5698,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$41:$BT$41</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$42:$BT$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5866,189 +5887,189 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$43:$BT$43</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$44:$BT$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>36</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6408,7 +6429,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="27632025" cy="7553325"/>
@@ -6953,19 +6974,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="166" t="str">
+      <c r="BK2" s="184" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="167"/>
-      <c r="BM2" s="167"/>
-      <c r="BN2" s="167"/>
-      <c r="BO2" s="167"/>
-      <c r="BP2" s="167"/>
-      <c r="BQ2" s="167"/>
-      <c r="BR2" s="167"/>
-      <c r="BS2" s="167"/>
-      <c r="BT2" s="167"/>
+      <c r="BL2" s="185"/>
+      <c r="BM2" s="185"/>
+      <c r="BN2" s="185"/>
+      <c r="BO2" s="185"/>
+      <c r="BP2" s="185"/>
+      <c r="BQ2" s="185"/>
+      <c r="BR2" s="185"/>
+      <c r="BS2" s="185"/>
+      <c r="BT2" s="185"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -6993,7 +7014,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="168" t="s">
+      <c r="K4" s="186" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7070,7 +7091,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="169"/>
+      <c r="K5" s="187"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7145,7 +7166,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="169"/>
+      <c r="K6" s="187"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7220,7 +7241,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="169"/>
+      <c r="K7" s="187"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7295,7 +7316,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="170"/>
+      <c r="K8" s="188"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7361,124 +7382,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="171" t="s">
+      <c r="B9" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="173" t="s">
+      <c r="C9" s="191" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="175" t="s">
+      <c r="D9" s="193" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="177" t="s">
+      <c r="E9" s="195" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="178"/>
-      <c r="G9" s="179"/>
-      <c r="H9" s="180" t="s">
+      <c r="F9" s="196"/>
+      <c r="G9" s="197"/>
+      <c r="H9" s="198" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="185" t="s">
+      <c r="I9" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="187" t="s">
+      <c r="J9" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="189" t="s">
+      <c r="K9" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="190" t="s">
+      <c r="L9" s="171" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="192" t="s">
+      <c r="M9" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="164"/>
-      <c r="O9" s="164"/>
-      <c r="P9" s="164"/>
-      <c r="Q9" s="193"/>
-      <c r="R9" s="194" t="s">
+      <c r="N9" s="174"/>
+      <c r="O9" s="174"/>
+      <c r="P9" s="174"/>
+      <c r="Q9" s="175"/>
+      <c r="R9" s="176" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="164"/>
-      <c r="T9" s="164"/>
-      <c r="U9" s="164"/>
-      <c r="V9" s="193"/>
-      <c r="W9" s="194" t="s">
+      <c r="S9" s="174"/>
+      <c r="T9" s="174"/>
+      <c r="U9" s="174"/>
+      <c r="V9" s="175"/>
+      <c r="W9" s="176" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="164"/>
-      <c r="Y9" s="164"/>
-      <c r="Z9" s="164"/>
-      <c r="AA9" s="165"/>
-      <c r="AB9" s="195" t="s">
+      <c r="X9" s="174"/>
+      <c r="Y9" s="174"/>
+      <c r="Z9" s="174"/>
+      <c r="AA9" s="177"/>
+      <c r="AB9" s="178" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="164"/>
-      <c r="AD9" s="164"/>
-      <c r="AE9" s="164"/>
-      <c r="AF9" s="193"/>
-      <c r="AG9" s="196" t="s">
+      <c r="AC9" s="174"/>
+      <c r="AD9" s="174"/>
+      <c r="AE9" s="174"/>
+      <c r="AF9" s="175"/>
+      <c r="AG9" s="179" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="164"/>
-      <c r="AI9" s="164"/>
-      <c r="AJ9" s="164"/>
-      <c r="AK9" s="193"/>
-      <c r="AL9" s="196" t="s">
+      <c r="AH9" s="174"/>
+      <c r="AI9" s="174"/>
+      <c r="AJ9" s="174"/>
+      <c r="AK9" s="175"/>
+      <c r="AL9" s="179" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="164"/>
-      <c r="AN9" s="164"/>
-      <c r="AO9" s="164"/>
-      <c r="AP9" s="165"/>
-      <c r="AQ9" s="197" t="s">
+      <c r="AM9" s="174"/>
+      <c r="AN9" s="174"/>
+      <c r="AO9" s="174"/>
+      <c r="AP9" s="177"/>
+      <c r="AQ9" s="180" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="164"/>
-      <c r="AS9" s="164"/>
-      <c r="AT9" s="164"/>
-      <c r="AU9" s="193"/>
-      <c r="AV9" s="198" t="s">
+      <c r="AR9" s="174"/>
+      <c r="AS9" s="174"/>
+      <c r="AT9" s="174"/>
+      <c r="AU9" s="175"/>
+      <c r="AV9" s="181" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="164"/>
-      <c r="AX9" s="164"/>
-      <c r="AY9" s="164"/>
-      <c r="AZ9" s="193"/>
-      <c r="BA9" s="198" t="s">
+      <c r="AW9" s="174"/>
+      <c r="AX9" s="174"/>
+      <c r="AY9" s="174"/>
+      <c r="AZ9" s="175"/>
+      <c r="BA9" s="181" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="164"/>
-      <c r="BC9" s="164"/>
-      <c r="BD9" s="164"/>
-      <c r="BE9" s="165"/>
-      <c r="BF9" s="199" t="s">
+      <c r="BB9" s="174"/>
+      <c r="BC9" s="174"/>
+      <c r="BD9" s="174"/>
+      <c r="BE9" s="177"/>
+      <c r="BF9" s="182" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="164"/>
-      <c r="BH9" s="164"/>
-      <c r="BI9" s="164"/>
-      <c r="BJ9" s="193"/>
-      <c r="BK9" s="163" t="s">
+      <c r="BG9" s="174"/>
+      <c r="BH9" s="174"/>
+      <c r="BI9" s="174"/>
+      <c r="BJ9" s="175"/>
+      <c r="BK9" s="183" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="164"/>
-      <c r="BM9" s="164"/>
-      <c r="BN9" s="164"/>
-      <c r="BO9" s="193"/>
-      <c r="BP9" s="163" t="s">
+      <c r="BL9" s="174"/>
+      <c r="BM9" s="174"/>
+      <c r="BN9" s="174"/>
+      <c r="BO9" s="175"/>
+      <c r="BP9" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="164"/>
-      <c r="BR9" s="164"/>
-      <c r="BS9" s="164"/>
-      <c r="BT9" s="165"/>
+      <c r="BQ9" s="174"/>
+      <c r="BR9" s="174"/>
+      <c r="BS9" s="174"/>
+      <c r="BT9" s="177"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="172"/>
-      <c r="C10" s="174"/>
-      <c r="D10" s="176"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="192"/>
+      <c r="D10" s="194"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7488,11 +7509,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="181"/>
-      <c r="I10" s="186"/>
-      <c r="J10" s="188"/>
-      <c r="K10" s="188"/>
-      <c r="L10" s="191"/>
+      <c r="H10" s="199"/>
+      <c r="I10" s="167"/>
+      <c r="J10" s="169"/>
+      <c r="K10" s="169"/>
+      <c r="L10" s="172"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11101,80 +11122,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="182" t="str">
+      <c r="B45" s="163" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="183"/>
-      <c r="D45" s="183"/>
-      <c r="E45" s="183"/>
-      <c r="F45" s="183"/>
-      <c r="G45" s="183"/>
-      <c r="H45" s="183"/>
-      <c r="I45" s="183"/>
-      <c r="J45" s="183"/>
-      <c r="K45" s="183"/>
-      <c r="L45" s="183"/>
-      <c r="M45" s="183"/>
-      <c r="N45" s="183"/>
-      <c r="O45" s="183"/>
-      <c r="P45" s="183"/>
-      <c r="Q45" s="183"/>
-      <c r="R45" s="183"/>
-      <c r="S45" s="183"/>
-      <c r="T45" s="183"/>
-      <c r="U45" s="183"/>
-      <c r="V45" s="183"/>
-      <c r="W45" s="183"/>
-      <c r="X45" s="183"/>
-      <c r="Y45" s="183"/>
-      <c r="Z45" s="183"/>
-      <c r="AA45" s="183"/>
-      <c r="AB45" s="183"/>
-      <c r="AC45" s="183"/>
-      <c r="AD45" s="183"/>
-      <c r="AE45" s="183"/>
-      <c r="AF45" s="183"/>
-      <c r="AG45" s="183"/>
-      <c r="AH45" s="183"/>
-      <c r="AI45" s="183"/>
-      <c r="AJ45" s="183"/>
-      <c r="AK45" s="183"/>
-      <c r="AL45" s="183"/>
-      <c r="AM45" s="183"/>
-      <c r="AN45" s="183"/>
-      <c r="AO45" s="183"/>
-      <c r="AP45" s="183"/>
-      <c r="AQ45" s="183"/>
-      <c r="AR45" s="183"/>
-      <c r="AS45" s="183"/>
-      <c r="AT45" s="183"/>
-      <c r="AU45" s="183"/>
-      <c r="AV45" s="183"/>
-      <c r="AW45" s="183"/>
-      <c r="AX45" s="183"/>
-      <c r="AY45" s="183"/>
-      <c r="AZ45" s="183"/>
-      <c r="BA45" s="183"/>
-      <c r="BB45" s="183"/>
-      <c r="BC45" s="183"/>
-      <c r="BD45" s="183"/>
-      <c r="BE45" s="183"/>
-      <c r="BF45" s="183"/>
-      <c r="BG45" s="183"/>
-      <c r="BH45" s="183"/>
-      <c r="BI45" s="183"/>
-      <c r="BJ45" s="183"/>
-      <c r="BK45" s="183"/>
-      <c r="BL45" s="183"/>
-      <c r="BM45" s="183"/>
-      <c r="BN45" s="183"/>
-      <c r="BO45" s="183"/>
-      <c r="BP45" s="183"/>
-      <c r="BQ45" s="183"/>
-      <c r="BR45" s="183"/>
-      <c r="BS45" s="183"/>
-      <c r="BT45" s="184"/>
+      <c r="C45" s="164"/>
+      <c r="D45" s="164"/>
+      <c r="E45" s="164"/>
+      <c r="F45" s="164"/>
+      <c r="G45" s="164"/>
+      <c r="H45" s="164"/>
+      <c r="I45" s="164"/>
+      <c r="J45" s="164"/>
+      <c r="K45" s="164"/>
+      <c r="L45" s="164"/>
+      <c r="M45" s="164"/>
+      <c r="N45" s="164"/>
+      <c r="O45" s="164"/>
+      <c r="P45" s="164"/>
+      <c r="Q45" s="164"/>
+      <c r="R45" s="164"/>
+      <c r="S45" s="164"/>
+      <c r="T45" s="164"/>
+      <c r="U45" s="164"/>
+      <c r="V45" s="164"/>
+      <c r="W45" s="164"/>
+      <c r="X45" s="164"/>
+      <c r="Y45" s="164"/>
+      <c r="Z45" s="164"/>
+      <c r="AA45" s="164"/>
+      <c r="AB45" s="164"/>
+      <c r="AC45" s="164"/>
+      <c r="AD45" s="164"/>
+      <c r="AE45" s="164"/>
+      <c r="AF45" s="164"/>
+      <c r="AG45" s="164"/>
+      <c r="AH45" s="164"/>
+      <c r="AI45" s="164"/>
+      <c r="AJ45" s="164"/>
+      <c r="AK45" s="164"/>
+      <c r="AL45" s="164"/>
+      <c r="AM45" s="164"/>
+      <c r="AN45" s="164"/>
+      <c r="AO45" s="164"/>
+      <c r="AP45" s="164"/>
+      <c r="AQ45" s="164"/>
+      <c r="AR45" s="164"/>
+      <c r="AS45" s="164"/>
+      <c r="AT45" s="164"/>
+      <c r="AU45" s="164"/>
+      <c r="AV45" s="164"/>
+      <c r="AW45" s="164"/>
+      <c r="AX45" s="164"/>
+      <c r="AY45" s="164"/>
+      <c r="AZ45" s="164"/>
+      <c r="BA45" s="164"/>
+      <c r="BB45" s="164"/>
+      <c r="BC45" s="164"/>
+      <c r="BD45" s="164"/>
+      <c r="BE45" s="164"/>
+      <c r="BF45" s="164"/>
+      <c r="BG45" s="164"/>
+      <c r="BH45" s="164"/>
+      <c r="BI45" s="164"/>
+      <c r="BJ45" s="164"/>
+      <c r="BK45" s="164"/>
+      <c r="BL45" s="164"/>
+      <c r="BM45" s="164"/>
+      <c r="BN45" s="164"/>
+      <c r="BO45" s="164"/>
+      <c r="BP45" s="164"/>
+      <c r="BQ45" s="164"/>
+      <c r="BR45" s="164"/>
+      <c r="BS45" s="164"/>
+      <c r="BT45" s="165"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12137,6 +12158,14 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12153,14 +12182,6 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12173,9 +12194,9 @@
     <tabColor rgb="FF7B3C16"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:BV1005"/>
+  <dimension ref="B1:BV1006"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -12289,7 +12310,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="168" t="s">
+      <c r="K3" s="186" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12366,7 +12387,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="169"/>
+      <c r="K4" s="187"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12440,7 +12461,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="169"/>
+      <c r="K5" s="187"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12474,20 +12495,20 @@
       <c r="AO5" s="15"/>
       <c r="AP5" s="15"/>
       <c r="AQ5" s="19"/>
-      <c r="AR5" s="15"/>
-      <c r="AS5" s="15"/>
-      <c r="AT5" s="15"/>
-      <c r="AU5" s="15"/>
-      <c r="AV5" s="15"/>
-      <c r="AW5" s="15"/>
-      <c r="AX5" s="15"/>
-      <c r="AY5" s="15"/>
-      <c r="AZ5" s="15"/>
-      <c r="BA5" s="15"/>
-      <c r="BB5" s="15"/>
-      <c r="BC5" s="15"/>
-      <c r="BD5" s="15"/>
-      <c r="BE5" s="15"/>
+      <c r="AR5" s="19"/>
+      <c r="AS5" s="19"/>
+      <c r="AT5" s="19"/>
+      <c r="AU5" s="19"/>
+      <c r="AV5" s="19"/>
+      <c r="AW5" s="19"/>
+      <c r="AX5" s="19"/>
+      <c r="AY5" s="19"/>
+      <c r="AZ5" s="19"/>
+      <c r="BA5" s="19"/>
+      <c r="BB5" s="19"/>
+      <c r="BC5" s="19"/>
+      <c r="BD5" s="19"/>
+      <c r="BE5" s="202"/>
       <c r="BF5" s="15"/>
       <c r="BG5" s="15"/>
       <c r="BH5" s="15"/>
@@ -12514,7 +12535,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="169"/>
+      <c r="K6" s="187"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12589,7 +12610,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="170"/>
+      <c r="K7" s="188"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12655,124 +12676,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="171" t="s">
+      <c r="B8" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="173" t="s">
+      <c r="C8" s="191" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="175" t="s">
+      <c r="D8" s="193" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="177" t="s">
+      <c r="E8" s="195" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="178"/>
-      <c r="G8" s="179"/>
-      <c r="H8" s="180" t="s">
+      <c r="F8" s="196"/>
+      <c r="G8" s="197"/>
+      <c r="H8" s="198" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="185" t="s">
+      <c r="I8" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="187" t="s">
+      <c r="J8" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="189" t="s">
+      <c r="K8" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="190" t="s">
+      <c r="L8" s="171" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="192" t="s">
+      <c r="M8" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="164"/>
-      <c r="O8" s="164"/>
-      <c r="P8" s="164"/>
-      <c r="Q8" s="193"/>
-      <c r="R8" s="194" t="s">
+      <c r="N8" s="174"/>
+      <c r="O8" s="174"/>
+      <c r="P8" s="174"/>
+      <c r="Q8" s="175"/>
+      <c r="R8" s="176" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="164"/>
-      <c r="T8" s="164"/>
-      <c r="U8" s="164"/>
-      <c r="V8" s="193"/>
-      <c r="W8" s="194" t="s">
+      <c r="S8" s="174"/>
+      <c r="T8" s="174"/>
+      <c r="U8" s="174"/>
+      <c r="V8" s="175"/>
+      <c r="W8" s="176" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="164"/>
-      <c r="Y8" s="164"/>
-      <c r="Z8" s="164"/>
-      <c r="AA8" s="165"/>
-      <c r="AB8" s="195" t="s">
+      <c r="X8" s="174"/>
+      <c r="Y8" s="174"/>
+      <c r="Z8" s="174"/>
+      <c r="AA8" s="177"/>
+      <c r="AB8" s="178" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="164"/>
-      <c r="AD8" s="164"/>
-      <c r="AE8" s="164"/>
-      <c r="AF8" s="193"/>
-      <c r="AG8" s="196" t="s">
+      <c r="AC8" s="174"/>
+      <c r="AD8" s="174"/>
+      <c r="AE8" s="174"/>
+      <c r="AF8" s="175"/>
+      <c r="AG8" s="179" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="164"/>
-      <c r="AI8" s="164"/>
-      <c r="AJ8" s="164"/>
-      <c r="AK8" s="193"/>
-      <c r="AL8" s="196" t="s">
+      <c r="AH8" s="174"/>
+      <c r="AI8" s="174"/>
+      <c r="AJ8" s="174"/>
+      <c r="AK8" s="175"/>
+      <c r="AL8" s="179" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="164"/>
-      <c r="AN8" s="164"/>
-      <c r="AO8" s="164"/>
-      <c r="AP8" s="165"/>
-      <c r="AQ8" s="197" t="s">
+      <c r="AM8" s="174"/>
+      <c r="AN8" s="174"/>
+      <c r="AO8" s="174"/>
+      <c r="AP8" s="177"/>
+      <c r="AQ8" s="180" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="164"/>
-      <c r="AS8" s="164"/>
-      <c r="AT8" s="164"/>
-      <c r="AU8" s="193"/>
-      <c r="AV8" s="198" t="s">
+      <c r="AR8" s="174"/>
+      <c r="AS8" s="174"/>
+      <c r="AT8" s="174"/>
+      <c r="AU8" s="175"/>
+      <c r="AV8" s="181" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="164"/>
-      <c r="AX8" s="164"/>
-      <c r="AY8" s="164"/>
-      <c r="AZ8" s="193"/>
-      <c r="BA8" s="198" t="s">
+      <c r="AW8" s="174"/>
+      <c r="AX8" s="174"/>
+      <c r="AY8" s="174"/>
+      <c r="AZ8" s="175"/>
+      <c r="BA8" s="181" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="164"/>
-      <c r="BC8" s="164"/>
-      <c r="BD8" s="164"/>
-      <c r="BE8" s="165"/>
-      <c r="BF8" s="199" t="s">
+      <c r="BB8" s="174"/>
+      <c r="BC8" s="174"/>
+      <c r="BD8" s="174"/>
+      <c r="BE8" s="177"/>
+      <c r="BF8" s="182" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="164"/>
-      <c r="BH8" s="164"/>
-      <c r="BI8" s="164"/>
-      <c r="BJ8" s="193"/>
-      <c r="BK8" s="163" t="s">
+      <c r="BG8" s="174"/>
+      <c r="BH8" s="174"/>
+      <c r="BI8" s="174"/>
+      <c r="BJ8" s="175"/>
+      <c r="BK8" s="183" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="164"/>
-      <c r="BM8" s="164"/>
-      <c r="BN8" s="164"/>
-      <c r="BO8" s="193"/>
-      <c r="BP8" s="163" t="s">
+      <c r="BL8" s="174"/>
+      <c r="BM8" s="174"/>
+      <c r="BN8" s="174"/>
+      <c r="BO8" s="175"/>
+      <c r="BP8" s="183" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="164"/>
-      <c r="BR8" s="164"/>
-      <c r="BS8" s="164"/>
-      <c r="BT8" s="165"/>
+      <c r="BQ8" s="174"/>
+      <c r="BR8" s="174"/>
+      <c r="BS8" s="174"/>
+      <c r="BT8" s="177"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="172"/>
-      <c r="C9" s="174"/>
-      <c r="D9" s="176"/>
+      <c r="B9" s="190"/>
+      <c r="C9" s="192"/>
+      <c r="D9" s="194"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12782,11 +12803,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="181"/>
-      <c r="I9" s="186"/>
-      <c r="J9" s="188"/>
-      <c r="K9" s="188"/>
-      <c r="L9" s="191"/>
+      <c r="H9" s="199"/>
+      <c r="I9" s="167"/>
+      <c r="J9" s="169"/>
+      <c r="K9" s="169"/>
+      <c r="L9" s="172"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -12995,7 +13016,7 @@
       <c r="J10" s="47"/>
       <c r="K10" s="48"/>
       <c r="L10" s="49">
-        <f t="shared" ref="L10:L39" si="0">F10/E10</f>
+        <f t="shared" ref="L10:L40" si="0">F10/E10</f>
         <v>1</v>
       </c>
       <c r="M10" s="50"/>
@@ -14727,16 +14748,16 @@
       </c>
       <c r="D28" s="74"/>
       <c r="E28" s="42">
-        <f t="shared" ref="E28:G28" si="6">SUM(E29:E34)</f>
-        <v>8</v>
+        <f>SUM(E29:E35)</f>
+        <v>17</v>
       </c>
       <c r="F28" s="43">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f>SUM(F29:F35)</f>
+        <v>12</v>
       </c>
       <c r="G28" s="44">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>SUM(G29:G35)</f>
+        <v>5</v>
       </c>
       <c r="H28" s="75">
         <v>3</v>
@@ -14746,7 +14767,7 @@
       <c r="K28" s="77"/>
       <c r="L28" s="49">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="M28" s="50"/>
       <c r="N28" s="51"/>
@@ -14826,7 +14847,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="58">
-        <f t="shared" ref="G29:G34" si="7">E29-F29</f>
+        <f t="shared" ref="G29:G35" si="6">E29-F29</f>
         <v>0</v>
       </c>
       <c r="H29" s="59">
@@ -14839,7 +14860,7 @@
         <v>45398</v>
       </c>
       <c r="K29" s="62">
-        <f t="shared" ref="K29:K34" si="8">J29-I29+1</f>
+        <f t="shared" ref="K29:K35" si="7">J29-I29+1</f>
         <v>1</v>
       </c>
       <c r="L29" s="63">
@@ -14923,7 +14944,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H30" s="59">
@@ -14933,11 +14954,11 @@
         <v>45399</v>
       </c>
       <c r="J30" s="61">
-        <v>45405</v>
+        <v>45406</v>
       </c>
       <c r="K30" s="62">
-        <f t="shared" si="8"/>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>8</v>
       </c>
       <c r="L30" s="63">
         <f t="shared" si="0"/>
@@ -14980,7 +15001,7 @@
       <c r="AU30" s="65"/>
       <c r="AV30" s="112"/>
       <c r="AW30" s="112"/>
-      <c r="AX30" s="70"/>
+      <c r="AX30" s="112"/>
       <c r="AY30" s="70"/>
       <c r="AZ30" s="70"/>
       <c r="BA30" s="65"/>
@@ -15021,7 +15042,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H31" s="59">
@@ -15034,7 +15055,7 @@
         <v>45401</v>
       </c>
       <c r="K31" s="62">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="L31" s="63">
@@ -15119,7 +15140,7 @@
         <v>2</v>
       </c>
       <c r="G32" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H32" s="59">
@@ -15132,7 +15153,7 @@
         <v>45401</v>
       </c>
       <c r="K32" s="62">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="L32" s="63">
@@ -15201,35 +15222,41 @@
       <c r="BT32" s="68"/>
     </row>
     <row r="33" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="53">
-        <v>3.3</v>
-      </c>
-      <c r="C33" s="54" t="s">
-        <v>237</v>
-      </c>
-      <c r="D33" s="55" t="s">
+      <c r="B33" s="53" t="s">
+        <v>241</v>
+      </c>
+      <c r="C33" s="203" t="s">
+        <v>242</v>
+      </c>
+      <c r="D33" s="157" t="s">
         <v>208</v>
       </c>
-      <c r="E33" s="56"/>
-      <c r="F33" s="57"/>
+      <c r="E33" s="56">
+        <v>4</v>
+      </c>
+      <c r="F33" s="57">
+        <v>4</v>
+      </c>
       <c r="G33" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H33" s="59">
         <v>3</v>
       </c>
-      <c r="I33" s="60">
-        <v>45405</v>
-      </c>
-      <c r="J33" s="61"/>
+      <c r="I33" s="158">
+        <v>45404</v>
+      </c>
+      <c r="J33" s="61">
+        <v>45406</v>
+      </c>
       <c r="K33" s="62">
-        <f t="shared" si="8"/>
-        <v>-45404</v>
-      </c>
-      <c r="L33" s="63" t="e">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="L33" s="63">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M33" s="64"/>
       <c r="N33" s="65"/>
@@ -15265,10 +15292,9 @@
       <c r="AR33" s="65"/>
       <c r="AS33" s="65"/>
       <c r="AT33" s="65"/>
-      <c r="AU33" s="65"/>
-      <c r="AV33" s="112"/>
-      <c r="AW33" s="112"/>
-      <c r="AX33" s="70"/>
+      <c r="AV33" s="201"/>
+      <c r="AW33" s="201"/>
+      <c r="AX33" s="201"/>
       <c r="AY33" s="70"/>
       <c r="AZ33" s="70"/>
       <c r="BA33" s="65"/>
@@ -15294,26 +15320,36 @@
     </row>
     <row r="34" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="54"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="56"/>
+        <v>240</v>
+      </c>
+      <c r="C34" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="D34" s="55" t="s">
+        <v>234</v>
+      </c>
+      <c r="E34" s="56">
+        <v>5</v>
+      </c>
       <c r="F34" s="57"/>
       <c r="G34" s="58">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H34" s="59"/>
-      <c r="I34" s="60"/>
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="H34" s="59">
+        <v>3</v>
+      </c>
+      <c r="I34" s="60">
+        <v>45405</v>
+      </c>
       <c r="J34" s="61"/>
       <c r="K34" s="62">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="L34" s="63" t="e">
+        <f t="shared" si="7"/>
+        <v>-45404</v>
+      </c>
+      <c r="L34" s="63">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M34" s="64"/>
       <c r="N34" s="65"/>
@@ -15351,8 +15387,8 @@
       <c r="AT34" s="65"/>
       <c r="AU34" s="65"/>
       <c r="AV34" s="70"/>
-      <c r="AW34" s="70"/>
-      <c r="AX34" s="70"/>
+      <c r="AW34" s="112"/>
+      <c r="AX34" s="112"/>
       <c r="AY34" s="70"/>
       <c r="AZ34" s="70"/>
       <c r="BA34" s="65"/>
@@ -15377,193 +15413,191 @@
       <c r="BT34" s="68"/>
     </row>
     <row r="35" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="53">
-        <v>4</v>
-      </c>
-      <c r="C35" s="73"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="42">
-        <f t="shared" ref="E35:G35" si="9">SUM(E36:E39)</f>
+      <c r="B35" s="53"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="58">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F35" s="43">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="44">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="H35" s="75"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="77"/>
-      <c r="L35" s="49" t="e">
+      <c r="H35" s="59"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="62">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L35" s="63" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M35" s="50"/>
-      <c r="N35" s="51"/>
-      <c r="O35" s="51"/>
-      <c r="P35" s="51"/>
-      <c r="Q35" s="51"/>
-      <c r="R35" s="51"/>
-      <c r="S35" s="51"/>
-      <c r="T35" s="51"/>
-      <c r="U35" s="51"/>
-      <c r="V35" s="51"/>
-      <c r="W35" s="51"/>
-      <c r="X35" s="51"/>
-      <c r="Y35" s="51"/>
-      <c r="Z35" s="51"/>
-      <c r="AA35" s="52"/>
-      <c r="AB35" s="50"/>
-      <c r="AC35" s="51"/>
-      <c r="AD35" s="51"/>
-      <c r="AE35" s="51"/>
-      <c r="AF35" s="51"/>
-      <c r="AG35" s="51"/>
-      <c r="AH35" s="51"/>
-      <c r="AI35" s="51"/>
-      <c r="AJ35" s="51"/>
-      <c r="AK35" s="51"/>
-      <c r="AL35" s="51"/>
-      <c r="AM35" s="51"/>
-      <c r="AN35" s="51"/>
-      <c r="AO35" s="51"/>
-      <c r="AP35" s="52"/>
-      <c r="AQ35" s="50"/>
-      <c r="AR35" s="51"/>
-      <c r="AS35" s="51"/>
-      <c r="AT35" s="51"/>
-      <c r="AU35" s="51"/>
-      <c r="AV35" s="51"/>
-      <c r="AW35" s="51"/>
-      <c r="AX35" s="51"/>
-      <c r="AY35" s="51"/>
-      <c r="AZ35" s="51"/>
-      <c r="BA35" s="51"/>
-      <c r="BB35" s="51"/>
-      <c r="BC35" s="51"/>
-      <c r="BD35" s="51"/>
-      <c r="BE35" s="52"/>
-      <c r="BF35" s="50"/>
-      <c r="BG35" s="51"/>
-      <c r="BH35" s="51"/>
-      <c r="BI35" s="51"/>
-      <c r="BJ35" s="51"/>
-      <c r="BK35" s="51"/>
-      <c r="BL35" s="51"/>
-      <c r="BM35" s="51"/>
-      <c r="BN35" s="51"/>
-      <c r="BO35" s="51"/>
-      <c r="BP35" s="51"/>
-      <c r="BQ35" s="51"/>
-      <c r="BR35" s="51"/>
-      <c r="BS35" s="51"/>
-      <c r="BT35" s="52"/>
+      <c r="M35" s="64"/>
+      <c r="N35" s="65"/>
+      <c r="O35" s="65"/>
+      <c r="P35" s="65"/>
+      <c r="Q35" s="65"/>
+      <c r="R35" s="67"/>
+      <c r="S35" s="67"/>
+      <c r="T35" s="67"/>
+      <c r="U35" s="67"/>
+      <c r="V35" s="67"/>
+      <c r="W35" s="65"/>
+      <c r="X35" s="65"/>
+      <c r="Y35" s="65"/>
+      <c r="Z35" s="65"/>
+      <c r="AA35" s="68"/>
+      <c r="AB35" s="64"/>
+      <c r="AC35" s="65"/>
+      <c r="AD35" s="65"/>
+      <c r="AE35" s="65"/>
+      <c r="AF35" s="65"/>
+      <c r="AG35" s="69"/>
+      <c r="AH35" s="69"/>
+      <c r="AI35" s="69"/>
+      <c r="AJ35" s="69"/>
+      <c r="AK35" s="69"/>
+      <c r="AL35" s="65"/>
+      <c r="AM35" s="65"/>
+      <c r="AN35" s="65"/>
+      <c r="AO35" s="65"/>
+      <c r="AP35" s="68"/>
+      <c r="AQ35" s="64"/>
+      <c r="AR35" s="65"/>
+      <c r="AS35" s="65"/>
+      <c r="AT35" s="65"/>
+      <c r="AU35" s="65"/>
+      <c r="AV35" s="70"/>
+      <c r="AW35" s="70"/>
+      <c r="AX35" s="70"/>
+      <c r="AY35" s="70"/>
+      <c r="AZ35" s="70"/>
+      <c r="BA35" s="65"/>
+      <c r="BB35" s="65"/>
+      <c r="BC35" s="65"/>
+      <c r="BD35" s="65"/>
+      <c r="BE35" s="68"/>
+      <c r="BF35" s="64"/>
+      <c r="BG35" s="65"/>
+      <c r="BH35" s="65"/>
+      <c r="BI35" s="65"/>
+      <c r="BJ35" s="65"/>
+      <c r="BK35" s="71"/>
+      <c r="BL35" s="71"/>
+      <c r="BM35" s="71"/>
+      <c r="BN35" s="71"/>
+      <c r="BO35" s="71"/>
+      <c r="BP35" s="65"/>
+      <c r="BQ35" s="65"/>
+      <c r="BR35" s="65"/>
+      <c r="BS35" s="65"/>
+      <c r="BT35" s="68"/>
     </row>
     <row r="36" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="53">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="58">
-        <f t="shared" ref="G36:G39" si="10">E36-F36</f>
+        <v>4</v>
+      </c>
+      <c r="C36" s="73"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="42">
+        <f t="shared" ref="E36:G36" si="8">SUM(E37:E40)</f>
         <v>0</v>
       </c>
-      <c r="H36" s="59"/>
-      <c r="I36" s="60"/>
-      <c r="J36" s="61"/>
-      <c r="K36" s="62">
-        <f t="shared" ref="K36:K39" si="11">J36-I36+1</f>
-        <v>1</v>
-      </c>
-      <c r="L36" s="63" t="e">
+      <c r="F36" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="44">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="75"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="77"/>
+      <c r="L36" s="49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M36" s="64"/>
-      <c r="N36" s="65"/>
-      <c r="O36" s="65"/>
-      <c r="P36" s="65"/>
-      <c r="Q36" s="65"/>
-      <c r="R36" s="67"/>
-      <c r="S36" s="67"/>
-      <c r="T36" s="67"/>
-      <c r="U36" s="67"/>
-      <c r="V36" s="67"/>
-      <c r="W36" s="65"/>
-      <c r="X36" s="65"/>
-      <c r="Y36" s="65"/>
-      <c r="Z36" s="65"/>
-      <c r="AA36" s="68"/>
-      <c r="AB36" s="64"/>
-      <c r="AC36" s="65"/>
-      <c r="AD36" s="65"/>
-      <c r="AE36" s="65"/>
-      <c r="AF36" s="65"/>
-      <c r="AG36" s="69"/>
-      <c r="AH36" s="69"/>
-      <c r="AI36" s="69"/>
-      <c r="AJ36" s="69"/>
-      <c r="AK36" s="69"/>
-      <c r="AL36" s="65"/>
-      <c r="AM36" s="65"/>
-      <c r="AN36" s="65"/>
-      <c r="AO36" s="65"/>
-      <c r="AP36" s="68"/>
-      <c r="AQ36" s="64"/>
-      <c r="AR36" s="65"/>
-      <c r="AS36" s="65"/>
-      <c r="AT36" s="65"/>
-      <c r="AU36" s="65"/>
-      <c r="AV36" s="70"/>
-      <c r="AW36" s="70"/>
-      <c r="AX36" s="70"/>
-      <c r="AY36" s="70"/>
-      <c r="AZ36" s="70"/>
-      <c r="BA36" s="65"/>
-      <c r="BB36" s="65"/>
-      <c r="BC36" s="65"/>
-      <c r="BD36" s="65"/>
-      <c r="BE36" s="68"/>
-      <c r="BF36" s="113"/>
-      <c r="BG36" s="65"/>
-      <c r="BH36" s="65"/>
-      <c r="BI36" s="65"/>
-      <c r="BJ36" s="65"/>
-      <c r="BK36" s="71"/>
-      <c r="BL36" s="71"/>
-      <c r="BM36" s="71"/>
-      <c r="BN36" s="71"/>
-      <c r="BO36" s="71"/>
-      <c r="BP36" s="65"/>
-      <c r="BQ36" s="65"/>
-      <c r="BR36" s="65"/>
-      <c r="BS36" s="65"/>
-      <c r="BT36" s="68"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="51"/>
+      <c r="O36" s="51"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="51"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="51"/>
+      <c r="U36" s="51"/>
+      <c r="V36" s="51"/>
+      <c r="W36" s="51"/>
+      <c r="X36" s="51"/>
+      <c r="Y36" s="51"/>
+      <c r="Z36" s="51"/>
+      <c r="AA36" s="52"/>
+      <c r="AB36" s="50"/>
+      <c r="AC36" s="51"/>
+      <c r="AD36" s="51"/>
+      <c r="AE36" s="51"/>
+      <c r="AF36" s="51"/>
+      <c r="AG36" s="51"/>
+      <c r="AH36" s="51"/>
+      <c r="AI36" s="51"/>
+      <c r="AJ36" s="51"/>
+      <c r="AK36" s="51"/>
+      <c r="AL36" s="51"/>
+      <c r="AM36" s="51"/>
+      <c r="AN36" s="51"/>
+      <c r="AO36" s="51"/>
+      <c r="AP36" s="52"/>
+      <c r="AQ36" s="50"/>
+      <c r="AR36" s="51"/>
+      <c r="AS36" s="51"/>
+      <c r="AT36" s="51"/>
+      <c r="AU36" s="51"/>
+      <c r="AV36" s="51"/>
+      <c r="AW36" s="51"/>
+      <c r="AX36" s="51"/>
+      <c r="AY36" s="51"/>
+      <c r="AZ36" s="51"/>
+      <c r="BA36" s="51"/>
+      <c r="BB36" s="51"/>
+      <c r="BC36" s="51"/>
+      <c r="BD36" s="51"/>
+      <c r="BE36" s="52"/>
+      <c r="BF36" s="50"/>
+      <c r="BG36" s="51"/>
+      <c r="BH36" s="51"/>
+      <c r="BI36" s="51"/>
+      <c r="BJ36" s="51"/>
+      <c r="BK36" s="51"/>
+      <c r="BL36" s="51"/>
+      <c r="BM36" s="51"/>
+      <c r="BN36" s="51"/>
+      <c r="BO36" s="51"/>
+      <c r="BP36" s="51"/>
+      <c r="BQ36" s="51"/>
+      <c r="BR36" s="51"/>
+      <c r="BS36" s="51"/>
+      <c r="BT36" s="52"/>
     </row>
     <row r="37" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="53">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C37" s="54"/>
       <c r="D37" s="55"/>
       <c r="E37" s="56"/>
       <c r="F37" s="57"/>
       <c r="G37" s="58">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="G37:G40" si="9">E37-F37</f>
         <v>0</v>
       </c>
       <c r="H37" s="59"/>
       <c r="I37" s="60"/>
       <c r="J37" s="61"/>
       <c r="K37" s="62">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="K37:K40" si="10">J37-I37+1</f>
         <v>1</v>
       </c>
       <c r="L37" s="63" t="e">
@@ -15615,7 +15649,7 @@
       <c r="BC37" s="65"/>
       <c r="BD37" s="65"/>
       <c r="BE37" s="68"/>
-      <c r="BF37" s="64"/>
+      <c r="BF37" s="113"/>
       <c r="BG37" s="65"/>
       <c r="BH37" s="65"/>
       <c r="BI37" s="65"/>
@@ -15633,21 +15667,21 @@
     </row>
     <row r="38" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="53">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="C38" s="54"/>
-      <c r="D38" s="80"/>
+      <c r="D38" s="55"/>
       <c r="E38" s="56"/>
       <c r="F38" s="57"/>
       <c r="G38" s="58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H38" s="59"/>
       <c r="I38" s="60"/>
       <c r="J38" s="61"/>
       <c r="K38" s="62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="L38" s="63" t="e">
@@ -15715,1205 +15749,1288 @@
       <c r="BS38" s="65"/>
       <c r="BT38" s="68"/>
     </row>
-    <row r="39" spans="2:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="82"/>
-      <c r="D39" s="83"/>
-      <c r="E39" s="84"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="86">
+    <row r="39" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="53">
+        <v>4.3</v>
+      </c>
+      <c r="C39" s="54"/>
+      <c r="D39" s="80"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="58">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="59"/>
+      <c r="I39" s="60"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="62">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H39" s="87"/>
-      <c r="I39" s="88"/>
-      <c r="J39" s="89"/>
-      <c r="K39" s="90">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="L39" s="91" t="e">
+      <c r="L39" s="63" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M39" s="92"/>
-      <c r="N39" s="93"/>
-      <c r="O39" s="93"/>
-      <c r="P39" s="93"/>
-      <c r="Q39" s="93"/>
-      <c r="R39" s="94"/>
-      <c r="S39" s="94"/>
-      <c r="T39" s="94"/>
-      <c r="U39" s="94"/>
-      <c r="V39" s="94"/>
-      <c r="W39" s="93"/>
-      <c r="X39" s="93"/>
-      <c r="Y39" s="93"/>
-      <c r="Z39" s="93"/>
-      <c r="AA39" s="95"/>
-      <c r="AB39" s="92"/>
-      <c r="AC39" s="93"/>
-      <c r="AD39" s="93"/>
-      <c r="AE39" s="93"/>
-      <c r="AF39" s="93"/>
-      <c r="AG39" s="96"/>
-      <c r="AH39" s="96"/>
-      <c r="AI39" s="96"/>
-      <c r="AJ39" s="96"/>
-      <c r="AK39" s="96"/>
-      <c r="AL39" s="93"/>
-      <c r="AM39" s="93"/>
-      <c r="AN39" s="93"/>
-      <c r="AO39" s="93"/>
-      <c r="AP39" s="95"/>
-      <c r="AQ39" s="92"/>
-      <c r="AR39" s="93"/>
-      <c r="AS39" s="93"/>
-      <c r="AT39" s="93"/>
-      <c r="AU39" s="93"/>
-      <c r="AV39" s="97"/>
-      <c r="AW39" s="97"/>
-      <c r="AX39" s="97"/>
-      <c r="AY39" s="97"/>
-      <c r="AZ39" s="97"/>
-      <c r="BA39" s="93"/>
-      <c r="BB39" s="93"/>
-      <c r="BC39" s="93"/>
-      <c r="BD39" s="93"/>
-      <c r="BE39" s="95"/>
-      <c r="BF39" s="92"/>
-      <c r="BG39" s="93"/>
-      <c r="BH39" s="93"/>
-      <c r="BI39" s="93"/>
-      <c r="BJ39" s="93"/>
-      <c r="BK39" s="98"/>
-      <c r="BL39" s="98"/>
-      <c r="BM39" s="98"/>
-      <c r="BN39" s="98"/>
-      <c r="BO39" s="98"/>
-      <c r="BP39" s="93"/>
-      <c r="BQ39" s="93"/>
-      <c r="BR39" s="93"/>
-      <c r="BS39" s="93"/>
-      <c r="BT39" s="95"/>
+      <c r="M39" s="64"/>
+      <c r="N39" s="65"/>
+      <c r="O39" s="65"/>
+      <c r="P39" s="65"/>
+      <c r="Q39" s="65"/>
+      <c r="R39" s="67"/>
+      <c r="S39" s="67"/>
+      <c r="T39" s="67"/>
+      <c r="U39" s="67"/>
+      <c r="V39" s="67"/>
+      <c r="W39" s="65"/>
+      <c r="X39" s="65"/>
+      <c r="Y39" s="65"/>
+      <c r="Z39" s="65"/>
+      <c r="AA39" s="68"/>
+      <c r="AB39" s="64"/>
+      <c r="AC39" s="65"/>
+      <c r="AD39" s="65"/>
+      <c r="AE39" s="65"/>
+      <c r="AF39" s="65"/>
+      <c r="AG39" s="69"/>
+      <c r="AH39" s="69"/>
+      <c r="AI39" s="69"/>
+      <c r="AJ39" s="69"/>
+      <c r="AK39" s="69"/>
+      <c r="AL39" s="65"/>
+      <c r="AM39" s="65"/>
+      <c r="AN39" s="65"/>
+      <c r="AO39" s="65"/>
+      <c r="AP39" s="68"/>
+      <c r="AQ39" s="64"/>
+      <c r="AR39" s="65"/>
+      <c r="AS39" s="65"/>
+      <c r="AT39" s="65"/>
+      <c r="AU39" s="65"/>
+      <c r="AV39" s="70"/>
+      <c r="AW39" s="70"/>
+      <c r="AX39" s="70"/>
+      <c r="AY39" s="70"/>
+      <c r="AZ39" s="70"/>
+      <c r="BA39" s="65"/>
+      <c r="BB39" s="65"/>
+      <c r="BC39" s="65"/>
+      <c r="BD39" s="65"/>
+      <c r="BE39" s="68"/>
+      <c r="BF39" s="64"/>
+      <c r="BG39" s="65"/>
+      <c r="BH39" s="65"/>
+      <c r="BI39" s="65"/>
+      <c r="BJ39" s="65"/>
+      <c r="BK39" s="71"/>
+      <c r="BL39" s="71"/>
+      <c r="BM39" s="71"/>
+      <c r="BN39" s="71"/>
+      <c r="BO39" s="71"/>
+      <c r="BP39" s="65"/>
+      <c r="BQ39" s="65"/>
+      <c r="BR39" s="65"/>
+      <c r="BS39" s="65"/>
+      <c r="BT39" s="68"/>
     </row>
-    <row r="40" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E40" s="99" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" s="99" t="s">
-        <v>30</v>
-      </c>
-      <c r="G40" s="99" t="s">
-        <v>31</v>
-      </c>
-      <c r="H40" s="99" t="s">
-        <v>73</v>
-      </c>
-      <c r="I40" s="99" t="s">
-        <v>74</v>
-      </c>
+    <row r="40" spans="2:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="82"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="84"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="86">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="87"/>
+      <c r="I40" s="88"/>
+      <c r="J40" s="89"/>
+      <c r="K40" s="90">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="L40" s="91" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M40" s="92"/>
+      <c r="N40" s="93"/>
+      <c r="O40" s="93"/>
+      <c r="P40" s="93"/>
+      <c r="Q40" s="93"/>
+      <c r="R40" s="94"/>
+      <c r="S40" s="94"/>
+      <c r="T40" s="94"/>
+      <c r="U40" s="94"/>
+      <c r="V40" s="94"/>
+      <c r="W40" s="93"/>
+      <c r="X40" s="93"/>
+      <c r="Y40" s="93"/>
+      <c r="Z40" s="93"/>
+      <c r="AA40" s="95"/>
+      <c r="AB40" s="92"/>
+      <c r="AC40" s="93"/>
+      <c r="AD40" s="93"/>
+      <c r="AE40" s="93"/>
+      <c r="AF40" s="93"/>
+      <c r="AG40" s="96"/>
+      <c r="AH40" s="96"/>
+      <c r="AI40" s="96"/>
+      <c r="AJ40" s="96"/>
+      <c r="AK40" s="96"/>
+      <c r="AL40" s="93"/>
+      <c r="AM40" s="93"/>
+      <c r="AN40" s="93"/>
+      <c r="AO40" s="93"/>
+      <c r="AP40" s="95"/>
+      <c r="AQ40" s="92"/>
+      <c r="AR40" s="93"/>
+      <c r="AS40" s="93"/>
+      <c r="AT40" s="93"/>
+      <c r="AU40" s="93"/>
+      <c r="AV40" s="97"/>
+      <c r="AW40" s="97"/>
+      <c r="AX40" s="97"/>
+      <c r="AY40" s="97"/>
+      <c r="AZ40" s="97"/>
+      <c r="BA40" s="93"/>
+      <c r="BB40" s="93"/>
+      <c r="BC40" s="93"/>
+      <c r="BD40" s="93"/>
+      <c r="BE40" s="95"/>
+      <c r="BF40" s="92"/>
+      <c r="BG40" s="93"/>
+      <c r="BH40" s="93"/>
+      <c r="BI40" s="93"/>
+      <c r="BJ40" s="93"/>
+      <c r="BK40" s="98"/>
+      <c r="BL40" s="98"/>
+      <c r="BM40" s="98"/>
+      <c r="BN40" s="98"/>
+      <c r="BO40" s="98"/>
+      <c r="BP40" s="93"/>
+      <c r="BQ40" s="93"/>
+      <c r="BR40" s="93"/>
+      <c r="BS40" s="93"/>
+      <c r="BT40" s="95"/>
     </row>
     <row r="41" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D41" s="100" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" s="101">
-        <f>SUM(E11:E16,E18:E21,E29:E34,E36:E39)</f>
-        <v>36</v>
-      </c>
-      <c r="F41" s="101">
-        <f>SUM(F11:F16,F18:F21,F29:F34,F36:F39)</f>
-        <v>36</v>
-      </c>
-      <c r="G41" s="101">
-        <f>SUM(G11:G16,G18:G21,G29:G34,G36:G39)</f>
-        <v>0</v>
-      </c>
-      <c r="H41" s="101">
-        <v>60</v>
-      </c>
-      <c r="I41" s="101">
-        <f>E41/H41</f>
-        <v>0.6</v>
-      </c>
-      <c r="L41" s="102" t="s">
-        <v>77</v>
-      </c>
-      <c r="M41" s="103">
-        <v>1</v>
-      </c>
-      <c r="N41" s="103">
-        <v>2</v>
-      </c>
-      <c r="O41" s="103">
-        <v>3</v>
-      </c>
-      <c r="P41" s="103">
-        <v>4</v>
-      </c>
-      <c r="Q41" s="103">
-        <v>5</v>
-      </c>
-      <c r="R41" s="103">
-        <v>6</v>
-      </c>
-      <c r="S41" s="103">
-        <v>7</v>
-      </c>
-      <c r="T41" s="103">
-        <v>8</v>
-      </c>
-      <c r="U41" s="103">
-        <v>9</v>
-      </c>
-      <c r="V41" s="103">
-        <v>10</v>
-      </c>
-      <c r="W41" s="103">
-        <v>11</v>
-      </c>
-      <c r="X41" s="103">
-        <v>12</v>
-      </c>
-      <c r="Y41" s="103">
-        <v>13</v>
-      </c>
-      <c r="Z41" s="103">
-        <v>14</v>
-      </c>
-      <c r="AA41" s="103">
-        <v>15</v>
-      </c>
-      <c r="AB41" s="103">
-        <v>16</v>
-      </c>
-      <c r="AC41" s="103">
-        <v>17</v>
-      </c>
-      <c r="AD41" s="103">
-        <v>18</v>
-      </c>
-      <c r="AE41" s="103">
-        <v>19</v>
-      </c>
-      <c r="AF41" s="103">
-        <v>20</v>
-      </c>
-      <c r="AG41" s="103">
-        <v>21</v>
-      </c>
-      <c r="AH41" s="103">
-        <v>22</v>
-      </c>
-      <c r="AI41" s="103">
-        <v>23</v>
-      </c>
-      <c r="AJ41" s="103">
-        <v>24</v>
-      </c>
-      <c r="AK41" s="103">
-        <v>25</v>
-      </c>
-      <c r="AL41" s="103">
-        <v>26</v>
-      </c>
-      <c r="AM41" s="103">
-        <v>27</v>
-      </c>
-      <c r="AN41" s="103">
-        <v>28</v>
-      </c>
-      <c r="AO41" s="103">
+      <c r="E41" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="AP41" s="103">
+      <c r="F41" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="AQ41" s="103">
+      <c r="G41" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="AR41" s="103">
-        <v>32</v>
-      </c>
-      <c r="AS41" s="103">
-        <v>33</v>
-      </c>
-      <c r="AT41" s="103">
-        <v>34</v>
-      </c>
-      <c r="AU41" s="103">
-        <v>35</v>
-      </c>
-      <c r="AV41" s="103">
-        <v>36</v>
-      </c>
-      <c r="AW41" s="103">
-        <v>37</v>
-      </c>
-      <c r="AX41" s="103">
-        <v>38</v>
-      </c>
-      <c r="AY41" s="103">
-        <v>39</v>
-      </c>
-      <c r="AZ41" s="103">
-        <v>40</v>
-      </c>
-      <c r="BA41" s="103">
-        <v>41</v>
-      </c>
-      <c r="BB41" s="103">
-        <v>42</v>
-      </c>
-      <c r="BC41" s="103">
-        <v>43</v>
-      </c>
-      <c r="BD41" s="103">
-        <v>44</v>
-      </c>
-      <c r="BE41" s="103">
-        <v>45</v>
-      </c>
-      <c r="BF41" s="103">
-        <v>46</v>
-      </c>
-      <c r="BG41" s="103">
-        <v>47</v>
-      </c>
-      <c r="BH41" s="103">
-        <v>48</v>
-      </c>
-      <c r="BI41" s="103">
-        <v>49</v>
-      </c>
-      <c r="BJ41" s="103">
-        <v>50</v>
-      </c>
-      <c r="BK41" s="103">
-        <v>51</v>
-      </c>
-      <c r="BL41" s="103">
-        <v>52</v>
-      </c>
-      <c r="BM41" s="103">
-        <v>53</v>
-      </c>
-      <c r="BN41" s="103">
-        <v>54</v>
-      </c>
-      <c r="BO41" s="103">
-        <v>55</v>
-      </c>
-      <c r="BP41" s="103">
-        <v>56</v>
-      </c>
-      <c r="BQ41" s="103">
-        <v>57</v>
-      </c>
-      <c r="BR41" s="103">
-        <v>58</v>
-      </c>
-      <c r="BS41" s="103">
-        <v>59</v>
-      </c>
-      <c r="BT41" s="103">
-        <v>60</v>
-      </c>
-      <c r="BV41" s="100" t="s">
-        <v>76</v>
+      <c r="H41" s="99" t="s">
+        <v>73</v>
+      </c>
+      <c r="I41" s="99" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H42" s="104" t="s">
-        <v>78</v>
+      <c r="C42" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" s="101">
+        <f>SUM(E11:E16,E18:E21,E29:E35,E37:E40)</f>
+        <v>45</v>
+      </c>
+      <c r="F42" s="101">
+        <f>SUM(F11:F16,F18:F21,F29:F35,F37:F40)</f>
+        <v>40</v>
+      </c>
+      <c r="G42" s="101">
+        <f>SUM(G11:G16,G18:G21,G29:G35,G37:G40)</f>
+        <v>5</v>
+      </c>
+      <c r="H42" s="101">
+        <v>60</v>
+      </c>
+      <c r="I42" s="101">
+        <f>E42/H42</f>
+        <v>0.75</v>
       </c>
       <c r="L42" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="M42" s="105">
-        <f>E41</f>
+        <v>77</v>
+      </c>
+      <c r="M42" s="103">
+        <v>1</v>
+      </c>
+      <c r="N42" s="103">
+        <v>2</v>
+      </c>
+      <c r="O42" s="103">
+        <v>3</v>
+      </c>
+      <c r="P42" s="103">
+        <v>4</v>
+      </c>
+      <c r="Q42" s="103">
+        <v>5</v>
+      </c>
+      <c r="R42" s="103">
+        <v>6</v>
+      </c>
+      <c r="S42" s="103">
+        <v>7</v>
+      </c>
+      <c r="T42" s="103">
+        <v>8</v>
+      </c>
+      <c r="U42" s="103">
+        <v>9</v>
+      </c>
+      <c r="V42" s="103">
+        <v>10</v>
+      </c>
+      <c r="W42" s="103">
+        <v>11</v>
+      </c>
+      <c r="X42" s="103">
+        <v>12</v>
+      </c>
+      <c r="Y42" s="103">
+        <v>13</v>
+      </c>
+      <c r="Z42" s="103">
+        <v>14</v>
+      </c>
+      <c r="AA42" s="103">
+        <v>15</v>
+      </c>
+      <c r="AB42" s="103">
+        <v>16</v>
+      </c>
+      <c r="AC42" s="103">
+        <v>17</v>
+      </c>
+      <c r="AD42" s="103">
+        <v>18</v>
+      </c>
+      <c r="AE42" s="103">
+        <v>19</v>
+      </c>
+      <c r="AF42" s="103">
+        <v>20</v>
+      </c>
+      <c r="AG42" s="103">
+        <v>21</v>
+      </c>
+      <c r="AH42" s="103">
+        <v>22</v>
+      </c>
+      <c r="AI42" s="103">
+        <v>23</v>
+      </c>
+      <c r="AJ42" s="103">
+        <v>24</v>
+      </c>
+      <c r="AK42" s="103">
+        <v>25</v>
+      </c>
+      <c r="AL42" s="103">
+        <v>26</v>
+      </c>
+      <c r="AM42" s="103">
+        <v>27</v>
+      </c>
+      <c r="AN42" s="103">
+        <v>28</v>
+      </c>
+      <c r="AO42" s="103">
+        <v>29</v>
+      </c>
+      <c r="AP42" s="103">
+        <v>30</v>
+      </c>
+      <c r="AQ42" s="103">
+        <v>31</v>
+      </c>
+      <c r="AR42" s="103">
+        <v>32</v>
+      </c>
+      <c r="AS42" s="103">
+        <v>33</v>
+      </c>
+      <c r="AT42" s="103">
+        <v>34</v>
+      </c>
+      <c r="AU42" s="103">
+        <v>35</v>
+      </c>
+      <c r="AV42" s="103">
         <v>36</v>
       </c>
-      <c r="N42" s="106">
-        <f>M42-I41</f>
-        <v>35.4</v>
-      </c>
-      <c r="O42" s="106">
-        <f>N42-I41</f>
-        <v>34.799999999999997</v>
-      </c>
-      <c r="P42" s="106">
-        <f>O42-I41</f>
-        <v>34.199999999999996</v>
-      </c>
-      <c r="Q42" s="106">
-        <f>P42-I41</f>
-        <v>33.599999999999994</v>
-      </c>
-      <c r="R42" s="106">
-        <f>Q42-I41</f>
-        <v>32.999999999999993</v>
-      </c>
-      <c r="S42" s="106">
-        <f>R42-I41</f>
-        <v>32.399999999999991</v>
-      </c>
-      <c r="T42" s="106">
-        <f>S42-I41</f>
-        <v>31.79999999999999</v>
-      </c>
-      <c r="U42" s="106">
-        <f>T42-I41</f>
-        <v>31.199999999999989</v>
-      </c>
-      <c r="V42" s="106">
-        <f>U42-I41</f>
-        <v>30.599999999999987</v>
-      </c>
-      <c r="W42" s="106">
-        <f>V42-I41</f>
-        <v>29.999999999999986</v>
-      </c>
-      <c r="X42" s="106">
-        <f>W42-I41</f>
-        <v>29.399999999999984</v>
-      </c>
-      <c r="Y42" s="106">
-        <f>X42-I41</f>
-        <v>28.799999999999983</v>
-      </c>
-      <c r="Z42" s="106">
-        <f>Y42-I41</f>
-        <v>28.199999999999982</v>
-      </c>
-      <c r="AA42" s="106">
-        <f>Z42-I41</f>
-        <v>27.59999999999998</v>
-      </c>
-      <c r="AB42" s="106">
-        <f>AA42-I41</f>
-        <v>26.999999999999979</v>
-      </c>
-      <c r="AC42" s="106">
-        <f>AB42-I41</f>
-        <v>26.399999999999977</v>
-      </c>
-      <c r="AD42" s="106">
-        <f>AC42-I41</f>
-        <v>25.799999999999976</v>
-      </c>
-      <c r="AE42" s="106">
-        <f>AD42-I41</f>
-        <v>25.199999999999974</v>
-      </c>
-      <c r="AF42" s="106">
-        <f>AE42-I41</f>
-        <v>24.599999999999973</v>
-      </c>
-      <c r="AG42" s="106">
-        <f>AF42-I41</f>
-        <v>23.999999999999972</v>
-      </c>
-      <c r="AH42" s="106">
-        <f>AG42-I41</f>
-        <v>23.39999999999997</v>
-      </c>
-      <c r="AI42" s="106">
-        <f>AH42-I41</f>
-        <v>22.799999999999969</v>
-      </c>
-      <c r="AJ42" s="106">
-        <f>AI42-I41</f>
-        <v>22.199999999999967</v>
-      </c>
-      <c r="AK42" s="106">
-        <f>AJ42-I41</f>
-        <v>21.599999999999966</v>
-      </c>
-      <c r="AL42" s="106">
-        <f>AK42-I41</f>
-        <v>20.999999999999964</v>
-      </c>
-      <c r="AM42" s="106">
-        <f>AL42-I41</f>
-        <v>20.399999999999963</v>
-      </c>
-      <c r="AN42" s="106">
-        <f>AM42-I41</f>
-        <v>19.799999999999962</v>
-      </c>
-      <c r="AO42" s="106">
-        <f>AN42-I41</f>
-        <v>19.19999999999996</v>
-      </c>
-      <c r="AP42" s="106">
-        <f>AO42-I41</f>
-        <v>18.599999999999959</v>
-      </c>
-      <c r="AQ42" s="106">
-        <f>AP42-I41</f>
-        <v>17.999999999999957</v>
-      </c>
-      <c r="AR42" s="106">
-        <f>AQ42-I41</f>
-        <v>17.399999999999956</v>
-      </c>
-      <c r="AS42" s="106">
-        <f>AR42-I41</f>
-        <v>16.799999999999955</v>
-      </c>
-      <c r="AT42" s="106">
-        <f>AS42-I41</f>
-        <v>16.199999999999953</v>
-      </c>
-      <c r="AU42" s="106">
-        <f>AT42-I41</f>
-        <v>15.599999999999953</v>
-      </c>
-      <c r="AV42" s="106">
-        <f>AU42-I41</f>
-        <v>14.999999999999954</v>
-      </c>
-      <c r="AW42" s="106">
-        <f>AV42-I41</f>
-        <v>14.399999999999954</v>
-      </c>
-      <c r="AX42" s="106">
-        <f>AW42-I41</f>
-        <v>13.799999999999955</v>
-      </c>
-      <c r="AY42" s="106">
-        <f>AX42-I41</f>
-        <v>13.199999999999955</v>
-      </c>
-      <c r="AZ42" s="106">
-        <f>AY42-I41</f>
-        <v>12.599999999999955</v>
-      </c>
-      <c r="BA42" s="106">
-        <f>AZ42-I41</f>
-        <v>11.999999999999956</v>
-      </c>
-      <c r="BB42" s="106">
-        <f>BA42-I41</f>
-        <v>11.399999999999956</v>
-      </c>
-      <c r="BC42" s="106">
-        <f>BB42-I41</f>
-        <v>10.799999999999956</v>
-      </c>
-      <c r="BD42" s="106">
-        <f>BC42-I41</f>
-        <v>10.199999999999957</v>
-      </c>
-      <c r="BE42" s="106">
-        <f>BD42-I41</f>
-        <v>9.599999999999957</v>
-      </c>
-      <c r="BF42" s="106">
-        <f>BE42-I41</f>
-        <v>8.9999999999999574</v>
-      </c>
-      <c r="BG42" s="106">
-        <f>BF42-I41</f>
-        <v>8.3999999999999577</v>
-      </c>
-      <c r="BH42" s="106">
-        <f>BG42-I41</f>
-        <v>7.7999999999999581</v>
-      </c>
-      <c r="BI42" s="106">
-        <f>BH42-I41</f>
-        <v>7.1999999999999584</v>
-      </c>
-      <c r="BJ42" s="106">
-        <f>BI42-I41</f>
-        <v>6.5999999999999588</v>
-      </c>
-      <c r="BK42" s="106">
-        <f>BJ42-I41</f>
-        <v>5.9999999999999591</v>
-      </c>
-      <c r="BL42" s="106">
-        <f>BK42-I41</f>
-        <v>5.3999999999999595</v>
-      </c>
-      <c r="BM42" s="106">
-        <f>BL42-I41</f>
-        <v>4.7999999999999599</v>
-      </c>
-      <c r="BN42" s="106">
-        <f>BM42-I41</f>
-        <v>4.1999999999999602</v>
-      </c>
-      <c r="BO42" s="106">
-        <f>BN42-I41</f>
-        <v>3.5999999999999601</v>
-      </c>
-      <c r="BP42" s="106">
-        <f>BO42-I41</f>
-        <v>2.99999999999996</v>
-      </c>
-      <c r="BQ42" s="106">
-        <f>BP42-I41</f>
-        <v>2.3999999999999599</v>
-      </c>
-      <c r="BR42" s="106">
-        <f>BQ42-I41</f>
-        <v>1.7999999999999599</v>
-      </c>
-      <c r="BS42" s="106">
-        <f>BR42-I41</f>
-        <v>1.1999999999999598</v>
-      </c>
-      <c r="BT42" s="106">
-        <f>BS42-I41</f>
-        <v>0.59999999999995979</v>
-      </c>
-      <c r="BV42" s="101"/>
+      <c r="AW42" s="103">
+        <v>37</v>
+      </c>
+      <c r="AX42" s="103">
+        <v>38</v>
+      </c>
+      <c r="AY42" s="103">
+        <v>39</v>
+      </c>
+      <c r="AZ42" s="103">
+        <v>40</v>
+      </c>
+      <c r="BA42" s="103">
+        <v>41</v>
+      </c>
+      <c r="BB42" s="103">
+        <v>42</v>
+      </c>
+      <c r="BC42" s="103">
+        <v>43</v>
+      </c>
+      <c r="BD42" s="103">
+        <v>44</v>
+      </c>
+      <c r="BE42" s="103">
+        <v>45</v>
+      </c>
+      <c r="BF42" s="103">
+        <v>46</v>
+      </c>
+      <c r="BG42" s="103">
+        <v>47</v>
+      </c>
+      <c r="BH42" s="103">
+        <v>48</v>
+      </c>
+      <c r="BI42" s="103">
+        <v>49</v>
+      </c>
+      <c r="BJ42" s="103">
+        <v>50</v>
+      </c>
+      <c r="BK42" s="103">
+        <v>51</v>
+      </c>
+      <c r="BL42" s="103">
+        <v>52</v>
+      </c>
+      <c r="BM42" s="103">
+        <v>53</v>
+      </c>
+      <c r="BN42" s="103">
+        <v>54</v>
+      </c>
+      <c r="BO42" s="103">
+        <v>55</v>
+      </c>
+      <c r="BP42" s="103">
+        <v>56</v>
+      </c>
+      <c r="BQ42" s="103">
+        <v>57</v>
+      </c>
+      <c r="BR42" s="103">
+        <v>58</v>
+      </c>
+      <c r="BS42" s="103">
+        <v>59</v>
+      </c>
+      <c r="BT42" s="103">
+        <v>60</v>
+      </c>
+      <c r="BV42" s="100" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="43" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="L43" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="M43" s="105">
+        <f>E42</f>
+        <v>45</v>
+      </c>
+      <c r="N43" s="106">
+        <f>M43-I42</f>
+        <v>44.25</v>
+      </c>
+      <c r="O43" s="106">
+        <f>N43-I42</f>
+        <v>43.5</v>
+      </c>
+      <c r="P43" s="106">
+        <f>O43-I42</f>
+        <v>42.75</v>
+      </c>
+      <c r="Q43" s="106">
+        <f>P43-I42</f>
+        <v>42</v>
+      </c>
+      <c r="R43" s="106">
+        <f>Q43-I42</f>
+        <v>41.25</v>
+      </c>
+      <c r="S43" s="106">
+        <f>R43-I42</f>
+        <v>40.5</v>
+      </c>
+      <c r="T43" s="106">
+        <f>S43-I42</f>
+        <v>39.75</v>
+      </c>
+      <c r="U43" s="106">
+        <f>T43-I42</f>
+        <v>39</v>
+      </c>
+      <c r="V43" s="106">
+        <f>U43-I42</f>
+        <v>38.25</v>
+      </c>
+      <c r="W43" s="106">
+        <f>V43-I42</f>
+        <v>37.5</v>
+      </c>
+      <c r="X43" s="106">
+        <f>W43-I42</f>
+        <v>36.75</v>
+      </c>
+      <c r="Y43" s="106">
+        <f>X43-I42</f>
+        <v>36</v>
+      </c>
+      <c r="Z43" s="106">
+        <f>Y43-I42</f>
+        <v>35.25</v>
+      </c>
+      <c r="AA43" s="106">
+        <f>Z43-I42</f>
+        <v>34.5</v>
+      </c>
+      <c r="AB43" s="106">
+        <f>AA43-I42</f>
+        <v>33.75</v>
+      </c>
+      <c r="AC43" s="106">
+        <f>AB43-I42</f>
+        <v>33</v>
+      </c>
+      <c r="AD43" s="106">
+        <f>AC43-I42</f>
+        <v>32.25</v>
+      </c>
+      <c r="AE43" s="106">
+        <f>AD43-I42</f>
+        <v>31.5</v>
+      </c>
+      <c r="AF43" s="106">
+        <f>AE43-I42</f>
+        <v>30.75</v>
+      </c>
+      <c r="AG43" s="106">
+        <f>AF43-I42</f>
+        <v>30</v>
+      </c>
+      <c r="AH43" s="106">
+        <f>AG43-I42</f>
+        <v>29.25</v>
+      </c>
+      <c r="AI43" s="106">
+        <f>AH43-I42</f>
+        <v>28.5</v>
+      </c>
+      <c r="AJ43" s="106">
+        <f>AI43-I42</f>
+        <v>27.75</v>
+      </c>
+      <c r="AK43" s="106">
+        <f>AJ43-I42</f>
+        <v>27</v>
+      </c>
+      <c r="AL43" s="106">
+        <f>AK43-I42</f>
+        <v>26.25</v>
+      </c>
+      <c r="AM43" s="106">
+        <f>AL43-I42</f>
+        <v>25.5</v>
+      </c>
+      <c r="AN43" s="106">
+        <f>AM43-I42</f>
+        <v>24.75</v>
+      </c>
+      <c r="AO43" s="106">
+        <f>AN43-I42</f>
+        <v>24</v>
+      </c>
+      <c r="AP43" s="106">
+        <f>AO43-I42</f>
+        <v>23.25</v>
+      </c>
+      <c r="AQ43" s="106">
+        <f>AP43-I42</f>
+        <v>22.5</v>
+      </c>
+      <c r="AR43" s="106">
+        <f>AQ43-I42</f>
+        <v>21.75</v>
+      </c>
+      <c r="AS43" s="106">
+        <f>AR43-I42</f>
+        <v>21</v>
+      </c>
+      <c r="AT43" s="106">
+        <f>AS43-I42</f>
+        <v>20.25</v>
+      </c>
+      <c r="AU43" s="106">
+        <f>AT43-I42</f>
+        <v>19.5</v>
+      </c>
+      <c r="AV43" s="106">
+        <f>AU43-I42</f>
+        <v>18.75</v>
+      </c>
+      <c r="AW43" s="106">
+        <f>AV43-I42</f>
+        <v>18</v>
+      </c>
+      <c r="AX43" s="106">
+        <f>AW43-I42</f>
+        <v>17.25</v>
+      </c>
+      <c r="AY43" s="106">
+        <f>AX43-I42</f>
+        <v>16.5</v>
+      </c>
+      <c r="AZ43" s="106">
+        <f>AY43-I42</f>
+        <v>15.75</v>
+      </c>
+      <c r="BA43" s="106">
+        <f>AZ43-I42</f>
+        <v>15</v>
+      </c>
+      <c r="BB43" s="106">
+        <f>BA43-I42</f>
+        <v>14.25</v>
+      </c>
+      <c r="BC43" s="106">
+        <f>BB43-I42</f>
+        <v>13.5</v>
+      </c>
+      <c r="BD43" s="106">
+        <f>BC43-I42</f>
+        <v>12.75</v>
+      </c>
+      <c r="BE43" s="106">
+        <f>BD43-I42</f>
+        <v>12</v>
+      </c>
+      <c r="BF43" s="106">
+        <f>BE43-I42</f>
+        <v>11.25</v>
+      </c>
+      <c r="BG43" s="106">
+        <f>BF43-I42</f>
+        <v>10.5</v>
+      </c>
+      <c r="BH43" s="106">
+        <f>BG43-I42</f>
+        <v>9.75</v>
+      </c>
+      <c r="BI43" s="106">
+        <f>BH43-I42</f>
+        <v>9</v>
+      </c>
+      <c r="BJ43" s="106">
+        <f>BI43-I42</f>
+        <v>8.25</v>
+      </c>
+      <c r="BK43" s="106">
+        <f>BJ43-I42</f>
+        <v>7.5</v>
+      </c>
+      <c r="BL43" s="106">
+        <f>BK43-I42</f>
+        <v>6.75</v>
+      </c>
+      <c r="BM43" s="106">
+        <f>BL43-I42</f>
+        <v>6</v>
+      </c>
+      <c r="BN43" s="106">
+        <f>BM43-I42</f>
+        <v>5.25</v>
+      </c>
+      <c r="BO43" s="106">
+        <f>BN43-I42</f>
+        <v>4.5</v>
+      </c>
+      <c r="BP43" s="106">
+        <f>BO43-I42</f>
+        <v>3.75</v>
+      </c>
+      <c r="BQ43" s="106">
+        <f>BP43-I42</f>
+        <v>3</v>
+      </c>
+      <c r="BR43" s="106">
+        <f>BQ43-I42</f>
+        <v>2.25</v>
+      </c>
+      <c r="BS43" s="106">
+        <f>BR43-I42</f>
+        <v>1.5</v>
+      </c>
+      <c r="BT43" s="106">
+        <f>BS43-I42</f>
+        <v>0.75</v>
+      </c>
+      <c r="BV43" s="101"/>
+    </row>
+    <row r="44" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L44" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="M43" s="105">
-        <f>E41</f>
-        <v>36</v>
-      </c>
-      <c r="N43" s="105">
-        <f t="shared" ref="N43:BT43" si="12">M45</f>
-        <v>36</v>
-      </c>
-      <c r="O43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="P43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="Q43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="R43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="S43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="T43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="U43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="V43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="W43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="X43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="Y43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="Z43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AA43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AB43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AC43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AD43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AE43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AF43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AG43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AH43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AI43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AJ43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AK43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AL43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AM43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AN43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AO43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AP43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AQ43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AR43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AS43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AT43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AU43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AV43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AW43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AX43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AY43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="AZ43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BA43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BB43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BC43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BD43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BE43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BF43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BG43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BH43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BI43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BJ43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BK43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BL43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BM43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BN43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BO43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BP43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BQ43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BR43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BS43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BT43" s="105">
-        <f t="shared" si="12"/>
-        <v>36</v>
-      </c>
-      <c r="BV43" s="101">
-        <f t="shared" ref="BV43:BV45" si="13">SUM(M43:BT43)</f>
-        <v>2160</v>
-      </c>
-    </row>
-    <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K44" s="107" t="s">
-        <v>80</v>
-      </c>
-      <c r="L44" s="102" t="s">
-        <v>81</v>
-      </c>
-      <c r="M44" s="57"/>
-      <c r="N44" s="57"/>
-      <c r="O44" s="57"/>
-      <c r="P44" s="57"/>
-      <c r="Q44" s="57"/>
-      <c r="R44" s="57"/>
-      <c r="S44" s="57"/>
-      <c r="T44" s="57"/>
-      <c r="U44" s="57"/>
-      <c r="V44" s="57"/>
-      <c r="W44" s="57"/>
-      <c r="X44" s="57"/>
-      <c r="Y44" s="57"/>
-      <c r="Z44" s="57"/>
-      <c r="AA44" s="57"/>
-      <c r="AB44" s="57"/>
-      <c r="AC44" s="57"/>
-      <c r="AD44" s="57"/>
-      <c r="AE44" s="57"/>
-      <c r="AF44" s="57"/>
-      <c r="AG44" s="57"/>
-      <c r="AH44" s="57"/>
-      <c r="AI44" s="57"/>
-      <c r="AJ44" s="57"/>
-      <c r="AK44" s="57"/>
-      <c r="AL44" s="57"/>
-      <c r="AM44" s="57"/>
-      <c r="AN44" s="57"/>
-      <c r="AO44" s="57"/>
-      <c r="AP44" s="57"/>
-      <c r="AQ44" s="57"/>
-      <c r="AR44" s="57"/>
-      <c r="AS44" s="57"/>
-      <c r="AT44" s="57"/>
-      <c r="AU44" s="57"/>
-      <c r="AV44" s="57"/>
-      <c r="AW44" s="57"/>
-      <c r="AX44" s="57"/>
-      <c r="AY44" s="57"/>
-      <c r="AZ44" s="57"/>
-      <c r="BA44" s="57"/>
-      <c r="BB44" s="57"/>
-      <c r="BC44" s="57"/>
-      <c r="BD44" s="57"/>
-      <c r="BE44" s="57"/>
-      <c r="BF44" s="57"/>
-      <c r="BG44" s="57"/>
-      <c r="BH44" s="57"/>
-      <c r="BI44" s="57"/>
-      <c r="BJ44" s="57"/>
-      <c r="BK44" s="57"/>
-      <c r="BL44" s="57"/>
-      <c r="BM44" s="57"/>
-      <c r="BN44" s="57"/>
-      <c r="BO44" s="57"/>
-      <c r="BP44" s="57"/>
-      <c r="BQ44" s="57"/>
-      <c r="BR44" s="57"/>
-      <c r="BS44" s="57"/>
-      <c r="BT44" s="57"/>
+      <c r="M44" s="105">
+        <f>E42</f>
+        <v>45</v>
+      </c>
+      <c r="N44" s="105">
+        <f t="shared" ref="N44:BT44" si="11">M46</f>
+        <v>45</v>
+      </c>
+      <c r="O44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="P44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="Q44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="R44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="S44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="T44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="U44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="V44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="W44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="X44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="Y44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="Z44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AA44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AB44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AC44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AD44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AE44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AF44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AG44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AH44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AI44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AJ44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AK44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AL44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AM44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AN44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AO44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AP44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AQ44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AR44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AS44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AT44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AU44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AV44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AW44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AX44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AY44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="AZ44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BA44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BB44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BC44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BD44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BE44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BF44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BG44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BH44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BI44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BJ44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BK44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BL44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BM44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BN44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BO44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BP44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BQ44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BR44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BS44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="BT44" s="105">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
       <c r="BV44" s="101">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" ref="BV44:BV46" si="12">SUM(M44:BT44)</f>
+        <v>2700</v>
       </c>
     </row>
     <row r="45" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K45" s="107" t="s">
+        <v>80</v>
+      </c>
       <c r="L45" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="M45" s="57"/>
+      <c r="N45" s="57"/>
+      <c r="O45" s="57"/>
+      <c r="P45" s="57"/>
+      <c r="Q45" s="57"/>
+      <c r="R45" s="57"/>
+      <c r="S45" s="57"/>
+      <c r="T45" s="57"/>
+      <c r="U45" s="57"/>
+      <c r="V45" s="57"/>
+      <c r="W45" s="57"/>
+      <c r="X45" s="57"/>
+      <c r="Y45" s="57"/>
+      <c r="Z45" s="57"/>
+      <c r="AA45" s="57"/>
+      <c r="AB45" s="57"/>
+      <c r="AC45" s="57"/>
+      <c r="AD45" s="57"/>
+      <c r="AE45" s="57"/>
+      <c r="AF45" s="57"/>
+      <c r="AG45" s="57"/>
+      <c r="AH45" s="57"/>
+      <c r="AI45" s="57"/>
+      <c r="AJ45" s="57"/>
+      <c r="AK45" s="57"/>
+      <c r="AL45" s="57"/>
+      <c r="AM45" s="57"/>
+      <c r="AN45" s="57"/>
+      <c r="AO45" s="57"/>
+      <c r="AP45" s="57"/>
+      <c r="AQ45" s="57"/>
+      <c r="AR45" s="57"/>
+      <c r="AS45" s="57"/>
+      <c r="AT45" s="57"/>
+      <c r="AU45" s="57"/>
+      <c r="AV45" s="57"/>
+      <c r="AW45" s="57"/>
+      <c r="AX45" s="57"/>
+      <c r="AY45" s="57"/>
+      <c r="AZ45" s="57"/>
+      <c r="BA45" s="57"/>
+      <c r="BB45" s="57"/>
+      <c r="BC45" s="57"/>
+      <c r="BD45" s="57"/>
+      <c r="BE45" s="57"/>
+      <c r="BF45" s="57"/>
+      <c r="BG45" s="57"/>
+      <c r="BH45" s="57"/>
+      <c r="BI45" s="57"/>
+      <c r="BJ45" s="57"/>
+      <c r="BK45" s="57"/>
+      <c r="BL45" s="57"/>
+      <c r="BM45" s="57"/>
+      <c r="BN45" s="57"/>
+      <c r="BO45" s="57"/>
+      <c r="BP45" s="57"/>
+      <c r="BQ45" s="57"/>
+      <c r="BR45" s="57"/>
+      <c r="BS45" s="57"/>
+      <c r="BT45" s="57"/>
+      <c r="BV45" s="101">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L46" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M45" s="105">
-        <f t="shared" ref="M45:BT45" si="14">M43-M44</f>
-        <v>36</v>
-      </c>
-      <c r="N45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="O45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="P45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="Q45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="R45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="S45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="T45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="U45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="V45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="W45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="X45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="Y45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="Z45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AA45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AB45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AC45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AD45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AE45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AF45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AG45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AH45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AI45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AJ45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AK45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AL45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AM45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AN45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AO45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AP45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AQ45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AR45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AS45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AT45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AU45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AV45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AW45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AX45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AY45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="AZ45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BA45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BB45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BC45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BD45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BE45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BF45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BG45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BH45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BI45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BJ45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BK45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BL45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BM45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BN45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BO45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BP45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BQ45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BR45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BS45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BT45" s="105">
-        <f t="shared" si="14"/>
-        <v>36</v>
-      </c>
-      <c r="BV45" s="101">
+      <c r="M46" s="105">
+        <f t="shared" ref="M46:BT46" si="13">M44-M45</f>
+        <v>45</v>
+      </c>
+      <c r="N46" s="105">
         <f t="shared" si="13"/>
-        <v>2160</v>
+        <v>45</v>
+      </c>
+      <c r="O46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="P46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="Q46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="R46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="S46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="T46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="U46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="V46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="W46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="X46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="Y46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="Z46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AA46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AB46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AC46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AD46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AE46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AF46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AG46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AH46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AI46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AJ46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AK46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AL46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AM46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AN46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AO46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AP46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AQ46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AR46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AS46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AT46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AU46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AV46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AW46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AX46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AY46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="AZ46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BA46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BB46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BC46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BD46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BE46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BF46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BG46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BH46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BI46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BJ46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BK46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BL46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BM46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BN46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BO46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BP46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BQ46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BR46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BS46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BT46" s="105">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="BV46" s="101">
+        <f t="shared" si="12"/>
+        <v>2700</v>
       </c>
     </row>
-    <row r="46" spans="2:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="3:54" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E49" s="200" t="s">
+    <row r="47" spans="2:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="3:54" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="200" t="s">
         <v>83</v>
       </c>
-      <c r="F49" s="183"/>
-      <c r="G49" s="183"/>
-      <c r="H49" s="183"/>
-      <c r="I49" s="183"/>
-      <c r="J49" s="183"/>
-      <c r="K49" s="183"/>
-      <c r="L49" s="183"/>
-      <c r="M49" s="183"/>
-      <c r="N49" s="183"/>
-      <c r="O49" s="183"/>
-      <c r="P49" s="183"/>
-      <c r="Q49" s="183"/>
-      <c r="R49" s="183"/>
-      <c r="S49" s="183"/>
-      <c r="T49" s="183"/>
-      <c r="U49" s="183"/>
-      <c r="V49" s="183"/>
-      <c r="W49" s="183"/>
-      <c r="X49" s="183"/>
-      <c r="Y49" s="183"/>
-      <c r="Z49" s="183"/>
-      <c r="AA49" s="183"/>
-      <c r="AB49" s="183"/>
-      <c r="AC49" s="183"/>
-      <c r="AD49" s="183"/>
-      <c r="AE49" s="183"/>
-      <c r="AF49" s="183"/>
-      <c r="AG49" s="183"/>
-      <c r="AH49" s="183"/>
-      <c r="AI49" s="183"/>
-      <c r="AJ49" s="183"/>
-      <c r="AK49" s="183"/>
-      <c r="AL49" s="183"/>
-      <c r="AM49" s="183"/>
-      <c r="AN49" s="183"/>
-      <c r="AO49" s="183"/>
-      <c r="AP49" s="183"/>
-      <c r="AQ49" s="183"/>
-      <c r="AR49" s="183"/>
-      <c r="AS49" s="183"/>
-      <c r="AT49" s="183"/>
-      <c r="AU49" s="183"/>
-      <c r="AV49" s="183"/>
-      <c r="AW49" s="183"/>
-      <c r="AX49" s="183"/>
-      <c r="AY49" s="183"/>
-      <c r="AZ49" s="183"/>
-      <c r="BA49" s="183"/>
-      <c r="BB49" s="184"/>
+      <c r="F50" s="164"/>
+      <c r="G50" s="164"/>
+      <c r="H50" s="164"/>
+      <c r="I50" s="164"/>
+      <c r="J50" s="164"/>
+      <c r="K50" s="164"/>
+      <c r="L50" s="164"/>
+      <c r="M50" s="164"/>
+      <c r="N50" s="164"/>
+      <c r="O50" s="164"/>
+      <c r="P50" s="164"/>
+      <c r="Q50" s="164"/>
+      <c r="R50" s="164"/>
+      <c r="S50" s="164"/>
+      <c r="T50" s="164"/>
+      <c r="U50" s="164"/>
+      <c r="V50" s="164"/>
+      <c r="W50" s="164"/>
+      <c r="X50" s="164"/>
+      <c r="Y50" s="164"/>
+      <c r="Z50" s="164"/>
+      <c r="AA50" s="164"/>
+      <c r="AB50" s="164"/>
+      <c r="AC50" s="164"/>
+      <c r="AD50" s="164"/>
+      <c r="AE50" s="164"/>
+      <c r="AF50" s="164"/>
+      <c r="AG50" s="164"/>
+      <c r="AH50" s="164"/>
+      <c r="AI50" s="164"/>
+      <c r="AJ50" s="164"/>
+      <c r="AK50" s="164"/>
+      <c r="AL50" s="164"/>
+      <c r="AM50" s="164"/>
+      <c r="AN50" s="164"/>
+      <c r="AO50" s="164"/>
+      <c r="AP50" s="164"/>
+      <c r="AQ50" s="164"/>
+      <c r="AR50" s="164"/>
+      <c r="AS50" s="164"/>
+      <c r="AT50" s="164"/>
+      <c r="AU50" s="164"/>
+      <c r="AV50" s="164"/>
+      <c r="AW50" s="164"/>
+      <c r="AX50" s="164"/>
+      <c r="AY50" s="164"/>
+      <c r="AZ50" s="164"/>
+      <c r="BA50" s="164"/>
+      <c r="BB50" s="165"/>
     </row>
-    <row r="50" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="3:54" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="108"/>
-      <c r="D54" s="108"/>
+    <row r="54" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="3:54" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="108"/>
+      <c r="D55" s="108"/>
     </row>
-    <row r="55" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17864,9 +17981,17 @@
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E49:BB49"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="E50:BB50"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
     <mergeCell ref="BP8:BT8"/>
@@ -17882,13 +18007,6 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
continuing personal page logic (managed to pass data from central server to nodejs server)
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\Progetto\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5522C1E9-48E9-4E59-BFFD-826E5EECC68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2F8BE4-242E-4A30-9C0E-61CE7F845882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2495,53 +2495,16 @@
     <xf numFmtId="14" fontId="24" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2572,13 +2535,50 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6974,19 +6974,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="184" t="str">
+      <c r="BK2" s="169" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="185"/>
-      <c r="BM2" s="185"/>
-      <c r="BN2" s="185"/>
-      <c r="BO2" s="185"/>
-      <c r="BP2" s="185"/>
-      <c r="BQ2" s="185"/>
-      <c r="BR2" s="185"/>
-      <c r="BS2" s="185"/>
-      <c r="BT2" s="185"/>
+      <c r="BL2" s="170"/>
+      <c r="BM2" s="170"/>
+      <c r="BN2" s="170"/>
+      <c r="BO2" s="170"/>
+      <c r="BP2" s="170"/>
+      <c r="BQ2" s="170"/>
+      <c r="BR2" s="170"/>
+      <c r="BS2" s="170"/>
+      <c r="BT2" s="170"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -7014,7 +7014,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="186" t="s">
+      <c r="K4" s="171" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7091,7 +7091,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="187"/>
+      <c r="K5" s="172"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7166,7 +7166,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="187"/>
+      <c r="K6" s="172"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7241,7 +7241,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="187"/>
+      <c r="K7" s="172"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7316,7 +7316,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="188"/>
+      <c r="K8" s="173"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7382,124 +7382,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="189" t="s">
+      <c r="B9" s="174" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="191" t="s">
+      <c r="C9" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="193" t="s">
+      <c r="D9" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="195" t="s">
+      <c r="E9" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="196"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="198" t="s">
+      <c r="F9" s="181"/>
+      <c r="G9" s="182"/>
+      <c r="H9" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="166" t="s">
+      <c r="I9" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="168" t="s">
+      <c r="J9" s="190" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="170" t="s">
+      <c r="K9" s="192" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="171" t="s">
+      <c r="L9" s="193" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="173" t="s">
+      <c r="M9" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="174"/>
-      <c r="O9" s="174"/>
-      <c r="P9" s="174"/>
-      <c r="Q9" s="175"/>
-      <c r="R9" s="176" t="s">
+      <c r="N9" s="167"/>
+      <c r="O9" s="167"/>
+      <c r="P9" s="167"/>
+      <c r="Q9" s="196"/>
+      <c r="R9" s="197" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="174"/>
-      <c r="T9" s="174"/>
-      <c r="U9" s="174"/>
-      <c r="V9" s="175"/>
-      <c r="W9" s="176" t="s">
+      <c r="S9" s="167"/>
+      <c r="T9" s="167"/>
+      <c r="U9" s="167"/>
+      <c r="V9" s="196"/>
+      <c r="W9" s="197" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="174"/>
-      <c r="Y9" s="174"/>
-      <c r="Z9" s="174"/>
-      <c r="AA9" s="177"/>
-      <c r="AB9" s="178" t="s">
+      <c r="X9" s="167"/>
+      <c r="Y9" s="167"/>
+      <c r="Z9" s="167"/>
+      <c r="AA9" s="168"/>
+      <c r="AB9" s="198" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="174"/>
-      <c r="AD9" s="174"/>
-      <c r="AE9" s="174"/>
-      <c r="AF9" s="175"/>
-      <c r="AG9" s="179" t="s">
+      <c r="AC9" s="167"/>
+      <c r="AD9" s="167"/>
+      <c r="AE9" s="167"/>
+      <c r="AF9" s="196"/>
+      <c r="AG9" s="199" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="174"/>
-      <c r="AI9" s="174"/>
-      <c r="AJ9" s="174"/>
-      <c r="AK9" s="175"/>
-      <c r="AL9" s="179" t="s">
+      <c r="AH9" s="167"/>
+      <c r="AI9" s="167"/>
+      <c r="AJ9" s="167"/>
+      <c r="AK9" s="196"/>
+      <c r="AL9" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="174"/>
-      <c r="AN9" s="174"/>
-      <c r="AO9" s="174"/>
-      <c r="AP9" s="177"/>
-      <c r="AQ9" s="180" t="s">
+      <c r="AM9" s="167"/>
+      <c r="AN9" s="167"/>
+      <c r="AO9" s="167"/>
+      <c r="AP9" s="168"/>
+      <c r="AQ9" s="200" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="174"/>
-      <c r="AS9" s="174"/>
-      <c r="AT9" s="174"/>
-      <c r="AU9" s="175"/>
-      <c r="AV9" s="181" t="s">
+      <c r="AR9" s="167"/>
+      <c r="AS9" s="167"/>
+      <c r="AT9" s="167"/>
+      <c r="AU9" s="196"/>
+      <c r="AV9" s="201" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="174"/>
-      <c r="AX9" s="174"/>
-      <c r="AY9" s="174"/>
-      <c r="AZ9" s="175"/>
-      <c r="BA9" s="181" t="s">
+      <c r="AW9" s="167"/>
+      <c r="AX9" s="167"/>
+      <c r="AY9" s="167"/>
+      <c r="AZ9" s="196"/>
+      <c r="BA9" s="201" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="174"/>
-      <c r="BC9" s="174"/>
-      <c r="BD9" s="174"/>
-      <c r="BE9" s="177"/>
-      <c r="BF9" s="182" t="s">
+      <c r="BB9" s="167"/>
+      <c r="BC9" s="167"/>
+      <c r="BD9" s="167"/>
+      <c r="BE9" s="168"/>
+      <c r="BF9" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="174"/>
-      <c r="BH9" s="174"/>
-      <c r="BI9" s="174"/>
-      <c r="BJ9" s="175"/>
-      <c r="BK9" s="183" t="s">
+      <c r="BG9" s="167"/>
+      <c r="BH9" s="167"/>
+      <c r="BI9" s="167"/>
+      <c r="BJ9" s="196"/>
+      <c r="BK9" s="166" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="174"/>
-      <c r="BM9" s="174"/>
-      <c r="BN9" s="174"/>
-      <c r="BO9" s="175"/>
-      <c r="BP9" s="183" t="s">
+      <c r="BL9" s="167"/>
+      <c r="BM9" s="167"/>
+      <c r="BN9" s="167"/>
+      <c r="BO9" s="196"/>
+      <c r="BP9" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="174"/>
-      <c r="BR9" s="174"/>
-      <c r="BS9" s="174"/>
-      <c r="BT9" s="177"/>
+      <c r="BQ9" s="167"/>
+      <c r="BR9" s="167"/>
+      <c r="BS9" s="167"/>
+      <c r="BT9" s="168"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="190"/>
-      <c r="C10" s="192"/>
-      <c r="D10" s="194"/>
+      <c r="B10" s="175"/>
+      <c r="C10" s="177"/>
+      <c r="D10" s="179"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7509,11 +7509,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="199"/>
-      <c r="I10" s="167"/>
-      <c r="J10" s="169"/>
-      <c r="K10" s="169"/>
-      <c r="L10" s="172"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="189"/>
+      <c r="J10" s="191"/>
+      <c r="K10" s="191"/>
+      <c r="L10" s="194"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11122,80 +11122,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="163" t="str">
+      <c r="B45" s="185" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="164"/>
-      <c r="D45" s="164"/>
-      <c r="E45" s="164"/>
-      <c r="F45" s="164"/>
-      <c r="G45" s="164"/>
-      <c r="H45" s="164"/>
-      <c r="I45" s="164"/>
-      <c r="J45" s="164"/>
-      <c r="K45" s="164"/>
-      <c r="L45" s="164"/>
-      <c r="M45" s="164"/>
-      <c r="N45" s="164"/>
-      <c r="O45" s="164"/>
-      <c r="P45" s="164"/>
-      <c r="Q45" s="164"/>
-      <c r="R45" s="164"/>
-      <c r="S45" s="164"/>
-      <c r="T45" s="164"/>
-      <c r="U45" s="164"/>
-      <c r="V45" s="164"/>
-      <c r="W45" s="164"/>
-      <c r="X45" s="164"/>
-      <c r="Y45" s="164"/>
-      <c r="Z45" s="164"/>
-      <c r="AA45" s="164"/>
-      <c r="AB45" s="164"/>
-      <c r="AC45" s="164"/>
-      <c r="AD45" s="164"/>
-      <c r="AE45" s="164"/>
-      <c r="AF45" s="164"/>
-      <c r="AG45" s="164"/>
-      <c r="AH45" s="164"/>
-      <c r="AI45" s="164"/>
-      <c r="AJ45" s="164"/>
-      <c r="AK45" s="164"/>
-      <c r="AL45" s="164"/>
-      <c r="AM45" s="164"/>
-      <c r="AN45" s="164"/>
-      <c r="AO45" s="164"/>
-      <c r="AP45" s="164"/>
-      <c r="AQ45" s="164"/>
-      <c r="AR45" s="164"/>
-      <c r="AS45" s="164"/>
-      <c r="AT45" s="164"/>
-      <c r="AU45" s="164"/>
-      <c r="AV45" s="164"/>
-      <c r="AW45" s="164"/>
-      <c r="AX45" s="164"/>
-      <c r="AY45" s="164"/>
-      <c r="AZ45" s="164"/>
-      <c r="BA45" s="164"/>
-      <c r="BB45" s="164"/>
-      <c r="BC45" s="164"/>
-      <c r="BD45" s="164"/>
-      <c r="BE45" s="164"/>
-      <c r="BF45" s="164"/>
-      <c r="BG45" s="164"/>
-      <c r="BH45" s="164"/>
-      <c r="BI45" s="164"/>
-      <c r="BJ45" s="164"/>
-      <c r="BK45" s="164"/>
-      <c r="BL45" s="164"/>
-      <c r="BM45" s="164"/>
-      <c r="BN45" s="164"/>
-      <c r="BO45" s="164"/>
-      <c r="BP45" s="164"/>
-      <c r="BQ45" s="164"/>
-      <c r="BR45" s="164"/>
-      <c r="BS45" s="164"/>
-      <c r="BT45" s="165"/>
+      <c r="C45" s="186"/>
+      <c r="D45" s="186"/>
+      <c r="E45" s="186"/>
+      <c r="F45" s="186"/>
+      <c r="G45" s="186"/>
+      <c r="H45" s="186"/>
+      <c r="I45" s="186"/>
+      <c r="J45" s="186"/>
+      <c r="K45" s="186"/>
+      <c r="L45" s="186"/>
+      <c r="M45" s="186"/>
+      <c r="N45" s="186"/>
+      <c r="O45" s="186"/>
+      <c r="P45" s="186"/>
+      <c r="Q45" s="186"/>
+      <c r="R45" s="186"/>
+      <c r="S45" s="186"/>
+      <c r="T45" s="186"/>
+      <c r="U45" s="186"/>
+      <c r="V45" s="186"/>
+      <c r="W45" s="186"/>
+      <c r="X45" s="186"/>
+      <c r="Y45" s="186"/>
+      <c r="Z45" s="186"/>
+      <c r="AA45" s="186"/>
+      <c r="AB45" s="186"/>
+      <c r="AC45" s="186"/>
+      <c r="AD45" s="186"/>
+      <c r="AE45" s="186"/>
+      <c r="AF45" s="186"/>
+      <c r="AG45" s="186"/>
+      <c r="AH45" s="186"/>
+      <c r="AI45" s="186"/>
+      <c r="AJ45" s="186"/>
+      <c r="AK45" s="186"/>
+      <c r="AL45" s="186"/>
+      <c r="AM45" s="186"/>
+      <c r="AN45" s="186"/>
+      <c r="AO45" s="186"/>
+      <c r="AP45" s="186"/>
+      <c r="AQ45" s="186"/>
+      <c r="AR45" s="186"/>
+      <c r="AS45" s="186"/>
+      <c r="AT45" s="186"/>
+      <c r="AU45" s="186"/>
+      <c r="AV45" s="186"/>
+      <c r="AW45" s="186"/>
+      <c r="AX45" s="186"/>
+      <c r="AY45" s="186"/>
+      <c r="AZ45" s="186"/>
+      <c r="BA45" s="186"/>
+      <c r="BB45" s="186"/>
+      <c r="BC45" s="186"/>
+      <c r="BD45" s="186"/>
+      <c r="BE45" s="186"/>
+      <c r="BF45" s="186"/>
+      <c r="BG45" s="186"/>
+      <c r="BH45" s="186"/>
+      <c r="BI45" s="186"/>
+      <c r="BJ45" s="186"/>
+      <c r="BK45" s="186"/>
+      <c r="BL45" s="186"/>
+      <c r="BM45" s="186"/>
+      <c r="BN45" s="186"/>
+      <c r="BO45" s="186"/>
+      <c r="BP45" s="186"/>
+      <c r="BQ45" s="186"/>
+      <c r="BR45" s="186"/>
+      <c r="BS45" s="186"/>
+      <c r="BT45" s="187"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12158,14 +12158,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12182,6 +12174,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12197,7 +12197,7 @@
   <dimension ref="B1:BV1006"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="AX34" sqref="AX34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12310,7 +12310,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="186" t="s">
+      <c r="K3" s="171" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12387,7 +12387,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="187"/>
+      <c r="K4" s="172"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12461,7 +12461,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="187"/>
+      <c r="K5" s="172"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12508,7 +12508,7 @@
       <c r="BB5" s="19"/>
       <c r="BC5" s="19"/>
       <c r="BD5" s="19"/>
-      <c r="BE5" s="202"/>
+      <c r="BE5" s="164"/>
       <c r="BF5" s="15"/>
       <c r="BG5" s="15"/>
       <c r="BH5" s="15"/>
@@ -12535,7 +12535,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="187"/>
+      <c r="K6" s="172"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12610,7 +12610,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="188"/>
+      <c r="K7" s="173"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12676,124 +12676,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="189" t="s">
+      <c r="B8" s="174" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="191" t="s">
+      <c r="C8" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="193" t="s">
+      <c r="D8" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="195" t="s">
+      <c r="E8" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="196"/>
-      <c r="G8" s="197"/>
-      <c r="H8" s="198" t="s">
+      <c r="F8" s="181"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="166" t="s">
+      <c r="I8" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="168" t="s">
+      <c r="J8" s="190" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="170" t="s">
+      <c r="K8" s="192" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="171" t="s">
+      <c r="L8" s="193" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="173" t="s">
+      <c r="M8" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="174"/>
-      <c r="O8" s="174"/>
-      <c r="P8" s="174"/>
-      <c r="Q8" s="175"/>
-      <c r="R8" s="176" t="s">
+      <c r="N8" s="167"/>
+      <c r="O8" s="167"/>
+      <c r="P8" s="167"/>
+      <c r="Q8" s="196"/>
+      <c r="R8" s="197" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="174"/>
-      <c r="T8" s="174"/>
-      <c r="U8" s="174"/>
-      <c r="V8" s="175"/>
-      <c r="W8" s="176" t="s">
+      <c r="S8" s="167"/>
+      <c r="T8" s="167"/>
+      <c r="U8" s="167"/>
+      <c r="V8" s="196"/>
+      <c r="W8" s="197" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="174"/>
-      <c r="Y8" s="174"/>
-      <c r="Z8" s="174"/>
-      <c r="AA8" s="177"/>
-      <c r="AB8" s="178" t="s">
+      <c r="X8" s="167"/>
+      <c r="Y8" s="167"/>
+      <c r="Z8" s="167"/>
+      <c r="AA8" s="168"/>
+      <c r="AB8" s="198" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="174"/>
-      <c r="AD8" s="174"/>
-      <c r="AE8" s="174"/>
-      <c r="AF8" s="175"/>
-      <c r="AG8" s="179" t="s">
+      <c r="AC8" s="167"/>
+      <c r="AD8" s="167"/>
+      <c r="AE8" s="167"/>
+      <c r="AF8" s="196"/>
+      <c r="AG8" s="199" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="174"/>
-      <c r="AI8" s="174"/>
-      <c r="AJ8" s="174"/>
-      <c r="AK8" s="175"/>
-      <c r="AL8" s="179" t="s">
+      <c r="AH8" s="167"/>
+      <c r="AI8" s="167"/>
+      <c r="AJ8" s="167"/>
+      <c r="AK8" s="196"/>
+      <c r="AL8" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="174"/>
-      <c r="AN8" s="174"/>
-      <c r="AO8" s="174"/>
-      <c r="AP8" s="177"/>
-      <c r="AQ8" s="180" t="s">
+      <c r="AM8" s="167"/>
+      <c r="AN8" s="167"/>
+      <c r="AO8" s="167"/>
+      <c r="AP8" s="168"/>
+      <c r="AQ8" s="200" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="174"/>
-      <c r="AS8" s="174"/>
-      <c r="AT8" s="174"/>
-      <c r="AU8" s="175"/>
-      <c r="AV8" s="181" t="s">
+      <c r="AR8" s="167"/>
+      <c r="AS8" s="167"/>
+      <c r="AT8" s="167"/>
+      <c r="AU8" s="196"/>
+      <c r="AV8" s="201" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="174"/>
-      <c r="AX8" s="174"/>
-      <c r="AY8" s="174"/>
-      <c r="AZ8" s="175"/>
-      <c r="BA8" s="181" t="s">
+      <c r="AW8" s="167"/>
+      <c r="AX8" s="167"/>
+      <c r="AY8" s="167"/>
+      <c r="AZ8" s="196"/>
+      <c r="BA8" s="201" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="174"/>
-      <c r="BC8" s="174"/>
-      <c r="BD8" s="174"/>
-      <c r="BE8" s="177"/>
-      <c r="BF8" s="182" t="s">
+      <c r="BB8" s="167"/>
+      <c r="BC8" s="167"/>
+      <c r="BD8" s="167"/>
+      <c r="BE8" s="168"/>
+      <c r="BF8" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="174"/>
-      <c r="BH8" s="174"/>
-      <c r="BI8" s="174"/>
-      <c r="BJ8" s="175"/>
-      <c r="BK8" s="183" t="s">
+      <c r="BG8" s="167"/>
+      <c r="BH8" s="167"/>
+      <c r="BI8" s="167"/>
+      <c r="BJ8" s="196"/>
+      <c r="BK8" s="166" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="174"/>
-      <c r="BM8" s="174"/>
-      <c r="BN8" s="174"/>
-      <c r="BO8" s="175"/>
-      <c r="BP8" s="183" t="s">
+      <c r="BL8" s="167"/>
+      <c r="BM8" s="167"/>
+      <c r="BN8" s="167"/>
+      <c r="BO8" s="196"/>
+      <c r="BP8" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="174"/>
-      <c r="BR8" s="174"/>
-      <c r="BS8" s="174"/>
-      <c r="BT8" s="177"/>
+      <c r="BQ8" s="167"/>
+      <c r="BR8" s="167"/>
+      <c r="BS8" s="167"/>
+      <c r="BT8" s="168"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="190"/>
-      <c r="C9" s="192"/>
-      <c r="D9" s="194"/>
+      <c r="B9" s="175"/>
+      <c r="C9" s="177"/>
+      <c r="D9" s="179"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12803,11 +12803,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="199"/>
-      <c r="I9" s="167"/>
-      <c r="J9" s="169"/>
-      <c r="K9" s="169"/>
-      <c r="L9" s="172"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="189"/>
+      <c r="J9" s="191"/>
+      <c r="K9" s="191"/>
+      <c r="L9" s="194"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -14753,11 +14753,11 @@
       </c>
       <c r="F28" s="43">
         <f>SUM(F29:F35)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G28" s="44">
         <f>SUM(G29:G35)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H28" s="75">
         <v>3</v>
@@ -14767,7 +14767,7 @@
       <c r="K28" s="77"/>
       <c r="L28" s="49">
         <f t="shared" si="0"/>
-        <v>0.70588235294117652</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="M28" s="50"/>
       <c r="N28" s="51"/>
@@ -15225,7 +15225,7 @@
       <c r="B33" s="53" t="s">
         <v>241</v>
       </c>
-      <c r="C33" s="203" t="s">
+      <c r="C33" s="165" t="s">
         <v>242</v>
       </c>
       <c r="D33" s="157" t="s">
@@ -15292,9 +15292,9 @@
       <c r="AR33" s="65"/>
       <c r="AS33" s="65"/>
       <c r="AT33" s="65"/>
-      <c r="AV33" s="201"/>
-      <c r="AW33" s="201"/>
-      <c r="AX33" s="201"/>
+      <c r="AV33" s="163"/>
+      <c r="AW33" s="163"/>
+      <c r="AX33" s="163"/>
       <c r="AY33" s="70"/>
       <c r="AZ33" s="70"/>
       <c r="BA33" s="65"/>
@@ -15331,10 +15331,12 @@
       <c r="E34" s="56">
         <v>5</v>
       </c>
-      <c r="F34" s="57"/>
+      <c r="F34" s="57">
+        <v>3</v>
+      </c>
       <c r="G34" s="58">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H34" s="59">
         <v>3</v>
@@ -15349,7 +15351,7 @@
       </c>
       <c r="L34" s="63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="M34" s="64"/>
       <c r="N34" s="65"/>
@@ -15947,11 +15949,11 @@
       </c>
       <c r="F42" s="101">
         <f>SUM(F11:F16,F18:F21,F29:F35,F37:F40)</f>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G42" s="101">
         <f>SUM(G11:G16,G18:G21,G29:G35,G37:G40)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H42" s="101">
         <v>60</v>
@@ -16970,58 +16972,58 @@
     <row r="48" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="3:54" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E50" s="200" t="s">
+      <c r="E50" s="203" t="s">
         <v>83</v>
       </c>
-      <c r="F50" s="164"/>
-      <c r="G50" s="164"/>
-      <c r="H50" s="164"/>
-      <c r="I50" s="164"/>
-      <c r="J50" s="164"/>
-      <c r="K50" s="164"/>
-      <c r="L50" s="164"/>
-      <c r="M50" s="164"/>
-      <c r="N50" s="164"/>
-      <c r="O50" s="164"/>
-      <c r="P50" s="164"/>
-      <c r="Q50" s="164"/>
-      <c r="R50" s="164"/>
-      <c r="S50" s="164"/>
-      <c r="T50" s="164"/>
-      <c r="U50" s="164"/>
-      <c r="V50" s="164"/>
-      <c r="W50" s="164"/>
-      <c r="X50" s="164"/>
-      <c r="Y50" s="164"/>
-      <c r="Z50" s="164"/>
-      <c r="AA50" s="164"/>
-      <c r="AB50" s="164"/>
-      <c r="AC50" s="164"/>
-      <c r="AD50" s="164"/>
-      <c r="AE50" s="164"/>
-      <c r="AF50" s="164"/>
-      <c r="AG50" s="164"/>
-      <c r="AH50" s="164"/>
-      <c r="AI50" s="164"/>
-      <c r="AJ50" s="164"/>
-      <c r="AK50" s="164"/>
-      <c r="AL50" s="164"/>
-      <c r="AM50" s="164"/>
-      <c r="AN50" s="164"/>
-      <c r="AO50" s="164"/>
-      <c r="AP50" s="164"/>
-      <c r="AQ50" s="164"/>
-      <c r="AR50" s="164"/>
-      <c r="AS50" s="164"/>
-      <c r="AT50" s="164"/>
-      <c r="AU50" s="164"/>
-      <c r="AV50" s="164"/>
-      <c r="AW50" s="164"/>
-      <c r="AX50" s="164"/>
-      <c r="AY50" s="164"/>
-      <c r="AZ50" s="164"/>
-      <c r="BA50" s="164"/>
-      <c r="BB50" s="165"/>
+      <c r="F50" s="186"/>
+      <c r="G50" s="186"/>
+      <c r="H50" s="186"/>
+      <c r="I50" s="186"/>
+      <c r="J50" s="186"/>
+      <c r="K50" s="186"/>
+      <c r="L50" s="186"/>
+      <c r="M50" s="186"/>
+      <c r="N50" s="186"/>
+      <c r="O50" s="186"/>
+      <c r="P50" s="186"/>
+      <c r="Q50" s="186"/>
+      <c r="R50" s="186"/>
+      <c r="S50" s="186"/>
+      <c r="T50" s="186"/>
+      <c r="U50" s="186"/>
+      <c r="V50" s="186"/>
+      <c r="W50" s="186"/>
+      <c r="X50" s="186"/>
+      <c r="Y50" s="186"/>
+      <c r="Z50" s="186"/>
+      <c r="AA50" s="186"/>
+      <c r="AB50" s="186"/>
+      <c r="AC50" s="186"/>
+      <c r="AD50" s="186"/>
+      <c r="AE50" s="186"/>
+      <c r="AF50" s="186"/>
+      <c r="AG50" s="186"/>
+      <c r="AH50" s="186"/>
+      <c r="AI50" s="186"/>
+      <c r="AJ50" s="186"/>
+      <c r="AK50" s="186"/>
+      <c r="AL50" s="186"/>
+      <c r="AM50" s="186"/>
+      <c r="AN50" s="186"/>
+      <c r="AO50" s="186"/>
+      <c r="AP50" s="186"/>
+      <c r="AQ50" s="186"/>
+      <c r="AR50" s="186"/>
+      <c r="AS50" s="186"/>
+      <c r="AT50" s="186"/>
+      <c r="AU50" s="186"/>
+      <c r="AV50" s="186"/>
+      <c r="AW50" s="186"/>
+      <c r="AX50" s="186"/>
+      <c r="AY50" s="186"/>
+      <c r="AZ50" s="186"/>
+      <c r="BA50" s="186"/>
+      <c r="BB50" s="187"/>
     </row>
     <row r="51" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17984,13 +17986,6 @@
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
     <mergeCell ref="E50:BB50"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
@@ -18007,6 +18002,13 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
integration for certification service, frontend, recognition service
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valer\Desktop\Università\magistrale\Lab-Mec\AnimalDex\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e15298e05a6af3ae/Università/Magistrale/LabAdvProg/Proj/AnimalDex/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B35C558-D3F0-4404-AF1C-3CFF9CF59032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{9B35C558-D3F0-4404-AF1C-3CFF9CF59032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FC14953-2EF4-4A62-BFBC-257CCA5F2E9A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5760" yWindow="696" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLE Gantt Chart &amp; Burndown" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="257">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -798,6 +798,15 @@
   </si>
   <si>
     <t>Animaldex Search Bar and Personaldex filter</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>3.11</t>
+  </si>
+  <si>
+    <t>Cookie management and integration</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="78">
+  <borders count="79">
     <border>
       <left/>
       <right/>
@@ -2122,11 +2131,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2533,53 +2553,11 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2610,9 +2588,53 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -5004,7 +5026,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$49</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5061,7 +5083,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$46:$BT$46</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$48:$BT$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5250,7 +5272,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$49:$BT$49</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$51:$BT$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5297,7 +5319,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$47</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5320,7 +5342,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$46:$BT$46</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$48:$BT$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5509,7 +5531,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$47:$BT$47</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$49:$BT$49</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5708,7 +5730,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$48</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$L$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5731,7 +5753,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$46:$BT$46</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$48:$BT$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5920,7 +5942,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$48:$BT$48</c:f>
+              <c:f>'BLANK Gantt Chart &amp; Burndown'!$M$50:$BT$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6462,7 +6484,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="27632025" cy="7553325"/>
@@ -7007,19 +7029,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="187" t="str">
+      <c r="BK2" s="169" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="188"/>
-      <c r="BM2" s="188"/>
-      <c r="BN2" s="188"/>
-      <c r="BO2" s="188"/>
-      <c r="BP2" s="188"/>
-      <c r="BQ2" s="188"/>
-      <c r="BR2" s="188"/>
-      <c r="BS2" s="188"/>
-      <c r="BT2" s="188"/>
+      <c r="BL2" s="170"/>
+      <c r="BM2" s="170"/>
+      <c r="BN2" s="170"/>
+      <c r="BO2" s="170"/>
+      <c r="BP2" s="170"/>
+      <c r="BQ2" s="170"/>
+      <c r="BR2" s="170"/>
+      <c r="BS2" s="170"/>
+      <c r="BT2" s="170"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -7047,7 +7069,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="189" t="s">
+      <c r="K4" s="171" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7124,7 +7146,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="190"/>
+      <c r="K5" s="172"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7199,7 +7221,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="190"/>
+      <c r="K6" s="172"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7274,7 +7296,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="190"/>
+      <c r="K7" s="172"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7349,7 +7371,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="191"/>
+      <c r="K8" s="173"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7415,124 +7437,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="192" t="s">
+      <c r="B9" s="174" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="194" t="s">
+      <c r="C9" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="196" t="s">
+      <c r="D9" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="198" t="s">
+      <c r="E9" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="199"/>
-      <c r="G9" s="200"/>
-      <c r="H9" s="201" t="s">
+      <c r="F9" s="181"/>
+      <c r="G9" s="182"/>
+      <c r="H9" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="169" t="s">
+      <c r="I9" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="171" t="s">
+      <c r="J9" s="190" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="173" t="s">
+      <c r="K9" s="192" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="174" t="s">
+      <c r="L9" s="193" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="176" t="s">
+      <c r="M9" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="177"/>
-      <c r="O9" s="177"/>
-      <c r="P9" s="177"/>
-      <c r="Q9" s="178"/>
-      <c r="R9" s="179" t="s">
+      <c r="N9" s="167"/>
+      <c r="O9" s="167"/>
+      <c r="P9" s="167"/>
+      <c r="Q9" s="196"/>
+      <c r="R9" s="197" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="177"/>
-      <c r="T9" s="177"/>
-      <c r="U9" s="177"/>
-      <c r="V9" s="178"/>
-      <c r="W9" s="179" t="s">
+      <c r="S9" s="167"/>
+      <c r="T9" s="167"/>
+      <c r="U9" s="167"/>
+      <c r="V9" s="196"/>
+      <c r="W9" s="197" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="177"/>
-      <c r="Y9" s="177"/>
-      <c r="Z9" s="177"/>
-      <c r="AA9" s="180"/>
-      <c r="AB9" s="181" t="s">
+      <c r="X9" s="167"/>
+      <c r="Y9" s="167"/>
+      <c r="Z9" s="167"/>
+      <c r="AA9" s="168"/>
+      <c r="AB9" s="198" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="177"/>
-      <c r="AD9" s="177"/>
-      <c r="AE9" s="177"/>
-      <c r="AF9" s="178"/>
-      <c r="AG9" s="182" t="s">
+      <c r="AC9" s="167"/>
+      <c r="AD9" s="167"/>
+      <c r="AE9" s="167"/>
+      <c r="AF9" s="196"/>
+      <c r="AG9" s="199" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="177"/>
-      <c r="AI9" s="177"/>
-      <c r="AJ9" s="177"/>
-      <c r="AK9" s="178"/>
-      <c r="AL9" s="182" t="s">
+      <c r="AH9" s="167"/>
+      <c r="AI9" s="167"/>
+      <c r="AJ9" s="167"/>
+      <c r="AK9" s="196"/>
+      <c r="AL9" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="177"/>
-      <c r="AN9" s="177"/>
-      <c r="AO9" s="177"/>
-      <c r="AP9" s="180"/>
-      <c r="AQ9" s="183" t="s">
+      <c r="AM9" s="167"/>
+      <c r="AN9" s="167"/>
+      <c r="AO9" s="167"/>
+      <c r="AP9" s="168"/>
+      <c r="AQ9" s="200" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="177"/>
-      <c r="AS9" s="177"/>
-      <c r="AT9" s="177"/>
-      <c r="AU9" s="178"/>
-      <c r="AV9" s="184" t="s">
+      <c r="AR9" s="167"/>
+      <c r="AS9" s="167"/>
+      <c r="AT9" s="167"/>
+      <c r="AU9" s="196"/>
+      <c r="AV9" s="201" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="177"/>
-      <c r="AX9" s="177"/>
-      <c r="AY9" s="177"/>
-      <c r="AZ9" s="178"/>
-      <c r="BA9" s="184" t="s">
+      <c r="AW9" s="167"/>
+      <c r="AX9" s="167"/>
+      <c r="AY9" s="167"/>
+      <c r="AZ9" s="196"/>
+      <c r="BA9" s="201" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="177"/>
-      <c r="BC9" s="177"/>
-      <c r="BD9" s="177"/>
-      <c r="BE9" s="180"/>
-      <c r="BF9" s="185" t="s">
+      <c r="BB9" s="167"/>
+      <c r="BC9" s="167"/>
+      <c r="BD9" s="167"/>
+      <c r="BE9" s="168"/>
+      <c r="BF9" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="177"/>
-      <c r="BH9" s="177"/>
-      <c r="BI9" s="177"/>
-      <c r="BJ9" s="178"/>
-      <c r="BK9" s="186" t="s">
+      <c r="BG9" s="167"/>
+      <c r="BH9" s="167"/>
+      <c r="BI9" s="167"/>
+      <c r="BJ9" s="196"/>
+      <c r="BK9" s="166" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="177"/>
-      <c r="BM9" s="177"/>
-      <c r="BN9" s="177"/>
-      <c r="BO9" s="178"/>
-      <c r="BP9" s="186" t="s">
+      <c r="BL9" s="167"/>
+      <c r="BM9" s="167"/>
+      <c r="BN9" s="167"/>
+      <c r="BO9" s="196"/>
+      <c r="BP9" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="177"/>
-      <c r="BR9" s="177"/>
-      <c r="BS9" s="177"/>
-      <c r="BT9" s="180"/>
+      <c r="BQ9" s="167"/>
+      <c r="BR9" s="167"/>
+      <c r="BS9" s="167"/>
+      <c r="BT9" s="168"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="193"/>
-      <c r="C10" s="195"/>
-      <c r="D10" s="197"/>
+      <c r="B10" s="175"/>
+      <c r="C10" s="177"/>
+      <c r="D10" s="179"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7542,11 +7564,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="202"/>
-      <c r="I10" s="170"/>
-      <c r="J10" s="172"/>
-      <c r="K10" s="172"/>
-      <c r="L10" s="175"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="189"/>
+      <c r="J10" s="191"/>
+      <c r="K10" s="191"/>
+      <c r="L10" s="194"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11155,80 +11177,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="166" t="str">
+      <c r="B45" s="185" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="167"/>
-      <c r="D45" s="167"/>
-      <c r="E45" s="167"/>
-      <c r="F45" s="167"/>
-      <c r="G45" s="167"/>
-      <c r="H45" s="167"/>
-      <c r="I45" s="167"/>
-      <c r="J45" s="167"/>
-      <c r="K45" s="167"/>
-      <c r="L45" s="167"/>
-      <c r="M45" s="167"/>
-      <c r="N45" s="167"/>
-      <c r="O45" s="167"/>
-      <c r="P45" s="167"/>
-      <c r="Q45" s="167"/>
-      <c r="R45" s="167"/>
-      <c r="S45" s="167"/>
-      <c r="T45" s="167"/>
-      <c r="U45" s="167"/>
-      <c r="V45" s="167"/>
-      <c r="W45" s="167"/>
-      <c r="X45" s="167"/>
-      <c r="Y45" s="167"/>
-      <c r="Z45" s="167"/>
-      <c r="AA45" s="167"/>
-      <c r="AB45" s="167"/>
-      <c r="AC45" s="167"/>
-      <c r="AD45" s="167"/>
-      <c r="AE45" s="167"/>
-      <c r="AF45" s="167"/>
-      <c r="AG45" s="167"/>
-      <c r="AH45" s="167"/>
-      <c r="AI45" s="167"/>
-      <c r="AJ45" s="167"/>
-      <c r="AK45" s="167"/>
-      <c r="AL45" s="167"/>
-      <c r="AM45" s="167"/>
-      <c r="AN45" s="167"/>
-      <c r="AO45" s="167"/>
-      <c r="AP45" s="167"/>
-      <c r="AQ45" s="167"/>
-      <c r="AR45" s="167"/>
-      <c r="AS45" s="167"/>
-      <c r="AT45" s="167"/>
-      <c r="AU45" s="167"/>
-      <c r="AV45" s="167"/>
-      <c r="AW45" s="167"/>
-      <c r="AX45" s="167"/>
-      <c r="AY45" s="167"/>
-      <c r="AZ45" s="167"/>
-      <c r="BA45" s="167"/>
-      <c r="BB45" s="167"/>
-      <c r="BC45" s="167"/>
-      <c r="BD45" s="167"/>
-      <c r="BE45" s="167"/>
-      <c r="BF45" s="167"/>
-      <c r="BG45" s="167"/>
-      <c r="BH45" s="167"/>
-      <c r="BI45" s="167"/>
-      <c r="BJ45" s="167"/>
-      <c r="BK45" s="167"/>
-      <c r="BL45" s="167"/>
-      <c r="BM45" s="167"/>
-      <c r="BN45" s="167"/>
-      <c r="BO45" s="167"/>
-      <c r="BP45" s="167"/>
-      <c r="BQ45" s="167"/>
-      <c r="BR45" s="167"/>
-      <c r="BS45" s="167"/>
-      <c r="BT45" s="168"/>
+      <c r="C45" s="186"/>
+      <c r="D45" s="186"/>
+      <c r="E45" s="186"/>
+      <c r="F45" s="186"/>
+      <c r="G45" s="186"/>
+      <c r="H45" s="186"/>
+      <c r="I45" s="186"/>
+      <c r="J45" s="186"/>
+      <c r="K45" s="186"/>
+      <c r="L45" s="186"/>
+      <c r="M45" s="186"/>
+      <c r="N45" s="186"/>
+      <c r="O45" s="186"/>
+      <c r="P45" s="186"/>
+      <c r="Q45" s="186"/>
+      <c r="R45" s="186"/>
+      <c r="S45" s="186"/>
+      <c r="T45" s="186"/>
+      <c r="U45" s="186"/>
+      <c r="V45" s="186"/>
+      <c r="W45" s="186"/>
+      <c r="X45" s="186"/>
+      <c r="Y45" s="186"/>
+      <c r="Z45" s="186"/>
+      <c r="AA45" s="186"/>
+      <c r="AB45" s="186"/>
+      <c r="AC45" s="186"/>
+      <c r="AD45" s="186"/>
+      <c r="AE45" s="186"/>
+      <c r="AF45" s="186"/>
+      <c r="AG45" s="186"/>
+      <c r="AH45" s="186"/>
+      <c r="AI45" s="186"/>
+      <c r="AJ45" s="186"/>
+      <c r="AK45" s="186"/>
+      <c r="AL45" s="186"/>
+      <c r="AM45" s="186"/>
+      <c r="AN45" s="186"/>
+      <c r="AO45" s="186"/>
+      <c r="AP45" s="186"/>
+      <c r="AQ45" s="186"/>
+      <c r="AR45" s="186"/>
+      <c r="AS45" s="186"/>
+      <c r="AT45" s="186"/>
+      <c r="AU45" s="186"/>
+      <c r="AV45" s="186"/>
+      <c r="AW45" s="186"/>
+      <c r="AX45" s="186"/>
+      <c r="AY45" s="186"/>
+      <c r="AZ45" s="186"/>
+      <c r="BA45" s="186"/>
+      <c r="BB45" s="186"/>
+      <c r="BC45" s="186"/>
+      <c r="BD45" s="186"/>
+      <c r="BE45" s="186"/>
+      <c r="BF45" s="186"/>
+      <c r="BG45" s="186"/>
+      <c r="BH45" s="186"/>
+      <c r="BI45" s="186"/>
+      <c r="BJ45" s="186"/>
+      <c r="BK45" s="186"/>
+      <c r="BL45" s="186"/>
+      <c r="BM45" s="186"/>
+      <c r="BN45" s="186"/>
+      <c r="BO45" s="186"/>
+      <c r="BP45" s="186"/>
+      <c r="BQ45" s="186"/>
+      <c r="BR45" s="186"/>
+      <c r="BS45" s="186"/>
+      <c r="BT45" s="187"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12191,14 +12213,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12215,6 +12229,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12227,10 +12249,10 @@
     <tabColor rgb="FF7B3C16"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:BV1010"/>
+  <dimension ref="B1:BV1012"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BE40" sqref="BE40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12343,7 +12365,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="189" t="s">
+      <c r="K3" s="171" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12420,7 +12442,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="190"/>
+      <c r="K4" s="172"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12494,7 +12516,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="190"/>
+      <c r="K5" s="172"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12568,7 +12590,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="190"/>
+      <c r="K6" s="172"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12643,7 +12665,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="191"/>
+      <c r="K7" s="173"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12709,124 +12731,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="192" t="s">
+      <c r="B8" s="174" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="194" t="s">
+      <c r="C8" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="196" t="s">
+      <c r="D8" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="198" t="s">
+      <c r="E8" s="180" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="199"/>
-      <c r="G8" s="200"/>
-      <c r="H8" s="201" t="s">
+      <c r="F8" s="181"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="169" t="s">
+      <c r="I8" s="188" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="171" t="s">
+      <c r="J8" s="190" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="173" t="s">
+      <c r="K8" s="192" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="174" t="s">
+      <c r="L8" s="193" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="176" t="s">
+      <c r="M8" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="177"/>
-      <c r="O8" s="177"/>
-      <c r="P8" s="177"/>
-      <c r="Q8" s="178"/>
-      <c r="R8" s="179" t="s">
+      <c r="N8" s="167"/>
+      <c r="O8" s="167"/>
+      <c r="P8" s="167"/>
+      <c r="Q8" s="196"/>
+      <c r="R8" s="197" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="177"/>
-      <c r="T8" s="177"/>
-      <c r="U8" s="177"/>
-      <c r="V8" s="178"/>
-      <c r="W8" s="179" t="s">
+      <c r="S8" s="167"/>
+      <c r="T8" s="167"/>
+      <c r="U8" s="167"/>
+      <c r="V8" s="196"/>
+      <c r="W8" s="197" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="177"/>
-      <c r="Y8" s="177"/>
-      <c r="Z8" s="177"/>
-      <c r="AA8" s="180"/>
-      <c r="AB8" s="181" t="s">
+      <c r="X8" s="167"/>
+      <c r="Y8" s="167"/>
+      <c r="Z8" s="167"/>
+      <c r="AA8" s="168"/>
+      <c r="AB8" s="198" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="177"/>
-      <c r="AD8" s="177"/>
-      <c r="AE8" s="177"/>
-      <c r="AF8" s="178"/>
-      <c r="AG8" s="182" t="s">
+      <c r="AC8" s="167"/>
+      <c r="AD8" s="167"/>
+      <c r="AE8" s="167"/>
+      <c r="AF8" s="196"/>
+      <c r="AG8" s="199" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="177"/>
-      <c r="AI8" s="177"/>
-      <c r="AJ8" s="177"/>
-      <c r="AK8" s="178"/>
-      <c r="AL8" s="182" t="s">
+      <c r="AH8" s="167"/>
+      <c r="AI8" s="167"/>
+      <c r="AJ8" s="167"/>
+      <c r="AK8" s="196"/>
+      <c r="AL8" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="177"/>
-      <c r="AN8" s="177"/>
-      <c r="AO8" s="177"/>
-      <c r="AP8" s="180"/>
-      <c r="AQ8" s="183" t="s">
+      <c r="AM8" s="167"/>
+      <c r="AN8" s="167"/>
+      <c r="AO8" s="167"/>
+      <c r="AP8" s="168"/>
+      <c r="AQ8" s="200" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="177"/>
-      <c r="AS8" s="177"/>
-      <c r="AT8" s="177"/>
-      <c r="AU8" s="178"/>
-      <c r="AV8" s="184" t="s">
+      <c r="AR8" s="167"/>
+      <c r="AS8" s="167"/>
+      <c r="AT8" s="167"/>
+      <c r="AU8" s="196"/>
+      <c r="AV8" s="201" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="177"/>
-      <c r="AX8" s="177"/>
-      <c r="AY8" s="177"/>
-      <c r="AZ8" s="178"/>
-      <c r="BA8" s="184" t="s">
+      <c r="AW8" s="167"/>
+      <c r="AX8" s="167"/>
+      <c r="AY8" s="167"/>
+      <c r="AZ8" s="196"/>
+      <c r="BA8" s="201" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="177"/>
-      <c r="BC8" s="177"/>
-      <c r="BD8" s="177"/>
-      <c r="BE8" s="180"/>
-      <c r="BF8" s="185" t="s">
+      <c r="BB8" s="167"/>
+      <c r="BC8" s="167"/>
+      <c r="BD8" s="167"/>
+      <c r="BE8" s="168"/>
+      <c r="BF8" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="177"/>
-      <c r="BH8" s="177"/>
-      <c r="BI8" s="177"/>
-      <c r="BJ8" s="178"/>
-      <c r="BK8" s="186" t="s">
+      <c r="BG8" s="167"/>
+      <c r="BH8" s="167"/>
+      <c r="BI8" s="167"/>
+      <c r="BJ8" s="196"/>
+      <c r="BK8" s="166" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="177"/>
-      <c r="BM8" s="177"/>
-      <c r="BN8" s="177"/>
-      <c r="BO8" s="178"/>
-      <c r="BP8" s="186" t="s">
+      <c r="BL8" s="167"/>
+      <c r="BM8" s="167"/>
+      <c r="BN8" s="167"/>
+      <c r="BO8" s="196"/>
+      <c r="BP8" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="177"/>
-      <c r="BR8" s="177"/>
-      <c r="BS8" s="177"/>
-      <c r="BT8" s="180"/>
+      <c r="BQ8" s="167"/>
+      <c r="BR8" s="167"/>
+      <c r="BS8" s="167"/>
+      <c r="BT8" s="168"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="193"/>
-      <c r="C9" s="195"/>
-      <c r="D9" s="197"/>
+      <c r="B9" s="175"/>
+      <c r="C9" s="177"/>
+      <c r="D9" s="179"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12836,11 +12858,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="202"/>
-      <c r="I9" s="170"/>
-      <c r="J9" s="172"/>
-      <c r="K9" s="172"/>
-      <c r="L9" s="175"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="189"/>
+      <c r="J9" s="191"/>
+      <c r="K9" s="191"/>
+      <c r="L9" s="194"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -13049,7 +13071,7 @@
       <c r="J10" s="47"/>
       <c r="K10" s="48"/>
       <c r="L10" s="49">
-        <f t="shared" ref="L10:L44" si="0">F10/E10</f>
+        <f t="shared" ref="L10:L46" si="0">F10/E10</f>
         <v>1</v>
       </c>
       <c r="M10" s="50"/>
@@ -14893,7 +14915,7 @@
         <v>45398</v>
       </c>
       <c r="K29" s="62">
-        <f t="shared" ref="K29:K39" si="7">J29-I29+1</f>
+        <f t="shared" ref="K29:K40" si="7">J29-I29+1</f>
         <v>1</v>
       </c>
       <c r="L29" s="63">
@@ -15940,115 +15962,117 @@
       <c r="BT39" s="68"/>
     </row>
     <row r="40" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="53">
+      <c r="B40" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="C40" s="165" t="s">
+        <v>256</v>
+      </c>
+      <c r="D40" s="157" t="s">
+        <v>211</v>
+      </c>
+      <c r="E40" s="56">
         <v>4</v>
       </c>
-      <c r="C40" s="73"/>
-      <c r="D40" s="74"/>
-      <c r="E40" s="42">
-        <f t="shared" ref="E40:G40" si="8">SUM(E41:E44)</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="43">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="44">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H40" s="75"/>
-      <c r="I40" s="76"/>
-      <c r="J40" s="77"/>
-      <c r="K40" s="77"/>
-      <c r="L40" s="49" t="e">
+      <c r="F40" s="57">
+        <v>5</v>
+      </c>
+      <c r="G40" s="58">
+        <f>E40-F40</f>
+        <v>-1</v>
+      </c>
+      <c r="H40" s="59">
+        <v>2</v>
+      </c>
+      <c r="I40" s="158">
+        <v>45414</v>
+      </c>
+      <c r="J40" s="61">
+        <v>45416</v>
+      </c>
+      <c r="K40" s="62">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="L40" s="63">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M40" s="50"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="51"/>
-      <c r="P40" s="51"/>
-      <c r="Q40" s="51"/>
-      <c r="R40" s="51"/>
-      <c r="S40" s="51"/>
-      <c r="T40" s="51"/>
-      <c r="U40" s="51"/>
-      <c r="V40" s="51"/>
-      <c r="W40" s="51"/>
-      <c r="X40" s="51"/>
-      <c r="Y40" s="51"/>
-      <c r="Z40" s="51"/>
-      <c r="AA40" s="52"/>
-      <c r="AB40" s="50"/>
-      <c r="AC40" s="51"/>
-      <c r="AD40" s="51"/>
-      <c r="AE40" s="51"/>
-      <c r="AF40" s="51"/>
-      <c r="AG40" s="51"/>
-      <c r="AH40" s="51"/>
-      <c r="AI40" s="51"/>
-      <c r="AJ40" s="51"/>
-      <c r="AK40" s="51"/>
-      <c r="AL40" s="51"/>
-      <c r="AM40" s="51"/>
-      <c r="AN40" s="51"/>
-      <c r="AO40" s="51"/>
-      <c r="AP40" s="52"/>
-      <c r="AQ40" s="50"/>
-      <c r="AR40" s="51"/>
-      <c r="AS40" s="51"/>
-      <c r="AT40" s="51"/>
-      <c r="AU40" s="51"/>
-      <c r="AV40" s="51"/>
-      <c r="AW40" s="51"/>
-      <c r="AX40" s="51"/>
-      <c r="AY40" s="51"/>
-      <c r="AZ40" s="51"/>
-      <c r="BA40" s="51"/>
-      <c r="BB40" s="51"/>
-      <c r="BC40" s="51"/>
-      <c r="BD40" s="51"/>
-      <c r="BE40" s="52"/>
-      <c r="BF40" s="50"/>
-      <c r="BG40" s="51"/>
-      <c r="BH40" s="51"/>
-      <c r="BI40" s="51"/>
-      <c r="BJ40" s="51"/>
-      <c r="BK40" s="51"/>
-      <c r="BL40" s="51"/>
-      <c r="BM40" s="51"/>
-      <c r="BN40" s="51"/>
-      <c r="BO40" s="51"/>
-      <c r="BP40" s="51"/>
-      <c r="BQ40" s="51"/>
-      <c r="BR40" s="51"/>
-      <c r="BS40" s="51"/>
-      <c r="BT40" s="52"/>
+        <v>1.25</v>
+      </c>
+      <c r="M40" s="64"/>
+      <c r="N40" s="65"/>
+      <c r="O40" s="65"/>
+      <c r="P40" s="65"/>
+      <c r="Q40" s="65"/>
+      <c r="R40" s="67"/>
+      <c r="S40" s="67"/>
+      <c r="T40" s="67"/>
+      <c r="U40" s="67"/>
+      <c r="V40" s="67"/>
+      <c r="W40" s="65"/>
+      <c r="X40" s="65"/>
+      <c r="Y40" s="65"/>
+      <c r="Z40" s="65"/>
+      <c r="AA40" s="68"/>
+      <c r="AB40" s="64"/>
+      <c r="AC40" s="65"/>
+      <c r="AD40" s="65"/>
+      <c r="AE40" s="65"/>
+      <c r="AF40" s="65"/>
+      <c r="AG40" s="69"/>
+      <c r="AH40" s="69"/>
+      <c r="AI40" s="69"/>
+      <c r="AJ40" s="69"/>
+      <c r="AK40" s="69"/>
+      <c r="AL40" s="65"/>
+      <c r="AM40" s="65"/>
+      <c r="AN40" s="65"/>
+      <c r="AO40" s="65"/>
+      <c r="AP40" s="68"/>
+      <c r="AQ40" s="64"/>
+      <c r="AR40" s="65"/>
+      <c r="AS40" s="65"/>
+      <c r="AT40" s="65"/>
+      <c r="AU40" s="65"/>
+      <c r="AV40" s="70"/>
+      <c r="AW40" s="70"/>
+      <c r="AX40" s="70"/>
+      <c r="AY40" s="70"/>
+      <c r="AZ40" s="70"/>
+      <c r="BA40" s="65"/>
+      <c r="BB40" s="65"/>
+      <c r="BC40" s="204"/>
+      <c r="BD40" s="204"/>
+      <c r="BE40" s="205"/>
+      <c r="BF40" s="64"/>
+      <c r="BG40" s="65"/>
+      <c r="BH40" s="65"/>
+      <c r="BI40" s="65"/>
+      <c r="BJ40" s="65"/>
+      <c r="BK40" s="71"/>
+      <c r="BL40" s="71"/>
+      <c r="BM40" s="71"/>
+      <c r="BN40" s="71"/>
+      <c r="BO40" s="71"/>
+      <c r="BP40" s="65"/>
+      <c r="BQ40" s="65"/>
+      <c r="BR40" s="65"/>
+      <c r="BS40" s="65"/>
+      <c r="BT40" s="68"/>
     </row>
     <row r="41" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="53">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C41" s="54"/>
-      <c r="D41" s="55"/>
+      <c r="B41" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="C41" s="165"/>
+      <c r="D41" s="157"/>
       <c r="E41" s="56"/>
       <c r="F41" s="57"/>
-      <c r="G41" s="58">
-        <f t="shared" ref="G41:G44" si="9">E41-F41</f>
-        <v>0</v>
-      </c>
+      <c r="G41" s="58"/>
       <c r="H41" s="59"/>
-      <c r="I41" s="60"/>
+      <c r="I41" s="158"/>
       <c r="J41" s="61"/>
-      <c r="K41" s="62">
-        <f t="shared" ref="K41:K44" si="10">J41-I41+1</f>
-        <v>1</v>
-      </c>
-      <c r="L41" s="63" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K41" s="62"/>
+      <c r="L41" s="63"/>
       <c r="M41" s="64"/>
       <c r="N41" s="65"/>
       <c r="O41" s="65"/>
@@ -16093,8 +16117,8 @@
       <c r="BB41" s="65"/>
       <c r="BC41" s="65"/>
       <c r="BD41" s="65"/>
-      <c r="BE41" s="68"/>
-      <c r="BF41" s="113"/>
+      <c r="BE41" s="65"/>
+      <c r="BF41" s="64"/>
       <c r="BG41" s="65"/>
       <c r="BH41" s="65"/>
       <c r="BI41" s="65"/>
@@ -16112,105 +16136,108 @@
     </row>
     <row r="42" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="53">
-        <v>4.2</v>
-      </c>
-      <c r="C42" s="54"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="57"/>
-      <c r="G42" s="58">
-        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="C42" s="73"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="42">
+        <f t="shared" ref="E42:G42" si="8">SUM(E43:E46)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="59"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="61"/>
-      <c r="K42" s="62">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="L42" s="63" t="e">
+      <c r="F42" s="43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G42" s="44">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H42" s="75"/>
+      <c r="I42" s="76"/>
+      <c r="J42" s="77"/>
+      <c r="K42" s="77"/>
+      <c r="L42" s="49" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M42" s="64"/>
-      <c r="N42" s="65"/>
-      <c r="O42" s="65"/>
-      <c r="P42" s="65"/>
-      <c r="Q42" s="65"/>
-      <c r="R42" s="67"/>
-      <c r="S42" s="67"/>
-      <c r="T42" s="67"/>
-      <c r="U42" s="67"/>
-      <c r="V42" s="67"/>
-      <c r="W42" s="65"/>
-      <c r="X42" s="65"/>
-      <c r="Y42" s="65"/>
-      <c r="Z42" s="65"/>
-      <c r="AA42" s="68"/>
-      <c r="AB42" s="64"/>
-      <c r="AC42" s="65"/>
-      <c r="AD42" s="65"/>
-      <c r="AE42" s="65"/>
-      <c r="AF42" s="65"/>
-      <c r="AG42" s="69"/>
-      <c r="AH42" s="69"/>
-      <c r="AI42" s="69"/>
-      <c r="AJ42" s="69"/>
-      <c r="AK42" s="69"/>
-      <c r="AL42" s="65"/>
-      <c r="AM42" s="65"/>
-      <c r="AN42" s="65"/>
-      <c r="AO42" s="65"/>
-      <c r="AP42" s="68"/>
-      <c r="AQ42" s="64"/>
-      <c r="AR42" s="65"/>
-      <c r="AS42" s="65"/>
-      <c r="AT42" s="65"/>
-      <c r="AU42" s="65"/>
-      <c r="AV42" s="70"/>
-      <c r="AW42" s="70"/>
-      <c r="AX42" s="70"/>
-      <c r="AY42" s="70"/>
-      <c r="AZ42" s="70"/>
-      <c r="BA42" s="65"/>
-      <c r="BB42" s="65"/>
-      <c r="BC42" s="65"/>
-      <c r="BD42" s="65"/>
-      <c r="BE42" s="68"/>
-      <c r="BF42" s="64"/>
-      <c r="BG42" s="65"/>
-      <c r="BH42" s="65"/>
-      <c r="BI42" s="65"/>
-      <c r="BJ42" s="65"/>
-      <c r="BK42" s="71"/>
-      <c r="BL42" s="71"/>
-      <c r="BM42" s="71"/>
-      <c r="BN42" s="71"/>
-      <c r="BO42" s="71"/>
-      <c r="BP42" s="65"/>
-      <c r="BQ42" s="65"/>
-      <c r="BR42" s="65"/>
-      <c r="BS42" s="65"/>
-      <c r="BT42" s="68"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="51"/>
+      <c r="O42" s="51"/>
+      <c r="P42" s="51"/>
+      <c r="Q42" s="51"/>
+      <c r="R42" s="51"/>
+      <c r="S42" s="51"/>
+      <c r="T42" s="51"/>
+      <c r="U42" s="51"/>
+      <c r="V42" s="51"/>
+      <c r="W42" s="51"/>
+      <c r="X42" s="51"/>
+      <c r="Y42" s="51"/>
+      <c r="Z42" s="51"/>
+      <c r="AA42" s="52"/>
+      <c r="AB42" s="50"/>
+      <c r="AC42" s="51"/>
+      <c r="AD42" s="51"/>
+      <c r="AE42" s="51"/>
+      <c r="AF42" s="51"/>
+      <c r="AG42" s="51"/>
+      <c r="AH42" s="51"/>
+      <c r="AI42" s="51"/>
+      <c r="AJ42" s="51"/>
+      <c r="AK42" s="51"/>
+      <c r="AL42" s="51"/>
+      <c r="AM42" s="51"/>
+      <c r="AN42" s="51"/>
+      <c r="AO42" s="51"/>
+      <c r="AP42" s="52"/>
+      <c r="AQ42" s="50"/>
+      <c r="AR42" s="51"/>
+      <c r="AS42" s="51"/>
+      <c r="AT42" s="51"/>
+      <c r="AU42" s="51"/>
+      <c r="AV42" s="51"/>
+      <c r="AW42" s="51"/>
+      <c r="AX42" s="51"/>
+      <c r="AY42" s="51"/>
+      <c r="AZ42" s="51"/>
+      <c r="BA42" s="51"/>
+      <c r="BB42" s="51"/>
+      <c r="BC42" s="51"/>
+      <c r="BD42" s="51"/>
+      <c r="BE42" s="52"/>
+      <c r="BF42" s="50"/>
+      <c r="BG42" s="51"/>
+      <c r="BH42" s="51"/>
+      <c r="BI42" s="51"/>
+      <c r="BJ42" s="51"/>
+      <c r="BK42" s="51"/>
+      <c r="BL42" s="51"/>
+      <c r="BM42" s="51"/>
+      <c r="BN42" s="51"/>
+      <c r="BO42" s="51"/>
+      <c r="BP42" s="51"/>
+      <c r="BQ42" s="51"/>
+      <c r="BR42" s="51"/>
+      <c r="BS42" s="51"/>
+      <c r="BT42" s="52"/>
     </row>
     <row r="43" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="53">
-        <v>4.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C43" s="54"/>
-      <c r="D43" s="80"/>
+      <c r="D43" s="55"/>
       <c r="E43" s="56"/>
       <c r="F43" s="57"/>
       <c r="G43" s="58">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="G43:G46" si="9">E43-F43</f>
         <v>0</v>
       </c>
       <c r="H43" s="59"/>
       <c r="I43" s="60"/>
       <c r="J43" s="61"/>
       <c r="K43" s="62">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="K43:K46" si="10">J43-I43+1</f>
         <v>1</v>
       </c>
       <c r="L43" s="63" t="e">
@@ -16262,7 +16289,7 @@
       <c r="BC43" s="65"/>
       <c r="BD43" s="65"/>
       <c r="BE43" s="68"/>
-      <c r="BF43" s="64"/>
+      <c r="BF43" s="113"/>
       <c r="BG43" s="65"/>
       <c r="BH43" s="65"/>
       <c r="BI43" s="65"/>
@@ -16278,1206 +16305,1372 @@
       <c r="BS43" s="65"/>
       <c r="BT43" s="68"/>
     </row>
-    <row r="44" spans="2:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="82"/>
-      <c r="D44" s="83"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="85"/>
-      <c r="G44" s="86">
+    <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="53">
+        <v>4.2</v>
+      </c>
+      <c r="C44" s="54"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="58">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H44" s="87"/>
-      <c r="I44" s="88"/>
-      <c r="J44" s="89"/>
-      <c r="K44" s="90">
+      <c r="H44" s="59"/>
+      <c r="I44" s="60"/>
+      <c r="J44" s="61"/>
+      <c r="K44" s="62">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="L44" s="91" t="e">
+      <c r="L44" s="63" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M44" s="92"/>
-      <c r="N44" s="93"/>
-      <c r="O44" s="93"/>
-      <c r="P44" s="93"/>
-      <c r="Q44" s="93"/>
-      <c r="R44" s="94"/>
-      <c r="S44" s="94"/>
-      <c r="T44" s="94"/>
-      <c r="U44" s="94"/>
-      <c r="V44" s="94"/>
-      <c r="W44" s="93"/>
-      <c r="X44" s="93"/>
-      <c r="Y44" s="93"/>
-      <c r="Z44" s="93"/>
-      <c r="AA44" s="95"/>
-      <c r="AB44" s="92"/>
-      <c r="AC44" s="93"/>
-      <c r="AD44" s="93"/>
-      <c r="AE44" s="93"/>
-      <c r="AF44" s="93"/>
-      <c r="AG44" s="96"/>
-      <c r="AH44" s="96"/>
-      <c r="AI44" s="96"/>
-      <c r="AJ44" s="96"/>
-      <c r="AK44" s="96"/>
-      <c r="AL44" s="93"/>
-      <c r="AM44" s="93"/>
-      <c r="AN44" s="93"/>
-      <c r="AO44" s="93"/>
-      <c r="AP44" s="95"/>
-      <c r="AQ44" s="92"/>
-      <c r="AR44" s="93"/>
-      <c r="AS44" s="93"/>
-      <c r="AT44" s="93"/>
-      <c r="AU44" s="93"/>
-      <c r="AV44" s="97"/>
-      <c r="AW44" s="97"/>
-      <c r="AX44" s="97"/>
-      <c r="AY44" s="97"/>
-      <c r="AZ44" s="97"/>
-      <c r="BA44" s="93"/>
-      <c r="BB44" s="93"/>
-      <c r="BC44" s="93"/>
-      <c r="BD44" s="93"/>
-      <c r="BE44" s="95"/>
-      <c r="BF44" s="92"/>
-      <c r="BG44" s="93"/>
-      <c r="BH44" s="93"/>
-      <c r="BI44" s="93"/>
-      <c r="BJ44" s="93"/>
-      <c r="BK44" s="98"/>
-      <c r="BL44" s="98"/>
-      <c r="BM44" s="98"/>
-      <c r="BN44" s="98"/>
-      <c r="BO44" s="98"/>
-      <c r="BP44" s="93"/>
-      <c r="BQ44" s="93"/>
-      <c r="BR44" s="93"/>
-      <c r="BS44" s="93"/>
-      <c r="BT44" s="95"/>
+      <c r="M44" s="64"/>
+      <c r="N44" s="65"/>
+      <c r="O44" s="65"/>
+      <c r="P44" s="65"/>
+      <c r="Q44" s="65"/>
+      <c r="R44" s="67"/>
+      <c r="S44" s="67"/>
+      <c r="T44" s="67"/>
+      <c r="U44" s="67"/>
+      <c r="V44" s="67"/>
+      <c r="W44" s="65"/>
+      <c r="X44" s="65"/>
+      <c r="Y44" s="65"/>
+      <c r="Z44" s="65"/>
+      <c r="AA44" s="68"/>
+      <c r="AB44" s="64"/>
+      <c r="AC44" s="65"/>
+      <c r="AD44" s="65"/>
+      <c r="AE44" s="65"/>
+      <c r="AF44" s="65"/>
+      <c r="AG44" s="69"/>
+      <c r="AH44" s="69"/>
+      <c r="AI44" s="69"/>
+      <c r="AJ44" s="69"/>
+      <c r="AK44" s="69"/>
+      <c r="AL44" s="65"/>
+      <c r="AM44" s="65"/>
+      <c r="AN44" s="65"/>
+      <c r="AO44" s="65"/>
+      <c r="AP44" s="68"/>
+      <c r="AQ44" s="64"/>
+      <c r="AR44" s="65"/>
+      <c r="AS44" s="65"/>
+      <c r="AT44" s="65"/>
+      <c r="AU44" s="65"/>
+      <c r="AV44" s="70"/>
+      <c r="AW44" s="70"/>
+      <c r="AX44" s="70"/>
+      <c r="AY44" s="70"/>
+      <c r="AZ44" s="70"/>
+      <c r="BA44" s="65"/>
+      <c r="BB44" s="65"/>
+      <c r="BC44" s="65"/>
+      <c r="BD44" s="65"/>
+      <c r="BE44" s="68"/>
+      <c r="BF44" s="64"/>
+      <c r="BG44" s="65"/>
+      <c r="BH44" s="65"/>
+      <c r="BI44" s="65"/>
+      <c r="BJ44" s="65"/>
+      <c r="BK44" s="71"/>
+      <c r="BL44" s="71"/>
+      <c r="BM44" s="71"/>
+      <c r="BN44" s="71"/>
+      <c r="BO44" s="71"/>
+      <c r="BP44" s="65"/>
+      <c r="BQ44" s="65"/>
+      <c r="BR44" s="65"/>
+      <c r="BS44" s="65"/>
+      <c r="BT44" s="68"/>
     </row>
-    <row r="45" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E45" s="99" t="s">
-        <v>29</v>
-      </c>
-      <c r="F45" s="99" t="s">
-        <v>30</v>
-      </c>
-      <c r="G45" s="99" t="s">
-        <v>31</v>
-      </c>
-      <c r="H45" s="99" t="s">
-        <v>73</v>
-      </c>
-      <c r="I45" s="99" t="s">
-        <v>74</v>
-      </c>
+    <row r="45" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="53">
+        <v>4.3</v>
+      </c>
+      <c r="C45" s="54"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="58">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H45" s="59"/>
+      <c r="I45" s="60"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="62">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="L45" s="63" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M45" s="64"/>
+      <c r="N45" s="65"/>
+      <c r="O45" s="65"/>
+      <c r="P45" s="65"/>
+      <c r="Q45" s="65"/>
+      <c r="R45" s="67"/>
+      <c r="S45" s="67"/>
+      <c r="T45" s="67"/>
+      <c r="U45" s="67"/>
+      <c r="V45" s="67"/>
+      <c r="W45" s="65"/>
+      <c r="X45" s="65"/>
+      <c r="Y45" s="65"/>
+      <c r="Z45" s="65"/>
+      <c r="AA45" s="68"/>
+      <c r="AB45" s="64"/>
+      <c r="AC45" s="65"/>
+      <c r="AD45" s="65"/>
+      <c r="AE45" s="65"/>
+      <c r="AF45" s="65"/>
+      <c r="AG45" s="69"/>
+      <c r="AH45" s="69"/>
+      <c r="AI45" s="69"/>
+      <c r="AJ45" s="69"/>
+      <c r="AK45" s="69"/>
+      <c r="AL45" s="65"/>
+      <c r="AM45" s="65"/>
+      <c r="AN45" s="65"/>
+      <c r="AO45" s="65"/>
+      <c r="AP45" s="68"/>
+      <c r="AQ45" s="64"/>
+      <c r="AR45" s="65"/>
+      <c r="AS45" s="65"/>
+      <c r="AT45" s="65"/>
+      <c r="AU45" s="65"/>
+      <c r="AV45" s="70"/>
+      <c r="AW45" s="70"/>
+      <c r="AX45" s="70"/>
+      <c r="AY45" s="70"/>
+      <c r="AZ45" s="70"/>
+      <c r="BA45" s="65"/>
+      <c r="BB45" s="65"/>
+      <c r="BC45" s="65"/>
+      <c r="BD45" s="65"/>
+      <c r="BE45" s="68"/>
+      <c r="BF45" s="64"/>
+      <c r="BG45" s="65"/>
+      <c r="BH45" s="65"/>
+      <c r="BI45" s="65"/>
+      <c r="BJ45" s="65"/>
+      <c r="BK45" s="71"/>
+      <c r="BL45" s="71"/>
+      <c r="BM45" s="71"/>
+      <c r="BN45" s="71"/>
+      <c r="BO45" s="71"/>
+      <c r="BP45" s="65"/>
+      <c r="BQ45" s="65"/>
+      <c r="BR45" s="65"/>
+      <c r="BS45" s="65"/>
+      <c r="BT45" s="68"/>
     </row>
-    <row r="46" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D46" s="100" t="s">
-        <v>76</v>
-      </c>
-      <c r="E46" s="101">
-        <f>SUM(E11:E16,E18:E21,E29:E37,E41:E44)</f>
-        <v>49</v>
-      </c>
-      <c r="F46" s="101">
-        <f>SUM(F11:F16,F18:F21,F29:F37,F41:F44)</f>
-        <v>51</v>
-      </c>
-      <c r="G46" s="101">
-        <f>SUM(G11:G16,G18:G21,G29:G37,G41:G44)</f>
-        <v>-2</v>
-      </c>
-      <c r="H46" s="101">
-        <v>60</v>
-      </c>
-      <c r="I46" s="101">
-        <f>E46/H46</f>
-        <v>0.81666666666666665</v>
-      </c>
-      <c r="L46" s="102" t="s">
-        <v>77</v>
-      </c>
-      <c r="M46" s="103">
+    <row r="46" spans="2:74" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="82"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="84"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="86">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H46" s="87"/>
+      <c r="I46" s="88"/>
+      <c r="J46" s="89"/>
+      <c r="K46" s="90">
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="N46" s="103">
-        <v>2</v>
-      </c>
-      <c r="O46" s="103">
-        <v>3</v>
-      </c>
-      <c r="P46" s="103">
-        <v>4</v>
-      </c>
-      <c r="Q46" s="103">
-        <v>5</v>
-      </c>
-      <c r="R46" s="103">
-        <v>6</v>
-      </c>
-      <c r="S46" s="103">
-        <v>7</v>
-      </c>
-      <c r="T46" s="103">
-        <v>8</v>
-      </c>
-      <c r="U46" s="103">
-        <v>9</v>
-      </c>
-      <c r="V46" s="103">
-        <v>10</v>
-      </c>
-      <c r="W46" s="103">
-        <v>11</v>
-      </c>
-      <c r="X46" s="103">
-        <v>12</v>
-      </c>
-      <c r="Y46" s="103">
-        <v>13</v>
-      </c>
-      <c r="Z46" s="103">
-        <v>14</v>
-      </c>
-      <c r="AA46" s="103">
-        <v>15</v>
-      </c>
-      <c r="AB46" s="103">
-        <v>16</v>
-      </c>
-      <c r="AC46" s="103">
-        <v>17</v>
-      </c>
-      <c r="AD46" s="103">
-        <v>18</v>
-      </c>
-      <c r="AE46" s="103">
-        <v>19</v>
-      </c>
-      <c r="AF46" s="103">
-        <v>20</v>
-      </c>
-      <c r="AG46" s="103">
-        <v>21</v>
-      </c>
-      <c r="AH46" s="103">
-        <v>22</v>
-      </c>
-      <c r="AI46" s="103">
-        <v>23</v>
-      </c>
-      <c r="AJ46" s="103">
-        <v>24</v>
-      </c>
-      <c r="AK46" s="103">
-        <v>25</v>
-      </c>
-      <c r="AL46" s="103">
-        <v>26</v>
-      </c>
-      <c r="AM46" s="103">
-        <v>27</v>
-      </c>
-      <c r="AN46" s="103">
-        <v>28</v>
-      </c>
-      <c r="AO46" s="103">
-        <v>29</v>
-      </c>
-      <c r="AP46" s="103">
-        <v>30</v>
-      </c>
-      <c r="AQ46" s="103">
-        <v>31</v>
-      </c>
-      <c r="AR46" s="103">
-        <v>32</v>
-      </c>
-      <c r="AS46" s="103">
-        <v>33</v>
-      </c>
-      <c r="AT46" s="103">
-        <v>34</v>
-      </c>
-      <c r="AU46" s="103">
-        <v>35</v>
-      </c>
-      <c r="AV46" s="103">
-        <v>36</v>
-      </c>
-      <c r="AW46" s="103">
-        <v>37</v>
-      </c>
-      <c r="AX46" s="103">
-        <v>38</v>
-      </c>
-      <c r="AY46" s="103">
-        <v>39</v>
-      </c>
-      <c r="AZ46" s="103">
-        <v>40</v>
-      </c>
-      <c r="BA46" s="103">
-        <v>41</v>
-      </c>
-      <c r="BB46" s="103">
-        <v>42</v>
-      </c>
-      <c r="BC46" s="103">
-        <v>43</v>
-      </c>
-      <c r="BD46" s="103">
-        <v>44</v>
-      </c>
-      <c r="BE46" s="103">
-        <v>45</v>
-      </c>
-      <c r="BF46" s="103">
-        <v>46</v>
-      </c>
-      <c r="BG46" s="103">
-        <v>47</v>
-      </c>
-      <c r="BH46" s="103">
-        <v>48</v>
-      </c>
-      <c r="BI46" s="103">
-        <v>49</v>
-      </c>
-      <c r="BJ46" s="103">
-        <v>50</v>
-      </c>
-      <c r="BK46" s="103">
-        <v>51</v>
-      </c>
-      <c r="BL46" s="103">
-        <v>52</v>
-      </c>
-      <c r="BM46" s="103">
-        <v>53</v>
-      </c>
-      <c r="BN46" s="103">
-        <v>54</v>
-      </c>
-      <c r="BO46" s="103">
-        <v>55</v>
-      </c>
-      <c r="BP46" s="103">
-        <v>56</v>
-      </c>
-      <c r="BQ46" s="103">
-        <v>57</v>
-      </c>
-      <c r="BR46" s="103">
-        <v>58</v>
-      </c>
-      <c r="BS46" s="103">
-        <v>59</v>
-      </c>
-      <c r="BT46" s="103">
-        <v>60</v>
-      </c>
-      <c r="BV46" s="100" t="s">
-        <v>76</v>
-      </c>
+      <c r="L46" s="91" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M46" s="92"/>
+      <c r="N46" s="93"/>
+      <c r="O46" s="93"/>
+      <c r="P46" s="93"/>
+      <c r="Q46" s="93"/>
+      <c r="R46" s="94"/>
+      <c r="S46" s="94"/>
+      <c r="T46" s="94"/>
+      <c r="U46" s="94"/>
+      <c r="V46" s="94"/>
+      <c r="W46" s="93"/>
+      <c r="X46" s="93"/>
+      <c r="Y46" s="93"/>
+      <c r="Z46" s="93"/>
+      <c r="AA46" s="95"/>
+      <c r="AB46" s="92"/>
+      <c r="AC46" s="93"/>
+      <c r="AD46" s="93"/>
+      <c r="AE46" s="93"/>
+      <c r="AF46" s="93"/>
+      <c r="AG46" s="96"/>
+      <c r="AH46" s="96"/>
+      <c r="AI46" s="96"/>
+      <c r="AJ46" s="96"/>
+      <c r="AK46" s="96"/>
+      <c r="AL46" s="93"/>
+      <c r="AM46" s="93"/>
+      <c r="AN46" s="93"/>
+      <c r="AO46" s="93"/>
+      <c r="AP46" s="95"/>
+      <c r="AQ46" s="92"/>
+      <c r="AR46" s="93"/>
+      <c r="AS46" s="93"/>
+      <c r="AT46" s="93"/>
+      <c r="AU46" s="93"/>
+      <c r="AV46" s="97"/>
+      <c r="AW46" s="97"/>
+      <c r="AX46" s="97"/>
+      <c r="AY46" s="97"/>
+      <c r="AZ46" s="97"/>
+      <c r="BA46" s="93"/>
+      <c r="BB46" s="93"/>
+      <c r="BC46" s="93"/>
+      <c r="BD46" s="93"/>
+      <c r="BE46" s="95"/>
+      <c r="BF46" s="92"/>
+      <c r="BG46" s="93"/>
+      <c r="BH46" s="93"/>
+      <c r="BI46" s="93"/>
+      <c r="BJ46" s="93"/>
+      <c r="BK46" s="98"/>
+      <c r="BL46" s="98"/>
+      <c r="BM46" s="98"/>
+      <c r="BN46" s="98"/>
+      <c r="BO46" s="98"/>
+      <c r="BP46" s="93"/>
+      <c r="BQ46" s="93"/>
+      <c r="BR46" s="93"/>
+      <c r="BS46" s="93"/>
+      <c r="BT46" s="95"/>
     </row>
     <row r="47" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H47" s="104" t="s">
-        <v>78</v>
-      </c>
-      <c r="L47" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="M47" s="105">
-        <f>E46</f>
-        <v>49</v>
-      </c>
-      <c r="N47" s="106">
-        <f>M47-I46</f>
-        <v>48.18333333333333</v>
-      </c>
-      <c r="O47" s="106">
-        <f>N47-I46</f>
-        <v>47.36666666666666</v>
-      </c>
-      <c r="P47" s="106">
-        <f>O47-I46</f>
-        <v>46.54999999999999</v>
-      </c>
-      <c r="Q47" s="106">
-        <f>P47-I46</f>
-        <v>45.73333333333332</v>
-      </c>
-      <c r="R47" s="106">
-        <f>Q47-I46</f>
-        <v>44.91666666666665</v>
-      </c>
-      <c r="S47" s="106">
-        <f>R47-I46</f>
-        <v>44.09999999999998</v>
-      </c>
-      <c r="T47" s="106">
-        <f>S47-I46</f>
-        <v>43.28333333333331</v>
-      </c>
-      <c r="U47" s="106">
-        <f>T47-I46</f>
-        <v>42.46666666666664</v>
-      </c>
-      <c r="V47" s="106">
-        <f>U47-I46</f>
-        <v>41.64999999999997</v>
-      </c>
-      <c r="W47" s="106">
-        <f>V47-I46</f>
-        <v>40.8333333333333</v>
-      </c>
-      <c r="X47" s="106">
-        <f>W47-I46</f>
-        <v>40.01666666666663</v>
-      </c>
-      <c r="Y47" s="106">
-        <f>X47-I46</f>
-        <v>39.19999999999996</v>
-      </c>
-      <c r="Z47" s="106">
-        <f>Y47-I46</f>
-        <v>38.38333333333329</v>
-      </c>
-      <c r="AA47" s="106">
-        <f>Z47-I46</f>
-        <v>37.56666666666662</v>
-      </c>
-      <c r="AB47" s="106">
-        <f>AA47-I46</f>
-        <v>36.74999999999995</v>
-      </c>
-      <c r="AC47" s="106">
-        <f>AB47-I46</f>
-        <v>35.93333333333328</v>
-      </c>
-      <c r="AD47" s="106">
-        <f>AC47-I46</f>
-        <v>35.11666666666661</v>
-      </c>
-      <c r="AE47" s="106">
-        <f>AD47-I46</f>
-        <v>34.29999999999994</v>
-      </c>
-      <c r="AF47" s="106">
-        <f>AE47-I46</f>
-        <v>33.48333333333327</v>
-      </c>
-      <c r="AG47" s="106">
-        <f>AF47-I46</f>
-        <v>32.6666666666666</v>
-      </c>
-      <c r="AH47" s="106">
-        <f>AG47-I46</f>
-        <v>31.849999999999934</v>
-      </c>
-      <c r="AI47" s="106">
-        <f>AH47-I46</f>
-        <v>31.033333333333267</v>
-      </c>
-      <c r="AJ47" s="106">
-        <f>AI47-I46</f>
-        <v>30.216666666666601</v>
-      </c>
-      <c r="AK47" s="106">
-        <f>AJ47-I46</f>
-        <v>29.399999999999935</v>
-      </c>
-      <c r="AL47" s="106">
-        <f>AK47-I46</f>
-        <v>28.583333333333268</v>
-      </c>
-      <c r="AM47" s="106">
-        <f>AL47-I46</f>
-        <v>27.766666666666602</v>
-      </c>
-      <c r="AN47" s="106">
-        <f>AM47-I46</f>
-        <v>26.949999999999935</v>
-      </c>
-      <c r="AO47" s="106">
-        <f>AN47-I46</f>
-        <v>26.133333333333269</v>
-      </c>
-      <c r="AP47" s="106">
-        <f>AO47-I46</f>
-        <v>25.316666666666602</v>
-      </c>
-      <c r="AQ47" s="106">
-        <f>AP47-I46</f>
-        <v>24.499999999999936</v>
-      </c>
-      <c r="AR47" s="106">
-        <f>AQ47-I46</f>
-        <v>23.68333333333327</v>
-      </c>
-      <c r="AS47" s="106">
-        <f>AR47-I46</f>
-        <v>22.866666666666603</v>
-      </c>
-      <c r="AT47" s="106">
-        <f>AS47-I46</f>
-        <v>22.049999999999937</v>
-      </c>
-      <c r="AU47" s="106">
-        <f>AT47-I46</f>
-        <v>21.23333333333327</v>
-      </c>
-      <c r="AV47" s="106">
-        <f>AU47-I46</f>
-        <v>20.416666666666604</v>
-      </c>
-      <c r="AW47" s="106">
-        <f>AV47-I46</f>
-        <v>19.599999999999937</v>
-      </c>
-      <c r="AX47" s="106">
-        <f>AW47-I46</f>
-        <v>18.783333333333271</v>
-      </c>
-      <c r="AY47" s="106">
-        <f>AX47-I46</f>
-        <v>17.966666666666605</v>
-      </c>
-      <c r="AZ47" s="106">
-        <f>AY47-I46</f>
-        <v>17.149999999999938</v>
-      </c>
-      <c r="BA47" s="106">
-        <f>AZ47-I46</f>
-        <v>16.333333333333272</v>
-      </c>
-      <c r="BB47" s="106">
-        <f>BA47-I46</f>
-        <v>15.516666666666605</v>
-      </c>
-      <c r="BC47" s="106">
-        <f>BB47-I46</f>
-        <v>14.699999999999939</v>
-      </c>
-      <c r="BD47" s="106">
-        <f>BC47-I46</f>
-        <v>13.883333333333272</v>
-      </c>
-      <c r="BE47" s="106">
-        <f>BD47-I46</f>
-        <v>13.066666666666606</v>
-      </c>
-      <c r="BF47" s="106">
-        <f>BE47-I46</f>
-        <v>12.24999999999994</v>
-      </c>
-      <c r="BG47" s="106">
-        <f>BF47-I46</f>
-        <v>11.433333333333273</v>
-      </c>
-      <c r="BH47" s="106">
-        <f>BG47-I46</f>
-        <v>10.616666666666607</v>
-      </c>
-      <c r="BI47" s="106">
-        <f>BH47-I46</f>
-        <v>9.7999999999999403</v>
-      </c>
-      <c r="BJ47" s="106">
-        <f>BI47-I46</f>
-        <v>8.9833333333332739</v>
-      </c>
-      <c r="BK47" s="106">
-        <f>BJ47-I46</f>
-        <v>8.1666666666666075</v>
-      </c>
-      <c r="BL47" s="106">
-        <f>BK47-I46</f>
-        <v>7.349999999999941</v>
-      </c>
-      <c r="BM47" s="106">
-        <f>BL47-I46</f>
-        <v>6.5333333333332746</v>
-      </c>
-      <c r="BN47" s="106">
-        <f>BM47-I46</f>
-        <v>5.7166666666666082</v>
-      </c>
-      <c r="BO47" s="106">
-        <f>BN47-I46</f>
-        <v>4.8999999999999417</v>
-      </c>
-      <c r="BP47" s="106">
-        <f>BO47-I46</f>
-        <v>4.0833333333332753</v>
-      </c>
-      <c r="BQ47" s="106">
-        <f>BP47-I46</f>
-        <v>3.2666666666666089</v>
-      </c>
-      <c r="BR47" s="106">
-        <f>BQ47-I46</f>
-        <v>2.4499999999999424</v>
-      </c>
-      <c r="BS47" s="106">
-        <f>BR47-I46</f>
-        <v>1.6333333333332758</v>
-      </c>
-      <c r="BT47" s="106">
-        <f>BS47-I46</f>
-        <v>0.81666666666660914</v>
-      </c>
-      <c r="BV47" s="101"/>
+      <c r="E47" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" s="99" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" s="99" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="99" t="s">
+        <v>73</v>
+      </c>
+      <c r="I47" s="99" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="48" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="101">
+        <f>SUM(E11:E16,E18:E21,E29:E37,E43:E46)</f>
+        <v>49</v>
+      </c>
+      <c r="F48" s="101">
+        <f>SUM(F11:F16,F18:F21,F29:F37,F43:F46)</f>
+        <v>51</v>
+      </c>
+      <c r="G48" s="101">
+        <f>SUM(G11:G16,G18:G21,G29:G37,G43:G46)</f>
+        <v>-2</v>
+      </c>
+      <c r="H48" s="101">
+        <v>60</v>
+      </c>
+      <c r="I48" s="101">
+        <f>E48/H48</f>
+        <v>0.81666666666666665</v>
+      </c>
       <c r="L48" s="102" t="s">
+        <v>77</v>
+      </c>
+      <c r="M48" s="103">
+        <v>1</v>
+      </c>
+      <c r="N48" s="103">
+        <v>2</v>
+      </c>
+      <c r="O48" s="103">
+        <v>3</v>
+      </c>
+      <c r="P48" s="103">
+        <v>4</v>
+      </c>
+      <c r="Q48" s="103">
+        <v>5</v>
+      </c>
+      <c r="R48" s="103">
+        <v>6</v>
+      </c>
+      <c r="S48" s="103">
+        <v>7</v>
+      </c>
+      <c r="T48" s="103">
+        <v>8</v>
+      </c>
+      <c r="U48" s="103">
+        <v>9</v>
+      </c>
+      <c r="V48" s="103">
+        <v>10</v>
+      </c>
+      <c r="W48" s="103">
+        <v>11</v>
+      </c>
+      <c r="X48" s="103">
+        <v>12</v>
+      </c>
+      <c r="Y48" s="103">
+        <v>13</v>
+      </c>
+      <c r="Z48" s="103">
+        <v>14</v>
+      </c>
+      <c r="AA48" s="103">
+        <v>15</v>
+      </c>
+      <c r="AB48" s="103">
+        <v>16</v>
+      </c>
+      <c r="AC48" s="103">
+        <v>17</v>
+      </c>
+      <c r="AD48" s="103">
+        <v>18</v>
+      </c>
+      <c r="AE48" s="103">
+        <v>19</v>
+      </c>
+      <c r="AF48" s="103">
+        <v>20</v>
+      </c>
+      <c r="AG48" s="103">
+        <v>21</v>
+      </c>
+      <c r="AH48" s="103">
+        <v>22</v>
+      </c>
+      <c r="AI48" s="103">
+        <v>23</v>
+      </c>
+      <c r="AJ48" s="103">
+        <v>24</v>
+      </c>
+      <c r="AK48" s="103">
+        <v>25</v>
+      </c>
+      <c r="AL48" s="103">
+        <v>26</v>
+      </c>
+      <c r="AM48" s="103">
+        <v>27</v>
+      </c>
+      <c r="AN48" s="103">
+        <v>28</v>
+      </c>
+      <c r="AO48" s="103">
         <v>29</v>
       </c>
-      <c r="M48" s="105">
-        <f>E46</f>
+      <c r="AP48" s="103">
+        <v>30</v>
+      </c>
+      <c r="AQ48" s="103">
+        <v>31</v>
+      </c>
+      <c r="AR48" s="103">
+        <v>32</v>
+      </c>
+      <c r="AS48" s="103">
+        <v>33</v>
+      </c>
+      <c r="AT48" s="103">
+        <v>34</v>
+      </c>
+      <c r="AU48" s="103">
+        <v>35</v>
+      </c>
+      <c r="AV48" s="103">
+        <v>36</v>
+      </c>
+      <c r="AW48" s="103">
+        <v>37</v>
+      </c>
+      <c r="AX48" s="103">
+        <v>38</v>
+      </c>
+      <c r="AY48" s="103">
+        <v>39</v>
+      </c>
+      <c r="AZ48" s="103">
+        <v>40</v>
+      </c>
+      <c r="BA48" s="103">
+        <v>41</v>
+      </c>
+      <c r="BB48" s="103">
+        <v>42</v>
+      </c>
+      <c r="BC48" s="103">
+        <v>43</v>
+      </c>
+      <c r="BD48" s="103">
+        <v>44</v>
+      </c>
+      <c r="BE48" s="103">
+        <v>45</v>
+      </c>
+      <c r="BF48" s="103">
+        <v>46</v>
+      </c>
+      <c r="BG48" s="103">
+        <v>47</v>
+      </c>
+      <c r="BH48" s="103">
+        <v>48</v>
+      </c>
+      <c r="BI48" s="103">
         <v>49</v>
       </c>
-      <c r="N48" s="105">
-        <f t="shared" ref="N48:BT48" si="11">M50</f>
+      <c r="BJ48" s="103">
+        <v>50</v>
+      </c>
+      <c r="BK48" s="103">
+        <v>51</v>
+      </c>
+      <c r="BL48" s="103">
+        <v>52</v>
+      </c>
+      <c r="BM48" s="103">
+        <v>53</v>
+      </c>
+      <c r="BN48" s="103">
+        <v>54</v>
+      </c>
+      <c r="BO48" s="103">
+        <v>55</v>
+      </c>
+      <c r="BP48" s="103">
+        <v>56</v>
+      </c>
+      <c r="BQ48" s="103">
+        <v>57</v>
+      </c>
+      <c r="BR48" s="103">
+        <v>58</v>
+      </c>
+      <c r="BS48" s="103">
+        <v>59</v>
+      </c>
+      <c r="BT48" s="103">
+        <v>60</v>
+      </c>
+      <c r="BV48" s="100" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="3:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H49" s="104" t="s">
+        <v>78</v>
+      </c>
+      <c r="L49" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="M49" s="105">
+        <f>E48</f>
         <v>49</v>
       </c>
-      <c r="O48" s="105">
+      <c r="N49" s="106">
+        <f>M49-I48</f>
+        <v>48.18333333333333</v>
+      </c>
+      <c r="O49" s="106">
+        <f>N49-I48</f>
+        <v>47.36666666666666</v>
+      </c>
+      <c r="P49" s="106">
+        <f>O49-I48</f>
+        <v>46.54999999999999</v>
+      </c>
+      <c r="Q49" s="106">
+        <f>P49-I48</f>
+        <v>45.73333333333332</v>
+      </c>
+      <c r="R49" s="106">
+        <f>Q49-I48</f>
+        <v>44.91666666666665</v>
+      </c>
+      <c r="S49" s="106">
+        <f>R49-I48</f>
+        <v>44.09999999999998</v>
+      </c>
+      <c r="T49" s="106">
+        <f>S49-I48</f>
+        <v>43.28333333333331</v>
+      </c>
+      <c r="U49" s="106">
+        <f>T49-I48</f>
+        <v>42.46666666666664</v>
+      </c>
+      <c r="V49" s="106">
+        <f>U49-I48</f>
+        <v>41.64999999999997</v>
+      </c>
+      <c r="W49" s="106">
+        <f>V49-I48</f>
+        <v>40.8333333333333</v>
+      </c>
+      <c r="X49" s="106">
+        <f>W49-I48</f>
+        <v>40.01666666666663</v>
+      </c>
+      <c r="Y49" s="106">
+        <f>X49-I48</f>
+        <v>39.19999999999996</v>
+      </c>
+      <c r="Z49" s="106">
+        <f>Y49-I48</f>
+        <v>38.38333333333329</v>
+      </c>
+      <c r="AA49" s="106">
+        <f>Z49-I48</f>
+        <v>37.56666666666662</v>
+      </c>
+      <c r="AB49" s="106">
+        <f>AA49-I48</f>
+        <v>36.74999999999995</v>
+      </c>
+      <c r="AC49" s="106">
+        <f>AB49-I48</f>
+        <v>35.93333333333328</v>
+      </c>
+      <c r="AD49" s="106">
+        <f>AC49-I48</f>
+        <v>35.11666666666661</v>
+      </c>
+      <c r="AE49" s="106">
+        <f>AD49-I48</f>
+        <v>34.29999999999994</v>
+      </c>
+      <c r="AF49" s="106">
+        <f>AE49-I48</f>
+        <v>33.48333333333327</v>
+      </c>
+      <c r="AG49" s="106">
+        <f>AF49-I48</f>
+        <v>32.6666666666666</v>
+      </c>
+      <c r="AH49" s="106">
+        <f>AG49-I48</f>
+        <v>31.849999999999934</v>
+      </c>
+      <c r="AI49" s="106">
+        <f>AH49-I48</f>
+        <v>31.033333333333267</v>
+      </c>
+      <c r="AJ49" s="106">
+        <f>AI49-I48</f>
+        <v>30.216666666666601</v>
+      </c>
+      <c r="AK49" s="106">
+        <f>AJ49-I48</f>
+        <v>29.399999999999935</v>
+      </c>
+      <c r="AL49" s="106">
+        <f>AK49-I48</f>
+        <v>28.583333333333268</v>
+      </c>
+      <c r="AM49" s="106">
+        <f>AL49-I48</f>
+        <v>27.766666666666602</v>
+      </c>
+      <c r="AN49" s="106">
+        <f>AM49-I48</f>
+        <v>26.949999999999935</v>
+      </c>
+      <c r="AO49" s="106">
+        <f>AN49-I48</f>
+        <v>26.133333333333269</v>
+      </c>
+      <c r="AP49" s="106">
+        <f>AO49-I48</f>
+        <v>25.316666666666602</v>
+      </c>
+      <c r="AQ49" s="106">
+        <f>AP49-I48</f>
+        <v>24.499999999999936</v>
+      </c>
+      <c r="AR49" s="106">
+        <f>AQ49-I48</f>
+        <v>23.68333333333327</v>
+      </c>
+      <c r="AS49" s="106">
+        <f>AR49-I48</f>
+        <v>22.866666666666603</v>
+      </c>
+      <c r="AT49" s="106">
+        <f>AS49-I48</f>
+        <v>22.049999999999937</v>
+      </c>
+      <c r="AU49" s="106">
+        <f>AT49-I48</f>
+        <v>21.23333333333327</v>
+      </c>
+      <c r="AV49" s="106">
+        <f>AU49-I48</f>
+        <v>20.416666666666604</v>
+      </c>
+      <c r="AW49" s="106">
+        <f>AV49-I48</f>
+        <v>19.599999999999937</v>
+      </c>
+      <c r="AX49" s="106">
+        <f>AW49-I48</f>
+        <v>18.783333333333271</v>
+      </c>
+      <c r="AY49" s="106">
+        <f>AX49-I48</f>
+        <v>17.966666666666605</v>
+      </c>
+      <c r="AZ49" s="106">
+        <f>AY49-I48</f>
+        <v>17.149999999999938</v>
+      </c>
+      <c r="BA49" s="106">
+        <f>AZ49-I48</f>
+        <v>16.333333333333272</v>
+      </c>
+      <c r="BB49" s="106">
+        <f>BA49-I48</f>
+        <v>15.516666666666605</v>
+      </c>
+      <c r="BC49" s="106">
+        <f>BB49-I48</f>
+        <v>14.699999999999939</v>
+      </c>
+      <c r="BD49" s="106">
+        <f>BC49-I48</f>
+        <v>13.883333333333272</v>
+      </c>
+      <c r="BE49" s="106">
+        <f>BD49-I48</f>
+        <v>13.066666666666606</v>
+      </c>
+      <c r="BF49" s="106">
+        <f>BE49-I48</f>
+        <v>12.24999999999994</v>
+      </c>
+      <c r="BG49" s="106">
+        <f>BF49-I48</f>
+        <v>11.433333333333273</v>
+      </c>
+      <c r="BH49" s="106">
+        <f>BG49-I48</f>
+        <v>10.616666666666607</v>
+      </c>
+      <c r="BI49" s="106">
+        <f>BH49-I48</f>
+        <v>9.7999999999999403</v>
+      </c>
+      <c r="BJ49" s="106">
+        <f>BI49-I48</f>
+        <v>8.9833333333332739</v>
+      </c>
+      <c r="BK49" s="106">
+        <f>BJ49-I48</f>
+        <v>8.1666666666666075</v>
+      </c>
+      <c r="BL49" s="106">
+        <f>BK49-I48</f>
+        <v>7.349999999999941</v>
+      </c>
+      <c r="BM49" s="106">
+        <f>BL49-I48</f>
+        <v>6.5333333333332746</v>
+      </c>
+      <c r="BN49" s="106">
+        <f>BM49-I48</f>
+        <v>5.7166666666666082</v>
+      </c>
+      <c r="BO49" s="106">
+        <f>BN49-I48</f>
+        <v>4.8999999999999417</v>
+      </c>
+      <c r="BP49" s="106">
+        <f>BO49-I48</f>
+        <v>4.0833333333332753</v>
+      </c>
+      <c r="BQ49" s="106">
+        <f>BP49-I48</f>
+        <v>3.2666666666666089</v>
+      </c>
+      <c r="BR49" s="106">
+        <f>BQ49-I48</f>
+        <v>2.4499999999999424</v>
+      </c>
+      <c r="BS49" s="106">
+        <f>BR49-I48</f>
+        <v>1.6333333333332758</v>
+      </c>
+      <c r="BT49" s="106">
+        <f>BS49-I48</f>
+        <v>0.81666666666660914</v>
+      </c>
+      <c r="BV49" s="101"/>
+    </row>
+    <row r="50" spans="3:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L50" s="102" t="s">
+        <v>29</v>
+      </c>
+      <c r="M50" s="105">
+        <f>E48</f>
+        <v>49</v>
+      </c>
+      <c r="N50" s="105">
+        <f t="shared" ref="N50:BT50" si="11">M52</f>
+        <v>49</v>
+      </c>
+      <c r="O50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="P48" s="105">
+      <c r="P50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="Q48" s="105">
+      <c r="Q50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="R48" s="105">
+      <c r="R50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="S48" s="105">
+      <c r="S50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="T48" s="105">
+      <c r="T50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="U48" s="105">
+      <c r="U50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="V48" s="105">
+      <c r="V50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="W48" s="105">
+      <c r="W50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="X48" s="105">
+      <c r="X50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="Y48" s="105">
+      <c r="Y50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="Z48" s="105">
+      <c r="Z50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AA48" s="105">
+      <c r="AA50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AB48" s="105">
+      <c r="AB50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AC48" s="105">
+      <c r="AC50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AD48" s="105">
+      <c r="AD50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AE48" s="105">
+      <c r="AE50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AF48" s="105">
+      <c r="AF50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AG48" s="105">
+      <c r="AG50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AH48" s="105">
+      <c r="AH50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AI48" s="105">
+      <c r="AI50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AJ48" s="105">
+      <c r="AJ50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AK48" s="105">
+      <c r="AK50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AL48" s="105">
+      <c r="AL50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AM48" s="105">
+      <c r="AM50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AN48" s="105">
+      <c r="AN50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AO48" s="105">
+      <c r="AO50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AP48" s="105">
+      <c r="AP50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AQ48" s="105">
+      <c r="AQ50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AR48" s="105">
+      <c r="AR50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AS48" s="105">
+      <c r="AS50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AT48" s="105">
+      <c r="AT50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AU48" s="105">
+      <c r="AU50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AV48" s="105">
+      <c r="AV50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AW48" s="105">
+      <c r="AW50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AX48" s="105">
+      <c r="AX50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AY48" s="105">
+      <c r="AY50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="AZ48" s="105">
+      <c r="AZ50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BA48" s="105">
+      <c r="BA50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BB48" s="105">
+      <c r="BB50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BC48" s="105">
+      <c r="BC50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BD48" s="105">
+      <c r="BD50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BE48" s="105">
+      <c r="BE50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BF48" s="105">
+      <c r="BF50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BG48" s="105">
+      <c r="BG50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BH48" s="105">
+      <c r="BH50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BI48" s="105">
+      <c r="BI50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BJ48" s="105">
+      <c r="BJ50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BK48" s="105">
+      <c r="BK50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BL48" s="105">
+      <c r="BL50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BM48" s="105">
+      <c r="BM50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BN48" s="105">
+      <c r="BN50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BO48" s="105">
+      <c r="BO50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BP48" s="105">
+      <c r="BP50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BQ48" s="105">
+      <c r="BQ50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BR48" s="105">
+      <c r="BR50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BS48" s="105">
+      <c r="BS50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BT48" s="105">
+      <c r="BT50" s="105">
         <f t="shared" si="11"/>
         <v>49</v>
       </c>
-      <c r="BV48" s="101">
-        <f t="shared" ref="BV48:BV50" si="12">SUM(M48:BT48)</f>
+      <c r="BV50" s="101">
+        <f t="shared" ref="BV50:BV52" si="12">SUM(M50:BT50)</f>
         <v>2940</v>
       </c>
     </row>
-    <row r="49" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K49" s="107" t="s">
+    <row r="51" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K51" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="L49" s="102" t="s">
+      <c r="L51" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="M49" s="57"/>
-      <c r="N49" s="57"/>
-      <c r="O49" s="57"/>
-      <c r="P49" s="57"/>
-      <c r="Q49" s="57"/>
-      <c r="R49" s="57"/>
-      <c r="S49" s="57"/>
-      <c r="T49" s="57"/>
-      <c r="U49" s="57"/>
-      <c r="V49" s="57"/>
-      <c r="W49" s="57"/>
-      <c r="X49" s="57"/>
-      <c r="Y49" s="57"/>
-      <c r="Z49" s="57"/>
-      <c r="AA49" s="57"/>
-      <c r="AB49" s="57"/>
-      <c r="AC49" s="57"/>
-      <c r="AD49" s="57"/>
-      <c r="AE49" s="57"/>
-      <c r="AF49" s="57"/>
-      <c r="AG49" s="57"/>
-      <c r="AH49" s="57"/>
-      <c r="AI49" s="57"/>
-      <c r="AJ49" s="57"/>
-      <c r="AK49" s="57"/>
-      <c r="AL49" s="57"/>
-      <c r="AM49" s="57"/>
-      <c r="AN49" s="57"/>
-      <c r="AO49" s="57"/>
-      <c r="AP49" s="57"/>
-      <c r="AQ49" s="57"/>
-      <c r="AR49" s="57"/>
-      <c r="AS49" s="57"/>
-      <c r="AT49" s="57"/>
-      <c r="AU49" s="57"/>
-      <c r="AV49" s="57"/>
-      <c r="AW49" s="57"/>
-      <c r="AX49" s="57"/>
-      <c r="AY49" s="57"/>
-      <c r="AZ49" s="57"/>
-      <c r="BA49" s="57"/>
-      <c r="BB49" s="57"/>
-      <c r="BC49" s="57"/>
-      <c r="BD49" s="57"/>
-      <c r="BE49" s="57"/>
-      <c r="BF49" s="57"/>
-      <c r="BG49" s="57"/>
-      <c r="BH49" s="57"/>
-      <c r="BI49" s="57"/>
-      <c r="BJ49" s="57"/>
-      <c r="BK49" s="57"/>
-      <c r="BL49" s="57"/>
-      <c r="BM49" s="57"/>
-      <c r="BN49" s="57"/>
-      <c r="BO49" s="57"/>
-      <c r="BP49" s="57"/>
-      <c r="BQ49" s="57"/>
-      <c r="BR49" s="57"/>
-      <c r="BS49" s="57"/>
-      <c r="BT49" s="57"/>
-      <c r="BV49" s="101">
+      <c r="M51" s="57"/>
+      <c r="N51" s="57"/>
+      <c r="O51" s="57"/>
+      <c r="P51" s="57"/>
+      <c r="Q51" s="57"/>
+      <c r="R51" s="57"/>
+      <c r="S51" s="57"/>
+      <c r="T51" s="57"/>
+      <c r="U51" s="57"/>
+      <c r="V51" s="57"/>
+      <c r="W51" s="57"/>
+      <c r="X51" s="57"/>
+      <c r="Y51" s="57"/>
+      <c r="Z51" s="57"/>
+      <c r="AA51" s="57"/>
+      <c r="AB51" s="57"/>
+      <c r="AC51" s="57"/>
+      <c r="AD51" s="57"/>
+      <c r="AE51" s="57"/>
+      <c r="AF51" s="57"/>
+      <c r="AG51" s="57"/>
+      <c r="AH51" s="57"/>
+      <c r="AI51" s="57"/>
+      <c r="AJ51" s="57"/>
+      <c r="AK51" s="57"/>
+      <c r="AL51" s="57"/>
+      <c r="AM51" s="57"/>
+      <c r="AN51" s="57"/>
+      <c r="AO51" s="57"/>
+      <c r="AP51" s="57"/>
+      <c r="AQ51" s="57"/>
+      <c r="AR51" s="57"/>
+      <c r="AS51" s="57"/>
+      <c r="AT51" s="57"/>
+      <c r="AU51" s="57"/>
+      <c r="AV51" s="57"/>
+      <c r="AW51" s="57"/>
+      <c r="AX51" s="57"/>
+      <c r="AY51" s="57"/>
+      <c r="AZ51" s="57"/>
+      <c r="BA51" s="57"/>
+      <c r="BB51" s="57"/>
+      <c r="BC51" s="57"/>
+      <c r="BD51" s="57"/>
+      <c r="BE51" s="57"/>
+      <c r="BF51" s="57"/>
+      <c r="BG51" s="57"/>
+      <c r="BH51" s="57"/>
+      <c r="BI51" s="57"/>
+      <c r="BJ51" s="57"/>
+      <c r="BK51" s="57"/>
+      <c r="BL51" s="57"/>
+      <c r="BM51" s="57"/>
+      <c r="BN51" s="57"/>
+      <c r="BO51" s="57"/>
+      <c r="BP51" s="57"/>
+      <c r="BQ51" s="57"/>
+      <c r="BR51" s="57"/>
+      <c r="BS51" s="57"/>
+      <c r="BT51" s="57"/>
+      <c r="BV51" s="101">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L50" s="102" t="s">
+    <row r="52" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L52" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M50" s="105">
-        <f t="shared" ref="M50:BT50" si="13">M48-M49</f>
+      <c r="M52" s="105">
+        <f t="shared" ref="M52:BT52" si="13">M50-M51</f>
         <v>49</v>
       </c>
-      <c r="N50" s="105">
+      <c r="N52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="O50" s="105">
+      <c r="O52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="P50" s="105">
+      <c r="P52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="Q50" s="105">
+      <c r="Q52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="R50" s="105">
+      <c r="R52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="S50" s="105">
+      <c r="S52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="T50" s="105">
+      <c r="T52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="U50" s="105">
+      <c r="U52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="V50" s="105">
+      <c r="V52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="W50" s="105">
+      <c r="W52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="X50" s="105">
+      <c r="X52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="Y50" s="105">
+      <c r="Y52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="Z50" s="105">
+      <c r="Z52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AA50" s="105">
+      <c r="AA52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AB50" s="105">
+      <c r="AB52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AC50" s="105">
+      <c r="AC52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AD50" s="105">
+      <c r="AD52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AE50" s="105">
+      <c r="AE52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AF50" s="105">
+      <c r="AF52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AG50" s="105">
+      <c r="AG52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AH50" s="105">
+      <c r="AH52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AI50" s="105">
+      <c r="AI52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AJ50" s="105">
+      <c r="AJ52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AK50" s="105">
+      <c r="AK52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AL50" s="105">
+      <c r="AL52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AM50" s="105">
+      <c r="AM52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AN50" s="105">
+      <c r="AN52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AO50" s="105">
+      <c r="AO52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AP50" s="105">
+      <c r="AP52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AQ50" s="105">
+      <c r="AQ52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AR50" s="105">
+      <c r="AR52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AS50" s="105">
+      <c r="AS52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AT50" s="105">
+      <c r="AT52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AU50" s="105">
+      <c r="AU52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AV50" s="105">
+      <c r="AV52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AW50" s="105">
+      <c r="AW52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AX50" s="105">
+      <c r="AX52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AY50" s="105">
+      <c r="AY52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="AZ50" s="105">
+      <c r="AZ52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BA50" s="105">
+      <c r="BA52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BB50" s="105">
+      <c r="BB52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BC50" s="105">
+      <c r="BC52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BD50" s="105">
+      <c r="BD52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BE50" s="105">
+      <c r="BE52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BF50" s="105">
+      <c r="BF52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BG50" s="105">
+      <c r="BG52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BH50" s="105">
+      <c r="BH52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BI50" s="105">
+      <c r="BI52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BJ50" s="105">
+      <c r="BJ52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BK50" s="105">
+      <c r="BK52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BL50" s="105">
+      <c r="BL52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BM50" s="105">
+      <c r="BM52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BN50" s="105">
+      <c r="BN52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BO50" s="105">
+      <c r="BO52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BP50" s="105">
+      <c r="BP52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BQ50" s="105">
+      <c r="BQ52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BR50" s="105">
+      <c r="BR52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BS50" s="105">
+      <c r="BS52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BT50" s="105">
+      <c r="BT52" s="105">
         <f t="shared" si="13"/>
         <v>49</v>
       </c>
-      <c r="BV50" s="101">
+      <c r="BV52" s="101">
         <f t="shared" si="12"/>
         <v>2940</v>
       </c>
     </row>
-    <row r="51" spans="3:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="3:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="3:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E54" s="203" t="s">
+    <row r="53" spans="3:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="3:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="3:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E56" s="203" t="s">
         <v>83</v>
       </c>
-      <c r="F54" s="167"/>
-      <c r="G54" s="167"/>
-      <c r="H54" s="167"/>
-      <c r="I54" s="167"/>
-      <c r="J54" s="167"/>
-      <c r="K54" s="167"/>
-      <c r="L54" s="167"/>
-      <c r="M54" s="167"/>
-      <c r="N54" s="167"/>
-      <c r="O54" s="167"/>
-      <c r="P54" s="167"/>
-      <c r="Q54" s="167"/>
-      <c r="R54" s="167"/>
-      <c r="S54" s="167"/>
-      <c r="T54" s="167"/>
-      <c r="U54" s="167"/>
-      <c r="V54" s="167"/>
-      <c r="W54" s="167"/>
-      <c r="X54" s="167"/>
-      <c r="Y54" s="167"/>
-      <c r="Z54" s="167"/>
-      <c r="AA54" s="167"/>
-      <c r="AB54" s="167"/>
-      <c r="AC54" s="167"/>
-      <c r="AD54" s="167"/>
-      <c r="AE54" s="167"/>
-      <c r="AF54" s="167"/>
-      <c r="AG54" s="167"/>
-      <c r="AH54" s="167"/>
-      <c r="AI54" s="167"/>
-      <c r="AJ54" s="167"/>
-      <c r="AK54" s="167"/>
-      <c r="AL54" s="167"/>
-      <c r="AM54" s="167"/>
-      <c r="AN54" s="167"/>
-      <c r="AO54" s="167"/>
-      <c r="AP54" s="167"/>
-      <c r="AQ54" s="167"/>
-      <c r="AR54" s="167"/>
-      <c r="AS54" s="167"/>
-      <c r="AT54" s="167"/>
-      <c r="AU54" s="167"/>
-      <c r="AV54" s="167"/>
-      <c r="AW54" s="167"/>
-      <c r="AX54" s="167"/>
-      <c r="AY54" s="167"/>
-      <c r="AZ54" s="167"/>
-      <c r="BA54" s="167"/>
-      <c r="BB54" s="168"/>
+      <c r="F56" s="186"/>
+      <c r="G56" s="186"/>
+      <c r="H56" s="186"/>
+      <c r="I56" s="186"/>
+      <c r="J56" s="186"/>
+      <c r="K56" s="186"/>
+      <c r="L56" s="186"/>
+      <c r="M56" s="186"/>
+      <c r="N56" s="186"/>
+      <c r="O56" s="186"/>
+      <c r="P56" s="186"/>
+      <c r="Q56" s="186"/>
+      <c r="R56" s="186"/>
+      <c r="S56" s="186"/>
+      <c r="T56" s="186"/>
+      <c r="U56" s="186"/>
+      <c r="V56" s="186"/>
+      <c r="W56" s="186"/>
+      <c r="X56" s="186"/>
+      <c r="Y56" s="186"/>
+      <c r="Z56" s="186"/>
+      <c r="AA56" s="186"/>
+      <c r="AB56" s="186"/>
+      <c r="AC56" s="186"/>
+      <c r="AD56" s="186"/>
+      <c r="AE56" s="186"/>
+      <c r="AF56" s="186"/>
+      <c r="AG56" s="186"/>
+      <c r="AH56" s="186"/>
+      <c r="AI56" s="186"/>
+      <c r="AJ56" s="186"/>
+      <c r="AK56" s="186"/>
+      <c r="AL56" s="186"/>
+      <c r="AM56" s="186"/>
+      <c r="AN56" s="186"/>
+      <c r="AO56" s="186"/>
+      <c r="AP56" s="186"/>
+      <c r="AQ56" s="186"/>
+      <c r="AR56" s="186"/>
+      <c r="AS56" s="186"/>
+      <c r="AT56" s="186"/>
+      <c r="AU56" s="186"/>
+      <c r="AV56" s="186"/>
+      <c r="AW56" s="186"/>
+      <c r="AX56" s="186"/>
+      <c r="AY56" s="186"/>
+      <c r="AZ56" s="186"/>
+      <c r="BA56" s="186"/>
+      <c r="BB56" s="187"/>
     </row>
-    <row r="55" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="3:74" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C59" s="108"/>
-      <c r="D59" s="108"/>
+    <row r="59" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="3:74" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C61" s="108"/>
+      <c r="D61" s="108"/>
     </row>
-    <row r="60" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18427,16 +18620,11 @@
     <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="E54:BB54"/>
+    <mergeCell ref="E56:BB56"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
     <mergeCell ref="BP8:BT8"/>
@@ -18452,6 +18640,13 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18467,8 +18662,8 @@
   </sheetPr>
   <dimension ref="B1:K999"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18547,8 +18742,8 @@
       </c>
     </row>
     <row r="4" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="161">
-        <v>3</v>
+      <c r="B4" s="161" t="s">
+        <v>228</v>
       </c>
       <c r="C4" s="115" t="s">
         <v>155</v>
@@ -20240,7 +20435,7 @@
   </sheetPr>
   <dimension ref="B1:G1003"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update of user and operator personal info completed
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA61E50-8956-4F82-952F-7BADE9288C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924F84E4-D806-4D05-846D-1F57D799F6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -836,7 +836,7 @@
     <t>ScoreBoard</t>
   </si>
   <si>
-    <t>Updating personal info user and operator</t>
+    <t>Updating personal info of user and operator</t>
   </si>
 </sst>
 </file>
@@ -2585,11 +2585,53 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2620,48 +2662,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5566,184 +5566,184 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>57.033333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>56.066666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57</c:v>
+                  <c:v>55.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56</c:v>
+                  <c:v>54.133333333333326</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55</c:v>
+                  <c:v>53.166666666666657</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>52.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>51.23333333333332</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52</c:v>
+                  <c:v>50.266666666666652</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51</c:v>
+                  <c:v>49.299999999999983</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>48.333333333333314</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49</c:v>
+                  <c:v>47.366666666666646</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>48</c:v>
+                  <c:v>46.399999999999977</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47</c:v>
+                  <c:v>45.433333333333309</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>46</c:v>
+                  <c:v>44.46666666666664</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>45</c:v>
+                  <c:v>43.499999999999972</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>44</c:v>
+                  <c:v>42.533333333333303</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43</c:v>
+                  <c:v>41.566666666666634</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42</c:v>
+                  <c:v>40.599999999999966</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41</c:v>
+                  <c:v>39.633333333333297</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>40</c:v>
+                  <c:v>38.666666666666629</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>39</c:v>
+                  <c:v>37.69999999999996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>38</c:v>
+                  <c:v>36.733333333333292</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>37</c:v>
+                  <c:v>35.766666666666623</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>36</c:v>
+                  <c:v>34.799999999999955</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>35</c:v>
+                  <c:v>33.833333333333286</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>34</c:v>
+                  <c:v>32.866666666666617</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>33</c:v>
+                  <c:v>31.899999999999952</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>32</c:v>
+                  <c:v>30.933333333333287</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>31</c:v>
+                  <c:v>29.966666666666622</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30</c:v>
+                  <c:v>28.999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>29</c:v>
+                  <c:v>28.033333333333292</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>28</c:v>
+                  <c:v>27.066666666666627</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>27</c:v>
+                  <c:v>26.099999999999962</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>26</c:v>
+                  <c:v>25.133333333333297</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>25</c:v>
+                  <c:v>24.166666666666632</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>24</c:v>
+                  <c:v>23.199999999999967</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>23</c:v>
+                  <c:v>22.233333333333302</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22</c:v>
+                  <c:v>21.266666666666637</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>21</c:v>
+                  <c:v>20.299999999999972</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>20</c:v>
+                  <c:v>19.333333333333307</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>19</c:v>
+                  <c:v>18.366666666666642</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>18</c:v>
+                  <c:v>17.399999999999977</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>17</c:v>
+                  <c:v>16.433333333333312</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>16</c:v>
+                  <c:v>15.466666666666645</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>15</c:v>
+                  <c:v>14.499999999999979</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>14</c:v>
+                  <c:v>13.533333333333312</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>13</c:v>
+                  <c:v>12.566666666666645</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>12</c:v>
+                  <c:v>11.599999999999978</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>11</c:v>
+                  <c:v>10.633333333333312</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>10</c:v>
+                  <c:v>9.6666666666666448</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>9</c:v>
+                  <c:v>8.699999999999978</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>8</c:v>
+                  <c:v>7.7333333333333112</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>7</c:v>
+                  <c:v>6.7666666666666444</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>6</c:v>
+                  <c:v>5.7999999999999776</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>5</c:v>
+                  <c:v>4.8333333333333108</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4</c:v>
+                  <c:v>3.866666666666644</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3</c:v>
+                  <c:v>2.8999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2</c:v>
+                  <c:v>1.9333333333333105</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1</c:v>
+                  <c:v>0.9666666666666438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5977,184 +5977,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>60</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7059,19 +7059,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="171" t="str">
+      <c r="BK2" s="189" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="172"/>
-      <c r="BM2" s="172"/>
-      <c r="BN2" s="172"/>
-      <c r="BO2" s="172"/>
-      <c r="BP2" s="172"/>
-      <c r="BQ2" s="172"/>
-      <c r="BR2" s="172"/>
-      <c r="BS2" s="172"/>
-      <c r="BT2" s="172"/>
+      <c r="BL2" s="190"/>
+      <c r="BM2" s="190"/>
+      <c r="BN2" s="190"/>
+      <c r="BO2" s="190"/>
+      <c r="BP2" s="190"/>
+      <c r="BQ2" s="190"/>
+      <c r="BR2" s="190"/>
+      <c r="BS2" s="190"/>
+      <c r="BT2" s="190"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -7099,7 +7099,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="173" t="s">
+      <c r="K4" s="191" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7176,7 +7176,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="174"/>
+      <c r="K5" s="192"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7251,7 +7251,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="174"/>
+      <c r="K6" s="192"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7326,7 +7326,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="174"/>
+      <c r="K7" s="192"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7401,7 +7401,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="175"/>
+      <c r="K8" s="193"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7467,124 +7467,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="176" t="s">
+      <c r="B9" s="194" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="178" t="s">
+      <c r="C9" s="196" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="180" t="s">
+      <c r="D9" s="198" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="182" t="s">
+      <c r="E9" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="183"/>
-      <c r="G9" s="184"/>
-      <c r="H9" s="185" t="s">
+      <c r="F9" s="201"/>
+      <c r="G9" s="202"/>
+      <c r="H9" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="190" t="s">
+      <c r="I9" s="171" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="192" t="s">
+      <c r="J9" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="194" t="s">
+      <c r="K9" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="195" t="s">
+      <c r="L9" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="197" t="s">
+      <c r="M9" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="169"/>
-      <c r="O9" s="169"/>
-      <c r="P9" s="169"/>
-      <c r="Q9" s="198"/>
-      <c r="R9" s="199" t="s">
+      <c r="N9" s="179"/>
+      <c r="O9" s="179"/>
+      <c r="P9" s="179"/>
+      <c r="Q9" s="180"/>
+      <c r="R9" s="181" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="169"/>
-      <c r="T9" s="169"/>
-      <c r="U9" s="169"/>
-      <c r="V9" s="198"/>
-      <c r="W9" s="199" t="s">
+      <c r="S9" s="179"/>
+      <c r="T9" s="179"/>
+      <c r="U9" s="179"/>
+      <c r="V9" s="180"/>
+      <c r="W9" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="169"/>
-      <c r="Y9" s="169"/>
-      <c r="Z9" s="169"/>
-      <c r="AA9" s="170"/>
-      <c r="AB9" s="200" t="s">
+      <c r="X9" s="179"/>
+      <c r="Y9" s="179"/>
+      <c r="Z9" s="179"/>
+      <c r="AA9" s="182"/>
+      <c r="AB9" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="169"/>
-      <c r="AD9" s="169"/>
-      <c r="AE9" s="169"/>
-      <c r="AF9" s="198"/>
-      <c r="AG9" s="201" t="s">
+      <c r="AC9" s="179"/>
+      <c r="AD9" s="179"/>
+      <c r="AE9" s="179"/>
+      <c r="AF9" s="180"/>
+      <c r="AG9" s="184" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="169"/>
-      <c r="AI9" s="169"/>
-      <c r="AJ9" s="169"/>
-      <c r="AK9" s="198"/>
-      <c r="AL9" s="201" t="s">
+      <c r="AH9" s="179"/>
+      <c r="AI9" s="179"/>
+      <c r="AJ9" s="179"/>
+      <c r="AK9" s="180"/>
+      <c r="AL9" s="184" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="169"/>
-      <c r="AN9" s="169"/>
-      <c r="AO9" s="169"/>
-      <c r="AP9" s="170"/>
-      <c r="AQ9" s="202" t="s">
+      <c r="AM9" s="179"/>
+      <c r="AN9" s="179"/>
+      <c r="AO9" s="179"/>
+      <c r="AP9" s="182"/>
+      <c r="AQ9" s="185" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="169"/>
-      <c r="AS9" s="169"/>
-      <c r="AT9" s="169"/>
-      <c r="AU9" s="198"/>
-      <c r="AV9" s="203" t="s">
+      <c r="AR9" s="179"/>
+      <c r="AS9" s="179"/>
+      <c r="AT9" s="179"/>
+      <c r="AU9" s="180"/>
+      <c r="AV9" s="186" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="169"/>
-      <c r="AX9" s="169"/>
-      <c r="AY9" s="169"/>
-      <c r="AZ9" s="198"/>
-      <c r="BA9" s="203" t="s">
+      <c r="AW9" s="179"/>
+      <c r="AX9" s="179"/>
+      <c r="AY9" s="179"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="169"/>
-      <c r="BC9" s="169"/>
-      <c r="BD9" s="169"/>
-      <c r="BE9" s="170"/>
-      <c r="BF9" s="204" t="s">
+      <c r="BB9" s="179"/>
+      <c r="BC9" s="179"/>
+      <c r="BD9" s="179"/>
+      <c r="BE9" s="182"/>
+      <c r="BF9" s="187" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="169"/>
-      <c r="BH9" s="169"/>
-      <c r="BI9" s="169"/>
-      <c r="BJ9" s="198"/>
-      <c r="BK9" s="168" t="s">
+      <c r="BG9" s="179"/>
+      <c r="BH9" s="179"/>
+      <c r="BI9" s="179"/>
+      <c r="BJ9" s="180"/>
+      <c r="BK9" s="188" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="169"/>
-      <c r="BM9" s="169"/>
-      <c r="BN9" s="169"/>
-      <c r="BO9" s="198"/>
-      <c r="BP9" s="168" t="s">
+      <c r="BL9" s="179"/>
+      <c r="BM9" s="179"/>
+      <c r="BN9" s="179"/>
+      <c r="BO9" s="180"/>
+      <c r="BP9" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="169"/>
-      <c r="BR9" s="169"/>
-      <c r="BS9" s="169"/>
-      <c r="BT9" s="170"/>
+      <c r="BQ9" s="179"/>
+      <c r="BR9" s="179"/>
+      <c r="BS9" s="179"/>
+      <c r="BT9" s="182"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="177"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="181"/>
+      <c r="B10" s="195"/>
+      <c r="C10" s="197"/>
+      <c r="D10" s="199"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7594,11 +7594,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="186"/>
-      <c r="I10" s="191"/>
-      <c r="J10" s="193"/>
-      <c r="K10" s="193"/>
-      <c r="L10" s="196"/>
+      <c r="H10" s="204"/>
+      <c r="I10" s="172"/>
+      <c r="J10" s="174"/>
+      <c r="K10" s="174"/>
+      <c r="L10" s="177"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11207,80 +11207,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="187" t="str">
+      <c r="B45" s="168" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="188"/>
-      <c r="D45" s="188"/>
-      <c r="E45" s="188"/>
-      <c r="F45" s="188"/>
-      <c r="G45" s="188"/>
-      <c r="H45" s="188"/>
-      <c r="I45" s="188"/>
-      <c r="J45" s="188"/>
-      <c r="K45" s="188"/>
-      <c r="L45" s="188"/>
-      <c r="M45" s="188"/>
-      <c r="N45" s="188"/>
-      <c r="O45" s="188"/>
-      <c r="P45" s="188"/>
-      <c r="Q45" s="188"/>
-      <c r="R45" s="188"/>
-      <c r="S45" s="188"/>
-      <c r="T45" s="188"/>
-      <c r="U45" s="188"/>
-      <c r="V45" s="188"/>
-      <c r="W45" s="188"/>
-      <c r="X45" s="188"/>
-      <c r="Y45" s="188"/>
-      <c r="Z45" s="188"/>
-      <c r="AA45" s="188"/>
-      <c r="AB45" s="188"/>
-      <c r="AC45" s="188"/>
-      <c r="AD45" s="188"/>
-      <c r="AE45" s="188"/>
-      <c r="AF45" s="188"/>
-      <c r="AG45" s="188"/>
-      <c r="AH45" s="188"/>
-      <c r="AI45" s="188"/>
-      <c r="AJ45" s="188"/>
-      <c r="AK45" s="188"/>
-      <c r="AL45" s="188"/>
-      <c r="AM45" s="188"/>
-      <c r="AN45" s="188"/>
-      <c r="AO45" s="188"/>
-      <c r="AP45" s="188"/>
-      <c r="AQ45" s="188"/>
-      <c r="AR45" s="188"/>
-      <c r="AS45" s="188"/>
-      <c r="AT45" s="188"/>
-      <c r="AU45" s="188"/>
-      <c r="AV45" s="188"/>
-      <c r="AW45" s="188"/>
-      <c r="AX45" s="188"/>
-      <c r="AY45" s="188"/>
-      <c r="AZ45" s="188"/>
-      <c r="BA45" s="188"/>
-      <c r="BB45" s="188"/>
-      <c r="BC45" s="188"/>
-      <c r="BD45" s="188"/>
-      <c r="BE45" s="188"/>
-      <c r="BF45" s="188"/>
-      <c r="BG45" s="188"/>
-      <c r="BH45" s="188"/>
-      <c r="BI45" s="188"/>
-      <c r="BJ45" s="188"/>
-      <c r="BK45" s="188"/>
-      <c r="BL45" s="188"/>
-      <c r="BM45" s="188"/>
-      <c r="BN45" s="188"/>
-      <c r="BO45" s="188"/>
-      <c r="BP45" s="188"/>
-      <c r="BQ45" s="188"/>
-      <c r="BR45" s="188"/>
-      <c r="BS45" s="188"/>
-      <c r="BT45" s="189"/>
+      <c r="C45" s="169"/>
+      <c r="D45" s="169"/>
+      <c r="E45" s="169"/>
+      <c r="F45" s="169"/>
+      <c r="G45" s="169"/>
+      <c r="H45" s="169"/>
+      <c r="I45" s="169"/>
+      <c r="J45" s="169"/>
+      <c r="K45" s="169"/>
+      <c r="L45" s="169"/>
+      <c r="M45" s="169"/>
+      <c r="N45" s="169"/>
+      <c r="O45" s="169"/>
+      <c r="P45" s="169"/>
+      <c r="Q45" s="169"/>
+      <c r="R45" s="169"/>
+      <c r="S45" s="169"/>
+      <c r="T45" s="169"/>
+      <c r="U45" s="169"/>
+      <c r="V45" s="169"/>
+      <c r="W45" s="169"/>
+      <c r="X45" s="169"/>
+      <c r="Y45" s="169"/>
+      <c r="Z45" s="169"/>
+      <c r="AA45" s="169"/>
+      <c r="AB45" s="169"/>
+      <c r="AC45" s="169"/>
+      <c r="AD45" s="169"/>
+      <c r="AE45" s="169"/>
+      <c r="AF45" s="169"/>
+      <c r="AG45" s="169"/>
+      <c r="AH45" s="169"/>
+      <c r="AI45" s="169"/>
+      <c r="AJ45" s="169"/>
+      <c r="AK45" s="169"/>
+      <c r="AL45" s="169"/>
+      <c r="AM45" s="169"/>
+      <c r="AN45" s="169"/>
+      <c r="AO45" s="169"/>
+      <c r="AP45" s="169"/>
+      <c r="AQ45" s="169"/>
+      <c r="AR45" s="169"/>
+      <c r="AS45" s="169"/>
+      <c r="AT45" s="169"/>
+      <c r="AU45" s="169"/>
+      <c r="AV45" s="169"/>
+      <c r="AW45" s="169"/>
+      <c r="AX45" s="169"/>
+      <c r="AY45" s="169"/>
+      <c r="AZ45" s="169"/>
+      <c r="BA45" s="169"/>
+      <c r="BB45" s="169"/>
+      <c r="BC45" s="169"/>
+      <c r="BD45" s="169"/>
+      <c r="BE45" s="169"/>
+      <c r="BF45" s="169"/>
+      <c r="BG45" s="169"/>
+      <c r="BH45" s="169"/>
+      <c r="BI45" s="169"/>
+      <c r="BJ45" s="169"/>
+      <c r="BK45" s="169"/>
+      <c r="BL45" s="169"/>
+      <c r="BM45" s="169"/>
+      <c r="BN45" s="169"/>
+      <c r="BO45" s="169"/>
+      <c r="BP45" s="169"/>
+      <c r="BQ45" s="169"/>
+      <c r="BR45" s="169"/>
+      <c r="BS45" s="169"/>
+      <c r="BT45" s="170"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12243,6 +12243,14 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12259,14 +12267,6 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12282,7 +12282,7 @@
   <dimension ref="B1:BV1012"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BK45" sqref="BK45"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12395,7 +12395,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="173" t="s">
+      <c r="K3" s="191" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12472,7 +12472,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="174"/>
+      <c r="K4" s="192"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12546,7 +12546,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="174"/>
+      <c r="K5" s="192"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12620,7 +12620,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="174"/>
+      <c r="K6" s="192"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12695,7 +12695,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="175"/>
+      <c r="K7" s="193"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12761,124 +12761,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="176" t="s">
+      <c r="B8" s="194" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="178" t="s">
+      <c r="C8" s="196" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="180" t="s">
+      <c r="D8" s="198" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="182" t="s">
+      <c r="E8" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="183"/>
-      <c r="G8" s="184"/>
-      <c r="H8" s="185" t="s">
+      <c r="F8" s="201"/>
+      <c r="G8" s="202"/>
+      <c r="H8" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="190" t="s">
+      <c r="I8" s="171" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="192" t="s">
+      <c r="J8" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="194" t="s">
+      <c r="K8" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="195" t="s">
+      <c r="L8" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="197" t="s">
+      <c r="M8" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="169"/>
-      <c r="O8" s="169"/>
-      <c r="P8" s="169"/>
-      <c r="Q8" s="198"/>
-      <c r="R8" s="199" t="s">
+      <c r="N8" s="179"/>
+      <c r="O8" s="179"/>
+      <c r="P8" s="179"/>
+      <c r="Q8" s="180"/>
+      <c r="R8" s="181" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="169"/>
-      <c r="T8" s="169"/>
-      <c r="U8" s="169"/>
-      <c r="V8" s="198"/>
-      <c r="W8" s="199" t="s">
+      <c r="S8" s="179"/>
+      <c r="T8" s="179"/>
+      <c r="U8" s="179"/>
+      <c r="V8" s="180"/>
+      <c r="W8" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="169"/>
-      <c r="Y8" s="169"/>
-      <c r="Z8" s="169"/>
-      <c r="AA8" s="170"/>
-      <c r="AB8" s="200" t="s">
+      <c r="X8" s="179"/>
+      <c r="Y8" s="179"/>
+      <c r="Z8" s="179"/>
+      <c r="AA8" s="182"/>
+      <c r="AB8" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="169"/>
-      <c r="AD8" s="169"/>
-      <c r="AE8" s="169"/>
-      <c r="AF8" s="198"/>
-      <c r="AG8" s="201" t="s">
+      <c r="AC8" s="179"/>
+      <c r="AD8" s="179"/>
+      <c r="AE8" s="179"/>
+      <c r="AF8" s="180"/>
+      <c r="AG8" s="184" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="169"/>
-      <c r="AI8" s="169"/>
-      <c r="AJ8" s="169"/>
-      <c r="AK8" s="198"/>
-      <c r="AL8" s="201" t="s">
+      <c r="AH8" s="179"/>
+      <c r="AI8" s="179"/>
+      <c r="AJ8" s="179"/>
+      <c r="AK8" s="180"/>
+      <c r="AL8" s="184" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="169"/>
-      <c r="AN8" s="169"/>
-      <c r="AO8" s="169"/>
-      <c r="AP8" s="170"/>
-      <c r="AQ8" s="202" t="s">
+      <c r="AM8" s="179"/>
+      <c r="AN8" s="179"/>
+      <c r="AO8" s="179"/>
+      <c r="AP8" s="182"/>
+      <c r="AQ8" s="185" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="169"/>
-      <c r="AS8" s="169"/>
-      <c r="AT8" s="169"/>
-      <c r="AU8" s="198"/>
-      <c r="AV8" s="203" t="s">
+      <c r="AR8" s="179"/>
+      <c r="AS8" s="179"/>
+      <c r="AT8" s="179"/>
+      <c r="AU8" s="180"/>
+      <c r="AV8" s="186" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="169"/>
-      <c r="AX8" s="169"/>
-      <c r="AY8" s="169"/>
-      <c r="AZ8" s="198"/>
-      <c r="BA8" s="203" t="s">
+      <c r="AW8" s="179"/>
+      <c r="AX8" s="179"/>
+      <c r="AY8" s="179"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="169"/>
-      <c r="BC8" s="169"/>
-      <c r="BD8" s="169"/>
-      <c r="BE8" s="170"/>
-      <c r="BF8" s="204" t="s">
+      <c r="BB8" s="179"/>
+      <c r="BC8" s="179"/>
+      <c r="BD8" s="179"/>
+      <c r="BE8" s="182"/>
+      <c r="BF8" s="187" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="169"/>
-      <c r="BH8" s="169"/>
-      <c r="BI8" s="169"/>
-      <c r="BJ8" s="198"/>
-      <c r="BK8" s="168" t="s">
+      <c r="BG8" s="179"/>
+      <c r="BH8" s="179"/>
+      <c r="BI8" s="179"/>
+      <c r="BJ8" s="180"/>
+      <c r="BK8" s="188" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="169"/>
-      <c r="BM8" s="169"/>
-      <c r="BN8" s="169"/>
-      <c r="BO8" s="198"/>
-      <c r="BP8" s="168" t="s">
+      <c r="BL8" s="179"/>
+      <c r="BM8" s="179"/>
+      <c r="BN8" s="179"/>
+      <c r="BO8" s="180"/>
+      <c r="BP8" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="169"/>
-      <c r="BR8" s="169"/>
-      <c r="BS8" s="169"/>
-      <c r="BT8" s="170"/>
+      <c r="BQ8" s="179"/>
+      <c r="BR8" s="179"/>
+      <c r="BS8" s="179"/>
+      <c r="BT8" s="182"/>
     </row>
     <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="177"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="181"/>
+      <c r="B9" s="195"/>
+      <c r="C9" s="197"/>
+      <c r="D9" s="199"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12888,11 +12888,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="186"/>
-      <c r="I9" s="191"/>
-      <c r="J9" s="193"/>
-      <c r="K9" s="193"/>
-      <c r="L9" s="196"/>
+      <c r="H9" s="204"/>
+      <c r="I9" s="172"/>
+      <c r="J9" s="174"/>
+      <c r="K9" s="174"/>
+      <c r="L9" s="177"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -16197,15 +16197,15 @@
       <c r="D42" s="74"/>
       <c r="E42" s="42">
         <f t="shared" ref="E42:G42" si="8">SUM(E43:E46)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F42" s="43">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G42" s="44">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H42" s="75"/>
       <c r="I42" s="76"/>
@@ -16213,7 +16213,7 @@
       <c r="K42" s="77"/>
       <c r="L42" s="49">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>1</v>
       </c>
       <c r="M42" s="50"/>
       <c r="N42" s="51"/>
@@ -16482,14 +16482,14 @@
         <v>262</v>
       </c>
       <c r="E45" s="56">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F45" s="57">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G45" s="58">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H45" s="59">
         <v>4</v>
@@ -16506,7 +16506,7 @@
       </c>
       <c r="L45" s="63">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>1</v>
       </c>
       <c r="M45" s="64"/>
       <c r="N45" s="65"/>
@@ -16679,22 +16679,22 @@
       </c>
       <c r="E48" s="101">
         <f>SUM(E11:E16,E18:E21,E29:E37,E43:E46)</f>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F48" s="101">
         <f>SUM(F11:F16,F18:F21,F29:F37,F43:F46)</f>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G48" s="101">
         <f>SUM(G11:G16,G18:G21,G29:G37,G43:G46)</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="H48" s="101">
         <v>60</v>
       </c>
       <c r="I48" s="101">
         <f>E48/H48</f>
-        <v>1</v>
+        <v>0.96666666666666667</v>
       </c>
       <c r="L48" s="102" t="s">
         <v>77</v>
@@ -16892,243 +16892,243 @@
       </c>
       <c r="M49" s="105">
         <f>E48</f>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N49" s="106">
         <f>M49-I48</f>
-        <v>59</v>
+        <v>57.033333333333331</v>
       </c>
       <c r="O49" s="106">
         <f>N49-I48</f>
-        <v>58</v>
+        <v>56.066666666666663</v>
       </c>
       <c r="P49" s="106">
         <f>O49-I48</f>
-        <v>57</v>
+        <v>55.099999999999994</v>
       </c>
       <c r="Q49" s="106">
         <f>P49-I48</f>
-        <v>56</v>
+        <v>54.133333333333326</v>
       </c>
       <c r="R49" s="106">
         <f>Q49-I48</f>
-        <v>55</v>
+        <v>53.166666666666657</v>
       </c>
       <c r="S49" s="106">
         <f>R49-I48</f>
-        <v>54</v>
+        <v>52.199999999999989</v>
       </c>
       <c r="T49" s="106">
         <f>S49-I48</f>
-        <v>53</v>
+        <v>51.23333333333332</v>
       </c>
       <c r="U49" s="106">
         <f>T49-I48</f>
-        <v>52</v>
+        <v>50.266666666666652</v>
       </c>
       <c r="V49" s="106">
         <f>U49-I48</f>
-        <v>51</v>
+        <v>49.299999999999983</v>
       </c>
       <c r="W49" s="106">
         <f>V49-I48</f>
-        <v>50</v>
+        <v>48.333333333333314</v>
       </c>
       <c r="X49" s="106">
         <f>W49-I48</f>
-        <v>49</v>
+        <v>47.366666666666646</v>
       </c>
       <c r="Y49" s="106">
         <f>X49-I48</f>
-        <v>48</v>
+        <v>46.399999999999977</v>
       </c>
       <c r="Z49" s="106">
         <f>Y49-I48</f>
-        <v>47</v>
+        <v>45.433333333333309</v>
       </c>
       <c r="AA49" s="106">
         <f>Z49-I48</f>
-        <v>46</v>
+        <v>44.46666666666664</v>
       </c>
       <c r="AB49" s="106">
         <f>AA49-I48</f>
-        <v>45</v>
+        <v>43.499999999999972</v>
       </c>
       <c r="AC49" s="106">
         <f>AB49-I48</f>
-        <v>44</v>
+        <v>42.533333333333303</v>
       </c>
       <c r="AD49" s="106">
         <f>AC49-I48</f>
-        <v>43</v>
+        <v>41.566666666666634</v>
       </c>
       <c r="AE49" s="106">
         <f>AD49-I48</f>
-        <v>42</v>
+        <v>40.599999999999966</v>
       </c>
       <c r="AF49" s="106">
         <f>AE49-I48</f>
-        <v>41</v>
+        <v>39.633333333333297</v>
       </c>
       <c r="AG49" s="106">
         <f>AF49-I48</f>
-        <v>40</v>
+        <v>38.666666666666629</v>
       </c>
       <c r="AH49" s="106">
         <f>AG49-I48</f>
-        <v>39</v>
+        <v>37.69999999999996</v>
       </c>
       <c r="AI49" s="106">
         <f>AH49-I48</f>
-        <v>38</v>
+        <v>36.733333333333292</v>
       </c>
       <c r="AJ49" s="106">
         <f>AI49-I48</f>
-        <v>37</v>
+        <v>35.766666666666623</v>
       </c>
       <c r="AK49" s="106">
         <f>AJ49-I48</f>
-        <v>36</v>
+        <v>34.799999999999955</v>
       </c>
       <c r="AL49" s="106">
         <f>AK49-I48</f>
-        <v>35</v>
+        <v>33.833333333333286</v>
       </c>
       <c r="AM49" s="106">
         <f>AL49-I48</f>
-        <v>34</v>
+        <v>32.866666666666617</v>
       </c>
       <c r="AN49" s="106">
         <f>AM49-I48</f>
-        <v>33</v>
+        <v>31.899999999999952</v>
       </c>
       <c r="AO49" s="106">
         <f>AN49-I48</f>
-        <v>32</v>
+        <v>30.933333333333287</v>
       </c>
       <c r="AP49" s="106">
         <f>AO49-I48</f>
-        <v>31</v>
+        <v>29.966666666666622</v>
       </c>
       <c r="AQ49" s="106">
         <f>AP49-I48</f>
-        <v>30</v>
+        <v>28.999999999999957</v>
       </c>
       <c r="AR49" s="106">
         <f>AQ49-I48</f>
-        <v>29</v>
+        <v>28.033333333333292</v>
       </c>
       <c r="AS49" s="106">
         <f>AR49-I48</f>
-        <v>28</v>
+        <v>27.066666666666627</v>
       </c>
       <c r="AT49" s="106">
         <f>AS49-I48</f>
-        <v>27</v>
+        <v>26.099999999999962</v>
       </c>
       <c r="AU49" s="106">
         <f>AT49-I48</f>
-        <v>26</v>
+        <v>25.133333333333297</v>
       </c>
       <c r="AV49" s="106">
         <f>AU49-I48</f>
-        <v>25</v>
+        <v>24.166666666666632</v>
       </c>
       <c r="AW49" s="106">
         <f>AV49-I48</f>
-        <v>24</v>
+        <v>23.199999999999967</v>
       </c>
       <c r="AX49" s="106">
         <f>AW49-I48</f>
-        <v>23</v>
+        <v>22.233333333333302</v>
       </c>
       <c r="AY49" s="106">
         <f>AX49-I48</f>
-        <v>22</v>
+        <v>21.266666666666637</v>
       </c>
       <c r="AZ49" s="106">
         <f>AY49-I48</f>
-        <v>21</v>
+        <v>20.299999999999972</v>
       </c>
       <c r="BA49" s="106">
         <f>AZ49-I48</f>
-        <v>20</v>
+        <v>19.333333333333307</v>
       </c>
       <c r="BB49" s="106">
         <f>BA49-I48</f>
-        <v>19</v>
+        <v>18.366666666666642</v>
       </c>
       <c r="BC49" s="106">
         <f>BB49-I48</f>
-        <v>18</v>
+        <v>17.399999999999977</v>
       </c>
       <c r="BD49" s="106">
         <f>BC49-I48</f>
-        <v>17</v>
+        <v>16.433333333333312</v>
       </c>
       <c r="BE49" s="106">
         <f>BD49-I48</f>
-        <v>16</v>
+        <v>15.466666666666645</v>
       </c>
       <c r="BF49" s="106">
         <f>BE49-I48</f>
-        <v>15</v>
+        <v>14.499999999999979</v>
       </c>
       <c r="BG49" s="106">
         <f>BF49-I48</f>
-        <v>14</v>
+        <v>13.533333333333312</v>
       </c>
       <c r="BH49" s="106">
         <f>BG49-I48</f>
-        <v>13</v>
+        <v>12.566666666666645</v>
       </c>
       <c r="BI49" s="106">
         <f>BH49-I48</f>
-        <v>12</v>
+        <v>11.599999999999978</v>
       </c>
       <c r="BJ49" s="106">
         <f>BI49-I48</f>
-        <v>11</v>
+        <v>10.633333333333312</v>
       </c>
       <c r="BK49" s="106">
         <f>BJ49-I48</f>
-        <v>10</v>
+        <v>9.6666666666666448</v>
       </c>
       <c r="BL49" s="106">
         <f>BK49-I48</f>
-        <v>9</v>
+        <v>8.699999999999978</v>
       </c>
       <c r="BM49" s="106">
         <f>BL49-I48</f>
-        <v>8</v>
+        <v>7.7333333333333112</v>
       </c>
       <c r="BN49" s="106">
         <f>BM49-I48</f>
-        <v>7</v>
+        <v>6.7666666666666444</v>
       </c>
       <c r="BO49" s="106">
         <f>BN49-I48</f>
-        <v>6</v>
+        <v>5.7999999999999776</v>
       </c>
       <c r="BP49" s="106">
         <f>BO49-I48</f>
-        <v>5</v>
+        <v>4.8333333333333108</v>
       </c>
       <c r="BQ49" s="106">
         <f>BP49-I48</f>
-        <v>4</v>
+        <v>3.866666666666644</v>
       </c>
       <c r="BR49" s="106">
         <f>BQ49-I48</f>
-        <v>3</v>
+        <v>2.8999999999999773</v>
       </c>
       <c r="BS49" s="106">
         <f>BR49-I48</f>
-        <v>2</v>
+        <v>1.9333333333333105</v>
       </c>
       <c r="BT49" s="106">
         <f>BS49-I48</f>
-        <v>1</v>
+        <v>0.9666666666666438</v>
       </c>
       <c r="BV49" s="101"/>
     </row>
@@ -17138,247 +17138,247 @@
       </c>
       <c r="M50" s="105">
         <f>E48</f>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N50" s="105">
         <f t="shared" ref="N50:BT50" si="11">M52</f>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="U50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="V50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="W50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="X50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Y50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Z50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AA50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AB50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AC50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AD50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AE50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AF50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AG50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AH50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AI50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AJ50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AK50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AL50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AM50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AN50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AO50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AP50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AQ50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AR50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AS50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AT50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AU50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AV50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AW50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AX50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AY50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AZ50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BA50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BB50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BC50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BD50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BE50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BF50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BG50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BH50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BI50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BJ50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BK50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BL50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BM50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BN50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BO50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BP50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BQ50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BR50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BS50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BT50" s="105">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BV50" s="101">
         <f t="shared" ref="BV50:BV52" si="12">SUM(M50:BT50)</f>
-        <v>3600</v>
+        <v>3480</v>
       </c>
     </row>
     <row r="51" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17459,247 +17459,247 @@
       </c>
       <c r="M52" s="105">
         <f t="shared" ref="M52:BT52" si="13">M50-M51</f>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="U52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="V52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="W52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="X52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Y52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Z52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AA52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AB52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AC52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AD52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AE52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AF52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AG52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AH52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AI52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AJ52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AK52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AL52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AM52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AN52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AO52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AP52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AQ52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AR52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AS52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AT52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AU52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AV52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AW52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AX52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AY52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AZ52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BA52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BB52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BC52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BD52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BE52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BF52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BG52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BH52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BI52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BJ52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BK52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BL52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BM52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BN52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BO52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BP52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BQ52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BR52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BS52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BT52" s="105">
         <f t="shared" si="13"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BV52" s="101">
         <f t="shared" si="12"/>
-        <v>3600</v>
+        <v>3480</v>
       </c>
     </row>
     <row r="53" spans="3:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17709,55 +17709,55 @@
       <c r="E56" s="205" t="s">
         <v>83</v>
       </c>
-      <c r="F56" s="188"/>
-      <c r="G56" s="188"/>
-      <c r="H56" s="188"/>
-      <c r="I56" s="188"/>
-      <c r="J56" s="188"/>
-      <c r="K56" s="188"/>
-      <c r="L56" s="188"/>
-      <c r="M56" s="188"/>
-      <c r="N56" s="188"/>
-      <c r="O56" s="188"/>
-      <c r="P56" s="188"/>
-      <c r="Q56" s="188"/>
-      <c r="R56" s="188"/>
-      <c r="S56" s="188"/>
-      <c r="T56" s="188"/>
-      <c r="U56" s="188"/>
-      <c r="V56" s="188"/>
-      <c r="W56" s="188"/>
-      <c r="X56" s="188"/>
-      <c r="Y56" s="188"/>
-      <c r="Z56" s="188"/>
-      <c r="AA56" s="188"/>
-      <c r="AB56" s="188"/>
-      <c r="AC56" s="188"/>
-      <c r="AD56" s="188"/>
-      <c r="AE56" s="188"/>
-      <c r="AF56" s="188"/>
-      <c r="AG56" s="188"/>
-      <c r="AH56" s="188"/>
-      <c r="AI56" s="188"/>
-      <c r="AJ56" s="188"/>
-      <c r="AK56" s="188"/>
-      <c r="AL56" s="188"/>
-      <c r="AM56" s="188"/>
-      <c r="AN56" s="188"/>
-      <c r="AO56" s="188"/>
-      <c r="AP56" s="188"/>
-      <c r="AQ56" s="188"/>
-      <c r="AR56" s="188"/>
-      <c r="AS56" s="188"/>
-      <c r="AT56" s="188"/>
-      <c r="AU56" s="188"/>
-      <c r="AV56" s="188"/>
-      <c r="AW56" s="188"/>
-      <c r="AX56" s="188"/>
-      <c r="AY56" s="188"/>
-      <c r="AZ56" s="188"/>
-      <c r="BA56" s="188"/>
-      <c r="BB56" s="189"/>
+      <c r="F56" s="169"/>
+      <c r="G56" s="169"/>
+      <c r="H56" s="169"/>
+      <c r="I56" s="169"/>
+      <c r="J56" s="169"/>
+      <c r="K56" s="169"/>
+      <c r="L56" s="169"/>
+      <c r="M56" s="169"/>
+      <c r="N56" s="169"/>
+      <c r="O56" s="169"/>
+      <c r="P56" s="169"/>
+      <c r="Q56" s="169"/>
+      <c r="R56" s="169"/>
+      <c r="S56" s="169"/>
+      <c r="T56" s="169"/>
+      <c r="U56" s="169"/>
+      <c r="V56" s="169"/>
+      <c r="W56" s="169"/>
+      <c r="X56" s="169"/>
+      <c r="Y56" s="169"/>
+      <c r="Z56" s="169"/>
+      <c r="AA56" s="169"/>
+      <c r="AB56" s="169"/>
+      <c r="AC56" s="169"/>
+      <c r="AD56" s="169"/>
+      <c r="AE56" s="169"/>
+      <c r="AF56" s="169"/>
+      <c r="AG56" s="169"/>
+      <c r="AH56" s="169"/>
+      <c r="AI56" s="169"/>
+      <c r="AJ56" s="169"/>
+      <c r="AK56" s="169"/>
+      <c r="AL56" s="169"/>
+      <c r="AM56" s="169"/>
+      <c r="AN56" s="169"/>
+      <c r="AO56" s="169"/>
+      <c r="AP56" s="169"/>
+      <c r="AQ56" s="169"/>
+      <c r="AR56" s="169"/>
+      <c r="AS56" s="169"/>
+      <c r="AT56" s="169"/>
+      <c r="AU56" s="169"/>
+      <c r="AV56" s="169"/>
+      <c r="AW56" s="169"/>
+      <c r="AX56" s="169"/>
+      <c r="AY56" s="169"/>
+      <c r="AZ56" s="169"/>
+      <c r="BA56" s="169"/>
+      <c r="BB56" s="170"/>
     </row>
     <row r="57" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18720,6 +18720,13 @@
     <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
     <mergeCell ref="E56:BB56"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
@@ -18736,13 +18743,6 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
first version with special events
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e15298e05a6af3ae/Università/Magistrale/LabAdvProg/Proj/AnimalDex/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{924F84E4-D806-4D05-846D-1F57D799F6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D61F7C90-3883-41A6-8B7A-B2E90F4B4ED7}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{924F84E4-D806-4D05-846D-1F57D799F6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{041F41A6-F001-41A2-8D1D-0EF76C1A63C1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="270">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -840,6 +840,12 @@
   </si>
   <si>
     <t>Winner announcement</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>Adding special events</t>
   </si>
 </sst>
 </file>
@@ -2588,11 +2594,53 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2623,48 +2671,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5059,7 +5065,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$51</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5116,7 +5122,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$48:$BT$48</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$49:$BT$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5305,7 +5311,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$51:$BT$51</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$52:$BT$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5352,7 +5358,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$49</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5375,7 +5381,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$48:$BT$48</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$49:$BT$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5564,189 +5570,189 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$49:$BT$49</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$50:$BT$50</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60.966666666666669</c:v>
+                  <c:v>66.86666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59.933333333333337</c:v>
+                  <c:v>65.73333333333332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.900000000000006</c:v>
+                  <c:v>64.59999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57.866666666666674</c:v>
+                  <c:v>63.466666666666647</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.833333333333343</c:v>
+                  <c:v>62.333333333333314</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55.800000000000011</c:v>
+                  <c:v>61.199999999999982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54.76666666666668</c:v>
+                  <c:v>60.066666666666649</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53.733333333333348</c:v>
+                  <c:v>58.933333333333316</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.700000000000017</c:v>
+                  <c:v>57.799999999999983</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>51.666666666666686</c:v>
+                  <c:v>56.66666666666665</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50.633333333333354</c:v>
+                  <c:v>55.533333333333317</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>49.600000000000023</c:v>
+                  <c:v>54.399999999999984</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>48.566666666666691</c:v>
+                  <c:v>53.266666666666652</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>47.53333333333336</c:v>
+                  <c:v>52.133333333333319</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>46.500000000000028</c:v>
+                  <c:v>50.999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>45.466666666666697</c:v>
+                  <c:v>49.866666666666653</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44.433333333333366</c:v>
+                  <c:v>48.73333333333332</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43.400000000000034</c:v>
+                  <c:v>47.599999999999987</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42.366666666666703</c:v>
+                  <c:v>46.466666666666654</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41.333333333333371</c:v>
+                  <c:v>45.333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>40.30000000000004</c:v>
+                  <c:v>44.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>39.266666666666708</c:v>
+                  <c:v>43.066666666666656</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>38.233333333333377</c:v>
+                  <c:v>41.933333333333323</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>37.200000000000045</c:v>
+                  <c:v>40.79999999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36.166666666666714</c:v>
+                  <c:v>39.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>35.133333333333383</c:v>
+                  <c:v>38.533333333333324</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>34.100000000000051</c:v>
+                  <c:v>37.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>33.06666666666672</c:v>
+                  <c:v>36.266666666666659</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>32.033333333333388</c:v>
+                  <c:v>35.133333333333326</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>31.000000000000053</c:v>
+                  <c:v>33.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>29.966666666666718</c:v>
+                  <c:v>32.86666666666666</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>28.933333333333383</c:v>
+                  <c:v>31.733333333333327</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>27.900000000000048</c:v>
+                  <c:v>30.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>26.866666666666713</c:v>
+                  <c:v>29.466666666666661</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>25.833333333333378</c:v>
+                  <c:v>28.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>24.800000000000043</c:v>
+                  <c:v>27.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>23.766666666666708</c:v>
+                  <c:v>26.066666666666663</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>22.733333333333373</c:v>
+                  <c:v>24.93333333333333</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>21.700000000000038</c:v>
+                  <c:v>23.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>20.666666666666703</c:v>
+                  <c:v>22.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>19.633333333333368</c:v>
+                  <c:v>21.533333333333331</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>18.600000000000033</c:v>
+                  <c:v>20.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>17.566666666666698</c:v>
+                  <c:v>19.266666666666666</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>16.533333333333363</c:v>
+                  <c:v>18.133333333333333</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>15.50000000000003</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>14.466666666666697</c:v>
+                  <c:v>15.866666666666667</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>13.433333333333364</c:v>
+                  <c:v>14.733333333333334</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>12.400000000000031</c:v>
+                  <c:v>13.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>11.366666666666697</c:v>
+                  <c:v>12.466666666666669</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>10.333333333333364</c:v>
+                  <c:v>11.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>9.3000000000000309</c:v>
+                  <c:v>10.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>8.2666666666666977</c:v>
+                  <c:v>9.06666666666667</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>7.2333333333333645</c:v>
+                  <c:v>7.9333333333333371</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>6.2000000000000313</c:v>
+                  <c:v>6.8000000000000043</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>5.166666666666698</c:v>
+                  <c:v>5.6666666666666714</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.1333333333333648</c:v>
+                  <c:v>4.5333333333333385</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3.1000000000000316</c:v>
+                  <c:v>3.4000000000000052</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.0666666666666984</c:v>
+                  <c:v>2.2666666666666719</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.033333333333365</c:v>
+                  <c:v>1.1333333333333386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5763,7 +5769,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$50</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5786,7 +5792,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$48:$BT$48</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$49:$BT$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5975,189 +5981,189 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$50:$BT$50</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$51:$BT$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>62</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6517,7 +6523,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="27632025" cy="7553325"/>
@@ -6579,6 +6585,10 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7062,19 +7072,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="171" t="str">
+      <c r="BK2" s="189" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="172"/>
-      <c r="BM2" s="172"/>
-      <c r="BN2" s="172"/>
-      <c r="BO2" s="172"/>
-      <c r="BP2" s="172"/>
-      <c r="BQ2" s="172"/>
-      <c r="BR2" s="172"/>
-      <c r="BS2" s="172"/>
-      <c r="BT2" s="172"/>
+      <c r="BL2" s="190"/>
+      <c r="BM2" s="190"/>
+      <c r="BN2" s="190"/>
+      <c r="BO2" s="190"/>
+      <c r="BP2" s="190"/>
+      <c r="BQ2" s="190"/>
+      <c r="BR2" s="190"/>
+      <c r="BS2" s="190"/>
+      <c r="BT2" s="190"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -7102,7 +7112,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="173" t="s">
+      <c r="K4" s="191" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7179,7 +7189,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="174"/>
+      <c r="K5" s="192"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7254,7 +7264,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="174"/>
+      <c r="K6" s="192"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7329,7 +7339,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="174"/>
+      <c r="K7" s="192"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7404,7 +7414,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="175"/>
+      <c r="K8" s="193"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7470,124 +7480,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="176" t="s">
+      <c r="B9" s="194" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="178" t="s">
+      <c r="C9" s="196" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="180" t="s">
+      <c r="D9" s="198" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="182" t="s">
+      <c r="E9" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="183"/>
-      <c r="G9" s="184"/>
-      <c r="H9" s="185" t="s">
+      <c r="F9" s="201"/>
+      <c r="G9" s="202"/>
+      <c r="H9" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="190" t="s">
+      <c r="I9" s="171" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="192" t="s">
+      <c r="J9" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="194" t="s">
+      <c r="K9" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="195" t="s">
+      <c r="L9" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="197" t="s">
+      <c r="M9" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="169"/>
-      <c r="O9" s="169"/>
-      <c r="P9" s="169"/>
-      <c r="Q9" s="198"/>
-      <c r="R9" s="199" t="s">
+      <c r="N9" s="179"/>
+      <c r="O9" s="179"/>
+      <c r="P9" s="179"/>
+      <c r="Q9" s="180"/>
+      <c r="R9" s="181" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="169"/>
-      <c r="T9" s="169"/>
-      <c r="U9" s="169"/>
-      <c r="V9" s="198"/>
-      <c r="W9" s="199" t="s">
+      <c r="S9" s="179"/>
+      <c r="T9" s="179"/>
+      <c r="U9" s="179"/>
+      <c r="V9" s="180"/>
+      <c r="W9" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="169"/>
-      <c r="Y9" s="169"/>
-      <c r="Z9" s="169"/>
-      <c r="AA9" s="170"/>
-      <c r="AB9" s="200" t="s">
+      <c r="X9" s="179"/>
+      <c r="Y9" s="179"/>
+      <c r="Z9" s="179"/>
+      <c r="AA9" s="182"/>
+      <c r="AB9" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="169"/>
-      <c r="AD9" s="169"/>
-      <c r="AE9" s="169"/>
-      <c r="AF9" s="198"/>
-      <c r="AG9" s="201" t="s">
+      <c r="AC9" s="179"/>
+      <c r="AD9" s="179"/>
+      <c r="AE9" s="179"/>
+      <c r="AF9" s="180"/>
+      <c r="AG9" s="184" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="169"/>
-      <c r="AI9" s="169"/>
-      <c r="AJ9" s="169"/>
-      <c r="AK9" s="198"/>
-      <c r="AL9" s="201" t="s">
+      <c r="AH9" s="179"/>
+      <c r="AI9" s="179"/>
+      <c r="AJ9" s="179"/>
+      <c r="AK9" s="180"/>
+      <c r="AL9" s="184" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="169"/>
-      <c r="AN9" s="169"/>
-      <c r="AO9" s="169"/>
-      <c r="AP9" s="170"/>
-      <c r="AQ9" s="202" t="s">
+      <c r="AM9" s="179"/>
+      <c r="AN9" s="179"/>
+      <c r="AO9" s="179"/>
+      <c r="AP9" s="182"/>
+      <c r="AQ9" s="185" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="169"/>
-      <c r="AS9" s="169"/>
-      <c r="AT9" s="169"/>
-      <c r="AU9" s="198"/>
-      <c r="AV9" s="203" t="s">
+      <c r="AR9" s="179"/>
+      <c r="AS9" s="179"/>
+      <c r="AT9" s="179"/>
+      <c r="AU9" s="180"/>
+      <c r="AV9" s="186" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="169"/>
-      <c r="AX9" s="169"/>
-      <c r="AY9" s="169"/>
-      <c r="AZ9" s="198"/>
-      <c r="BA9" s="203" t="s">
+      <c r="AW9" s="179"/>
+      <c r="AX9" s="179"/>
+      <c r="AY9" s="179"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="169"/>
-      <c r="BC9" s="169"/>
-      <c r="BD9" s="169"/>
-      <c r="BE9" s="170"/>
-      <c r="BF9" s="204" t="s">
+      <c r="BB9" s="179"/>
+      <c r="BC9" s="179"/>
+      <c r="BD9" s="179"/>
+      <c r="BE9" s="182"/>
+      <c r="BF9" s="187" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="169"/>
-      <c r="BH9" s="169"/>
-      <c r="BI9" s="169"/>
-      <c r="BJ9" s="198"/>
-      <c r="BK9" s="168" t="s">
+      <c r="BG9" s="179"/>
+      <c r="BH9" s="179"/>
+      <c r="BI9" s="179"/>
+      <c r="BJ9" s="180"/>
+      <c r="BK9" s="188" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="169"/>
-      <c r="BM9" s="169"/>
-      <c r="BN9" s="169"/>
-      <c r="BO9" s="198"/>
-      <c r="BP9" s="168" t="s">
+      <c r="BL9" s="179"/>
+      <c r="BM9" s="179"/>
+      <c r="BN9" s="179"/>
+      <c r="BO9" s="180"/>
+      <c r="BP9" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="169"/>
-      <c r="BR9" s="169"/>
-      <c r="BS9" s="169"/>
-      <c r="BT9" s="170"/>
+      <c r="BQ9" s="179"/>
+      <c r="BR9" s="179"/>
+      <c r="BS9" s="179"/>
+      <c r="BT9" s="182"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="177"/>
-      <c r="C10" s="179"/>
-      <c r="D10" s="181"/>
+      <c r="B10" s="195"/>
+      <c r="C10" s="197"/>
+      <c r="D10" s="199"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7597,11 +7607,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="186"/>
-      <c r="I10" s="191"/>
-      <c r="J10" s="193"/>
-      <c r="K10" s="193"/>
-      <c r="L10" s="196"/>
+      <c r="H10" s="204"/>
+      <c r="I10" s="172"/>
+      <c r="J10" s="174"/>
+      <c r="K10" s="174"/>
+      <c r="L10" s="177"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11210,80 +11220,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="187" t="str">
+      <c r="B45" s="168" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="188"/>
-      <c r="D45" s="188"/>
-      <c r="E45" s="188"/>
-      <c r="F45" s="188"/>
-      <c r="G45" s="188"/>
-      <c r="H45" s="188"/>
-      <c r="I45" s="188"/>
-      <c r="J45" s="188"/>
-      <c r="K45" s="188"/>
-      <c r="L45" s="188"/>
-      <c r="M45" s="188"/>
-      <c r="N45" s="188"/>
-      <c r="O45" s="188"/>
-      <c r="P45" s="188"/>
-      <c r="Q45" s="188"/>
-      <c r="R45" s="188"/>
-      <c r="S45" s="188"/>
-      <c r="T45" s="188"/>
-      <c r="U45" s="188"/>
-      <c r="V45" s="188"/>
-      <c r="W45" s="188"/>
-      <c r="X45" s="188"/>
-      <c r="Y45" s="188"/>
-      <c r="Z45" s="188"/>
-      <c r="AA45" s="188"/>
-      <c r="AB45" s="188"/>
-      <c r="AC45" s="188"/>
-      <c r="AD45" s="188"/>
-      <c r="AE45" s="188"/>
-      <c r="AF45" s="188"/>
-      <c r="AG45" s="188"/>
-      <c r="AH45" s="188"/>
-      <c r="AI45" s="188"/>
-      <c r="AJ45" s="188"/>
-      <c r="AK45" s="188"/>
-      <c r="AL45" s="188"/>
-      <c r="AM45" s="188"/>
-      <c r="AN45" s="188"/>
-      <c r="AO45" s="188"/>
-      <c r="AP45" s="188"/>
-      <c r="AQ45" s="188"/>
-      <c r="AR45" s="188"/>
-      <c r="AS45" s="188"/>
-      <c r="AT45" s="188"/>
-      <c r="AU45" s="188"/>
-      <c r="AV45" s="188"/>
-      <c r="AW45" s="188"/>
-      <c r="AX45" s="188"/>
-      <c r="AY45" s="188"/>
-      <c r="AZ45" s="188"/>
-      <c r="BA45" s="188"/>
-      <c r="BB45" s="188"/>
-      <c r="BC45" s="188"/>
-      <c r="BD45" s="188"/>
-      <c r="BE45" s="188"/>
-      <c r="BF45" s="188"/>
-      <c r="BG45" s="188"/>
-      <c r="BH45" s="188"/>
-      <c r="BI45" s="188"/>
-      <c r="BJ45" s="188"/>
-      <c r="BK45" s="188"/>
-      <c r="BL45" s="188"/>
-      <c r="BM45" s="188"/>
-      <c r="BN45" s="188"/>
-      <c r="BO45" s="188"/>
-      <c r="BP45" s="188"/>
-      <c r="BQ45" s="188"/>
-      <c r="BR45" s="188"/>
-      <c r="BS45" s="188"/>
-      <c r="BT45" s="189"/>
+      <c r="C45" s="169"/>
+      <c r="D45" s="169"/>
+      <c r="E45" s="169"/>
+      <c r="F45" s="169"/>
+      <c r="G45" s="169"/>
+      <c r="H45" s="169"/>
+      <c r="I45" s="169"/>
+      <c r="J45" s="169"/>
+      <c r="K45" s="169"/>
+      <c r="L45" s="169"/>
+      <c r="M45" s="169"/>
+      <c r="N45" s="169"/>
+      <c r="O45" s="169"/>
+      <c r="P45" s="169"/>
+      <c r="Q45" s="169"/>
+      <c r="R45" s="169"/>
+      <c r="S45" s="169"/>
+      <c r="T45" s="169"/>
+      <c r="U45" s="169"/>
+      <c r="V45" s="169"/>
+      <c r="W45" s="169"/>
+      <c r="X45" s="169"/>
+      <c r="Y45" s="169"/>
+      <c r="Z45" s="169"/>
+      <c r="AA45" s="169"/>
+      <c r="AB45" s="169"/>
+      <c r="AC45" s="169"/>
+      <c r="AD45" s="169"/>
+      <c r="AE45" s="169"/>
+      <c r="AF45" s="169"/>
+      <c r="AG45" s="169"/>
+      <c r="AH45" s="169"/>
+      <c r="AI45" s="169"/>
+      <c r="AJ45" s="169"/>
+      <c r="AK45" s="169"/>
+      <c r="AL45" s="169"/>
+      <c r="AM45" s="169"/>
+      <c r="AN45" s="169"/>
+      <c r="AO45" s="169"/>
+      <c r="AP45" s="169"/>
+      <c r="AQ45" s="169"/>
+      <c r="AR45" s="169"/>
+      <c r="AS45" s="169"/>
+      <c r="AT45" s="169"/>
+      <c r="AU45" s="169"/>
+      <c r="AV45" s="169"/>
+      <c r="AW45" s="169"/>
+      <c r="AX45" s="169"/>
+      <c r="AY45" s="169"/>
+      <c r="AZ45" s="169"/>
+      <c r="BA45" s="169"/>
+      <c r="BB45" s="169"/>
+      <c r="BC45" s="169"/>
+      <c r="BD45" s="169"/>
+      <c r="BE45" s="169"/>
+      <c r="BF45" s="169"/>
+      <c r="BG45" s="169"/>
+      <c r="BH45" s="169"/>
+      <c r="BI45" s="169"/>
+      <c r="BJ45" s="169"/>
+      <c r="BK45" s="169"/>
+      <c r="BL45" s="169"/>
+      <c r="BM45" s="169"/>
+      <c r="BN45" s="169"/>
+      <c r="BO45" s="169"/>
+      <c r="BP45" s="169"/>
+      <c r="BQ45" s="169"/>
+      <c r="BR45" s="169"/>
+      <c r="BS45" s="169"/>
+      <c r="BT45" s="170"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12246,6 +12256,14 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12262,14 +12280,6 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12282,10 +12292,10 @@
     <tabColor rgb="FF7B3C16"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:BV1012"/>
+  <dimension ref="B1:BV1013"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BO46" sqref="BO46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12398,7 +12408,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="173" t="s">
+      <c r="K3" s="191" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12475,7 +12485,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="174"/>
+      <c r="K4" s="192"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12549,7 +12559,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="174"/>
+      <c r="K5" s="192"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12623,7 +12633,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="174"/>
+      <c r="K6" s="192"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -12688,7 +12698,7 @@
       <c r="BS6" s="113"/>
       <c r="BT6" s="113"/>
     </row>
-    <row r="7" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:72" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -12698,7 +12708,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="175"/>
+      <c r="K7" s="193"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -12764,124 +12774,124 @@
       <c r="BT7" s="17"/>
     </row>
     <row r="8" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="176" t="s">
+      <c r="B8" s="194" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="178" t="s">
+      <c r="C8" s="196" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="180" t="s">
+      <c r="D8" s="198" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="182" t="s">
+      <c r="E8" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="183"/>
-      <c r="G8" s="184"/>
-      <c r="H8" s="185" t="s">
+      <c r="F8" s="201"/>
+      <c r="G8" s="202"/>
+      <c r="H8" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="190" t="s">
+      <c r="I8" s="171" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="192" t="s">
+      <c r="J8" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="194" t="s">
+      <c r="K8" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="195" t="s">
+      <c r="L8" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="197" t="s">
+      <c r="M8" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="169"/>
-      <c r="O8" s="169"/>
-      <c r="P8" s="169"/>
-      <c r="Q8" s="198"/>
-      <c r="R8" s="199" t="s">
+      <c r="N8" s="179"/>
+      <c r="O8" s="179"/>
+      <c r="P8" s="179"/>
+      <c r="Q8" s="180"/>
+      <c r="R8" s="181" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="169"/>
-      <c r="T8" s="169"/>
-      <c r="U8" s="169"/>
-      <c r="V8" s="198"/>
-      <c r="W8" s="199" t="s">
+      <c r="S8" s="179"/>
+      <c r="T8" s="179"/>
+      <c r="U8" s="179"/>
+      <c r="V8" s="180"/>
+      <c r="W8" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="169"/>
-      <c r="Y8" s="169"/>
-      <c r="Z8" s="169"/>
-      <c r="AA8" s="170"/>
-      <c r="AB8" s="200" t="s">
+      <c r="X8" s="179"/>
+      <c r="Y8" s="179"/>
+      <c r="Z8" s="179"/>
+      <c r="AA8" s="182"/>
+      <c r="AB8" s="183" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="169"/>
-      <c r="AD8" s="169"/>
-      <c r="AE8" s="169"/>
-      <c r="AF8" s="198"/>
-      <c r="AG8" s="201" t="s">
+      <c r="AC8" s="179"/>
+      <c r="AD8" s="179"/>
+      <c r="AE8" s="179"/>
+      <c r="AF8" s="180"/>
+      <c r="AG8" s="184" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="169"/>
-      <c r="AI8" s="169"/>
-      <c r="AJ8" s="169"/>
-      <c r="AK8" s="198"/>
-      <c r="AL8" s="201" t="s">
+      <c r="AH8" s="179"/>
+      <c r="AI8" s="179"/>
+      <c r="AJ8" s="179"/>
+      <c r="AK8" s="180"/>
+      <c r="AL8" s="184" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="169"/>
-      <c r="AN8" s="169"/>
-      <c r="AO8" s="169"/>
-      <c r="AP8" s="170"/>
-      <c r="AQ8" s="202" t="s">
+      <c r="AM8" s="179"/>
+      <c r="AN8" s="179"/>
+      <c r="AO8" s="179"/>
+      <c r="AP8" s="182"/>
+      <c r="AQ8" s="185" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="169"/>
-      <c r="AS8" s="169"/>
-      <c r="AT8" s="169"/>
-      <c r="AU8" s="198"/>
-      <c r="AV8" s="203" t="s">
+      <c r="AR8" s="179"/>
+      <c r="AS8" s="179"/>
+      <c r="AT8" s="179"/>
+      <c r="AU8" s="180"/>
+      <c r="AV8" s="186" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="169"/>
-      <c r="AX8" s="169"/>
-      <c r="AY8" s="169"/>
-      <c r="AZ8" s="198"/>
-      <c r="BA8" s="203" t="s">
+      <c r="AW8" s="179"/>
+      <c r="AX8" s="179"/>
+      <c r="AY8" s="179"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="169"/>
-      <c r="BC8" s="169"/>
-      <c r="BD8" s="169"/>
-      <c r="BE8" s="170"/>
-      <c r="BF8" s="204" t="s">
+      <c r="BB8" s="179"/>
+      <c r="BC8" s="179"/>
+      <c r="BD8" s="179"/>
+      <c r="BE8" s="182"/>
+      <c r="BF8" s="187" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="169"/>
-      <c r="BH8" s="169"/>
-      <c r="BI8" s="169"/>
-      <c r="BJ8" s="198"/>
-      <c r="BK8" s="168" t="s">
+      <c r="BG8" s="179"/>
+      <c r="BH8" s="179"/>
+      <c r="BI8" s="179"/>
+      <c r="BJ8" s="180"/>
+      <c r="BK8" s="188" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="169"/>
-      <c r="BM8" s="169"/>
-      <c r="BN8" s="169"/>
-      <c r="BO8" s="198"/>
-      <c r="BP8" s="168" t="s">
+      <c r="BL8" s="179"/>
+      <c r="BM8" s="179"/>
+      <c r="BN8" s="179"/>
+      <c r="BO8" s="180"/>
+      <c r="BP8" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="169"/>
-      <c r="BR8" s="169"/>
-      <c r="BS8" s="169"/>
-      <c r="BT8" s="170"/>
+      <c r="BQ8" s="179"/>
+      <c r="BR8" s="179"/>
+      <c r="BS8" s="179"/>
+      <c r="BT8" s="182"/>
     </row>
-    <row r="9" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="177"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="181"/>
+    <row r="9" spans="2:72" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="195"/>
+      <c r="C9" s="197"/>
+      <c r="D9" s="199"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -12891,11 +12901,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="186"/>
-      <c r="I9" s="191"/>
-      <c r="J9" s="193"/>
-      <c r="K9" s="193"/>
-      <c r="L9" s="196"/>
+      <c r="H9" s="204"/>
+      <c r="I9" s="172"/>
+      <c r="J9" s="174"/>
+      <c r="K9" s="174"/>
+      <c r="L9" s="177"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -13077,7 +13087,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:72" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B10" s="39">
         <v>1</v>
       </c>
@@ -13104,7 +13114,7 @@
       <c r="J10" s="47"/>
       <c r="K10" s="48"/>
       <c r="L10" s="49">
-        <f t="shared" ref="L10:L46" si="0">F10/E10</f>
+        <f t="shared" ref="L10:L47" si="0">F10/E10</f>
         <v>1</v>
       </c>
       <c r="M10" s="50"/>
@@ -15309,7 +15319,7 @@
       <c r="BS32" s="65"/>
       <c r="BT32" s="68"/>
     </row>
-    <row r="33" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="53" t="s">
         <v>239</v>
       </c>
@@ -15406,7 +15416,7 @@
       <c r="BS33" s="65"/>
       <c r="BT33" s="68"/>
     </row>
-    <row r="34" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="53" t="s">
         <v>238</v>
       </c>
@@ -15504,7 +15514,7 @@
       <c r="BS34" s="65"/>
       <c r="BT34" s="68"/>
     </row>
-    <row r="35" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="53" t="s">
         <v>241</v>
       </c>
@@ -15602,7 +15612,7 @@
       <c r="BS35" s="65"/>
       <c r="BT35" s="68"/>
     </row>
-    <row r="36" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="53" t="s">
         <v>243</v>
       </c>
@@ -15700,7 +15710,7 @@
       <c r="BS36" s="65"/>
       <c r="BT36" s="68"/>
     </row>
-    <row r="37" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="53" t="s">
         <v>247</v>
       </c>
@@ -15798,7 +15808,7 @@
       <c r="BS37" s="65"/>
       <c r="BT37" s="68"/>
     </row>
-    <row r="38" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="53" t="s">
         <v>246</v>
       </c>
@@ -15896,7 +15906,7 @@
       <c r="BS38" s="65"/>
       <c r="BT38" s="68"/>
     </row>
-    <row r="39" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="53" t="s">
         <v>251</v>
       </c>
@@ -15994,7 +16004,7 @@
       <c r="BS39" s="65"/>
       <c r="BT39" s="68"/>
     </row>
-    <row r="40" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="53" t="s">
         <v>253</v>
       </c>
@@ -16092,7 +16102,7 @@
       <c r="BS40" s="65"/>
       <c r="BT40" s="68"/>
     </row>
-    <row r="41" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="53" t="s">
         <v>254</v>
       </c>
@@ -16190,7 +16200,7 @@
       <c r="BS41" s="65"/>
       <c r="BT41" s="68"/>
     </row>
-    <row r="42" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="53">
         <v>4</v>
       </c>
@@ -16199,16 +16209,16 @@
       </c>
       <c r="D42" s="74"/>
       <c r="E42" s="42">
-        <f t="shared" ref="E42:G42" si="8">SUM(E43:E46)</f>
-        <v>13</v>
+        <f>SUM(E43:E47)</f>
+        <v>19</v>
       </c>
       <c r="F42" s="43">
-        <f t="shared" si="8"/>
-        <v>14</v>
+        <f>SUM(F43:F47)</f>
+        <v>17</v>
       </c>
       <c r="G42" s="44">
-        <f t="shared" si="8"/>
-        <v>-1</v>
+        <f>SUM(G43:G47)</f>
+        <v>2</v>
       </c>
       <c r="H42" s="75"/>
       <c r="I42" s="76"/>
@@ -16216,7 +16226,7 @@
       <c r="K42" s="77"/>
       <c r="L42" s="49">
         <f t="shared" si="0"/>
-        <v>1.0769230769230769</v>
+        <v>0.89473684210526316</v>
       </c>
       <c r="M42" s="50"/>
       <c r="N42" s="51"/>
@@ -16279,7 +16289,7 @@
       <c r="BS42" s="51"/>
       <c r="BT42" s="52"/>
     </row>
-    <row r="43" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="53">
         <v>4.0999999999999996</v>
       </c>
@@ -16296,7 +16306,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="58">
-        <f t="shared" ref="G43:G46" si="9">E43-F43</f>
+        <f t="shared" ref="G43:G47" si="8">E43-F43</f>
         <v>0</v>
       </c>
       <c r="H43" s="59">
@@ -16309,7 +16319,7 @@
         <v>45421</v>
       </c>
       <c r="K43" s="62">
-        <f t="shared" ref="K43:K46" si="10">J43-I43+1</f>
+        <f t="shared" ref="K43:K47" si="9">J43-I43+1</f>
         <v>1</v>
       </c>
       <c r="L43" s="63">
@@ -16376,7 +16386,7 @@
       <c r="BS43" s="65"/>
       <c r="BT43" s="68"/>
     </row>
-    <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="53">
         <v>4.2</v>
       </c>
@@ -16393,7 +16403,7 @@
         <v>2</v>
       </c>
       <c r="G44" s="58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H44" s="59">
@@ -16406,7 +16416,7 @@
         <v>45422</v>
       </c>
       <c r="K44" s="62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="L44" s="63">
@@ -16474,7 +16484,7 @@
       <c r="BS44" s="65"/>
       <c r="BT44" s="68"/>
     </row>
-    <row r="45" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="53">
         <v>4.3</v>
       </c>
@@ -16491,7 +16501,7 @@
         <v>6</v>
       </c>
       <c r="G45" s="58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H45" s="59">
@@ -16504,7 +16514,7 @@
         <v>45424</v>
       </c>
       <c r="K45" s="62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="L45" s="63">
@@ -16572,7 +16582,7 @@
       <c r="BS45" s="65"/>
       <c r="BT45" s="68"/>
     </row>
-    <row r="46" spans="2:74" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:72" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="81" t="s">
         <v>71</v>
       </c>
@@ -16589,7 +16599,7 @@
         <v>5</v>
       </c>
       <c r="G46" s="86">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="G46" si="10">E46-F46</f>
         <v>-1</v>
       </c>
       <c r="H46" s="87">
@@ -16602,11 +16612,11 @@
         <v>45429</v>
       </c>
       <c r="K46" s="90">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="K46" si="11">J46-I46+1</f>
         <v>3</v>
       </c>
       <c r="L46" s="91">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L46" si="12">F46/E46</f>
         <v>1.25</v>
       </c>
       <c r="M46" s="92"/>
@@ -16670,1121 +16680,1216 @@
       <c r="BS46" s="93"/>
       <c r="BT46" s="95"/>
     </row>
-    <row r="47" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E47" s="99" t="s">
+    <row r="47" spans="2:72" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="81" t="s">
+        <v>268</v>
+      </c>
+      <c r="C47" s="82" t="s">
+        <v>269</v>
+      </c>
+      <c r="D47" s="83" t="s">
+        <v>211</v>
+      </c>
+      <c r="E47" s="84">
+        <v>6</v>
+      </c>
+      <c r="F47" s="85">
+        <v>3</v>
+      </c>
+      <c r="G47" s="86">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="H47" s="87">
+        <v>4</v>
+      </c>
+      <c r="I47" s="88">
+        <v>45433</v>
+      </c>
+      <c r="J47" s="89"/>
+      <c r="K47" s="90">
+        <f t="shared" si="9"/>
+        <v>-45432</v>
+      </c>
+      <c r="L47" s="91">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="M47" s="92"/>
+      <c r="N47" s="93"/>
+      <c r="O47" s="93"/>
+      <c r="P47" s="93"/>
+      <c r="Q47" s="93"/>
+      <c r="R47" s="94"/>
+      <c r="S47" s="94"/>
+      <c r="T47" s="94"/>
+      <c r="U47" s="94"/>
+      <c r="V47" s="94"/>
+      <c r="W47" s="93"/>
+      <c r="X47" s="93"/>
+      <c r="Y47" s="93"/>
+      <c r="Z47" s="93"/>
+      <c r="AA47" s="95"/>
+      <c r="AB47" s="92"/>
+      <c r="AC47" s="93"/>
+      <c r="AD47" s="93"/>
+      <c r="AE47" s="93"/>
+      <c r="AF47" s="93"/>
+      <c r="AG47" s="96"/>
+      <c r="AH47" s="96"/>
+      <c r="AI47" s="96"/>
+      <c r="AJ47" s="96"/>
+      <c r="AK47" s="96"/>
+      <c r="AL47" s="93"/>
+      <c r="AM47" s="93"/>
+      <c r="AN47" s="93"/>
+      <c r="AO47" s="93"/>
+      <c r="AP47" s="95"/>
+      <c r="AQ47" s="92"/>
+      <c r="AR47" s="93"/>
+      <c r="AS47" s="93"/>
+      <c r="AT47" s="93"/>
+      <c r="AU47" s="93"/>
+      <c r="AV47" s="97"/>
+      <c r="AW47" s="97"/>
+      <c r="AX47" s="97"/>
+      <c r="AY47" s="97"/>
+      <c r="AZ47" s="97"/>
+      <c r="BA47" s="93"/>
+      <c r="BB47" s="93"/>
+      <c r="BC47" s="93"/>
+      <c r="BD47" s="93"/>
+      <c r="BE47" s="95"/>
+      <c r="BF47" s="92"/>
+      <c r="BG47" s="93"/>
+      <c r="BH47" s="93"/>
+      <c r="BI47" s="93"/>
+      <c r="BJ47" s="93"/>
+      <c r="BK47" s="98"/>
+      <c r="BL47" s="98"/>
+      <c r="BM47" s="98"/>
+      <c r="BN47" s="98"/>
+      <c r="BO47" s="98"/>
+      <c r="BP47" s="93"/>
+      <c r="BQ47" s="113"/>
+      <c r="BR47" s="113"/>
+      <c r="BS47" s="93"/>
+      <c r="BT47" s="95"/>
+    </row>
+    <row r="48" spans="2:72" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E48" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="F47" s="99" t="s">
+      <c r="F48" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="G47" s="99" t="s">
+      <c r="G48" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="H47" s="99" t="s">
+      <c r="H48" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="I47" s="99" t="s">
+      <c r="I48" s="99" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" s="100" t="s">
-        <v>76</v>
-      </c>
-      <c r="E48" s="101">
-        <f>SUM(E11:E16,E18:E21,E29:E37,E43:E46)</f>
-        <v>62</v>
-      </c>
-      <c r="F48" s="101">
-        <f>SUM(F11:F16,F18:F21,F29:F37,F43:F46)</f>
-        <v>65</v>
-      </c>
-      <c r="G48" s="101">
-        <f>SUM(G11:G16,G18:G21,G29:G37,G43:G46)</f>
-        <v>-3</v>
-      </c>
-      <c r="H48" s="101">
-        <v>60</v>
-      </c>
-      <c r="I48" s="101">
-        <f>E48/H48</f>
-        <v>1.0333333333333334</v>
-      </c>
-      <c r="L48" s="102" t="s">
-        <v>77</v>
-      </c>
-      <c r="M48" s="103">
-        <v>1</v>
-      </c>
-      <c r="N48" s="103">
-        <v>2</v>
-      </c>
-      <c r="O48" s="103">
-        <v>3</v>
-      </c>
-      <c r="P48" s="103">
-        <v>4</v>
-      </c>
-      <c r="Q48" s="103">
-        <v>5</v>
-      </c>
-      <c r="R48" s="103">
-        <v>6</v>
-      </c>
-      <c r="S48" s="103">
-        <v>7</v>
-      </c>
-      <c r="T48" s="103">
-        <v>8</v>
-      </c>
-      <c r="U48" s="103">
-        <v>9</v>
-      </c>
-      <c r="V48" s="103">
-        <v>10</v>
-      </c>
-      <c r="W48" s="103">
-        <v>11</v>
-      </c>
-      <c r="X48" s="103">
-        <v>12</v>
-      </c>
-      <c r="Y48" s="103">
-        <v>13</v>
-      </c>
-      <c r="Z48" s="103">
-        <v>14</v>
-      </c>
-      <c r="AA48" s="103">
-        <v>15</v>
-      </c>
-      <c r="AB48" s="103">
-        <v>16</v>
-      </c>
-      <c r="AC48" s="103">
-        <v>17</v>
-      </c>
-      <c r="AD48" s="103">
-        <v>18</v>
-      </c>
-      <c r="AE48" s="103">
-        <v>19</v>
-      </c>
-      <c r="AF48" s="103">
-        <v>20</v>
-      </c>
-      <c r="AG48" s="103">
-        <v>21</v>
-      </c>
-      <c r="AH48" s="103">
-        <v>22</v>
-      </c>
-      <c r="AI48" s="103">
-        <v>23</v>
-      </c>
-      <c r="AJ48" s="103">
-        <v>24</v>
-      </c>
-      <c r="AK48" s="103">
-        <v>25</v>
-      </c>
-      <c r="AL48" s="103">
-        <v>26</v>
-      </c>
-      <c r="AM48" s="103">
-        <v>27</v>
-      </c>
-      <c r="AN48" s="103">
-        <v>28</v>
-      </c>
-      <c r="AO48" s="103">
-        <v>29</v>
-      </c>
-      <c r="AP48" s="103">
-        <v>30</v>
-      </c>
-      <c r="AQ48" s="103">
-        <v>31</v>
-      </c>
-      <c r="AR48" s="103">
-        <v>32</v>
-      </c>
-      <c r="AS48" s="103">
-        <v>33</v>
-      </c>
-      <c r="AT48" s="103">
-        <v>34</v>
-      </c>
-      <c r="AU48" s="103">
-        <v>35</v>
-      </c>
-      <c r="AV48" s="103">
-        <v>36</v>
-      </c>
-      <c r="AW48" s="103">
-        <v>37</v>
-      </c>
-      <c r="AX48" s="103">
-        <v>38</v>
-      </c>
-      <c r="AY48" s="103">
-        <v>39</v>
-      </c>
-      <c r="AZ48" s="103">
-        <v>40</v>
-      </c>
-      <c r="BA48" s="103">
-        <v>41</v>
-      </c>
-      <c r="BB48" s="103">
-        <v>42</v>
-      </c>
-      <c r="BC48" s="103">
-        <v>43</v>
-      </c>
-      <c r="BD48" s="103">
-        <v>44</v>
-      </c>
-      <c r="BE48" s="103">
-        <v>45</v>
-      </c>
-      <c r="BF48" s="103">
-        <v>46</v>
-      </c>
-      <c r="BG48" s="103">
-        <v>47</v>
-      </c>
-      <c r="BH48" s="103">
-        <v>48</v>
-      </c>
-      <c r="BI48" s="103">
-        <v>49</v>
-      </c>
-      <c r="BJ48" s="103">
-        <v>50</v>
-      </c>
-      <c r="BK48" s="103">
-        <v>51</v>
-      </c>
-      <c r="BL48" s="103">
-        <v>52</v>
-      </c>
-      <c r="BM48" s="103">
-        <v>53</v>
-      </c>
-      <c r="BN48" s="103">
-        <v>54</v>
-      </c>
-      <c r="BO48" s="103">
-        <v>55</v>
-      </c>
-      <c r="BP48" s="103">
-        <v>56</v>
-      </c>
-      <c r="BQ48" s="103">
-        <v>57</v>
-      </c>
-      <c r="BR48" s="103">
-        <v>58</v>
-      </c>
-      <c r="BS48" s="103">
-        <v>59</v>
-      </c>
-      <c r="BT48" s="103">
-        <v>60</v>
-      </c>
-      <c r="BV48" s="100" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="49" spans="3:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H49" s="104" t="s">
-        <v>78</v>
+      <c r="C49" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="101">
+        <f>SUM(E11:E16,E18:E21,E29:E37,E43:E47)</f>
+        <v>68</v>
+      </c>
+      <c r="F49" s="101">
+        <f>SUM(F11:F16,F18:F21,F29:F37,F43:F47)</f>
+        <v>68</v>
+      </c>
+      <c r="G49" s="101">
+        <f>SUM(G11:G16,G18:G21,G29:G37,G43:G47)</f>
+        <v>0</v>
+      </c>
+      <c r="H49" s="101">
+        <v>60</v>
+      </c>
+      <c r="I49" s="101">
+        <f>E49/H49</f>
+        <v>1.1333333333333333</v>
       </c>
       <c r="L49" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="M49" s="105">
-        <f>E48</f>
-        <v>62</v>
-      </c>
-      <c r="N49" s="106">
-        <f>M49-I48</f>
-        <v>60.966666666666669</v>
-      </c>
-      <c r="O49" s="106">
-        <f>N49-I48</f>
-        <v>59.933333333333337</v>
-      </c>
-      <c r="P49" s="106">
-        <f>O49-I48</f>
-        <v>58.900000000000006</v>
-      </c>
-      <c r="Q49" s="106">
-        <f>P49-I48</f>
-        <v>57.866666666666674</v>
-      </c>
-      <c r="R49" s="106">
-        <f>Q49-I48</f>
-        <v>56.833333333333343</v>
-      </c>
-      <c r="S49" s="106">
-        <f>R49-I48</f>
-        <v>55.800000000000011</v>
-      </c>
-      <c r="T49" s="106">
-        <f>S49-I48</f>
-        <v>54.76666666666668</v>
-      </c>
-      <c r="U49" s="106">
-        <f>T49-I48</f>
-        <v>53.733333333333348</v>
-      </c>
-      <c r="V49" s="106">
-        <f>U49-I48</f>
-        <v>52.700000000000017</v>
-      </c>
-      <c r="W49" s="106">
-        <f>V49-I48</f>
-        <v>51.666666666666686</v>
-      </c>
-      <c r="X49" s="106">
-        <f>W49-I48</f>
-        <v>50.633333333333354</v>
-      </c>
-      <c r="Y49" s="106">
-        <f>X49-I48</f>
-        <v>49.600000000000023</v>
-      </c>
-      <c r="Z49" s="106">
-        <f>Y49-I48</f>
-        <v>48.566666666666691</v>
-      </c>
-      <c r="AA49" s="106">
-        <f>Z49-I48</f>
-        <v>47.53333333333336</v>
-      </c>
-      <c r="AB49" s="106">
-        <f>AA49-I48</f>
-        <v>46.500000000000028</v>
-      </c>
-      <c r="AC49" s="106">
-        <f>AB49-I48</f>
-        <v>45.466666666666697</v>
-      </c>
-      <c r="AD49" s="106">
-        <f>AC49-I48</f>
-        <v>44.433333333333366</v>
-      </c>
-      <c r="AE49" s="106">
-        <f>AD49-I48</f>
-        <v>43.400000000000034</v>
-      </c>
-      <c r="AF49" s="106">
-        <f>AE49-I48</f>
-        <v>42.366666666666703</v>
-      </c>
-      <c r="AG49" s="106">
-        <f>AF49-I48</f>
-        <v>41.333333333333371</v>
-      </c>
-      <c r="AH49" s="106">
-        <f>AG49-I48</f>
-        <v>40.30000000000004</v>
-      </c>
-      <c r="AI49" s="106">
-        <f>AH49-I48</f>
-        <v>39.266666666666708</v>
-      </c>
-      <c r="AJ49" s="106">
-        <f>AI49-I48</f>
-        <v>38.233333333333377</v>
-      </c>
-      <c r="AK49" s="106">
-        <f>AJ49-I48</f>
-        <v>37.200000000000045</v>
-      </c>
-      <c r="AL49" s="106">
-        <f>AK49-I48</f>
-        <v>36.166666666666714</v>
-      </c>
-      <c r="AM49" s="106">
-        <f>AL49-I48</f>
-        <v>35.133333333333383</v>
-      </c>
-      <c r="AN49" s="106">
-        <f>AM49-I48</f>
-        <v>34.100000000000051</v>
-      </c>
-      <c r="AO49" s="106">
-        <f>AN49-I48</f>
-        <v>33.06666666666672</v>
-      </c>
-      <c r="AP49" s="106">
-        <f>AO49-I48</f>
-        <v>32.033333333333388</v>
-      </c>
-      <c r="AQ49" s="106">
-        <f>AP49-I48</f>
-        <v>31.000000000000053</v>
-      </c>
-      <c r="AR49" s="106">
-        <f>AQ49-I48</f>
-        <v>29.966666666666718</v>
-      </c>
-      <c r="AS49" s="106">
-        <f>AR49-I48</f>
-        <v>28.933333333333383</v>
-      </c>
-      <c r="AT49" s="106">
-        <f>AS49-I48</f>
-        <v>27.900000000000048</v>
-      </c>
-      <c r="AU49" s="106">
-        <f>AT49-I48</f>
-        <v>26.866666666666713</v>
-      </c>
-      <c r="AV49" s="106">
-        <f>AU49-I48</f>
-        <v>25.833333333333378</v>
-      </c>
-      <c r="AW49" s="106">
-        <f>AV49-I48</f>
-        <v>24.800000000000043</v>
-      </c>
-      <c r="AX49" s="106">
-        <f>AW49-I48</f>
-        <v>23.766666666666708</v>
-      </c>
-      <c r="AY49" s="106">
-        <f>AX49-I48</f>
-        <v>22.733333333333373</v>
-      </c>
-      <c r="AZ49" s="106">
-        <f>AY49-I48</f>
-        <v>21.700000000000038</v>
-      </c>
-      <c r="BA49" s="106">
-        <f>AZ49-I48</f>
-        <v>20.666666666666703</v>
-      </c>
-      <c r="BB49" s="106">
-        <f>BA49-I48</f>
-        <v>19.633333333333368</v>
-      </c>
-      <c r="BC49" s="106">
-        <f>BB49-I48</f>
-        <v>18.600000000000033</v>
-      </c>
-      <c r="BD49" s="106">
-        <f>BC49-I48</f>
-        <v>17.566666666666698</v>
-      </c>
-      <c r="BE49" s="106">
-        <f>BD49-I48</f>
-        <v>16.533333333333363</v>
-      </c>
-      <c r="BF49" s="106">
-        <f>BE49-I48</f>
-        <v>15.50000000000003</v>
-      </c>
-      <c r="BG49" s="106">
-        <f>BF49-I48</f>
-        <v>14.466666666666697</v>
-      </c>
-      <c r="BH49" s="106">
-        <f>BG49-I48</f>
-        <v>13.433333333333364</v>
-      </c>
-      <c r="BI49" s="106">
-        <f>BH49-I48</f>
-        <v>12.400000000000031</v>
-      </c>
-      <c r="BJ49" s="106">
-        <f>BI49-I48</f>
-        <v>11.366666666666697</v>
-      </c>
-      <c r="BK49" s="106">
-        <f>BJ49-I48</f>
-        <v>10.333333333333364</v>
-      </c>
-      <c r="BL49" s="106">
-        <f>BK49-I48</f>
-        <v>9.3000000000000309</v>
-      </c>
-      <c r="BM49" s="106">
-        <f>BL49-I48</f>
-        <v>8.2666666666666977</v>
-      </c>
-      <c r="BN49" s="106">
-        <f>BM49-I48</f>
-        <v>7.2333333333333645</v>
-      </c>
-      <c r="BO49" s="106">
-        <f>BN49-I48</f>
-        <v>6.2000000000000313</v>
-      </c>
-      <c r="BP49" s="106">
-        <f>BO49-I48</f>
-        <v>5.166666666666698</v>
-      </c>
-      <c r="BQ49" s="106">
-        <f>BP49-I48</f>
-        <v>4.1333333333333648</v>
-      </c>
-      <c r="BR49" s="106">
-        <f>BQ49-I48</f>
-        <v>3.1000000000000316</v>
-      </c>
-      <c r="BS49" s="106">
-        <f>BR49-I48</f>
-        <v>2.0666666666666984</v>
-      </c>
-      <c r="BT49" s="106">
-        <f>BS49-I48</f>
-        <v>1.033333333333365</v>
-      </c>
-      <c r="BV49" s="101"/>
+        <v>77</v>
+      </c>
+      <c r="M49" s="103">
+        <v>1</v>
+      </c>
+      <c r="N49" s="103">
+        <v>2</v>
+      </c>
+      <c r="O49" s="103">
+        <v>3</v>
+      </c>
+      <c r="P49" s="103">
+        <v>4</v>
+      </c>
+      <c r="Q49" s="103">
+        <v>5</v>
+      </c>
+      <c r="R49" s="103">
+        <v>6</v>
+      </c>
+      <c r="S49" s="103">
+        <v>7</v>
+      </c>
+      <c r="T49" s="103">
+        <v>8</v>
+      </c>
+      <c r="U49" s="103">
+        <v>9</v>
+      </c>
+      <c r="V49" s="103">
+        <v>10</v>
+      </c>
+      <c r="W49" s="103">
+        <v>11</v>
+      </c>
+      <c r="X49" s="103">
+        <v>12</v>
+      </c>
+      <c r="Y49" s="103">
+        <v>13</v>
+      </c>
+      <c r="Z49" s="103">
+        <v>14</v>
+      </c>
+      <c r="AA49" s="103">
+        <v>15</v>
+      </c>
+      <c r="AB49" s="103">
+        <v>16</v>
+      </c>
+      <c r="AC49" s="103">
+        <v>17</v>
+      </c>
+      <c r="AD49" s="103">
+        <v>18</v>
+      </c>
+      <c r="AE49" s="103">
+        <v>19</v>
+      </c>
+      <c r="AF49" s="103">
+        <v>20</v>
+      </c>
+      <c r="AG49" s="103">
+        <v>21</v>
+      </c>
+      <c r="AH49" s="103">
+        <v>22</v>
+      </c>
+      <c r="AI49" s="103">
+        <v>23</v>
+      </c>
+      <c r="AJ49" s="103">
+        <v>24</v>
+      </c>
+      <c r="AK49" s="103">
+        <v>25</v>
+      </c>
+      <c r="AL49" s="103">
+        <v>26</v>
+      </c>
+      <c r="AM49" s="103">
+        <v>27</v>
+      </c>
+      <c r="AN49" s="103">
+        <v>28</v>
+      </c>
+      <c r="AO49" s="103">
+        <v>29</v>
+      </c>
+      <c r="AP49" s="103">
+        <v>30</v>
+      </c>
+      <c r="AQ49" s="103">
+        <v>31</v>
+      </c>
+      <c r="AR49" s="103">
+        <v>32</v>
+      </c>
+      <c r="AS49" s="103">
+        <v>33</v>
+      </c>
+      <c r="AT49" s="103">
+        <v>34</v>
+      </c>
+      <c r="AU49" s="103">
+        <v>35</v>
+      </c>
+      <c r="AV49" s="103">
+        <v>36</v>
+      </c>
+      <c r="AW49" s="103">
+        <v>37</v>
+      </c>
+      <c r="AX49" s="103">
+        <v>38</v>
+      </c>
+      <c r="AY49" s="103">
+        <v>39</v>
+      </c>
+      <c r="AZ49" s="103">
+        <v>40</v>
+      </c>
+      <c r="BA49" s="103">
+        <v>41</v>
+      </c>
+      <c r="BB49" s="103">
+        <v>42</v>
+      </c>
+      <c r="BC49" s="103">
+        <v>43</v>
+      </c>
+      <c r="BD49" s="103">
+        <v>44</v>
+      </c>
+      <c r="BE49" s="103">
+        <v>45</v>
+      </c>
+      <c r="BF49" s="103">
+        <v>46</v>
+      </c>
+      <c r="BG49" s="103">
+        <v>47</v>
+      </c>
+      <c r="BH49" s="103">
+        <v>48</v>
+      </c>
+      <c r="BI49" s="103">
+        <v>49</v>
+      </c>
+      <c r="BJ49" s="103">
+        <v>50</v>
+      </c>
+      <c r="BK49" s="103">
+        <v>51</v>
+      </c>
+      <c r="BL49" s="103">
+        <v>52</v>
+      </c>
+      <c r="BM49" s="103">
+        <v>53</v>
+      </c>
+      <c r="BN49" s="103">
+        <v>54</v>
+      </c>
+      <c r="BO49" s="103">
+        <v>55</v>
+      </c>
+      <c r="BP49" s="103">
+        <v>56</v>
+      </c>
+      <c r="BQ49" s="103">
+        <v>57</v>
+      </c>
+      <c r="BR49" s="103">
+        <v>58</v>
+      </c>
+      <c r="BS49" s="103">
+        <v>59</v>
+      </c>
+      <c r="BT49" s="103">
+        <v>60</v>
+      </c>
+      <c r="BV49" s="100" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="50" spans="3:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H50" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="L50" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="M50" s="105">
+        <f>E49</f>
+        <v>68</v>
+      </c>
+      <c r="N50" s="106">
+        <f>M50-I49</f>
+        <v>66.86666666666666</v>
+      </c>
+      <c r="O50" s="106">
+        <f>N50-I49</f>
+        <v>65.73333333333332</v>
+      </c>
+      <c r="P50" s="106">
+        <f>O50-I49</f>
+        <v>64.59999999999998</v>
+      </c>
+      <c r="Q50" s="106">
+        <f>P50-I49</f>
+        <v>63.466666666666647</v>
+      </c>
+      <c r="R50" s="106">
+        <f>Q50-I49</f>
+        <v>62.333333333333314</v>
+      </c>
+      <c r="S50" s="106">
+        <f>R50-I49</f>
+        <v>61.199999999999982</v>
+      </c>
+      <c r="T50" s="106">
+        <f>S50-I49</f>
+        <v>60.066666666666649</v>
+      </c>
+      <c r="U50" s="106">
+        <f>T50-I49</f>
+        <v>58.933333333333316</v>
+      </c>
+      <c r="V50" s="106">
+        <f>U50-I49</f>
+        <v>57.799999999999983</v>
+      </c>
+      <c r="W50" s="106">
+        <f>V50-I49</f>
+        <v>56.66666666666665</v>
+      </c>
+      <c r="X50" s="106">
+        <f>W50-I49</f>
+        <v>55.533333333333317</v>
+      </c>
+      <c r="Y50" s="106">
+        <f>X50-I49</f>
+        <v>54.399999999999984</v>
+      </c>
+      <c r="Z50" s="106">
+        <f>Y50-I49</f>
+        <v>53.266666666666652</v>
+      </c>
+      <c r="AA50" s="106">
+        <f>Z50-I49</f>
+        <v>52.133333333333319</v>
+      </c>
+      <c r="AB50" s="106">
+        <f>AA50-I49</f>
+        <v>50.999999999999986</v>
+      </c>
+      <c r="AC50" s="106">
+        <f>AB50-I49</f>
+        <v>49.866666666666653</v>
+      </c>
+      <c r="AD50" s="106">
+        <f>AC50-I49</f>
+        <v>48.73333333333332</v>
+      </c>
+      <c r="AE50" s="106">
+        <f>AD50-I49</f>
+        <v>47.599999999999987</v>
+      </c>
+      <c r="AF50" s="106">
+        <f>AE50-I49</f>
+        <v>46.466666666666654</v>
+      </c>
+      <c r="AG50" s="106">
+        <f>AF50-I49</f>
+        <v>45.333333333333321</v>
+      </c>
+      <c r="AH50" s="106">
+        <f>AG50-I49</f>
+        <v>44.199999999999989</v>
+      </c>
+      <c r="AI50" s="106">
+        <f>AH50-I49</f>
+        <v>43.066666666666656</v>
+      </c>
+      <c r="AJ50" s="106">
+        <f>AI50-I49</f>
+        <v>41.933333333333323</v>
+      </c>
+      <c r="AK50" s="106">
+        <f>AJ50-I49</f>
+        <v>40.79999999999999</v>
+      </c>
+      <c r="AL50" s="106">
+        <f>AK50-I49</f>
+        <v>39.666666666666657</v>
+      </c>
+      <c r="AM50" s="106">
+        <f>AL50-I49</f>
+        <v>38.533333333333324</v>
+      </c>
+      <c r="AN50" s="106">
+        <f>AM50-I49</f>
+        <v>37.399999999999991</v>
+      </c>
+      <c r="AO50" s="106">
+        <f>AN50-I49</f>
+        <v>36.266666666666659</v>
+      </c>
+      <c r="AP50" s="106">
+        <f>AO50-I49</f>
+        <v>35.133333333333326</v>
+      </c>
+      <c r="AQ50" s="106">
+        <f>AP50-I49</f>
+        <v>33.999999999999993</v>
+      </c>
+      <c r="AR50" s="106">
+        <f>AQ50-I49</f>
+        <v>32.86666666666666</v>
+      </c>
+      <c r="AS50" s="106">
+        <f>AR50-I49</f>
+        <v>31.733333333333327</v>
+      </c>
+      <c r="AT50" s="106">
+        <f>AS50-I49</f>
+        <v>30.599999999999994</v>
+      </c>
+      <c r="AU50" s="106">
+        <f>AT50-I49</f>
+        <v>29.466666666666661</v>
+      </c>
+      <c r="AV50" s="106">
+        <f>AU50-I49</f>
+        <v>28.333333333333329</v>
+      </c>
+      <c r="AW50" s="106">
+        <f>AV50-I49</f>
+        <v>27.199999999999996</v>
+      </c>
+      <c r="AX50" s="106">
+        <f>AW50-I49</f>
+        <v>26.066666666666663</v>
+      </c>
+      <c r="AY50" s="106">
+        <f>AX50-I49</f>
+        <v>24.93333333333333</v>
+      </c>
+      <c r="AZ50" s="106">
+        <f>AY50-I49</f>
+        <v>23.799999999999997</v>
+      </c>
+      <c r="BA50" s="106">
+        <f>AZ50-I49</f>
+        <v>22.666666666666664</v>
+      </c>
+      <c r="BB50" s="106">
+        <f>BA50-I49</f>
+        <v>21.533333333333331</v>
+      </c>
+      <c r="BC50" s="106">
+        <f>BB50-I49</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="BD50" s="106">
+        <f>BC50-I49</f>
+        <v>19.266666666666666</v>
+      </c>
+      <c r="BE50" s="106">
+        <f>BD50-I49</f>
+        <v>18.133333333333333</v>
+      </c>
+      <c r="BF50" s="106">
+        <f>BE50-I49</f>
+        <v>17</v>
+      </c>
+      <c r="BG50" s="106">
+        <f>BF50-I49</f>
+        <v>15.866666666666667</v>
+      </c>
+      <c r="BH50" s="106">
+        <f>BG50-I49</f>
+        <v>14.733333333333334</v>
+      </c>
+      <c r="BI50" s="106">
+        <f>BH50-I49</f>
+        <v>13.600000000000001</v>
+      </c>
+      <c r="BJ50" s="106">
+        <f>BI50-I49</f>
+        <v>12.466666666666669</v>
+      </c>
+      <c r="BK50" s="106">
+        <f>BJ50-I49</f>
+        <v>11.333333333333336</v>
+      </c>
+      <c r="BL50" s="106">
+        <f>BK50-I49</f>
+        <v>10.200000000000003</v>
+      </c>
+      <c r="BM50" s="106">
+        <f>BL50-I49</f>
+        <v>9.06666666666667</v>
+      </c>
+      <c r="BN50" s="106">
+        <f>BM50-I49</f>
+        <v>7.9333333333333371</v>
+      </c>
+      <c r="BO50" s="106">
+        <f>BN50-I49</f>
+        <v>6.8000000000000043</v>
+      </c>
+      <c r="BP50" s="106">
+        <f>BO50-I49</f>
+        <v>5.6666666666666714</v>
+      </c>
+      <c r="BQ50" s="106">
+        <f>BP50-I49</f>
+        <v>4.5333333333333385</v>
+      </c>
+      <c r="BR50" s="106">
+        <f>BQ50-I49</f>
+        <v>3.4000000000000052</v>
+      </c>
+      <c r="BS50" s="106">
+        <f>BR50-I49</f>
+        <v>2.2666666666666719</v>
+      </c>
+      <c r="BT50" s="106">
+        <f>BS50-I49</f>
+        <v>1.1333333333333386</v>
+      </c>
+      <c r="BV50" s="101"/>
+    </row>
+    <row r="51" spans="3:74" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L51" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="M50" s="105">
-        <f>E48</f>
-        <v>62</v>
-      </c>
-      <c r="N50" s="105">
-        <f t="shared" ref="N50:BT50" si="11">M52</f>
-        <v>62</v>
-      </c>
-      <c r="O50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="P50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="Q50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="R50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="S50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="T50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="U50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="V50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="W50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="X50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="Y50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="Z50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AA50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AB50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AC50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AD50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AE50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AF50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AG50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AH50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AI50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AJ50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AK50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AL50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AM50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AN50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AO50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AP50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AQ50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AR50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AS50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AT50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AU50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AV50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AW50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AX50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AY50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="AZ50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BA50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BB50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BC50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BD50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BE50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BF50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BG50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BH50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BI50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BJ50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BK50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BL50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BM50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BN50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BO50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BP50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BQ50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BR50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BS50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BT50" s="105">
-        <f t="shared" si="11"/>
-        <v>62</v>
-      </c>
-      <c r="BV50" s="101">
-        <f t="shared" ref="BV50:BV52" si="12">SUM(M50:BT50)</f>
-        <v>3720</v>
-      </c>
-    </row>
-    <row r="51" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K51" s="107" t="s">
-        <v>80</v>
-      </c>
-      <c r="L51" s="102" t="s">
-        <v>81</v>
-      </c>
-      <c r="M51" s="57"/>
-      <c r="N51" s="57"/>
-      <c r="O51" s="57"/>
-      <c r="P51" s="57"/>
-      <c r="Q51" s="57"/>
-      <c r="R51" s="57"/>
-      <c r="S51" s="57"/>
-      <c r="T51" s="57"/>
-      <c r="U51" s="57"/>
-      <c r="V51" s="57"/>
-      <c r="W51" s="57"/>
-      <c r="X51" s="57"/>
-      <c r="Y51" s="57"/>
-      <c r="Z51" s="57"/>
-      <c r="AA51" s="57"/>
-      <c r="AB51" s="57"/>
-      <c r="AC51" s="57"/>
-      <c r="AD51" s="57"/>
-      <c r="AE51" s="57"/>
-      <c r="AF51" s="57"/>
-      <c r="AG51" s="57"/>
-      <c r="AH51" s="57"/>
-      <c r="AI51" s="57"/>
-      <c r="AJ51" s="57"/>
-      <c r="AK51" s="57"/>
-      <c r="AL51" s="57"/>
-      <c r="AM51" s="57"/>
-      <c r="AN51" s="57"/>
-      <c r="AO51" s="57"/>
-      <c r="AP51" s="57"/>
-      <c r="AQ51" s="57"/>
-      <c r="AR51" s="57"/>
-      <c r="AS51" s="57"/>
-      <c r="AT51" s="57"/>
-      <c r="AU51" s="57"/>
-      <c r="AV51" s="57"/>
-      <c r="AW51" s="57"/>
-      <c r="AX51" s="57"/>
-      <c r="AY51" s="57"/>
-      <c r="AZ51" s="57"/>
-      <c r="BA51" s="57"/>
-      <c r="BB51" s="57"/>
-      <c r="BC51" s="57"/>
-      <c r="BD51" s="57"/>
-      <c r="BE51" s="57"/>
-      <c r="BF51" s="57"/>
-      <c r="BG51" s="57"/>
-      <c r="BH51" s="57"/>
-      <c r="BI51" s="57"/>
-      <c r="BJ51" s="57"/>
-      <c r="BK51" s="57"/>
-      <c r="BL51" s="57"/>
-      <c r="BM51" s="57"/>
-      <c r="BN51" s="57"/>
-      <c r="BO51" s="57"/>
-      <c r="BP51" s="57"/>
-      <c r="BQ51" s="57"/>
-      <c r="BR51" s="57"/>
-      <c r="BS51" s="57"/>
-      <c r="BT51" s="57"/>
+      <c r="M51" s="105">
+        <f>E49</f>
+        <v>68</v>
+      </c>
+      <c r="N51" s="105">
+        <f t="shared" ref="N51:BT51" si="13">M53</f>
+        <v>68</v>
+      </c>
+      <c r="O51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="P51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="Q51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="R51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="S51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="T51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="U51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="V51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="W51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="X51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="Y51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="Z51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AA51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AB51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AC51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AD51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AE51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AF51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AG51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AH51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AI51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AJ51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AK51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AL51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AM51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AN51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AO51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AP51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AQ51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AR51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AS51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AT51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AU51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AV51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AW51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AX51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AY51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="AZ51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BA51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BB51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BC51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BD51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BE51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BF51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BG51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BH51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BI51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BJ51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BK51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BL51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BM51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BN51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BO51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BP51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BQ51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BR51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BS51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="BT51" s="105">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
       <c r="BV51" s="101">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" ref="BV51:BV53" si="14">SUM(M51:BT51)</f>
+        <v>4080</v>
       </c>
     </row>
     <row r="52" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K52" s="107" t="s">
+        <v>80</v>
+      </c>
       <c r="L52" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="M52" s="57"/>
+      <c r="N52" s="57"/>
+      <c r="O52" s="57"/>
+      <c r="P52" s="57"/>
+      <c r="Q52" s="57"/>
+      <c r="R52" s="57"/>
+      <c r="S52" s="57"/>
+      <c r="T52" s="57"/>
+      <c r="U52" s="57"/>
+      <c r="V52" s="57"/>
+      <c r="W52" s="57"/>
+      <c r="X52" s="57"/>
+      <c r="Y52" s="57"/>
+      <c r="Z52" s="57"/>
+      <c r="AA52" s="57"/>
+      <c r="AB52" s="57"/>
+      <c r="AC52" s="57"/>
+      <c r="AD52" s="57"/>
+      <c r="AE52" s="57"/>
+      <c r="AF52" s="57"/>
+      <c r="AG52" s="57"/>
+      <c r="AH52" s="57"/>
+      <c r="AI52" s="57"/>
+      <c r="AJ52" s="57"/>
+      <c r="AK52" s="57"/>
+      <c r="AL52" s="57"/>
+      <c r="AM52" s="57"/>
+      <c r="AN52" s="57"/>
+      <c r="AO52" s="57"/>
+      <c r="AP52" s="57"/>
+      <c r="AQ52" s="57"/>
+      <c r="AR52" s="57"/>
+      <c r="AS52" s="57"/>
+      <c r="AT52" s="57"/>
+      <c r="AU52" s="57"/>
+      <c r="AV52" s="57"/>
+      <c r="AW52" s="57"/>
+      <c r="AX52" s="57"/>
+      <c r="AY52" s="57"/>
+      <c r="AZ52" s="57"/>
+      <c r="BA52" s="57"/>
+      <c r="BB52" s="57"/>
+      <c r="BC52" s="57"/>
+      <c r="BD52" s="57"/>
+      <c r="BE52" s="57"/>
+      <c r="BF52" s="57"/>
+      <c r="BG52" s="57"/>
+      <c r="BH52" s="57"/>
+      <c r="BI52" s="57"/>
+      <c r="BJ52" s="57"/>
+      <c r="BK52" s="57"/>
+      <c r="BL52" s="57"/>
+      <c r="BM52" s="57"/>
+      <c r="BN52" s="57"/>
+      <c r="BO52" s="57"/>
+      <c r="BP52" s="57"/>
+      <c r="BQ52" s="57"/>
+      <c r="BR52" s="57"/>
+      <c r="BS52" s="57"/>
+      <c r="BT52" s="57"/>
+      <c r="BV52" s="101">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L53" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M52" s="105">
-        <f t="shared" ref="M52:BT52" si="13">M50-M51</f>
-        <v>62</v>
-      </c>
-      <c r="N52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="O52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="P52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="Q52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="R52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="S52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="T52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="U52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="V52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="W52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="X52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="Y52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="Z52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AA52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AB52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AC52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AD52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AE52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AF52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AG52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AH52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AI52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AJ52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AK52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AL52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AM52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AN52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AO52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AP52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AQ52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AR52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AS52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AT52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AU52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AV52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AW52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AX52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AY52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="AZ52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BA52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BB52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BC52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BD52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BE52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BF52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BG52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BH52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BI52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BJ52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BK52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BL52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BM52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BN52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BO52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BP52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BQ52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BR52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BS52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BT52" s="105">
-        <f t="shared" si="13"/>
-        <v>62</v>
-      </c>
-      <c r="BV52" s="101">
-        <f t="shared" si="12"/>
-        <v>3720</v>
+      <c r="M53" s="105">
+        <f t="shared" ref="M53:BT53" si="15">M51-M52</f>
+        <v>68</v>
+      </c>
+      <c r="N53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="O53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="P53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="Q53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="R53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="S53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="T53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="U53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="V53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="W53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="X53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="Y53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="Z53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AA53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AB53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AC53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AD53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AE53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AF53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AG53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AH53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AI53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AJ53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AK53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AL53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AM53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AN53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AO53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AP53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AQ53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AR53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AS53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AT53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AU53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AV53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AW53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AX53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AY53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="AZ53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BA53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BB53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BC53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BD53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BE53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BF53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BG53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BH53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BI53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BJ53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BK53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BL53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BM53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BN53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BO53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BP53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BQ53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BR53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BS53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BT53" s="105">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="BV53" s="101">
+        <f t="shared" si="14"/>
+        <v>4080</v>
       </c>
     </row>
-    <row r="53" spans="3:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="3:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="3:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E56" s="205" t="s">
+    <row r="54" spans="3:74" ht="381.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="3:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="3:74" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E57" s="205" t="s">
         <v>83</v>
       </c>
-      <c r="F56" s="188"/>
-      <c r="G56" s="188"/>
-      <c r="H56" s="188"/>
-      <c r="I56" s="188"/>
-      <c r="J56" s="188"/>
-      <c r="K56" s="188"/>
-      <c r="L56" s="188"/>
-      <c r="M56" s="188"/>
-      <c r="N56" s="188"/>
-      <c r="O56" s="188"/>
-      <c r="P56" s="188"/>
-      <c r="Q56" s="188"/>
-      <c r="R56" s="188"/>
-      <c r="S56" s="188"/>
-      <c r="T56" s="188"/>
-      <c r="U56" s="188"/>
-      <c r="V56" s="188"/>
-      <c r="W56" s="188"/>
-      <c r="X56" s="188"/>
-      <c r="Y56" s="188"/>
-      <c r="Z56" s="188"/>
-      <c r="AA56" s="188"/>
-      <c r="AB56" s="188"/>
-      <c r="AC56" s="188"/>
-      <c r="AD56" s="188"/>
-      <c r="AE56" s="188"/>
-      <c r="AF56" s="188"/>
-      <c r="AG56" s="188"/>
-      <c r="AH56" s="188"/>
-      <c r="AI56" s="188"/>
-      <c r="AJ56" s="188"/>
-      <c r="AK56" s="188"/>
-      <c r="AL56" s="188"/>
-      <c r="AM56" s="188"/>
-      <c r="AN56" s="188"/>
-      <c r="AO56" s="188"/>
-      <c r="AP56" s="188"/>
-      <c r="AQ56" s="188"/>
-      <c r="AR56" s="188"/>
-      <c r="AS56" s="188"/>
-      <c r="AT56" s="188"/>
-      <c r="AU56" s="188"/>
-      <c r="AV56" s="188"/>
-      <c r="AW56" s="188"/>
-      <c r="AX56" s="188"/>
-      <c r="AY56" s="188"/>
-      <c r="AZ56" s="188"/>
-      <c r="BA56" s="188"/>
-      <c r="BB56" s="189"/>
+      <c r="F57" s="169"/>
+      <c r="G57" s="169"/>
+      <c r="H57" s="169"/>
+      <c r="I57" s="169"/>
+      <c r="J57" s="169"/>
+      <c r="K57" s="169"/>
+      <c r="L57" s="169"/>
+      <c r="M57" s="169"/>
+      <c r="N57" s="169"/>
+      <c r="O57" s="169"/>
+      <c r="P57" s="169"/>
+      <c r="Q57" s="169"/>
+      <c r="R57" s="169"/>
+      <c r="S57" s="169"/>
+      <c r="T57" s="169"/>
+      <c r="U57" s="169"/>
+      <c r="V57" s="169"/>
+      <c r="W57" s="169"/>
+      <c r="X57" s="169"/>
+      <c r="Y57" s="169"/>
+      <c r="Z57" s="169"/>
+      <c r="AA57" s="169"/>
+      <c r="AB57" s="169"/>
+      <c r="AC57" s="169"/>
+      <c r="AD57" s="169"/>
+      <c r="AE57" s="169"/>
+      <c r="AF57" s="169"/>
+      <c r="AG57" s="169"/>
+      <c r="AH57" s="169"/>
+      <c r="AI57" s="169"/>
+      <c r="AJ57" s="169"/>
+      <c r="AK57" s="169"/>
+      <c r="AL57" s="169"/>
+      <c r="AM57" s="169"/>
+      <c r="AN57" s="169"/>
+      <c r="AO57" s="169"/>
+      <c r="AP57" s="169"/>
+      <c r="AQ57" s="169"/>
+      <c r="AR57" s="169"/>
+      <c r="AS57" s="169"/>
+      <c r="AT57" s="169"/>
+      <c r="AU57" s="169"/>
+      <c r="AV57" s="169"/>
+      <c r="AW57" s="169"/>
+      <c r="AX57" s="169"/>
+      <c r="AY57" s="169"/>
+      <c r="AZ57" s="169"/>
+      <c r="BA57" s="169"/>
+      <c r="BB57" s="170"/>
     </row>
-    <row r="57" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="3:74" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C61" s="108"/>
-      <c r="D61" s="108"/>
+    <row r="61" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="3:74" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C62" s="108"/>
+      <c r="D62" s="108"/>
     </row>
-    <row r="62" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="3:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18735,9 +18840,17 @@
     <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E56:BB56"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="E57:BB57"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
     <mergeCell ref="BP8:BT8"/>
@@ -18753,13 +18866,6 @@
     <mergeCell ref="AQ8:AU8"/>
     <mergeCell ref="AV8:AZ8"/>
     <mergeCell ref="BA8:BE8"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
user profile image almost finished (just a matter of conversion)
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE631D72-4E8C-4F0B-B999-F7AA0785FC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E632141D-8B2C-4186-90BD-A6C58A571114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="287">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -894,6 +894,9 @@
   </si>
   <si>
     <t>show user list for admin</t>
+  </si>
+  <si>
+    <t>Catalano and Di Paolo</t>
   </si>
 </sst>
 </file>
@@ -12578,8 +12581,8 @@
   </sheetPr>
   <dimension ref="B1:CN1017"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="CE54" sqref="CE54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12599,7 +12602,7 @@
     <col min="78" max="78" width="3" customWidth="1"/>
     <col min="79" max="79" width="3.125" customWidth="1"/>
     <col min="80" max="80" width="3.5" customWidth="1"/>
-    <col min="81" max="81" width="4.5" customWidth="1"/>
+    <col min="81" max="81" width="3" customWidth="1"/>
     <col min="82" max="83" width="3.5" customWidth="1"/>
     <col min="84" max="84" width="4" customWidth="1"/>
     <col min="85" max="85" width="3.25" customWidth="1"/>
@@ -18033,17 +18036,17 @@
         <v>276</v>
       </c>
       <c r="D48" s="176" t="s">
-        <v>208</v>
+        <v>286</v>
       </c>
       <c r="E48" s="170">
+        <v>8</v>
+      </c>
+      <c r="F48" s="170">
         <v>6</v>
-      </c>
-      <c r="F48" s="170">
-        <v>3</v>
       </c>
       <c r="G48" s="171">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H48" s="169">
         <v>4.5</v>
@@ -18058,7 +18061,7 @@
       </c>
       <c r="L48" s="174">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="M48" s="92"/>
       <c r="N48" s="92"/>
@@ -18128,7 +18131,7 @@
       <c r="BZ48" s="178"/>
       <c r="CA48" s="182"/>
       <c r="CB48" s="182"/>
-      <c r="CC48" s="182"/>
+      <c r="CC48" s="179"/>
       <c r="CD48" s="182"/>
       <c r="CE48" s="93"/>
       <c r="CF48" s="93"/>
@@ -20592,8 +20595,8 @@
   </sheetPr>
   <dimension ref="B1:K999"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="74" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showGridLines="0" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
users list for admin completed
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E632141D-8B2C-4186-90BD-A6C58A571114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D11C9A-3738-49AD-8584-FD57760943B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2751,11 +2751,53 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="34" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2786,48 +2828,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="29" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7359,19 +7359,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="192" t="str">
+      <c r="BK2" s="210" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="193"/>
-      <c r="BM2" s="193"/>
-      <c r="BN2" s="193"/>
-      <c r="BO2" s="193"/>
-      <c r="BP2" s="193"/>
-      <c r="BQ2" s="193"/>
-      <c r="BR2" s="193"/>
-      <c r="BS2" s="193"/>
-      <c r="BT2" s="193"/>
+      <c r="BL2" s="211"/>
+      <c r="BM2" s="211"/>
+      <c r="BN2" s="211"/>
+      <c r="BO2" s="211"/>
+      <c r="BP2" s="211"/>
+      <c r="BQ2" s="211"/>
+      <c r="BR2" s="211"/>
+      <c r="BS2" s="211"/>
+      <c r="BT2" s="211"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -7399,7 +7399,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="194" t="s">
+      <c r="K4" s="212" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7476,7 +7476,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="195"/>
+      <c r="K5" s="213"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7551,7 +7551,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="195"/>
+      <c r="K6" s="213"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7626,7 +7626,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="195"/>
+      <c r="K7" s="213"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7701,7 +7701,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="196"/>
+      <c r="K8" s="214"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7767,124 +7767,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="197" t="s">
+      <c r="B9" s="215" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="199" t="s">
+      <c r="C9" s="217" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="201" t="s">
+      <c r="D9" s="219" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="203" t="s">
+      <c r="E9" s="221" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="204"/>
-      <c r="G9" s="205"/>
-      <c r="H9" s="206" t="s">
+      <c r="F9" s="222"/>
+      <c r="G9" s="223"/>
+      <c r="H9" s="224" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="211" t="s">
+      <c r="I9" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="213" t="s">
+      <c r="J9" s="194" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="215" t="s">
+      <c r="K9" s="196" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="216" t="s">
+      <c r="L9" s="197" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="218" t="s">
+      <c r="M9" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="190"/>
-      <c r="O9" s="190"/>
-      <c r="P9" s="190"/>
-      <c r="Q9" s="219"/>
-      <c r="R9" s="220" t="s">
+      <c r="N9" s="200"/>
+      <c r="O9" s="200"/>
+      <c r="P9" s="200"/>
+      <c r="Q9" s="201"/>
+      <c r="R9" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="190"/>
-      <c r="T9" s="190"/>
-      <c r="U9" s="190"/>
-      <c r="V9" s="219"/>
-      <c r="W9" s="220" t="s">
+      <c r="S9" s="200"/>
+      <c r="T9" s="200"/>
+      <c r="U9" s="200"/>
+      <c r="V9" s="201"/>
+      <c r="W9" s="202" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="190"/>
-      <c r="Y9" s="190"/>
-      <c r="Z9" s="190"/>
-      <c r="AA9" s="191"/>
-      <c r="AB9" s="221" t="s">
+      <c r="X9" s="200"/>
+      <c r="Y9" s="200"/>
+      <c r="Z9" s="200"/>
+      <c r="AA9" s="203"/>
+      <c r="AB9" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="190"/>
-      <c r="AD9" s="190"/>
-      <c r="AE9" s="190"/>
-      <c r="AF9" s="219"/>
-      <c r="AG9" s="222" t="s">
+      <c r="AC9" s="200"/>
+      <c r="AD9" s="200"/>
+      <c r="AE9" s="200"/>
+      <c r="AF9" s="201"/>
+      <c r="AG9" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="190"/>
-      <c r="AI9" s="190"/>
-      <c r="AJ9" s="190"/>
-      <c r="AK9" s="219"/>
-      <c r="AL9" s="222" t="s">
+      <c r="AH9" s="200"/>
+      <c r="AI9" s="200"/>
+      <c r="AJ9" s="200"/>
+      <c r="AK9" s="201"/>
+      <c r="AL9" s="205" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="190"/>
-      <c r="AN9" s="190"/>
-      <c r="AO9" s="190"/>
-      <c r="AP9" s="191"/>
-      <c r="AQ9" s="223" t="s">
+      <c r="AM9" s="200"/>
+      <c r="AN9" s="200"/>
+      <c r="AO9" s="200"/>
+      <c r="AP9" s="203"/>
+      <c r="AQ9" s="206" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="190"/>
-      <c r="AS9" s="190"/>
-      <c r="AT9" s="190"/>
-      <c r="AU9" s="219"/>
-      <c r="AV9" s="224" t="s">
+      <c r="AR9" s="200"/>
+      <c r="AS9" s="200"/>
+      <c r="AT9" s="200"/>
+      <c r="AU9" s="201"/>
+      <c r="AV9" s="207" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="190"/>
-      <c r="AX9" s="190"/>
-      <c r="AY9" s="190"/>
-      <c r="AZ9" s="219"/>
-      <c r="BA9" s="224" t="s">
+      <c r="AW9" s="200"/>
+      <c r="AX9" s="200"/>
+      <c r="AY9" s="200"/>
+      <c r="AZ9" s="201"/>
+      <c r="BA9" s="207" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="190"/>
-      <c r="BC9" s="190"/>
-      <c r="BD9" s="190"/>
-      <c r="BE9" s="191"/>
-      <c r="BF9" s="225" t="s">
+      <c r="BB9" s="200"/>
+      <c r="BC9" s="200"/>
+      <c r="BD9" s="200"/>
+      <c r="BE9" s="203"/>
+      <c r="BF9" s="208" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="190"/>
-      <c r="BH9" s="190"/>
-      <c r="BI9" s="190"/>
-      <c r="BJ9" s="219"/>
-      <c r="BK9" s="189" t="s">
+      <c r="BG9" s="200"/>
+      <c r="BH9" s="200"/>
+      <c r="BI9" s="200"/>
+      <c r="BJ9" s="201"/>
+      <c r="BK9" s="209" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="190"/>
-      <c r="BM9" s="190"/>
-      <c r="BN9" s="190"/>
-      <c r="BO9" s="219"/>
-      <c r="BP9" s="189" t="s">
+      <c r="BL9" s="200"/>
+      <c r="BM9" s="200"/>
+      <c r="BN9" s="200"/>
+      <c r="BO9" s="201"/>
+      <c r="BP9" s="209" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="190"/>
-      <c r="BR9" s="190"/>
-      <c r="BS9" s="190"/>
-      <c r="BT9" s="191"/>
+      <c r="BQ9" s="200"/>
+      <c r="BR9" s="200"/>
+      <c r="BS9" s="200"/>
+      <c r="BT9" s="203"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="198"/>
-      <c r="C10" s="200"/>
-      <c r="D10" s="202"/>
+      <c r="B10" s="216"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="220"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7894,11 +7894,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="207"/>
-      <c r="I10" s="212"/>
-      <c r="J10" s="214"/>
-      <c r="K10" s="214"/>
-      <c r="L10" s="217"/>
+      <c r="H10" s="225"/>
+      <c r="I10" s="193"/>
+      <c r="J10" s="195"/>
+      <c r="K10" s="195"/>
+      <c r="L10" s="198"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11507,80 +11507,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="208" t="str">
+      <c r="B45" s="189" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="209"/>
-      <c r="D45" s="209"/>
-      <c r="E45" s="209"/>
-      <c r="F45" s="209"/>
-      <c r="G45" s="209"/>
-      <c r="H45" s="209"/>
-      <c r="I45" s="209"/>
-      <c r="J45" s="209"/>
-      <c r="K45" s="209"/>
-      <c r="L45" s="209"/>
-      <c r="M45" s="209"/>
-      <c r="N45" s="209"/>
-      <c r="O45" s="209"/>
-      <c r="P45" s="209"/>
-      <c r="Q45" s="209"/>
-      <c r="R45" s="209"/>
-      <c r="S45" s="209"/>
-      <c r="T45" s="209"/>
-      <c r="U45" s="209"/>
-      <c r="V45" s="209"/>
-      <c r="W45" s="209"/>
-      <c r="X45" s="209"/>
-      <c r="Y45" s="209"/>
-      <c r="Z45" s="209"/>
-      <c r="AA45" s="209"/>
-      <c r="AB45" s="209"/>
-      <c r="AC45" s="209"/>
-      <c r="AD45" s="209"/>
-      <c r="AE45" s="209"/>
-      <c r="AF45" s="209"/>
-      <c r="AG45" s="209"/>
-      <c r="AH45" s="209"/>
-      <c r="AI45" s="209"/>
-      <c r="AJ45" s="209"/>
-      <c r="AK45" s="209"/>
-      <c r="AL45" s="209"/>
-      <c r="AM45" s="209"/>
-      <c r="AN45" s="209"/>
-      <c r="AO45" s="209"/>
-      <c r="AP45" s="209"/>
-      <c r="AQ45" s="209"/>
-      <c r="AR45" s="209"/>
-      <c r="AS45" s="209"/>
-      <c r="AT45" s="209"/>
-      <c r="AU45" s="209"/>
-      <c r="AV45" s="209"/>
-      <c r="AW45" s="209"/>
-      <c r="AX45" s="209"/>
-      <c r="AY45" s="209"/>
-      <c r="AZ45" s="209"/>
-      <c r="BA45" s="209"/>
-      <c r="BB45" s="209"/>
-      <c r="BC45" s="209"/>
-      <c r="BD45" s="209"/>
-      <c r="BE45" s="209"/>
-      <c r="BF45" s="209"/>
-      <c r="BG45" s="209"/>
-      <c r="BH45" s="209"/>
-      <c r="BI45" s="209"/>
-      <c r="BJ45" s="209"/>
-      <c r="BK45" s="209"/>
-      <c r="BL45" s="209"/>
-      <c r="BM45" s="209"/>
-      <c r="BN45" s="209"/>
-      <c r="BO45" s="209"/>
-      <c r="BP45" s="209"/>
-      <c r="BQ45" s="209"/>
-      <c r="BR45" s="209"/>
-      <c r="BS45" s="209"/>
-      <c r="BT45" s="210"/>
+      <c r="C45" s="190"/>
+      <c r="D45" s="190"/>
+      <c r="E45" s="190"/>
+      <c r="F45" s="190"/>
+      <c r="G45" s="190"/>
+      <c r="H45" s="190"/>
+      <c r="I45" s="190"/>
+      <c r="J45" s="190"/>
+      <c r="K45" s="190"/>
+      <c r="L45" s="190"/>
+      <c r="M45" s="190"/>
+      <c r="N45" s="190"/>
+      <c r="O45" s="190"/>
+      <c r="P45" s="190"/>
+      <c r="Q45" s="190"/>
+      <c r="R45" s="190"/>
+      <c r="S45" s="190"/>
+      <c r="T45" s="190"/>
+      <c r="U45" s="190"/>
+      <c r="V45" s="190"/>
+      <c r="W45" s="190"/>
+      <c r="X45" s="190"/>
+      <c r="Y45" s="190"/>
+      <c r="Z45" s="190"/>
+      <c r="AA45" s="190"/>
+      <c r="AB45" s="190"/>
+      <c r="AC45" s="190"/>
+      <c r="AD45" s="190"/>
+      <c r="AE45" s="190"/>
+      <c r="AF45" s="190"/>
+      <c r="AG45" s="190"/>
+      <c r="AH45" s="190"/>
+      <c r="AI45" s="190"/>
+      <c r="AJ45" s="190"/>
+      <c r="AK45" s="190"/>
+      <c r="AL45" s="190"/>
+      <c r="AM45" s="190"/>
+      <c r="AN45" s="190"/>
+      <c r="AO45" s="190"/>
+      <c r="AP45" s="190"/>
+      <c r="AQ45" s="190"/>
+      <c r="AR45" s="190"/>
+      <c r="AS45" s="190"/>
+      <c r="AT45" s="190"/>
+      <c r="AU45" s="190"/>
+      <c r="AV45" s="190"/>
+      <c r="AW45" s="190"/>
+      <c r="AX45" s="190"/>
+      <c r="AY45" s="190"/>
+      <c r="AZ45" s="190"/>
+      <c r="BA45" s="190"/>
+      <c r="BB45" s="190"/>
+      <c r="BC45" s="190"/>
+      <c r="BD45" s="190"/>
+      <c r="BE45" s="190"/>
+      <c r="BF45" s="190"/>
+      <c r="BG45" s="190"/>
+      <c r="BH45" s="190"/>
+      <c r="BI45" s="190"/>
+      <c r="BJ45" s="190"/>
+      <c r="BK45" s="190"/>
+      <c r="BL45" s="190"/>
+      <c r="BM45" s="190"/>
+      <c r="BN45" s="190"/>
+      <c r="BO45" s="190"/>
+      <c r="BP45" s="190"/>
+      <c r="BQ45" s="190"/>
+      <c r="BR45" s="190"/>
+      <c r="BS45" s="190"/>
+      <c r="BT45" s="191"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12543,6 +12543,14 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12559,14 +12567,6 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12581,8 +12581,8 @@
   </sheetPr>
   <dimension ref="B1:CN1017"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CE54" sqref="CE54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="CD54" sqref="CD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12603,7 +12603,8 @@
     <col min="79" max="79" width="3.125" customWidth="1"/>
     <col min="80" max="80" width="3.5" customWidth="1"/>
     <col min="81" max="81" width="3" customWidth="1"/>
-    <col min="82" max="83" width="3.5" customWidth="1"/>
+    <col min="82" max="82" width="2.75" customWidth="1"/>
+    <col min="83" max="83" width="3.5" customWidth="1"/>
     <col min="84" max="84" width="4" customWidth="1"/>
     <col min="85" max="85" width="3.25" customWidth="1"/>
     <col min="86" max="86" width="4.25" customWidth="1"/>
@@ -12712,7 +12713,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="194" t="s">
+      <c r="K3" s="212" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12809,7 +12810,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="195"/>
+      <c r="K4" s="213"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12903,7 +12904,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="195"/>
+      <c r="K5" s="213"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12997,7 +12998,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="195"/>
+      <c r="K6" s="213"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -13092,7 +13093,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="196"/>
+      <c r="K7" s="214"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -13178,119 +13179,119 @@
       <c r="CN7" s="179"/>
     </row>
     <row r="8" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="197" t="s">
+      <c r="B8" s="215" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="199" t="s">
+      <c r="C8" s="217" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="201" t="s">
+      <c r="D8" s="219" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="203" t="s">
+      <c r="E8" s="221" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="204"/>
-      <c r="G8" s="205"/>
-      <c r="H8" s="206" t="s">
+      <c r="F8" s="222"/>
+      <c r="G8" s="223"/>
+      <c r="H8" s="224" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="211" t="s">
+      <c r="I8" s="192" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="213" t="s">
+      <c r="J8" s="194" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="215" t="s">
+      <c r="K8" s="196" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="216" t="s">
+      <c r="L8" s="197" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="218" t="s">
+      <c r="M8" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="190"/>
-      <c r="O8" s="190"/>
-      <c r="P8" s="190"/>
-      <c r="Q8" s="219"/>
-      <c r="R8" s="220" t="s">
+      <c r="N8" s="200"/>
+      <c r="O8" s="200"/>
+      <c r="P8" s="200"/>
+      <c r="Q8" s="201"/>
+      <c r="R8" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="190"/>
-      <c r="T8" s="190"/>
-      <c r="U8" s="190"/>
-      <c r="V8" s="219"/>
-      <c r="W8" s="220" t="s">
+      <c r="S8" s="200"/>
+      <c r="T8" s="200"/>
+      <c r="U8" s="200"/>
+      <c r="V8" s="201"/>
+      <c r="W8" s="202" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="190"/>
-      <c r="Y8" s="190"/>
-      <c r="Z8" s="190"/>
-      <c r="AA8" s="191"/>
-      <c r="AB8" s="221" t="s">
+      <c r="X8" s="200"/>
+      <c r="Y8" s="200"/>
+      <c r="Z8" s="200"/>
+      <c r="AA8" s="203"/>
+      <c r="AB8" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="190"/>
-      <c r="AD8" s="190"/>
-      <c r="AE8" s="190"/>
-      <c r="AF8" s="219"/>
-      <c r="AG8" s="222" t="s">
+      <c r="AC8" s="200"/>
+      <c r="AD8" s="200"/>
+      <c r="AE8" s="200"/>
+      <c r="AF8" s="201"/>
+      <c r="AG8" s="205" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="190"/>
-      <c r="AI8" s="190"/>
-      <c r="AJ8" s="190"/>
-      <c r="AK8" s="219"/>
-      <c r="AL8" s="222" t="s">
+      <c r="AH8" s="200"/>
+      <c r="AI8" s="200"/>
+      <c r="AJ8" s="200"/>
+      <c r="AK8" s="201"/>
+      <c r="AL8" s="205" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="190"/>
-      <c r="AN8" s="190"/>
-      <c r="AO8" s="190"/>
-      <c r="AP8" s="191"/>
-      <c r="AQ8" s="223" t="s">
+      <c r="AM8" s="200"/>
+      <c r="AN8" s="200"/>
+      <c r="AO8" s="200"/>
+      <c r="AP8" s="203"/>
+      <c r="AQ8" s="206" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="190"/>
-      <c r="AS8" s="190"/>
-      <c r="AT8" s="190"/>
-      <c r="AU8" s="219"/>
-      <c r="AV8" s="224" t="s">
+      <c r="AR8" s="200"/>
+      <c r="AS8" s="200"/>
+      <c r="AT8" s="200"/>
+      <c r="AU8" s="201"/>
+      <c r="AV8" s="207" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="190"/>
-      <c r="AX8" s="190"/>
-      <c r="AY8" s="190"/>
-      <c r="AZ8" s="219"/>
-      <c r="BA8" s="224" t="s">
+      <c r="AW8" s="200"/>
+      <c r="AX8" s="200"/>
+      <c r="AY8" s="200"/>
+      <c r="AZ8" s="201"/>
+      <c r="BA8" s="207" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="190"/>
-      <c r="BC8" s="190"/>
-      <c r="BD8" s="190"/>
-      <c r="BE8" s="191"/>
+      <c r="BB8" s="200"/>
+      <c r="BC8" s="200"/>
+      <c r="BD8" s="200"/>
+      <c r="BE8" s="203"/>
       <c r="BF8" s="230" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="190"/>
-      <c r="BH8" s="190"/>
-      <c r="BI8" s="190"/>
-      <c r="BJ8" s="219"/>
-      <c r="BK8" s="189" t="s">
+      <c r="BG8" s="200"/>
+      <c r="BH8" s="200"/>
+      <c r="BI8" s="200"/>
+      <c r="BJ8" s="201"/>
+      <c r="BK8" s="209" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="190"/>
-      <c r="BM8" s="190"/>
-      <c r="BN8" s="190"/>
-      <c r="BO8" s="219"/>
-      <c r="BP8" s="189" t="s">
+      <c r="BL8" s="200"/>
+      <c r="BM8" s="200"/>
+      <c r="BN8" s="200"/>
+      <c r="BO8" s="201"/>
+      <c r="BP8" s="209" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="190"/>
-      <c r="BR8" s="190"/>
-      <c r="BS8" s="190"/>
-      <c r="BT8" s="191"/>
+      <c r="BQ8" s="200"/>
+      <c r="BR8" s="200"/>
+      <c r="BS8" s="200"/>
+      <c r="BT8" s="203"/>
       <c r="BU8" s="226" t="s">
         <v>278</v>
       </c>
@@ -13321,9 +13322,9 @@
       <c r="CN8" s="228"/>
     </row>
     <row r="9" spans="2:92" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="198"/>
-      <c r="C9" s="200"/>
-      <c r="D9" s="202"/>
+      <c r="B9" s="216"/>
+      <c r="C9" s="218"/>
+      <c r="D9" s="220"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -13333,11 +13334,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="207"/>
-      <c r="I9" s="212"/>
-      <c r="J9" s="214"/>
-      <c r="K9" s="214"/>
-      <c r="L9" s="217"/>
+      <c r="H9" s="225"/>
+      <c r="I9" s="193"/>
+      <c r="J9" s="195"/>
+      <c r="K9" s="195"/>
+      <c r="L9" s="198"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -18383,11 +18384,11 @@
         <v>5</v>
       </c>
       <c r="F51" s="85">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G51" s="86">
         <f t="shared" ref="G51" si="16">E51-F51</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H51" s="87">
         <v>5</v>
@@ -18395,14 +18396,16 @@
       <c r="I51" s="88">
         <v>45503</v>
       </c>
-      <c r="J51" s="89"/>
+      <c r="J51" s="89">
+        <v>45506</v>
+      </c>
       <c r="K51" s="90">
         <f t="shared" ref="K51" si="17">J51-I51+1</f>
-        <v>-45502</v>
+        <v>4</v>
       </c>
       <c r="L51" s="91">
         <f t="shared" ref="L51" si="18">F51/E51</f>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="M51" s="92"/>
       <c r="N51" s="93"/>
@@ -18473,7 +18476,7 @@
       <c r="CA51" s="179"/>
       <c r="CB51" s="178"/>
       <c r="CC51" s="65"/>
-      <c r="CD51" s="65"/>
+      <c r="CD51" s="179"/>
       <c r="CE51" s="65"/>
       <c r="CF51" s="65"/>
       <c r="CG51" s="178"/>
@@ -19541,55 +19544,55 @@
       <c r="E61" s="229" t="s">
         <v>83</v>
       </c>
-      <c r="F61" s="209"/>
-      <c r="G61" s="209"/>
-      <c r="H61" s="209"/>
-      <c r="I61" s="209"/>
-      <c r="J61" s="209"/>
-      <c r="K61" s="209"/>
-      <c r="L61" s="209"/>
-      <c r="M61" s="209"/>
-      <c r="N61" s="209"/>
-      <c r="O61" s="209"/>
-      <c r="P61" s="209"/>
-      <c r="Q61" s="209"/>
-      <c r="R61" s="209"/>
-      <c r="S61" s="209"/>
-      <c r="T61" s="209"/>
-      <c r="U61" s="209"/>
-      <c r="V61" s="209"/>
-      <c r="W61" s="209"/>
-      <c r="X61" s="209"/>
-      <c r="Y61" s="209"/>
-      <c r="Z61" s="209"/>
-      <c r="AA61" s="209"/>
-      <c r="AB61" s="209"/>
-      <c r="AC61" s="209"/>
-      <c r="AD61" s="209"/>
-      <c r="AE61" s="209"/>
-      <c r="AF61" s="209"/>
-      <c r="AG61" s="209"/>
-      <c r="AH61" s="209"/>
-      <c r="AI61" s="209"/>
-      <c r="AJ61" s="209"/>
-      <c r="AK61" s="209"/>
-      <c r="AL61" s="209"/>
-      <c r="AM61" s="209"/>
-      <c r="AN61" s="209"/>
-      <c r="AO61" s="209"/>
-      <c r="AP61" s="209"/>
-      <c r="AQ61" s="209"/>
-      <c r="AR61" s="209"/>
-      <c r="AS61" s="209"/>
-      <c r="AT61" s="209"/>
-      <c r="AU61" s="209"/>
-      <c r="AV61" s="209"/>
-      <c r="AW61" s="209"/>
-      <c r="AX61" s="209"/>
-      <c r="AY61" s="209"/>
-      <c r="AZ61" s="209"/>
-      <c r="BA61" s="209"/>
-      <c r="BB61" s="210"/>
+      <c r="F61" s="190"/>
+      <c r="G61" s="190"/>
+      <c r="H61" s="190"/>
+      <c r="I61" s="190"/>
+      <c r="J61" s="190"/>
+      <c r="K61" s="190"/>
+      <c r="L61" s="190"/>
+      <c r="M61" s="190"/>
+      <c r="N61" s="190"/>
+      <c r="O61" s="190"/>
+      <c r="P61" s="190"/>
+      <c r="Q61" s="190"/>
+      <c r="R61" s="190"/>
+      <c r="S61" s="190"/>
+      <c r="T61" s="190"/>
+      <c r="U61" s="190"/>
+      <c r="V61" s="190"/>
+      <c r="W61" s="190"/>
+      <c r="X61" s="190"/>
+      <c r="Y61" s="190"/>
+      <c r="Z61" s="190"/>
+      <c r="AA61" s="190"/>
+      <c r="AB61" s="190"/>
+      <c r="AC61" s="190"/>
+      <c r="AD61" s="190"/>
+      <c r="AE61" s="190"/>
+      <c r="AF61" s="190"/>
+      <c r="AG61" s="190"/>
+      <c r="AH61" s="190"/>
+      <c r="AI61" s="190"/>
+      <c r="AJ61" s="190"/>
+      <c r="AK61" s="190"/>
+      <c r="AL61" s="190"/>
+      <c r="AM61" s="190"/>
+      <c r="AN61" s="190"/>
+      <c r="AO61" s="190"/>
+      <c r="AP61" s="190"/>
+      <c r="AQ61" s="190"/>
+      <c r="AR61" s="190"/>
+      <c r="AS61" s="190"/>
+      <c r="AT61" s="190"/>
+      <c r="AU61" s="190"/>
+      <c r="AV61" s="190"/>
+      <c r="AW61" s="190"/>
+      <c r="AX61" s="190"/>
+      <c r="AY61" s="190"/>
+      <c r="AZ61" s="190"/>
+      <c r="BA61" s="190"/>
+      <c r="BB61" s="191"/>
     </row>
     <row r="62" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20552,6 +20555,17 @@
     <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="AL8:AP8"/>
+    <mergeCell ref="AQ8:AU8"/>
+    <mergeCell ref="AV8:AZ8"/>
+    <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
     <mergeCell ref="BU8:BY8"/>
     <mergeCell ref="BZ8:CD8"/>
     <mergeCell ref="CE8:CI8"/>
@@ -20568,17 +20582,6 @@
     <mergeCell ref="W8:AA8"/>
     <mergeCell ref="AB8:AF8"/>
     <mergeCell ref="AG8:AK8"/>
-    <mergeCell ref="AL8:AP8"/>
-    <mergeCell ref="AQ8:AU8"/>
-    <mergeCell ref="AV8:AZ8"/>
-    <mergeCell ref="BA8:BE8"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22310,18 +22313,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20 G26 G3:G18 G23 G28:G35">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="formula" val="$I$3"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G21">
     <cfRule type="colorScale" priority="12">
       <colorScale>
@@ -22378,6 +22369,18 @@
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G26 G20 G3:G18 G23 G28:G35">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="formula" val="$I$3"/>
         <cfvo type="formula" val="$I$4"/>
         <cfvo type="formula" val="$I$5"/>
         <color rgb="FFF8E5DA"/>

</xml_diff>

<commit_message>
user profile image and admin users list completed
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D11C9A-3738-49AD-8584-FD57760943B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4992212A-A1DF-458E-B161-B65AC95C59D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2751,53 +2751,11 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="34" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2828,6 +2786,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="29" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7359,19 +7359,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="210" t="str">
+      <c r="BK2" s="192" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="211"/>
-      <c r="BM2" s="211"/>
-      <c r="BN2" s="211"/>
-      <c r="BO2" s="211"/>
-      <c r="BP2" s="211"/>
-      <c r="BQ2" s="211"/>
-      <c r="BR2" s="211"/>
-      <c r="BS2" s="211"/>
-      <c r="BT2" s="211"/>
+      <c r="BL2" s="193"/>
+      <c r="BM2" s="193"/>
+      <c r="BN2" s="193"/>
+      <c r="BO2" s="193"/>
+      <c r="BP2" s="193"/>
+      <c r="BQ2" s="193"/>
+      <c r="BR2" s="193"/>
+      <c r="BS2" s="193"/>
+      <c r="BT2" s="193"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -7399,7 +7399,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="212" t="s">
+      <c r="K4" s="194" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7476,7 +7476,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="213"/>
+      <c r="K5" s="195"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7551,7 +7551,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="213"/>
+      <c r="K6" s="195"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7626,7 +7626,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="213"/>
+      <c r="K7" s="195"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7701,7 +7701,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="214"/>
+      <c r="K8" s="196"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7767,124 +7767,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="215" t="s">
+      <c r="B9" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="217" t="s">
+      <c r="C9" s="199" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="219" t="s">
+      <c r="D9" s="201" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="221" t="s">
+      <c r="E9" s="203" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="222"/>
-      <c r="G9" s="223"/>
-      <c r="H9" s="224" t="s">
+      <c r="F9" s="204"/>
+      <c r="G9" s="205"/>
+      <c r="H9" s="206" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="192" t="s">
+      <c r="I9" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="194" t="s">
+      <c r="J9" s="213" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="196" t="s">
+      <c r="K9" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="197" t="s">
+      <c r="L9" s="216" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="199" t="s">
+      <c r="M9" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="200"/>
-      <c r="O9" s="200"/>
-      <c r="P9" s="200"/>
-      <c r="Q9" s="201"/>
-      <c r="R9" s="202" t="s">
+      <c r="N9" s="190"/>
+      <c r="O9" s="190"/>
+      <c r="P9" s="190"/>
+      <c r="Q9" s="219"/>
+      <c r="R9" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="200"/>
-      <c r="T9" s="200"/>
-      <c r="U9" s="200"/>
-      <c r="V9" s="201"/>
-      <c r="W9" s="202" t="s">
+      <c r="S9" s="190"/>
+      <c r="T9" s="190"/>
+      <c r="U9" s="190"/>
+      <c r="V9" s="219"/>
+      <c r="W9" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="200"/>
-      <c r="Y9" s="200"/>
-      <c r="Z9" s="200"/>
-      <c r="AA9" s="203"/>
-      <c r="AB9" s="204" t="s">
+      <c r="X9" s="190"/>
+      <c r="Y9" s="190"/>
+      <c r="Z9" s="190"/>
+      <c r="AA9" s="191"/>
+      <c r="AB9" s="221" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="200"/>
-      <c r="AD9" s="200"/>
-      <c r="AE9" s="200"/>
-      <c r="AF9" s="201"/>
-      <c r="AG9" s="205" t="s">
+      <c r="AC9" s="190"/>
+      <c r="AD9" s="190"/>
+      <c r="AE9" s="190"/>
+      <c r="AF9" s="219"/>
+      <c r="AG9" s="222" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="200"/>
-      <c r="AI9" s="200"/>
-      <c r="AJ9" s="200"/>
-      <c r="AK9" s="201"/>
-      <c r="AL9" s="205" t="s">
+      <c r="AH9" s="190"/>
+      <c r="AI9" s="190"/>
+      <c r="AJ9" s="190"/>
+      <c r="AK9" s="219"/>
+      <c r="AL9" s="222" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="200"/>
-      <c r="AN9" s="200"/>
-      <c r="AO9" s="200"/>
-      <c r="AP9" s="203"/>
-      <c r="AQ9" s="206" t="s">
+      <c r="AM9" s="190"/>
+      <c r="AN9" s="190"/>
+      <c r="AO9" s="190"/>
+      <c r="AP9" s="191"/>
+      <c r="AQ9" s="223" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="200"/>
-      <c r="AS9" s="200"/>
-      <c r="AT9" s="200"/>
-      <c r="AU9" s="201"/>
-      <c r="AV9" s="207" t="s">
+      <c r="AR9" s="190"/>
+      <c r="AS9" s="190"/>
+      <c r="AT9" s="190"/>
+      <c r="AU9" s="219"/>
+      <c r="AV9" s="224" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="200"/>
-      <c r="AX9" s="200"/>
-      <c r="AY9" s="200"/>
-      <c r="AZ9" s="201"/>
-      <c r="BA9" s="207" t="s">
+      <c r="AW9" s="190"/>
+      <c r="AX9" s="190"/>
+      <c r="AY9" s="190"/>
+      <c r="AZ9" s="219"/>
+      <c r="BA9" s="224" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="200"/>
-      <c r="BC9" s="200"/>
-      <c r="BD9" s="200"/>
-      <c r="BE9" s="203"/>
-      <c r="BF9" s="208" t="s">
+      <c r="BB9" s="190"/>
+      <c r="BC9" s="190"/>
+      <c r="BD9" s="190"/>
+      <c r="BE9" s="191"/>
+      <c r="BF9" s="225" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="200"/>
-      <c r="BH9" s="200"/>
-      <c r="BI9" s="200"/>
-      <c r="BJ9" s="201"/>
-      <c r="BK9" s="209" t="s">
+      <c r="BG9" s="190"/>
+      <c r="BH9" s="190"/>
+      <c r="BI9" s="190"/>
+      <c r="BJ9" s="219"/>
+      <c r="BK9" s="189" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="200"/>
-      <c r="BM9" s="200"/>
-      <c r="BN9" s="200"/>
-      <c r="BO9" s="201"/>
-      <c r="BP9" s="209" t="s">
+      <c r="BL9" s="190"/>
+      <c r="BM9" s="190"/>
+      <c r="BN9" s="190"/>
+      <c r="BO9" s="219"/>
+      <c r="BP9" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="200"/>
-      <c r="BR9" s="200"/>
-      <c r="BS9" s="200"/>
-      <c r="BT9" s="203"/>
+      <c r="BQ9" s="190"/>
+      <c r="BR9" s="190"/>
+      <c r="BS9" s="190"/>
+      <c r="BT9" s="191"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="216"/>
-      <c r="C10" s="218"/>
-      <c r="D10" s="220"/>
+      <c r="B10" s="198"/>
+      <c r="C10" s="200"/>
+      <c r="D10" s="202"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -7894,11 +7894,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="225"/>
-      <c r="I10" s="193"/>
-      <c r="J10" s="195"/>
-      <c r="K10" s="195"/>
-      <c r="L10" s="198"/>
+      <c r="H10" s="207"/>
+      <c r="I10" s="212"/>
+      <c r="J10" s="214"/>
+      <c r="K10" s="214"/>
+      <c r="L10" s="217"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11507,80 +11507,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="189" t="str">
+      <c r="B45" s="208" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="190"/>
-      <c r="D45" s="190"/>
-      <c r="E45" s="190"/>
-      <c r="F45" s="190"/>
-      <c r="G45" s="190"/>
-      <c r="H45" s="190"/>
-      <c r="I45" s="190"/>
-      <c r="J45" s="190"/>
-      <c r="K45" s="190"/>
-      <c r="L45" s="190"/>
-      <c r="M45" s="190"/>
-      <c r="N45" s="190"/>
-      <c r="O45" s="190"/>
-      <c r="P45" s="190"/>
-      <c r="Q45" s="190"/>
-      <c r="R45" s="190"/>
-      <c r="S45" s="190"/>
-      <c r="T45" s="190"/>
-      <c r="U45" s="190"/>
-      <c r="V45" s="190"/>
-      <c r="W45" s="190"/>
-      <c r="X45" s="190"/>
-      <c r="Y45" s="190"/>
-      <c r="Z45" s="190"/>
-      <c r="AA45" s="190"/>
-      <c r="AB45" s="190"/>
-      <c r="AC45" s="190"/>
-      <c r="AD45" s="190"/>
-      <c r="AE45" s="190"/>
-      <c r="AF45" s="190"/>
-      <c r="AG45" s="190"/>
-      <c r="AH45" s="190"/>
-      <c r="AI45" s="190"/>
-      <c r="AJ45" s="190"/>
-      <c r="AK45" s="190"/>
-      <c r="AL45" s="190"/>
-      <c r="AM45" s="190"/>
-      <c r="AN45" s="190"/>
-      <c r="AO45" s="190"/>
-      <c r="AP45" s="190"/>
-      <c r="AQ45" s="190"/>
-      <c r="AR45" s="190"/>
-      <c r="AS45" s="190"/>
-      <c r="AT45" s="190"/>
-      <c r="AU45" s="190"/>
-      <c r="AV45" s="190"/>
-      <c r="AW45" s="190"/>
-      <c r="AX45" s="190"/>
-      <c r="AY45" s="190"/>
-      <c r="AZ45" s="190"/>
-      <c r="BA45" s="190"/>
-      <c r="BB45" s="190"/>
-      <c r="BC45" s="190"/>
-      <c r="BD45" s="190"/>
-      <c r="BE45" s="190"/>
-      <c r="BF45" s="190"/>
-      <c r="BG45" s="190"/>
-      <c r="BH45" s="190"/>
-      <c r="BI45" s="190"/>
-      <c r="BJ45" s="190"/>
-      <c r="BK45" s="190"/>
-      <c r="BL45" s="190"/>
-      <c r="BM45" s="190"/>
-      <c r="BN45" s="190"/>
-      <c r="BO45" s="190"/>
-      <c r="BP45" s="190"/>
-      <c r="BQ45" s="190"/>
-      <c r="BR45" s="190"/>
-      <c r="BS45" s="190"/>
-      <c r="BT45" s="191"/>
+      <c r="C45" s="209"/>
+      <c r="D45" s="209"/>
+      <c r="E45" s="209"/>
+      <c r="F45" s="209"/>
+      <c r="G45" s="209"/>
+      <c r="H45" s="209"/>
+      <c r="I45" s="209"/>
+      <c r="J45" s="209"/>
+      <c r="K45" s="209"/>
+      <c r="L45" s="209"/>
+      <c r="M45" s="209"/>
+      <c r="N45" s="209"/>
+      <c r="O45" s="209"/>
+      <c r="P45" s="209"/>
+      <c r="Q45" s="209"/>
+      <c r="R45" s="209"/>
+      <c r="S45" s="209"/>
+      <c r="T45" s="209"/>
+      <c r="U45" s="209"/>
+      <c r="V45" s="209"/>
+      <c r="W45" s="209"/>
+      <c r="X45" s="209"/>
+      <c r="Y45" s="209"/>
+      <c r="Z45" s="209"/>
+      <c r="AA45" s="209"/>
+      <c r="AB45" s="209"/>
+      <c r="AC45" s="209"/>
+      <c r="AD45" s="209"/>
+      <c r="AE45" s="209"/>
+      <c r="AF45" s="209"/>
+      <c r="AG45" s="209"/>
+      <c r="AH45" s="209"/>
+      <c r="AI45" s="209"/>
+      <c r="AJ45" s="209"/>
+      <c r="AK45" s="209"/>
+      <c r="AL45" s="209"/>
+      <c r="AM45" s="209"/>
+      <c r="AN45" s="209"/>
+      <c r="AO45" s="209"/>
+      <c r="AP45" s="209"/>
+      <c r="AQ45" s="209"/>
+      <c r="AR45" s="209"/>
+      <c r="AS45" s="209"/>
+      <c r="AT45" s="209"/>
+      <c r="AU45" s="209"/>
+      <c r="AV45" s="209"/>
+      <c r="AW45" s="209"/>
+      <c r="AX45" s="209"/>
+      <c r="AY45" s="209"/>
+      <c r="AZ45" s="209"/>
+      <c r="BA45" s="209"/>
+      <c r="BB45" s="209"/>
+      <c r="BC45" s="209"/>
+      <c r="BD45" s="209"/>
+      <c r="BE45" s="209"/>
+      <c r="BF45" s="209"/>
+      <c r="BG45" s="209"/>
+      <c r="BH45" s="209"/>
+      <c r="BI45" s="209"/>
+      <c r="BJ45" s="209"/>
+      <c r="BK45" s="209"/>
+      <c r="BL45" s="209"/>
+      <c r="BM45" s="209"/>
+      <c r="BN45" s="209"/>
+      <c r="BO45" s="209"/>
+      <c r="BP45" s="209"/>
+      <c r="BQ45" s="209"/>
+      <c r="BR45" s="209"/>
+      <c r="BS45" s="209"/>
+      <c r="BT45" s="210"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12543,14 +12543,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12567,6 +12559,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12581,8 +12581,8 @@
   </sheetPr>
   <dimension ref="B1:CN1017"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CD54" sqref="CD54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12713,7 +12713,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="212" t="s">
+      <c r="K3" s="194" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12810,7 +12810,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="213"/>
+      <c r="K4" s="195"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -12904,7 +12904,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="213"/>
+      <c r="K5" s="195"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -12998,7 +12998,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="213"/>
+      <c r="K6" s="195"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -13093,7 +13093,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="214"/>
+      <c r="K7" s="196"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -13179,119 +13179,119 @@
       <c r="CN7" s="179"/>
     </row>
     <row r="8" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="215" t="s">
+      <c r="B8" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="217" t="s">
+      <c r="C8" s="199" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="219" t="s">
+      <c r="D8" s="201" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="221" t="s">
+      <c r="E8" s="203" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="222"/>
-      <c r="G8" s="223"/>
-      <c r="H8" s="224" t="s">
+      <c r="F8" s="204"/>
+      <c r="G8" s="205"/>
+      <c r="H8" s="206" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="192" t="s">
+      <c r="I8" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="194" t="s">
+      <c r="J8" s="213" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="196" t="s">
+      <c r="K8" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="197" t="s">
+      <c r="L8" s="216" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="199" t="s">
+      <c r="M8" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="200"/>
-      <c r="O8" s="200"/>
-      <c r="P8" s="200"/>
-      <c r="Q8" s="201"/>
-      <c r="R8" s="202" t="s">
+      <c r="N8" s="190"/>
+      <c r="O8" s="190"/>
+      <c r="P8" s="190"/>
+      <c r="Q8" s="219"/>
+      <c r="R8" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="200"/>
-      <c r="T8" s="200"/>
-      <c r="U8" s="200"/>
-      <c r="V8" s="201"/>
-      <c r="W8" s="202" t="s">
+      <c r="S8" s="190"/>
+      <c r="T8" s="190"/>
+      <c r="U8" s="190"/>
+      <c r="V8" s="219"/>
+      <c r="W8" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="200"/>
-      <c r="Y8" s="200"/>
-      <c r="Z8" s="200"/>
-      <c r="AA8" s="203"/>
-      <c r="AB8" s="204" t="s">
+      <c r="X8" s="190"/>
+      <c r="Y8" s="190"/>
+      <c r="Z8" s="190"/>
+      <c r="AA8" s="191"/>
+      <c r="AB8" s="221" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="200"/>
-      <c r="AD8" s="200"/>
-      <c r="AE8" s="200"/>
-      <c r="AF8" s="201"/>
-      <c r="AG8" s="205" t="s">
+      <c r="AC8" s="190"/>
+      <c r="AD8" s="190"/>
+      <c r="AE8" s="190"/>
+      <c r="AF8" s="219"/>
+      <c r="AG8" s="222" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="200"/>
-      <c r="AI8" s="200"/>
-      <c r="AJ8" s="200"/>
-      <c r="AK8" s="201"/>
-      <c r="AL8" s="205" t="s">
+      <c r="AH8" s="190"/>
+      <c r="AI8" s="190"/>
+      <c r="AJ8" s="190"/>
+      <c r="AK8" s="219"/>
+      <c r="AL8" s="222" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="200"/>
-      <c r="AN8" s="200"/>
-      <c r="AO8" s="200"/>
-      <c r="AP8" s="203"/>
-      <c r="AQ8" s="206" t="s">
+      <c r="AM8" s="190"/>
+      <c r="AN8" s="190"/>
+      <c r="AO8" s="190"/>
+      <c r="AP8" s="191"/>
+      <c r="AQ8" s="223" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="200"/>
-      <c r="AS8" s="200"/>
-      <c r="AT8" s="200"/>
-      <c r="AU8" s="201"/>
-      <c r="AV8" s="207" t="s">
+      <c r="AR8" s="190"/>
+      <c r="AS8" s="190"/>
+      <c r="AT8" s="190"/>
+      <c r="AU8" s="219"/>
+      <c r="AV8" s="224" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="200"/>
-      <c r="AX8" s="200"/>
-      <c r="AY8" s="200"/>
-      <c r="AZ8" s="201"/>
-      <c r="BA8" s="207" t="s">
+      <c r="AW8" s="190"/>
+      <c r="AX8" s="190"/>
+      <c r="AY8" s="190"/>
+      <c r="AZ8" s="219"/>
+      <c r="BA8" s="224" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="200"/>
-      <c r="BC8" s="200"/>
-      <c r="BD8" s="200"/>
-      <c r="BE8" s="203"/>
+      <c r="BB8" s="190"/>
+      <c r="BC8" s="190"/>
+      <c r="BD8" s="190"/>
+      <c r="BE8" s="191"/>
       <c r="BF8" s="230" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="200"/>
-      <c r="BH8" s="200"/>
-      <c r="BI8" s="200"/>
-      <c r="BJ8" s="201"/>
-      <c r="BK8" s="209" t="s">
+      <c r="BG8" s="190"/>
+      <c r="BH8" s="190"/>
+      <c r="BI8" s="190"/>
+      <c r="BJ8" s="219"/>
+      <c r="BK8" s="189" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="200"/>
-      <c r="BM8" s="200"/>
-      <c r="BN8" s="200"/>
-      <c r="BO8" s="201"/>
-      <c r="BP8" s="209" t="s">
+      <c r="BL8" s="190"/>
+      <c r="BM8" s="190"/>
+      <c r="BN8" s="190"/>
+      <c r="BO8" s="219"/>
+      <c r="BP8" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="200"/>
-      <c r="BR8" s="200"/>
-      <c r="BS8" s="200"/>
-      <c r="BT8" s="203"/>
+      <c r="BQ8" s="190"/>
+      <c r="BR8" s="190"/>
+      <c r="BS8" s="190"/>
+      <c r="BT8" s="191"/>
       <c r="BU8" s="226" t="s">
         <v>278</v>
       </c>
@@ -13322,9 +13322,9 @@
       <c r="CN8" s="228"/>
     </row>
     <row r="9" spans="2:92" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="216"/>
-      <c r="C9" s="218"/>
-      <c r="D9" s="220"/>
+      <c r="B9" s="198"/>
+      <c r="C9" s="200"/>
+      <c r="D9" s="202"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -13334,11 +13334,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="225"/>
-      <c r="I9" s="193"/>
-      <c r="J9" s="195"/>
-      <c r="K9" s="195"/>
-      <c r="L9" s="198"/>
+      <c r="H9" s="207"/>
+      <c r="I9" s="212"/>
+      <c r="J9" s="214"/>
+      <c r="K9" s="214"/>
+      <c r="L9" s="217"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -18055,10 +18055,12 @@
       <c r="I48" s="172">
         <v>45425</v>
       </c>
-      <c r="J48" s="172"/>
+      <c r="J48" s="172">
+        <v>45506</v>
+      </c>
       <c r="K48" s="173">
         <f t="shared" si="9"/>
-        <v>-45424</v>
+        <v>82</v>
       </c>
       <c r="L48" s="174">
         <f t="shared" si="0"/>
@@ -18133,7 +18135,7 @@
       <c r="CA48" s="182"/>
       <c r="CB48" s="182"/>
       <c r="CC48" s="179"/>
-      <c r="CD48" s="182"/>
+      <c r="CD48" s="179"/>
       <c r="CE48" s="93"/>
       <c r="CF48" s="93"/>
       <c r="CG48" s="93"/>
@@ -19544,55 +19546,55 @@
       <c r="E61" s="229" t="s">
         <v>83</v>
       </c>
-      <c r="F61" s="190"/>
-      <c r="G61" s="190"/>
-      <c r="H61" s="190"/>
-      <c r="I61" s="190"/>
-      <c r="J61" s="190"/>
-      <c r="K61" s="190"/>
-      <c r="L61" s="190"/>
-      <c r="M61" s="190"/>
-      <c r="N61" s="190"/>
-      <c r="O61" s="190"/>
-      <c r="P61" s="190"/>
-      <c r="Q61" s="190"/>
-      <c r="R61" s="190"/>
-      <c r="S61" s="190"/>
-      <c r="T61" s="190"/>
-      <c r="U61" s="190"/>
-      <c r="V61" s="190"/>
-      <c r="W61" s="190"/>
-      <c r="X61" s="190"/>
-      <c r="Y61" s="190"/>
-      <c r="Z61" s="190"/>
-      <c r="AA61" s="190"/>
-      <c r="AB61" s="190"/>
-      <c r="AC61" s="190"/>
-      <c r="AD61" s="190"/>
-      <c r="AE61" s="190"/>
-      <c r="AF61" s="190"/>
-      <c r="AG61" s="190"/>
-      <c r="AH61" s="190"/>
-      <c r="AI61" s="190"/>
-      <c r="AJ61" s="190"/>
-      <c r="AK61" s="190"/>
-      <c r="AL61" s="190"/>
-      <c r="AM61" s="190"/>
-      <c r="AN61" s="190"/>
-      <c r="AO61" s="190"/>
-      <c r="AP61" s="190"/>
-      <c r="AQ61" s="190"/>
-      <c r="AR61" s="190"/>
-      <c r="AS61" s="190"/>
-      <c r="AT61" s="190"/>
-      <c r="AU61" s="190"/>
-      <c r="AV61" s="190"/>
-      <c r="AW61" s="190"/>
-      <c r="AX61" s="190"/>
-      <c r="AY61" s="190"/>
-      <c r="AZ61" s="190"/>
-      <c r="BA61" s="190"/>
-      <c r="BB61" s="191"/>
+      <c r="F61" s="209"/>
+      <c r="G61" s="209"/>
+      <c r="H61" s="209"/>
+      <c r="I61" s="209"/>
+      <c r="J61" s="209"/>
+      <c r="K61" s="209"/>
+      <c r="L61" s="209"/>
+      <c r="M61" s="209"/>
+      <c r="N61" s="209"/>
+      <c r="O61" s="209"/>
+      <c r="P61" s="209"/>
+      <c r="Q61" s="209"/>
+      <c r="R61" s="209"/>
+      <c r="S61" s="209"/>
+      <c r="T61" s="209"/>
+      <c r="U61" s="209"/>
+      <c r="V61" s="209"/>
+      <c r="W61" s="209"/>
+      <c r="X61" s="209"/>
+      <c r="Y61" s="209"/>
+      <c r="Z61" s="209"/>
+      <c r="AA61" s="209"/>
+      <c r="AB61" s="209"/>
+      <c r="AC61" s="209"/>
+      <c r="AD61" s="209"/>
+      <c r="AE61" s="209"/>
+      <c r="AF61" s="209"/>
+      <c r="AG61" s="209"/>
+      <c r="AH61" s="209"/>
+      <c r="AI61" s="209"/>
+      <c r="AJ61" s="209"/>
+      <c r="AK61" s="209"/>
+      <c r="AL61" s="209"/>
+      <c r="AM61" s="209"/>
+      <c r="AN61" s="209"/>
+      <c r="AO61" s="209"/>
+      <c r="AP61" s="209"/>
+      <c r="AQ61" s="209"/>
+      <c r="AR61" s="209"/>
+      <c r="AS61" s="209"/>
+      <c r="AT61" s="209"/>
+      <c r="AU61" s="209"/>
+      <c r="AV61" s="209"/>
+      <c r="AW61" s="209"/>
+      <c r="AX61" s="209"/>
+      <c r="AY61" s="209"/>
+      <c r="AZ61" s="209"/>
+      <c r="BA61" s="209"/>
+      <c r="BB61" s="210"/>
     </row>
     <row r="62" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20555,17 +20557,6 @@
     <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="AL8:AP8"/>
-    <mergeCell ref="AQ8:AU8"/>
-    <mergeCell ref="AV8:AZ8"/>
-    <mergeCell ref="BA8:BE8"/>
-    <mergeCell ref="K3:K7"/>
     <mergeCell ref="BU8:BY8"/>
     <mergeCell ref="BZ8:CD8"/>
     <mergeCell ref="CE8:CI8"/>
@@ -20582,6 +20573,17 @@
     <mergeCell ref="W8:AA8"/>
     <mergeCell ref="AB8:AF8"/>
     <mergeCell ref="AG8:AK8"/>
+    <mergeCell ref="AL8:AP8"/>
+    <mergeCell ref="AQ8:AU8"/>
+    <mergeCell ref="AV8:AZ8"/>
+    <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22313,6 +22315,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G20 G26 G3:G18 G23 G28:G35">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="formula" val="$I$3"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G21">
     <cfRule type="colorScale" priority="12">
       <colorScale>
@@ -22369,18 +22383,6 @@
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G26 G20 G3:G18 G23 G28:G35">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="formula" val="$I$3"/>
         <cfvo type="formula" val="$I$4"/>
         <cfvo type="formula" val="$I$5"/>
         <color rgb="FFF8E5DA"/>

</xml_diff>

<commit_message>
deleting comments in forum
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\AnimalDex\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF032EB-2ADE-48C1-BAEA-00182C5291D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLE Gantt Chart &amp; Burndown" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
     <sheet name="Release Backlog" sheetId="3" r:id="rId3"/>
     <sheet name="User Stories or Tasks" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="309">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -951,12 +945,24 @@
   </si>
   <si>
     <t>Profile image update  and centralDB restructuring</t>
+  </si>
+  <si>
+    <t>forum delete comments and replies by user and admin</t>
+  </si>
+  <si>
+    <t>Catalano/Di Paolo</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2342,7 +2348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2795,53 +2801,12 @@
     <xf numFmtId="49" fontId="24" fillId="17" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2872,6 +2837,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="29" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2887,7 +2894,7 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="34">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2968,60 +2975,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFEB9C"/>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="0" shrinkToFit="0"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="0" shrinkToFit="0"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="0" shrinkToFit="0"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
       <alignment wrapText="0" shrinkToFit="0"/>
@@ -3637,7 +3590,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="1"/>
@@ -3669,6 +3622,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3732,7 +3686,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -4011,7 +3965,10 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6309-415A-9B2A-8CEC22EBC916}"/>
+            </c:ext>
             <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
               <c14:invertSolidFillFmt>
                 <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
@@ -4026,9 +3983,6 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6309-415A-9B2A-8CEC22EBC916}"/>
-            </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
@@ -4040,8 +3994,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="207150080"/>
-        <c:axId val="191458688"/>
+        <c:axId val="196275200"/>
+        <c:axId val="180579712"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4451,7 +4405,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6309-415A-9B2A-8CEC22EBC916}"/>
             </c:ext>
@@ -4862,7 +4816,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6309-415A-9B2A-8CEC22EBC916}"/>
             </c:ext>
@@ -5273,7 +5227,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6309-415A-9B2A-8CEC22EBC916}"/>
             </c:ext>
@@ -5289,11 +5243,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="207149568"/>
-        <c:axId val="191458112"/>
+        <c:axId val="196274688"/>
+        <c:axId val="180579136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="207149568"/>
+        <c:axId val="196274688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5317,6 +5271,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5338,7 +5293,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191458112"/>
+        <c:crossAx val="180579136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5346,7 +5301,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191458112"/>
+        <c:axId val="180579136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5390,6 +5345,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5414,12 +5370,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207149568"/>
+        <c:crossAx val="196274688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="207150080"/>
+        <c:axId val="196275200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5429,7 +5385,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191458688"/>
+        <c:crossAx val="180579712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5437,7 +5393,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191458688"/>
+        <c:axId val="180579712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5481,6 +5437,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5505,7 +5462,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="207150080"/>
+        <c:crossAx val="196275200"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5517,6 +5474,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -5552,7 +5510,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="1"/>
@@ -5584,6 +5542,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5598,7 +5557,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$59</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5647,7 +5606,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -5655,7 +5614,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$56:$BT$56</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$57:$BT$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5844,14 +5803,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$59:$BT$59</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$60:$BT$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0B83-4C3C-A1FB-BFF5EF056244}"/>
+            </c:ext>
             <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
               <c14:invertSolidFillFmt>
                 <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
@@ -5866,9 +5828,6 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0B83-4C3C-A1FB-BFF5EF056244}"/>
-            </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
@@ -5880,8 +5839,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="226655232"/>
-        <c:axId val="191462144"/>
+        <c:axId val="215710720"/>
+        <c:axId val="180583168"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5891,7 +5850,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$57</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5914,7 +5873,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$56:$BT$56</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$57:$BT$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6103,7 +6062,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$57:$BT$57</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$58:$BT$58</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6291,7 +6250,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0B83-4C3C-A1FB-BFF5EF056244}"/>
             </c:ext>
@@ -6302,7 +6261,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$58</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6325,7 +6284,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$56:$BT$56</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$57:$BT$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6514,7 +6473,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$58:$BT$58</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$59:$BT$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6702,7 +6661,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0B83-4C3C-A1FB-BFF5EF056244}"/>
             </c:ext>
@@ -6718,11 +6677,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="226654208"/>
-        <c:axId val="191461568"/>
+        <c:axId val="215709696"/>
+        <c:axId val="180582592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="226654208"/>
+        <c:axId val="215709696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6746,6 +6705,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6767,7 +6727,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191461568"/>
+        <c:crossAx val="180582592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6775,7 +6735,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191461568"/>
+        <c:axId val="180582592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6819,6 +6779,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6843,12 +6804,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226654208"/>
+        <c:crossAx val="215709696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="226655232"/>
+        <c:axId val="215710720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6858,7 +6819,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191462144"/>
+        <c:crossAx val="180583168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6866,7 +6827,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191462144"/>
+        <c:axId val="180583168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6910,6 +6871,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6934,7 +6896,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226655232"/>
+        <c:crossAx val="215710720"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6946,6 +6908,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -6995,7 +6958,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7026,7 +6989,7 @@
         <xdr:cNvPr id="3" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7056,7 +7019,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="27632025" cy="7553325"/>
@@ -7065,7 +7028,7 @@
         <xdr:cNvPr id="2" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7096,7 +7059,7 @@
         <xdr:cNvPr id="3" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7121,45 +7084,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella2" displayName="Tabella2" ref="B2:G38" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34">
-  <autoFilter ref="B2:G38" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabella2" displayName="Tabella2" ref="B2:G38" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
+  <autoFilter ref="B2:G38"/>
+  <sortState ref="B3:G38">
     <sortCondition ref="B2:B38"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SPRINT"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TASK TITLE"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TASK DESCRIPTION"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TASK OWNER"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="WORK ESTIMATE IN HOURS"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="STATUS"/>
+    <tableColumn id="1" name="SPRINT"/>
+    <tableColumn id="2" name="TASK TITLE"/>
+    <tableColumn id="3" name="TASK DESCRIPTION"/>
+    <tableColumn id="4" name="TASK OWNER"/>
+    <tableColumn id="5" name="WORK ESTIMATE IN HOURS"/>
+    <tableColumn id="6" name="STATUS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabella1" displayName="Tabella1" ref="B3:G43" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
-  <autoFilter ref="B3:G43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:G43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="B3:G43" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28">
+  <autoFilter ref="B3:G43"/>
+  <sortState ref="B4:G43">
     <sortCondition ref="D3:D43"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TASK TITLE" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="TASK DESCRIPTION" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="COMPONENT" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="PRIORITY" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ADDED BY" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="DATED ADDED" dataDxfId="25"/>
+    <tableColumn id="1" name="TASK TITLE" dataDxfId="27"/>
+    <tableColumn id="2" name="TASK DESCRIPTION" dataDxfId="26"/>
+    <tableColumn id="6" name="COMPONENT" dataDxfId="25"/>
+    <tableColumn id="3" name="PRIORITY" dataDxfId="24"/>
+    <tableColumn id="4" name="ADDED BY" dataDxfId="23"/>
+    <tableColumn id="5" name="DATED ADDED" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7197,7 +7160,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -7269,7 +7232,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7442,7 +7405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF7B3C16"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -7601,19 +7564,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="209" t="str">
+      <c r="BK2" s="192" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="210"/>
-      <c r="BM2" s="210"/>
-      <c r="BN2" s="210"/>
-      <c r="BO2" s="210"/>
-      <c r="BP2" s="210"/>
-      <c r="BQ2" s="210"/>
-      <c r="BR2" s="210"/>
-      <c r="BS2" s="210"/>
-      <c r="BT2" s="210"/>
+      <c r="BL2" s="193"/>
+      <c r="BM2" s="193"/>
+      <c r="BN2" s="193"/>
+      <c r="BO2" s="193"/>
+      <c r="BP2" s="193"/>
+      <c r="BQ2" s="193"/>
+      <c r="BR2" s="193"/>
+      <c r="BS2" s="193"/>
+      <c r="BT2" s="193"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -7641,7 +7604,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="211" t="s">
+      <c r="K4" s="194" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7718,7 +7681,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="212"/>
+      <c r="K5" s="195"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7793,7 +7756,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="212"/>
+      <c r="K6" s="195"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7868,7 +7831,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="212"/>
+      <c r="K7" s="195"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7943,7 +7906,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="213"/>
+      <c r="K8" s="196"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -8009,124 +7972,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="214" t="s">
+      <c r="B9" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="216" t="s">
+      <c r="C9" s="199" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="218" t="s">
+      <c r="D9" s="201" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="220" t="s">
+      <c r="E9" s="203" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="221"/>
-      <c r="G9" s="222"/>
-      <c r="H9" s="223" t="s">
+      <c r="F9" s="204"/>
+      <c r="G9" s="205"/>
+      <c r="H9" s="206" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="191" t="s">
+      <c r="I9" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="193" t="s">
+      <c r="J9" s="213" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="195" t="s">
+      <c r="K9" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="196" t="s">
+      <c r="L9" s="216" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="198" t="s">
+      <c r="M9" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="199"/>
-      <c r="O9" s="199"/>
-      <c r="P9" s="199"/>
-      <c r="Q9" s="200"/>
-      <c r="R9" s="201" t="s">
+      <c r="N9" s="190"/>
+      <c r="O9" s="190"/>
+      <c r="P9" s="190"/>
+      <c r="Q9" s="219"/>
+      <c r="R9" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="199"/>
-      <c r="T9" s="199"/>
-      <c r="U9" s="199"/>
-      <c r="V9" s="200"/>
-      <c r="W9" s="201" t="s">
+      <c r="S9" s="190"/>
+      <c r="T9" s="190"/>
+      <c r="U9" s="190"/>
+      <c r="V9" s="219"/>
+      <c r="W9" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="199"/>
-      <c r="Y9" s="199"/>
-      <c r="Z9" s="199"/>
-      <c r="AA9" s="202"/>
-      <c r="AB9" s="203" t="s">
+      <c r="X9" s="190"/>
+      <c r="Y9" s="190"/>
+      <c r="Z9" s="190"/>
+      <c r="AA9" s="191"/>
+      <c r="AB9" s="221" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="199"/>
-      <c r="AD9" s="199"/>
-      <c r="AE9" s="199"/>
-      <c r="AF9" s="200"/>
-      <c r="AG9" s="204" t="s">
+      <c r="AC9" s="190"/>
+      <c r="AD9" s="190"/>
+      <c r="AE9" s="190"/>
+      <c r="AF9" s="219"/>
+      <c r="AG9" s="222" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="199"/>
-      <c r="AI9" s="199"/>
-      <c r="AJ9" s="199"/>
-      <c r="AK9" s="200"/>
-      <c r="AL9" s="204" t="s">
+      <c r="AH9" s="190"/>
+      <c r="AI9" s="190"/>
+      <c r="AJ9" s="190"/>
+      <c r="AK9" s="219"/>
+      <c r="AL9" s="222" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="199"/>
-      <c r="AN9" s="199"/>
-      <c r="AO9" s="199"/>
-      <c r="AP9" s="202"/>
-      <c r="AQ9" s="205" t="s">
+      <c r="AM9" s="190"/>
+      <c r="AN9" s="190"/>
+      <c r="AO9" s="190"/>
+      <c r="AP9" s="191"/>
+      <c r="AQ9" s="223" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="199"/>
-      <c r="AS9" s="199"/>
-      <c r="AT9" s="199"/>
-      <c r="AU9" s="200"/>
-      <c r="AV9" s="206" t="s">
+      <c r="AR9" s="190"/>
+      <c r="AS9" s="190"/>
+      <c r="AT9" s="190"/>
+      <c r="AU9" s="219"/>
+      <c r="AV9" s="224" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="199"/>
-      <c r="AX9" s="199"/>
-      <c r="AY9" s="199"/>
-      <c r="AZ9" s="200"/>
-      <c r="BA9" s="206" t="s">
+      <c r="AW9" s="190"/>
+      <c r="AX9" s="190"/>
+      <c r="AY9" s="190"/>
+      <c r="AZ9" s="219"/>
+      <c r="BA9" s="224" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="199"/>
-      <c r="BC9" s="199"/>
-      <c r="BD9" s="199"/>
-      <c r="BE9" s="202"/>
-      <c r="BF9" s="207" t="s">
+      <c r="BB9" s="190"/>
+      <c r="BC9" s="190"/>
+      <c r="BD9" s="190"/>
+      <c r="BE9" s="191"/>
+      <c r="BF9" s="225" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="199"/>
-      <c r="BH9" s="199"/>
-      <c r="BI9" s="199"/>
-      <c r="BJ9" s="200"/>
-      <c r="BK9" s="208" t="s">
+      <c r="BG9" s="190"/>
+      <c r="BH9" s="190"/>
+      <c r="BI9" s="190"/>
+      <c r="BJ9" s="219"/>
+      <c r="BK9" s="189" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="199"/>
-      <c r="BM9" s="199"/>
-      <c r="BN9" s="199"/>
-      <c r="BO9" s="200"/>
-      <c r="BP9" s="208" t="s">
+      <c r="BL9" s="190"/>
+      <c r="BM9" s="190"/>
+      <c r="BN9" s="190"/>
+      <c r="BO9" s="219"/>
+      <c r="BP9" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="199"/>
-      <c r="BR9" s="199"/>
-      <c r="BS9" s="199"/>
-      <c r="BT9" s="202"/>
+      <c r="BQ9" s="190"/>
+      <c r="BR9" s="190"/>
+      <c r="BS9" s="190"/>
+      <c r="BT9" s="191"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="215"/>
-      <c r="C10" s="217"/>
-      <c r="D10" s="219"/>
+      <c r="B10" s="198"/>
+      <c r="C10" s="200"/>
+      <c r="D10" s="202"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -8136,11 +8099,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="224"/>
-      <c r="I10" s="192"/>
-      <c r="J10" s="194"/>
-      <c r="K10" s="194"/>
-      <c r="L10" s="197"/>
+      <c r="H10" s="207"/>
+      <c r="I10" s="212"/>
+      <c r="J10" s="214"/>
+      <c r="K10" s="214"/>
+      <c r="L10" s="217"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11749,80 +11712,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="188" t="str">
+      <c r="B45" s="208" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="189"/>
-      <c r="D45" s="189"/>
-      <c r="E45" s="189"/>
-      <c r="F45" s="189"/>
-      <c r="G45" s="189"/>
-      <c r="H45" s="189"/>
-      <c r="I45" s="189"/>
-      <c r="J45" s="189"/>
-      <c r="K45" s="189"/>
-      <c r="L45" s="189"/>
-      <c r="M45" s="189"/>
-      <c r="N45" s="189"/>
-      <c r="O45" s="189"/>
-      <c r="P45" s="189"/>
-      <c r="Q45" s="189"/>
-      <c r="R45" s="189"/>
-      <c r="S45" s="189"/>
-      <c r="T45" s="189"/>
-      <c r="U45" s="189"/>
-      <c r="V45" s="189"/>
-      <c r="W45" s="189"/>
-      <c r="X45" s="189"/>
-      <c r="Y45" s="189"/>
-      <c r="Z45" s="189"/>
-      <c r="AA45" s="189"/>
-      <c r="AB45" s="189"/>
-      <c r="AC45" s="189"/>
-      <c r="AD45" s="189"/>
-      <c r="AE45" s="189"/>
-      <c r="AF45" s="189"/>
-      <c r="AG45" s="189"/>
-      <c r="AH45" s="189"/>
-      <c r="AI45" s="189"/>
-      <c r="AJ45" s="189"/>
-      <c r="AK45" s="189"/>
-      <c r="AL45" s="189"/>
-      <c r="AM45" s="189"/>
-      <c r="AN45" s="189"/>
-      <c r="AO45" s="189"/>
-      <c r="AP45" s="189"/>
-      <c r="AQ45" s="189"/>
-      <c r="AR45" s="189"/>
-      <c r="AS45" s="189"/>
-      <c r="AT45" s="189"/>
-      <c r="AU45" s="189"/>
-      <c r="AV45" s="189"/>
-      <c r="AW45" s="189"/>
-      <c r="AX45" s="189"/>
-      <c r="AY45" s="189"/>
-      <c r="AZ45" s="189"/>
-      <c r="BA45" s="189"/>
-      <c r="BB45" s="189"/>
-      <c r="BC45" s="189"/>
-      <c r="BD45" s="189"/>
-      <c r="BE45" s="189"/>
-      <c r="BF45" s="189"/>
-      <c r="BG45" s="189"/>
-      <c r="BH45" s="189"/>
-      <c r="BI45" s="189"/>
-      <c r="BJ45" s="189"/>
-      <c r="BK45" s="189"/>
-      <c r="BL45" s="189"/>
-      <c r="BM45" s="189"/>
-      <c r="BN45" s="189"/>
-      <c r="BO45" s="189"/>
-      <c r="BP45" s="189"/>
-      <c r="BQ45" s="189"/>
-      <c r="BR45" s="189"/>
-      <c r="BS45" s="189"/>
-      <c r="BT45" s="190"/>
+      <c r="C45" s="209"/>
+      <c r="D45" s="209"/>
+      <c r="E45" s="209"/>
+      <c r="F45" s="209"/>
+      <c r="G45" s="209"/>
+      <c r="H45" s="209"/>
+      <c r="I45" s="209"/>
+      <c r="J45" s="209"/>
+      <c r="K45" s="209"/>
+      <c r="L45" s="209"/>
+      <c r="M45" s="209"/>
+      <c r="N45" s="209"/>
+      <c r="O45" s="209"/>
+      <c r="P45" s="209"/>
+      <c r="Q45" s="209"/>
+      <c r="R45" s="209"/>
+      <c r="S45" s="209"/>
+      <c r="T45" s="209"/>
+      <c r="U45" s="209"/>
+      <c r="V45" s="209"/>
+      <c r="W45" s="209"/>
+      <c r="X45" s="209"/>
+      <c r="Y45" s="209"/>
+      <c r="Z45" s="209"/>
+      <c r="AA45" s="209"/>
+      <c r="AB45" s="209"/>
+      <c r="AC45" s="209"/>
+      <c r="AD45" s="209"/>
+      <c r="AE45" s="209"/>
+      <c r="AF45" s="209"/>
+      <c r="AG45" s="209"/>
+      <c r="AH45" s="209"/>
+      <c r="AI45" s="209"/>
+      <c r="AJ45" s="209"/>
+      <c r="AK45" s="209"/>
+      <c r="AL45" s="209"/>
+      <c r="AM45" s="209"/>
+      <c r="AN45" s="209"/>
+      <c r="AO45" s="209"/>
+      <c r="AP45" s="209"/>
+      <c r="AQ45" s="209"/>
+      <c r="AR45" s="209"/>
+      <c r="AS45" s="209"/>
+      <c r="AT45" s="209"/>
+      <c r="AU45" s="209"/>
+      <c r="AV45" s="209"/>
+      <c r="AW45" s="209"/>
+      <c r="AX45" s="209"/>
+      <c r="AY45" s="209"/>
+      <c r="AZ45" s="209"/>
+      <c r="BA45" s="209"/>
+      <c r="BB45" s="209"/>
+      <c r="BC45" s="209"/>
+      <c r="BD45" s="209"/>
+      <c r="BE45" s="209"/>
+      <c r="BF45" s="209"/>
+      <c r="BG45" s="209"/>
+      <c r="BH45" s="209"/>
+      <c r="BI45" s="209"/>
+      <c r="BJ45" s="209"/>
+      <c r="BK45" s="209"/>
+      <c r="BL45" s="209"/>
+      <c r="BM45" s="209"/>
+      <c r="BN45" s="209"/>
+      <c r="BO45" s="209"/>
+      <c r="BP45" s="209"/>
+      <c r="BQ45" s="209"/>
+      <c r="BR45" s="209"/>
+      <c r="BS45" s="209"/>
+      <c r="BT45" s="210"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12785,14 +12748,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12809,6 +12764,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12816,15 +12779,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF7B3C16"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:CN1020"/>
+  <dimension ref="B1:CN1021"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="K24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD54"/>
+    <sheetView showGridLines="0" topLeftCell="D19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12954,7 +12917,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="211" t="s">
+      <c r="K3" s="194" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -13051,7 +13014,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="212"/>
+      <c r="K4" s="195"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -13145,7 +13108,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="212"/>
+      <c r="K5" s="195"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -13239,7 +13202,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="212"/>
+      <c r="K6" s="195"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -13334,7 +13297,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="213"/>
+      <c r="K7" s="196"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -13420,152 +13383,152 @@
       <c r="CN7" s="175"/>
     </row>
     <row r="8" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="214" t="s">
+      <c r="B8" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="216" t="s">
+      <c r="C8" s="199" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="218" t="s">
+      <c r="D8" s="201" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="220" t="s">
+      <c r="E8" s="203" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="221"/>
-      <c r="G8" s="222"/>
-      <c r="H8" s="223" t="s">
+      <c r="F8" s="204"/>
+      <c r="G8" s="205"/>
+      <c r="H8" s="206" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="191" t="s">
+      <c r="I8" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="193" t="s">
+      <c r="J8" s="213" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="195" t="s">
+      <c r="K8" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="196" t="s">
+      <c r="L8" s="216" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="198" t="s">
+      <c r="M8" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="199"/>
-      <c r="O8" s="199"/>
-      <c r="P8" s="199"/>
-      <c r="Q8" s="200"/>
-      <c r="R8" s="201" t="s">
+      <c r="N8" s="190"/>
+      <c r="O8" s="190"/>
+      <c r="P8" s="190"/>
+      <c r="Q8" s="219"/>
+      <c r="R8" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="199"/>
-      <c r="T8" s="199"/>
-      <c r="U8" s="199"/>
-      <c r="V8" s="200"/>
-      <c r="W8" s="201" t="s">
+      <c r="S8" s="190"/>
+      <c r="T8" s="190"/>
+      <c r="U8" s="190"/>
+      <c r="V8" s="219"/>
+      <c r="W8" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="199"/>
-      <c r="Y8" s="199"/>
-      <c r="Z8" s="199"/>
-      <c r="AA8" s="202"/>
-      <c r="AB8" s="203" t="s">
+      <c r="X8" s="190"/>
+      <c r="Y8" s="190"/>
+      <c r="Z8" s="190"/>
+      <c r="AA8" s="191"/>
+      <c r="AB8" s="221" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="199"/>
-      <c r="AD8" s="199"/>
-      <c r="AE8" s="199"/>
-      <c r="AF8" s="200"/>
-      <c r="AG8" s="204" t="s">
+      <c r="AC8" s="190"/>
+      <c r="AD8" s="190"/>
+      <c r="AE8" s="190"/>
+      <c r="AF8" s="219"/>
+      <c r="AG8" s="222" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="199"/>
-      <c r="AI8" s="199"/>
-      <c r="AJ8" s="199"/>
-      <c r="AK8" s="200"/>
-      <c r="AL8" s="204" t="s">
+      <c r="AH8" s="190"/>
+      <c r="AI8" s="190"/>
+      <c r="AJ8" s="190"/>
+      <c r="AK8" s="219"/>
+      <c r="AL8" s="222" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="199"/>
-      <c r="AN8" s="199"/>
-      <c r="AO8" s="199"/>
-      <c r="AP8" s="202"/>
-      <c r="AQ8" s="205" t="s">
+      <c r="AM8" s="190"/>
+      <c r="AN8" s="190"/>
+      <c r="AO8" s="190"/>
+      <c r="AP8" s="191"/>
+      <c r="AQ8" s="223" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="199"/>
-      <c r="AS8" s="199"/>
-      <c r="AT8" s="199"/>
-      <c r="AU8" s="200"/>
-      <c r="AV8" s="206" t="s">
+      <c r="AR8" s="190"/>
+      <c r="AS8" s="190"/>
+      <c r="AT8" s="190"/>
+      <c r="AU8" s="219"/>
+      <c r="AV8" s="224" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="199"/>
-      <c r="AX8" s="199"/>
-      <c r="AY8" s="199"/>
-      <c r="AZ8" s="200"/>
-      <c r="BA8" s="206" t="s">
+      <c r="AW8" s="190"/>
+      <c r="AX8" s="190"/>
+      <c r="AY8" s="190"/>
+      <c r="AZ8" s="219"/>
+      <c r="BA8" s="224" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="199"/>
-      <c r="BC8" s="199"/>
-      <c r="BD8" s="199"/>
-      <c r="BE8" s="202"/>
-      <c r="BF8" s="229" t="s">
+      <c r="BB8" s="190"/>
+      <c r="BC8" s="190"/>
+      <c r="BD8" s="190"/>
+      <c r="BE8" s="191"/>
+      <c r="BF8" s="230" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="199"/>
-      <c r="BH8" s="199"/>
-      <c r="BI8" s="199"/>
-      <c r="BJ8" s="200"/>
-      <c r="BK8" s="208" t="s">
+      <c r="BG8" s="190"/>
+      <c r="BH8" s="190"/>
+      <c r="BI8" s="190"/>
+      <c r="BJ8" s="219"/>
+      <c r="BK8" s="189" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="199"/>
-      <c r="BM8" s="199"/>
-      <c r="BN8" s="199"/>
-      <c r="BO8" s="200"/>
-      <c r="BP8" s="208" t="s">
+      <c r="BL8" s="190"/>
+      <c r="BM8" s="190"/>
+      <c r="BN8" s="190"/>
+      <c r="BO8" s="219"/>
+      <c r="BP8" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="199"/>
-      <c r="BR8" s="199"/>
-      <c r="BS8" s="199"/>
-      <c r="BT8" s="202"/>
-      <c r="BU8" s="225" t="s">
+      <c r="BQ8" s="190"/>
+      <c r="BR8" s="190"/>
+      <c r="BS8" s="190"/>
+      <c r="BT8" s="191"/>
+      <c r="BU8" s="226" t="s">
         <v>275</v>
       </c>
-      <c r="BV8" s="226"/>
-      <c r="BW8" s="226"/>
-      <c r="BX8" s="226"/>
-      <c r="BY8" s="227"/>
-      <c r="BZ8" s="225" t="s">
+      <c r="BV8" s="227"/>
+      <c r="BW8" s="227"/>
+      <c r="BX8" s="227"/>
+      <c r="BY8" s="228"/>
+      <c r="BZ8" s="226" t="s">
         <v>276</v>
       </c>
-      <c r="CA8" s="226"/>
-      <c r="CB8" s="226"/>
-      <c r="CC8" s="226"/>
-      <c r="CD8" s="227"/>
-      <c r="CE8" s="225" t="s">
+      <c r="CA8" s="227"/>
+      <c r="CB8" s="227"/>
+      <c r="CC8" s="227"/>
+      <c r="CD8" s="228"/>
+      <c r="CE8" s="226" t="s">
         <v>277</v>
       </c>
-      <c r="CF8" s="226"/>
-      <c r="CG8" s="226"/>
-      <c r="CH8" s="226"/>
-      <c r="CI8" s="227"/>
-      <c r="CJ8" s="225" t="s">
+      <c r="CF8" s="227"/>
+      <c r="CG8" s="227"/>
+      <c r="CH8" s="227"/>
+      <c r="CI8" s="228"/>
+      <c r="CJ8" s="226" t="s">
         <v>278</v>
       </c>
-      <c r="CK8" s="226"/>
-      <c r="CL8" s="226"/>
-      <c r="CM8" s="226"/>
-      <c r="CN8" s="227"/>
+      <c r="CK8" s="227"/>
+      <c r="CL8" s="227"/>
+      <c r="CM8" s="227"/>
+      <c r="CN8" s="228"/>
     </row>
     <row r="9" spans="2:92" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="215"/>
-      <c r="C9" s="217"/>
-      <c r="D9" s="219"/>
+      <c r="B9" s="198"/>
+      <c r="C9" s="200"/>
+      <c r="D9" s="202"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -13575,11 +13538,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="224"/>
-      <c r="I9" s="192"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="194"/>
-      <c r="L9" s="197"/>
+      <c r="H9" s="207"/>
+      <c r="I9" s="212"/>
+      <c r="J9" s="214"/>
+      <c r="K9" s="214"/>
+      <c r="L9" s="217"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -19204,1114 +19167,1231 @@
       <c r="CM55" s="65"/>
       <c r="CN55" s="65"/>
     </row>
-    <row r="56" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="4" t="s">
+    <row r="56" spans="2:92" s="188" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="179" t="s">
+        <v>307</v>
+      </c>
+      <c r="C56" s="180" t="s">
+        <v>305</v>
+      </c>
+      <c r="D56" s="186" t="s">
+        <v>306</v>
+      </c>
+      <c r="E56" s="84">
+        <v>2</v>
+      </c>
+      <c r="F56" s="85">
+        <v>2</v>
+      </c>
+      <c r="G56" s="86">
+        <f t="shared" ref="G56" si="31">E56-F56</f>
+        <v>0</v>
+      </c>
+      <c r="H56" s="87">
+        <v>5</v>
+      </c>
+      <c r="I56" s="88">
+        <v>45510</v>
+      </c>
+      <c r="J56" s="89">
+        <v>45511</v>
+      </c>
+      <c r="K56" s="90">
+        <f t="shared" ref="K56" si="32">J56-I56+1</f>
+        <v>2</v>
+      </c>
+      <c r="L56" s="91">
+        <f t="shared" ref="L56" si="33">F56/E56</f>
+        <v>1</v>
+      </c>
+      <c r="M56" s="92"/>
+      <c r="N56" s="93"/>
+      <c r="O56" s="93"/>
+      <c r="P56" s="93"/>
+      <c r="Q56" s="93"/>
+      <c r="R56" s="94"/>
+      <c r="S56" s="94"/>
+      <c r="T56" s="94"/>
+      <c r="U56" s="94"/>
+      <c r="V56" s="94"/>
+      <c r="W56" s="93"/>
+      <c r="X56" s="93"/>
+      <c r="Y56" s="93"/>
+      <c r="Z56" s="93"/>
+      <c r="AA56" s="95"/>
+      <c r="AB56" s="92"/>
+      <c r="AC56" s="93"/>
+      <c r="AD56" s="93"/>
+      <c r="AE56" s="93"/>
+      <c r="AF56" s="93"/>
+      <c r="AG56" s="96"/>
+      <c r="AH56" s="96"/>
+      <c r="AI56" s="96"/>
+      <c r="AJ56" s="96"/>
+      <c r="AK56" s="96"/>
+      <c r="AL56" s="93"/>
+      <c r="AM56" s="93"/>
+      <c r="AN56" s="93"/>
+      <c r="AO56" s="93"/>
+      <c r="AP56" s="95"/>
+      <c r="AQ56" s="92"/>
+      <c r="AR56" s="93"/>
+      <c r="AS56" s="93"/>
+      <c r="AT56" s="93"/>
+      <c r="AU56" s="93"/>
+      <c r="AV56" s="97"/>
+      <c r="AW56" s="97"/>
+      <c r="AX56" s="97"/>
+      <c r="AY56" s="97"/>
+      <c r="AZ56" s="97"/>
+      <c r="BA56" s="93"/>
+      <c r="BB56" s="93"/>
+      <c r="BC56" s="93"/>
+      <c r="BD56" s="93"/>
+      <c r="BE56" s="95"/>
+      <c r="BF56" s="92"/>
+      <c r="BG56" s="93"/>
+      <c r="BH56" s="93"/>
+      <c r="BI56" s="93"/>
+      <c r="BJ56" s="93"/>
+      <c r="BK56" s="182"/>
+      <c r="BL56" s="183"/>
+      <c r="BM56" s="184"/>
+      <c r="BN56" s="183"/>
+      <c r="BO56" s="183"/>
+      <c r="BP56" s="65"/>
+      <c r="BQ56" s="65"/>
+      <c r="BR56" s="174"/>
+      <c r="BS56" s="65"/>
+      <c r="BT56" s="65"/>
+      <c r="BU56" s="65"/>
+      <c r="BV56" s="65"/>
+      <c r="BW56" s="174"/>
+      <c r="BX56" s="65"/>
+      <c r="BY56" s="65"/>
+      <c r="BZ56" s="65"/>
+      <c r="CA56" s="174"/>
+      <c r="CB56" s="174"/>
+      <c r="CC56" s="65"/>
+      <c r="CD56" s="65"/>
+      <c r="CE56" s="65"/>
+      <c r="CF56" s="175"/>
+      <c r="CG56" s="174"/>
+      <c r="CH56" s="65"/>
+      <c r="CI56" s="65"/>
+      <c r="CJ56" s="65"/>
+      <c r="CK56" s="65"/>
+      <c r="CL56" s="174"/>
+      <c r="CM56" s="65"/>
+      <c r="CN56" s="65"/>
+    </row>
+    <row r="57" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D56" s="100" t="s">
+      <c r="D57" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="E56" s="101">
+      <c r="E57" s="101">
         <f>SUM(E11:E16,E18:E21,E29:E37,E43:E47)</f>
         <v>68</v>
       </c>
-      <c r="F56" s="101">
+      <c r="F57" s="101">
         <f>SUM(F11:F16,F18:F21,F29:F37,F43:F47)</f>
         <v>68</v>
       </c>
-      <c r="G56" s="101">
+      <c r="G57" s="101">
         <f>SUM(G11:G16,G18:G21,G29:G37,G43:G47)</f>
         <v>0</v>
       </c>
-      <c r="H56" s="101">
+      <c r="H57" s="101">
         <v>60</v>
       </c>
-      <c r="I56" s="101">
-        <f>E56/H56</f>
+      <c r="I57" s="101">
+        <f>E57/H57</f>
         <v>1.1333333333333333</v>
       </c>
-      <c r="L56" s="102" t="s">
+      <c r="L57" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="M56" s="103">
+      <c r="M57" s="103">
         <v>1</v>
       </c>
-      <c r="N56" s="103">
+      <c r="N57" s="103">
         <v>2</v>
       </c>
-      <c r="O56" s="103">
+      <c r="O57" s="103">
         <v>3</v>
       </c>
-      <c r="P56" s="103">
+      <c r="P57" s="103">
         <v>4</v>
       </c>
-      <c r="Q56" s="103">
+      <c r="Q57" s="103">
         <v>5</v>
       </c>
-      <c r="R56" s="103">
+      <c r="R57" s="103">
         <v>6</v>
       </c>
-      <c r="S56" s="103">
+      <c r="S57" s="103">
         <v>7</v>
       </c>
-      <c r="T56" s="103">
+      <c r="T57" s="103">
         <v>8</v>
       </c>
-      <c r="U56" s="103">
+      <c r="U57" s="103">
         <v>9</v>
       </c>
-      <c r="V56" s="103">
+      <c r="V57" s="103">
         <v>10</v>
       </c>
-      <c r="W56" s="103">
+      <c r="W57" s="103">
         <v>11</v>
       </c>
-      <c r="X56" s="103">
+      <c r="X57" s="103">
         <v>12</v>
       </c>
-      <c r="Y56" s="103">
+      <c r="Y57" s="103">
         <v>13</v>
       </c>
-      <c r="Z56" s="103">
+      <c r="Z57" s="103">
         <v>14</v>
       </c>
-      <c r="AA56" s="103">
+      <c r="AA57" s="103">
         <v>15</v>
       </c>
-      <c r="AB56" s="103">
+      <c r="AB57" s="103">
         <v>16</v>
       </c>
-      <c r="AC56" s="103">
+      <c r="AC57" s="103">
         <v>17</v>
       </c>
-      <c r="AD56" s="103">
+      <c r="AD57" s="103">
         <v>18</v>
       </c>
-      <c r="AE56" s="103">
+      <c r="AE57" s="103">
         <v>19</v>
       </c>
-      <c r="AF56" s="103">
+      <c r="AF57" s="103">
         <v>20</v>
       </c>
-      <c r="AG56" s="103">
+      <c r="AG57" s="103">
         <v>21</v>
       </c>
-      <c r="AH56" s="103">
+      <c r="AH57" s="103">
         <v>22</v>
       </c>
-      <c r="AI56" s="103">
+      <c r="AI57" s="103">
         <v>23</v>
       </c>
-      <c r="AJ56" s="103">
+      <c r="AJ57" s="103">
         <v>24</v>
       </c>
-      <c r="AK56" s="103">
+      <c r="AK57" s="103">
         <v>25</v>
       </c>
-      <c r="AL56" s="103">
+      <c r="AL57" s="103">
         <v>26</v>
       </c>
-      <c r="AM56" s="103">
+      <c r="AM57" s="103">
         <v>27</v>
       </c>
-      <c r="AN56" s="103">
+      <c r="AN57" s="103">
         <v>28</v>
       </c>
-      <c r="AO56" s="103">
+      <c r="AO57" s="103">
         <v>29</v>
       </c>
-      <c r="AP56" s="103">
+      <c r="AP57" s="103">
         <v>30</v>
       </c>
-      <c r="AQ56" s="103">
+      <c r="AQ57" s="103">
         <v>31</v>
       </c>
-      <c r="AR56" s="103">
+      <c r="AR57" s="103">
         <v>32</v>
       </c>
-      <c r="AS56" s="103">
+      <c r="AS57" s="103">
         <v>33</v>
       </c>
-      <c r="AT56" s="103">
+      <c r="AT57" s="103">
         <v>34</v>
       </c>
-      <c r="AU56" s="103">
+      <c r="AU57" s="103">
         <v>35</v>
       </c>
-      <c r="AV56" s="103">
+      <c r="AV57" s="103">
         <v>36</v>
       </c>
-      <c r="AW56" s="103">
+      <c r="AW57" s="103">
         <v>37</v>
       </c>
-      <c r="AX56" s="103">
+      <c r="AX57" s="103">
         <v>38</v>
       </c>
-      <c r="AY56" s="103">
+      <c r="AY57" s="103">
         <v>39</v>
       </c>
-      <c r="AZ56" s="103">
+      <c r="AZ57" s="103">
         <v>40</v>
       </c>
-      <c r="BA56" s="103">
+      <c r="BA57" s="103">
         <v>41</v>
       </c>
-      <c r="BB56" s="103">
+      <c r="BB57" s="103">
         <v>42</v>
       </c>
-      <c r="BC56" s="103">
+      <c r="BC57" s="103">
         <v>43</v>
       </c>
-      <c r="BD56" s="103">
+      <c r="BD57" s="103">
         <v>44</v>
       </c>
-      <c r="BE56" s="103">
+      <c r="BE57" s="103">
         <v>45</v>
       </c>
-      <c r="BF56" s="103">
+      <c r="BF57" s="103">
         <v>46</v>
       </c>
-      <c r="BG56" s="103">
+      <c r="BG57" s="103">
         <v>47</v>
       </c>
-      <c r="BH56" s="103">
+      <c r="BH57" s="103">
         <v>48</v>
       </c>
-      <c r="BI56" s="103">
+      <c r="BI57" s="103">
         <v>49</v>
       </c>
-      <c r="BJ56" s="103">
+      <c r="BJ57" s="103">
         <v>50</v>
       </c>
-      <c r="BK56" s="103">
+      <c r="BK57" s="103">
         <v>51</v>
       </c>
-      <c r="BL56" s="103">
+      <c r="BL57" s="103">
         <v>52</v>
       </c>
-      <c r="BM56" s="103">
+      <c r="BM57" s="103">
         <v>53</v>
       </c>
-      <c r="BN56" s="103">
+      <c r="BN57" s="103">
         <v>54</v>
       </c>
-      <c r="BO56" s="103">
+      <c r="BO57" s="103">
         <v>55</v>
       </c>
-      <c r="BP56" s="103">
+      <c r="BP57" s="103">
         <v>56</v>
       </c>
-      <c r="BQ56" s="103">
+      <c r="BQ57" s="103">
         <v>57</v>
       </c>
-      <c r="BR56" s="103">
+      <c r="BR57" s="103">
         <v>58</v>
       </c>
-      <c r="BS56" s="103">
+      <c r="BS57" s="103">
         <v>59</v>
       </c>
-      <c r="BT56" s="103">
+      <c r="BT57" s="103">
         <v>60</v>
       </c>
-      <c r="BV56" s="100" t="s">
+      <c r="BV57" s="100" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="57" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H57" s="104" t="s">
-        <v>78</v>
-      </c>
-      <c r="L57" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="M57" s="105">
-        <f>E56</f>
-        <v>68</v>
-      </c>
-      <c r="N57" s="106">
-        <f>M57-I56</f>
-        <v>66.86666666666666</v>
-      </c>
-      <c r="O57" s="106">
-        <f>N57-I56</f>
-        <v>65.73333333333332</v>
-      </c>
-      <c r="P57" s="106">
-        <f>O57-I56</f>
-        <v>64.59999999999998</v>
-      </c>
-      <c r="Q57" s="106">
-        <f>P57-I56</f>
-        <v>63.466666666666647</v>
-      </c>
-      <c r="R57" s="106">
-        <f>Q57-I56</f>
-        <v>62.333333333333314</v>
-      </c>
-      <c r="S57" s="106">
-        <f>R57-I56</f>
-        <v>61.199999999999982</v>
-      </c>
-      <c r="T57" s="106">
-        <f>S57-I56</f>
-        <v>60.066666666666649</v>
-      </c>
-      <c r="U57" s="106">
-        <f>T57-I56</f>
-        <v>58.933333333333316</v>
-      </c>
-      <c r="V57" s="106">
-        <f>U57-I56</f>
-        <v>57.799999999999983</v>
-      </c>
-      <c r="W57" s="106">
-        <f>V57-I56</f>
-        <v>56.66666666666665</v>
-      </c>
-      <c r="X57" s="106">
-        <f>W57-I56</f>
-        <v>55.533333333333317</v>
-      </c>
-      <c r="Y57" s="106">
-        <f>X57-I56</f>
-        <v>54.399999999999984</v>
-      </c>
-      <c r="Z57" s="106">
-        <f>Y57-I56</f>
-        <v>53.266666666666652</v>
-      </c>
-      <c r="AA57" s="106">
-        <f>Z57-I56</f>
-        <v>52.133333333333319</v>
-      </c>
-      <c r="AB57" s="106">
-        <f>AA57-I56</f>
-        <v>50.999999999999986</v>
-      </c>
-      <c r="AC57" s="106">
-        <f>AB57-I56</f>
-        <v>49.866666666666653</v>
-      </c>
-      <c r="AD57" s="106">
-        <f>AC57-I56</f>
-        <v>48.73333333333332</v>
-      </c>
-      <c r="AE57" s="106">
-        <f>AD57-I56</f>
-        <v>47.599999999999987</v>
-      </c>
-      <c r="AF57" s="106">
-        <f>AE57-I56</f>
-        <v>46.466666666666654</v>
-      </c>
-      <c r="AG57" s="106">
-        <f>AF57-I56</f>
-        <v>45.333333333333321</v>
-      </c>
-      <c r="AH57" s="106">
-        <f>AG57-I56</f>
-        <v>44.199999999999989</v>
-      </c>
-      <c r="AI57" s="106">
-        <f>AH57-I56</f>
-        <v>43.066666666666656</v>
-      </c>
-      <c r="AJ57" s="106">
-        <f>AI57-I56</f>
-        <v>41.933333333333323</v>
-      </c>
-      <c r="AK57" s="106">
-        <f>AJ57-I56</f>
-        <v>40.79999999999999</v>
-      </c>
-      <c r="AL57" s="106">
-        <f>AK57-I56</f>
-        <v>39.666666666666657</v>
-      </c>
-      <c r="AM57" s="106">
-        <f>AL57-I56</f>
-        <v>38.533333333333324</v>
-      </c>
-      <c r="AN57" s="106">
-        <f>AM57-I56</f>
-        <v>37.399999999999991</v>
-      </c>
-      <c r="AO57" s="106">
-        <f>AN57-I56</f>
-        <v>36.266666666666659</v>
-      </c>
-      <c r="AP57" s="106">
-        <f>AO57-I56</f>
-        <v>35.133333333333326</v>
-      </c>
-      <c r="AQ57" s="106">
-        <f>AP57-I56</f>
-        <v>33.999999999999993</v>
-      </c>
-      <c r="AR57" s="106">
-        <f>AQ57-I56</f>
-        <v>32.86666666666666</v>
-      </c>
-      <c r="AS57" s="106">
-        <f>AR57-I56</f>
-        <v>31.733333333333327</v>
-      </c>
-      <c r="AT57" s="106">
-        <f>AS57-I56</f>
-        <v>30.599999999999994</v>
-      </c>
-      <c r="AU57" s="106">
-        <f>AT57-I56</f>
-        <v>29.466666666666661</v>
-      </c>
-      <c r="AV57" s="106">
-        <f>AU57-I56</f>
-        <v>28.333333333333329</v>
-      </c>
-      <c r="AW57" s="106">
-        <f>AV57-I56</f>
-        <v>27.199999999999996</v>
-      </c>
-      <c r="AX57" s="106">
-        <f>AW57-I56</f>
-        <v>26.066666666666663</v>
-      </c>
-      <c r="AY57" s="106">
-        <f>AX57-I56</f>
-        <v>24.93333333333333</v>
-      </c>
-      <c r="AZ57" s="106">
-        <f>AY57-I56</f>
-        <v>23.799999999999997</v>
-      </c>
-      <c r="BA57" s="106">
-        <f>AZ57-I56</f>
-        <v>22.666666666666664</v>
-      </c>
-      <c r="BB57" s="106">
-        <f>BA57-I56</f>
-        <v>21.533333333333331</v>
-      </c>
-      <c r="BC57" s="106">
-        <f>BB57-I56</f>
-        <v>20.399999999999999</v>
-      </c>
-      <c r="BD57" s="106">
-        <f>BC57-I56</f>
-        <v>19.266666666666666</v>
-      </c>
-      <c r="BE57" s="106">
-        <f>BD57-I56</f>
-        <v>18.133333333333333</v>
-      </c>
-      <c r="BF57" s="106">
-        <f>BE57-I56</f>
-        <v>17</v>
-      </c>
-      <c r="BG57" s="106">
-        <f>BF57-I56</f>
-        <v>15.866666666666667</v>
-      </c>
-      <c r="BH57" s="106">
-        <f>BG57-I56</f>
-        <v>14.733333333333334</v>
-      </c>
-      <c r="BI57" s="106">
-        <f>BH57-I56</f>
-        <v>13.600000000000001</v>
-      </c>
-      <c r="BJ57" s="106">
-        <f>BI57-I56</f>
-        <v>12.466666666666669</v>
-      </c>
-      <c r="BK57" s="106">
-        <f>BJ57-I56</f>
-        <v>11.333333333333336</v>
-      </c>
-      <c r="BL57" s="106">
-        <f>BK57-I56</f>
-        <v>10.200000000000003</v>
-      </c>
-      <c r="BM57" s="106">
-        <f>BL57-I56</f>
-        <v>9.06666666666667</v>
-      </c>
-      <c r="BN57" s="106">
-        <f>BM57-I56</f>
-        <v>7.9333333333333371</v>
-      </c>
-      <c r="BO57" s="106">
-        <f>BN57-I56</f>
-        <v>6.8000000000000043</v>
-      </c>
-      <c r="BP57" s="106">
-        <f>BO57-I56</f>
-        <v>5.6666666666666714</v>
-      </c>
-      <c r="BQ57" s="106">
-        <f>BP57-I56</f>
-        <v>4.5333333333333385</v>
-      </c>
-      <c r="BR57" s="106">
-        <f>BQ57-I56</f>
-        <v>3.4000000000000052</v>
-      </c>
-      <c r="BS57" s="106">
-        <f>BR57-I56</f>
-        <v>2.2666666666666719</v>
-      </c>
-      <c r="BT57" s="106">
-        <f>BS57-I56</f>
-        <v>1.1333333333333386</v>
-      </c>
-      <c r="BV57" s="101"/>
     </row>
     <row r="58" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="L58" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="M58" s="105">
+        <f>E57</f>
+        <v>68</v>
+      </c>
+      <c r="N58" s="106">
+        <f>M58-I57</f>
+        <v>66.86666666666666</v>
+      </c>
+      <c r="O58" s="106">
+        <f>N58-I57</f>
+        <v>65.73333333333332</v>
+      </c>
+      <c r="P58" s="106">
+        <f>O58-I57</f>
+        <v>64.59999999999998</v>
+      </c>
+      <c r="Q58" s="106">
+        <f>P58-I57</f>
+        <v>63.466666666666647</v>
+      </c>
+      <c r="R58" s="106">
+        <f>Q58-I57</f>
+        <v>62.333333333333314</v>
+      </c>
+      <c r="S58" s="106">
+        <f>R58-I57</f>
+        <v>61.199999999999982</v>
+      </c>
+      <c r="T58" s="106">
+        <f>S58-I57</f>
+        <v>60.066666666666649</v>
+      </c>
+      <c r="U58" s="106">
+        <f>T58-I57</f>
+        <v>58.933333333333316</v>
+      </c>
+      <c r="V58" s="106">
+        <f>U58-I57</f>
+        <v>57.799999999999983</v>
+      </c>
+      <c r="W58" s="106">
+        <f>V58-I57</f>
+        <v>56.66666666666665</v>
+      </c>
+      <c r="X58" s="106">
+        <f>W58-I57</f>
+        <v>55.533333333333317</v>
+      </c>
+      <c r="Y58" s="106">
+        <f>X58-I57</f>
+        <v>54.399999999999984</v>
+      </c>
+      <c r="Z58" s="106">
+        <f>Y58-I57</f>
+        <v>53.266666666666652</v>
+      </c>
+      <c r="AA58" s="106">
+        <f>Z58-I57</f>
+        <v>52.133333333333319</v>
+      </c>
+      <c r="AB58" s="106">
+        <f>AA58-I57</f>
+        <v>50.999999999999986</v>
+      </c>
+      <c r="AC58" s="106">
+        <f>AB58-I57</f>
+        <v>49.866666666666653</v>
+      </c>
+      <c r="AD58" s="106">
+        <f>AC58-I57</f>
+        <v>48.73333333333332</v>
+      </c>
+      <c r="AE58" s="106">
+        <f>AD58-I57</f>
+        <v>47.599999999999987</v>
+      </c>
+      <c r="AF58" s="106">
+        <f>AE58-I57</f>
+        <v>46.466666666666654</v>
+      </c>
+      <c r="AG58" s="106">
+        <f>AF58-I57</f>
+        <v>45.333333333333321</v>
+      </c>
+      <c r="AH58" s="106">
+        <f>AG58-I57</f>
+        <v>44.199999999999989</v>
+      </c>
+      <c r="AI58" s="106">
+        <f>AH58-I57</f>
+        <v>43.066666666666656</v>
+      </c>
+      <c r="AJ58" s="106">
+        <f>AI58-I57</f>
+        <v>41.933333333333323</v>
+      </c>
+      <c r="AK58" s="106">
+        <f>AJ58-I57</f>
+        <v>40.79999999999999</v>
+      </c>
+      <c r="AL58" s="106">
+        <f>AK58-I57</f>
+        <v>39.666666666666657</v>
+      </c>
+      <c r="AM58" s="106">
+        <f>AL58-I57</f>
+        <v>38.533333333333324</v>
+      </c>
+      <c r="AN58" s="106">
+        <f>AM58-I57</f>
+        <v>37.399999999999991</v>
+      </c>
+      <c r="AO58" s="106">
+        <f>AN58-I57</f>
+        <v>36.266666666666659</v>
+      </c>
+      <c r="AP58" s="106">
+        <f>AO58-I57</f>
+        <v>35.133333333333326</v>
+      </c>
+      <c r="AQ58" s="106">
+        <f>AP58-I57</f>
+        <v>33.999999999999993</v>
+      </c>
+      <c r="AR58" s="106">
+        <f>AQ58-I57</f>
+        <v>32.86666666666666</v>
+      </c>
+      <c r="AS58" s="106">
+        <f>AR58-I57</f>
+        <v>31.733333333333327</v>
+      </c>
+      <c r="AT58" s="106">
+        <f>AS58-I57</f>
+        <v>30.599999999999994</v>
+      </c>
+      <c r="AU58" s="106">
+        <f>AT58-I57</f>
+        <v>29.466666666666661</v>
+      </c>
+      <c r="AV58" s="106">
+        <f>AU58-I57</f>
+        <v>28.333333333333329</v>
+      </c>
+      <c r="AW58" s="106">
+        <f>AV58-I57</f>
+        <v>27.199999999999996</v>
+      </c>
+      <c r="AX58" s="106">
+        <f>AW58-I57</f>
+        <v>26.066666666666663</v>
+      </c>
+      <c r="AY58" s="106">
+        <f>AX58-I57</f>
+        <v>24.93333333333333</v>
+      </c>
+      <c r="AZ58" s="106">
+        <f>AY58-I57</f>
+        <v>23.799999999999997</v>
+      </c>
+      <c r="BA58" s="106">
+        <f>AZ58-I57</f>
+        <v>22.666666666666664</v>
+      </c>
+      <c r="BB58" s="106">
+        <f>BA58-I57</f>
+        <v>21.533333333333331</v>
+      </c>
+      <c r="BC58" s="106">
+        <f>BB58-I57</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="BD58" s="106">
+        <f>BC58-I57</f>
+        <v>19.266666666666666</v>
+      </c>
+      <c r="BE58" s="106">
+        <f>BD58-I57</f>
+        <v>18.133333333333333</v>
+      </c>
+      <c r="BF58" s="106">
+        <f>BE58-I57</f>
+        <v>17</v>
+      </c>
+      <c r="BG58" s="106">
+        <f>BF58-I57</f>
+        <v>15.866666666666667</v>
+      </c>
+      <c r="BH58" s="106">
+        <f>BG58-I57</f>
+        <v>14.733333333333334</v>
+      </c>
+      <c r="BI58" s="106">
+        <f>BH58-I57</f>
+        <v>13.600000000000001</v>
+      </c>
+      <c r="BJ58" s="106">
+        <f>BI58-I57</f>
+        <v>12.466666666666669</v>
+      </c>
+      <c r="BK58" s="106">
+        <f>BJ58-I57</f>
+        <v>11.333333333333336</v>
+      </c>
+      <c r="BL58" s="106">
+        <f>BK58-I57</f>
+        <v>10.200000000000003</v>
+      </c>
+      <c r="BM58" s="106">
+        <f>BL58-I57</f>
+        <v>9.06666666666667</v>
+      </c>
+      <c r="BN58" s="106">
+        <f>BM58-I57</f>
+        <v>7.9333333333333371</v>
+      </c>
+      <c r="BO58" s="106">
+        <f>BN58-I57</f>
+        <v>6.8000000000000043</v>
+      </c>
+      <c r="BP58" s="106">
+        <f>BO58-I57</f>
+        <v>5.6666666666666714</v>
+      </c>
+      <c r="BQ58" s="106">
+        <f>BP58-I57</f>
+        <v>4.5333333333333385</v>
+      </c>
+      <c r="BR58" s="106">
+        <f>BQ58-I57</f>
+        <v>3.4000000000000052</v>
+      </c>
+      <c r="BS58" s="106">
+        <f>BR58-I57</f>
+        <v>2.2666666666666719</v>
+      </c>
+      <c r="BT58" s="106">
+        <f>BS58-I57</f>
+        <v>1.1333333333333386</v>
+      </c>
+      <c r="BV58" s="101"/>
+    </row>
+    <row r="59" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L59" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="M58" s="105">
-        <f>E56</f>
+      <c r="M59" s="105">
+        <f>E57</f>
         <v>68</v>
       </c>
-      <c r="N58" s="105">
-        <f t="shared" ref="N58:BT58" si="31">M60</f>
+      <c r="N59" s="105">
+        <f t="shared" ref="N59:BT59" si="34">M61</f>
         <v>68</v>
       </c>
-      <c r="O58" s="105">
-        <f t="shared" si="31"/>
+      <c r="O59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="P58" s="105">
-        <f t="shared" si="31"/>
+      <c r="P59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="Q58" s="105">
-        <f t="shared" si="31"/>
+      <c r="Q59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="R58" s="105">
-        <f t="shared" si="31"/>
+      <c r="R59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="S58" s="105">
-        <f t="shared" si="31"/>
+      <c r="S59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="T58" s="105">
-        <f t="shared" si="31"/>
+      <c r="T59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="U58" s="105">
-        <f t="shared" si="31"/>
+      <c r="U59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="V58" s="105">
-        <f t="shared" si="31"/>
+      <c r="V59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="W58" s="105">
-        <f t="shared" si="31"/>
+      <c r="W59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="X58" s="105">
-        <f t="shared" si="31"/>
+      <c r="X59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="Y58" s="105">
-        <f t="shared" si="31"/>
+      <c r="Y59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="Z58" s="105">
-        <f t="shared" si="31"/>
+      <c r="Z59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AA58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AA59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AB58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AB59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AC58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AC59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AD58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AD59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AE58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AE59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AF58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AF59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AG58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AG59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AH58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AH59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AI58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AI59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AJ58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AJ59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AK58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AK59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AL58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AL59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AM58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AM59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AN58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AN59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AO58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AO59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AP58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AP59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AQ58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AQ59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AR58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AR59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AS58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AS59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AT58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AT59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AU58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AU59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AV58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AV59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AW58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AW59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AX58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AX59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AY58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AY59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="AZ58" s="105">
-        <f t="shared" si="31"/>
+      <c r="AZ59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BA58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BA59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BB58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BB59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BC58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BC59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BD58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BD59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BE58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BE59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BF58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BF59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BG58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BG59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BH58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BH59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BI58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BI59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BJ58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BJ59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BK58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BK59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BL58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BL59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BM58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BM59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BN58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BN59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BO58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BO59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BP58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BP59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BQ58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BQ59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BR58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BR59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BS58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BS59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BT58" s="105">
-        <f t="shared" si="31"/>
+      <c r="BT59" s="105">
+        <f t="shared" si="34"/>
         <v>68</v>
       </c>
-      <c r="BV58" s="101">
-        <f t="shared" ref="BV58:BV60" si="32">SUM(M58:BT58)</f>
+      <c r="BV59" s="101">
+        <f t="shared" ref="BV59:BV61" si="35">SUM(M59:BT59)</f>
         <v>4080</v>
-      </c>
-    </row>
-    <row r="59" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K59" s="107" t="s">
-        <v>80</v>
-      </c>
-      <c r="L59" s="102" t="s">
-        <v>81</v>
-      </c>
-      <c r="M59" s="57"/>
-      <c r="N59" s="57"/>
-      <c r="O59" s="57"/>
-      <c r="P59" s="57"/>
-      <c r="Q59" s="57"/>
-      <c r="R59" s="57"/>
-      <c r="S59" s="57"/>
-      <c r="T59" s="57"/>
-      <c r="U59" s="57"/>
-      <c r="V59" s="57"/>
-      <c r="W59" s="57"/>
-      <c r="X59" s="57"/>
-      <c r="Y59" s="57"/>
-      <c r="Z59" s="57"/>
-      <c r="AA59" s="57"/>
-      <c r="AB59" s="57"/>
-      <c r="AC59" s="57"/>
-      <c r="AD59" s="57"/>
-      <c r="AE59" s="57"/>
-      <c r="AF59" s="57"/>
-      <c r="AG59" s="57"/>
-      <c r="AH59" s="57"/>
-      <c r="AI59" s="57"/>
-      <c r="AJ59" s="57"/>
-      <c r="AK59" s="57"/>
-      <c r="AL59" s="57"/>
-      <c r="AM59" s="57"/>
-      <c r="AN59" s="57"/>
-      <c r="AO59" s="57"/>
-      <c r="AP59" s="57"/>
-      <c r="AQ59" s="57"/>
-      <c r="AR59" s="57"/>
-      <c r="AS59" s="57"/>
-      <c r="AT59" s="57"/>
-      <c r="AU59" s="57"/>
-      <c r="AV59" s="57"/>
-      <c r="AW59" s="57"/>
-      <c r="AX59" s="57"/>
-      <c r="AY59" s="57"/>
-      <c r="AZ59" s="57"/>
-      <c r="BA59" s="57"/>
-      <c r="BB59" s="57"/>
-      <c r="BC59" s="57"/>
-      <c r="BD59" s="57"/>
-      <c r="BE59" s="57"/>
-      <c r="BF59" s="57"/>
-      <c r="BG59" s="57"/>
-      <c r="BH59" s="57"/>
-      <c r="BI59" s="57"/>
-      <c r="BJ59" s="57"/>
-      <c r="BK59" s="57"/>
-      <c r="BL59" s="57"/>
-      <c r="BM59" s="57"/>
-      <c r="BN59" s="57"/>
-      <c r="BO59" s="57"/>
-      <c r="BP59" s="57"/>
-      <c r="BQ59" s="57"/>
-      <c r="BR59" s="57"/>
-      <c r="BS59" s="57"/>
-      <c r="BT59" s="57"/>
-      <c r="BV59" s="101">
-        <f t="shared" si="32"/>
-        <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K60" s="107" t="s">
+        <v>80</v>
+      </c>
       <c r="L60" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="M60" s="57"/>
+      <c r="N60" s="57"/>
+      <c r="O60" s="57"/>
+      <c r="P60" s="57"/>
+      <c r="Q60" s="57"/>
+      <c r="R60" s="57"/>
+      <c r="S60" s="57"/>
+      <c r="T60" s="57"/>
+      <c r="U60" s="57"/>
+      <c r="V60" s="57"/>
+      <c r="W60" s="57"/>
+      <c r="X60" s="57"/>
+      <c r="Y60" s="57"/>
+      <c r="Z60" s="57"/>
+      <c r="AA60" s="57"/>
+      <c r="AB60" s="57"/>
+      <c r="AC60" s="57"/>
+      <c r="AD60" s="57"/>
+      <c r="AE60" s="57"/>
+      <c r="AF60" s="57"/>
+      <c r="AG60" s="57"/>
+      <c r="AH60" s="57"/>
+      <c r="AI60" s="57"/>
+      <c r="AJ60" s="57"/>
+      <c r="AK60" s="57"/>
+      <c r="AL60" s="57"/>
+      <c r="AM60" s="57"/>
+      <c r="AN60" s="57"/>
+      <c r="AO60" s="57"/>
+      <c r="AP60" s="57"/>
+      <c r="AQ60" s="57"/>
+      <c r="AR60" s="57"/>
+      <c r="AS60" s="57"/>
+      <c r="AT60" s="57"/>
+      <c r="AU60" s="57"/>
+      <c r="AV60" s="57"/>
+      <c r="AW60" s="57"/>
+      <c r="AX60" s="57"/>
+      <c r="AY60" s="57"/>
+      <c r="AZ60" s="57"/>
+      <c r="BA60" s="57"/>
+      <c r="BB60" s="57"/>
+      <c r="BC60" s="57"/>
+      <c r="BD60" s="57"/>
+      <c r="BE60" s="57"/>
+      <c r="BF60" s="57"/>
+      <c r="BG60" s="57"/>
+      <c r="BH60" s="57"/>
+      <c r="BI60" s="57"/>
+      <c r="BJ60" s="57"/>
+      <c r="BK60" s="57"/>
+      <c r="BL60" s="57"/>
+      <c r="BM60" s="57"/>
+      <c r="BN60" s="57"/>
+      <c r="BO60" s="57"/>
+      <c r="BP60" s="57"/>
+      <c r="BQ60" s="57"/>
+      <c r="BR60" s="57"/>
+      <c r="BS60" s="57"/>
+      <c r="BT60" s="57"/>
+      <c r="BV60" s="101">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L61" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M60" s="105">
-        <f t="shared" ref="M60:BT60" si="33">M58-M59</f>
+      <c r="M61" s="105">
+        <f t="shared" ref="M61:BT61" si="36">M59-M60</f>
         <v>68</v>
       </c>
-      <c r="N60" s="105">
-        <f t="shared" si="33"/>
+      <c r="N61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="O60" s="105">
-        <f t="shared" si="33"/>
+      <c r="O61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="P60" s="105">
-        <f t="shared" si="33"/>
+      <c r="P61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="Q60" s="105">
-        <f t="shared" si="33"/>
+      <c r="Q61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="R60" s="105">
-        <f t="shared" si="33"/>
+      <c r="R61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="S60" s="105">
-        <f t="shared" si="33"/>
+      <c r="S61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="T60" s="105">
-        <f t="shared" si="33"/>
+      <c r="T61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="U60" s="105">
-        <f t="shared" si="33"/>
+      <c r="U61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="V60" s="105">
-        <f t="shared" si="33"/>
+      <c r="V61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="W60" s="105">
-        <f t="shared" si="33"/>
+      <c r="W61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="X60" s="105">
-        <f t="shared" si="33"/>
+      <c r="X61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="Y60" s="105">
-        <f t="shared" si="33"/>
+      <c r="Y61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="Z60" s="105">
-        <f t="shared" si="33"/>
+      <c r="Z61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AA60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AA61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AB60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AB61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AC60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AC61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AD60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AD61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AE60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AE61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AF60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AF61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AG60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AG61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AH60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AH61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AI60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AI61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AJ60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AJ61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AK60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AK61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AL60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AL61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AM60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AM61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AN60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AN61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AO60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AO61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AP60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AP61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AQ60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AQ61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AR60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AR61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AS60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AS61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AT60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AT61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AU60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AU61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AV60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AV61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AW60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AW61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AX60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AX61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AY60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AY61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="AZ60" s="105">
-        <f t="shared" si="33"/>
+      <c r="AZ61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BA60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BA61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BB60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BB61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BC60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BC61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BD60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BD61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BE60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BE61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BF60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BF61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BG60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BG61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BH60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BH61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BI60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BI61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BJ60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BJ61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BK60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BK61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BL60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BL61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BM60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BM61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BN60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BN61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BO60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BO61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BP60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BP61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BQ60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BQ61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BR60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BR61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BS60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BS61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BT60" s="105">
-        <f t="shared" si="33"/>
+      <c r="BT61" s="105">
+        <f t="shared" si="36"/>
         <v>68</v>
       </c>
-      <c r="BV60" s="101">
-        <f t="shared" si="32"/>
+      <c r="BV61" s="101">
+        <f t="shared" si="35"/>
         <v>4080</v>
       </c>
     </row>
-    <row r="61" spans="2:92" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:92" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:92" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E64" s="228" t="s">
+    <row r="62" spans="2:92" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:92" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="3:54" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E65" s="229" t="s">
         <v>83</v>
       </c>
-      <c r="F64" s="189"/>
-      <c r="G64" s="189"/>
-      <c r="H64" s="189"/>
-      <c r="I64" s="189"/>
-      <c r="J64" s="189"/>
-      <c r="K64" s="189"/>
-      <c r="L64" s="189"/>
-      <c r="M64" s="189"/>
-      <c r="N64" s="189"/>
-      <c r="O64" s="189"/>
-      <c r="P64" s="189"/>
-      <c r="Q64" s="189"/>
-      <c r="R64" s="189"/>
-      <c r="S64" s="189"/>
-      <c r="T64" s="189"/>
-      <c r="U64" s="189"/>
-      <c r="V64" s="189"/>
-      <c r="W64" s="189"/>
-      <c r="X64" s="189"/>
-      <c r="Y64" s="189"/>
-      <c r="Z64" s="189"/>
-      <c r="AA64" s="189"/>
-      <c r="AB64" s="189"/>
-      <c r="AC64" s="189"/>
-      <c r="AD64" s="189"/>
-      <c r="AE64" s="189"/>
-      <c r="AF64" s="189"/>
-      <c r="AG64" s="189"/>
-      <c r="AH64" s="189"/>
-      <c r="AI64" s="189"/>
-      <c r="AJ64" s="189"/>
-      <c r="AK64" s="189"/>
-      <c r="AL64" s="189"/>
-      <c r="AM64" s="189"/>
-      <c r="AN64" s="189"/>
-      <c r="AO64" s="189"/>
-      <c r="AP64" s="189"/>
-      <c r="AQ64" s="189"/>
-      <c r="AR64" s="189"/>
-      <c r="AS64" s="189"/>
-      <c r="AT64" s="189"/>
-      <c r="AU64" s="189"/>
-      <c r="AV64" s="189"/>
-      <c r="AW64" s="189"/>
-      <c r="AX64" s="189"/>
-      <c r="AY64" s="189"/>
-      <c r="AZ64" s="189"/>
-      <c r="BA64" s="189"/>
-      <c r="BB64" s="190"/>
+      <c r="F65" s="209"/>
+      <c r="G65" s="209"/>
+      <c r="H65" s="209"/>
+      <c r="I65" s="209"/>
+      <c r="J65" s="209"/>
+      <c r="K65" s="209"/>
+      <c r="L65" s="209"/>
+      <c r="M65" s="209"/>
+      <c r="N65" s="209"/>
+      <c r="O65" s="209"/>
+      <c r="P65" s="209"/>
+      <c r="Q65" s="209"/>
+      <c r="R65" s="209"/>
+      <c r="S65" s="209"/>
+      <c r="T65" s="209"/>
+      <c r="U65" s="209"/>
+      <c r="V65" s="209"/>
+      <c r="W65" s="209"/>
+      <c r="X65" s="209"/>
+      <c r="Y65" s="209"/>
+      <c r="Z65" s="209"/>
+      <c r="AA65" s="209"/>
+      <c r="AB65" s="209"/>
+      <c r="AC65" s="209"/>
+      <c r="AD65" s="209"/>
+      <c r="AE65" s="209"/>
+      <c r="AF65" s="209"/>
+      <c r="AG65" s="209"/>
+      <c r="AH65" s="209"/>
+      <c r="AI65" s="209"/>
+      <c r="AJ65" s="209"/>
+      <c r="AK65" s="209"/>
+      <c r="AL65" s="209"/>
+      <c r="AM65" s="209"/>
+      <c r="AN65" s="209"/>
+      <c r="AO65" s="209"/>
+      <c r="AP65" s="209"/>
+      <c r="AQ65" s="209"/>
+      <c r="AR65" s="209"/>
+      <c r="AS65" s="209"/>
+      <c r="AT65" s="209"/>
+      <c r="AU65" s="209"/>
+      <c r="AV65" s="209"/>
+      <c r="AW65" s="209"/>
+      <c r="AX65" s="209"/>
+      <c r="AY65" s="209"/>
+      <c r="AZ65" s="209"/>
+      <c r="BA65" s="209"/>
+      <c r="BB65" s="210"/>
     </row>
-    <row r="65" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="3:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="108"/>
-      <c r="D69" s="108"/>
+    <row r="66" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="3:54" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="108"/>
+      <c r="D70" s="108"/>
     </row>
-    <row r="70" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -21252,24 +21332,14 @@
     <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="AL8:AP8"/>
-    <mergeCell ref="AQ8:AU8"/>
-    <mergeCell ref="AV8:AZ8"/>
-    <mergeCell ref="BA8:BE8"/>
-    <mergeCell ref="K3:K7"/>
     <mergeCell ref="BU8:BY8"/>
     <mergeCell ref="BZ8:CD8"/>
     <mergeCell ref="CE8:CI8"/>
     <mergeCell ref="CJ8:CN8"/>
-    <mergeCell ref="E64:BB64"/>
+    <mergeCell ref="E65:BB65"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
     <mergeCell ref="BP8:BT8"/>
@@ -21281,6 +21351,17 @@
     <mergeCell ref="W8:AA8"/>
     <mergeCell ref="AB8:AF8"/>
     <mergeCell ref="AG8:AK8"/>
+    <mergeCell ref="AL8:AP8"/>
+    <mergeCell ref="AQ8:AU8"/>
+    <mergeCell ref="AV8:AZ8"/>
+    <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21290,7 +21371,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFDD8047"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -21298,7 +21379,7 @@
   <dimension ref="B1:K999"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -21982,7 +22063,7 @@
       </c>
       <c r="F36" s="149"/>
       <c r="G36" s="119" t="s">
-        <v>89</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -23004,12 +23085,12 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G27">
-    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23024,7 +23105,7 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="50" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23051,7 +23132,7 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23066,7 +23147,7 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="43" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23093,7 +23174,7 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23108,28 +23189,28 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="40" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28 G30:G34">
-    <cfRule type="cellIs" dxfId="17" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="56" operator="equal">
       <formula>$I$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="57" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="58" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="12" priority="58" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH(("Not Started"),(G28))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:G34">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(G29))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="15">
@@ -23156,12 +23237,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="12" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="63" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I5">
-    <cfRule type="containsText" dxfId="11" priority="60" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="8" priority="60" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(I3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="61">
@@ -23176,7 +23257,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="10" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="62" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23191,12 +23272,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(G37))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="12">
@@ -23268,10 +23349,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G28 G30:G34" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G28 G30:G34">
       <formula1>$I$3:$I$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F35" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F35">
       <formula1>$K$3:$K$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -23284,7 +23365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFEAB290"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
User/Admin delete comments and replies completed + forum improved
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\AnimalDex\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADFCD1F-3BE6-4569-8114-A78C8D912DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLE Gantt Chart &amp; Burndown" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
     <sheet name="Release Backlog" sheetId="3" r:id="rId3"/>
     <sheet name="User Stories or Tasks" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="310">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -956,13 +962,16 @@
     <t>5.7</t>
   </si>
   <si>
-    <t>In progress</t>
+    <t>5.8</t>
+  </si>
+  <si>
+    <t>forum improved features</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2348,7 +2357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="231">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2801,12 +2810,53 @@
     <xf numFmtId="49" fontId="24" fillId="17" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2837,48 +2887,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="29" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2894,33 +2902,15 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="31">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="0" shrinkToFit="0"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
       <alignment wrapText="0" shrinkToFit="0"/>
@@ -2969,30 +2959,12 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="0" shrinkToFit="0"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFEB9C"/>
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
       <alignment wrapText="0" shrinkToFit="0"/>
@@ -3023,12 +2995,12 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
       <alignment wrapText="0" shrinkToFit="0"/>
@@ -3047,24 +3019,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFEB9C"/>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="0" shrinkToFit="0"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
       <alignment wrapText="0" shrinkToFit="0"/>
@@ -3590,7 +3544,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="1"/>
@@ -3622,7 +3576,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3686,7 +3639,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -3965,10 +3918,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6309-415A-9B2A-8CEC22EBC916}"/>
-            </c:ext>
+          <c:extLst>
             <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
               <c14:invertSolidFillFmt>
                 <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
@@ -3982,6 +3932,9 @@
                   </a:ln>
                 </c14:spPr>
               </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6309-415A-9B2A-8CEC22EBC916}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4405,7 +4358,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6309-415A-9B2A-8CEC22EBC916}"/>
             </c:ext>
@@ -4816,7 +4769,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6309-415A-9B2A-8CEC22EBC916}"/>
             </c:ext>
@@ -5227,7 +5180,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6309-415A-9B2A-8CEC22EBC916}"/>
             </c:ext>
@@ -5271,7 +5224,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5345,7 +5297,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5437,7 +5388,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5474,7 +5424,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -5510,7 +5459,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="1"/>
@@ -5542,7 +5491,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5557,7 +5505,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$60</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$61</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5606,7 +5554,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -5614,7 +5562,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$57:$BT$57</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$58:$BT$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5803,17 +5751,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$60:$BT$60</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$61:$BT$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0B83-4C3C-A1FB-BFF5EF056244}"/>
-            </c:ext>
+          <c:extLst>
             <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
               <c14:invertSolidFillFmt>
                 <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
@@ -5827,6 +5772,9 @@
                   </a:ln>
                 </c14:spPr>
               </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0B83-4C3C-A1FB-BFF5EF056244}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5850,7 +5798,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$58</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5873,7 +5821,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$57:$BT$57</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$58:$BT$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6062,7 +6010,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$58:$BT$58</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$59:$BT$59</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6250,7 +6198,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0B83-4C3C-A1FB-BFF5EF056244}"/>
             </c:ext>
@@ -6261,7 +6209,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$59</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6284,7 +6232,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$57:$BT$57</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$58:$BT$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6473,7 +6421,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$59:$BT$59</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$60:$BT$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6661,7 +6609,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0B83-4C3C-A1FB-BFF5EF056244}"/>
             </c:ext>
@@ -6705,7 +6653,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6779,7 +6726,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6871,7 +6817,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -6908,7 +6853,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -6958,7 +6902,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6989,7 +6933,7 @@
         <xdr:cNvPr id="3" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7019,7 +6963,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="27632025" cy="7553325"/>
@@ -7028,7 +6972,7 @@
         <xdr:cNvPr id="2" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7059,7 +7003,7 @@
         <xdr:cNvPr id="3" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7084,45 +7028,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabella2" displayName="Tabella2" ref="B2:G38" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
-  <autoFilter ref="B2:G38"/>
-  <sortState ref="B3:G38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella2" displayName="Tabella2" ref="B2:G38" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28">
+  <autoFilter ref="B2:G38" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G38">
     <sortCondition ref="B2:B38"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="SPRINT"/>
-    <tableColumn id="2" name="TASK TITLE"/>
-    <tableColumn id="3" name="TASK DESCRIPTION"/>
-    <tableColumn id="4" name="TASK OWNER"/>
-    <tableColumn id="5" name="WORK ESTIMATE IN HOURS"/>
-    <tableColumn id="6" name="STATUS"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SPRINT"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TASK TITLE"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TASK DESCRIPTION"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TASK OWNER"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="WORK ESTIMATE IN HOURS"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="STATUS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="B3:G43" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28">
-  <autoFilter ref="B3:G43"/>
-  <sortState ref="B4:G43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabella1" displayName="Tabella1" ref="B3:G43" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25">
+  <autoFilter ref="B3:G43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:G43">
     <sortCondition ref="D3:D43"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="TASK TITLE" dataDxfId="27"/>
-    <tableColumn id="2" name="TASK DESCRIPTION" dataDxfId="26"/>
-    <tableColumn id="6" name="COMPONENT" dataDxfId="25"/>
-    <tableColumn id="3" name="PRIORITY" dataDxfId="24"/>
-    <tableColumn id="4" name="ADDED BY" dataDxfId="23"/>
-    <tableColumn id="5" name="DATED ADDED" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TASK TITLE" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="TASK DESCRIPTION" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="COMPONENT" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="PRIORITY" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ADDED BY" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="DATED ADDED" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7160,7 +7104,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -7232,7 +7176,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7405,7 +7349,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF7B3C16"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -7564,19 +7508,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="192" t="str">
+      <c r="BK2" s="209" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="193"/>
-      <c r="BM2" s="193"/>
-      <c r="BN2" s="193"/>
-      <c r="BO2" s="193"/>
-      <c r="BP2" s="193"/>
-      <c r="BQ2" s="193"/>
-      <c r="BR2" s="193"/>
-      <c r="BS2" s="193"/>
-      <c r="BT2" s="193"/>
+      <c r="BL2" s="210"/>
+      <c r="BM2" s="210"/>
+      <c r="BN2" s="210"/>
+      <c r="BO2" s="210"/>
+      <c r="BP2" s="210"/>
+      <c r="BQ2" s="210"/>
+      <c r="BR2" s="210"/>
+      <c r="BS2" s="210"/>
+      <c r="BT2" s="210"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -7604,7 +7548,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="194" t="s">
+      <c r="K4" s="211" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7681,7 +7625,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="195"/>
+      <c r="K5" s="212"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7756,7 +7700,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="195"/>
+      <c r="K6" s="212"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7831,7 +7775,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="195"/>
+      <c r="K7" s="212"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7906,7 +7850,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="196"/>
+      <c r="K8" s="213"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7972,124 +7916,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="197" t="s">
+      <c r="B9" s="214" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="199" t="s">
+      <c r="C9" s="216" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="201" t="s">
+      <c r="D9" s="218" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="203" t="s">
+      <c r="E9" s="220" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="204"/>
-      <c r="G9" s="205"/>
-      <c r="H9" s="206" t="s">
+      <c r="F9" s="221"/>
+      <c r="G9" s="222"/>
+      <c r="H9" s="223" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="211" t="s">
+      <c r="I9" s="191" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="213" t="s">
+      <c r="J9" s="193" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="215" t="s">
+      <c r="K9" s="195" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="216" t="s">
+      <c r="L9" s="196" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="218" t="s">
+      <c r="M9" s="198" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="190"/>
-      <c r="O9" s="190"/>
-      <c r="P9" s="190"/>
-      <c r="Q9" s="219"/>
-      <c r="R9" s="220" t="s">
+      <c r="N9" s="199"/>
+      <c r="O9" s="199"/>
+      <c r="P9" s="199"/>
+      <c r="Q9" s="200"/>
+      <c r="R9" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="190"/>
-      <c r="T9" s="190"/>
-      <c r="U9" s="190"/>
-      <c r="V9" s="219"/>
-      <c r="W9" s="220" t="s">
+      <c r="S9" s="199"/>
+      <c r="T9" s="199"/>
+      <c r="U9" s="199"/>
+      <c r="V9" s="200"/>
+      <c r="W9" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="190"/>
-      <c r="Y9" s="190"/>
-      <c r="Z9" s="190"/>
-      <c r="AA9" s="191"/>
-      <c r="AB9" s="221" t="s">
+      <c r="X9" s="199"/>
+      <c r="Y9" s="199"/>
+      <c r="Z9" s="199"/>
+      <c r="AA9" s="202"/>
+      <c r="AB9" s="203" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="190"/>
-      <c r="AD9" s="190"/>
-      <c r="AE9" s="190"/>
-      <c r="AF9" s="219"/>
-      <c r="AG9" s="222" t="s">
+      <c r="AC9" s="199"/>
+      <c r="AD9" s="199"/>
+      <c r="AE9" s="199"/>
+      <c r="AF9" s="200"/>
+      <c r="AG9" s="204" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="190"/>
-      <c r="AI9" s="190"/>
-      <c r="AJ9" s="190"/>
-      <c r="AK9" s="219"/>
-      <c r="AL9" s="222" t="s">
+      <c r="AH9" s="199"/>
+      <c r="AI9" s="199"/>
+      <c r="AJ9" s="199"/>
+      <c r="AK9" s="200"/>
+      <c r="AL9" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="190"/>
-      <c r="AN9" s="190"/>
-      <c r="AO9" s="190"/>
-      <c r="AP9" s="191"/>
-      <c r="AQ9" s="223" t="s">
+      <c r="AM9" s="199"/>
+      <c r="AN9" s="199"/>
+      <c r="AO9" s="199"/>
+      <c r="AP9" s="202"/>
+      <c r="AQ9" s="205" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="190"/>
-      <c r="AS9" s="190"/>
-      <c r="AT9" s="190"/>
-      <c r="AU9" s="219"/>
-      <c r="AV9" s="224" t="s">
+      <c r="AR9" s="199"/>
+      <c r="AS9" s="199"/>
+      <c r="AT9" s="199"/>
+      <c r="AU9" s="200"/>
+      <c r="AV9" s="206" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="190"/>
-      <c r="AX9" s="190"/>
-      <c r="AY9" s="190"/>
-      <c r="AZ9" s="219"/>
-      <c r="BA9" s="224" t="s">
+      <c r="AW9" s="199"/>
+      <c r="AX9" s="199"/>
+      <c r="AY9" s="199"/>
+      <c r="AZ9" s="200"/>
+      <c r="BA9" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="190"/>
-      <c r="BC9" s="190"/>
-      <c r="BD9" s="190"/>
-      <c r="BE9" s="191"/>
-      <c r="BF9" s="225" t="s">
+      <c r="BB9" s="199"/>
+      <c r="BC9" s="199"/>
+      <c r="BD9" s="199"/>
+      <c r="BE9" s="202"/>
+      <c r="BF9" s="207" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="190"/>
-      <c r="BH9" s="190"/>
-      <c r="BI9" s="190"/>
-      <c r="BJ9" s="219"/>
-      <c r="BK9" s="189" t="s">
+      <c r="BG9" s="199"/>
+      <c r="BH9" s="199"/>
+      <c r="BI9" s="199"/>
+      <c r="BJ9" s="200"/>
+      <c r="BK9" s="208" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="190"/>
-      <c r="BM9" s="190"/>
-      <c r="BN9" s="190"/>
-      <c r="BO9" s="219"/>
-      <c r="BP9" s="189" t="s">
+      <c r="BL9" s="199"/>
+      <c r="BM9" s="199"/>
+      <c r="BN9" s="199"/>
+      <c r="BO9" s="200"/>
+      <c r="BP9" s="208" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="190"/>
-      <c r="BR9" s="190"/>
-      <c r="BS9" s="190"/>
-      <c r="BT9" s="191"/>
+      <c r="BQ9" s="199"/>
+      <c r="BR9" s="199"/>
+      <c r="BS9" s="199"/>
+      <c r="BT9" s="202"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="198"/>
-      <c r="C10" s="200"/>
-      <c r="D10" s="202"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="217"/>
+      <c r="D10" s="219"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -8099,11 +8043,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="207"/>
-      <c r="I10" s="212"/>
-      <c r="J10" s="214"/>
-      <c r="K10" s="214"/>
-      <c r="L10" s="217"/>
+      <c r="H10" s="224"/>
+      <c r="I10" s="192"/>
+      <c r="J10" s="194"/>
+      <c r="K10" s="194"/>
+      <c r="L10" s="197"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11712,80 +11656,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="208" t="str">
+      <c r="B45" s="188" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="209"/>
-      <c r="D45" s="209"/>
-      <c r="E45" s="209"/>
-      <c r="F45" s="209"/>
-      <c r="G45" s="209"/>
-      <c r="H45" s="209"/>
-      <c r="I45" s="209"/>
-      <c r="J45" s="209"/>
-      <c r="K45" s="209"/>
-      <c r="L45" s="209"/>
-      <c r="M45" s="209"/>
-      <c r="N45" s="209"/>
-      <c r="O45" s="209"/>
-      <c r="P45" s="209"/>
-      <c r="Q45" s="209"/>
-      <c r="R45" s="209"/>
-      <c r="S45" s="209"/>
-      <c r="T45" s="209"/>
-      <c r="U45" s="209"/>
-      <c r="V45" s="209"/>
-      <c r="W45" s="209"/>
-      <c r="X45" s="209"/>
-      <c r="Y45" s="209"/>
-      <c r="Z45" s="209"/>
-      <c r="AA45" s="209"/>
-      <c r="AB45" s="209"/>
-      <c r="AC45" s="209"/>
-      <c r="AD45" s="209"/>
-      <c r="AE45" s="209"/>
-      <c r="AF45" s="209"/>
-      <c r="AG45" s="209"/>
-      <c r="AH45" s="209"/>
-      <c r="AI45" s="209"/>
-      <c r="AJ45" s="209"/>
-      <c r="AK45" s="209"/>
-      <c r="AL45" s="209"/>
-      <c r="AM45" s="209"/>
-      <c r="AN45" s="209"/>
-      <c r="AO45" s="209"/>
-      <c r="AP45" s="209"/>
-      <c r="AQ45" s="209"/>
-      <c r="AR45" s="209"/>
-      <c r="AS45" s="209"/>
-      <c r="AT45" s="209"/>
-      <c r="AU45" s="209"/>
-      <c r="AV45" s="209"/>
-      <c r="AW45" s="209"/>
-      <c r="AX45" s="209"/>
-      <c r="AY45" s="209"/>
-      <c r="AZ45" s="209"/>
-      <c r="BA45" s="209"/>
-      <c r="BB45" s="209"/>
-      <c r="BC45" s="209"/>
-      <c r="BD45" s="209"/>
-      <c r="BE45" s="209"/>
-      <c r="BF45" s="209"/>
-      <c r="BG45" s="209"/>
-      <c r="BH45" s="209"/>
-      <c r="BI45" s="209"/>
-      <c r="BJ45" s="209"/>
-      <c r="BK45" s="209"/>
-      <c r="BL45" s="209"/>
-      <c r="BM45" s="209"/>
-      <c r="BN45" s="209"/>
-      <c r="BO45" s="209"/>
-      <c r="BP45" s="209"/>
-      <c r="BQ45" s="209"/>
-      <c r="BR45" s="209"/>
-      <c r="BS45" s="209"/>
-      <c r="BT45" s="210"/>
+      <c r="C45" s="189"/>
+      <c r="D45" s="189"/>
+      <c r="E45" s="189"/>
+      <c r="F45" s="189"/>
+      <c r="G45" s="189"/>
+      <c r="H45" s="189"/>
+      <c r="I45" s="189"/>
+      <c r="J45" s="189"/>
+      <c r="K45" s="189"/>
+      <c r="L45" s="189"/>
+      <c r="M45" s="189"/>
+      <c r="N45" s="189"/>
+      <c r="O45" s="189"/>
+      <c r="P45" s="189"/>
+      <c r="Q45" s="189"/>
+      <c r="R45" s="189"/>
+      <c r="S45" s="189"/>
+      <c r="T45" s="189"/>
+      <c r="U45" s="189"/>
+      <c r="V45" s="189"/>
+      <c r="W45" s="189"/>
+      <c r="X45" s="189"/>
+      <c r="Y45" s="189"/>
+      <c r="Z45" s="189"/>
+      <c r="AA45" s="189"/>
+      <c r="AB45" s="189"/>
+      <c r="AC45" s="189"/>
+      <c r="AD45" s="189"/>
+      <c r="AE45" s="189"/>
+      <c r="AF45" s="189"/>
+      <c r="AG45" s="189"/>
+      <c r="AH45" s="189"/>
+      <c r="AI45" s="189"/>
+      <c r="AJ45" s="189"/>
+      <c r="AK45" s="189"/>
+      <c r="AL45" s="189"/>
+      <c r="AM45" s="189"/>
+      <c r="AN45" s="189"/>
+      <c r="AO45" s="189"/>
+      <c r="AP45" s="189"/>
+      <c r="AQ45" s="189"/>
+      <c r="AR45" s="189"/>
+      <c r="AS45" s="189"/>
+      <c r="AT45" s="189"/>
+      <c r="AU45" s="189"/>
+      <c r="AV45" s="189"/>
+      <c r="AW45" s="189"/>
+      <c r="AX45" s="189"/>
+      <c r="AY45" s="189"/>
+      <c r="AZ45" s="189"/>
+      <c r="BA45" s="189"/>
+      <c r="BB45" s="189"/>
+      <c r="BC45" s="189"/>
+      <c r="BD45" s="189"/>
+      <c r="BE45" s="189"/>
+      <c r="BF45" s="189"/>
+      <c r="BG45" s="189"/>
+      <c r="BH45" s="189"/>
+      <c r="BI45" s="189"/>
+      <c r="BJ45" s="189"/>
+      <c r="BK45" s="189"/>
+      <c r="BL45" s="189"/>
+      <c r="BM45" s="189"/>
+      <c r="BN45" s="189"/>
+      <c r="BO45" s="189"/>
+      <c r="BP45" s="189"/>
+      <c r="BQ45" s="189"/>
+      <c r="BR45" s="189"/>
+      <c r="BS45" s="189"/>
+      <c r="BT45" s="190"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12748,6 +12692,14 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12764,14 +12716,6 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12779,15 +12723,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF7B3C16"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:CN1021"/>
+  <dimension ref="B1:CN1022"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12917,7 +12861,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="194" t="s">
+      <c r="K3" s="211" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -13014,7 +12958,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="195"/>
+      <c r="K4" s="212"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -13108,7 +13052,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="195"/>
+      <c r="K5" s="212"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -13202,7 +13146,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="195"/>
+      <c r="K6" s="212"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -13297,7 +13241,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="196"/>
+      <c r="K7" s="213"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -13383,152 +13327,152 @@
       <c r="CN7" s="175"/>
     </row>
     <row r="8" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="197" t="s">
+      <c r="B8" s="214" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="199" t="s">
+      <c r="C8" s="216" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="201" t="s">
+      <c r="D8" s="218" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="203" t="s">
+      <c r="E8" s="220" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="204"/>
-      <c r="G8" s="205"/>
-      <c r="H8" s="206" t="s">
+      <c r="F8" s="221"/>
+      <c r="G8" s="222"/>
+      <c r="H8" s="223" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="211" t="s">
+      <c r="I8" s="191" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="213" t="s">
+      <c r="J8" s="193" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="215" t="s">
+      <c r="K8" s="195" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="216" t="s">
+      <c r="L8" s="196" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="218" t="s">
+      <c r="M8" s="198" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="190"/>
-      <c r="O8" s="190"/>
-      <c r="P8" s="190"/>
-      <c r="Q8" s="219"/>
-      <c r="R8" s="220" t="s">
+      <c r="N8" s="199"/>
+      <c r="O8" s="199"/>
+      <c r="P8" s="199"/>
+      <c r="Q8" s="200"/>
+      <c r="R8" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="190"/>
-      <c r="T8" s="190"/>
-      <c r="U8" s="190"/>
-      <c r="V8" s="219"/>
-      <c r="W8" s="220" t="s">
+      <c r="S8" s="199"/>
+      <c r="T8" s="199"/>
+      <c r="U8" s="199"/>
+      <c r="V8" s="200"/>
+      <c r="W8" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="190"/>
-      <c r="Y8" s="190"/>
-      <c r="Z8" s="190"/>
-      <c r="AA8" s="191"/>
-      <c r="AB8" s="221" t="s">
+      <c r="X8" s="199"/>
+      <c r="Y8" s="199"/>
+      <c r="Z8" s="199"/>
+      <c r="AA8" s="202"/>
+      <c r="AB8" s="203" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="190"/>
-      <c r="AD8" s="190"/>
-      <c r="AE8" s="190"/>
-      <c r="AF8" s="219"/>
-      <c r="AG8" s="222" t="s">
+      <c r="AC8" s="199"/>
+      <c r="AD8" s="199"/>
+      <c r="AE8" s="199"/>
+      <c r="AF8" s="200"/>
+      <c r="AG8" s="204" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="190"/>
-      <c r="AI8" s="190"/>
-      <c r="AJ8" s="190"/>
-      <c r="AK8" s="219"/>
-      <c r="AL8" s="222" t="s">
+      <c r="AH8" s="199"/>
+      <c r="AI8" s="199"/>
+      <c r="AJ8" s="199"/>
+      <c r="AK8" s="200"/>
+      <c r="AL8" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="190"/>
-      <c r="AN8" s="190"/>
-      <c r="AO8" s="190"/>
-      <c r="AP8" s="191"/>
-      <c r="AQ8" s="223" t="s">
+      <c r="AM8" s="199"/>
+      <c r="AN8" s="199"/>
+      <c r="AO8" s="199"/>
+      <c r="AP8" s="202"/>
+      <c r="AQ8" s="205" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="190"/>
-      <c r="AS8" s="190"/>
-      <c r="AT8" s="190"/>
-      <c r="AU8" s="219"/>
-      <c r="AV8" s="224" t="s">
+      <c r="AR8" s="199"/>
+      <c r="AS8" s="199"/>
+      <c r="AT8" s="199"/>
+      <c r="AU8" s="200"/>
+      <c r="AV8" s="206" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="190"/>
-      <c r="AX8" s="190"/>
-      <c r="AY8" s="190"/>
-      <c r="AZ8" s="219"/>
-      <c r="BA8" s="224" t="s">
+      <c r="AW8" s="199"/>
+      <c r="AX8" s="199"/>
+      <c r="AY8" s="199"/>
+      <c r="AZ8" s="200"/>
+      <c r="BA8" s="206" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="190"/>
-      <c r="BC8" s="190"/>
-      <c r="BD8" s="190"/>
-      <c r="BE8" s="191"/>
-      <c r="BF8" s="230" t="s">
+      <c r="BB8" s="199"/>
+      <c r="BC8" s="199"/>
+      <c r="BD8" s="199"/>
+      <c r="BE8" s="202"/>
+      <c r="BF8" s="229" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="190"/>
-      <c r="BH8" s="190"/>
-      <c r="BI8" s="190"/>
-      <c r="BJ8" s="219"/>
-      <c r="BK8" s="189" t="s">
+      <c r="BG8" s="199"/>
+      <c r="BH8" s="199"/>
+      <c r="BI8" s="199"/>
+      <c r="BJ8" s="200"/>
+      <c r="BK8" s="208" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="190"/>
-      <c r="BM8" s="190"/>
-      <c r="BN8" s="190"/>
-      <c r="BO8" s="219"/>
-      <c r="BP8" s="189" t="s">
+      <c r="BL8" s="199"/>
+      <c r="BM8" s="199"/>
+      <c r="BN8" s="199"/>
+      <c r="BO8" s="200"/>
+      <c r="BP8" s="208" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="190"/>
-      <c r="BR8" s="190"/>
-      <c r="BS8" s="190"/>
-      <c r="BT8" s="191"/>
-      <c r="BU8" s="226" t="s">
+      <c r="BQ8" s="199"/>
+      <c r="BR8" s="199"/>
+      <c r="BS8" s="199"/>
+      <c r="BT8" s="202"/>
+      <c r="BU8" s="225" t="s">
         <v>275</v>
       </c>
-      <c r="BV8" s="227"/>
-      <c r="BW8" s="227"/>
-      <c r="BX8" s="227"/>
-      <c r="BY8" s="228"/>
-      <c r="BZ8" s="226" t="s">
+      <c r="BV8" s="226"/>
+      <c r="BW8" s="226"/>
+      <c r="BX8" s="226"/>
+      <c r="BY8" s="227"/>
+      <c r="BZ8" s="225" t="s">
         <v>276</v>
       </c>
-      <c r="CA8" s="227"/>
-      <c r="CB8" s="227"/>
-      <c r="CC8" s="227"/>
-      <c r="CD8" s="228"/>
-      <c r="CE8" s="226" t="s">
+      <c r="CA8" s="226"/>
+      <c r="CB8" s="226"/>
+      <c r="CC8" s="226"/>
+      <c r="CD8" s="227"/>
+      <c r="CE8" s="225" t="s">
         <v>277</v>
       </c>
-      <c r="CF8" s="227"/>
-      <c r="CG8" s="227"/>
-      <c r="CH8" s="227"/>
-      <c r="CI8" s="228"/>
-      <c r="CJ8" s="226" t="s">
+      <c r="CF8" s="226"/>
+      <c r="CG8" s="226"/>
+      <c r="CH8" s="226"/>
+      <c r="CI8" s="227"/>
+      <c r="CJ8" s="225" t="s">
         <v>278</v>
       </c>
-      <c r="CK8" s="227"/>
-      <c r="CL8" s="227"/>
-      <c r="CM8" s="227"/>
-      <c r="CN8" s="228"/>
+      <c r="CK8" s="226"/>
+      <c r="CL8" s="226"/>
+      <c r="CM8" s="226"/>
+      <c r="CN8" s="227"/>
     </row>
     <row r="9" spans="2:92" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="198"/>
-      <c r="C9" s="200"/>
-      <c r="D9" s="202"/>
+      <c r="B9" s="215"/>
+      <c r="C9" s="217"/>
+      <c r="D9" s="219"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -13538,11 +13482,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="207"/>
-      <c r="I9" s="212"/>
-      <c r="J9" s="214"/>
-      <c r="K9" s="214"/>
-      <c r="L9" s="217"/>
+      <c r="H9" s="224"/>
+      <c r="I9" s="192"/>
+      <c r="J9" s="194"/>
+      <c r="K9" s="194"/>
+      <c r="L9" s="197"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -19167,7 +19111,7 @@
       <c r="CM55" s="65"/>
       <c r="CN55" s="65"/>
     </row>
-    <row r="56" spans="2:92" s="188" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:92" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="179" t="s">
         <v>307</v>
       </c>
@@ -19194,11 +19138,11 @@
         <v>45510</v>
       </c>
       <c r="J56" s="89">
-        <v>45511</v>
+        <v>45510</v>
       </c>
       <c r="K56" s="90">
         <f t="shared" ref="K56" si="32">J56-I56+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L56" s="91">
         <f t="shared" ref="L56" si="33">F56/E56</f>
@@ -19285,1104 +19229,1221 @@
       <c r="CM56" s="65"/>
       <c r="CN56" s="65"/>
     </row>
-    <row r="57" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="4" t="s">
+    <row r="57" spans="2:92" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="179" t="s">
+        <v>308</v>
+      </c>
+      <c r="C57" s="180" t="s">
+        <v>309</v>
+      </c>
+      <c r="D57" s="186" t="s">
+        <v>207</v>
+      </c>
+      <c r="E57" s="84">
+        <v>1</v>
+      </c>
+      <c r="F57" s="85">
+        <v>1</v>
+      </c>
+      <c r="G57" s="86">
+        <f t="shared" ref="G57" si="34">E57-F57</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="87">
+        <v>5</v>
+      </c>
+      <c r="I57" s="88">
+        <v>45510</v>
+      </c>
+      <c r="J57" s="89">
+        <v>45510</v>
+      </c>
+      <c r="K57" s="90">
+        <f t="shared" ref="K57" si="35">J57-I57+1</f>
+        <v>1</v>
+      </c>
+      <c r="L57" s="91">
+        <f t="shared" ref="L57" si="36">F57/E57</f>
+        <v>1</v>
+      </c>
+      <c r="M57" s="92"/>
+      <c r="N57" s="93"/>
+      <c r="O57" s="93"/>
+      <c r="P57" s="93"/>
+      <c r="Q57" s="93"/>
+      <c r="R57" s="94"/>
+      <c r="S57" s="94"/>
+      <c r="T57" s="94"/>
+      <c r="U57" s="94"/>
+      <c r="V57" s="94"/>
+      <c r="W57" s="93"/>
+      <c r="X57" s="93"/>
+      <c r="Y57" s="93"/>
+      <c r="Z57" s="93"/>
+      <c r="AA57" s="95"/>
+      <c r="AB57" s="92"/>
+      <c r="AC57" s="93"/>
+      <c r="AD57" s="93"/>
+      <c r="AE57" s="93"/>
+      <c r="AF57" s="93"/>
+      <c r="AG57" s="96"/>
+      <c r="AH57" s="96"/>
+      <c r="AI57" s="96"/>
+      <c r="AJ57" s="96"/>
+      <c r="AK57" s="96"/>
+      <c r="AL57" s="93"/>
+      <c r="AM57" s="93"/>
+      <c r="AN57" s="93"/>
+      <c r="AO57" s="93"/>
+      <c r="AP57" s="95"/>
+      <c r="AQ57" s="92"/>
+      <c r="AR57" s="93"/>
+      <c r="AS57" s="93"/>
+      <c r="AT57" s="93"/>
+      <c r="AU57" s="93"/>
+      <c r="AV57" s="97"/>
+      <c r="AW57" s="97"/>
+      <c r="AX57" s="97"/>
+      <c r="AY57" s="97"/>
+      <c r="AZ57" s="97"/>
+      <c r="BA57" s="93"/>
+      <c r="BB57" s="93"/>
+      <c r="BC57" s="93"/>
+      <c r="BD57" s="93"/>
+      <c r="BE57" s="95"/>
+      <c r="BF57" s="92"/>
+      <c r="BG57" s="93"/>
+      <c r="BH57" s="93"/>
+      <c r="BI57" s="93"/>
+      <c r="BJ57" s="93"/>
+      <c r="BK57" s="182"/>
+      <c r="BL57" s="183"/>
+      <c r="BM57" s="184"/>
+      <c r="BN57" s="183"/>
+      <c r="BO57" s="183"/>
+      <c r="BP57" s="65"/>
+      <c r="BQ57" s="65"/>
+      <c r="BR57" s="174"/>
+      <c r="BS57" s="65"/>
+      <c r="BT57" s="65"/>
+      <c r="BU57" s="65"/>
+      <c r="BV57" s="65"/>
+      <c r="BW57" s="174"/>
+      <c r="BX57" s="65"/>
+      <c r="BY57" s="65"/>
+      <c r="BZ57" s="65"/>
+      <c r="CA57" s="174"/>
+      <c r="CB57" s="174"/>
+      <c r="CC57" s="65"/>
+      <c r="CD57" s="65"/>
+      <c r="CE57" s="65"/>
+      <c r="CF57" s="175"/>
+      <c r="CG57" s="174"/>
+      <c r="CH57" s="65"/>
+      <c r="CI57" s="65"/>
+      <c r="CJ57" s="65"/>
+      <c r="CK57" s="65"/>
+      <c r="CL57" s="174"/>
+      <c r="CM57" s="65"/>
+      <c r="CN57" s="65"/>
+    </row>
+    <row r="58" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D57" s="100" t="s">
+      <c r="D58" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="E57" s="101">
+      <c r="E58" s="101">
         <f>SUM(E11:E16,E18:E21,E29:E37,E43:E47)</f>
         <v>68</v>
       </c>
-      <c r="F57" s="101">
+      <c r="F58" s="101">
         <f>SUM(F11:F16,F18:F21,F29:F37,F43:F47)</f>
         <v>68</v>
       </c>
-      <c r="G57" s="101">
+      <c r="G58" s="101">
         <f>SUM(G11:G16,G18:G21,G29:G37,G43:G47)</f>
         <v>0</v>
       </c>
-      <c r="H57" s="101">
+      <c r="H58" s="101">
         <v>60</v>
       </c>
-      <c r="I57" s="101">
-        <f>E57/H57</f>
+      <c r="I58" s="101">
+        <f>E58/H58</f>
         <v>1.1333333333333333</v>
       </c>
-      <c r="L57" s="102" t="s">
+      <c r="L58" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="M57" s="103">
+      <c r="M58" s="103">
         <v>1</v>
       </c>
-      <c r="N57" s="103">
+      <c r="N58" s="103">
         <v>2</v>
       </c>
-      <c r="O57" s="103">
+      <c r="O58" s="103">
         <v>3</v>
       </c>
-      <c r="P57" s="103">
+      <c r="P58" s="103">
         <v>4</v>
       </c>
-      <c r="Q57" s="103">
+      <c r="Q58" s="103">
         <v>5</v>
       </c>
-      <c r="R57" s="103">
+      <c r="R58" s="103">
         <v>6</v>
       </c>
-      <c r="S57" s="103">
+      <c r="S58" s="103">
         <v>7</v>
       </c>
-      <c r="T57" s="103">
+      <c r="T58" s="103">
         <v>8</v>
       </c>
-      <c r="U57" s="103">
+      <c r="U58" s="103">
         <v>9</v>
       </c>
-      <c r="V57" s="103">
+      <c r="V58" s="103">
         <v>10</v>
       </c>
-      <c r="W57" s="103">
+      <c r="W58" s="103">
         <v>11</v>
       </c>
-      <c r="X57" s="103">
+      <c r="X58" s="103">
         <v>12</v>
       </c>
-      <c r="Y57" s="103">
+      <c r="Y58" s="103">
         <v>13</v>
       </c>
-      <c r="Z57" s="103">
+      <c r="Z58" s="103">
         <v>14</v>
       </c>
-      <c r="AA57" s="103">
+      <c r="AA58" s="103">
         <v>15</v>
       </c>
-      <c r="AB57" s="103">
+      <c r="AB58" s="103">
         <v>16</v>
       </c>
-      <c r="AC57" s="103">
+      <c r="AC58" s="103">
         <v>17</v>
       </c>
-      <c r="AD57" s="103">
+      <c r="AD58" s="103">
         <v>18</v>
       </c>
-      <c r="AE57" s="103">
+      <c r="AE58" s="103">
         <v>19</v>
       </c>
-      <c r="AF57" s="103">
+      <c r="AF58" s="103">
         <v>20</v>
       </c>
-      <c r="AG57" s="103">
+      <c r="AG58" s="103">
         <v>21</v>
       </c>
-      <c r="AH57" s="103">
+      <c r="AH58" s="103">
         <v>22</v>
       </c>
-      <c r="AI57" s="103">
+      <c r="AI58" s="103">
         <v>23</v>
       </c>
-      <c r="AJ57" s="103">
+      <c r="AJ58" s="103">
         <v>24</v>
       </c>
-      <c r="AK57" s="103">
+      <c r="AK58" s="103">
         <v>25</v>
       </c>
-      <c r="AL57" s="103">
+      <c r="AL58" s="103">
         <v>26</v>
       </c>
-      <c r="AM57" s="103">
+      <c r="AM58" s="103">
         <v>27</v>
       </c>
-      <c r="AN57" s="103">
+      <c r="AN58" s="103">
         <v>28</v>
       </c>
-      <c r="AO57" s="103">
+      <c r="AO58" s="103">
         <v>29</v>
       </c>
-      <c r="AP57" s="103">
+      <c r="AP58" s="103">
         <v>30</v>
       </c>
-      <c r="AQ57" s="103">
+      <c r="AQ58" s="103">
         <v>31</v>
       </c>
-      <c r="AR57" s="103">
+      <c r="AR58" s="103">
         <v>32</v>
       </c>
-      <c r="AS57" s="103">
+      <c r="AS58" s="103">
         <v>33</v>
       </c>
-      <c r="AT57" s="103">
+      <c r="AT58" s="103">
         <v>34</v>
       </c>
-      <c r="AU57" s="103">
+      <c r="AU58" s="103">
         <v>35</v>
       </c>
-      <c r="AV57" s="103">
+      <c r="AV58" s="103">
         <v>36</v>
       </c>
-      <c r="AW57" s="103">
+      <c r="AW58" s="103">
         <v>37</v>
       </c>
-      <c r="AX57" s="103">
+      <c r="AX58" s="103">
         <v>38</v>
       </c>
-      <c r="AY57" s="103">
+      <c r="AY58" s="103">
         <v>39</v>
       </c>
-      <c r="AZ57" s="103">
+      <c r="AZ58" s="103">
         <v>40</v>
       </c>
-      <c r="BA57" s="103">
+      <c r="BA58" s="103">
         <v>41</v>
       </c>
-      <c r="BB57" s="103">
+      <c r="BB58" s="103">
         <v>42</v>
       </c>
-      <c r="BC57" s="103">
+      <c r="BC58" s="103">
         <v>43</v>
       </c>
-      <c r="BD57" s="103">
+      <c r="BD58" s="103">
         <v>44</v>
       </c>
-      <c r="BE57" s="103">
+      <c r="BE58" s="103">
         <v>45</v>
       </c>
-      <c r="BF57" s="103">
+      <c r="BF58" s="103">
         <v>46</v>
       </c>
-      <c r="BG57" s="103">
+      <c r="BG58" s="103">
         <v>47</v>
       </c>
-      <c r="BH57" s="103">
+      <c r="BH58" s="103">
         <v>48</v>
       </c>
-      <c r="BI57" s="103">
+      <c r="BI58" s="103">
         <v>49</v>
       </c>
-      <c r="BJ57" s="103">
+      <c r="BJ58" s="103">
         <v>50</v>
       </c>
-      <c r="BK57" s="103">
+      <c r="BK58" s="103">
         <v>51</v>
       </c>
-      <c r="BL57" s="103">
+      <c r="BL58" s="103">
         <v>52</v>
       </c>
-      <c r="BM57" s="103">
+      <c r="BM58" s="103">
         <v>53</v>
       </c>
-      <c r="BN57" s="103">
+      <c r="BN58" s="103">
         <v>54</v>
       </c>
-      <c r="BO57" s="103">
+      <c r="BO58" s="103">
         <v>55</v>
       </c>
-      <c r="BP57" s="103">
+      <c r="BP58" s="103">
         <v>56</v>
       </c>
-      <c r="BQ57" s="103">
+      <c r="BQ58" s="103">
         <v>57</v>
       </c>
-      <c r="BR57" s="103">
+      <c r="BR58" s="103">
         <v>58</v>
       </c>
-      <c r="BS57" s="103">
+      <c r="BS58" s="103">
         <v>59</v>
       </c>
-      <c r="BT57" s="103">
+      <c r="BT58" s="103">
         <v>60</v>
       </c>
-      <c r="BV57" s="100" t="s">
+      <c r="BV58" s="100" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="58" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H58" s="104" t="s">
-        <v>78</v>
-      </c>
-      <c r="L58" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="M58" s="105">
-        <f>E57</f>
-        <v>68</v>
-      </c>
-      <c r="N58" s="106">
-        <f>M58-I57</f>
-        <v>66.86666666666666</v>
-      </c>
-      <c r="O58" s="106">
-        <f>N58-I57</f>
-        <v>65.73333333333332</v>
-      </c>
-      <c r="P58" s="106">
-        <f>O58-I57</f>
-        <v>64.59999999999998</v>
-      </c>
-      <c r="Q58" s="106">
-        <f>P58-I57</f>
-        <v>63.466666666666647</v>
-      </c>
-      <c r="R58" s="106">
-        <f>Q58-I57</f>
-        <v>62.333333333333314</v>
-      </c>
-      <c r="S58" s="106">
-        <f>R58-I57</f>
-        <v>61.199999999999982</v>
-      </c>
-      <c r="T58" s="106">
-        <f>S58-I57</f>
-        <v>60.066666666666649</v>
-      </c>
-      <c r="U58" s="106">
-        <f>T58-I57</f>
-        <v>58.933333333333316</v>
-      </c>
-      <c r="V58" s="106">
-        <f>U58-I57</f>
-        <v>57.799999999999983</v>
-      </c>
-      <c r="W58" s="106">
-        <f>V58-I57</f>
-        <v>56.66666666666665</v>
-      </c>
-      <c r="X58" s="106">
-        <f>W58-I57</f>
-        <v>55.533333333333317</v>
-      </c>
-      <c r="Y58" s="106">
-        <f>X58-I57</f>
-        <v>54.399999999999984</v>
-      </c>
-      <c r="Z58" s="106">
-        <f>Y58-I57</f>
-        <v>53.266666666666652</v>
-      </c>
-      <c r="AA58" s="106">
-        <f>Z58-I57</f>
-        <v>52.133333333333319</v>
-      </c>
-      <c r="AB58" s="106">
-        <f>AA58-I57</f>
-        <v>50.999999999999986</v>
-      </c>
-      <c r="AC58" s="106">
-        <f>AB58-I57</f>
-        <v>49.866666666666653</v>
-      </c>
-      <c r="AD58" s="106">
-        <f>AC58-I57</f>
-        <v>48.73333333333332</v>
-      </c>
-      <c r="AE58" s="106">
-        <f>AD58-I57</f>
-        <v>47.599999999999987</v>
-      </c>
-      <c r="AF58" s="106">
-        <f>AE58-I57</f>
-        <v>46.466666666666654</v>
-      </c>
-      <c r="AG58" s="106">
-        <f>AF58-I57</f>
-        <v>45.333333333333321</v>
-      </c>
-      <c r="AH58" s="106">
-        <f>AG58-I57</f>
-        <v>44.199999999999989</v>
-      </c>
-      <c r="AI58" s="106">
-        <f>AH58-I57</f>
-        <v>43.066666666666656</v>
-      </c>
-      <c r="AJ58" s="106">
-        <f>AI58-I57</f>
-        <v>41.933333333333323</v>
-      </c>
-      <c r="AK58" s="106">
-        <f>AJ58-I57</f>
-        <v>40.79999999999999</v>
-      </c>
-      <c r="AL58" s="106">
-        <f>AK58-I57</f>
-        <v>39.666666666666657</v>
-      </c>
-      <c r="AM58" s="106">
-        <f>AL58-I57</f>
-        <v>38.533333333333324</v>
-      </c>
-      <c r="AN58" s="106">
-        <f>AM58-I57</f>
-        <v>37.399999999999991</v>
-      </c>
-      <c r="AO58" s="106">
-        <f>AN58-I57</f>
-        <v>36.266666666666659</v>
-      </c>
-      <c r="AP58" s="106">
-        <f>AO58-I57</f>
-        <v>35.133333333333326</v>
-      </c>
-      <c r="AQ58" s="106">
-        <f>AP58-I57</f>
-        <v>33.999999999999993</v>
-      </c>
-      <c r="AR58" s="106">
-        <f>AQ58-I57</f>
-        <v>32.86666666666666</v>
-      </c>
-      <c r="AS58" s="106">
-        <f>AR58-I57</f>
-        <v>31.733333333333327</v>
-      </c>
-      <c r="AT58" s="106">
-        <f>AS58-I57</f>
-        <v>30.599999999999994</v>
-      </c>
-      <c r="AU58" s="106">
-        <f>AT58-I57</f>
-        <v>29.466666666666661</v>
-      </c>
-      <c r="AV58" s="106">
-        <f>AU58-I57</f>
-        <v>28.333333333333329</v>
-      </c>
-      <c r="AW58" s="106">
-        <f>AV58-I57</f>
-        <v>27.199999999999996</v>
-      </c>
-      <c r="AX58" s="106">
-        <f>AW58-I57</f>
-        <v>26.066666666666663</v>
-      </c>
-      <c r="AY58" s="106">
-        <f>AX58-I57</f>
-        <v>24.93333333333333</v>
-      </c>
-      <c r="AZ58" s="106">
-        <f>AY58-I57</f>
-        <v>23.799999999999997</v>
-      </c>
-      <c r="BA58" s="106">
-        <f>AZ58-I57</f>
-        <v>22.666666666666664</v>
-      </c>
-      <c r="BB58" s="106">
-        <f>BA58-I57</f>
-        <v>21.533333333333331</v>
-      </c>
-      <c r="BC58" s="106">
-        <f>BB58-I57</f>
-        <v>20.399999999999999</v>
-      </c>
-      <c r="BD58" s="106">
-        <f>BC58-I57</f>
-        <v>19.266666666666666</v>
-      </c>
-      <c r="BE58" s="106">
-        <f>BD58-I57</f>
-        <v>18.133333333333333</v>
-      </c>
-      <c r="BF58" s="106">
-        <f>BE58-I57</f>
-        <v>17</v>
-      </c>
-      <c r="BG58" s="106">
-        <f>BF58-I57</f>
-        <v>15.866666666666667</v>
-      </c>
-      <c r="BH58" s="106">
-        <f>BG58-I57</f>
-        <v>14.733333333333334</v>
-      </c>
-      <c r="BI58" s="106">
-        <f>BH58-I57</f>
-        <v>13.600000000000001</v>
-      </c>
-      <c r="BJ58" s="106">
-        <f>BI58-I57</f>
-        <v>12.466666666666669</v>
-      </c>
-      <c r="BK58" s="106">
-        <f>BJ58-I57</f>
-        <v>11.333333333333336</v>
-      </c>
-      <c r="BL58" s="106">
-        <f>BK58-I57</f>
-        <v>10.200000000000003</v>
-      </c>
-      <c r="BM58" s="106">
-        <f>BL58-I57</f>
-        <v>9.06666666666667</v>
-      </c>
-      <c r="BN58" s="106">
-        <f>BM58-I57</f>
-        <v>7.9333333333333371</v>
-      </c>
-      <c r="BO58" s="106">
-        <f>BN58-I57</f>
-        <v>6.8000000000000043</v>
-      </c>
-      <c r="BP58" s="106">
-        <f>BO58-I57</f>
-        <v>5.6666666666666714</v>
-      </c>
-      <c r="BQ58" s="106">
-        <f>BP58-I57</f>
-        <v>4.5333333333333385</v>
-      </c>
-      <c r="BR58" s="106">
-        <f>BQ58-I57</f>
-        <v>3.4000000000000052</v>
-      </c>
-      <c r="BS58" s="106">
-        <f>BR58-I57</f>
-        <v>2.2666666666666719</v>
-      </c>
-      <c r="BT58" s="106">
-        <f>BS58-I57</f>
-        <v>1.1333333333333386</v>
-      </c>
-      <c r="BV58" s="101"/>
     </row>
     <row r="59" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H59" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="L59" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="M59" s="105">
+        <f>E58</f>
+        <v>68</v>
+      </c>
+      <c r="N59" s="106">
+        <f>M59-I58</f>
+        <v>66.86666666666666</v>
+      </c>
+      <c r="O59" s="106">
+        <f>N59-I58</f>
+        <v>65.73333333333332</v>
+      </c>
+      <c r="P59" s="106">
+        <f>O59-I58</f>
+        <v>64.59999999999998</v>
+      </c>
+      <c r="Q59" s="106">
+        <f>P59-I58</f>
+        <v>63.466666666666647</v>
+      </c>
+      <c r="R59" s="106">
+        <f>Q59-I58</f>
+        <v>62.333333333333314</v>
+      </c>
+      <c r="S59" s="106">
+        <f>R59-I58</f>
+        <v>61.199999999999982</v>
+      </c>
+      <c r="T59" s="106">
+        <f>S59-I58</f>
+        <v>60.066666666666649</v>
+      </c>
+      <c r="U59" s="106">
+        <f>T59-I58</f>
+        <v>58.933333333333316</v>
+      </c>
+      <c r="V59" s="106">
+        <f>U59-I58</f>
+        <v>57.799999999999983</v>
+      </c>
+      <c r="W59" s="106">
+        <f>V59-I58</f>
+        <v>56.66666666666665</v>
+      </c>
+      <c r="X59" s="106">
+        <f>W59-I58</f>
+        <v>55.533333333333317</v>
+      </c>
+      <c r="Y59" s="106">
+        <f>X59-I58</f>
+        <v>54.399999999999984</v>
+      </c>
+      <c r="Z59" s="106">
+        <f>Y59-I58</f>
+        <v>53.266666666666652</v>
+      </c>
+      <c r="AA59" s="106">
+        <f>Z59-I58</f>
+        <v>52.133333333333319</v>
+      </c>
+      <c r="AB59" s="106">
+        <f>AA59-I58</f>
+        <v>50.999999999999986</v>
+      </c>
+      <c r="AC59" s="106">
+        <f>AB59-I58</f>
+        <v>49.866666666666653</v>
+      </c>
+      <c r="AD59" s="106">
+        <f>AC59-I58</f>
+        <v>48.73333333333332</v>
+      </c>
+      <c r="AE59" s="106">
+        <f>AD59-I58</f>
+        <v>47.599999999999987</v>
+      </c>
+      <c r="AF59" s="106">
+        <f>AE59-I58</f>
+        <v>46.466666666666654</v>
+      </c>
+      <c r="AG59" s="106">
+        <f>AF59-I58</f>
+        <v>45.333333333333321</v>
+      </c>
+      <c r="AH59" s="106">
+        <f>AG59-I58</f>
+        <v>44.199999999999989</v>
+      </c>
+      <c r="AI59" s="106">
+        <f>AH59-I58</f>
+        <v>43.066666666666656</v>
+      </c>
+      <c r="AJ59" s="106">
+        <f>AI59-I58</f>
+        <v>41.933333333333323</v>
+      </c>
+      <c r="AK59" s="106">
+        <f>AJ59-I58</f>
+        <v>40.79999999999999</v>
+      </c>
+      <c r="AL59" s="106">
+        <f>AK59-I58</f>
+        <v>39.666666666666657</v>
+      </c>
+      <c r="AM59" s="106">
+        <f>AL59-I58</f>
+        <v>38.533333333333324</v>
+      </c>
+      <c r="AN59" s="106">
+        <f>AM59-I58</f>
+        <v>37.399999999999991</v>
+      </c>
+      <c r="AO59" s="106">
+        <f>AN59-I58</f>
+        <v>36.266666666666659</v>
+      </c>
+      <c r="AP59" s="106">
+        <f>AO59-I58</f>
+        <v>35.133333333333326</v>
+      </c>
+      <c r="AQ59" s="106">
+        <f>AP59-I58</f>
+        <v>33.999999999999993</v>
+      </c>
+      <c r="AR59" s="106">
+        <f>AQ59-I58</f>
+        <v>32.86666666666666</v>
+      </c>
+      <c r="AS59" s="106">
+        <f>AR59-I58</f>
+        <v>31.733333333333327</v>
+      </c>
+      <c r="AT59" s="106">
+        <f>AS59-I58</f>
+        <v>30.599999999999994</v>
+      </c>
+      <c r="AU59" s="106">
+        <f>AT59-I58</f>
+        <v>29.466666666666661</v>
+      </c>
+      <c r="AV59" s="106">
+        <f>AU59-I58</f>
+        <v>28.333333333333329</v>
+      </c>
+      <c r="AW59" s="106">
+        <f>AV59-I58</f>
+        <v>27.199999999999996</v>
+      </c>
+      <c r="AX59" s="106">
+        <f>AW59-I58</f>
+        <v>26.066666666666663</v>
+      </c>
+      <c r="AY59" s="106">
+        <f>AX59-I58</f>
+        <v>24.93333333333333</v>
+      </c>
+      <c r="AZ59" s="106">
+        <f>AY59-I58</f>
+        <v>23.799999999999997</v>
+      </c>
+      <c r="BA59" s="106">
+        <f>AZ59-I58</f>
+        <v>22.666666666666664</v>
+      </c>
+      <c r="BB59" s="106">
+        <f>BA59-I58</f>
+        <v>21.533333333333331</v>
+      </c>
+      <c r="BC59" s="106">
+        <f>BB59-I58</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="BD59" s="106">
+        <f>BC59-I58</f>
+        <v>19.266666666666666</v>
+      </c>
+      <c r="BE59" s="106">
+        <f>BD59-I58</f>
+        <v>18.133333333333333</v>
+      </c>
+      <c r="BF59" s="106">
+        <f>BE59-I58</f>
+        <v>17</v>
+      </c>
+      <c r="BG59" s="106">
+        <f>BF59-I58</f>
+        <v>15.866666666666667</v>
+      </c>
+      <c r="BH59" s="106">
+        <f>BG59-I58</f>
+        <v>14.733333333333334</v>
+      </c>
+      <c r="BI59" s="106">
+        <f>BH59-I58</f>
+        <v>13.600000000000001</v>
+      </c>
+      <c r="BJ59" s="106">
+        <f>BI59-I58</f>
+        <v>12.466666666666669</v>
+      </c>
+      <c r="BK59" s="106">
+        <f>BJ59-I58</f>
+        <v>11.333333333333336</v>
+      </c>
+      <c r="BL59" s="106">
+        <f>BK59-I58</f>
+        <v>10.200000000000003</v>
+      </c>
+      <c r="BM59" s="106">
+        <f>BL59-I58</f>
+        <v>9.06666666666667</v>
+      </c>
+      <c r="BN59" s="106">
+        <f>BM59-I58</f>
+        <v>7.9333333333333371</v>
+      </c>
+      <c r="BO59" s="106">
+        <f>BN59-I58</f>
+        <v>6.8000000000000043</v>
+      </c>
+      <c r="BP59" s="106">
+        <f>BO59-I58</f>
+        <v>5.6666666666666714</v>
+      </c>
+      <c r="BQ59" s="106">
+        <f>BP59-I58</f>
+        <v>4.5333333333333385</v>
+      </c>
+      <c r="BR59" s="106">
+        <f>BQ59-I58</f>
+        <v>3.4000000000000052</v>
+      </c>
+      <c r="BS59" s="106">
+        <f>BR59-I58</f>
+        <v>2.2666666666666719</v>
+      </c>
+      <c r="BT59" s="106">
+        <f>BS59-I58</f>
+        <v>1.1333333333333386</v>
+      </c>
+      <c r="BV59" s="101"/>
+    </row>
+    <row r="60" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L60" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="M59" s="105">
-        <f>E57</f>
+      <c r="M60" s="105">
+        <f>E58</f>
         <v>68</v>
       </c>
-      <c r="N59" s="105">
-        <f t="shared" ref="N59:BT59" si="34">M61</f>
+      <c r="N60" s="105">
+        <f t="shared" ref="N60:BT60" si="37">M62</f>
         <v>68</v>
       </c>
-      <c r="O59" s="105">
-        <f t="shared" si="34"/>
+      <c r="O60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="P59" s="105">
-        <f t="shared" si="34"/>
+      <c r="P60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="Q59" s="105">
-        <f t="shared" si="34"/>
+      <c r="Q60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="R59" s="105">
-        <f t="shared" si="34"/>
+      <c r="R60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="S59" s="105">
-        <f t="shared" si="34"/>
+      <c r="S60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="T59" s="105">
-        <f t="shared" si="34"/>
+      <c r="T60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="U59" s="105">
-        <f t="shared" si="34"/>
+      <c r="U60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="V59" s="105">
-        <f t="shared" si="34"/>
+      <c r="V60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="W59" s="105">
-        <f t="shared" si="34"/>
+      <c r="W60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="X59" s="105">
-        <f t="shared" si="34"/>
+      <c r="X60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="Y59" s="105">
-        <f t="shared" si="34"/>
+      <c r="Y60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="Z59" s="105">
-        <f t="shared" si="34"/>
+      <c r="Z60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AA59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AA60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AB59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AB60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AC59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AC60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AD59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AD60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AE59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AE60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AF59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AF60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AG59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AG60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AH59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AH60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AI59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AI60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AJ59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AJ60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AK59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AK60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AL59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AL60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AM59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AM60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AN59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AN60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AO59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AO60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AP59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AP60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AQ59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AQ60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AR59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AR60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AS59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AS60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AT59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AT60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AU59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AU60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AV59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AV60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AW59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AW60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AX59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AX60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AY59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AY60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="AZ59" s="105">
-        <f t="shared" si="34"/>
+      <c r="AZ60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BA59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BA60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BB59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BB60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BC59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BC60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BD59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BD60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BE59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BE60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BF59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BF60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BG59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BG60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BH59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BH60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BI59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BI60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BJ59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BJ60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BK59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BK60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BL59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BL60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BM59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BM60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BN59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BN60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BO59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BO60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BP59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BP60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BQ59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BQ60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BR59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BR60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BS59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BS60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BT59" s="105">
-        <f t="shared" si="34"/>
+      <c r="BT60" s="105">
+        <f t="shared" si="37"/>
         <v>68</v>
       </c>
-      <c r="BV59" s="101">
-        <f t="shared" ref="BV59:BV61" si="35">SUM(M59:BT59)</f>
+      <c r="BV60" s="101">
+        <f t="shared" ref="BV60:BV62" si="38">SUM(M60:BT60)</f>
         <v>4080</v>
-      </c>
-    </row>
-    <row r="60" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K60" s="107" t="s">
-        <v>80</v>
-      </c>
-      <c r="L60" s="102" t="s">
-        <v>81</v>
-      </c>
-      <c r="M60" s="57"/>
-      <c r="N60" s="57"/>
-      <c r="O60" s="57"/>
-      <c r="P60" s="57"/>
-      <c r="Q60" s="57"/>
-      <c r="R60" s="57"/>
-      <c r="S60" s="57"/>
-      <c r="T60" s="57"/>
-      <c r="U60" s="57"/>
-      <c r="V60" s="57"/>
-      <c r="W60" s="57"/>
-      <c r="X60" s="57"/>
-      <c r="Y60" s="57"/>
-      <c r="Z60" s="57"/>
-      <c r="AA60" s="57"/>
-      <c r="AB60" s="57"/>
-      <c r="AC60" s="57"/>
-      <c r="AD60" s="57"/>
-      <c r="AE60" s="57"/>
-      <c r="AF60" s="57"/>
-      <c r="AG60" s="57"/>
-      <c r="AH60" s="57"/>
-      <c r="AI60" s="57"/>
-      <c r="AJ60" s="57"/>
-      <c r="AK60" s="57"/>
-      <c r="AL60" s="57"/>
-      <c r="AM60" s="57"/>
-      <c r="AN60" s="57"/>
-      <c r="AO60" s="57"/>
-      <c r="AP60" s="57"/>
-      <c r="AQ60" s="57"/>
-      <c r="AR60" s="57"/>
-      <c r="AS60" s="57"/>
-      <c r="AT60" s="57"/>
-      <c r="AU60" s="57"/>
-      <c r="AV60" s="57"/>
-      <c r="AW60" s="57"/>
-      <c r="AX60" s="57"/>
-      <c r="AY60" s="57"/>
-      <c r="AZ60" s="57"/>
-      <c r="BA60" s="57"/>
-      <c r="BB60" s="57"/>
-      <c r="BC60" s="57"/>
-      <c r="BD60" s="57"/>
-      <c r="BE60" s="57"/>
-      <c r="BF60" s="57"/>
-      <c r="BG60" s="57"/>
-      <c r="BH60" s="57"/>
-      <c r="BI60" s="57"/>
-      <c r="BJ60" s="57"/>
-      <c r="BK60" s="57"/>
-      <c r="BL60" s="57"/>
-      <c r="BM60" s="57"/>
-      <c r="BN60" s="57"/>
-      <c r="BO60" s="57"/>
-      <c r="BP60" s="57"/>
-      <c r="BQ60" s="57"/>
-      <c r="BR60" s="57"/>
-      <c r="BS60" s="57"/>
-      <c r="BT60" s="57"/>
-      <c r="BV60" s="101">
-        <f t="shared" si="35"/>
-        <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K61" s="107" t="s">
+        <v>80</v>
+      </c>
       <c r="L61" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="M61" s="57"/>
+      <c r="N61" s="57"/>
+      <c r="O61" s="57"/>
+      <c r="P61" s="57"/>
+      <c r="Q61" s="57"/>
+      <c r="R61" s="57"/>
+      <c r="S61" s="57"/>
+      <c r="T61" s="57"/>
+      <c r="U61" s="57"/>
+      <c r="V61" s="57"/>
+      <c r="W61" s="57"/>
+      <c r="X61" s="57"/>
+      <c r="Y61" s="57"/>
+      <c r="Z61" s="57"/>
+      <c r="AA61" s="57"/>
+      <c r="AB61" s="57"/>
+      <c r="AC61" s="57"/>
+      <c r="AD61" s="57"/>
+      <c r="AE61" s="57"/>
+      <c r="AF61" s="57"/>
+      <c r="AG61" s="57"/>
+      <c r="AH61" s="57"/>
+      <c r="AI61" s="57"/>
+      <c r="AJ61" s="57"/>
+      <c r="AK61" s="57"/>
+      <c r="AL61" s="57"/>
+      <c r="AM61" s="57"/>
+      <c r="AN61" s="57"/>
+      <c r="AO61" s="57"/>
+      <c r="AP61" s="57"/>
+      <c r="AQ61" s="57"/>
+      <c r="AR61" s="57"/>
+      <c r="AS61" s="57"/>
+      <c r="AT61" s="57"/>
+      <c r="AU61" s="57"/>
+      <c r="AV61" s="57"/>
+      <c r="AW61" s="57"/>
+      <c r="AX61" s="57"/>
+      <c r="AY61" s="57"/>
+      <c r="AZ61" s="57"/>
+      <c r="BA61" s="57"/>
+      <c r="BB61" s="57"/>
+      <c r="BC61" s="57"/>
+      <c r="BD61" s="57"/>
+      <c r="BE61" s="57"/>
+      <c r="BF61" s="57"/>
+      <c r="BG61" s="57"/>
+      <c r="BH61" s="57"/>
+      <c r="BI61" s="57"/>
+      <c r="BJ61" s="57"/>
+      <c r="BK61" s="57"/>
+      <c r="BL61" s="57"/>
+      <c r="BM61" s="57"/>
+      <c r="BN61" s="57"/>
+      <c r="BO61" s="57"/>
+      <c r="BP61" s="57"/>
+      <c r="BQ61" s="57"/>
+      <c r="BR61" s="57"/>
+      <c r="BS61" s="57"/>
+      <c r="BT61" s="57"/>
+      <c r="BV61" s="101">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L62" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M61" s="105">
-        <f t="shared" ref="M61:BT61" si="36">M59-M60</f>
+      <c r="M62" s="105">
+        <f t="shared" ref="M62:BT62" si="39">M60-M61</f>
         <v>68</v>
       </c>
-      <c r="N61" s="105">
-        <f t="shared" si="36"/>
+      <c r="N62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="O61" s="105">
-        <f t="shared" si="36"/>
+      <c r="O62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="P61" s="105">
-        <f t="shared" si="36"/>
+      <c r="P62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="Q61" s="105">
-        <f t="shared" si="36"/>
+      <c r="Q62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="R61" s="105">
-        <f t="shared" si="36"/>
+      <c r="R62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="S61" s="105">
-        <f t="shared" si="36"/>
+      <c r="S62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="T61" s="105">
-        <f t="shared" si="36"/>
+      <c r="T62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="U61" s="105">
-        <f t="shared" si="36"/>
+      <c r="U62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="V61" s="105">
-        <f t="shared" si="36"/>
+      <c r="V62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="W61" s="105">
-        <f t="shared" si="36"/>
+      <c r="W62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="X61" s="105">
-        <f t="shared" si="36"/>
+      <c r="X62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="Y61" s="105">
-        <f t="shared" si="36"/>
+      <c r="Y62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="Z61" s="105">
-        <f t="shared" si="36"/>
+      <c r="Z62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AA61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AA62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AB61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AB62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AC61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AC62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AD61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AD62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AE61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AE62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AF61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AF62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AG61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AG62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AH61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AH62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AI61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AI62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AJ61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AJ62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AK61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AK62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AL61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AL62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AM61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AM62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AN61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AN62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AO61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AO62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AP61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AP62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AQ61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AQ62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AR61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AR62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AS61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AS62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AT61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AT62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AU61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AU62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AV61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AV62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AW61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AW62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AX61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AX62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AY61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AY62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="AZ61" s="105">
-        <f t="shared" si="36"/>
+      <c r="AZ62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BA61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BA62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BB61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BB62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BC61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BC62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BD61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BD62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BE61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BE62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BF61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BF62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BG61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BG62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BH61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BH62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BI61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BI62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BJ61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BJ62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BK61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BK62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BL61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BL62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BM61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BM62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BN61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BN62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BO61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BO62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BP61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BP62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BQ61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BQ62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BR61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BR62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BS61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BS62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BT61" s="105">
-        <f t="shared" si="36"/>
+      <c r="BT62" s="105">
+        <f t="shared" si="39"/>
         <v>68</v>
       </c>
-      <c r="BV61" s="101">
-        <f t="shared" si="35"/>
+      <c r="BV62" s="101">
+        <f t="shared" si="38"/>
         <v>4080</v>
       </c>
     </row>
-    <row r="62" spans="2:92" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:92" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="3:54" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E65" s="229" t="s">
+    <row r="63" spans="2:92" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:92" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="3:54" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E66" s="228" t="s">
         <v>83</v>
       </c>
-      <c r="F65" s="209"/>
-      <c r="G65" s="209"/>
-      <c r="H65" s="209"/>
-      <c r="I65" s="209"/>
-      <c r="J65" s="209"/>
-      <c r="K65" s="209"/>
-      <c r="L65" s="209"/>
-      <c r="M65" s="209"/>
-      <c r="N65" s="209"/>
-      <c r="O65" s="209"/>
-      <c r="P65" s="209"/>
-      <c r="Q65" s="209"/>
-      <c r="R65" s="209"/>
-      <c r="S65" s="209"/>
-      <c r="T65" s="209"/>
-      <c r="U65" s="209"/>
-      <c r="V65" s="209"/>
-      <c r="W65" s="209"/>
-      <c r="X65" s="209"/>
-      <c r="Y65" s="209"/>
-      <c r="Z65" s="209"/>
-      <c r="AA65" s="209"/>
-      <c r="AB65" s="209"/>
-      <c r="AC65" s="209"/>
-      <c r="AD65" s="209"/>
-      <c r="AE65" s="209"/>
-      <c r="AF65" s="209"/>
-      <c r="AG65" s="209"/>
-      <c r="AH65" s="209"/>
-      <c r="AI65" s="209"/>
-      <c r="AJ65" s="209"/>
-      <c r="AK65" s="209"/>
-      <c r="AL65" s="209"/>
-      <c r="AM65" s="209"/>
-      <c r="AN65" s="209"/>
-      <c r="AO65" s="209"/>
-      <c r="AP65" s="209"/>
-      <c r="AQ65" s="209"/>
-      <c r="AR65" s="209"/>
-      <c r="AS65" s="209"/>
-      <c r="AT65" s="209"/>
-      <c r="AU65" s="209"/>
-      <c r="AV65" s="209"/>
-      <c r="AW65" s="209"/>
-      <c r="AX65" s="209"/>
-      <c r="AY65" s="209"/>
-      <c r="AZ65" s="209"/>
-      <c r="BA65" s="209"/>
-      <c r="BB65" s="210"/>
+      <c r="F66" s="189"/>
+      <c r="G66" s="189"/>
+      <c r="H66" s="189"/>
+      <c r="I66" s="189"/>
+      <c r="J66" s="189"/>
+      <c r="K66" s="189"/>
+      <c r="L66" s="189"/>
+      <c r="M66" s="189"/>
+      <c r="N66" s="189"/>
+      <c r="O66" s="189"/>
+      <c r="P66" s="189"/>
+      <c r="Q66" s="189"/>
+      <c r="R66" s="189"/>
+      <c r="S66" s="189"/>
+      <c r="T66" s="189"/>
+      <c r="U66" s="189"/>
+      <c r="V66" s="189"/>
+      <c r="W66" s="189"/>
+      <c r="X66" s="189"/>
+      <c r="Y66" s="189"/>
+      <c r="Z66" s="189"/>
+      <c r="AA66" s="189"/>
+      <c r="AB66" s="189"/>
+      <c r="AC66" s="189"/>
+      <c r="AD66" s="189"/>
+      <c r="AE66" s="189"/>
+      <c r="AF66" s="189"/>
+      <c r="AG66" s="189"/>
+      <c r="AH66" s="189"/>
+      <c r="AI66" s="189"/>
+      <c r="AJ66" s="189"/>
+      <c r="AK66" s="189"/>
+      <c r="AL66" s="189"/>
+      <c r="AM66" s="189"/>
+      <c r="AN66" s="189"/>
+      <c r="AO66" s="189"/>
+      <c r="AP66" s="189"/>
+      <c r="AQ66" s="189"/>
+      <c r="AR66" s="189"/>
+      <c r="AS66" s="189"/>
+      <c r="AT66" s="189"/>
+      <c r="AU66" s="189"/>
+      <c r="AV66" s="189"/>
+      <c r="AW66" s="189"/>
+      <c r="AX66" s="189"/>
+      <c r="AY66" s="189"/>
+      <c r="AZ66" s="189"/>
+      <c r="BA66" s="189"/>
+      <c r="BB66" s="190"/>
     </row>
-    <row r="66" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="3:54" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C70" s="108"/>
-      <c r="D70" s="108"/>
+    <row r="70" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="3:54" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="108"/>
+      <c r="D71" s="108"/>
     </row>
-    <row r="71" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -21333,13 +21394,25 @@
     <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="AL8:AP8"/>
+    <mergeCell ref="AQ8:AU8"/>
+    <mergeCell ref="AV8:AZ8"/>
+    <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
     <mergeCell ref="BU8:BY8"/>
     <mergeCell ref="BZ8:CD8"/>
     <mergeCell ref="CE8:CI8"/>
     <mergeCell ref="CJ8:CN8"/>
-    <mergeCell ref="E65:BB65"/>
+    <mergeCell ref="E66:BB66"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
     <mergeCell ref="BP8:BT8"/>
@@ -21351,17 +21424,6 @@
     <mergeCell ref="W8:AA8"/>
     <mergeCell ref="AB8:AF8"/>
     <mergeCell ref="AG8:AK8"/>
-    <mergeCell ref="AL8:AP8"/>
-    <mergeCell ref="AQ8:AU8"/>
-    <mergeCell ref="AV8:AZ8"/>
-    <mergeCell ref="BA8:BE8"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21371,15 +21433,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFDD8047"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B1:K999"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22048,7 +22110,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="115">
         <v>5</v>
       </c>
@@ -22062,8 +22124,8 @@
         <v>285</v>
       </c>
       <c r="F36" s="149"/>
-      <c r="G36" s="119" t="s">
-        <v>308</v>
+      <c r="G36" s="185" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -23085,12 +23147,12 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="25" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G27">
-    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23105,7 +23167,7 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="50" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23132,7 +23194,7 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23147,7 +23209,7 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="43" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23174,7 +23236,7 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23189,28 +23251,28 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="40" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28 G30:G34">
-    <cfRule type="cellIs" dxfId="14" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="56" operator="equal">
       <formula>$I$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="57" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="58" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="9" priority="58" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH(("Not Started"),(G28))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:G34">
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="7" priority="14" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(G29))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="15">
@@ -23236,13 +23298,75 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35:G38">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH(("In Progress"),(G35))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+      <formula>$I$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36:G37">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
+      <formula>$I$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G38">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>$I$3</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="9" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="63" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I5">
-    <cfRule type="containsText" dxfId="8" priority="60" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="1" priority="60" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(I3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="61">
@@ -23257,7 +23381,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="7" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="62" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23271,88 +23395,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
-      <formula>$I$5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
-    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH(("In Progress"),(G37))))</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G36">
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH(("In Progress"),(G36))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G36">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
-      <formula>$I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH(("In Progress"),(G35))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G38">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH(("In Progress"),(G38))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G38">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>$I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G28 G30:G34">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G28 G30:G34" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>$I$3:$I$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F35">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F35" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>$K$3:$K$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -23365,7 +23412,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFEAB290"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
modify comments and replies forum completed
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADFCD1F-3BE6-4569-8114-A78C8D912DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA9D699-41CC-4ADF-907F-6F59031D09B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLE Gantt Chart &amp; Burndown" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="312">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -966,6 +966,12 @@
   </si>
   <si>
     <t>forum improved features</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>modify comments and replies forum</t>
   </si>
 </sst>
 </file>
@@ -2810,53 +2816,11 @@
     <xf numFmtId="49" fontId="24" fillId="17" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2887,6 +2851,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="29" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2902,7 +2908,25 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="0" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -5505,7 +5529,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$61</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5562,7 +5586,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$58:$BT$58</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$59:$BT$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5751,7 +5775,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$61:$BT$61</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$62:$BT$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -5798,7 +5822,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$59</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5821,7 +5845,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$58:$BT$58</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$59:$BT$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6010,7 +6034,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$59:$BT$59</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$60:$BT$60</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6209,7 +6233,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$L$60</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$L$61</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6232,7 +6256,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$58:$BT$58</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$59:$BT$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6421,7 +6445,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'AD Gantt Chart &amp; Burndown'!$M$60:$BT$60</c:f>
+              <c:f>'AD Gantt Chart &amp; Burndown'!$M$61:$BT$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -6963,7 +6987,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="27632025" cy="7553325"/>
@@ -7028,7 +7052,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella2" displayName="Tabella2" ref="B2:G38" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella2" displayName="Tabella2" ref="B2:G38" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29">
   <autoFilter ref="B2:G38" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G38">
     <sortCondition ref="B2:B38"/>
@@ -7046,18 +7070,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabella1" displayName="Tabella1" ref="B3:G43" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabella1" displayName="Tabella1" ref="B3:G43" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26">
   <autoFilter ref="B3:G43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:G43">
     <sortCondition ref="D3:D43"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TASK TITLE" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="TASK DESCRIPTION" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="COMPONENT" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="PRIORITY" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ADDED BY" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="DATED ADDED" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TASK TITLE" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="TASK DESCRIPTION" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="COMPONENT" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="PRIORITY" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="ADDED BY" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="DATED ADDED" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7508,19 +7532,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="209" t="str">
+      <c r="BK2" s="191" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="210"/>
-      <c r="BM2" s="210"/>
-      <c r="BN2" s="210"/>
-      <c r="BO2" s="210"/>
-      <c r="BP2" s="210"/>
-      <c r="BQ2" s="210"/>
-      <c r="BR2" s="210"/>
-      <c r="BS2" s="210"/>
-      <c r="BT2" s="210"/>
+      <c r="BL2" s="192"/>
+      <c r="BM2" s="192"/>
+      <c r="BN2" s="192"/>
+      <c r="BO2" s="192"/>
+      <c r="BP2" s="192"/>
+      <c r="BQ2" s="192"/>
+      <c r="BR2" s="192"/>
+      <c r="BS2" s="192"/>
+      <c r="BT2" s="192"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -7548,7 +7572,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="211" t="s">
+      <c r="K4" s="193" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -7625,7 +7649,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="212"/>
+      <c r="K5" s="194"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -7700,7 +7724,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="212"/>
+      <c r="K6" s="194"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -7775,7 +7799,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="212"/>
+      <c r="K7" s="194"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -7850,7 +7874,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="213"/>
+      <c r="K8" s="195"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -7916,124 +7940,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="214" t="s">
+      <c r="B9" s="196" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="216" t="s">
+      <c r="C9" s="198" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="218" t="s">
+      <c r="D9" s="200" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="220" t="s">
+      <c r="E9" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="221"/>
-      <c r="G9" s="222"/>
-      <c r="H9" s="223" t="s">
+      <c r="F9" s="203"/>
+      <c r="G9" s="204"/>
+      <c r="H9" s="205" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="191" t="s">
+      <c r="I9" s="210" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="193" t="s">
+      <c r="J9" s="212" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="195" t="s">
+      <c r="K9" s="214" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="196" t="s">
+      <c r="L9" s="215" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="198" t="s">
+      <c r="M9" s="217" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="199"/>
-      <c r="O9" s="199"/>
-      <c r="P9" s="199"/>
-      <c r="Q9" s="200"/>
-      <c r="R9" s="201" t="s">
+      <c r="N9" s="189"/>
+      <c r="O9" s="189"/>
+      <c r="P9" s="189"/>
+      <c r="Q9" s="218"/>
+      <c r="R9" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="199"/>
-      <c r="T9" s="199"/>
-      <c r="U9" s="199"/>
-      <c r="V9" s="200"/>
-      <c r="W9" s="201" t="s">
+      <c r="S9" s="189"/>
+      <c r="T9" s="189"/>
+      <c r="U9" s="189"/>
+      <c r="V9" s="218"/>
+      <c r="W9" s="219" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="199"/>
-      <c r="Y9" s="199"/>
-      <c r="Z9" s="199"/>
-      <c r="AA9" s="202"/>
-      <c r="AB9" s="203" t="s">
+      <c r="X9" s="189"/>
+      <c r="Y9" s="189"/>
+      <c r="Z9" s="189"/>
+      <c r="AA9" s="190"/>
+      <c r="AB9" s="220" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="199"/>
-      <c r="AD9" s="199"/>
-      <c r="AE9" s="199"/>
-      <c r="AF9" s="200"/>
-      <c r="AG9" s="204" t="s">
+      <c r="AC9" s="189"/>
+      <c r="AD9" s="189"/>
+      <c r="AE9" s="189"/>
+      <c r="AF9" s="218"/>
+      <c r="AG9" s="221" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="199"/>
-      <c r="AI9" s="199"/>
-      <c r="AJ9" s="199"/>
-      <c r="AK9" s="200"/>
-      <c r="AL9" s="204" t="s">
+      <c r="AH9" s="189"/>
+      <c r="AI9" s="189"/>
+      <c r="AJ9" s="189"/>
+      <c r="AK9" s="218"/>
+      <c r="AL9" s="221" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="199"/>
-      <c r="AN9" s="199"/>
-      <c r="AO9" s="199"/>
-      <c r="AP9" s="202"/>
-      <c r="AQ9" s="205" t="s">
+      <c r="AM9" s="189"/>
+      <c r="AN9" s="189"/>
+      <c r="AO9" s="189"/>
+      <c r="AP9" s="190"/>
+      <c r="AQ9" s="222" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="199"/>
-      <c r="AS9" s="199"/>
-      <c r="AT9" s="199"/>
-      <c r="AU9" s="200"/>
-      <c r="AV9" s="206" t="s">
+      <c r="AR9" s="189"/>
+      <c r="AS9" s="189"/>
+      <c r="AT9" s="189"/>
+      <c r="AU9" s="218"/>
+      <c r="AV9" s="223" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="199"/>
-      <c r="AX9" s="199"/>
-      <c r="AY9" s="199"/>
-      <c r="AZ9" s="200"/>
-      <c r="BA9" s="206" t="s">
+      <c r="AW9" s="189"/>
+      <c r="AX9" s="189"/>
+      <c r="AY9" s="189"/>
+      <c r="AZ9" s="218"/>
+      <c r="BA9" s="223" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="199"/>
-      <c r="BC9" s="199"/>
-      <c r="BD9" s="199"/>
-      <c r="BE9" s="202"/>
-      <c r="BF9" s="207" t="s">
+      <c r="BB9" s="189"/>
+      <c r="BC9" s="189"/>
+      <c r="BD9" s="189"/>
+      <c r="BE9" s="190"/>
+      <c r="BF9" s="224" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="199"/>
-      <c r="BH9" s="199"/>
-      <c r="BI9" s="199"/>
-      <c r="BJ9" s="200"/>
-      <c r="BK9" s="208" t="s">
+      <c r="BG9" s="189"/>
+      <c r="BH9" s="189"/>
+      <c r="BI9" s="189"/>
+      <c r="BJ9" s="218"/>
+      <c r="BK9" s="188" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="199"/>
-      <c r="BM9" s="199"/>
-      <c r="BN9" s="199"/>
-      <c r="BO9" s="200"/>
-      <c r="BP9" s="208" t="s">
+      <c r="BL9" s="189"/>
+      <c r="BM9" s="189"/>
+      <c r="BN9" s="189"/>
+      <c r="BO9" s="218"/>
+      <c r="BP9" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="199"/>
-      <c r="BR9" s="199"/>
-      <c r="BS9" s="199"/>
-      <c r="BT9" s="202"/>
+      <c r="BQ9" s="189"/>
+      <c r="BR9" s="189"/>
+      <c r="BS9" s="189"/>
+      <c r="BT9" s="190"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="215"/>
-      <c r="C10" s="217"/>
-      <c r="D10" s="219"/>
+      <c r="B10" s="197"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="201"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -8043,11 +8067,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="224"/>
-      <c r="I10" s="192"/>
-      <c r="J10" s="194"/>
-      <c r="K10" s="194"/>
-      <c r="L10" s="197"/>
+      <c r="H10" s="206"/>
+      <c r="I10" s="211"/>
+      <c r="J10" s="213"/>
+      <c r="K10" s="213"/>
+      <c r="L10" s="216"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -11656,80 +11680,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="188" t="str">
+      <c r="B45" s="207" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="189"/>
-      <c r="D45" s="189"/>
-      <c r="E45" s="189"/>
-      <c r="F45" s="189"/>
-      <c r="G45" s="189"/>
-      <c r="H45" s="189"/>
-      <c r="I45" s="189"/>
-      <c r="J45" s="189"/>
-      <c r="K45" s="189"/>
-      <c r="L45" s="189"/>
-      <c r="M45" s="189"/>
-      <c r="N45" s="189"/>
-      <c r="O45" s="189"/>
-      <c r="P45" s="189"/>
-      <c r="Q45" s="189"/>
-      <c r="R45" s="189"/>
-      <c r="S45" s="189"/>
-      <c r="T45" s="189"/>
-      <c r="U45" s="189"/>
-      <c r="V45" s="189"/>
-      <c r="W45" s="189"/>
-      <c r="X45" s="189"/>
-      <c r="Y45" s="189"/>
-      <c r="Z45" s="189"/>
-      <c r="AA45" s="189"/>
-      <c r="AB45" s="189"/>
-      <c r="AC45" s="189"/>
-      <c r="AD45" s="189"/>
-      <c r="AE45" s="189"/>
-      <c r="AF45" s="189"/>
-      <c r="AG45" s="189"/>
-      <c r="AH45" s="189"/>
-      <c r="AI45" s="189"/>
-      <c r="AJ45" s="189"/>
-      <c r="AK45" s="189"/>
-      <c r="AL45" s="189"/>
-      <c r="AM45" s="189"/>
-      <c r="AN45" s="189"/>
-      <c r="AO45" s="189"/>
-      <c r="AP45" s="189"/>
-      <c r="AQ45" s="189"/>
-      <c r="AR45" s="189"/>
-      <c r="AS45" s="189"/>
-      <c r="AT45" s="189"/>
-      <c r="AU45" s="189"/>
-      <c r="AV45" s="189"/>
-      <c r="AW45" s="189"/>
-      <c r="AX45" s="189"/>
-      <c r="AY45" s="189"/>
-      <c r="AZ45" s="189"/>
-      <c r="BA45" s="189"/>
-      <c r="BB45" s="189"/>
-      <c r="BC45" s="189"/>
-      <c r="BD45" s="189"/>
-      <c r="BE45" s="189"/>
-      <c r="BF45" s="189"/>
-      <c r="BG45" s="189"/>
-      <c r="BH45" s="189"/>
-      <c r="BI45" s="189"/>
-      <c r="BJ45" s="189"/>
-      <c r="BK45" s="189"/>
-      <c r="BL45" s="189"/>
-      <c r="BM45" s="189"/>
-      <c r="BN45" s="189"/>
-      <c r="BO45" s="189"/>
-      <c r="BP45" s="189"/>
-      <c r="BQ45" s="189"/>
-      <c r="BR45" s="189"/>
-      <c r="BS45" s="189"/>
-      <c r="BT45" s="190"/>
+      <c r="C45" s="208"/>
+      <c r="D45" s="208"/>
+      <c r="E45" s="208"/>
+      <c r="F45" s="208"/>
+      <c r="G45" s="208"/>
+      <c r="H45" s="208"/>
+      <c r="I45" s="208"/>
+      <c r="J45" s="208"/>
+      <c r="K45" s="208"/>
+      <c r="L45" s="208"/>
+      <c r="M45" s="208"/>
+      <c r="N45" s="208"/>
+      <c r="O45" s="208"/>
+      <c r="P45" s="208"/>
+      <c r="Q45" s="208"/>
+      <c r="R45" s="208"/>
+      <c r="S45" s="208"/>
+      <c r="T45" s="208"/>
+      <c r="U45" s="208"/>
+      <c r="V45" s="208"/>
+      <c r="W45" s="208"/>
+      <c r="X45" s="208"/>
+      <c r="Y45" s="208"/>
+      <c r="Z45" s="208"/>
+      <c r="AA45" s="208"/>
+      <c r="AB45" s="208"/>
+      <c r="AC45" s="208"/>
+      <c r="AD45" s="208"/>
+      <c r="AE45" s="208"/>
+      <c r="AF45" s="208"/>
+      <c r="AG45" s="208"/>
+      <c r="AH45" s="208"/>
+      <c r="AI45" s="208"/>
+      <c r="AJ45" s="208"/>
+      <c r="AK45" s="208"/>
+      <c r="AL45" s="208"/>
+      <c r="AM45" s="208"/>
+      <c r="AN45" s="208"/>
+      <c r="AO45" s="208"/>
+      <c r="AP45" s="208"/>
+      <c r="AQ45" s="208"/>
+      <c r="AR45" s="208"/>
+      <c r="AS45" s="208"/>
+      <c r="AT45" s="208"/>
+      <c r="AU45" s="208"/>
+      <c r="AV45" s="208"/>
+      <c r="AW45" s="208"/>
+      <c r="AX45" s="208"/>
+      <c r="AY45" s="208"/>
+      <c r="AZ45" s="208"/>
+      <c r="BA45" s="208"/>
+      <c r="BB45" s="208"/>
+      <c r="BC45" s="208"/>
+      <c r="BD45" s="208"/>
+      <c r="BE45" s="208"/>
+      <c r="BF45" s="208"/>
+      <c r="BG45" s="208"/>
+      <c r="BH45" s="208"/>
+      <c r="BI45" s="208"/>
+      <c r="BJ45" s="208"/>
+      <c r="BK45" s="208"/>
+      <c r="BL45" s="208"/>
+      <c r="BM45" s="208"/>
+      <c r="BN45" s="208"/>
+      <c r="BO45" s="208"/>
+      <c r="BP45" s="208"/>
+      <c r="BQ45" s="208"/>
+      <c r="BR45" s="208"/>
+      <c r="BS45" s="208"/>
+      <c r="BT45" s="209"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12692,14 +12716,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -12716,6 +12732,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12728,10 +12752,10 @@
     <tabColor rgb="FF7B3C16"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:CN1022"/>
+  <dimension ref="B1:CN1023"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+      <selection activeCell="CF29" sqref="CF1:CF1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12752,8 +12776,9 @@
     <col min="79" max="79" width="3.125" customWidth="1"/>
     <col min="80" max="80" width="3.5" customWidth="1"/>
     <col min="81" max="81" width="3" customWidth="1"/>
-    <col min="82" max="83" width="2.75" customWidth="1"/>
-    <col min="84" max="84" width="4" customWidth="1"/>
+    <col min="82" max="82" width="2.75" customWidth="1"/>
+    <col min="83" max="83" width="2.625" customWidth="1"/>
+    <col min="84" max="84" width="3.125" customWidth="1"/>
     <col min="85" max="85" width="3.25" customWidth="1"/>
     <col min="86" max="86" width="4.25" customWidth="1"/>
     <col min="87" max="87" width="3.75" customWidth="1"/>
@@ -12861,7 +12886,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="211" t="s">
+      <c r="K3" s="193" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -12958,7 +12983,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="212"/>
+      <c r="K4" s="194"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -13052,7 +13077,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="212"/>
+      <c r="K5" s="194"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -13146,7 +13171,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="212"/>
+      <c r="K6" s="194"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -13241,7 +13266,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="213"/>
+      <c r="K7" s="195"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -13327,119 +13352,119 @@
       <c r="CN7" s="175"/>
     </row>
     <row r="8" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="214" t="s">
+      <c r="B8" s="196" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="216" t="s">
+      <c r="C8" s="198" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="218" t="s">
+      <c r="D8" s="200" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="220" t="s">
+      <c r="E8" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="221"/>
-      <c r="G8" s="222"/>
-      <c r="H8" s="223" t="s">
+      <c r="F8" s="203"/>
+      <c r="G8" s="204"/>
+      <c r="H8" s="205" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="191" t="s">
+      <c r="I8" s="210" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="193" t="s">
+      <c r="J8" s="212" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="195" t="s">
+      <c r="K8" s="214" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="196" t="s">
+      <c r="L8" s="215" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="198" t="s">
+      <c r="M8" s="217" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="199"/>
-      <c r="O8" s="199"/>
-      <c r="P8" s="199"/>
-      <c r="Q8" s="200"/>
-      <c r="R8" s="201" t="s">
+      <c r="N8" s="189"/>
+      <c r="O8" s="189"/>
+      <c r="P8" s="189"/>
+      <c r="Q8" s="218"/>
+      <c r="R8" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="199"/>
-      <c r="T8" s="199"/>
-      <c r="U8" s="199"/>
-      <c r="V8" s="200"/>
-      <c r="W8" s="201" t="s">
+      <c r="S8" s="189"/>
+      <c r="T8" s="189"/>
+      <c r="U8" s="189"/>
+      <c r="V8" s="218"/>
+      <c r="W8" s="219" t="s">
         <v>19</v>
       </c>
-      <c r="X8" s="199"/>
-      <c r="Y8" s="199"/>
-      <c r="Z8" s="199"/>
-      <c r="AA8" s="202"/>
-      <c r="AB8" s="203" t="s">
+      <c r="X8" s="189"/>
+      <c r="Y8" s="189"/>
+      <c r="Z8" s="189"/>
+      <c r="AA8" s="190"/>
+      <c r="AB8" s="220" t="s">
         <v>20</v>
       </c>
-      <c r="AC8" s="199"/>
-      <c r="AD8" s="199"/>
-      <c r="AE8" s="199"/>
-      <c r="AF8" s="200"/>
-      <c r="AG8" s="204" t="s">
+      <c r="AC8" s="189"/>
+      <c r="AD8" s="189"/>
+      <c r="AE8" s="189"/>
+      <c r="AF8" s="218"/>
+      <c r="AG8" s="221" t="s">
         <v>21</v>
       </c>
-      <c r="AH8" s="199"/>
-      <c r="AI8" s="199"/>
-      <c r="AJ8" s="199"/>
-      <c r="AK8" s="200"/>
-      <c r="AL8" s="204" t="s">
+      <c r="AH8" s="189"/>
+      <c r="AI8" s="189"/>
+      <c r="AJ8" s="189"/>
+      <c r="AK8" s="218"/>
+      <c r="AL8" s="221" t="s">
         <v>22</v>
       </c>
-      <c r="AM8" s="199"/>
-      <c r="AN8" s="199"/>
-      <c r="AO8" s="199"/>
-      <c r="AP8" s="202"/>
-      <c r="AQ8" s="205" t="s">
+      <c r="AM8" s="189"/>
+      <c r="AN8" s="189"/>
+      <c r="AO8" s="189"/>
+      <c r="AP8" s="190"/>
+      <c r="AQ8" s="222" t="s">
         <v>23</v>
       </c>
-      <c r="AR8" s="199"/>
-      <c r="AS8" s="199"/>
-      <c r="AT8" s="199"/>
-      <c r="AU8" s="200"/>
-      <c r="AV8" s="206" t="s">
+      <c r="AR8" s="189"/>
+      <c r="AS8" s="189"/>
+      <c r="AT8" s="189"/>
+      <c r="AU8" s="218"/>
+      <c r="AV8" s="223" t="s">
         <v>24</v>
       </c>
-      <c r="AW8" s="199"/>
-      <c r="AX8" s="199"/>
-      <c r="AY8" s="199"/>
-      <c r="AZ8" s="200"/>
-      <c r="BA8" s="206" t="s">
+      <c r="AW8" s="189"/>
+      <c r="AX8" s="189"/>
+      <c r="AY8" s="189"/>
+      <c r="AZ8" s="218"/>
+      <c r="BA8" s="223" t="s">
         <v>25</v>
       </c>
-      <c r="BB8" s="199"/>
-      <c r="BC8" s="199"/>
-      <c r="BD8" s="199"/>
-      <c r="BE8" s="202"/>
+      <c r="BB8" s="189"/>
+      <c r="BC8" s="189"/>
+      <c r="BD8" s="189"/>
+      <c r="BE8" s="190"/>
       <c r="BF8" s="229" t="s">
         <v>26</v>
       </c>
-      <c r="BG8" s="199"/>
-      <c r="BH8" s="199"/>
-      <c r="BI8" s="199"/>
-      <c r="BJ8" s="200"/>
-      <c r="BK8" s="208" t="s">
+      <c r="BG8" s="189"/>
+      <c r="BH8" s="189"/>
+      <c r="BI8" s="189"/>
+      <c r="BJ8" s="218"/>
+      <c r="BK8" s="188" t="s">
         <v>27</v>
       </c>
-      <c r="BL8" s="199"/>
-      <c r="BM8" s="199"/>
-      <c r="BN8" s="199"/>
-      <c r="BO8" s="200"/>
-      <c r="BP8" s="208" t="s">
+      <c r="BL8" s="189"/>
+      <c r="BM8" s="189"/>
+      <c r="BN8" s="189"/>
+      <c r="BO8" s="218"/>
+      <c r="BP8" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="BQ8" s="199"/>
-      <c r="BR8" s="199"/>
-      <c r="BS8" s="199"/>
-      <c r="BT8" s="202"/>
+      <c r="BQ8" s="189"/>
+      <c r="BR8" s="189"/>
+      <c r="BS8" s="189"/>
+      <c r="BT8" s="190"/>
       <c r="BU8" s="225" t="s">
         <v>275</v>
       </c>
@@ -13470,9 +13495,9 @@
       <c r="CN8" s="227"/>
     </row>
     <row r="9" spans="2:92" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="215"/>
-      <c r="C9" s="217"/>
-      <c r="D9" s="219"/>
+      <c r="B9" s="197"/>
+      <c r="C9" s="199"/>
+      <c r="D9" s="201"/>
       <c r="E9" s="24" t="s">
         <v>29</v>
       </c>
@@ -13482,11 +13507,11 @@
       <c r="G9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="224"/>
-      <c r="I9" s="192"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="194"/>
-      <c r="L9" s="197"/>
+      <c r="H9" s="206"/>
+      <c r="I9" s="211"/>
+      <c r="J9" s="213"/>
+      <c r="K9" s="213"/>
+      <c r="L9" s="216"/>
       <c r="M9" s="27" t="s">
         <v>32</v>
       </c>
@@ -19347,1104 +19372,1221 @@
       <c r="CM57" s="65"/>
       <c r="CN57" s="65"/>
     </row>
-    <row r="58" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="4" t="s">
+    <row r="58" spans="2:92" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="179" t="s">
+        <v>310</v>
+      </c>
+      <c r="C58" s="180" t="s">
+        <v>311</v>
+      </c>
+      <c r="D58" s="186" t="s">
+        <v>306</v>
+      </c>
+      <c r="E58" s="84">
+        <v>2</v>
+      </c>
+      <c r="F58" s="85">
+        <v>1</v>
+      </c>
+      <c r="G58" s="86">
+        <f t="shared" ref="G58" si="37">E58-F58</f>
+        <v>1</v>
+      </c>
+      <c r="H58" s="87">
+        <v>5</v>
+      </c>
+      <c r="I58" s="88">
+        <v>45511</v>
+      </c>
+      <c r="J58" s="89">
+        <v>45511</v>
+      </c>
+      <c r="K58" s="90">
+        <f t="shared" ref="K58" si="38">J58-I58+1</f>
+        <v>1</v>
+      </c>
+      <c r="L58" s="91">
+        <f t="shared" ref="L58" si="39">F58/E58</f>
+        <v>0.5</v>
+      </c>
+      <c r="M58" s="92"/>
+      <c r="N58" s="93"/>
+      <c r="O58" s="93"/>
+      <c r="P58" s="93"/>
+      <c r="Q58" s="93"/>
+      <c r="R58" s="94"/>
+      <c r="S58" s="94"/>
+      <c r="T58" s="94"/>
+      <c r="U58" s="94"/>
+      <c r="V58" s="94"/>
+      <c r="W58" s="93"/>
+      <c r="X58" s="93"/>
+      <c r="Y58" s="93"/>
+      <c r="Z58" s="93"/>
+      <c r="AA58" s="95"/>
+      <c r="AB58" s="92"/>
+      <c r="AC58" s="93"/>
+      <c r="AD58" s="93"/>
+      <c r="AE58" s="93"/>
+      <c r="AF58" s="93"/>
+      <c r="AG58" s="96"/>
+      <c r="AH58" s="96"/>
+      <c r="AI58" s="96"/>
+      <c r="AJ58" s="96"/>
+      <c r="AK58" s="96"/>
+      <c r="AL58" s="93"/>
+      <c r="AM58" s="93"/>
+      <c r="AN58" s="93"/>
+      <c r="AO58" s="93"/>
+      <c r="AP58" s="95"/>
+      <c r="AQ58" s="92"/>
+      <c r="AR58" s="93"/>
+      <c r="AS58" s="93"/>
+      <c r="AT58" s="93"/>
+      <c r="AU58" s="93"/>
+      <c r="AV58" s="97"/>
+      <c r="AW58" s="97"/>
+      <c r="AX58" s="97"/>
+      <c r="AY58" s="97"/>
+      <c r="AZ58" s="97"/>
+      <c r="BA58" s="93"/>
+      <c r="BB58" s="93"/>
+      <c r="BC58" s="93"/>
+      <c r="BD58" s="93"/>
+      <c r="BE58" s="95"/>
+      <c r="BF58" s="92"/>
+      <c r="BG58" s="93"/>
+      <c r="BH58" s="93"/>
+      <c r="BI58" s="93"/>
+      <c r="BJ58" s="93"/>
+      <c r="BK58" s="182"/>
+      <c r="BL58" s="183"/>
+      <c r="BM58" s="184"/>
+      <c r="BN58" s="183"/>
+      <c r="BO58" s="183"/>
+      <c r="BP58" s="65"/>
+      <c r="BQ58" s="65"/>
+      <c r="BR58" s="174"/>
+      <c r="BS58" s="65"/>
+      <c r="BT58" s="65"/>
+      <c r="BU58" s="65"/>
+      <c r="BV58" s="65"/>
+      <c r="BW58" s="174"/>
+      <c r="BX58" s="65"/>
+      <c r="BY58" s="65"/>
+      <c r="BZ58" s="65"/>
+      <c r="CA58" s="174"/>
+      <c r="CB58" s="174"/>
+      <c r="CC58" s="65"/>
+      <c r="CD58" s="65"/>
+      <c r="CE58" s="65"/>
+      <c r="CF58" s="65"/>
+      <c r="CG58" s="175"/>
+      <c r="CH58" s="65"/>
+      <c r="CI58" s="65"/>
+      <c r="CJ58" s="65"/>
+      <c r="CK58" s="65"/>
+      <c r="CL58" s="174"/>
+      <c r="CM58" s="65"/>
+      <c r="CN58" s="65"/>
+    </row>
+    <row r="59" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D58" s="100" t="s">
+      <c r="D59" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="E58" s="101">
+      <c r="E59" s="101">
         <f>SUM(E11:E16,E18:E21,E29:E37,E43:E47)</f>
         <v>68</v>
       </c>
-      <c r="F58" s="101">
+      <c r="F59" s="101">
         <f>SUM(F11:F16,F18:F21,F29:F37,F43:F47)</f>
         <v>68</v>
       </c>
-      <c r="G58" s="101">
+      <c r="G59" s="101">
         <f>SUM(G11:G16,G18:G21,G29:G37,G43:G47)</f>
         <v>0</v>
       </c>
-      <c r="H58" s="101">
+      <c r="H59" s="101">
         <v>60</v>
       </c>
-      <c r="I58" s="101">
-        <f>E58/H58</f>
+      <c r="I59" s="101">
+        <f>E59/H59</f>
         <v>1.1333333333333333</v>
       </c>
-      <c r="L58" s="102" t="s">
+      <c r="L59" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="M58" s="103">
+      <c r="M59" s="103">
         <v>1</v>
       </c>
-      <c r="N58" s="103">
+      <c r="N59" s="103">
         <v>2</v>
       </c>
-      <c r="O58" s="103">
+      <c r="O59" s="103">
         <v>3</v>
       </c>
-      <c r="P58" s="103">
+      <c r="P59" s="103">
         <v>4</v>
       </c>
-      <c r="Q58" s="103">
+      <c r="Q59" s="103">
         <v>5</v>
       </c>
-      <c r="R58" s="103">
+      <c r="R59" s="103">
         <v>6</v>
       </c>
-      <c r="S58" s="103">
+      <c r="S59" s="103">
         <v>7</v>
       </c>
-      <c r="T58" s="103">
+      <c r="T59" s="103">
         <v>8</v>
       </c>
-      <c r="U58" s="103">
+      <c r="U59" s="103">
         <v>9</v>
       </c>
-      <c r="V58" s="103">
+      <c r="V59" s="103">
         <v>10</v>
       </c>
-      <c r="W58" s="103">
+      <c r="W59" s="103">
         <v>11</v>
       </c>
-      <c r="X58" s="103">
+      <c r="X59" s="103">
         <v>12</v>
       </c>
-      <c r="Y58" s="103">
+      <c r="Y59" s="103">
         <v>13</v>
       </c>
-      <c r="Z58" s="103">
+      <c r="Z59" s="103">
         <v>14</v>
       </c>
-      <c r="AA58" s="103">
+      <c r="AA59" s="103">
         <v>15</v>
       </c>
-      <c r="AB58" s="103">
+      <c r="AB59" s="103">
         <v>16</v>
       </c>
-      <c r="AC58" s="103">
+      <c r="AC59" s="103">
         <v>17</v>
       </c>
-      <c r="AD58" s="103">
+      <c r="AD59" s="103">
         <v>18</v>
       </c>
-      <c r="AE58" s="103">
+      <c r="AE59" s="103">
         <v>19</v>
       </c>
-      <c r="AF58" s="103">
+      <c r="AF59" s="103">
         <v>20</v>
       </c>
-      <c r="AG58" s="103">
+      <c r="AG59" s="103">
         <v>21</v>
       </c>
-      <c r="AH58" s="103">
+      <c r="AH59" s="103">
         <v>22</v>
       </c>
-      <c r="AI58" s="103">
+      <c r="AI59" s="103">
         <v>23</v>
       </c>
-      <c r="AJ58" s="103">
+      <c r="AJ59" s="103">
         <v>24</v>
       </c>
-      <c r="AK58" s="103">
+      <c r="AK59" s="103">
         <v>25</v>
       </c>
-      <c r="AL58" s="103">
+      <c r="AL59" s="103">
         <v>26</v>
       </c>
-      <c r="AM58" s="103">
+      <c r="AM59" s="103">
         <v>27</v>
       </c>
-      <c r="AN58" s="103">
+      <c r="AN59" s="103">
         <v>28</v>
       </c>
-      <c r="AO58" s="103">
+      <c r="AO59" s="103">
         <v>29</v>
       </c>
-      <c r="AP58" s="103">
+      <c r="AP59" s="103">
         <v>30</v>
       </c>
-      <c r="AQ58" s="103">
+      <c r="AQ59" s="103">
         <v>31</v>
       </c>
-      <c r="AR58" s="103">
+      <c r="AR59" s="103">
         <v>32</v>
       </c>
-      <c r="AS58" s="103">
+      <c r="AS59" s="103">
         <v>33</v>
       </c>
-      <c r="AT58" s="103">
+      <c r="AT59" s="103">
         <v>34</v>
       </c>
-      <c r="AU58" s="103">
+      <c r="AU59" s="103">
         <v>35</v>
       </c>
-      <c r="AV58" s="103">
+      <c r="AV59" s="103">
         <v>36</v>
       </c>
-      <c r="AW58" s="103">
+      <c r="AW59" s="103">
         <v>37</v>
       </c>
-      <c r="AX58" s="103">
+      <c r="AX59" s="103">
         <v>38</v>
       </c>
-      <c r="AY58" s="103">
+      <c r="AY59" s="103">
         <v>39</v>
       </c>
-      <c r="AZ58" s="103">
+      <c r="AZ59" s="103">
         <v>40</v>
       </c>
-      <c r="BA58" s="103">
+      <c r="BA59" s="103">
         <v>41</v>
       </c>
-      <c r="BB58" s="103">
+      <c r="BB59" s="103">
         <v>42</v>
       </c>
-      <c r="BC58" s="103">
+      <c r="BC59" s="103">
         <v>43</v>
       </c>
-      <c r="BD58" s="103">
+      <c r="BD59" s="103">
         <v>44</v>
       </c>
-      <c r="BE58" s="103">
+      <c r="BE59" s="103">
         <v>45</v>
       </c>
-      <c r="BF58" s="103">
+      <c r="BF59" s="103">
         <v>46</v>
       </c>
-      <c r="BG58" s="103">
+      <c r="BG59" s="103">
         <v>47</v>
       </c>
-      <c r="BH58" s="103">
+      <c r="BH59" s="103">
         <v>48</v>
       </c>
-      <c r="BI58" s="103">
+      <c r="BI59" s="103">
         <v>49</v>
       </c>
-      <c r="BJ58" s="103">
+      <c r="BJ59" s="103">
         <v>50</v>
       </c>
-      <c r="BK58" s="103">
+      <c r="BK59" s="103">
         <v>51</v>
       </c>
-      <c r="BL58" s="103">
+      <c r="BL59" s="103">
         <v>52</v>
       </c>
-      <c r="BM58" s="103">
+      <c r="BM59" s="103">
         <v>53</v>
       </c>
-      <c r="BN58" s="103">
+      <c r="BN59" s="103">
         <v>54</v>
       </c>
-      <c r="BO58" s="103">
+      <c r="BO59" s="103">
         <v>55</v>
       </c>
-      <c r="BP58" s="103">
+      <c r="BP59" s="103">
         <v>56</v>
       </c>
-      <c r="BQ58" s="103">
+      <c r="BQ59" s="103">
         <v>57</v>
       </c>
-      <c r="BR58" s="103">
+      <c r="BR59" s="103">
         <v>58</v>
       </c>
-      <c r="BS58" s="103">
+      <c r="BS59" s="103">
         <v>59</v>
       </c>
-      <c r="BT58" s="103">
+      <c r="BT59" s="103">
         <v>60</v>
       </c>
-      <c r="BV58" s="100" t="s">
+      <c r="BV59" s="100" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="59" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H59" s="104" t="s">
-        <v>78</v>
-      </c>
-      <c r="L59" s="102" t="s">
-        <v>79</v>
-      </c>
-      <c r="M59" s="105">
-        <f>E58</f>
-        <v>68</v>
-      </c>
-      <c r="N59" s="106">
-        <f>M59-I58</f>
-        <v>66.86666666666666</v>
-      </c>
-      <c r="O59" s="106">
-        <f>N59-I58</f>
-        <v>65.73333333333332</v>
-      </c>
-      <c r="P59" s="106">
-        <f>O59-I58</f>
-        <v>64.59999999999998</v>
-      </c>
-      <c r="Q59" s="106">
-        <f>P59-I58</f>
-        <v>63.466666666666647</v>
-      </c>
-      <c r="R59" s="106">
-        <f>Q59-I58</f>
-        <v>62.333333333333314</v>
-      </c>
-      <c r="S59" s="106">
-        <f>R59-I58</f>
-        <v>61.199999999999982</v>
-      </c>
-      <c r="T59" s="106">
-        <f>S59-I58</f>
-        <v>60.066666666666649</v>
-      </c>
-      <c r="U59" s="106">
-        <f>T59-I58</f>
-        <v>58.933333333333316</v>
-      </c>
-      <c r="V59" s="106">
-        <f>U59-I58</f>
-        <v>57.799999999999983</v>
-      </c>
-      <c r="W59" s="106">
-        <f>V59-I58</f>
-        <v>56.66666666666665</v>
-      </c>
-      <c r="X59" s="106">
-        <f>W59-I58</f>
-        <v>55.533333333333317</v>
-      </c>
-      <c r="Y59" s="106">
-        <f>X59-I58</f>
-        <v>54.399999999999984</v>
-      </c>
-      <c r="Z59" s="106">
-        <f>Y59-I58</f>
-        <v>53.266666666666652</v>
-      </c>
-      <c r="AA59" s="106">
-        <f>Z59-I58</f>
-        <v>52.133333333333319</v>
-      </c>
-      <c r="AB59" s="106">
-        <f>AA59-I58</f>
-        <v>50.999999999999986</v>
-      </c>
-      <c r="AC59" s="106">
-        <f>AB59-I58</f>
-        <v>49.866666666666653</v>
-      </c>
-      <c r="AD59" s="106">
-        <f>AC59-I58</f>
-        <v>48.73333333333332</v>
-      </c>
-      <c r="AE59" s="106">
-        <f>AD59-I58</f>
-        <v>47.599999999999987</v>
-      </c>
-      <c r="AF59" s="106">
-        <f>AE59-I58</f>
-        <v>46.466666666666654</v>
-      </c>
-      <c r="AG59" s="106">
-        <f>AF59-I58</f>
-        <v>45.333333333333321</v>
-      </c>
-      <c r="AH59" s="106">
-        <f>AG59-I58</f>
-        <v>44.199999999999989</v>
-      </c>
-      <c r="AI59" s="106">
-        <f>AH59-I58</f>
-        <v>43.066666666666656</v>
-      </c>
-      <c r="AJ59" s="106">
-        <f>AI59-I58</f>
-        <v>41.933333333333323</v>
-      </c>
-      <c r="AK59" s="106">
-        <f>AJ59-I58</f>
-        <v>40.79999999999999</v>
-      </c>
-      <c r="AL59" s="106">
-        <f>AK59-I58</f>
-        <v>39.666666666666657</v>
-      </c>
-      <c r="AM59" s="106">
-        <f>AL59-I58</f>
-        <v>38.533333333333324</v>
-      </c>
-      <c r="AN59" s="106">
-        <f>AM59-I58</f>
-        <v>37.399999999999991</v>
-      </c>
-      <c r="AO59" s="106">
-        <f>AN59-I58</f>
-        <v>36.266666666666659</v>
-      </c>
-      <c r="AP59" s="106">
-        <f>AO59-I58</f>
-        <v>35.133333333333326</v>
-      </c>
-      <c r="AQ59" s="106">
-        <f>AP59-I58</f>
-        <v>33.999999999999993</v>
-      </c>
-      <c r="AR59" s="106">
-        <f>AQ59-I58</f>
-        <v>32.86666666666666</v>
-      </c>
-      <c r="AS59" s="106">
-        <f>AR59-I58</f>
-        <v>31.733333333333327</v>
-      </c>
-      <c r="AT59" s="106">
-        <f>AS59-I58</f>
-        <v>30.599999999999994</v>
-      </c>
-      <c r="AU59" s="106">
-        <f>AT59-I58</f>
-        <v>29.466666666666661</v>
-      </c>
-      <c r="AV59" s="106">
-        <f>AU59-I58</f>
-        <v>28.333333333333329</v>
-      </c>
-      <c r="AW59" s="106">
-        <f>AV59-I58</f>
-        <v>27.199999999999996</v>
-      </c>
-      <c r="AX59" s="106">
-        <f>AW59-I58</f>
-        <v>26.066666666666663</v>
-      </c>
-      <c r="AY59" s="106">
-        <f>AX59-I58</f>
-        <v>24.93333333333333</v>
-      </c>
-      <c r="AZ59" s="106">
-        <f>AY59-I58</f>
-        <v>23.799999999999997</v>
-      </c>
-      <c r="BA59" s="106">
-        <f>AZ59-I58</f>
-        <v>22.666666666666664</v>
-      </c>
-      <c r="BB59" s="106">
-        <f>BA59-I58</f>
-        <v>21.533333333333331</v>
-      </c>
-      <c r="BC59" s="106">
-        <f>BB59-I58</f>
-        <v>20.399999999999999</v>
-      </c>
-      <c r="BD59" s="106">
-        <f>BC59-I58</f>
-        <v>19.266666666666666</v>
-      </c>
-      <c r="BE59" s="106">
-        <f>BD59-I58</f>
-        <v>18.133333333333333</v>
-      </c>
-      <c r="BF59" s="106">
-        <f>BE59-I58</f>
-        <v>17</v>
-      </c>
-      <c r="BG59" s="106">
-        <f>BF59-I58</f>
-        <v>15.866666666666667</v>
-      </c>
-      <c r="BH59" s="106">
-        <f>BG59-I58</f>
-        <v>14.733333333333334</v>
-      </c>
-      <c r="BI59" s="106">
-        <f>BH59-I58</f>
-        <v>13.600000000000001</v>
-      </c>
-      <c r="BJ59" s="106">
-        <f>BI59-I58</f>
-        <v>12.466666666666669</v>
-      </c>
-      <c r="BK59" s="106">
-        <f>BJ59-I58</f>
-        <v>11.333333333333336</v>
-      </c>
-      <c r="BL59" s="106">
-        <f>BK59-I58</f>
-        <v>10.200000000000003</v>
-      </c>
-      <c r="BM59" s="106">
-        <f>BL59-I58</f>
-        <v>9.06666666666667</v>
-      </c>
-      <c r="BN59" s="106">
-        <f>BM59-I58</f>
-        <v>7.9333333333333371</v>
-      </c>
-      <c r="BO59" s="106">
-        <f>BN59-I58</f>
-        <v>6.8000000000000043</v>
-      </c>
-      <c r="BP59" s="106">
-        <f>BO59-I58</f>
-        <v>5.6666666666666714</v>
-      </c>
-      <c r="BQ59" s="106">
-        <f>BP59-I58</f>
-        <v>4.5333333333333385</v>
-      </c>
-      <c r="BR59" s="106">
-        <f>BQ59-I58</f>
-        <v>3.4000000000000052</v>
-      </c>
-      <c r="BS59" s="106">
-        <f>BR59-I58</f>
-        <v>2.2666666666666719</v>
-      </c>
-      <c r="BT59" s="106">
-        <f>BS59-I58</f>
-        <v>1.1333333333333386</v>
-      </c>
-      <c r="BV59" s="101"/>
     </row>
     <row r="60" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H60" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="L60" s="102" t="s">
+        <v>79</v>
+      </c>
+      <c r="M60" s="105">
+        <f>E59</f>
+        <v>68</v>
+      </c>
+      <c r="N60" s="106">
+        <f>M60-I59</f>
+        <v>66.86666666666666</v>
+      </c>
+      <c r="O60" s="106">
+        <f>N60-I59</f>
+        <v>65.73333333333332</v>
+      </c>
+      <c r="P60" s="106">
+        <f>O60-I59</f>
+        <v>64.59999999999998</v>
+      </c>
+      <c r="Q60" s="106">
+        <f>P60-I59</f>
+        <v>63.466666666666647</v>
+      </c>
+      <c r="R60" s="106">
+        <f>Q60-I59</f>
+        <v>62.333333333333314</v>
+      </c>
+      <c r="S60" s="106">
+        <f>R60-I59</f>
+        <v>61.199999999999982</v>
+      </c>
+      <c r="T60" s="106">
+        <f>S60-I59</f>
+        <v>60.066666666666649</v>
+      </c>
+      <c r="U60" s="106">
+        <f>T60-I59</f>
+        <v>58.933333333333316</v>
+      </c>
+      <c r="V60" s="106">
+        <f>U60-I59</f>
+        <v>57.799999999999983</v>
+      </c>
+      <c r="W60" s="106">
+        <f>V60-I59</f>
+        <v>56.66666666666665</v>
+      </c>
+      <c r="X60" s="106">
+        <f>W60-I59</f>
+        <v>55.533333333333317</v>
+      </c>
+      <c r="Y60" s="106">
+        <f>X60-I59</f>
+        <v>54.399999999999984</v>
+      </c>
+      <c r="Z60" s="106">
+        <f>Y60-I59</f>
+        <v>53.266666666666652</v>
+      </c>
+      <c r="AA60" s="106">
+        <f>Z60-I59</f>
+        <v>52.133333333333319</v>
+      </c>
+      <c r="AB60" s="106">
+        <f>AA60-I59</f>
+        <v>50.999999999999986</v>
+      </c>
+      <c r="AC60" s="106">
+        <f>AB60-I59</f>
+        <v>49.866666666666653</v>
+      </c>
+      <c r="AD60" s="106">
+        <f>AC60-I59</f>
+        <v>48.73333333333332</v>
+      </c>
+      <c r="AE60" s="106">
+        <f>AD60-I59</f>
+        <v>47.599999999999987</v>
+      </c>
+      <c r="AF60" s="106">
+        <f>AE60-I59</f>
+        <v>46.466666666666654</v>
+      </c>
+      <c r="AG60" s="106">
+        <f>AF60-I59</f>
+        <v>45.333333333333321</v>
+      </c>
+      <c r="AH60" s="106">
+        <f>AG60-I59</f>
+        <v>44.199999999999989</v>
+      </c>
+      <c r="AI60" s="106">
+        <f>AH60-I59</f>
+        <v>43.066666666666656</v>
+      </c>
+      <c r="AJ60" s="106">
+        <f>AI60-I59</f>
+        <v>41.933333333333323</v>
+      </c>
+      <c r="AK60" s="106">
+        <f>AJ60-I59</f>
+        <v>40.79999999999999</v>
+      </c>
+      <c r="AL60" s="106">
+        <f>AK60-I59</f>
+        <v>39.666666666666657</v>
+      </c>
+      <c r="AM60" s="106">
+        <f>AL60-I59</f>
+        <v>38.533333333333324</v>
+      </c>
+      <c r="AN60" s="106">
+        <f>AM60-I59</f>
+        <v>37.399999999999991</v>
+      </c>
+      <c r="AO60" s="106">
+        <f>AN60-I59</f>
+        <v>36.266666666666659</v>
+      </c>
+      <c r="AP60" s="106">
+        <f>AO60-I59</f>
+        <v>35.133333333333326</v>
+      </c>
+      <c r="AQ60" s="106">
+        <f>AP60-I59</f>
+        <v>33.999999999999993</v>
+      </c>
+      <c r="AR60" s="106">
+        <f>AQ60-I59</f>
+        <v>32.86666666666666</v>
+      </c>
+      <c r="AS60" s="106">
+        <f>AR60-I59</f>
+        <v>31.733333333333327</v>
+      </c>
+      <c r="AT60" s="106">
+        <f>AS60-I59</f>
+        <v>30.599999999999994</v>
+      </c>
+      <c r="AU60" s="106">
+        <f>AT60-I59</f>
+        <v>29.466666666666661</v>
+      </c>
+      <c r="AV60" s="106">
+        <f>AU60-I59</f>
+        <v>28.333333333333329</v>
+      </c>
+      <c r="AW60" s="106">
+        <f>AV60-I59</f>
+        <v>27.199999999999996</v>
+      </c>
+      <c r="AX60" s="106">
+        <f>AW60-I59</f>
+        <v>26.066666666666663</v>
+      </c>
+      <c r="AY60" s="106">
+        <f>AX60-I59</f>
+        <v>24.93333333333333</v>
+      </c>
+      <c r="AZ60" s="106">
+        <f>AY60-I59</f>
+        <v>23.799999999999997</v>
+      </c>
+      <c r="BA60" s="106">
+        <f>AZ60-I59</f>
+        <v>22.666666666666664</v>
+      </c>
+      <c r="BB60" s="106">
+        <f>BA60-I59</f>
+        <v>21.533333333333331</v>
+      </c>
+      <c r="BC60" s="106">
+        <f>BB60-I59</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="BD60" s="106">
+        <f>BC60-I59</f>
+        <v>19.266666666666666</v>
+      </c>
+      <c r="BE60" s="106">
+        <f>BD60-I59</f>
+        <v>18.133333333333333</v>
+      </c>
+      <c r="BF60" s="106">
+        <f>BE60-I59</f>
+        <v>17</v>
+      </c>
+      <c r="BG60" s="106">
+        <f>BF60-I59</f>
+        <v>15.866666666666667</v>
+      </c>
+      <c r="BH60" s="106">
+        <f>BG60-I59</f>
+        <v>14.733333333333334</v>
+      </c>
+      <c r="BI60" s="106">
+        <f>BH60-I59</f>
+        <v>13.600000000000001</v>
+      </c>
+      <c r="BJ60" s="106">
+        <f>BI60-I59</f>
+        <v>12.466666666666669</v>
+      </c>
+      <c r="BK60" s="106">
+        <f>BJ60-I59</f>
+        <v>11.333333333333336</v>
+      </c>
+      <c r="BL60" s="106">
+        <f>BK60-I59</f>
+        <v>10.200000000000003</v>
+      </c>
+      <c r="BM60" s="106">
+        <f>BL60-I59</f>
+        <v>9.06666666666667</v>
+      </c>
+      <c r="BN60" s="106">
+        <f>BM60-I59</f>
+        <v>7.9333333333333371</v>
+      </c>
+      <c r="BO60" s="106">
+        <f>BN60-I59</f>
+        <v>6.8000000000000043</v>
+      </c>
+      <c r="BP60" s="106">
+        <f>BO60-I59</f>
+        <v>5.6666666666666714</v>
+      </c>
+      <c r="BQ60" s="106">
+        <f>BP60-I59</f>
+        <v>4.5333333333333385</v>
+      </c>
+      <c r="BR60" s="106">
+        <f>BQ60-I59</f>
+        <v>3.4000000000000052</v>
+      </c>
+      <c r="BS60" s="106">
+        <f>BR60-I59</f>
+        <v>2.2666666666666719</v>
+      </c>
+      <c r="BT60" s="106">
+        <f>BS60-I59</f>
+        <v>1.1333333333333386</v>
+      </c>
+      <c r="BV60" s="101"/>
+    </row>
+    <row r="61" spans="2:92" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L61" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="M60" s="105">
-        <f>E58</f>
+      <c r="M61" s="105">
+        <f>E59</f>
         <v>68</v>
       </c>
-      <c r="N60" s="105">
-        <f t="shared" ref="N60:BT60" si="37">M62</f>
+      <c r="N61" s="105">
+        <f t="shared" ref="N61:BT61" si="40">M63</f>
         <v>68</v>
       </c>
-      <c r="O60" s="105">
-        <f t="shared" si="37"/>
+      <c r="O61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="P60" s="105">
-        <f t="shared" si="37"/>
+      <c r="P61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="Q60" s="105">
-        <f t="shared" si="37"/>
+      <c r="Q61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="R60" s="105">
-        <f t="shared" si="37"/>
+      <c r="R61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="S60" s="105">
-        <f t="shared" si="37"/>
+      <c r="S61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="T60" s="105">
-        <f t="shared" si="37"/>
+      <c r="T61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="U60" s="105">
-        <f t="shared" si="37"/>
+      <c r="U61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="V60" s="105">
-        <f t="shared" si="37"/>
+      <c r="V61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="W60" s="105">
-        <f t="shared" si="37"/>
+      <c r="W61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="X60" s="105">
-        <f t="shared" si="37"/>
+      <c r="X61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="Y60" s="105">
-        <f t="shared" si="37"/>
+      <c r="Y61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="Z60" s="105">
-        <f t="shared" si="37"/>
+      <c r="Z61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AA60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AA61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AB60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AB61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AC60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AC61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AD60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AD61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AE60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AE61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AF60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AF61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AG60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AG61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AH60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AH61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AI60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AI61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AJ60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AJ61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AK60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AK61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AL60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AL61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AM60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AM61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AN60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AN61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AO60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AO61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AP60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AP61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AQ60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AQ61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AR60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AR61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AS60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AS61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AT60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AT61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AU60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AU61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AV60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AV61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AW60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AW61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AX60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AX61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AY60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AY61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="AZ60" s="105">
-        <f t="shared" si="37"/>
+      <c r="AZ61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BA60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BA61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BB60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BB61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BC60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BC61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BD60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BD61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BE60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BE61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BF60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BF61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BG60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BG61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BH60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BH61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BI60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BI61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BJ60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BJ61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BK60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BK61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BL60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BL61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BM60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BM61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BN60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BN61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BO60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BO61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BP60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BP61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BQ60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BQ61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BR60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BR61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BS60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BS61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BT60" s="105">
-        <f t="shared" si="37"/>
+      <c r="BT61" s="105">
+        <f t="shared" si="40"/>
         <v>68</v>
       </c>
-      <c r="BV60" s="101">
-        <f t="shared" ref="BV60:BV62" si="38">SUM(M60:BT60)</f>
+      <c r="BV61" s="101">
+        <f t="shared" ref="BV61:BV63" si="41">SUM(M61:BT61)</f>
         <v>4080</v>
-      </c>
-    </row>
-    <row r="61" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K61" s="107" t="s">
-        <v>80</v>
-      </c>
-      <c r="L61" s="102" t="s">
-        <v>81</v>
-      </c>
-      <c r="M61" s="57"/>
-      <c r="N61" s="57"/>
-      <c r="O61" s="57"/>
-      <c r="P61" s="57"/>
-      <c r="Q61" s="57"/>
-      <c r="R61" s="57"/>
-      <c r="S61" s="57"/>
-      <c r="T61" s="57"/>
-      <c r="U61" s="57"/>
-      <c r="V61" s="57"/>
-      <c r="W61" s="57"/>
-      <c r="X61" s="57"/>
-      <c r="Y61" s="57"/>
-      <c r="Z61" s="57"/>
-      <c r="AA61" s="57"/>
-      <c r="AB61" s="57"/>
-      <c r="AC61" s="57"/>
-      <c r="AD61" s="57"/>
-      <c r="AE61" s="57"/>
-      <c r="AF61" s="57"/>
-      <c r="AG61" s="57"/>
-      <c r="AH61" s="57"/>
-      <c r="AI61" s="57"/>
-      <c r="AJ61" s="57"/>
-      <c r="AK61" s="57"/>
-      <c r="AL61" s="57"/>
-      <c r="AM61" s="57"/>
-      <c r="AN61" s="57"/>
-      <c r="AO61" s="57"/>
-      <c r="AP61" s="57"/>
-      <c r="AQ61" s="57"/>
-      <c r="AR61" s="57"/>
-      <c r="AS61" s="57"/>
-      <c r="AT61" s="57"/>
-      <c r="AU61" s="57"/>
-      <c r="AV61" s="57"/>
-      <c r="AW61" s="57"/>
-      <c r="AX61" s="57"/>
-      <c r="AY61" s="57"/>
-      <c r="AZ61" s="57"/>
-      <c r="BA61" s="57"/>
-      <c r="BB61" s="57"/>
-      <c r="BC61" s="57"/>
-      <c r="BD61" s="57"/>
-      <c r="BE61" s="57"/>
-      <c r="BF61" s="57"/>
-      <c r="BG61" s="57"/>
-      <c r="BH61" s="57"/>
-      <c r="BI61" s="57"/>
-      <c r="BJ61" s="57"/>
-      <c r="BK61" s="57"/>
-      <c r="BL61" s="57"/>
-      <c r="BM61" s="57"/>
-      <c r="BN61" s="57"/>
-      <c r="BO61" s="57"/>
-      <c r="BP61" s="57"/>
-      <c r="BQ61" s="57"/>
-      <c r="BR61" s="57"/>
-      <c r="BS61" s="57"/>
-      <c r="BT61" s="57"/>
-      <c r="BV61" s="101">
-        <f t="shared" si="38"/>
-        <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K62" s="107" t="s">
+        <v>80</v>
+      </c>
       <c r="L62" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="M62" s="57"/>
+      <c r="N62" s="57"/>
+      <c r="O62" s="57"/>
+      <c r="P62" s="57"/>
+      <c r="Q62" s="57"/>
+      <c r="R62" s="57"/>
+      <c r="S62" s="57"/>
+      <c r="T62" s="57"/>
+      <c r="U62" s="57"/>
+      <c r="V62" s="57"/>
+      <c r="W62" s="57"/>
+      <c r="X62" s="57"/>
+      <c r="Y62" s="57"/>
+      <c r="Z62" s="57"/>
+      <c r="AA62" s="57"/>
+      <c r="AB62" s="57"/>
+      <c r="AC62" s="57"/>
+      <c r="AD62" s="57"/>
+      <c r="AE62" s="57"/>
+      <c r="AF62" s="57"/>
+      <c r="AG62" s="57"/>
+      <c r="AH62" s="57"/>
+      <c r="AI62" s="57"/>
+      <c r="AJ62" s="57"/>
+      <c r="AK62" s="57"/>
+      <c r="AL62" s="57"/>
+      <c r="AM62" s="57"/>
+      <c r="AN62" s="57"/>
+      <c r="AO62" s="57"/>
+      <c r="AP62" s="57"/>
+      <c r="AQ62" s="57"/>
+      <c r="AR62" s="57"/>
+      <c r="AS62" s="57"/>
+      <c r="AT62" s="57"/>
+      <c r="AU62" s="57"/>
+      <c r="AV62" s="57"/>
+      <c r="AW62" s="57"/>
+      <c r="AX62" s="57"/>
+      <c r="AY62" s="57"/>
+      <c r="AZ62" s="57"/>
+      <c r="BA62" s="57"/>
+      <c r="BB62" s="57"/>
+      <c r="BC62" s="57"/>
+      <c r="BD62" s="57"/>
+      <c r="BE62" s="57"/>
+      <c r="BF62" s="57"/>
+      <c r="BG62" s="57"/>
+      <c r="BH62" s="57"/>
+      <c r="BI62" s="57"/>
+      <c r="BJ62" s="57"/>
+      <c r="BK62" s="57"/>
+      <c r="BL62" s="57"/>
+      <c r="BM62" s="57"/>
+      <c r="BN62" s="57"/>
+      <c r="BO62" s="57"/>
+      <c r="BP62" s="57"/>
+      <c r="BQ62" s="57"/>
+      <c r="BR62" s="57"/>
+      <c r="BS62" s="57"/>
+      <c r="BT62" s="57"/>
+      <c r="BV62" s="101">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L63" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="M62" s="105">
-        <f t="shared" ref="M62:BT62" si="39">M60-M61</f>
+      <c r="M63" s="105">
+        <f t="shared" ref="M63:BT63" si="42">M61-M62</f>
         <v>68</v>
       </c>
-      <c r="N62" s="105">
-        <f t="shared" si="39"/>
+      <c r="N63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="O62" s="105">
-        <f t="shared" si="39"/>
+      <c r="O63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="P62" s="105">
-        <f t="shared" si="39"/>
+      <c r="P63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="Q62" s="105">
-        <f t="shared" si="39"/>
+      <c r="Q63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="R62" s="105">
-        <f t="shared" si="39"/>
+      <c r="R63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="S62" s="105">
-        <f t="shared" si="39"/>
+      <c r="S63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="T62" s="105">
-        <f t="shared" si="39"/>
+      <c r="T63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="U62" s="105">
-        <f t="shared" si="39"/>
+      <c r="U63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="V62" s="105">
-        <f t="shared" si="39"/>
+      <c r="V63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="W62" s="105">
-        <f t="shared" si="39"/>
+      <c r="W63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="X62" s="105">
-        <f t="shared" si="39"/>
+      <c r="X63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="Y62" s="105">
-        <f t="shared" si="39"/>
+      <c r="Y63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="Z62" s="105">
-        <f t="shared" si="39"/>
+      <c r="Z63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AA62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AA63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AB62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AB63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AC62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AC63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AD62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AD63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AE62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AE63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AF62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AF63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AG62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AG63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AH62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AH63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AI62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AI63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AJ62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AJ63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AK62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AK63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AL62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AL63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AM62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AM63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AN62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AN63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AO62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AO63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AP62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AP63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AQ62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AQ63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AR62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AR63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AS62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AS63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AT62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AT63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AU62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AU63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AV62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AV63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AW62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AW63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AX62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AX63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AY62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AY63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="AZ62" s="105">
-        <f t="shared" si="39"/>
+      <c r="AZ63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BA62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BA63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BB62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BB63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BC62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BC63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BD62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BD63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BE62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BE63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BF62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BF63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BG62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BG63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BH62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BH63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BI62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BI63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BJ62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BJ63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BK62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BK63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BL62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BL63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BM62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BM63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BN62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BN63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BO62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BO63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BP62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BP63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BQ62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BQ63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BR62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BR63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BS62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BS63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BT62" s="105">
-        <f t="shared" si="39"/>
+      <c r="BT63" s="105">
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
-      <c r="BV62" s="101">
-        <f t="shared" si="38"/>
+      <c r="BV63" s="101">
+        <f t="shared" si="41"/>
         <v>4080</v>
       </c>
     </row>
-    <row r="63" spans="2:92" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:92" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="3:54" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E66" s="228" t="s">
+    <row r="64" spans="2:92" ht="381.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="3:54" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="3:54" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E67" s="228" t="s">
         <v>83</v>
       </c>
-      <c r="F66" s="189"/>
-      <c r="G66" s="189"/>
-      <c r="H66" s="189"/>
-      <c r="I66" s="189"/>
-      <c r="J66" s="189"/>
-      <c r="K66" s="189"/>
-      <c r="L66" s="189"/>
-      <c r="M66" s="189"/>
-      <c r="N66" s="189"/>
-      <c r="O66" s="189"/>
-      <c r="P66" s="189"/>
-      <c r="Q66" s="189"/>
-      <c r="R66" s="189"/>
-      <c r="S66" s="189"/>
-      <c r="T66" s="189"/>
-      <c r="U66" s="189"/>
-      <c r="V66" s="189"/>
-      <c r="W66" s="189"/>
-      <c r="X66" s="189"/>
-      <c r="Y66" s="189"/>
-      <c r="Z66" s="189"/>
-      <c r="AA66" s="189"/>
-      <c r="AB66" s="189"/>
-      <c r="AC66" s="189"/>
-      <c r="AD66" s="189"/>
-      <c r="AE66" s="189"/>
-      <c r="AF66" s="189"/>
-      <c r="AG66" s="189"/>
-      <c r="AH66" s="189"/>
-      <c r="AI66" s="189"/>
-      <c r="AJ66" s="189"/>
-      <c r="AK66" s="189"/>
-      <c r="AL66" s="189"/>
-      <c r="AM66" s="189"/>
-      <c r="AN66" s="189"/>
-      <c r="AO66" s="189"/>
-      <c r="AP66" s="189"/>
-      <c r="AQ66" s="189"/>
-      <c r="AR66" s="189"/>
-      <c r="AS66" s="189"/>
-      <c r="AT66" s="189"/>
-      <c r="AU66" s="189"/>
-      <c r="AV66" s="189"/>
-      <c r="AW66" s="189"/>
-      <c r="AX66" s="189"/>
-      <c r="AY66" s="189"/>
-      <c r="AZ66" s="189"/>
-      <c r="BA66" s="189"/>
-      <c r="BB66" s="190"/>
+      <c r="F67" s="208"/>
+      <c r="G67" s="208"/>
+      <c r="H67" s="208"/>
+      <c r="I67" s="208"/>
+      <c r="J67" s="208"/>
+      <c r="K67" s="208"/>
+      <c r="L67" s="208"/>
+      <c r="M67" s="208"/>
+      <c r="N67" s="208"/>
+      <c r="O67" s="208"/>
+      <c r="P67" s="208"/>
+      <c r="Q67" s="208"/>
+      <c r="R67" s="208"/>
+      <c r="S67" s="208"/>
+      <c r="T67" s="208"/>
+      <c r="U67" s="208"/>
+      <c r="V67" s="208"/>
+      <c r="W67" s="208"/>
+      <c r="X67" s="208"/>
+      <c r="Y67" s="208"/>
+      <c r="Z67" s="208"/>
+      <c r="AA67" s="208"/>
+      <c r="AB67" s="208"/>
+      <c r="AC67" s="208"/>
+      <c r="AD67" s="208"/>
+      <c r="AE67" s="208"/>
+      <c r="AF67" s="208"/>
+      <c r="AG67" s="208"/>
+      <c r="AH67" s="208"/>
+      <c r="AI67" s="208"/>
+      <c r="AJ67" s="208"/>
+      <c r="AK67" s="208"/>
+      <c r="AL67" s="208"/>
+      <c r="AM67" s="208"/>
+      <c r="AN67" s="208"/>
+      <c r="AO67" s="208"/>
+      <c r="AP67" s="208"/>
+      <c r="AQ67" s="208"/>
+      <c r="AR67" s="208"/>
+      <c r="AS67" s="208"/>
+      <c r="AT67" s="208"/>
+      <c r="AU67" s="208"/>
+      <c r="AV67" s="208"/>
+      <c r="AW67" s="208"/>
+      <c r="AX67" s="208"/>
+      <c r="AY67" s="208"/>
+      <c r="AZ67" s="208"/>
+      <c r="BA67" s="208"/>
+      <c r="BB67" s="209"/>
     </row>
-    <row r="67" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="3:54" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C71" s="108"/>
-      <c r="D71" s="108"/>
+    <row r="71" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="3:54" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="108"/>
+      <c r="D72" s="108"/>
     </row>
-    <row r="72" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="3:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -21395,24 +21537,14 @@
     <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1021" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1022" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="AL8:AP8"/>
-    <mergeCell ref="AQ8:AU8"/>
-    <mergeCell ref="AV8:AZ8"/>
-    <mergeCell ref="BA8:BE8"/>
-    <mergeCell ref="K3:K7"/>
     <mergeCell ref="BU8:BY8"/>
     <mergeCell ref="BZ8:CD8"/>
     <mergeCell ref="CE8:CI8"/>
     <mergeCell ref="CJ8:CN8"/>
-    <mergeCell ref="E66:BB66"/>
+    <mergeCell ref="E67:BB67"/>
     <mergeCell ref="BF8:BJ8"/>
     <mergeCell ref="BK8:BO8"/>
     <mergeCell ref="BP8:BT8"/>
@@ -21424,6 +21556,17 @@
     <mergeCell ref="W8:AA8"/>
     <mergeCell ref="AB8:AF8"/>
     <mergeCell ref="AG8:AK8"/>
+    <mergeCell ref="AL8:AP8"/>
+    <mergeCell ref="AQ8:AU8"/>
+    <mergeCell ref="AV8:AZ8"/>
+    <mergeCell ref="BA8:BE8"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21440,8 +21583,8 @@
   </sheetPr>
   <dimension ref="B1:K999"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView showGridLines="0" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22106,8 +22249,8 @@
         <v>285</v>
       </c>
       <c r="F35" s="150"/>
-      <c r="G35" s="121" t="s">
-        <v>90</v>
+      <c r="G35" s="185" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -22160,8 +22303,8 @@
         <v>285</v>
       </c>
       <c r="F38" s="149"/>
-      <c r="G38" s="119" t="s">
-        <v>89</v>
+      <c r="G38" s="121" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -23127,7 +23270,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="F3:F35">
-    <cfRule type="colorScale" priority="79">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -23137,7 +23280,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G21">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
         <cfvo type="formula" val="$I$4"/>
@@ -23147,16 +23290,31 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G27">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="52" operator="equal">
+      <formula>$I$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
@@ -23167,11 +23325,38 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="50" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
+      <formula>$I$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="45" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G22">
+  <conditionalFormatting sqref="G25">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
@@ -23183,8 +23368,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G23">
-    <cfRule type="colorScale" priority="21">
+  <conditionalFormatting sqref="G26">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
         <cfvo type="formula" val="$I$4"/>
@@ -23194,12 +23379,12 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24">
-    <cfRule type="colorScale" priority="42">
+  <conditionalFormatting sqref="G27">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
         <cfvo type="formula" val="$I$4"/>
@@ -23209,73 +23394,31 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="43" operator="equal">
-      <formula>$I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G25">
-    <cfRule type="colorScale" priority="45">
-      <colorScale>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G26">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
-      <formula>$I$5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G27">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="42" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28 G30:G34">
-    <cfRule type="cellIs" dxfId="11" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="58" operator="equal">
       <formula>$I$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="59" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="58" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="10" priority="60" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH(("Not Started"),(G28))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:G34">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="containsText" dxfId="7" priority="14" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="8" priority="16" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(G29))))</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
         <cfvo type="formula" val="$I$4"/>
@@ -23287,7 +23430,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G34 G28">
-    <cfRule type="colorScale" priority="59">
+    <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="formula" val="$I$3"/>
         <cfvo type="formula" val="$I$4"/>
@@ -23299,7 +23442,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
         <cfvo type="formula" val="$I$4"/>
@@ -23310,13 +23453,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35:G38">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="In Progress">
+  <conditionalFormatting sqref="G35:G37">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH(("In Progress"),(G35))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G36">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="G35:G36">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
         <cfvo type="formula" val="$I$4"/>
@@ -23326,12 +23469,12 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G36:G37">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="G35:G37">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
         <cfvo type="formula" val="$I$4"/>
@@ -23341,8 +23484,48 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
       <formula>$I$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="cellIs" dxfId="3" priority="65" operator="equal">
+      <formula>$I$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I5">
+    <cfRule type="containsText" dxfId="2" priority="62" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH(("In Progress"),(I3))))</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="63">
+      <colorScale>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="1" priority="64" operator="equal">
+      <formula>$I$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K10">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFFFFF"/>
+        <color rgb="FFAFCAC4"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G38">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH(("In Progress"),(G38))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
@@ -23354,44 +23537,6 @@
         <color rgb="FFF8E5DA"/>
         <color rgb="FFF7EFDE"/>
         <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>$I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="2" priority="63" operator="equal">
-      <formula>$I$3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I5">
-    <cfRule type="containsText" dxfId="1" priority="60" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH(("In Progress"),(I3))))</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="61">
-      <colorScale>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="0" priority="62" operator="equal">
-      <formula>$I$5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K10">
-    <cfRule type="colorScale" priority="64">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FFAFCAC4"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Animaldex document to update again
</commit_message>
<xml_diff>
--- a/docs/AnimalDex.xlsx
+++ b/docs/AnimalDex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alessandro\Uni\Magistrale\LABAP\AnimalDex\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D3D3CE-13DA-45DC-84BA-9AF569EED3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29333913-CE4D-4DFD-B229-865EEAAC8F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLE Gantt Chart &amp; Burndown" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="342">
   <si>
     <t>SCRUM PROJECT MANAGEMENT GANTT CHART</t>
   </si>
@@ -1059,6 +1059,9 @@
   </si>
   <si>
     <t>Profile image pt2  and centralDB restructuring</t>
+  </si>
+  <si>
+    <t>Notification (Dieni/Baldi)</t>
   </si>
 </sst>
 </file>
@@ -3071,53 +3074,14 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="33" fillId="31" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3148,23 +3112,62 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="29" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7941,19 +7944,19 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
-      <c r="BK2" s="244" t="str">
+      <c r="BK2" s="227" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","https://goo.gl/ejIdKR")</f>
         <v>https://goo.gl/ejIdKR</v>
       </c>
-      <c r="BL2" s="245"/>
-      <c r="BM2" s="245"/>
-      <c r="BN2" s="245"/>
-      <c r="BO2" s="245"/>
-      <c r="BP2" s="245"/>
-      <c r="BQ2" s="245"/>
-      <c r="BR2" s="245"/>
-      <c r="BS2" s="245"/>
-      <c r="BT2" s="245"/>
+      <c r="BL2" s="228"/>
+      <c r="BM2" s="228"/>
+      <c r="BN2" s="228"/>
+      <c r="BO2" s="228"/>
+      <c r="BP2" s="228"/>
+      <c r="BQ2" s="228"/>
+      <c r="BR2" s="228"/>
+      <c r="BS2" s="228"/>
+      <c r="BT2" s="228"/>
     </row>
     <row r="3" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -7981,7 +7984,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="246" t="s">
+      <c r="K4" s="229" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8" t="s">
@@ -8058,7 +8061,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="247"/>
+      <c r="K5" s="230"/>
       <c r="L5" s="13" t="s">
         <v>4</v>
       </c>
@@ -8133,7 +8136,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="247"/>
+      <c r="K6" s="230"/>
       <c r="L6" s="18" t="s">
         <v>5</v>
       </c>
@@ -8208,7 +8211,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="247"/>
+      <c r="K7" s="230"/>
       <c r="L7" s="20" t="s">
         <v>6</v>
       </c>
@@ -8283,7 +8286,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="248"/>
+      <c r="K8" s="231"/>
       <c r="L8" s="22" t="s">
         <v>7</v>
       </c>
@@ -8349,124 +8352,124 @@
       <c r="BT8" s="17"/>
     </row>
     <row r="9" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="249" t="s">
+      <c r="B9" s="232" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="251" t="s">
+      <c r="C9" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="253" t="s">
+      <c r="D9" s="236" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="255" t="s">
+      <c r="E9" s="238" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="256"/>
-      <c r="G9" s="257"/>
-      <c r="H9" s="258" t="s">
+      <c r="F9" s="239"/>
+      <c r="G9" s="240"/>
+      <c r="H9" s="241" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="226" t="s">
+      <c r="I9" s="246" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="228" t="s">
+      <c r="J9" s="248" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="230" t="s">
+      <c r="K9" s="250" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="231" t="s">
+      <c r="L9" s="251" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="233" t="s">
+      <c r="M9" s="253" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="234"/>
-      <c r="O9" s="234"/>
-      <c r="P9" s="234"/>
-      <c r="Q9" s="235"/>
-      <c r="R9" s="236" t="s">
+      <c r="N9" s="225"/>
+      <c r="O9" s="225"/>
+      <c r="P9" s="225"/>
+      <c r="Q9" s="254"/>
+      <c r="R9" s="255" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="234"/>
-      <c r="T9" s="234"/>
-      <c r="U9" s="234"/>
-      <c r="V9" s="235"/>
-      <c r="W9" s="236" t="s">
+      <c r="S9" s="225"/>
+      <c r="T9" s="225"/>
+      <c r="U9" s="225"/>
+      <c r="V9" s="254"/>
+      <c r="W9" s="255" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="234"/>
-      <c r="Y9" s="234"/>
-      <c r="Z9" s="234"/>
-      <c r="AA9" s="237"/>
-      <c r="AB9" s="238" t="s">
+      <c r="X9" s="225"/>
+      <c r="Y9" s="225"/>
+      <c r="Z9" s="225"/>
+      <c r="AA9" s="226"/>
+      <c r="AB9" s="256" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="234"/>
-      <c r="AD9" s="234"/>
-      <c r="AE9" s="234"/>
-      <c r="AF9" s="235"/>
-      <c r="AG9" s="239" t="s">
+      <c r="AC9" s="225"/>
+      <c r="AD9" s="225"/>
+      <c r="AE9" s="225"/>
+      <c r="AF9" s="254"/>
+      <c r="AG9" s="257" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="234"/>
-      <c r="AI9" s="234"/>
-      <c r="AJ9" s="234"/>
-      <c r="AK9" s="235"/>
-      <c r="AL9" s="239" t="s">
+      <c r="AH9" s="225"/>
+      <c r="AI9" s="225"/>
+      <c r="AJ9" s="225"/>
+      <c r="AK9" s="254"/>
+      <c r="AL9" s="257" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="234"/>
-      <c r="AN9" s="234"/>
-      <c r="AO9" s="234"/>
-      <c r="AP9" s="237"/>
-      <c r="AQ9" s="240" t="s">
+      <c r="AM9" s="225"/>
+      <c r="AN9" s="225"/>
+      <c r="AO9" s="225"/>
+      <c r="AP9" s="226"/>
+      <c r="AQ9" s="258" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="234"/>
-      <c r="AS9" s="234"/>
-      <c r="AT9" s="234"/>
-      <c r="AU9" s="235"/>
-      <c r="AV9" s="241" t="s">
+      <c r="AR9" s="225"/>
+      <c r="AS9" s="225"/>
+      <c r="AT9" s="225"/>
+      <c r="AU9" s="254"/>
+      <c r="AV9" s="259" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="234"/>
-      <c r="AX9" s="234"/>
-      <c r="AY9" s="234"/>
-      <c r="AZ9" s="235"/>
-      <c r="BA9" s="241" t="s">
+      <c r="AW9" s="225"/>
+      <c r="AX9" s="225"/>
+      <c r="AY9" s="225"/>
+      <c r="AZ9" s="254"/>
+      <c r="BA9" s="259" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="234"/>
-      <c r="BC9" s="234"/>
-      <c r="BD9" s="234"/>
-      <c r="BE9" s="237"/>
-      <c r="BF9" s="242" t="s">
+      <c r="BB9" s="225"/>
+      <c r="BC9" s="225"/>
+      <c r="BD9" s="225"/>
+      <c r="BE9" s="226"/>
+      <c r="BF9" s="260" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="234"/>
-      <c r="BH9" s="234"/>
-      <c r="BI9" s="234"/>
-      <c r="BJ9" s="235"/>
-      <c r="BK9" s="243" t="s">
+      <c r="BG9" s="225"/>
+      <c r="BH9" s="225"/>
+      <c r="BI9" s="225"/>
+      <c r="BJ9" s="254"/>
+      <c r="BK9" s="224" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="234"/>
-      <c r="BM9" s="234"/>
-      <c r="BN9" s="234"/>
-      <c r="BO9" s="235"/>
-      <c r="BP9" s="243" t="s">
+      <c r="BL9" s="225"/>
+      <c r="BM9" s="225"/>
+      <c r="BN9" s="225"/>
+      <c r="BO9" s="254"/>
+      <c r="BP9" s="224" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="234"/>
-      <c r="BR9" s="234"/>
-      <c r="BS9" s="234"/>
-      <c r="BT9" s="237"/>
+      <c r="BQ9" s="225"/>
+      <c r="BR9" s="225"/>
+      <c r="BS9" s="225"/>
+      <c r="BT9" s="226"/>
     </row>
     <row r="10" spans="2:74" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="250"/>
-      <c r="C10" s="252"/>
-      <c r="D10" s="254"/>
+      <c r="B10" s="233"/>
+      <c r="C10" s="235"/>
+      <c r="D10" s="237"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -8476,11 +8479,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="259"/>
-      <c r="I10" s="227"/>
-      <c r="J10" s="229"/>
-      <c r="K10" s="229"/>
-      <c r="L10" s="232"/>
+      <c r="H10" s="242"/>
+      <c r="I10" s="247"/>
+      <c r="J10" s="249"/>
+      <c r="K10" s="249"/>
+      <c r="L10" s="252"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -12089,80 +12092,80 @@
     <row r="43" spans="2:74" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:74" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="223" t="str">
+      <c r="B45" s="243" t="str">
         <f>HYPERLINK("https://goo.gl/ejIdKR","CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET")</f>
         <v>CLICK HERE TO CREATE GANTT CHART TEMPLATES IN SMARTSHEET</v>
       </c>
-      <c r="C45" s="224"/>
-      <c r="D45" s="224"/>
-      <c r="E45" s="224"/>
-      <c r="F45" s="224"/>
-      <c r="G45" s="224"/>
-      <c r="H45" s="224"/>
-      <c r="I45" s="224"/>
-      <c r="J45" s="224"/>
-      <c r="K45" s="224"/>
-      <c r="L45" s="224"/>
-      <c r="M45" s="224"/>
-      <c r="N45" s="224"/>
-      <c r="O45" s="224"/>
-      <c r="P45" s="224"/>
-      <c r="Q45" s="224"/>
-      <c r="R45" s="224"/>
-      <c r="S45" s="224"/>
-      <c r="T45" s="224"/>
-      <c r="U45" s="224"/>
-      <c r="V45" s="224"/>
-      <c r="W45" s="224"/>
-      <c r="X45" s="224"/>
-      <c r="Y45" s="224"/>
-      <c r="Z45" s="224"/>
-      <c r="AA45" s="224"/>
-      <c r="AB45" s="224"/>
-      <c r="AC45" s="224"/>
-      <c r="AD45" s="224"/>
-      <c r="AE45" s="224"/>
-      <c r="AF45" s="224"/>
-      <c r="AG45" s="224"/>
-      <c r="AH45" s="224"/>
-      <c r="AI45" s="224"/>
-      <c r="AJ45" s="224"/>
-      <c r="AK45" s="224"/>
-      <c r="AL45" s="224"/>
-      <c r="AM45" s="224"/>
-      <c r="AN45" s="224"/>
-      <c r="AO45" s="224"/>
-      <c r="AP45" s="224"/>
-      <c r="AQ45" s="224"/>
-      <c r="AR45" s="224"/>
-      <c r="AS45" s="224"/>
-      <c r="AT45" s="224"/>
-      <c r="AU45" s="224"/>
-      <c r="AV45" s="224"/>
-      <c r="AW45" s="224"/>
-      <c r="AX45" s="224"/>
-      <c r="AY45" s="224"/>
-      <c r="AZ45" s="224"/>
-      <c r="BA45" s="224"/>
-      <c r="BB45" s="224"/>
-      <c r="BC45" s="224"/>
-      <c r="BD45" s="224"/>
-      <c r="BE45" s="224"/>
-      <c r="BF45" s="224"/>
-      <c r="BG45" s="224"/>
-      <c r="BH45" s="224"/>
-      <c r="BI45" s="224"/>
-      <c r="BJ45" s="224"/>
-      <c r="BK45" s="224"/>
-      <c r="BL45" s="224"/>
-      <c r="BM45" s="224"/>
-      <c r="BN45" s="224"/>
-      <c r="BO45" s="224"/>
-      <c r="BP45" s="224"/>
-      <c r="BQ45" s="224"/>
-      <c r="BR45" s="224"/>
-      <c r="BS45" s="224"/>
-      <c r="BT45" s="225"/>
+      <c r="C45" s="244"/>
+      <c r="D45" s="244"/>
+      <c r="E45" s="244"/>
+      <c r="F45" s="244"/>
+      <c r="G45" s="244"/>
+      <c r="H45" s="244"/>
+      <c r="I45" s="244"/>
+      <c r="J45" s="244"/>
+      <c r="K45" s="244"/>
+      <c r="L45" s="244"/>
+      <c r="M45" s="244"/>
+      <c r="N45" s="244"/>
+      <c r="O45" s="244"/>
+      <c r="P45" s="244"/>
+      <c r="Q45" s="244"/>
+      <c r="R45" s="244"/>
+      <c r="S45" s="244"/>
+      <c r="T45" s="244"/>
+      <c r="U45" s="244"/>
+      <c r="V45" s="244"/>
+      <c r="W45" s="244"/>
+      <c r="X45" s="244"/>
+      <c r="Y45" s="244"/>
+      <c r="Z45" s="244"/>
+      <c r="AA45" s="244"/>
+      <c r="AB45" s="244"/>
+      <c r="AC45" s="244"/>
+      <c r="AD45" s="244"/>
+      <c r="AE45" s="244"/>
+      <c r="AF45" s="244"/>
+      <c r="AG45" s="244"/>
+      <c r="AH45" s="244"/>
+      <c r="AI45" s="244"/>
+      <c r="AJ45" s="244"/>
+      <c r="AK45" s="244"/>
+      <c r="AL45" s="244"/>
+      <c r="AM45" s="244"/>
+      <c r="AN45" s="244"/>
+      <c r="AO45" s="244"/>
+      <c r="AP45" s="244"/>
+      <c r="AQ45" s="244"/>
+      <c r="AR45" s="244"/>
+      <c r="AS45" s="244"/>
+      <c r="AT45" s="244"/>
+      <c r="AU45" s="244"/>
+      <c r="AV45" s="244"/>
+      <c r="AW45" s="244"/>
+      <c r="AX45" s="244"/>
+      <c r="AY45" s="244"/>
+      <c r="AZ45" s="244"/>
+      <c r="BA45" s="244"/>
+      <c r="BB45" s="244"/>
+      <c r="BC45" s="244"/>
+      <c r="BD45" s="244"/>
+      <c r="BE45" s="244"/>
+      <c r="BF45" s="244"/>
+      <c r="BG45" s="244"/>
+      <c r="BH45" s="244"/>
+      <c r="BI45" s="244"/>
+      <c r="BJ45" s="244"/>
+      <c r="BK45" s="244"/>
+      <c r="BL45" s="244"/>
+      <c r="BM45" s="244"/>
+      <c r="BN45" s="244"/>
+      <c r="BO45" s="244"/>
+      <c r="BP45" s="244"/>
+      <c r="BQ45" s="244"/>
+      <c r="BR45" s="244"/>
+      <c r="BS45" s="244"/>
+      <c r="BT45" s="245"/>
     </row>
     <row r="46" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13125,14 +13128,6 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="BK2:BT2"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B45:BT45"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
@@ -13149,6 +13144,14 @@
     <mergeCell ref="BA9:BE9"/>
     <mergeCell ref="BF9:BJ9"/>
     <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="BK2:BT2"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -13163,7 +13166,7 @@
   </sheetPr>
   <dimension ref="B1:CX1034"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -13304,7 +13307,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="246" t="s">
+      <c r="K3" s="229" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="8" t="s">
@@ -13411,7 +13414,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="247"/>
+      <c r="K4" s="230"/>
       <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
@@ -13515,7 +13518,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="247"/>
+      <c r="K5" s="230"/>
       <c r="L5" s="18" t="s">
         <v>5</v>
       </c>
@@ -13619,7 +13622,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="247"/>
+      <c r="K6" s="230"/>
       <c r="L6" s="20" t="s">
         <v>6</v>
       </c>
@@ -13724,7 +13727,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="248"/>
+      <c r="K7" s="231"/>
       <c r="L7" s="22" t="s">
         <v>7</v>
       </c>
@@ -13925,166 +13928,166 @@
       <c r="CX8" s="192"/>
     </row>
     <row r="9" spans="2:102" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="249" t="s">
+      <c r="B9" s="232" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="251" t="s">
+      <c r="C9" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="253" t="s">
+      <c r="D9" s="236" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="255" t="s">
+      <c r="E9" s="238" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="256"/>
-      <c r="G9" s="257"/>
-      <c r="H9" s="258" t="s">
+      <c r="F9" s="239"/>
+      <c r="G9" s="240"/>
+      <c r="H9" s="241" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="226" t="s">
+      <c r="I9" s="246" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="228" t="s">
+      <c r="J9" s="248" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="230" t="s">
+      <c r="K9" s="250" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="231" t="s">
+      <c r="L9" s="251" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="233" t="s">
+      <c r="M9" s="253" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="234"/>
-      <c r="O9" s="234"/>
-      <c r="P9" s="234"/>
-      <c r="Q9" s="235"/>
-      <c r="R9" s="236" t="s">
+      <c r="N9" s="225"/>
+      <c r="O9" s="225"/>
+      <c r="P9" s="225"/>
+      <c r="Q9" s="254"/>
+      <c r="R9" s="255" t="s">
         <v>18</v>
       </c>
-      <c r="S9" s="234"/>
-      <c r="T9" s="234"/>
-      <c r="U9" s="234"/>
-      <c r="V9" s="235"/>
-      <c r="W9" s="236" t="s">
+      <c r="S9" s="225"/>
+      <c r="T9" s="225"/>
+      <c r="U9" s="225"/>
+      <c r="V9" s="254"/>
+      <c r="W9" s="255" t="s">
         <v>19</v>
       </c>
-      <c r="X9" s="234"/>
-      <c r="Y9" s="234"/>
-      <c r="Z9" s="234"/>
-      <c r="AA9" s="237"/>
-      <c r="AB9" s="238" t="s">
+      <c r="X9" s="225"/>
+      <c r="Y9" s="225"/>
+      <c r="Z9" s="225"/>
+      <c r="AA9" s="226"/>
+      <c r="AB9" s="256" t="s">
         <v>20</v>
       </c>
-      <c r="AC9" s="234"/>
-      <c r="AD9" s="234"/>
-      <c r="AE9" s="234"/>
-      <c r="AF9" s="235"/>
-      <c r="AG9" s="239" t="s">
+      <c r="AC9" s="225"/>
+      <c r="AD9" s="225"/>
+      <c r="AE9" s="225"/>
+      <c r="AF9" s="254"/>
+      <c r="AG9" s="257" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="234"/>
-      <c r="AI9" s="234"/>
-      <c r="AJ9" s="234"/>
-      <c r="AK9" s="235"/>
-      <c r="AL9" s="239" t="s">
+      <c r="AH9" s="225"/>
+      <c r="AI9" s="225"/>
+      <c r="AJ9" s="225"/>
+      <c r="AK9" s="254"/>
+      <c r="AL9" s="257" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="234"/>
-      <c r="AN9" s="234"/>
-      <c r="AO9" s="234"/>
-      <c r="AP9" s="237"/>
-      <c r="AQ9" s="240" t="s">
+      <c r="AM9" s="225"/>
+      <c r="AN9" s="225"/>
+      <c r="AO9" s="225"/>
+      <c r="AP9" s="226"/>
+      <c r="AQ9" s="258" t="s">
         <v>23</v>
       </c>
-      <c r="AR9" s="234"/>
-      <c r="AS9" s="234"/>
-      <c r="AT9" s="234"/>
-      <c r="AU9" s="235"/>
-      <c r="AV9" s="241" t="s">
+      <c r="AR9" s="225"/>
+      <c r="AS9" s="225"/>
+      <c r="AT9" s="225"/>
+      <c r="AU9" s="254"/>
+      <c r="AV9" s="259" t="s">
         <v>24</v>
       </c>
-      <c r="AW9" s="234"/>
-      <c r="AX9" s="234"/>
-      <c r="AY9" s="234"/>
-      <c r="AZ9" s="235"/>
-      <c r="BA9" s="241" t="s">
+      <c r="AW9" s="225"/>
+      <c r="AX9" s="225"/>
+      <c r="AY9" s="225"/>
+      <c r="AZ9" s="254"/>
+      <c r="BA9" s="259" t="s">
         <v>25</v>
       </c>
-      <c r="BB9" s="234"/>
-      <c r="BC9" s="234"/>
-      <c r="BD9" s="234"/>
-      <c r="BE9" s="237"/>
-      <c r="BF9" s="261" t="s">
+      <c r="BB9" s="225"/>
+      <c r="BC9" s="225"/>
+      <c r="BD9" s="225"/>
+      <c r="BE9" s="226"/>
+      <c r="BF9" s="268" t="s">
         <v>26</v>
       </c>
-      <c r="BG9" s="234"/>
-      <c r="BH9" s="234"/>
-      <c r="BI9" s="234"/>
-      <c r="BJ9" s="235"/>
-      <c r="BK9" s="243" t="s">
+      <c r="BG9" s="225"/>
+      <c r="BH9" s="225"/>
+      <c r="BI9" s="225"/>
+      <c r="BJ9" s="254"/>
+      <c r="BK9" s="224" t="s">
         <v>27</v>
       </c>
-      <c r="BL9" s="234"/>
-      <c r="BM9" s="234"/>
-      <c r="BN9" s="234"/>
-      <c r="BO9" s="235"/>
-      <c r="BP9" s="243" t="s">
+      <c r="BL9" s="225"/>
+      <c r="BM9" s="225"/>
+      <c r="BN9" s="225"/>
+      <c r="BO9" s="254"/>
+      <c r="BP9" s="224" t="s">
         <v>28</v>
       </c>
-      <c r="BQ9" s="234"/>
-      <c r="BR9" s="234"/>
-      <c r="BS9" s="234"/>
-      <c r="BT9" s="237"/>
-      <c r="BU9" s="262" t="s">
+      <c r="BQ9" s="225"/>
+      <c r="BR9" s="225"/>
+      <c r="BS9" s="225"/>
+      <c r="BT9" s="226"/>
+      <c r="BU9" s="264" t="s">
         <v>274</v>
       </c>
-      <c r="BV9" s="263"/>
-      <c r="BW9" s="263"/>
-      <c r="BX9" s="263"/>
-      <c r="BY9" s="264"/>
-      <c r="BZ9" s="262" t="s">
+      <c r="BV9" s="265"/>
+      <c r="BW9" s="265"/>
+      <c r="BX9" s="265"/>
+      <c r="BY9" s="266"/>
+      <c r="BZ9" s="264" t="s">
         <v>275</v>
       </c>
-      <c r="CA9" s="263"/>
-      <c r="CB9" s="263"/>
-      <c r="CC9" s="263"/>
-      <c r="CD9" s="264"/>
-      <c r="CE9" s="262" t="s">
+      <c r="CA9" s="265"/>
+      <c r="CB9" s="265"/>
+      <c r="CC9" s="265"/>
+      <c r="CD9" s="266"/>
+      <c r="CE9" s="264" t="s">
         <v>276</v>
       </c>
-      <c r="CF9" s="263"/>
-      <c r="CG9" s="263"/>
-      <c r="CH9" s="263"/>
-      <c r="CI9" s="264"/>
-      <c r="CJ9" s="262" t="s">
+      <c r="CF9" s="265"/>
+      <c r="CG9" s="265"/>
+      <c r="CH9" s="265"/>
+      <c r="CI9" s="266"/>
+      <c r="CJ9" s="264" t="s">
         <v>277</v>
       </c>
-      <c r="CK9" s="263"/>
-      <c r="CL9" s="263"/>
-      <c r="CM9" s="263"/>
-      <c r="CN9" s="264"/>
-      <c r="CO9" s="265" t="s">
+      <c r="CK9" s="265"/>
+      <c r="CL9" s="265"/>
+      <c r="CM9" s="265"/>
+      <c r="CN9" s="266"/>
+      <c r="CO9" s="261" t="s">
         <v>322</v>
       </c>
-      <c r="CP9" s="266"/>
-      <c r="CQ9" s="266"/>
-      <c r="CR9" s="266"/>
-      <c r="CS9" s="267"/>
-      <c r="CT9" s="265" t="s">
+      <c r="CP9" s="262"/>
+      <c r="CQ9" s="262"/>
+      <c r="CR9" s="262"/>
+      <c r="CS9" s="263"/>
+      <c r="CT9" s="261" t="s">
         <v>323</v>
       </c>
-      <c r="CU9" s="266"/>
-      <c r="CV9" s="266"/>
-      <c r="CW9" s="266"/>
-      <c r="CX9" s="267"/>
+      <c r="CU9" s="262"/>
+      <c r="CV9" s="262"/>
+      <c r="CW9" s="262"/>
+      <c r="CX9" s="263"/>
     </row>
     <row r="10" spans="2:102" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="250"/>
-      <c r="C10" s="252"/>
-      <c r="D10" s="254"/>
+      <c r="B10" s="233"/>
+      <c r="C10" s="235"/>
+      <c r="D10" s="237"/>
       <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
@@ -14094,11 +14097,11 @@
       <c r="G10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="259"/>
-      <c r="I10" s="227"/>
-      <c r="J10" s="229"/>
-      <c r="K10" s="229"/>
-      <c r="L10" s="232"/>
+      <c r="H10" s="242"/>
+      <c r="I10" s="247"/>
+      <c r="J10" s="249"/>
+      <c r="K10" s="249"/>
+      <c r="L10" s="252"/>
       <c r="M10" s="27" t="s">
         <v>32</v>
       </c>
@@ -15284,7 +15287,7 @@
       </c>
       <c r="I18" s="76"/>
       <c r="J18" s="77"/>
-      <c r="K18" s="268"/>
+      <c r="K18" s="223"/>
       <c r="L18" s="49">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -16685,7 +16688,7 @@
       </c>
       <c r="I29" s="76"/>
       <c r="J29" s="77"/>
-      <c r="K29" s="268"/>
+      <c r="K29" s="223"/>
       <c r="L29" s="49">
         <f t="shared" si="0"/>
         <v>1.0869565217391304</v>
@@ -18468,7 +18471,7 @@
       </c>
       <c r="I43" s="76"/>
       <c r="J43" s="77"/>
-      <c r="K43" s="268"/>
+      <c r="K43" s="223"/>
       <c r="L43" s="49">
         <f t="shared" si="0"/>
         <v>0.89473684210526316</v>
@@ -19353,7 +19356,7 @@
       </c>
       <c r="I50" s="76"/>
       <c r="J50" s="77"/>
-      <c r="K50" s="268"/>
+      <c r="K50" s="223"/>
       <c r="L50" s="49">
         <f t="shared" ref="L50:L51" si="13">F50/E50</f>
         <v>0.86956521739130432</v>
@@ -21132,7 +21135,7 @@
       </c>
       <c r="I64" s="76"/>
       <c r="J64" s="77"/>
-      <c r="K64" s="268"/>
+      <c r="K64" s="223"/>
       <c r="L64" s="49">
         <f t="shared" si="45"/>
         <v>1</v>
@@ -22930,58 +22933,58 @@
     <row r="76" spans="2:102" ht="223.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="2:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="2:102" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E78" s="260" t="s">
+      <c r="E78" s="267" t="s">
         <v>83</v>
       </c>
-      <c r="F78" s="224"/>
-      <c r="G78" s="224"/>
-      <c r="H78" s="224"/>
-      <c r="I78" s="224"/>
-      <c r="J78" s="224"/>
-      <c r="K78" s="224"/>
-      <c r="L78" s="224"/>
-      <c r="M78" s="224"/>
-      <c r="N78" s="224"/>
-      <c r="O78" s="224"/>
-      <c r="P78" s="224"/>
-      <c r="Q78" s="224"/>
-      <c r="R78" s="224"/>
-      <c r="S78" s="224"/>
-      <c r="T78" s="224"/>
-      <c r="U78" s="224"/>
-      <c r="V78" s="224"/>
-      <c r="W78" s="224"/>
-      <c r="X78" s="224"/>
-      <c r="Y78" s="224"/>
-      <c r="Z78" s="224"/>
-      <c r="AA78" s="224"/>
-      <c r="AB78" s="224"/>
-      <c r="AC78" s="224"/>
-      <c r="AD78" s="224"/>
-      <c r="AE78" s="224"/>
-      <c r="AF78" s="224"/>
-      <c r="AG78" s="224"/>
-      <c r="AH78" s="224"/>
-      <c r="AI78" s="224"/>
-      <c r="AJ78" s="224"/>
-      <c r="AK78" s="224"/>
-      <c r="AL78" s="224"/>
-      <c r="AM78" s="224"/>
-      <c r="AN78" s="224"/>
-      <c r="AO78" s="224"/>
-      <c r="AP78" s="224"/>
-      <c r="AQ78" s="224"/>
-      <c r="AR78" s="224"/>
-      <c r="AS78" s="224"/>
-      <c r="AT78" s="224"/>
-      <c r="AU78" s="224"/>
-      <c r="AV78" s="224"/>
-      <c r="AW78" s="224"/>
-      <c r="AX78" s="224"/>
-      <c r="AY78" s="224"/>
-      <c r="AZ78" s="224"/>
-      <c r="BA78" s="224"/>
-      <c r="BB78" s="225"/>
+      <c r="F78" s="244"/>
+      <c r="G78" s="244"/>
+      <c r="H78" s="244"/>
+      <c r="I78" s="244"/>
+      <c r="J78" s="244"/>
+      <c r="K78" s="244"/>
+      <c r="L78" s="244"/>
+      <c r="M78" s="244"/>
+      <c r="N78" s="244"/>
+      <c r="O78" s="244"/>
+      <c r="P78" s="244"/>
+      <c r="Q78" s="244"/>
+      <c r="R78" s="244"/>
+      <c r="S78" s="244"/>
+      <c r="T78" s="244"/>
+      <c r="U78" s="244"/>
+      <c r="V78" s="244"/>
+      <c r="W78" s="244"/>
+      <c r="X78" s="244"/>
+      <c r="Y78" s="244"/>
+      <c r="Z78" s="244"/>
+      <c r="AA78" s="244"/>
+      <c r="AB78" s="244"/>
+      <c r="AC78" s="244"/>
+      <c r="AD78" s="244"/>
+      <c r="AE78" s="244"/>
+      <c r="AF78" s="244"/>
+      <c r="AG78" s="244"/>
+      <c r="AH78" s="244"/>
+      <c r="AI78" s="244"/>
+      <c r="AJ78" s="244"/>
+      <c r="AK78" s="244"/>
+      <c r="AL78" s="244"/>
+      <c r="AM78" s="244"/>
+      <c r="AN78" s="244"/>
+      <c r="AO78" s="244"/>
+      <c r="AP78" s="244"/>
+      <c r="AQ78" s="244"/>
+      <c r="AR78" s="244"/>
+      <c r="AS78" s="244"/>
+      <c r="AT78" s="244"/>
+      <c r="AU78" s="244"/>
+      <c r="AV78" s="244"/>
+      <c r="AW78" s="244"/>
+      <c r="AX78" s="244"/>
+      <c r="AY78" s="244"/>
+      <c r="AZ78" s="244"/>
+      <c r="BA78" s="244"/>
+      <c r="BB78" s="245"/>
     </row>
     <row r="79" spans="2:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="2:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -23944,6 +23947,23 @@
     <row r="1034" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="E78:BB78"/>
+    <mergeCell ref="BF9:BJ9"/>
+    <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:Q9"/>
+    <mergeCell ref="R9:V9"/>
+    <mergeCell ref="W9:AA9"/>
+    <mergeCell ref="AB9:AF9"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="BU9:BY9"/>
+    <mergeCell ref="BZ9:CD9"/>
+    <mergeCell ref="CE9:CI9"/>
+    <mergeCell ref="CJ9:CN9"/>
     <mergeCell ref="CO9:CS9"/>
     <mergeCell ref="CT9:CX9"/>
     <mergeCell ref="I9:I10"/>
@@ -23956,23 +23976,6 @@
     <mergeCell ref="AQ9:AU9"/>
     <mergeCell ref="AV9:AZ9"/>
     <mergeCell ref="BA9:BE9"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="BU9:BY9"/>
-    <mergeCell ref="BZ9:CD9"/>
-    <mergeCell ref="CE9:CI9"/>
-    <mergeCell ref="CJ9:CN9"/>
-    <mergeCell ref="E78:BB78"/>
-    <mergeCell ref="BF9:BJ9"/>
-    <mergeCell ref="BK9:BO9"/>
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:Q9"/>
-    <mergeCell ref="R9:V9"/>
-    <mergeCell ref="W9:AA9"/>
-    <mergeCell ref="AB9:AF9"/>
-    <mergeCell ref="AG9:AK9"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23989,8 +23992,8 @@
   </sheetPr>
   <dimension ref="B1:K1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24592,7 +24595,7 @@
         <v>153</v>
       </c>
       <c r="E31" s="116" t="s">
-        <v>186</v>
+        <v>341</v>
       </c>
       <c r="F31" s="117"/>
       <c r="G31" s="118" t="s">
@@ -25717,6 +25720,9 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G21">
+    <cfRule type="cellIs" dxfId="24" priority="39" operator="equal">
+      <formula>$I$5</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
@@ -25727,11 +25733,11 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="39" operator="equal">
-      <formula>$I$5</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
+    <cfRule type="cellIs" dxfId="23" priority="64" operator="equal">
+      <formula>$I$3</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
@@ -25741,9 +25747,6 @@
         <color rgb="FFF7EFDE"/>
         <color rgb="FFE9E7E7"/>
       </colorScale>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="64" operator="equal">
-      <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
@@ -25771,6 +25774,9 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:G25">
+    <cfRule type="cellIs" dxfId="18" priority="36" operator="equal">
+      <formula>$I$5</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
@@ -25781,9 +25787,6 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="36" operator="equal">
-      <formula>$I$5</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:G27 G3:G21">
     <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="In Progress">
@@ -25791,6 +25794,9 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24:G25">
+    <cfRule type="cellIs" dxfId="16" priority="57" operator="equal">
+      <formula>$I$3</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
@@ -25800,9 +25806,6 @@
         <color rgb="FFF7EFDE"/>
         <color rgb="FFE9E7E7"/>
       </colorScale>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="57" operator="equal">
-      <formula>$I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
@@ -25833,16 +25836,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$4"/>
-        <cfvo type="formula" val="$I$5"/>
-        <color rgb="FFF8E5DA"/>
-        <color rgb="FFF7EFDE"/>
-        <color rgb="FFE9E7E7"/>
-      </colorScale>
-    </cfRule>
     <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>$I$5</formula>
     </cfRule>
@@ -25860,6 +25853,16 @@
       <formula>$I$3</formula>
     </cfRule>
     <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$4"/>
+        <cfvo type="formula" val="$I$5"/>
+        <color rgb="FFF8E5DA"/>
+        <color rgb="FFF7EFDE"/>
+        <color rgb="FFE9E7E7"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
         <cfvo type="formula" val="$I$4"/>
@@ -25929,6 +25932,9 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:G37">
+    <cfRule type="cellIs" dxfId="6" priority="22" operator="equal">
+      <formula>$I$3</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
@@ -25939,11 +25945,11 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="22" operator="equal">
-      <formula>$I$3</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:G38">
+    <cfRule type="cellIs" dxfId="5" priority="27" operator="equal">
+      <formula>$I$5</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
@@ -25954,9 +25960,6 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="27" operator="equal">
-      <formula>$I$5</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:G39">
     <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="In Progress">
@@ -25964,6 +25967,9 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+      <formula>$I$5</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
@@ -25974,9 +25980,6 @@
         <color rgb="FFE9E7E7"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
-      <formula>$I$5</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
     <cfRule type="cellIs" dxfId="2" priority="77" operator="equal">
@@ -25984,9 +25987,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I5">
-    <cfRule type="containsText" dxfId="1" priority="74" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH(("In Progress"),(I3))))</formula>
-    </cfRule>
     <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="formula" val="$I$4"/>
@@ -25996,6 +25996,9 @@
         <color rgb="FFF7EFDE"/>
         <color rgb="FFE9E7E7"/>
       </colorScale>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="74" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH(("In Progress"),(I3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">

</xml_diff>